<commit_message>
Use colors to distinguish providers. New graphs: cost per period and performance.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="186">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="3"/>
@@ -1383,6 +1383,10 @@
     <t>SK M40x1 m.</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>per year USD</t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
@@ -1789,7 +1793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="567">
+  <cellStyleXfs count="573">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2365,8 +2369,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -2486,6 +2496,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="62" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2505,7 +2518,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="567">
+  <cellStyles count="573">
     <cellStyle name="Calculation" xfId="344" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="346" builtinId="23" hidden="1"/>
     <cellStyle name="comment" xfId="120"/>
@@ -2784,6 +2797,9 @@
     <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="264" builtinId="17" customBuiltin="1"/>
@@ -3063,6 +3079,9 @@
     <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="342" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="345" builtinId="24" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3074,7 +3093,40 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="341" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3229,17 +3281,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -3456,8 +3497,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="-2125577592"/>
-        <c:axId val="-2125579704"/>
+        <c:axId val="2088531896"/>
+        <c:axId val="2088535352"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -3661,11 +3702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="-2125587464"/>
-        <c:axId val="-2125582488"/>
+        <c:axId val="2088544824"/>
+        <c:axId val="2088539096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125577592"/>
+        <c:axId val="2088531896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3686,7 +3727,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125579704"/>
+        <c:crossAx val="2088535352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3694,7 +3735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125579704"/>
+        <c:axId val="2088535352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3738,12 +3779,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125577592"/>
+        <c:crossAx val="2088531896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125582488"/>
+        <c:axId val="2088539096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3781,12 +3822,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125587464"/>
+        <c:crossAx val="2088544824"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2125587464"/>
+        <c:axId val="2088544824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3795,7 +3836,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125582488"/>
+        <c:crossAx val="2088539096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5942,8 +5983,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2130305976"/>
-        <c:axId val="-2142296712"/>
+        <c:axId val="2086761480"/>
+        <c:axId val="2086757720"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -8052,11 +8093,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122992344"/>
-        <c:axId val="-2130339688"/>
+        <c:axId val="2086751240"/>
+        <c:axId val="2086754152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2130305976"/>
+        <c:axId val="2086761480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8640.0"/>
@@ -8080,14 +8121,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142296712"/>
+        <c:crossAx val="2086757720"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="480.0"/>
         <c:minorUnit val="48.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2142296712"/>
+        <c:axId val="2086757720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000.0"/>
@@ -8119,12 +8160,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2130305976"/>
+        <c:crossAx val="2086761480"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2130339688"/>
+        <c:axId val="2086754152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000.0"/>
@@ -8157,13 +8198,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122992344"/>
+        <c:crossAx val="2086751240"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="400.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2122992344"/>
+        <c:axId val="2086751240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8173,7 +8214,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130339688"/>
+        <c:crossAx val="2086754152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8844,13 +8885,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EX33"/>
+  <dimension ref="A1:EY33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="U5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="U11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -8879,67 +8920,68 @@
     <col min="22" max="22" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.83203125" style="13" customWidth="1"/>
     <col min="24" max="24" width="20.83203125" customWidth="1"/>
-    <col min="25" max="25" width="28.1640625" customWidth="1"/>
-    <col min="26" max="26" width="22.1640625" customWidth="1"/>
-    <col min="27" max="27" width="28.1640625" customWidth="1"/>
-    <col min="28" max="28" width="21.5" customWidth="1"/>
+    <col min="25" max="25" width="20.83203125" style="13" customWidth="1"/>
+    <col min="26" max="26" width="28.1640625" customWidth="1"/>
+    <col min="27" max="27" width="22.1640625" customWidth="1"/>
+    <col min="28" max="28" width="28.1640625" customWidth="1"/>
+    <col min="29" max="29" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:154" s="4" customFormat="1" ht="26">
+    <row r="1" spans="1:155" s="4" customFormat="1" ht="26">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:154" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
+    <row r="3" spans="1:155" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
       <c r="J3" s="31"/>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
       <c r="P3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
       <c r="U3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="58" t="s">
+      <c r="V3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="1" t="s">
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3"/>
       <c r="AF3"/>
@@ -9065,8 +9107,9 @@
       <c r="EV3"/>
       <c r="EW3"/>
       <c r="EX3"/>
-    </row>
-    <row r="4" spans="1:154" s="13" customFormat="1" ht="42" customHeight="1" thickTop="1" thickBot="1">
+      <c r="EY3"/>
+    </row>
+    <row r="4" spans="1:155" s="13" customFormat="1" ht="42" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23" t="s">
@@ -9135,18 +9178,21 @@
       <c r="X4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23" t="s">
+      <c r="Y4" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="AA4" s="23" t="s">
+      <c r="AB4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="AB4" s="23" t="s">
+      <c r="AC4" s="23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:154" s="13" customFormat="1" ht="21" thickTop="1">
+    <row r="5" spans="1:155" s="13" customFormat="1" ht="21" thickTop="1">
       <c r="A5" s="29" t="s">
         <v>29</v>
       </c>
@@ -9207,23 +9253,24 @@
         <f>V5*720</f>
         <v>10368</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z5" s="32">
+      <c r="AA5" s="32">
         <f>X5/(D5*F5)</f>
         <v>74.141876430205954</v>
       </c>
-      <c r="AA5" s="14">
+      <c r="AB5" s="14">
         <f>D5*F5*1000/X5</f>
         <v>13.487654320987655</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AC5" s="32">
         <f>X5/(L5*N5)</f>
         <v>14580</v>
       </c>
     </row>
-    <row r="6" spans="1:154">
+    <row r="6" spans="1:155">
       <c r="A6" s="15" t="s">
         <v>88</v>
       </c>
@@ -9284,23 +9331,24 @@
         <f t="shared" ref="X6:X8" si="1">V6*720</f>
         <v>5184</v>
       </c>
-      <c r="Y6" s="16" t="s">
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z6" s="32">
-        <f t="shared" ref="Z6:Z16" si="2">X6/(D6*F6)</f>
+      <c r="AA6" s="32">
+        <f t="shared" ref="AA6:AA16" si="2">X6/(D6*F6)</f>
         <v>74.141876430205954</v>
       </c>
-      <c r="AA6" s="5">
-        <f t="shared" ref="AA6:AA9" si="3">D6*F6*1000/X6</f>
+      <c r="AB6" s="5">
+        <f t="shared" ref="AB6:AB9" si="3">D6*F6*1000/X6</f>
         <v>13.487654320987655</v>
       </c>
-      <c r="AB6" s="32">
-        <f t="shared" ref="AB6:AB33" si="4">X6/(L6*N6)</f>
+      <c r="AC6" s="32">
+        <f t="shared" ref="AC6:AC33" si="4">X6/(L6*N6)</f>
         <v>14580</v>
       </c>
     </row>
-    <row r="7" spans="1:154">
+    <row r="7" spans="1:155">
       <c r="B7" s="30" t="s">
         <v>50</v>
       </c>
@@ -9356,23 +9404,24 @@
         <f t="shared" si="1"/>
         <v>648</v>
       </c>
-      <c r="Y7" s="16" t="s">
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="Z7" s="32">
+      <c r="AA7" s="32">
         <f t="shared" si="2"/>
         <v>74.141876430205954</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AB7" s="5">
         <f t="shared" si="3"/>
         <v>13.487654320987655</v>
       </c>
-      <c r="AB7" s="32">
+      <c r="AC7" s="32">
         <f t="shared" si="4"/>
         <v>14580</v>
       </c>
     </row>
-    <row r="8" spans="1:154">
+    <row r="8" spans="1:155">
       <c r="A8" s="16" t="s">
         <v>120</v>
       </c>
@@ -9428,23 +9477,24 @@
         <f t="shared" si="1"/>
         <v>11404.8</v>
       </c>
-      <c r="Y8" s="16" t="s">
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="Z8" s="32">
+      <c r="AA8" s="32">
         <f t="shared" si="2"/>
         <v>81.556064073226537</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AB8" s="5">
         <f t="shared" si="3"/>
         <v>12.261503928170596</v>
       </c>
-      <c r="AB8" s="32">
+      <c r="AC8" s="32">
         <f t="shared" si="4"/>
         <v>14255.999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:154">
+    <row r="9" spans="1:155">
       <c r="A9" s="16"/>
       <c r="B9" s="30" t="s">
         <v>130</v>
@@ -9491,28 +9541,32 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="10" t="str">
-        <f>USDOLLAR(X9/720,2)&amp;"?"</f>
-        <v>$12.21?</v>
+        <f>USDOLLAR(X9/730,2)&amp;"?"</f>
+        <v>$12.05?</v>
       </c>
       <c r="W9" s="32"/>
-      <c r="X9" s="32">
+      <c r="X9" s="10">
         <v>8793.81</v>
       </c>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="32">
+      <c r="Y9" s="32">
+        <f>$X9*12</f>
+        <v>105525.72</v>
+      </c>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="32">
         <f t="shared" si="2"/>
         <v>62.884796910755142</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AB9" s="5">
         <f t="shared" si="3"/>
         <v>15.902094768934058</v>
       </c>
-      <c r="AB9" s="32">
+      <c r="AC9" s="32">
         <f t="shared" si="4"/>
         <v>10992.262499999999</v>
       </c>
     </row>
-    <row r="10" spans="1:154">
+    <row r="10" spans="1:155">
       <c r="A10" s="16"/>
       <c r="B10" s="30" t="s">
         <v>131</v>
@@ -9559,28 +9613,32 @@
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="10" t="str">
-        <f>USDOLLAR(X10/720,2)&amp;"?"</f>
-        <v>$10.23?</v>
+        <f>USDOLLAR(X10/730,2)&amp;"?"</f>
+        <v>$10.09?</v>
       </c>
       <c r="W10" s="32"/>
-      <c r="X10" s="32">
+      <c r="X10" s="10">
         <v>7365.75</v>
       </c>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="32">
-        <f t="shared" ref="Z10:Z11" si="5">X10/(D10*F10)</f>
+      <c r="Y10" s="32">
+        <f t="shared" ref="Y10:Y11" si="5">$X10*12</f>
+        <v>88389</v>
+      </c>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="32">
+        <f t="shared" ref="AA10:AA11" si="6">X10/(D10*F10)</f>
         <v>52.672697368421055</v>
       </c>
-      <c r="AA10" s="5">
-        <f t="shared" ref="AA10:AA11" si="6">D10*F10*1000/X10</f>
+      <c r="AB10" s="5">
+        <f t="shared" ref="AB10:AB11" si="7">D10*F10*1000/X10</f>
         <v>18.985167837626854</v>
       </c>
-      <c r="AB10" s="32">
-        <f t="shared" ref="AB10:AB11" si="7">X10/(L10*N10)</f>
+      <c r="AC10" s="32">
+        <f t="shared" ref="AC10:AC11" si="8">X10/(L10*N10)</f>
         <v>9207.1875</v>
       </c>
     </row>
-    <row r="11" spans="1:154">
+    <row r="11" spans="1:155">
       <c r="A11" s="16"/>
       <c r="B11" s="30" t="s">
         <v>132</v>
@@ -9627,28 +9685,33 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="10" t="str">
-        <f>USDOLLAR(X11/720,2)&amp;"?"</f>
-        <v>$7.13?</v>
+        <f>USDOLLAR(X11/730,2)&amp;"?"</f>
+        <v>$7.03?</v>
       </c>
       <c r="W11" s="32"/>
-      <c r="X11" s="32">
-        <v>5132.7777777777701</v>
-      </c>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="32">
-        <f t="shared" si="5"/>
-        <v>36.704646580218608</v>
-      </c>
-      <c r="AA11" s="5">
+      <c r="X11" s="10">
+        <f>Y11/12</f>
+        <v>5132.7777777777783</v>
+      </c>
+      <c r="Y11" s="32">
+        <f>184780/3</f>
+        <v>61593.333333333336</v>
+      </c>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="32">
         <f t="shared" si="6"/>
-        <v>27.24450698127507</v>
-      </c>
-      <c r="AB11" s="32">
+        <v>36.704646580218665</v>
+      </c>
+      <c r="AB11" s="5">
         <f t="shared" si="7"/>
-        <v>6415.9722222222126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:154">
+        <v>27.244506981275027</v>
+      </c>
+      <c r="AC11" s="32">
+        <f t="shared" si="8"/>
+        <v>6415.9722222222226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:155">
       <c r="B12" s="30"/>
       <c r="C12" s="38"/>
       <c r="D12" s="5"/>
@@ -9672,12 +9735,13 @@
       <c r="V12" s="26"/>
       <c r="W12" s="32"/>
       <c r="X12" s="32"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="22"/>
-    </row>
-    <row r="13" spans="1:154" ht="20">
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="22"/>
+    </row>
+    <row r="13" spans="1:155" ht="20">
       <c r="A13" s="29" t="s">
         <v>28</v>
       </c>
@@ -9747,23 +9811,24 @@
         <f>V13*720</f>
         <v>3816</v>
       </c>
-      <c r="Y13" s="16" t="s">
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="Z13" s="32">
+      <c r="AA13" s="32">
         <f>X13/(D13*F13)</f>
         <v>436.61327231121282</v>
       </c>
-      <c r="AA13" s="53">
+      <c r="AB13" s="53">
         <f>D13*F13*1000/X13</f>
         <v>2.2903563941299789</v>
       </c>
-      <c r="AB13" s="32">
+      <c r="AC13" s="32">
         <f>X13/(L13*N13)</f>
         <v>9540</v>
       </c>
     </row>
-    <row r="14" spans="1:154" s="13" customFormat="1" ht="20">
+    <row r="14" spans="1:155" s="13" customFormat="1" ht="20">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
         <v>133</v>
@@ -9828,23 +9893,24 @@
       <c r="X14" s="32">
         <v>2479</v>
       </c>
-      <c r="Y14" s="16" t="s">
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="Z14" s="32">
+      <c r="AA14" s="32">
         <f>X14/(D14*F14)</f>
         <v>283.63844393592677</v>
       </c>
-      <c r="AA14" s="53">
+      <c r="AB14" s="53">
         <f>D14*F14*1000/X14</f>
         <v>3.5256151674062122</v>
       </c>
-      <c r="AB14" s="32">
+      <c r="AC14" s="32">
         <f>X14/(L14*N14)</f>
         <v>6197.5</v>
       </c>
     </row>
-    <row r="15" spans="1:154">
+    <row r="15" spans="1:155">
       <c r="A15" s="16" t="s">
         <v>155</v>
       </c>
@@ -9903,30 +9969,31 @@
         <v>10</v>
       </c>
       <c r="V15" s="10" t="str">
-        <f t="shared" ref="V15:V16" si="8">USDOLLAR(X15/720,2)&amp;"?"</f>
-        <v>$2.12?</v>
+        <f>USDOLLAR(X15/730,2)&amp;"?"</f>
+        <v>$2.09?</v>
       </c>
       <c r="W15" s="32"/>
       <c r="X15" s="32">
         <v>1529</v>
       </c>
-      <c r="Y15" s="16" t="s">
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="Z15" s="32">
+      <c r="AA15" s="32">
         <f t="shared" si="2"/>
         <v>174.94279176201371</v>
       </c>
-      <c r="AA15" s="5">
+      <c r="AB15" s="5">
         <f>D15*F15*1000/X15</f>
         <v>5.7161543492478746</v>
       </c>
-      <c r="AB15" s="32">
+      <c r="AC15" s="32">
         <f t="shared" si="4"/>
         <v>2184.2857142857142</v>
       </c>
     </row>
-    <row r="16" spans="1:154">
+    <row r="16" spans="1:155">
       <c r="A16" s="16"/>
       <c r="B16" s="30" t="s">
         <v>101</v>
@@ -9983,30 +10050,31 @@
         <v>10</v>
       </c>
       <c r="V16" s="10" t="str">
-        <f t="shared" si="8"/>
-        <v>$2.61?</v>
+        <f>USDOLLAR(X16/730,2)&amp;"?"</f>
+        <v>$2.57?</v>
       </c>
       <c r="W16" s="32"/>
       <c r="X16" s="32">
         <v>1879</v>
       </c>
-      <c r="Y16" s="16" t="s">
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="Z16" s="32">
+      <c r="AA16" s="32">
         <f t="shared" si="2"/>
         <v>194.71502590673575</v>
       </c>
-      <c r="AA16" s="5">
+      <c r="AB16" s="5">
         <f>D16*F16*1000/X16</f>
         <v>5.1357104843001595</v>
       </c>
-      <c r="AB16" s="32">
+      <c r="AC16" s="32">
         <f t="shared" si="4"/>
         <v>2684.2857142857147</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:29">
       <c r="B17" s="30"/>
       <c r="C17" s="38"/>
       <c r="D17" s="5"/>
@@ -10030,12 +10098,13 @@
       <c r="V17" s="26"/>
       <c r="W17" s="32"/>
       <c r="X17" s="32"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="5"/>
-      <c r="AB17" s="32"/>
-    </row>
-    <row r="18" spans="1:28" ht="20">
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="32"/>
+    </row>
+    <row r="18" spans="1:29" ht="20">
       <c r="A18" s="29" t="s">
         <v>44</v>
       </c>
@@ -10093,23 +10162,24 @@
         <f>V18*720</f>
         <v>3600</v>
       </c>
-      <c r="Y18" s="16" t="s">
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="Z18" s="32">
-        <f t="shared" ref="Z18" si="9">X18/(D18*F18)</f>
+      <c r="AA18" s="32">
+        <f t="shared" ref="AA18" si="9">X18/(D18*F18)</f>
         <v>205.94965675057207</v>
       </c>
-      <c r="AA18" s="5">
+      <c r="AB18" s="5">
         <f>D18*F18*1000/X18</f>
         <v>4.8555555555555552</v>
       </c>
-      <c r="AB18" s="32">
+      <c r="AC18" s="32">
         <f t="shared" si="4"/>
         <v>4105.8394160583939</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:29">
       <c r="A19" s="16" t="s">
         <v>135</v>
       </c>
@@ -10160,12 +10230,13 @@
       <c r="V19" s="26"/>
       <c r="W19" s="32"/>
       <c r="X19" s="32"/>
-      <c r="Y19" s="16"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="32"/>
-    </row>
-    <row r="20" spans="1:28">
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="32"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="32"/>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" s="16" t="s">
         <v>68</v>
       </c>
@@ -10190,12 +10261,13 @@
       <c r="V20" s="26"/>
       <c r="W20" s="32"/>
       <c r="X20" s="32"/>
-      <c r="Y20" s="16"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="32"/>
-    </row>
-    <row r="21" spans="1:28">
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="32"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="32"/>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" s="16" t="s">
         <v>69</v>
       </c>
@@ -10220,12 +10292,13 @@
       <c r="V21" s="26"/>
       <c r="W21" s="32"/>
       <c r="X21" s="32"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="32"/>
-    </row>
-    <row r="22" spans="1:28">
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="32"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="32"/>
+    </row>
+    <row r="22" spans="1:29">
       <c r="B22" s="30"/>
       <c r="C22" s="38"/>
       <c r="E22" s="14"/>
@@ -10247,12 +10320,13 @@
       <c r="V22" s="26"/>
       <c r="W22" s="32"/>
       <c r="X22" s="32"/>
-      <c r="Y22" s="16"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="5"/>
-      <c r="AB22" s="32"/>
-    </row>
-    <row r="23" spans="1:28" ht="20">
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="32"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="32"/>
+    </row>
+    <row r="23" spans="1:29" ht="20">
       <c r="A23" s="29" t="s">
         <v>45</v>
       </c>
@@ -10313,8 +10387,8 @@
       </c>
       <c r="U23" s="5"/>
       <c r="V23" s="10" t="str">
-        <f t="shared" ref="V23:V30" si="10">USDOLLAR(X23/720,2)&amp;"?"</f>
-        <v>$10.42?</v>
+        <f>USDOLLAR(X23/730,2)&amp;"?"</f>
+        <v>$10.27?</v>
       </c>
       <c r="W23" s="32">
         <v>2649</v>
@@ -10322,21 +10396,22 @@
       <c r="X23" s="32">
         <v>7499</v>
       </c>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="32">
-        <f t="shared" ref="Z23:Z25" si="11">X23/(D23*F23)</f>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="32">
+        <f t="shared" ref="AA23:AA25" si="10">X23/(D23*F23)</f>
         <v>107.25114416475972</v>
       </c>
-      <c r="AA23" s="5">
-        <f t="shared" ref="AA23:AA25" si="12">D23*F23*1000/X23</f>
+      <c r="AB23" s="5">
+        <f t="shared" ref="AB23:AB25" si="11">D23*F23*1000/X23</f>
         <v>9.3239098546472867</v>
       </c>
-      <c r="AB23" s="32">
+      <c r="AC23" s="32">
         <f t="shared" si="4"/>
         <v>12498.333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:29">
       <c r="A24" s="16" t="s">
         <v>70</v>
       </c>
@@ -10397,8 +10472,8 @@
       </c>
       <c r="U24" s="5"/>
       <c r="V24" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$8.33?</v>
+        <f>USDOLLAR(X24/730,2)&amp;"?"</f>
+        <v>$8.22?</v>
       </c>
       <c r="W24" s="32">
         <v>1829</v>
@@ -10406,21 +10481,22 @@
       <c r="X24" s="32">
         <v>5999</v>
       </c>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="32">
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="32">
+        <f t="shared" si="10"/>
+        <v>109.56677381648159</v>
+      </c>
+      <c r="AB24" s="5">
         <f t="shared" si="11"/>
-        <v>109.56677381648159</v>
-      </c>
-      <c r="AA24" s="5">
-        <f t="shared" si="12"/>
         <v>9.126854475745958</v>
       </c>
-      <c r="AB24" s="32">
+      <c r="AC24" s="32">
         <f t="shared" si="4"/>
         <v>14997.5</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:29">
       <c r="B25" s="30" t="s">
         <v>111</v>
       </c>
@@ -10478,8 +10554,8 @@
       </c>
       <c r="U25" s="5"/>
       <c r="V25" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$5.28?</v>
+        <f>USDOLLAR(X25/730,2)&amp;"?"</f>
+        <v>$5.20?</v>
       </c>
       <c r="W25" s="32">
         <v>1329</v>
@@ -10487,21 +10563,22 @@
       <c r="X25" s="32">
         <v>3799</v>
       </c>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="32">
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="32">
+        <f t="shared" si="10"/>
+        <v>77.290852864583329</v>
+      </c>
+      <c r="AB25" s="5">
         <f t="shared" si="11"/>
-        <v>77.290852864583329</v>
-      </c>
-      <c r="AA25" s="5">
-        <f t="shared" si="12"/>
         <v>12.938141616214793</v>
       </c>
-      <c r="AB25" s="32">
+      <c r="AC25" s="32">
         <f t="shared" si="4"/>
         <v>9497.5</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:29">
       <c r="B26" s="30" t="s">
         <v>113</v>
       </c>
@@ -10559,8 +10636,8 @@
       </c>
       <c r="U26" s="5"/>
       <c r="V26" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$2.92?</v>
+        <f>USDOLLAR(X26/730,2)&amp;"?"</f>
+        <v>$2.88?</v>
       </c>
       <c r="W26" s="32">
         <v>749</v>
@@ -10568,21 +10645,22 @@
       <c r="X26" s="32">
         <v>2099</v>
       </c>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="32">
-        <f t="shared" ref="Z26:Z30" si="13">X26/(D26*F26)</f>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="32">
+        <f t="shared" ref="AA26:AA30" si="12">X26/(D26*F26)</f>
         <v>85.408528645833329</v>
       </c>
-      <c r="AA26" s="5">
-        <f t="shared" ref="AA26:AA30" si="14">D26*F26*1000/X26</f>
+      <c r="AB26" s="5">
+        <f t="shared" ref="AB26:AB30" si="13">D26*F26*1000/X26</f>
         <v>11.708432586946165</v>
       </c>
-      <c r="AB26" s="32">
-        <f t="shared" ref="AB26:AB30" si="15">X26/(L26*N26)</f>
+      <c r="AC26" s="32">
+        <f t="shared" ref="AC26:AC30" si="14">X26/(L26*N26)</f>
         <v>5766.4835164835167</v>
       </c>
     </row>
-    <row r="27" spans="1:28" s="13" customFormat="1">
+    <row r="27" spans="1:29" s="13" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="30" t="s">
         <v>139</v>
@@ -10641,8 +10719,8 @@
       </c>
       <c r="U27" s="5"/>
       <c r="V27" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$9.72?</v>
+        <f>USDOLLAR(X27/730,2)&amp;"?"</f>
+        <v>$9.59?</v>
       </c>
       <c r="W27" s="32">
         <v>2049</v>
@@ -10650,21 +10728,22 @@
       <c r="X27" s="32">
         <v>6999</v>
       </c>
-      <c r="Y27" s="16"/>
-      <c r="Z27" s="32">
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="32">
+        <f t="shared" si="12"/>
+        <v>74.406786868515056</v>
+      </c>
+      <c r="AB27" s="5">
         <f t="shared" si="13"/>
-        <v>74.406786868515056</v>
-      </c>
-      <c r="AA27" s="5">
+        <v>13.439634233461923</v>
+      </c>
+      <c r="AC27" s="32">
         <f t="shared" si="14"/>
-        <v>13.439634233461923</v>
-      </c>
-      <c r="AB27" s="32">
-        <f t="shared" si="15"/>
         <v>17497.5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" s="13" customFormat="1">
+    <row r="28" spans="1:29" s="13" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="30" t="s">
         <v>140</v>
@@ -10723,8 +10802,8 @@
       </c>
       <c r="U28" s="5"/>
       <c r="V28" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$11.94?</v>
+        <f>USDOLLAR(X28/730,2)&amp;"?"</f>
+        <v>$11.78?</v>
       </c>
       <c r="W28" s="32">
         <v>2599</v>
@@ -10732,21 +10811,22 @@
       <c r="X28" s="32">
         <v>8599</v>
       </c>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="32">
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="32">
+        <f t="shared" si="12"/>
+        <v>113.14473684210526</v>
+      </c>
+      <c r="AB28" s="5">
         <f t="shared" si="13"/>
-        <v>113.14473684210526</v>
-      </c>
-      <c r="AA28" s="5">
+        <v>8.838237004302826</v>
+      </c>
+      <c r="AC28" s="32">
         <f t="shared" si="14"/>
-        <v>8.838237004302826</v>
-      </c>
-      <c r="AB28" s="32">
-        <f t="shared" si="15"/>
         <v>21497.5</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:29">
       <c r="B29" s="30" t="s">
         <v>114</v>
       </c>
@@ -10802,8 +10882,8 @@
       <c r="T29" s="14"/>
       <c r="U29" s="5"/>
       <c r="V29" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$10.35?</v>
+        <f>USDOLLAR(X29/730,2)&amp;"?"</f>
+        <v>$10.20?</v>
       </c>
       <c r="W29" s="32">
         <v>2259</v>
@@ -10811,23 +10891,24 @@
       <c r="X29" s="32">
         <v>7449</v>
       </c>
-      <c r="Y29" s="16" t="s">
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="Z29" s="32">
+      <c r="AA29" s="32">
+        <f t="shared" si="12"/>
+        <v>196.02631578947367</v>
+      </c>
+      <c r="AB29" s="5">
         <f t="shared" si="13"/>
-        <v>196.02631578947367</v>
-      </c>
-      <c r="AA29" s="5">
+        <v>5.1013558866962008</v>
+      </c>
+      <c r="AC29" s="32">
         <f t="shared" si="14"/>
-        <v>5.1013558866962008</v>
-      </c>
-      <c r="AB29" s="32">
-        <f t="shared" si="15"/>
         <v>6796.5328467153277</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:29">
       <c r="B30" s="30" t="s">
         <v>115</v>
       </c>
@@ -10883,8 +10964,8 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v>$9.28?</v>
+        <f>USDOLLAR(X30/730,2)&amp;"?"</f>
+        <v>$9.15?</v>
       </c>
       <c r="W30" s="32">
         <v>1999</v>
@@ -10892,21 +10973,22 @@
       <c r="X30" s="32">
         <v>6679</v>
       </c>
-      <c r="Y30" s="16"/>
-      <c r="Z30" s="32">
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="32">
+        <f t="shared" si="12"/>
+        <v>175.76315789473685</v>
+      </c>
+      <c r="AB30" s="5">
         <f t="shared" si="13"/>
-        <v>175.76315789473685</v>
-      </c>
-      <c r="AA30" s="5">
+        <v>5.6894744722263813</v>
+      </c>
+      <c r="AC30" s="32">
         <f t="shared" si="14"/>
-        <v>5.6894744722263813</v>
-      </c>
-      <c r="AB30" s="32">
-        <f t="shared" si="15"/>
         <v>7617.4726277372265</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:29">
       <c r="B31" s="30"/>
       <c r="C31" s="38"/>
       <c r="E31" s="14"/>
@@ -10929,12 +11011,13 @@
       <c r="V31" s="26"/>
       <c r="W31" s="32"/>
       <c r="X31" s="32"/>
-      <c r="Y31" s="16"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="32"/>
-    </row>
-    <row r="32" spans="1:28" ht="20">
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="32"/>
+    </row>
+    <row r="32" spans="1:29" ht="20">
       <c r="A32" s="29" t="s">
         <v>52</v>
       </c>
@@ -10997,30 +11080,31 @@
         <v>0.1</v>
       </c>
       <c r="V32" s="10" t="str">
-        <f t="shared" ref="V32:V33" si="16">USDOLLAR(X32/720,2)&amp;"?"</f>
-        <v>$2.11?</v>
+        <f>USDOLLAR(X32/730,2)&amp;"?"</f>
+        <v>$2.08?</v>
       </c>
       <c r="W32" s="32"/>
       <c r="X32" s="32">
         <v>1519</v>
       </c>
-      <c r="Y32" s="16" t="s">
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="Z32" s="32">
-        <f t="shared" ref="Z32" si="17">X32/(D32*F32)</f>
+      <c r="AA32" s="32">
+        <f t="shared" ref="AA32" si="15">X32/(D32*F32)</f>
         <v>61.808268229166664</v>
       </c>
-      <c r="AA32" s="5">
-        <f t="shared" ref="AA32" si="18">D32*F32*1000/X32</f>
+      <c r="AB32" s="5">
+        <f t="shared" ref="AB32" si="16">D32*F32*1000/X32</f>
         <v>16.179065174456881</v>
       </c>
-      <c r="AB32" s="32">
+      <c r="AC32" s="32">
         <f t="shared" si="4"/>
         <v>5063.3333333333339</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:29">
       <c r="A33" s="16" t="s">
         <v>71</v>
       </c>
@@ -11083,25 +11167,26 @@
         <v>0.1</v>
       </c>
       <c r="V33" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>$2.33?</v>
+        <f>USDOLLAR(X33/730,2)&amp;"?"</f>
+        <v>$2.29?</v>
       </c>
       <c r="W33" s="32"/>
       <c r="X33" s="32">
         <v>1675</v>
       </c>
-      <c r="Y33" s="16" t="s">
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="Z33" s="32">
-        <f t="shared" ref="Z33" si="19">X33/(D33*F33)</f>
+      <c r="AA33" s="32">
+        <f t="shared" ref="AA33" si="17">X33/(D33*F33)</f>
         <v>244.73991817650494</v>
       </c>
-      <c r="AA33" s="5">
-        <f t="shared" ref="AA33" si="20">D33*F33*1000/X33</f>
+      <c r="AB33" s="5">
+        <f t="shared" ref="AB33" si="18">D33*F33*1000/X33</f>
         <v>4.0859701492537317</v>
       </c>
-      <c r="AB33" s="32">
+      <c r="AC33" s="32">
         <f t="shared" si="4"/>
         <v>5583.3333333333339</v>
       </c>
@@ -11114,7 +11199,7 @@
     <mergeCell ref="V3:X3"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <conditionalFormatting sqref="Z32">
+  <conditionalFormatting sqref="AA32">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -11126,7 +11211,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
+  <conditionalFormatting sqref="AB32">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -11138,7 +11223,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z33">
+  <conditionalFormatting sqref="AA33">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -11150,7 +11235,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33">
+  <conditionalFormatting sqref="AB33">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -11162,7 +11247,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z33">
+  <conditionalFormatting sqref="AA33">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -11174,7 +11259,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA33">
+  <conditionalFormatting sqref="AB33">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -11186,12 +11271,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:W13 A14:XFD27 A29:XFD33 A28:J28 P28:XFD28 Y13:XFD13 A5:XFD12">
-    <cfRule type="expression" dxfId="14" priority="13">
+  <conditionalFormatting sqref="A13:W13 A14:XFD27 A29:XFD33 A28:J28 P28:XFD28 Z13:XFD13 A5:XFD12">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z5:Z33">
+  <conditionalFormatting sqref="AA5:AA33">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -11203,7 +11288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5:AA33">
+  <conditionalFormatting sqref="AB5:AB33">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -11215,7 +11300,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z5:Z30">
+  <conditionalFormatting sqref="AA5:AA30">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -11227,7 +11312,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5:AA30">
+  <conditionalFormatting sqref="AB5:AB30">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -11239,7 +11324,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z5:Z32">
+  <conditionalFormatting sqref="AA5:AA32">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -11251,7 +11336,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5:AA32">
+  <conditionalFormatting sqref="AB5:AB32">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -11263,7 +11348,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB5:AB33">
+  <conditionalFormatting sqref="AC5:AC33">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -11275,7 +11360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z5:Z33">
+  <conditionalFormatting sqref="AA5:AA33">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -11287,7 +11372,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB5:AB33">
+  <conditionalFormatting sqref="AC5:AC33">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -11299,7 +11384,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5:AA33">
+  <conditionalFormatting sqref="AB5:AB33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -11313,9 +11398,6 @@
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="56" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="V10" formula="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11366,7 +11448,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" thickTop="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="30" t="str">
@@ -11374,91 +11456,91 @@
         <v>p2.16xlarge on-demand</v>
       </c>
       <c r="C3" s="18">
-        <f>+Sheet1!Z5</f>
+        <f>+Sheet1!AA5</f>
         <v>74.141876430205954</v>
       </c>
       <c r="D3" s="17">
-        <f>+Sheet1!AB5</f>
+        <f>+Sheet1!AC5</f>
         <v>14580</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="30" t="str">
         <f>+Sheet1!B6</f>
         <v>p2.8xlarge on-demand</v>
       </c>
       <c r="C4" s="18">
-        <f>+Sheet1!Z6</f>
+        <f>+Sheet1!AA6</f>
         <v>74.141876430205954</v>
       </c>
       <c r="D4" s="17">
-        <f>+Sheet1!AB6</f>
+        <f>+Sheet1!AC6</f>
         <v>14580</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="30" t="str">
         <f>+Sheet1!B7</f>
         <v>p2.xlarge on-demand</v>
       </c>
       <c r="C5" s="18">
-        <f>+Sheet1!Z7</f>
+        <f>+Sheet1!AA7</f>
         <v>74.141876430205954</v>
       </c>
       <c r="D5" s="17">
-        <f>+Sheet1!AB7</f>
+        <f>+Sheet1!AC7</f>
         <v>14580</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="30" t="str">
         <f>+Sheet1!B8</f>
         <v>p2 dedicated host On-demand</v>
       </c>
       <c r="C6" s="18">
-        <f>+Sheet1!Z8</f>
+        <f>+Sheet1!AA8</f>
         <v>81.556064073226537</v>
       </c>
       <c r="D6" s="17">
-        <f>+Sheet1!AB8</f>
+        <f>+Sheet1!AC8</f>
         <v>14255.999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1">
-      <c r="A7" s="59"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="30" t="str">
         <f>+Sheet1!B9</f>
         <v>p2 dedicated host 1y. no Up.</v>
       </c>
       <c r="C7" s="18">
-        <f>+Sheet1!Z9</f>
+        <f>+Sheet1!AA9</f>
         <v>62.884796910755142</v>
       </c>
       <c r="D7" s="17">
-        <f>+Sheet1!AB9</f>
+        <f>+Sheet1!AC9</f>
         <v>10992.262499999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1">
-      <c r="A8" s="59"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="30" t="str">
         <f>+Sheet1!B10</f>
         <v>p2 dedicated host 1y. Up.100%</v>
       </c>
       <c r="C8" s="18">
-        <f>+Sheet1!Z10</f>
+        <f>+Sheet1!AA10</f>
         <v>52.672697368421055</v>
       </c>
       <c r="D8" s="17">
-        <f>+Sheet1!AB10</f>
+        <f>+Sheet1!AC10</f>
         <v>9207.1875</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="30" t="str">
@@ -11466,41 +11548,41 @@
         <v>NVIDIA Tesla K80 hourly</v>
       </c>
       <c r="C9" s="18">
-        <f>+Sheet1!Z14</f>
+        <f>+Sheet1!AA14</f>
         <v>283.63844393592677</v>
       </c>
       <c r="D9" s="18">
-        <f>+Sheet1!AB14</f>
+        <f>+Sheet1!AC14</f>
         <v>6197.5</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="30" t="str">
         <f>+Sheet1!B15</f>
         <v>NVIDIA Tesla K80 2690v3</v>
       </c>
       <c r="C10" s="18">
-        <f>+Sheet1!Z15</f>
+        <f>+Sheet1!AA15</f>
         <v>174.94279176201371</v>
       </c>
       <c r="D10" s="18">
-        <f>+Sheet1!AB15</f>
+        <f>+Sheet1!AC15</f>
         <v>2184.2857142857142</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="30" t="str">
         <f>+Sheet1!B16</f>
         <v>NVIDIA Tesla M60 2690v3</v>
       </c>
       <c r="C11" s="18">
-        <f>+Sheet1!Z16</f>
+        <f>+Sheet1!AA16</f>
         <v>194.71502590673575</v>
       </c>
       <c r="D11" s="18">
-        <f>+Sheet1!AB16</f>
+        <f>+Sheet1!AC16</f>
         <v>2684.2857142857147</v>
       </c>
     </row>
@@ -11513,16 +11595,16 @@
         <v>NGD5</v>
       </c>
       <c r="C12" s="18">
-        <f>+Sheet1!Z18</f>
+        <f>+Sheet1!AA18</f>
         <v>205.94965675057207</v>
       </c>
       <c r="D12" s="18">
-        <f>+Sheet1!AB18</f>
+        <f>+Sheet1!AC18</f>
         <v>4105.8394160583939</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="60" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="30" t="str">
@@ -11530,121 +11612,121 @@
         <v>16-GPU x86 SERVER K80</v>
       </c>
       <c r="C13" s="18">
-        <f>+Sheet1!Z23</f>
+        <f>+Sheet1!AA23</f>
         <v>107.25114416475972</v>
       </c>
       <c r="D13" s="18">
-        <f>+Sheet1!AB23</f>
+        <f>+Sheet1!AC23</f>
         <v>12498.333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="59"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="30" t="str">
         <f>+Sheet1!B24</f>
         <v>8-GPU x86 SERVER M40</v>
       </c>
       <c r="C14" s="18">
-        <f>+Sheet1!Z24</f>
+        <f>+Sheet1!AA24</f>
         <v>109.56677381648159</v>
       </c>
       <c r="D14" s="18">
-        <f>+Sheet1!AB24</f>
+        <f>+Sheet1!AC24</f>
         <v>14997.5</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="59"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="30" t="str">
         <f>+Sheet1!B25</f>
         <v>8-GPU x86 SERVER</v>
       </c>
       <c r="C15" s="18">
-        <f>+Sheet1!Z25</f>
+        <f>+Sheet1!AA25</f>
         <v>77.290852864583329</v>
       </c>
       <c r="D15" s="18">
-        <f>+Sheet1!AB25</f>
+        <f>+Sheet1!AC25</f>
         <v>9497.5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="59"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="30" t="str">
         <f>+Sheet1!B26</f>
         <v>4-GPU x86 SERVER</v>
       </c>
       <c r="C16" s="18">
-        <f>+Sheet1!Z26</f>
+        <f>+Sheet1!AA26</f>
         <v>85.408528645833329</v>
       </c>
       <c r="D16" s="18">
-        <f>+Sheet1!AB26</f>
+        <f>+Sheet1!AC26</f>
         <v>5766.4835164835167</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="13" customFormat="1">
-      <c r="A17" s="59"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="30" t="str">
         <f>+Sheet1!B27</f>
         <v>8-GPU x86 SERVER P40</v>
       </c>
       <c r="C17" s="18">
-        <f>+Sheet1!Z27</f>
+        <f>+Sheet1!AA27</f>
         <v>74.406786868515056</v>
       </c>
       <c r="D17" s="18">
-        <f>+Sheet1!AB27</f>
+        <f>+Sheet1!AC27</f>
         <v>17497.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="13" customFormat="1">
-      <c r="A18" s="59"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="30" t="str">
         <f>+Sheet1!B28</f>
         <v>8-GPU x86 SERVER P100</v>
       </c>
       <c r="C18" s="18">
-        <f>+Sheet1!Z28</f>
+        <f>+Sheet1!AA28</f>
         <v>113.14473684210526</v>
       </c>
       <c r="D18" s="18">
-        <f>+Sheet1!AB28</f>
+        <f>+Sheet1!AC28</f>
         <v>21497.5</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="59"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="30" t="str">
         <f>+Sheet1!B29</f>
         <v>4-GPU POWER8/10 SERVER</v>
       </c>
       <c r="C19" s="18">
-        <f>+Sheet1!Z29</f>
+        <f>+Sheet1!AA29</f>
         <v>196.02631578947367</v>
       </c>
       <c r="D19" s="18">
-        <f>+Sheet1!AB29</f>
+        <f>+Sheet1!AC29</f>
         <v>6796.5328467153277</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="59"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="30" t="str">
         <f>+Sheet1!B30</f>
         <v>4-GPU POWER8/8 SERVER</v>
       </c>
       <c r="C20" s="18">
-        <f>+Sheet1!Z30</f>
+        <f>+Sheet1!AA30</f>
         <v>175.76315789473685</v>
       </c>
       <c r="D20" s="18">
-        <f>+Sheet1!AB30</f>
+        <f>+Sheet1!AC30</f>
         <v>7617.4726277372265</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="60" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="30" t="str">
@@ -11652,26 +11734,26 @@
         <v>Quad GPU model</v>
       </c>
       <c r="C21" s="18">
-        <f>+Sheet1!Z32</f>
+        <f>+Sheet1!AA32</f>
         <v>61.808268229166664</v>
       </c>
       <c r="D21" s="18">
-        <f>+Sheet1!AB32</f>
+        <f>+Sheet1!AC32</f>
         <v>5063.3333333333339</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="59"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="30" t="str">
         <f>+Sheet1!B33</f>
         <v>Tesla model</v>
       </c>
       <c r="C22" s="18">
-        <f>+Sheet1!Z33</f>
+        <f>+Sheet1!AA33</f>
         <v>244.73991817650494</v>
       </c>
       <c r="D22" s="18">
-        <f>+Sheet1!AB33</f>
+        <f>+Sheet1!AC33</f>
         <v>5583.3333333333339</v>
       </c>
     </row>
@@ -11905,8 +11987,11 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11956,7 +12041,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" thickTop="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="30" t="str">
@@ -11990,7 +12075,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1">
-      <c r="A3" s="59"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="30" t="str">
         <f>Sheet1!B6</f>
         <v>p2.8xlarge on-demand</v>
@@ -12022,7 +12107,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1">
-      <c r="A4" s="59"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="30" t="str">
         <f>Sheet1!B7</f>
         <v>p2.xlarge on-demand</v>
@@ -12054,7 +12139,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1">
-      <c r="A5" s="59"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="30" t="str">
         <f>Sheet1!B8</f>
         <v>p2 dedicated host On-demand</v>
@@ -12086,7 +12171,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="20" customHeight="1">
-      <c r="A6" s="59"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="30" t="str">
         <f>Sheet1!B9</f>
         <v>p2 dedicated host 1y. no Up.</v>
@@ -12096,12 +12181,9 @@
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
-      <c r="F6" s="27">
-        <f>Sheet1!X9</f>
-        <v>8793.81</v>
-      </c>
+      <c r="F6" s="27"/>
       <c r="G6" s="27">
-        <f>F6*12</f>
+        <f>Sheet1!$Y9</f>
         <v>105525.72</v>
       </c>
       <c r="H6" s="14">
@@ -12118,7 +12200,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1">
-      <c r="A7" s="59"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="30" t="str">
         <f>Sheet1!B10</f>
         <v>p2 dedicated host 1y. Up.100%</v>
@@ -12130,6 +12212,7 @@
       <c r="E7" s="27"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27">
+        <f>Sheet1!$Y10</f>
         <v>88389</v>
       </c>
       <c r="H7" s="14">
@@ -12146,7 +12229,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1">
-      <c r="A8" s="59" t="str">
+      <c r="A8" s="60" t="str">
         <f>Sheet1!$A$13</f>
         <v>Softlayer</v>
       </c>
@@ -12178,7 +12261,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="59"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="30" t="str">
         <f>Sheet1!B14</f>
         <v>NVIDIA Tesla K80 monthly</v>
@@ -12207,7 +12290,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="20" customHeight="1">
-      <c r="A10" s="59"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="30" t="str">
         <f>Sheet1!B15</f>
         <v>NVIDIA Tesla K80 2690v3</v>
@@ -12236,7 +12319,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1">
-      <c r="A11" s="59"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="30" t="str">
         <f>Sheet1!B16</f>
         <v>NVIDIA Tesla M60 2690v3</v>
@@ -12300,7 +12383,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1">
-      <c r="A13" s="59" t="str">
+      <c r="A13" s="60" t="str">
         <f>Sheet1!A23</f>
         <v>Cirrascale</v>
       </c>
@@ -12332,7 +12415,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A14" s="59"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="30" t="str">
         <f>Sheet1!B23&amp;" weekly"</f>
         <v>16-GPU x86 SERVER K80 weekly</v>
@@ -12361,7 +12444,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="59"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="30" t="str">
         <f>Sheet1!B24&amp;" monthly"</f>
         <v>8-GPU x86 SERVER M40 monthly</v>
@@ -12390,7 +12473,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1">
-      <c r="A16" s="59"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="30" t="str">
         <f>Sheet1!B24&amp;" weekly"</f>
         <v>8-GPU x86 SERVER M40 weekly</v>
@@ -12419,7 +12502,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A17" s="59"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="30" t="str">
         <f>Sheet1!B25&amp;" monthly"</f>
         <v>8-GPU x86 SERVER monthly</v>
@@ -12448,7 +12531,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="20" customHeight="1">
-      <c r="A18" s="59"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="30" t="str">
         <f>Sheet1!B25&amp;" weekly"</f>
         <v>8-GPU x86 SERVER weekly</v>
@@ -12477,7 +12560,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="59"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="30" t="str">
         <f>Sheet1!B26&amp;" monthly"</f>
         <v>4-GPU x86 SERVER monthly</v>
@@ -12506,7 +12589,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="20" customHeight="1">
-      <c r="A20" s="59"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="30" t="str">
         <f>Sheet1!B26&amp;" weekly"</f>
         <v>4-GPU x86 SERVER weekly</v>
@@ -12535,7 +12618,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A21" s="59"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="30" t="str">
         <f>Sheet1!B27&amp;" monthly"</f>
         <v>8-GPU x86 SERVER P40 monthly</v>
@@ -12564,7 +12647,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="59"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="30" t="str">
         <f>Sheet1!B27&amp;" weekly"</f>
         <v>8-GPU x86 SERVER P40 weekly</v>
@@ -12593,7 +12676,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="59"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="30" t="str">
         <f>Sheet1!B28&amp;" monthly"</f>
         <v>8-GPU x86 SERVER P100 monthly</v>
@@ -12622,7 +12705,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="59"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="30" t="str">
         <f>Sheet1!B28&amp;" weekly"</f>
         <v>8-GPU x86 SERVER P100 weekly</v>
@@ -12651,7 +12734,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="59"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="30" t="str">
         <f>Sheet1!B29&amp;" monthly"</f>
         <v>4-GPU POWER8/10 SERVER monthly</v>
@@ -12680,7 +12763,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="20" customHeight="1">
-      <c r="A26" s="59"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="30" t="str">
         <f>Sheet1!B29&amp;" weekly"</f>
         <v>4-GPU POWER8/10 SERVER weekly</v>
@@ -12709,7 +12792,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A27" s="59"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="30" t="str">
         <f>Sheet1!B30&amp;" monthly"</f>
         <v>4-GPU POWER8/8 SERVER monthly</v>
@@ -12738,7 +12821,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="20" customHeight="1">
-      <c r="A28" s="59"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="30" t="str">
         <f>Sheet1!B30&amp;" weekly"</f>
         <v>4-GPU POWER8/8 SERVER weekly</v>
@@ -12767,7 +12850,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="20" customHeight="1">
-      <c r="A29" s="59" t="str">
+      <c r="A29" s="60" t="str">
         <f>Sheet1!A32</f>
         <v>Sakura</v>
       </c>
@@ -12799,7 +12882,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="20" customHeight="1">
-      <c r="A30" s="59"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="30" t="str">
         <f>Sheet1!$B$33</f>
         <v>Tesla model</v>
@@ -12835,73 +12918,73 @@
     <mergeCell ref="A29:A30"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <conditionalFormatting sqref="B18:E18 G18:I18 B22:E22 G22:I22 B21:I21 B24 G24:I24 B26:E26 G26:I26 B29:I30 B28 G28:I28 F22:F28 B2:I17 B20 D20:I20 D24:E24 D28:E28">
-    <cfRule type="expression" dxfId="13" priority="14">
+  <conditionalFormatting sqref="B18:E18 G18:I18 B22:E22 G22:I22 B21:I21 B24 G24:I24 B26:E26 G26:I26 B29:I30 B28 G28:I28 F22:F28 B20 D20:I20 D24:E24 D28:E28 B2:I17">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:I19">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:E23 G23:I23">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:E25 G25:I25">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:E27 G27:I27">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J18 J20:J22 J24 J26 J28:J30">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12925,7 +13008,7 @@
   </sheetPr>
   <dimension ref="A1:CM338"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -13040,180 +13123,180 @@
       <c r="D1" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="64" t="str">
+      <c r="E1" s="65" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$B$2</f>
         <v>Amazon p2.16xlarge on-demand</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="62" t="str">
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="63" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$B$3</f>
         <v>Amazon p2.8xlarge on-demand</v>
       </c>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="61" t="str">
+      <c r="I1" s="63"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="62" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$B$4</f>
         <v>Amazon p2.xlarge on-demand</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="61" t="str">
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="62" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$B$5</f>
         <v>Amazon p2 dedicated host On-demand</v>
       </c>
-      <c r="O1" s="62"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="61" t="str">
+      <c r="O1" s="63"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="62" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$B$6</f>
         <v>Amazon p2 dedicated host 1y. no Up.</v>
       </c>
-      <c r="R1" s="62"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="61" t="str">
+      <c r="R1" s="63"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="62" t="str">
         <f>'cost-performance'!A2&amp;" "&amp;'cost-performance'!B7</f>
         <v>Amazon p2 dedicated host 1y. Up.100%</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="61" t="str">
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="62" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$B$8</f>
         <v>Softlayer NVIDIA Tesla K80 hourly</v>
       </c>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="61" t="str">
+      <c r="X1" s="63"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="62" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$B$9</f>
         <v>Softlayer NVIDIA Tesla K80 monthly</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="61" t="str">
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="62" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$B$10</f>
         <v>Softlayer NVIDIA Tesla K80 2690v3</v>
       </c>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="61" t="str">
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="62" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$B$11</f>
         <v>Softlayer NVIDIA Tesla M60 2690v3</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="61" t="str">
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="62" t="str">
         <f>'cost-performance'!$A$12&amp;" "&amp;'cost-performance'!$B$12</f>
         <v>Nimbix NGD5</v>
       </c>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="61" t="str">
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$13</f>
         <v>Cirrascale 16-GPU x86 SERVER K80 monthly</v>
       </c>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="61" t="str">
+      <c r="AM1" s="63"/>
+      <c r="AN1" s="64"/>
+      <c r="AO1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$14</f>
         <v>Cirrascale 16-GPU x86 SERVER K80 weekly</v>
       </c>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="61" t="str">
+      <c r="AP1" s="63"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$15</f>
         <v>Cirrascale 8-GPU x86 SERVER M40 monthly</v>
       </c>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="61" t="str">
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$16</f>
         <v>Cirrascale 8-GPU x86 SERVER M40 weekly</v>
       </c>
-      <c r="AV1" s="62"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="61" t="str">
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$17</f>
         <v>Cirrascale 8-GPU x86 SERVER monthly</v>
       </c>
-      <c r="AY1" s="62"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="61" t="str">
+      <c r="AY1" s="63"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$18</f>
         <v>Cirrascale 8-GPU x86 SERVER weekly</v>
       </c>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="61" t="str">
+      <c r="BB1" s="63"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$19</f>
         <v>Cirrascale 4-GPU x86 SERVER monthly</v>
       </c>
-      <c r="BE1" s="62"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="61" t="str">
+      <c r="BE1" s="63"/>
+      <c r="BF1" s="64"/>
+      <c r="BG1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$20</f>
         <v>Cirrascale 4-GPU x86 SERVER weekly</v>
       </c>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="63"/>
-      <c r="BJ1" s="61" t="str">
+      <c r="BH1" s="63"/>
+      <c r="BI1" s="64"/>
+      <c r="BJ1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$21</f>
         <v>Cirrascale 8-GPU x86 SERVER P40 monthly</v>
       </c>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="61" t="str">
+      <c r="BK1" s="63"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$22</f>
         <v>Cirrascale 8-GPU x86 SERVER P40 weekly</v>
       </c>
-      <c r="BN1" s="62"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="61" t="str">
+      <c r="BN1" s="63"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$23</f>
         <v>Cirrascale 8-GPU x86 SERVER P100 monthly</v>
       </c>
-      <c r="BQ1" s="62"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="61" t="str">
+      <c r="BQ1" s="63"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$24</f>
         <v>Cirrascale 8-GPU x86 SERVER P100 weekly</v>
       </c>
-      <c r="BT1" s="62"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="61" t="str">
+      <c r="BT1" s="63"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$25</f>
         <v>Cirrascale 4-GPU POWER8/10 SERVER monthly</v>
       </c>
-      <c r="BW1" s="62"/>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="61" t="str">
+      <c r="BW1" s="63"/>
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$26</f>
         <v>Cirrascale 4-GPU POWER8/10 SERVER weekly</v>
       </c>
-      <c r="BZ1" s="62"/>
-      <c r="CA1" s="63"/>
-      <c r="CB1" s="61" t="str">
+      <c r="BZ1" s="63"/>
+      <c r="CA1" s="64"/>
+      <c r="CB1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$27</f>
         <v>Cirrascale 4-GPU POWER8/8 SERVER monthly</v>
       </c>
-      <c r="CC1" s="62"/>
-      <c r="CD1" s="63"/>
-      <c r="CE1" s="61" t="str">
+      <c r="CC1" s="63"/>
+      <c r="CD1" s="64"/>
+      <c r="CE1" s="62" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$B$28</f>
         <v>Cirrascale 4-GPU POWER8/8 SERVER weekly</v>
       </c>
-      <c r="CF1" s="62"/>
-      <c r="CG1" s="63"/>
-      <c r="CH1" s="61" t="str">
+      <c r="CF1" s="63"/>
+      <c r="CG1" s="64"/>
+      <c r="CH1" s="62" t="str">
         <f>'cost-performance'!$A$29&amp;" "&amp;'cost-performance'!$B$29</f>
         <v>Sakura Quad GPU model</v>
       </c>
-      <c r="CI1" s="62"/>
-      <c r="CJ1" s="63"/>
-      <c r="CK1" s="61" t="str">
+      <c r="CI1" s="63"/>
+      <c r="CJ1" s="64"/>
+      <c r="CK1" s="62" t="str">
         <f>'cost-performance'!$A$29&amp;" "&amp;'cost-performance'!$B$30</f>
         <v>Sakura Tesla model</v>
       </c>
-      <c r="CL1" s="62"/>
-      <c r="CM1" s="63"/>
+      <c r="CL1" s="63"/>
+      <c r="CM1" s="64"/>
     </row>
     <row r="2" spans="1:91" ht="20" thickTop="1" thickBot="1">
       <c r="A2" s="23"/>
@@ -36089,6 +36172,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CB1:CD1"/>
+    <mergeCell ref="CE1:CG1"/>
+    <mergeCell ref="CH1:CJ1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="BM1:BO1"/>
+    <mergeCell ref="BP1:BR1"/>
+    <mergeCell ref="BS1:BU1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="BY1:CA1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AR1:AT1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -36098,26 +36201,6 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AU1:AW1"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="BD1:BF1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="BJ1:BL1"/>
-    <mergeCell ref="CB1:CD1"/>
-    <mergeCell ref="CE1:CG1"/>
-    <mergeCell ref="CH1:CJ1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="BM1:BO1"/>
-    <mergeCell ref="BP1:BR1"/>
-    <mergeCell ref="BS1:BU1"/>
-    <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="BY1:CA1"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added all data for table to cost-performance sheet, exported to cost-performance.csv. Added all data to JS table in plotTable().
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21160" yWindow="0" windowWidth="25980" windowHeight="26060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28180" windowHeight="28260" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="211">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="3"/>
@@ -996,10 +996,6 @@
   </si>
   <si>
     <t>Xeon E5-2686 v4</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>See comments to performance cells.</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1438,6 +1434,54 @@
     <t>GPU model</t>
     <phoneticPr fontId="3"/>
   </si>
+  <si>
+    <t>CPU model</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CPUs</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Memory (GB)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HDD prim.Type</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HDD prim.GB</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HDD sec.Type</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>HDD sec.GB</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Network</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
@@ -1645,7 +1689,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1691,8 +1735,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1843,8 +1893,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF797B7E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="576">
+  <cellStyleXfs count="588">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2429,8 +2488,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -2550,6 +2621,20 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="120" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="575"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="119" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2558,6 +2643,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="62" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="120" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="177" fontId="17" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2571,15 +2659,8 @@
     <xf numFmtId="177" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="120" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="120" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="575"/>
   </cellXfs>
-  <cellStyles count="576">
+  <cellStyles count="588">
     <cellStyle name="Calculation" xfId="344" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="346" builtinId="23" hidden="1"/>
     <cellStyle name="comment" xfId="120"/>
@@ -2862,6 +2943,18 @@
     <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="264" builtinId="17" customBuiltin="1"/>
@@ -3157,7 +3250,73 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="341" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3715,8 +3874,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="70"/>
-        <c:axId val="2129529416"/>
-        <c:axId val="2129041800"/>
+        <c:axId val="-2077585032"/>
+        <c:axId val="-2077318712"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -3920,11 +4079,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="300"/>
-        <c:axId val="2129229336"/>
-        <c:axId val="2120270072"/>
+        <c:axId val="-2077881528"/>
+        <c:axId val="-2077427384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129529416"/>
+        <c:axId val="-2077585032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3945,7 +4104,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129041800"/>
+        <c:crossAx val="-2077318712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3953,7 +4112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129041800"/>
+        <c:axId val="-2077318712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3997,12 +4156,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129529416"/>
+        <c:crossAx val="-2077585032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2120270072"/>
+        <c:axId val="-2077427384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4040,12 +4199,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129229336"/>
+        <c:crossAx val="-2077881528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2129229336"/>
+        <c:axId val="-2077881528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4054,7 +4213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120270072"/>
+        <c:crossAx val="-2077427384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6201,8 +6360,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128981080"/>
-        <c:axId val="2128984536"/>
+        <c:axId val="-2077355560"/>
+        <c:axId val="-2077352104"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -7962,7 +8121,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Softlayer NVIDIA Tesla K80 hourly GPU ($/Tflops)</c:v>
+                  <c:v>Softlayer NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4 hourly GPU ($/Tflops)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8311,11 +8470,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128991144"/>
-        <c:axId val="2128987960"/>
+        <c:axId val="-2077345496"/>
+        <c:axId val="-2077348680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128981080"/>
+        <c:axId val="-2077355560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8640.0"/>
@@ -8339,14 +8498,14 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128984536"/>
+        <c:crossAx val="-2077352104"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="480.0"/>
         <c:minorUnit val="48.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128984536"/>
+        <c:axId val="-2077352104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000.0"/>
@@ -8378,12 +8537,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2128981080"/>
+        <c:crossAx val="-2077355560"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128987960"/>
+        <c:axId val="-2077348680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20000.0"/>
@@ -8416,13 +8575,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128991144"/>
+        <c:crossAx val="-2077345496"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="400.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128991144"/>
+        <c:axId val="-2077345496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8432,7 +8591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128987960"/>
+        <c:crossAx val="-2077348680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9100,32 +9259,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:EY33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="T5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23" style="2" customWidth="1"/>
     <col min="2" max="2" width="38.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="13" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5" customWidth="1"/>
@@ -9153,40 +9312,40 @@
     <row r="3" spans="1:155" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
       <c r="J3" s="31"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
       <c r="P3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
       <c r="U3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="59" t="s">
+      <c r="V3" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
       <c r="Y3" s="58"/>
       <c r="Z3" s="1" t="s">
         <v>34</v>
@@ -9352,7 +9511,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>4</v>
@@ -9391,13 +9550,13 @@
         <v>15</v>
       </c>
       <c r="W4" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="X4" s="23" t="s">
         <v>24</v>
       </c>
       <c r="Y4" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Z4" s="23"/>
       <c r="AA4" s="23" t="s">
@@ -9460,9 +9619,7 @@
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
-      <c r="U5" s="14">
-        <v>20</v>
-      </c>
+      <c r="U5" s="14"/>
       <c r="V5" s="32">
         <v>14.4</v>
       </c>
@@ -9473,7 +9630,7 @@
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="16" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="AA5" s="32">
         <f>X5/(D5*F5)</f>
@@ -9490,7 +9647,7 @@
     </row>
     <row r="6" spans="1:155">
       <c r="A6" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>49</v>
@@ -9520,7 +9677,7 @@
       <c r="K6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="14">
         <v>32</v>
       </c>
       <c r="M6" s="5">
@@ -9538,9 +9695,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="5">
-        <v>10</v>
-      </c>
+      <c r="U6" s="5"/>
       <c r="V6" s="32">
         <v>7.2</v>
       </c>
@@ -9551,7 +9706,7 @@
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="16" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
       <c r="AA6" s="32">
         <f t="shared" ref="AA6:AA16" si="2">X6/(D6*F6)</f>
@@ -9595,7 +9750,7 @@
       <c r="K7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="14">
         <v>4</v>
       </c>
       <c r="M7" s="5">
@@ -9624,7 +9779,7 @@
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="16" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="AA7" s="32">
         <f t="shared" si="2"/>
@@ -9641,10 +9796,10 @@
     </row>
     <row r="8" spans="1:155">
       <c r="A8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="C8" s="38" t="s">
         <v>25</v>
@@ -9671,7 +9826,7 @@
       <c r="K8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="14">
         <v>2</v>
       </c>
       <c r="M8" s="5">
@@ -9697,7 +9852,7 @@
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA8" s="32">
         <f t="shared" si="2"/>
@@ -9715,7 +9870,7 @@
     <row r="9" spans="1:155">
       <c r="A9" s="16"/>
       <c r="B9" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>17</v>
@@ -9787,7 +9942,7 @@
     <row r="10" spans="1:155">
       <c r="A10" s="16"/>
       <c r="B10" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="38" t="s">
         <v>17</v>
@@ -9796,7 +9951,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -9805,14 +9960,14 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L10" s="5">
         <v>2</v>
@@ -9859,7 +10014,7 @@
     <row r="11" spans="1:155">
       <c r="A11" s="16"/>
       <c r="B11" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>17</v>
@@ -9868,7 +10023,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -9877,14 +10032,14 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="5">
         <v>2</v>
@@ -9964,7 +10119,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>30</v>
@@ -10049,7 +10204,7 @@
     <row r="14" spans="1:155" s="13" customFormat="1" ht="20">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>17</v>
@@ -10113,7 +10268,7 @@
       </c>
       <c r="Y14" s="32"/>
       <c r="Z14" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA14" s="32">
         <f>X14/(D14*F14)</f>
@@ -10130,10 +10285,10 @@
     </row>
     <row r="15" spans="1:155">
       <c r="A15" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>57</v>
@@ -10214,16 +10369,16 @@
     <row r="16" spans="1:155">
       <c r="A16" s="16"/>
       <c r="B16" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="5">
         <v>1</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="9">
         <v>9.65</v>
@@ -10232,14 +10387,14 @@
         <v>0.3</v>
       </c>
       <c r="H16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L16" s="5">
         <v>2</v>
@@ -10257,7 +10412,7 @@
         <v>64</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R16" s="5">
         <v>1000</v>
@@ -10399,7 +10554,7 @@
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>80</v>
@@ -10549,7 +10704,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>17</v>
@@ -10634,7 +10789,7 @@
         <v>70</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="38" t="s">
         <v>43</v>
@@ -10716,7 +10871,7 @@
     </row>
     <row r="25" spans="1:29">
       <c r="B25" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>67</v>
@@ -10798,7 +10953,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="B26" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="38" t="s">
         <v>54</v>
@@ -10823,7 +10978,7 @@
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L26" s="5">
         <v>2</v>
@@ -10841,13 +10996,13 @@
         <v>128</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R26" s="14">
         <v>256</v>
       </c>
       <c r="S26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T26" s="14">
         <v>4000</v>
@@ -10881,10 +11036,10 @@
     <row r="27" spans="1:29" s="13" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" s="13">
         <v>8</v>
@@ -10924,13 +11079,13 @@
         <v>256</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R27" s="14">
         <v>1000</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T27" s="14">
         <v>4000</v>
@@ -10964,10 +11119,10 @@
     <row r="28" spans="1:29" s="13" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="13">
         <v>8</v>
@@ -10989,7 +11144,7 @@
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L28" s="36">
         <v>2</v>
@@ -11007,13 +11162,13 @@
         <v>256</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R28" s="14">
         <v>1000</v>
       </c>
       <c r="S28" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T28" s="14">
         <v>4000</v>
@@ -11046,10 +11201,10 @@
     </row>
     <row r="29" spans="1:29">
       <c r="B29" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -11091,10 +11246,10 @@
         <v>1000</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R29" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
@@ -11111,7 +11266,7 @@
       </c>
       <c r="Y29" s="32"/>
       <c r="Z29" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA29" s="32">
         <f t="shared" si="13"/>
@@ -11128,10 +11283,10 @@
     </row>
     <row r="30" spans="1:29">
       <c r="B30" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -11173,10 +11328,10 @@
         <v>512</v>
       </c>
       <c r="Q30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R30" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
@@ -11490,7 +11645,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:W13 A14:XFD27 A29:XFD33 A28:J28 P28:XFD28 Z13:XFD13 A5:XFD12">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11627,6 +11782,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11666,7 +11822,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" thickTop="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="66" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="30" t="str">
@@ -11683,7 +11839,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" customHeight="1">
-      <c r="A4" s="60"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="30" t="str">
         <f>+Sheet1!B6</f>
         <v>p2.8xlarge on-demand</v>
@@ -11698,7 +11854,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" customHeight="1">
-      <c r="A5" s="60"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="30" t="str">
         <f>+Sheet1!B7</f>
         <v>p2.xlarge on-demand</v>
@@ -11713,7 +11869,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" customHeight="1">
-      <c r="A6" s="60"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="30" t="str">
         <f>+Sheet1!B8</f>
         <v>p2 dedicated host On-demand</v>
@@ -11728,7 +11884,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" customHeight="1">
-      <c r="A7" s="60"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="30" t="str">
         <f>+Sheet1!B9</f>
         <v>p2 dedicated host 1 year no Upfront</v>
@@ -11743,7 +11899,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="20" customHeight="1">
-      <c r="A8" s="60"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="30" t="str">
         <f>+Sheet1!B10</f>
         <v>p2 dedicated host 1 year 100% Upfront</v>
@@ -11758,7 +11914,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="66" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="30" t="str">
@@ -11775,7 +11931,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="60"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="30" t="str">
         <f>+Sheet1!B15</f>
         <v>NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</v>
@@ -11790,7 +11946,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="60"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="30" t="str">
         <f>+Sheet1!B16</f>
         <v>NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</v>
@@ -11822,7 +11978,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="66" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="30" t="str">
@@ -11839,7 +11995,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="60"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="30" t="str">
         <f>+Sheet1!B24</f>
         <v>8-GPU x86 SERVER M40</v>
@@ -11854,7 +12010,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="60"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="30" t="str">
         <f>+Sheet1!B25</f>
         <v>8-GPU x86 SERVER</v>
@@ -11869,7 +12025,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="60"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="30" t="str">
         <f>+Sheet1!B26</f>
         <v>4-GPU x86 SERVER</v>
@@ -11884,7 +12040,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" s="13" customFormat="1">
-      <c r="A17" s="60"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="30" t="str">
         <f>+Sheet1!B27</f>
         <v>8-GPU x86 SERVER P40</v>
@@ -11899,7 +12055,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" s="13" customFormat="1">
-      <c r="A18" s="60"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="30" t="str">
         <f>+Sheet1!B28</f>
         <v>8-GPU x86 SERVER P100</v>
@@ -11914,7 +12070,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="60"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="30" t="str">
         <f>+Sheet1!B29</f>
         <v>4-GPU POWER8/10 SERVER</v>
@@ -11929,7 +12085,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="60"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="30" t="str">
         <f>+Sheet1!B30</f>
         <v>4-GPU POWER8/8 SERVER</v>
@@ -11944,7 +12100,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="66" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="30" t="str">
@@ -11961,7 +12117,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="60"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="30" t="str">
         <f>+Sheet1!B33</f>
         <v>Tesla model</v>
@@ -12200,92 +12356,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:M30"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="13" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="13" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="13" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="9" width="14" style="13" customWidth="1"/>
-    <col min="10" max="10" width="27.1640625" customWidth="1"/>
-    <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="13" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+    <col min="22" max="22" width="142.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="12" customFormat="1" ht="21" thickBot="1">
+    <row r="1" spans="1:24" s="12" customFormat="1" ht="21" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="O1" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="R1" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="S1" s="62" t="s">
+        <v>204</v>
+      </c>
+      <c r="T1" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="U1" s="62" t="s">
+        <v>206</v>
+      </c>
+      <c r="V1" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="X1" s="1"/>
+    </row>
+    <row r="2" spans="1:24" ht="21" customHeight="1" thickTop="1">
+      <c r="A2" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>179</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" thickTop="1">
-      <c r="A2" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="66" t="s">
-        <v>180</v>
       </c>
       <c r="C2" s="30" t="str">
         <f>Sheet1!B5</f>
         <v>p2.16xlarge on-demand</v>
       </c>
-      <c r="D2" s="68" t="s">
-        <v>186</v>
+      <c r="D2" s="60" t="s">
+        <v>185</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="27">
         <f>Sheet1!V5</f>
@@ -12305,27 +12494,66 @@
         <f>Sheet1!F5*Sheet1!D5</f>
         <v>139.84</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="14" t="str">
+        <f>Sheet1!$C5</f>
+        <v>K80</v>
+      </c>
+      <c r="M2" s="14">
         <f>Sheet1!$D5</f>
         <v>16</v>
       </c>
-      <c r="M2" s="14" t="str">
-        <f>Sheet1!$C5</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="20" customHeight="1">
-      <c r="A3" s="60"/>
-      <c r="B3" s="66"/>
+      <c r="N2" s="61" t="str">
+        <f>Sheet1!$K5</f>
+        <v>Xeon E5-2686 v4</v>
+      </c>
+      <c r="O2" s="61">
+        <f>Sheet1!$L5</f>
+        <v>64</v>
+      </c>
+      <c r="P2" s="61">
+        <f>Sheet1!$P5</f>
+        <v>732</v>
+      </c>
+      <c r="Q2" s="27" t="str">
+        <f>IF(Sheet1!$Q5="","",Sheet1!$Q5)</f>
+        <v/>
+      </c>
+      <c r="R2" s="27" t="str">
+        <f>IF(Sheet1!$Q5="","",Sheet1!$Q5)</f>
+        <v/>
+      </c>
+      <c r="S2" s="63" t="str">
+        <f>IF(Sheet1!$S5="","",Sheet1!$S5)</f>
+        <v/>
+      </c>
+      <c r="T2" s="63" t="str">
+        <f>IF(Sheet1!$T5="","",Sheet1!$T5)</f>
+        <v/>
+      </c>
+      <c r="U2" s="63" t="str">
+        <f>IF(Sheet1!$U5="","",Sheet1!$U5)</f>
+        <v/>
+      </c>
+      <c r="V2" s="63" t="str">
+        <f>IF(Sheet1!$Z5="","",Sheet1!$Z5) &amp; " CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36."</f>
+        <v>Free Outbound Traffic = 1 GB/month.  CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36.</v>
+      </c>
+      <c r="X2" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="20" customHeight="1">
+      <c r="A3" s="66"/>
+      <c r="B3" s="68"/>
       <c r="C3" s="30" t="str">
         <f>Sheet1!B6</f>
         <v>p2.8xlarge on-demand</v>
       </c>
-      <c r="D3" s="68" t="s">
-        <v>187</v>
+      <c r="D3" s="60" t="s">
+        <v>186</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F3" s="27">
         <f>Sheet1!V6</f>
@@ -12345,27 +12573,66 @@
         <f>Sheet1!F6*Sheet1!D6</f>
         <v>69.92</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="14" t="str">
+        <f>Sheet1!$C6</f>
+        <v>K80</v>
+      </c>
+      <c r="M3" s="14">
         <f>Sheet1!$D6</f>
         <v>8</v>
       </c>
-      <c r="M3" s="14" t="str">
-        <f>Sheet1!$C6</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="20" customHeight="1">
-      <c r="A4" s="60"/>
-      <c r="B4" s="66"/>
+      <c r="N3" s="61" t="str">
+        <f>Sheet1!$K6</f>
+        <v>Xeon E5-2686 v4</v>
+      </c>
+      <c r="O3" s="61">
+        <f>Sheet1!$L6</f>
+        <v>32</v>
+      </c>
+      <c r="P3" s="61">
+        <f>IF(Sheet1!$P6="","",Sheet1!$P6)</f>
+        <v>488</v>
+      </c>
+      <c r="Q3" s="27" t="str">
+        <f>IF(Sheet1!$Q6="","",Sheet1!$Q6)</f>
+        <v/>
+      </c>
+      <c r="R3" s="27" t="str">
+        <f>IF(Sheet1!$R6="","",Sheet1!$R6)</f>
+        <v/>
+      </c>
+      <c r="S3" s="64" t="str">
+        <f>IF(Sheet1!$S6="","",Sheet1!$S6)</f>
+        <v/>
+      </c>
+      <c r="T3" s="64" t="str">
+        <f>IF(Sheet1!$T6="","",Sheet1!$T6)</f>
+        <v/>
+      </c>
+      <c r="U3" s="64" t="str">
+        <f>IF(Sheet1!$U6="","",Sheet1!$U6)</f>
+        <v/>
+      </c>
+      <c r="V3" s="63" t="str">
+        <f>IF(Sheet1!$Z6="","",Sheet1!$Z6) &amp; " CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36."</f>
+        <v>Free Outbound Traffic = 1 GB/month. CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36.</v>
+      </c>
+      <c r="X3" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="20" customHeight="1">
+      <c r="A4" s="66"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="30" t="str">
         <f>Sheet1!B7</f>
         <v>p2.xlarge on-demand</v>
       </c>
-      <c r="D4" s="68" t="s">
-        <v>188</v>
+      <c r="D4" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F4" s="27">
         <f>Sheet1!V7</f>
@@ -12385,27 +12652,66 @@
         <f>Sheet1!F7*Sheet1!D7</f>
         <v>8.74</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="14" t="str">
+        <f>Sheet1!$C7</f>
+        <v>K80</v>
+      </c>
+      <c r="M4" s="14">
         <f>Sheet1!$D7</f>
         <v>1</v>
       </c>
-      <c r="M4" s="14" t="str">
-        <f>Sheet1!$C7</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="20" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="66"/>
+      <c r="N4" s="61" t="str">
+        <f>Sheet1!$K7</f>
+        <v>Xeon E5-2686 v4</v>
+      </c>
+      <c r="O4" s="61">
+        <f>Sheet1!$L7</f>
+        <v>4</v>
+      </c>
+      <c r="P4" s="61">
+        <f>IF(Sheet1!$P7="","",Sheet1!$P7)</f>
+        <v>61</v>
+      </c>
+      <c r="Q4" s="27" t="str">
+        <f>IF(Sheet1!$Q7="","",Sheet1!$Q7)</f>
+        <v/>
+      </c>
+      <c r="R4" s="27" t="str">
+        <f>IF(Sheet1!$R7="","",Sheet1!$R7)</f>
+        <v/>
+      </c>
+      <c r="S4" s="63" t="str">
+        <f>IF(Sheet1!$S7="","",Sheet1!$S7)</f>
+        <v/>
+      </c>
+      <c r="T4" s="63" t="str">
+        <f>IF(Sheet1!$T7="","",Sheet1!$T7)</f>
+        <v/>
+      </c>
+      <c r="U4" s="63" t="str">
+        <f>IF(Sheet1!$U7="","",Sheet1!$U7)</f>
+        <v/>
+      </c>
+      <c r="V4" s="63" t="str">
+        <f>IF(Sheet1!$Z7="","",Sheet1!$Z7) &amp; " CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36."</f>
+        <v>Free Outbound Traffic = 1 GB/month.  CPU performance is approx. performance of Xeon E5-2690 v4 with 18 cores devided by 18 cores * 2 Hyper-threads = 36.</v>
+      </c>
+      <c r="X4" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="20" customHeight="1">
+      <c r="A5" s="66"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="30" t="str">
         <f>Sheet1!B8</f>
         <v>p2 dedicated host On-demand</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="27">
         <f>Sheet1!V8</f>
@@ -12425,27 +12731,66 @@
         <f>Sheet1!F8*Sheet1!D8</f>
         <v>139.84</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="14" t="str">
+        <f>Sheet1!$C8</f>
+        <v>K80</v>
+      </c>
+      <c r="M5" s="14">
         <f>Sheet1!$D8</f>
         <v>16</v>
       </c>
-      <c r="M5" s="14" t="str">
-        <f>Sheet1!$C8</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="20" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="66"/>
+      <c r="N5" s="61" t="str">
+        <f>Sheet1!$K8</f>
+        <v>Xeon E5-2686 v4</v>
+      </c>
+      <c r="O5" s="61">
+        <f>Sheet1!$L8</f>
+        <v>2</v>
+      </c>
+      <c r="P5" s="61" t="str">
+        <f>IF(Sheet1!$P8="","",Sheet1!$P8)</f>
+        <v/>
+      </c>
+      <c r="Q5" s="27" t="str">
+        <f>IF(Sheet1!$Q8="","",Sheet1!$Q8)</f>
+        <v/>
+      </c>
+      <c r="R5" s="27" t="str">
+        <f>IF(Sheet1!$R8="","",Sheet1!$R8)</f>
+        <v/>
+      </c>
+      <c r="S5" s="64" t="str">
+        <f>IF(Sheet1!$S8="","",Sheet1!$S8)</f>
+        <v/>
+      </c>
+      <c r="T5" s="64" t="str">
+        <f>IF(Sheet1!$T8="","",Sheet1!$T8)</f>
+        <v/>
+      </c>
+      <c r="U5" s="64" t="str">
+        <f>IF(Sheet1!$U8="","",Sheet1!$U8)</f>
+        <v/>
+      </c>
+      <c r="V5" s="64" t="str">
+        <f>IF(Sheet1!$Z8="","",Sheet1!$Z8)</f>
+        <v>Up to 56% of savings for 1- and 3-year terms.</v>
+      </c>
+      <c r="X5" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="20" customHeight="1">
+      <c r="A6" s="66"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="30" t="str">
         <f>Sheet1!B9</f>
         <v>p2 dedicated host 1 year no Upfront</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -12462,27 +12807,66 @@
         <f>Sheet1!F9*Sheet1!D9</f>
         <v>139.84</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="14" t="str">
+        <f>Sheet1!$C9</f>
+        <v>K80</v>
+      </c>
+      <c r="M6" s="14">
         <f>Sheet1!$D9</f>
         <v>16</v>
       </c>
-      <c r="M6" s="14" t="str">
-        <f>Sheet1!$C9</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="20" customHeight="1">
-      <c r="A7" s="60"/>
-      <c r="B7" s="66"/>
+      <c r="N6" s="61" t="str">
+        <f>Sheet1!$K9</f>
+        <v>Xeon E5-2686 v4</v>
+      </c>
+      <c r="O6" s="61">
+        <f>Sheet1!$L9</f>
+        <v>2</v>
+      </c>
+      <c r="P6" s="61" t="str">
+        <f>IF(Sheet1!$P9="","",Sheet1!$P9)</f>
+        <v/>
+      </c>
+      <c r="Q6" s="27" t="str">
+        <f>IF(Sheet1!$Q9="","",Sheet1!$Q9)</f>
+        <v/>
+      </c>
+      <c r="R6" s="27" t="str">
+        <f>IF(Sheet1!$R9="","",Sheet1!$R9)</f>
+        <v/>
+      </c>
+      <c r="S6" s="63" t="str">
+        <f>IF(Sheet1!$S9="","",Sheet1!$S9)</f>
+        <v/>
+      </c>
+      <c r="T6" s="63" t="str">
+        <f>IF(Sheet1!$T9="","",Sheet1!$T9)</f>
+        <v/>
+      </c>
+      <c r="U6" s="63" t="str">
+        <f>IF(Sheet1!$U9="","",Sheet1!$U9)</f>
+        <v/>
+      </c>
+      <c r="V6" s="63" t="str">
+        <f>IF(Sheet1!$Z9="","",Sheet1!$Z9)</f>
+        <v/>
+      </c>
+      <c r="X6" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="20" customHeight="1">
+      <c r="A7" s="66"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="30" t="str">
         <f>Sheet1!B10</f>
         <v>p2 dedicated host 1 year 100% Upfront</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
@@ -12499,22 +12883,61 @@
         <f>Sheet1!F10*Sheet1!D10</f>
         <v>139.84</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="14" t="str">
+        <f>Sheet1!$C10</f>
+        <v>K80</v>
+      </c>
+      <c r="M7" s="14">
         <f>Sheet1!$D10</f>
         <v>16</v>
       </c>
-      <c r="M7" s="14" t="str">
-        <f>Sheet1!$C10</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="20" customHeight="1">
-      <c r="A8" s="60" t="str">
+      <c r="N7" s="14" t="str">
+        <f>Sheet1!$K10</f>
+        <v>Xeon E5-2686 v5</v>
+      </c>
+      <c r="O7" s="14">
+        <f>Sheet1!$L10</f>
+        <v>2</v>
+      </c>
+      <c r="P7" s="61" t="str">
+        <f>IF(Sheet1!$P10="","",Sheet1!$P10)</f>
+        <v/>
+      </c>
+      <c r="Q7" s="27" t="str">
+        <f>IF(Sheet1!$Q10="","",Sheet1!$Q10)</f>
+        <v/>
+      </c>
+      <c r="R7" s="27" t="str">
+        <f>IF(Sheet1!$R10="","",Sheet1!$R10)</f>
+        <v/>
+      </c>
+      <c r="S7" s="64" t="str">
+        <f>IF(Sheet1!$S10="","",Sheet1!$S10)</f>
+        <v/>
+      </c>
+      <c r="T7" s="64" t="str">
+        <f>IF(Sheet1!$T10="","",Sheet1!$T10)</f>
+        <v/>
+      </c>
+      <c r="U7" s="64" t="str">
+        <f>IF(Sheet1!$U10="","",Sheet1!$U10)</f>
+        <v/>
+      </c>
+      <c r="V7" s="64" t="str">
+        <f>IF(Sheet1!$Z10="","",Sheet1!$Z10)</f>
+        <v/>
+      </c>
+      <c r="X7" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="20" customHeight="1">
+      <c r="A8" s="66" t="str">
         <f>Sheet1!$A$13</f>
         <v>Softlayer</v>
       </c>
-      <c r="B8" s="66" t="s">
-        <v>181</v>
+      <c r="B8" s="68" t="s">
+        <v>180</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>Sheet1!B13</f>
@@ -12522,7 +12945,7 @@
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" s="27">
         <f>Sheet1!V13</f>
@@ -12539,25 +12962,64 @@
         <f>Sheet1!F13*Sheet1!D13</f>
         <v>8.74</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="14" t="str">
+        <f>Sheet1!$C13</f>
+        <v>K80</v>
+      </c>
+      <c r="M8" s="14">
         <f>Sheet1!$D13</f>
         <v>1</v>
       </c>
-      <c r="M8" s="14" t="str">
-        <f>Sheet1!$C13</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="60"/>
-      <c r="B9" s="66"/>
+      <c r="N8" s="14" t="str">
+        <f>Sheet1!$K13</f>
+        <v>Xeon E5-2620 v4</v>
+      </c>
+      <c r="O8" s="14">
+        <f>Sheet1!$L13</f>
+        <v>2</v>
+      </c>
+      <c r="P8" s="14">
+        <f>IF(Sheet1!$P13="","",Sheet1!$P13)</f>
+        <v>128</v>
+      </c>
+      <c r="Q8" s="27" t="str">
+        <f>IF(Sheet1!$Q13="","",Sheet1!$Q13)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R8" s="27">
+        <f>IF(Sheet1!$R13="","",Sheet1!$R13)</f>
+        <v>800</v>
+      </c>
+      <c r="S8" s="63" t="str">
+        <f>IF(Sheet1!$S13="","",Sheet1!$S13)</f>
+        <v>SSD</v>
+      </c>
+      <c r="T8" s="63">
+        <f>IF(Sheet1!$T13="","",Sheet1!$T13)</f>
+        <v>800</v>
+      </c>
+      <c r="U8" s="63">
+        <f>IF(Sheet1!$U13="","",Sheet1!$U13)</f>
+        <v>0.1</v>
+      </c>
+      <c r="V8" s="63" t="str">
+        <f>IF(Sheet1!$Z13="","",Sheet1!$Z13)</f>
+        <v>Traffic limited to 500GB.</v>
+      </c>
+      <c r="X8" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A9" s="66"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="30" t="str">
         <f>Sheet1!B14</f>
         <v>NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4 monthly</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
@@ -12574,25 +13036,64 @@
         <f>Sheet1!F14*Sheet1!D14</f>
         <v>8.74</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="14" t="str">
+        <f>Sheet1!$C14</f>
+        <v>K80</v>
+      </c>
+      <c r="M9" s="14">
         <f>Sheet1!$D14</f>
         <v>1</v>
       </c>
-      <c r="M9" s="14" t="str">
-        <f>Sheet1!$C14</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="20" customHeight="1">
-      <c r="A10" s="60"/>
-      <c r="B10" s="66"/>
+      <c r="N9" s="14" t="str">
+        <f>Sheet1!$K14</f>
+        <v>Xeon E5-2620 v4</v>
+      </c>
+      <c r="O9" s="14">
+        <f>Sheet1!$L14</f>
+        <v>2</v>
+      </c>
+      <c r="P9" s="14">
+        <f>IF(Sheet1!$P14="","",Sheet1!$P14)</f>
+        <v>128</v>
+      </c>
+      <c r="Q9" s="27" t="str">
+        <f>IF(Sheet1!$Q14="","",Sheet1!$Q14)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R9" s="27">
+        <f>IF(Sheet1!$R14="","",Sheet1!$R14)</f>
+        <v>800</v>
+      </c>
+      <c r="S9" s="64" t="str">
+        <f>IF(Sheet1!$S14="","",Sheet1!$S14)</f>
+        <v>SSD</v>
+      </c>
+      <c r="T9" s="64">
+        <f>IF(Sheet1!$T14="","",Sheet1!$T14)</f>
+        <v>800</v>
+      </c>
+      <c r="U9" s="64">
+        <f>IF(Sheet1!$U14="","",Sheet1!$U14)</f>
+        <v>0.1</v>
+      </c>
+      <c r="V9" s="64" t="str">
+        <f>IF(Sheet1!$Z14="","",Sheet1!$Z14)</f>
+        <v>Traffic limited to 501GB.</v>
+      </c>
+      <c r="X9" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="20" customHeight="1">
+      <c r="A10" s="66"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="30" t="str">
         <f>Sheet1!B15</f>
         <v>NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
@@ -12609,25 +13110,64 @@
         <f>Sheet1!F15*Sheet1!D15</f>
         <v>8.74</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="14" t="str">
+        <f>Sheet1!$C15</f>
+        <v>K80</v>
+      </c>
+      <c r="M10" s="14">
         <f>Sheet1!$D15</f>
         <v>1</v>
       </c>
-      <c r="M10" s="14" t="str">
-        <f>Sheet1!$C15</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="20" customHeight="1">
-      <c r="A11" s="60"/>
-      <c r="B11" s="66"/>
+      <c r="N10" s="14" t="str">
+        <f>Sheet1!$K15</f>
+        <v>Xeon E5-2690 v3</v>
+      </c>
+      <c r="O10" s="14">
+        <f>Sheet1!$L15</f>
+        <v>2</v>
+      </c>
+      <c r="P10" s="14">
+        <f>IF(Sheet1!$P15="","",Sheet1!$P15)</f>
+        <v>24</v>
+      </c>
+      <c r="Q10" s="27" t="str">
+        <f>IF(Sheet1!$Q15="","",Sheet1!$Q15)</f>
+        <v>SATA</v>
+      </c>
+      <c r="R10" s="27">
+        <f>IF(Sheet1!$R15="","",Sheet1!$R15)</f>
+        <v>1000</v>
+      </c>
+      <c r="S10" s="63" t="str">
+        <f>IF(Sheet1!$S15="","",Sheet1!$S15)</f>
+        <v/>
+      </c>
+      <c r="T10" s="63" t="str">
+        <f>IF(Sheet1!$T15="","",Sheet1!$T15)</f>
+        <v/>
+      </c>
+      <c r="U10" s="63">
+        <f>IF(Sheet1!$U15="","",Sheet1!$U15)</f>
+        <v>10</v>
+      </c>
+      <c r="V10" s="63" t="str">
+        <f>IF(Sheet1!$Z15="","",Sheet1!$Z15)</f>
+        <v>Traffic limited to 500GB.</v>
+      </c>
+      <c r="X10" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="20" customHeight="1">
+      <c r="A11" s="66"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="30" t="str">
         <f>Sheet1!B16</f>
         <v>NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -12644,22 +13184,61 @@
         <f>Sheet1!F16*Sheet1!D16</f>
         <v>9.65</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="14" t="str">
+        <f>Sheet1!$C16</f>
+        <v>M60</v>
+      </c>
+      <c r="M11" s="14">
         <f>Sheet1!$D16</f>
         <v>1</v>
       </c>
-      <c r="M11" s="14" t="str">
-        <f>Sheet1!$C16</f>
-        <v>M60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="19">
+      <c r="N11" s="14" t="str">
+        <f>Sheet1!$K16</f>
+        <v>Xeon E5-2690 v3</v>
+      </c>
+      <c r="O11" s="14">
+        <f>Sheet1!$L16</f>
+        <v>2</v>
+      </c>
+      <c r="P11" s="14">
+        <f>IF(Sheet1!$P16="","",Sheet1!$P16)</f>
+        <v>64</v>
+      </c>
+      <c r="Q11" s="27" t="str">
+        <f>IF(Sheet1!$Q16="","",Sheet1!$Q16)</f>
+        <v>SATA</v>
+      </c>
+      <c r="R11" s="27">
+        <f>IF(Sheet1!$R16="","",Sheet1!$R16)</f>
+        <v>1000</v>
+      </c>
+      <c r="S11" s="64" t="str">
+        <f>IF(Sheet1!$S16="","",Sheet1!$S16)</f>
+        <v/>
+      </c>
+      <c r="T11" s="64" t="str">
+        <f>IF(Sheet1!$T16="","",Sheet1!$T16)</f>
+        <v/>
+      </c>
+      <c r="U11" s="64">
+        <f>IF(Sheet1!$U16="","",Sheet1!$U16)</f>
+        <v>10</v>
+      </c>
+      <c r="V11" s="64" t="str">
+        <f>IF(Sheet1!$Z16="","",Sheet1!$Z16)</f>
+        <v>Traffic limited to 500GB.</v>
+      </c>
+      <c r="X11" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="19">
       <c r="A12" s="33" t="str">
         <f>Sheet1!A18</f>
         <v>Nimbix</v>
       </c>
-      <c r="B12" s="67" t="s">
-        <v>182</v>
+      <c r="B12" s="59" t="s">
+        <v>181</v>
       </c>
       <c r="C12" s="30" t="str">
         <f>Sheet1!B18</f>
@@ -12667,17 +13246,14 @@
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="27">
         <f>Sheet1!V18</f>
         <v>5</v>
       </c>
       <c r="G12" s="27"/>
-      <c r="H12" s="27">
-        <f>Sheet1!X18</f>
-        <v>3600</v>
-      </c>
+      <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="14">
         <f>Sheet1!N18*Sheet1!L18</f>
@@ -12687,22 +13263,61 @@
         <f>Sheet1!F18*Sheet1!D18</f>
         <v>17.48</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="14" t="str">
+        <f>Sheet1!$C18</f>
+        <v>K80</v>
+      </c>
+      <c r="M12" s="14">
         <f>Sheet1!$D18</f>
         <v>2</v>
       </c>
-      <c r="M12" s="14" t="str">
-        <f>Sheet1!$C18</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="20" customHeight="1">
-      <c r="A13" s="60" t="str">
+      <c r="N12" s="14" t="str">
+        <f>Sheet1!$K18</f>
+        <v>POWER8?</v>
+      </c>
+      <c r="O12" s="14">
+        <f>Sheet1!$L18</f>
+        <v>2</v>
+      </c>
+      <c r="P12" s="61" t="str">
+        <f>IF(Sheet1!$P18="","",Sheet1!$P18)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="27" t="str">
+        <f>IF(Sheet1!$Q18="","",Sheet1!$Q18)</f>
+        <v/>
+      </c>
+      <c r="R12" s="27" t="str">
+        <f>IF(Sheet1!$R18="","",Sheet1!$R18)</f>
+        <v/>
+      </c>
+      <c r="S12" s="63" t="str">
+        <f>IF(Sheet1!$S18="","",Sheet1!$S18)</f>
+        <v/>
+      </c>
+      <c r="T12" s="63" t="str">
+        <f>IF(Sheet1!$T18="","",Sheet1!$T18)</f>
+        <v/>
+      </c>
+      <c r="U12" s="63" t="str">
+        <f>IF(Sheet1!$U18="","",Sheet1!$U18)</f>
+        <v/>
+      </c>
+      <c r="V12" s="63" t="str">
+        <f>IF(Sheet1!$Z18="","",Sheet1!$Z18)</f>
+        <v xml:space="preserve"> http://www-01.ibm.com/common/ssi/cgi-bin/ssialias?htmlfid=POB03046USEN</v>
+      </c>
+      <c r="X12" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="20" customHeight="1">
+      <c r="A13" s="66" t="str">
         <f>Sheet1!A23</f>
         <v>Cirrascale</v>
       </c>
-      <c r="B13" s="66" t="s">
-        <v>183</v>
+      <c r="B13" s="68" t="s">
+        <v>182</v>
       </c>
       <c r="C13" s="30" t="str">
         <f>Sheet1!B23&amp;" monthly"</f>
@@ -12710,7 +13325,7 @@
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
@@ -12727,25 +13342,64 @@
         <f>Sheet1!F23*Sheet1!D23</f>
         <v>69.92</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="14" t="str">
+        <f>Sheet1!$C23</f>
+        <v>K80</v>
+      </c>
+      <c r="M13" s="14">
         <f>Sheet1!$D23</f>
         <v>8</v>
       </c>
-      <c r="M13" s="14" t="str">
-        <f>Sheet1!$C23</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="66"/>
+      <c r="N13" s="14" t="str">
+        <f>Sheet1!$K23</f>
+        <v>Xeon E5-2667 v3</v>
+      </c>
+      <c r="O13" s="14">
+        <f>Sheet1!$L23</f>
+        <v>2</v>
+      </c>
+      <c r="P13" s="14">
+        <f>IF(Sheet1!$P23="","",Sheet1!$P23)</f>
+        <v>512</v>
+      </c>
+      <c r="Q13" s="27" t="str">
+        <f>IF(Sheet1!$Q23="","",Sheet1!$Q23)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R13" s="27">
+        <f>IF(Sheet1!$R23="","",Sheet1!$R23)</f>
+        <v>1000</v>
+      </c>
+      <c r="S13" s="64" t="str">
+        <f>IF(Sheet1!$S23="","",Sheet1!$S23)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T13" s="64">
+        <f>IF(Sheet1!$T23="","",Sheet1!$T23)</f>
+        <v>4000</v>
+      </c>
+      <c r="U13" s="64" t="str">
+        <f>IF(Sheet1!$U23="","",Sheet1!$U23)</f>
+        <v/>
+      </c>
+      <c r="V13" s="64" t="str">
+        <f>IF(Sheet1!$Z23="","",Sheet1!$Z23)</f>
+        <v/>
+      </c>
+      <c r="X13" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A14" s="66"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="30" t="str">
         <f>Sheet1!B23&amp;" weekly"</f>
         <v>16-GPU x86 SERVER K80 weekly</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="27">
@@ -12762,25 +13416,64 @@
         <f>Sheet1!F23*Sheet1!D23</f>
         <v>69.92</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="14" t="str">
+        <f>Sheet1!$C23</f>
+        <v>K80</v>
+      </c>
+      <c r="M14" s="14">
         <f>Sheet1!$D23</f>
         <v>8</v>
       </c>
-      <c r="M14" s="14" t="str">
-        <f>Sheet1!$C23</f>
-        <v>K80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="66"/>
+      <c r="N14" s="14" t="str">
+        <f>Sheet1!$K23</f>
+        <v>Xeon E5-2667 v3</v>
+      </c>
+      <c r="O14" s="14">
+        <f>Sheet1!$L23</f>
+        <v>2</v>
+      </c>
+      <c r="P14" s="14">
+        <f>IF(Sheet1!$P23="","",Sheet1!$P23)</f>
+        <v>512</v>
+      </c>
+      <c r="Q14" s="27" t="str">
+        <f>IF(Sheet1!$Q23="","",Sheet1!$Q23)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R14" s="27">
+        <f>IF(Sheet1!$R23="","",Sheet1!$R23)</f>
+        <v>1000</v>
+      </c>
+      <c r="S14" s="63" t="str">
+        <f>IF(Sheet1!$S23="","",Sheet1!$S23)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T14" s="63">
+        <f>IF(Sheet1!$T23="","",Sheet1!$T23)</f>
+        <v>4000</v>
+      </c>
+      <c r="U14" s="63" t="str">
+        <f>IF(Sheet1!$U23="","",Sheet1!$U23)</f>
+        <v/>
+      </c>
+      <c r="V14" s="63" t="str">
+        <f>IF(Sheet1!$Z23="","",Sheet1!$Z23)</f>
+        <v/>
+      </c>
+      <c r="X14" s="13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A15" s="66"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="30" t="str">
         <f>Sheet1!B24&amp;" monthly"</f>
         <v>8-GPU x86 SERVER M40 monthly</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
@@ -12797,25 +13490,64 @@
         <f>Sheet1!F24*Sheet1!D24</f>
         <v>54.752000000000002</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="14" t="str">
+        <f>Sheet1!$C24</f>
+        <v>M40</v>
+      </c>
+      <c r="M15" s="14">
         <f>Sheet1!$D24</f>
         <v>8</v>
       </c>
-      <c r="M15" s="14" t="str">
-        <f>Sheet1!$C24</f>
-        <v>M40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="20" customHeight="1">
-      <c r="A16" s="60"/>
-      <c r="B16" s="66"/>
+      <c r="N15" s="14" t="str">
+        <f>Sheet1!$K24</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O15" s="14">
+        <f>Sheet1!$L24</f>
+        <v>2</v>
+      </c>
+      <c r="P15" s="14">
+        <f>IF(Sheet1!$P24="","",Sheet1!$P24)</f>
+        <v>256</v>
+      </c>
+      <c r="Q15" s="27" t="str">
+        <f>IF(Sheet1!$Q24="","",Sheet1!$Q24)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R15" s="27">
+        <f>IF(Sheet1!$R24="","",Sheet1!$R24)</f>
+        <v>1000</v>
+      </c>
+      <c r="S15" s="64" t="str">
+        <f>IF(Sheet1!$S24="","",Sheet1!$S24)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T15" s="64">
+        <f>IF(Sheet1!$T24="","",Sheet1!$T24)</f>
+        <v>4000</v>
+      </c>
+      <c r="U15" s="64" t="str">
+        <f>IF(Sheet1!$U24="","",Sheet1!$U24)</f>
+        <v/>
+      </c>
+      <c r="V15" s="64" t="str">
+        <f>IF(Sheet1!$Z24="","",Sheet1!$Z24)</f>
+        <v/>
+      </c>
+      <c r="X15" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="20" customHeight="1">
+      <c r="A16" s="66"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="30" t="str">
         <f>Sheet1!B24&amp;" weekly"</f>
         <v>8-GPU x86 SERVER M40 weekly</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F16" s="27"/>
       <c r="G16" s="27">
@@ -12832,25 +13564,64 @@
         <f>Sheet1!F24*Sheet1!D24</f>
         <v>54.752000000000002</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="14" t="str">
+        <f>Sheet1!$C24</f>
+        <v>M40</v>
+      </c>
+      <c r="M16" s="14">
         <f>Sheet1!$D24</f>
         <v>8</v>
       </c>
-      <c r="M16" s="14" t="str">
-        <f>Sheet1!$C24</f>
-        <v>M40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A17" s="60"/>
-      <c r="B17" s="66"/>
+      <c r="N16" s="14" t="str">
+        <f>Sheet1!$K24</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O16" s="14">
+        <f>Sheet1!$L24</f>
+        <v>2</v>
+      </c>
+      <c r="P16" s="14">
+        <f>IF(Sheet1!$P24="","",Sheet1!$P24)</f>
+        <v>256</v>
+      </c>
+      <c r="Q16" s="27" t="str">
+        <f>IF(Sheet1!$Q24="","",Sheet1!$Q24)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R16" s="27">
+        <f>IF(Sheet1!$R24="","",Sheet1!$R24)</f>
+        <v>1000</v>
+      </c>
+      <c r="S16" s="63" t="str">
+        <f>IF(Sheet1!$S24="","",Sheet1!$S24)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T16" s="63">
+        <f>IF(Sheet1!$T24="","",Sheet1!$T24)</f>
+        <v>4000</v>
+      </c>
+      <c r="U16" s="63" t="str">
+        <f>IF(Sheet1!$U24="","",Sheet1!$U24)</f>
+        <v/>
+      </c>
+      <c r="V16" s="63" t="str">
+        <f>IF(Sheet1!$Z24="","",Sheet1!$Z24)</f>
+        <v/>
+      </c>
+      <c r="X16" s="13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A17" s="66"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="30" t="str">
         <f>Sheet1!B25&amp;" monthly"</f>
         <v>8-GPU x86 SERVER monthly</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
@@ -12867,25 +13638,64 @@
         <f>Sheet1!F25*Sheet1!D25</f>
         <v>49.152000000000001</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="14" t="str">
+        <f>Sheet1!$C25</f>
+        <v>GeForce GTX TITAN X</v>
+      </c>
+      <c r="M17" s="14">
         <f>Sheet1!$D25</f>
         <v>8</v>
       </c>
-      <c r="M17" s="14" t="str">
-        <f>Sheet1!$C25</f>
-        <v>GeForce GTX TITAN X</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="20" customHeight="1">
-      <c r="A18" s="60"/>
-      <c r="B18" s="66"/>
+      <c r="N17" s="14" t="str">
+        <f>Sheet1!$K25</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O17" s="14">
+        <f>Sheet1!$L25</f>
+        <v>2</v>
+      </c>
+      <c r="P17" s="14">
+        <f>IF(Sheet1!$P25="","",Sheet1!$P25)</f>
+        <v>256</v>
+      </c>
+      <c r="Q17" s="27" t="str">
+        <f>IF(Sheet1!$Q25="","",Sheet1!$Q25)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R17" s="27">
+        <f>IF(Sheet1!$R25="","",Sheet1!$R25)</f>
+        <v>1000</v>
+      </c>
+      <c r="S17" s="64" t="str">
+        <f>IF(Sheet1!$S25="","",Sheet1!$S25)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T17" s="64">
+        <f>IF(Sheet1!$T25="","",Sheet1!$T25)</f>
+        <v>4000</v>
+      </c>
+      <c r="U17" s="64" t="str">
+        <f>IF(Sheet1!$U25="","",Sheet1!$U25)</f>
+        <v/>
+      </c>
+      <c r="V17" s="64" t="str">
+        <f>IF(Sheet1!$Z25="","",Sheet1!$Z25)</f>
+        <v/>
+      </c>
+      <c r="X17" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="20" customHeight="1">
+      <c r="A18" s="66"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="30" t="str">
         <f>Sheet1!B25&amp;" weekly"</f>
         <v>8-GPU x86 SERVER weekly</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F18" s="27"/>
       <c r="G18" s="27">
@@ -12902,25 +13712,64 @@
         <f>Sheet1!F25*Sheet1!D25</f>
         <v>49.152000000000001</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="14" t="str">
+        <f>Sheet1!$C25</f>
+        <v>GeForce GTX TITAN X</v>
+      </c>
+      <c r="M18" s="14">
         <f>Sheet1!$D25</f>
         <v>8</v>
       </c>
-      <c r="M18" s="14" t="str">
-        <f>Sheet1!$C25</f>
-        <v>GeForce GTX TITAN X</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="60"/>
-      <c r="B19" s="66"/>
+      <c r="N18" s="14" t="str">
+        <f>Sheet1!$K25</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O18" s="14">
+        <f>Sheet1!$L25</f>
+        <v>2</v>
+      </c>
+      <c r="P18" s="14">
+        <f>IF(Sheet1!$P25="","",Sheet1!$P25)</f>
+        <v>256</v>
+      </c>
+      <c r="Q18" s="27" t="str">
+        <f>IF(Sheet1!$Q25="","",Sheet1!$Q25)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R18" s="27">
+        <f>IF(Sheet1!$R25="","",Sheet1!$R25)</f>
+        <v>1000</v>
+      </c>
+      <c r="S18" s="63" t="str">
+        <f>IF(Sheet1!$S25="","",Sheet1!$S25)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T18" s="63">
+        <f>IF(Sheet1!$T25="","",Sheet1!$T25)</f>
+        <v>4000</v>
+      </c>
+      <c r="U18" s="63" t="str">
+        <f>IF(Sheet1!$U25="","",Sheet1!$U25)</f>
+        <v/>
+      </c>
+      <c r="V18" s="63" t="str">
+        <f>IF(Sheet1!$Z25="","",Sheet1!$Z25)</f>
+        <v/>
+      </c>
+      <c r="X18" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A19" s="66"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="30" t="str">
         <f>Sheet1!B26&amp;" monthly"</f>
         <v>4-GPU x86 SERVER monthly</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
@@ -12937,25 +13786,64 @@
         <f>Sheet1!F26*Sheet1!D26</f>
         <v>24.576000000000001</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="14" t="str">
+        <f>Sheet1!$C26</f>
+        <v>GeForce GTX TITAN X</v>
+      </c>
+      <c r="M19" s="14">
         <f>Sheet1!$D26</f>
         <v>4</v>
       </c>
-      <c r="M19" s="14" t="str">
-        <f>Sheet1!$C26</f>
-        <v>GeForce GTX TITAN X</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="20" customHeight="1">
-      <c r="A20" s="60"/>
-      <c r="B20" s="66"/>
+      <c r="N19" s="14" t="str">
+        <f>Sheet1!$K26</f>
+        <v>Xeon E5-2670 v2</v>
+      </c>
+      <c r="O19" s="14">
+        <f>Sheet1!$L26</f>
+        <v>2</v>
+      </c>
+      <c r="P19" s="14">
+        <f>IF(Sheet1!$P26="","",Sheet1!$P26)</f>
+        <v>128</v>
+      </c>
+      <c r="Q19" s="27" t="str">
+        <f>IF(Sheet1!$Q26="","",Sheet1!$Q26)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R19" s="27">
+        <f>IF(Sheet1!$R26="","",Sheet1!$R26)</f>
+        <v>256</v>
+      </c>
+      <c r="S19" s="64" t="str">
+        <f>IF(Sheet1!$S26="","",Sheet1!$S26)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T19" s="64">
+        <f>IF(Sheet1!$T26="","",Sheet1!$T26)</f>
+        <v>4000</v>
+      </c>
+      <c r="U19" s="64" t="str">
+        <f>IF(Sheet1!$U26="","",Sheet1!$U26)</f>
+        <v/>
+      </c>
+      <c r="V19" s="64" t="str">
+        <f>IF(Sheet1!$Z26="","",Sheet1!$Z26)</f>
+        <v/>
+      </c>
+      <c r="X19" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="20" customHeight="1">
+      <c r="A20" s="66"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="30" t="str">
         <f>Sheet1!B26&amp;" weekly"</f>
         <v>4-GPU x86 SERVER weekly</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="27"/>
       <c r="G20" s="27">
@@ -12972,25 +13860,64 @@
         <f>Sheet1!F26*Sheet1!D26</f>
         <v>24.576000000000001</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="14" t="str">
+        <f>Sheet1!$C26</f>
+        <v>GeForce GTX TITAN X</v>
+      </c>
+      <c r="M20" s="14">
         <f>Sheet1!$D26</f>
         <v>4</v>
       </c>
-      <c r="M20" s="14" t="str">
-        <f>Sheet1!$C26</f>
-        <v>GeForce GTX TITAN X</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A21" s="60"/>
-      <c r="B21" s="66"/>
+      <c r="N20" s="14" t="str">
+        <f>Sheet1!$K26</f>
+        <v>Xeon E5-2670 v2</v>
+      </c>
+      <c r="O20" s="14">
+        <f>Sheet1!$L26</f>
+        <v>2</v>
+      </c>
+      <c r="P20" s="14">
+        <f>IF(Sheet1!$P26="","",Sheet1!$P26)</f>
+        <v>128</v>
+      </c>
+      <c r="Q20" s="27" t="str">
+        <f>IF(Sheet1!$Q26="","",Sheet1!$Q26)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R20" s="27">
+        <f>IF(Sheet1!$R26="","",Sheet1!$R26)</f>
+        <v>256</v>
+      </c>
+      <c r="S20" s="63" t="str">
+        <f>IF(Sheet1!$S26="","",Sheet1!$S26)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T20" s="63">
+        <f>IF(Sheet1!$T26="","",Sheet1!$T26)</f>
+        <v>4000</v>
+      </c>
+      <c r="U20" s="63" t="str">
+        <f>IF(Sheet1!$U26="","",Sheet1!$U26)</f>
+        <v/>
+      </c>
+      <c r="V20" s="63" t="str">
+        <f>IF(Sheet1!$Z26="","",Sheet1!$Z26)</f>
+        <v/>
+      </c>
+      <c r="X20" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A21" s="66"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="30" t="str">
         <f>Sheet1!B27&amp;" monthly"</f>
         <v>8-GPU x86 SERVER P40 monthly</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -13007,25 +13934,64 @@
         <f>Sheet1!F27*Sheet1!D27</f>
         <v>94.063999999999993</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="14" t="str">
+        <f>Sheet1!$C27</f>
+        <v>P40</v>
+      </c>
+      <c r="M21" s="14">
         <f>Sheet1!$D27</f>
         <v>8</v>
       </c>
-      <c r="M21" s="14" t="str">
-        <f>Sheet1!$C27</f>
-        <v>P40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="60"/>
-      <c r="B22" s="66"/>
+      <c r="N21" s="14" t="str">
+        <f>Sheet1!$K27</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O21" s="14">
+        <f>Sheet1!$L27</f>
+        <v>2</v>
+      </c>
+      <c r="P21" s="14">
+        <f>IF(Sheet1!$P27="","",Sheet1!$P27)</f>
+        <v>256</v>
+      </c>
+      <c r="Q21" s="27" t="str">
+        <f>IF(Sheet1!$Q27="","",Sheet1!$Q27)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R21" s="27">
+        <f>IF(Sheet1!$R27="","",Sheet1!$R27)</f>
+        <v>1000</v>
+      </c>
+      <c r="S21" s="64" t="str">
+        <f>IF(Sheet1!$S27="","",Sheet1!$S27)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T21" s="64">
+        <f>IF(Sheet1!$T27="","",Sheet1!$T27)</f>
+        <v>4000</v>
+      </c>
+      <c r="U21" s="64" t="str">
+        <f>IF(Sheet1!$U27="","",Sheet1!$U27)</f>
+        <v/>
+      </c>
+      <c r="V21" s="64" t="str">
+        <f>IF(Sheet1!$Z27="","",Sheet1!$Z27)</f>
+        <v/>
+      </c>
+      <c r="X21" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A22" s="66"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="30" t="str">
         <f>Sheet1!B27&amp;" weekly"</f>
         <v>8-GPU x86 SERVER P40 weekly</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="27"/>
       <c r="G22" s="27">
@@ -13042,25 +14008,64 @@
         <f>Sheet1!F27*Sheet1!D27</f>
         <v>94.063999999999993</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="14" t="str">
+        <f>Sheet1!$C27</f>
+        <v>P40</v>
+      </c>
+      <c r="M22" s="14">
         <f>Sheet1!$D27</f>
         <v>8</v>
       </c>
-      <c r="M22" s="14" t="str">
-        <f>Sheet1!$C27</f>
-        <v>P40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="60"/>
-      <c r="B23" s="66"/>
+      <c r="N22" s="14" t="str">
+        <f>Sheet1!$K27</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O22" s="14">
+        <f>Sheet1!$L27</f>
+        <v>2</v>
+      </c>
+      <c r="P22" s="14">
+        <f>IF(Sheet1!$P27="","",Sheet1!$P27)</f>
+        <v>256</v>
+      </c>
+      <c r="Q22" s="27" t="str">
+        <f>IF(Sheet1!$Q27="","",Sheet1!$Q27)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R22" s="27">
+        <f>IF(Sheet1!$R27="","",Sheet1!$R27)</f>
+        <v>1000</v>
+      </c>
+      <c r="S22" s="63" t="str">
+        <f>IF(Sheet1!$S27="","",Sheet1!$S27)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T22" s="63">
+        <f>IF(Sheet1!$T27="","",Sheet1!$T27)</f>
+        <v>4000</v>
+      </c>
+      <c r="U22" s="63" t="str">
+        <f>IF(Sheet1!$U27="","",Sheet1!$U27)</f>
+        <v/>
+      </c>
+      <c r="V22" s="63" t="str">
+        <f>IF(Sheet1!$Z27="","",Sheet1!$Z27)</f>
+        <v/>
+      </c>
+      <c r="X22" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="30" t="str">
         <f>Sheet1!B28&amp;" monthly"</f>
         <v>8-GPU x86 SERVER P100 monthly</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
@@ -13077,25 +14082,64 @@
         <f>Sheet1!F28*Sheet1!D28</f>
         <v>76</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="14" t="str">
+        <f>Sheet1!$C28</f>
+        <v>P100</v>
+      </c>
+      <c r="M23" s="14">
         <f>Sheet1!$D28</f>
         <v>8</v>
       </c>
-      <c r="M23" s="14" t="str">
-        <f>Sheet1!$C28</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="60"/>
-      <c r="B24" s="66"/>
+      <c r="N23" s="14" t="str">
+        <f>Sheet1!$K28</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O23" s="14">
+        <f>Sheet1!$L28</f>
+        <v>2</v>
+      </c>
+      <c r="P23" s="14">
+        <f>IF(Sheet1!$P28="","",Sheet1!$P28)</f>
+        <v>256</v>
+      </c>
+      <c r="Q23" s="27" t="str">
+        <f>IF(Sheet1!$Q28="","",Sheet1!$Q28)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R23" s="27">
+        <f>IF(Sheet1!$R28="","",Sheet1!$R28)</f>
+        <v>1000</v>
+      </c>
+      <c r="S23" s="64" t="str">
+        <f>IF(Sheet1!$S28="","",Sheet1!$S28)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T23" s="64">
+        <f>IF(Sheet1!$T28="","",Sheet1!$T28)</f>
+        <v>4000</v>
+      </c>
+      <c r="U23" s="64" t="str">
+        <f>IF(Sheet1!$U28="","",Sheet1!$U28)</f>
+        <v/>
+      </c>
+      <c r="V23" s="64" t="str">
+        <f>IF(Sheet1!$Z28="","",Sheet1!$Z28)</f>
+        <v/>
+      </c>
+      <c r="X23" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A24" s="66"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="30" t="str">
         <f>Sheet1!B28&amp;" weekly"</f>
         <v>8-GPU x86 SERVER P100 weekly</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27">
@@ -13112,25 +14156,64 @@
         <f>Sheet1!F28*Sheet1!D28</f>
         <v>76</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="14" t="str">
+        <f>Sheet1!$C28</f>
+        <v>P100</v>
+      </c>
+      <c r="M24" s="14">
         <f>Sheet1!$D28</f>
         <v>8</v>
       </c>
-      <c r="M24" s="14" t="str">
-        <f>Sheet1!$C28</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="60"/>
-      <c r="B25" s="66"/>
+      <c r="N24" s="14" t="str">
+        <f>Sheet1!$K28</f>
+        <v>Xeon E5-2630 v3</v>
+      </c>
+      <c r="O24" s="14">
+        <f>Sheet1!$L28</f>
+        <v>2</v>
+      </c>
+      <c r="P24" s="14">
+        <f>IF(Sheet1!$P28="","",Sheet1!$P28)</f>
+        <v>256</v>
+      </c>
+      <c r="Q24" s="27" t="str">
+        <f>IF(Sheet1!$Q28="","",Sheet1!$Q28)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R24" s="27">
+        <f>IF(Sheet1!$R28="","",Sheet1!$R28)</f>
+        <v>1000</v>
+      </c>
+      <c r="S24" s="63" t="str">
+        <f>IF(Sheet1!$S28="","",Sheet1!$S28)</f>
+        <v>SATA</v>
+      </c>
+      <c r="T24" s="63">
+        <f>IF(Sheet1!$T28="","",Sheet1!$T28)</f>
+        <v>4000</v>
+      </c>
+      <c r="U24" s="63" t="str">
+        <f>IF(Sheet1!$U28="","",Sheet1!$U28)</f>
+        <v/>
+      </c>
+      <c r="V24" s="63" t="str">
+        <f>IF(Sheet1!$Z28="","",Sheet1!$Z28)</f>
+        <v/>
+      </c>
+      <c r="X24" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A25" s="66"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="30" t="str">
         <f>Sheet1!B29&amp;" monthly"</f>
         <v>4-GPU POWER8/10 SERVER monthly</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
@@ -13147,25 +14230,64 @@
         <f>Sheet1!F29*Sheet1!D29</f>
         <v>38</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="14" t="str">
+        <f>Sheet1!$C29</f>
+        <v>P100</v>
+      </c>
+      <c r="M25" s="14">
         <f>Sheet1!$D29</f>
         <v>4</v>
       </c>
-      <c r="M25" s="14" t="str">
-        <f>Sheet1!$C29</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="20" customHeight="1">
-      <c r="A26" s="60"/>
-      <c r="B26" s="66"/>
+      <c r="N25" s="14" t="str">
+        <f>Sheet1!$K29</f>
+        <v>POWER8</v>
+      </c>
+      <c r="O25" s="14">
+        <f>Sheet1!$L29</f>
+        <v>2</v>
+      </c>
+      <c r="P25" s="14">
+        <f>IF(Sheet1!$P29="","",Sheet1!$P29)</f>
+        <v>1000</v>
+      </c>
+      <c r="Q25" s="27" t="str">
+        <f>IF(Sheet1!$Q29="","",Sheet1!$Q29)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R25" s="27" t="str">
+        <f>IF(Sheet1!$R29="","",Sheet1!$R29)</f>
+        <v>4 x 960</v>
+      </c>
+      <c r="S25" s="64" t="str">
+        <f>IF(Sheet1!$S29="","",Sheet1!$S29)</f>
+        <v/>
+      </c>
+      <c r="T25" s="64" t="str">
+        <f>IF(Sheet1!$T29="","",Sheet1!$T29)</f>
+        <v/>
+      </c>
+      <c r="U25" s="64" t="str">
+        <f>IF(Sheet1!$U29="","",Sheet1!$U29)</f>
+        <v/>
+      </c>
+      <c r="V25" s="64" t="str">
+        <f>IF(Sheet1!$Z29="","",Sheet1!$Z29)</f>
+        <v>Infiniband EDR (24.24Gb/s)</v>
+      </c>
+      <c r="X25" s="13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="20" customHeight="1">
+      <c r="A26" s="66"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="30" t="str">
         <f>Sheet1!B29&amp;" weekly"</f>
         <v>4-GPU POWER8/10 SERVER weekly</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27">
@@ -13182,25 +14304,64 @@
         <f>Sheet1!F29*Sheet1!D29</f>
         <v>38</v>
       </c>
-      <c r="L26" s="14">
+      <c r="L26" s="14" t="str">
+        <f>Sheet1!$C29</f>
+        <v>P100</v>
+      </c>
+      <c r="M26" s="14">
         <f>Sheet1!$D29</f>
         <v>4</v>
       </c>
-      <c r="M26" s="14" t="str">
-        <f>Sheet1!$C29</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A27" s="60"/>
-      <c r="B27" s="66"/>
+      <c r="N26" s="14" t="str">
+        <f>Sheet1!$K29</f>
+        <v>POWER8</v>
+      </c>
+      <c r="O26" s="14">
+        <f>Sheet1!$L29</f>
+        <v>2</v>
+      </c>
+      <c r="P26" s="14">
+        <f>IF(Sheet1!$P29="","",Sheet1!$P29)</f>
+        <v>1000</v>
+      </c>
+      <c r="Q26" s="27" t="str">
+        <f>IF(Sheet1!$Q29="","",Sheet1!$Q29)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R26" s="27" t="str">
+        <f>IF(Sheet1!$R29="","",Sheet1!$R29)</f>
+        <v>4 x 960</v>
+      </c>
+      <c r="S26" s="63" t="str">
+        <f>IF(Sheet1!$S29="","",Sheet1!$S29)</f>
+        <v/>
+      </c>
+      <c r="T26" s="63" t="str">
+        <f>IF(Sheet1!$T29="","",Sheet1!$T29)</f>
+        <v/>
+      </c>
+      <c r="U26" s="63" t="str">
+        <f>IF(Sheet1!$U29="","",Sheet1!$U29)</f>
+        <v/>
+      </c>
+      <c r="V26" s="63" t="str">
+        <f>IF(Sheet1!$Z29="","",Sheet1!$Z29)</f>
+        <v>Infiniband EDR (24.24Gb/s)</v>
+      </c>
+      <c r="X26" s="13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A27" s="66"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="30" t="str">
         <f>Sheet1!B30&amp;" monthly"</f>
         <v>4-GPU POWER8/8 SERVER monthly</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
@@ -13217,25 +14378,64 @@
         <f>Sheet1!F30*Sheet1!D30</f>
         <v>38</v>
       </c>
-      <c r="L27" s="14">
+      <c r="L27" s="14" t="str">
+        <f>Sheet1!$C30</f>
+        <v>P100</v>
+      </c>
+      <c r="M27" s="14">
         <f>Sheet1!$D30</f>
         <v>4</v>
       </c>
-      <c r="M27" s="14" t="str">
-        <f>Sheet1!$C30</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="20" customHeight="1">
-      <c r="A28" s="60"/>
-      <c r="B28" s="66"/>
+      <c r="N27" s="14" t="str">
+        <f>Sheet1!$K30</f>
+        <v>POWER8</v>
+      </c>
+      <c r="O27" s="14">
+        <f>Sheet1!$L30</f>
+        <v>2</v>
+      </c>
+      <c r="P27" s="14">
+        <f>IF(Sheet1!$P30="","",Sheet1!$P30)</f>
+        <v>512</v>
+      </c>
+      <c r="Q27" s="27" t="str">
+        <f>IF(Sheet1!$Q30="","",Sheet1!$Q30)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R27" s="27" t="str">
+        <f>IF(Sheet1!$R30="","",Sheet1!$R30)</f>
+        <v>2 x 960</v>
+      </c>
+      <c r="S27" s="64" t="str">
+        <f>IF(Sheet1!$S30="","",Sheet1!$S30)</f>
+        <v/>
+      </c>
+      <c r="T27" s="64" t="str">
+        <f>IF(Sheet1!$T30="","",Sheet1!$T30)</f>
+        <v/>
+      </c>
+      <c r="U27" s="64" t="str">
+        <f>IF(Sheet1!$U30="","",Sheet1!$U30)</f>
+        <v/>
+      </c>
+      <c r="V27" s="64" t="str">
+        <f>IF(Sheet1!$Z30="","",Sheet1!$Z30)</f>
+        <v/>
+      </c>
+      <c r="X27" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="20" customHeight="1">
+      <c r="A28" s="66"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="30" t="str">
         <f>Sheet1!B30&amp;" weekly"</f>
         <v>4-GPU POWER8/8 SERVER weekly</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F28" s="27"/>
       <c r="G28" s="27">
@@ -13252,22 +14452,61 @@
         <f>Sheet1!F30*Sheet1!D30</f>
         <v>38</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L28" s="14" t="str">
+        <f>Sheet1!$C30</f>
+        <v>P100</v>
+      </c>
+      <c r="M28" s="14">
         <f>Sheet1!$D30</f>
         <v>4</v>
       </c>
-      <c r="M28" s="14" t="str">
-        <f>Sheet1!$C30</f>
-        <v>P100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="20" customHeight="1">
-      <c r="A29" s="60" t="str">
+      <c r="N28" s="14" t="str">
+        <f>Sheet1!$K30</f>
+        <v>POWER8</v>
+      </c>
+      <c r="O28" s="14">
+        <f>Sheet1!$L30</f>
+        <v>2</v>
+      </c>
+      <c r="P28" s="14">
+        <f>IF(Sheet1!$P30="","",Sheet1!$P30)</f>
+        <v>512</v>
+      </c>
+      <c r="Q28" s="27" t="str">
+        <f>IF(Sheet1!$Q30="","",Sheet1!$Q30)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R28" s="27" t="str">
+        <f>IF(Sheet1!$R30="","",Sheet1!$R30)</f>
+        <v>2 x 960</v>
+      </c>
+      <c r="S28" s="63" t="str">
+        <f>IF(Sheet1!$S30="","",Sheet1!$S30)</f>
+        <v/>
+      </c>
+      <c r="T28" s="63" t="str">
+        <f>IF(Sheet1!$T30="","",Sheet1!$T30)</f>
+        <v/>
+      </c>
+      <c r="U28" s="63" t="str">
+        <f>IF(Sheet1!$U30="","",Sheet1!$U30)</f>
+        <v/>
+      </c>
+      <c r="V28" s="63" t="str">
+        <f>IF(Sheet1!$Z30="","",Sheet1!$Z30)</f>
+        <v/>
+      </c>
+      <c r="X28" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="20" customHeight="1">
+      <c r="A29" s="66" t="str">
         <f>Sheet1!A32</f>
         <v>Sakura</v>
       </c>
-      <c r="B29" s="66" t="s">
-        <v>184</v>
+      <c r="B29" s="68" t="s">
+        <v>183</v>
       </c>
       <c r="C29" s="30" t="str">
         <f>Sheet1!B32</f>
@@ -13275,7 +14514,7 @@
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
@@ -13292,25 +14531,64 @@
         <f>Sheet1!F32*Sheet1!D32</f>
         <v>24.576000000000001</v>
       </c>
-      <c r="L29" s="14">
+      <c r="L29" s="14" t="str">
+        <f>Sheet1!$C32</f>
+        <v>GeForce GTX TITAN X</v>
+      </c>
+      <c r="M29" s="14">
         <f>Sheet1!$D32</f>
         <v>4</v>
       </c>
-      <c r="M29" s="14" t="str">
-        <f>Sheet1!$C32</f>
-        <v>GeForce GTX TITAN X</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="20" customHeight="1">
-      <c r="A30" s="60"/>
-      <c r="B30" s="66"/>
+      <c r="N29" s="14" t="str">
+        <f>Sheet1!$K32</f>
+        <v>Xeon E5-2623 v3</v>
+      </c>
+      <c r="O29" s="14">
+        <f>Sheet1!$L32</f>
+        <v>2</v>
+      </c>
+      <c r="P29" s="14">
+        <f>IF(Sheet1!$P32="","",Sheet1!$P32)</f>
+        <v>128</v>
+      </c>
+      <c r="Q29" s="27" t="str">
+        <f>IF(Sheet1!$Q32="","",Sheet1!$Q32)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R29" s="27">
+        <f>IF(Sheet1!$R32="","",Sheet1!$R32)</f>
+        <v>480</v>
+      </c>
+      <c r="S29" s="64" t="str">
+        <f>IF(Sheet1!$S32="","",Sheet1!$S32)</f>
+        <v>SSD</v>
+      </c>
+      <c r="T29" s="64">
+        <f>IF(Sheet1!$T32="","",Sheet1!$T32)</f>
+        <v>480</v>
+      </c>
+      <c r="U29" s="64">
+        <f>IF(Sheet1!$U32="","",Sheet1!$U32)</f>
+        <v>0.1</v>
+      </c>
+      <c r="V29" s="64" t="str">
+        <f>IF(Sheet1!$Z32="","",Sheet1!$Z32)</f>
+        <v>Price includes one-time costs devided by 12 months.</v>
+      </c>
+      <c r="X29" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="20" customHeight="1">
+      <c r="A30" s="66"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="30" t="str">
         <f>Sheet1!$B$33</f>
         <v>Tesla model</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
@@ -13327,13 +14605,52 @@
         <f>Sheet1!F33*Sheet1!D33</f>
         <v>6.8440000000000003</v>
       </c>
-      <c r="L30" s="14">
+      <c r="L30" s="14" t="str">
+        <f>Sheet1!$C33</f>
+        <v>M40</v>
+      </c>
+      <c r="M30" s="14">
         <f>Sheet1!$D33</f>
         <v>1</v>
       </c>
-      <c r="M30" s="14" t="str">
-        <f>Sheet1!$C33</f>
-        <v>M40</v>
+      <c r="N30" s="14" t="str">
+        <f>Sheet1!$K33</f>
+        <v>Xeon E5-2623 v3</v>
+      </c>
+      <c r="O30" s="14">
+        <f>Sheet1!$L33</f>
+        <v>2</v>
+      </c>
+      <c r="P30" s="14">
+        <f>IF(Sheet1!$P33="","",Sheet1!$P33)</f>
+        <v>128</v>
+      </c>
+      <c r="Q30" s="27" t="str">
+        <f>IF(Sheet1!$Q33="","",Sheet1!$Q33)</f>
+        <v>SSD</v>
+      </c>
+      <c r="R30" s="27">
+        <f>IF(Sheet1!$R33="","",Sheet1!$R33)</f>
+        <v>480</v>
+      </c>
+      <c r="S30" s="63" t="str">
+        <f>IF(Sheet1!$S33="","",Sheet1!$S33)</f>
+        <v>SSD</v>
+      </c>
+      <c r="T30" s="63">
+        <f>IF(Sheet1!$T33="","",Sheet1!$T33)</f>
+        <v>480</v>
+      </c>
+      <c r="U30" s="63">
+        <f>IF(Sheet1!$U33="","",Sheet1!$U33)</f>
+        <v>0.1</v>
+      </c>
+      <c r="V30" s="63" t="str">
+        <f>IF(Sheet1!$Z33="","",Sheet1!$Z33)</f>
+        <v>Price includes one-time costs devided by 12 months.</v>
+      </c>
+      <c r="X30" s="13">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -13349,97 +14666,182 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <conditionalFormatting sqref="C18:G18 I18:K18 C22:G22 I22:K22 C21:K21 C24:D24 I24:K24 C26:G26 I26:K26 C29:K30 C28:D28 I28:K28 H22:H28 C20:D20 F20:K20 F24:G24 F28:G28 C2:K17">
-    <cfRule type="expression" dxfId="29" priority="19">
+    <cfRule type="expression" dxfId="35" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:K19">
-    <cfRule type="expression" dxfId="28" priority="18">
+    <cfRule type="expression" dxfId="34" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:G23 I23:K23">
-    <cfRule type="expression" dxfId="27" priority="17">
+    <cfRule type="expression" dxfId="33" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:G25 I25:K25">
-    <cfRule type="expression" dxfId="26" priority="16">
+    <cfRule type="expression" dxfId="32" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:G27 I27:K27">
-    <cfRule type="expression" dxfId="25" priority="15">
+    <cfRule type="expression" dxfId="31" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="24" priority="14">
+    <cfRule type="expression" dxfId="30" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="expression" dxfId="23" priority="9">
+  <conditionalFormatting sqref="M27">
+    <cfRule type="expression" dxfId="29" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L18 L20:L22 L24 L26 L28:L30">
-    <cfRule type="expression" dxfId="22" priority="13">
+  <conditionalFormatting sqref="M2:M18 M20:M22 M24 M26 M28:M30">
+    <cfRule type="expression" dxfId="28" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="expression" dxfId="21" priority="12">
+  <conditionalFormatting sqref="M19">
+    <cfRule type="expression" dxfId="27" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L23">
-    <cfRule type="expression" dxfId="20" priority="11">
+  <conditionalFormatting sqref="M23">
+    <cfRule type="expression" dxfId="26" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L25">
-    <cfRule type="expression" dxfId="19" priority="10">
+  <conditionalFormatting sqref="M25">
+    <cfRule type="expression" dxfId="25" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="24" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="17" priority="7">
+    <cfRule type="expression" dxfId="23" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="22" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M7">
-    <cfRule type="expression" dxfId="13" priority="5">
+  <conditionalFormatting sqref="L2:L7">
+    <cfRule type="expression" dxfId="21" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:M11">
-    <cfRule type="expression" dxfId="10" priority="4">
+  <conditionalFormatting sqref="L8:M11">
+    <cfRule type="expression" dxfId="20" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
-    <cfRule type="expression" dxfId="7" priority="3">
+  <conditionalFormatting sqref="L12:M12">
+    <cfRule type="expression" dxfId="19" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M13:M28">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="L13:M28">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M29:M30">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="L29:M30">
+    <cfRule type="expression" dxfId="17" priority="33">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N7">
+    <cfRule type="expression" dxfId="16" priority="27">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:N11">
+    <cfRule type="expression" dxfId="15" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12">
+    <cfRule type="expression" dxfId="14" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13:N28">
+    <cfRule type="expression" dxfId="13" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N30">
+    <cfRule type="expression" dxfId="12" priority="23">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P7">
+    <cfRule type="expression" dxfId="11" priority="22">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P8:P11">
+    <cfRule type="expression" dxfId="10" priority="21">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P13:P28">
+    <cfRule type="expression" dxfId="9" priority="19">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P29:P30">
+    <cfRule type="expression" dxfId="8" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q30">
+    <cfRule type="expression" dxfId="7" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P12">
+    <cfRule type="expression" dxfId="6" priority="12">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R30">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O7">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8:O11">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13:O28">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O29:O30">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13451,13 +14853,14 @@
     <hyperlink ref="D3:D4" r:id="rId5" display="https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22240"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="J20:K20" formula="1"/>
+    <ignoredError sqref="Q2 R2:S4 Q3:Q4 Q5:Q7 R5:S7 P8:S28 P5:P7 T3:U3 T5:V28 T4:U4 T2:U2" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="70"/>
     </ext>
   </extLst>
 </worksheet>
@@ -13465,13 +14868,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CM338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
@@ -13574,191 +14977,191 @@
   <sheetData>
     <row r="1" spans="1:91" s="14" customFormat="1" ht="21" customHeight="1" thickBot="1">
       <c r="A1" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="65" t="str">
+        <v>144</v>
+      </c>
+      <c r="E1" s="72" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$C$2</f>
         <v>Amazon p2.16xlarge on-demand</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="63" t="str">
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="70" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$C$3</f>
         <v>Amazon p2.8xlarge on-demand</v>
       </c>
-      <c r="I1" s="63"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="62" t="str">
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="69" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$C$4</f>
         <v>Amazon p2.xlarge on-demand</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="62" t="str">
+      <c r="L1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="69" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$C$5</f>
         <v>Amazon p2 dedicated host On-demand</v>
       </c>
-      <c r="O1" s="63"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="62" t="str">
+      <c r="O1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="69" t="str">
         <f>'cost-performance'!$A$2&amp;" "&amp;'cost-performance'!$C$6</f>
         <v>Amazon p2 dedicated host 1 year no Upfront</v>
       </c>
-      <c r="R1" s="63"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="62" t="str">
+      <c r="R1" s="70"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="69" t="str">
         <f>'cost-performance'!A2&amp;" "&amp;'cost-performance'!C7</f>
         <v>Amazon p2 dedicated host 1 year 100% Upfront</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="62" t="str">
+      <c r="U1" s="70"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="69" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$C$8</f>
         <v>Softlayer NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4 hourly</v>
       </c>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="62" t="str">
+      <c r="X1" s="70"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="69" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$C$9</f>
         <v>Softlayer NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4 monthly</v>
       </c>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="62" t="str">
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="69" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$C$10</f>
         <v>Softlayer NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</v>
       </c>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="62" t="str">
+      <c r="AD1" s="70"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="69" t="str">
         <f>'cost-performance'!$A$8&amp;" "&amp;'cost-performance'!$C$11</f>
         <v>Softlayer NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</v>
       </c>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="64"/>
-      <c r="AI1" s="62" t="str">
+      <c r="AG1" s="70"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="69" t="str">
         <f>'cost-performance'!$A$12&amp;" "&amp;'cost-performance'!$C$12</f>
         <v>Nimbix NGD5</v>
       </c>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="62" t="str">
+      <c r="AJ1" s="70"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$13</f>
         <v>Cirrascale 16-GPU x86 SERVER K80 monthly</v>
       </c>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="62" t="str">
+      <c r="AM1" s="70"/>
+      <c r="AN1" s="71"/>
+      <c r="AO1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$14</f>
         <v>Cirrascale 16-GPU x86 SERVER K80 weekly</v>
       </c>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="62" t="str">
+      <c r="AP1" s="70"/>
+      <c r="AQ1" s="71"/>
+      <c r="AR1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$15</f>
         <v>Cirrascale 8-GPU x86 SERVER M40 monthly</v>
       </c>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="62" t="str">
+      <c r="AS1" s="70"/>
+      <c r="AT1" s="71"/>
+      <c r="AU1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$16</f>
         <v>Cirrascale 8-GPU x86 SERVER M40 weekly</v>
       </c>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="62" t="str">
+      <c r="AV1" s="70"/>
+      <c r="AW1" s="71"/>
+      <c r="AX1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$17</f>
         <v>Cirrascale 8-GPU x86 SERVER monthly</v>
       </c>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="62" t="str">
+      <c r="AY1" s="70"/>
+      <c r="AZ1" s="71"/>
+      <c r="BA1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$18</f>
         <v>Cirrascale 8-GPU x86 SERVER weekly</v>
       </c>
-      <c r="BB1" s="63"/>
-      <c r="BC1" s="64"/>
-      <c r="BD1" s="62" t="str">
+      <c r="BB1" s="70"/>
+      <c r="BC1" s="71"/>
+      <c r="BD1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$19</f>
         <v>Cirrascale 4-GPU x86 SERVER monthly</v>
       </c>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="64"/>
-      <c r="BG1" s="62" t="str">
+      <c r="BE1" s="70"/>
+      <c r="BF1" s="71"/>
+      <c r="BG1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$20</f>
         <v>Cirrascale 4-GPU x86 SERVER weekly</v>
       </c>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="64"/>
-      <c r="BJ1" s="62" t="str">
+      <c r="BH1" s="70"/>
+      <c r="BI1" s="71"/>
+      <c r="BJ1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$21</f>
         <v>Cirrascale 8-GPU x86 SERVER P40 monthly</v>
       </c>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="64"/>
-      <c r="BM1" s="62" t="str">
+      <c r="BK1" s="70"/>
+      <c r="BL1" s="71"/>
+      <c r="BM1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$22</f>
         <v>Cirrascale 8-GPU x86 SERVER P40 weekly</v>
       </c>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="64"/>
-      <c r="BP1" s="62" t="str">
+      <c r="BN1" s="70"/>
+      <c r="BO1" s="71"/>
+      <c r="BP1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$23</f>
         <v>Cirrascale 8-GPU x86 SERVER P100 monthly</v>
       </c>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="64"/>
-      <c r="BS1" s="62" t="str">
+      <c r="BQ1" s="70"/>
+      <c r="BR1" s="71"/>
+      <c r="BS1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$24</f>
         <v>Cirrascale 8-GPU x86 SERVER P100 weekly</v>
       </c>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="64"/>
-      <c r="BV1" s="62" t="str">
+      <c r="BT1" s="70"/>
+      <c r="BU1" s="71"/>
+      <c r="BV1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$25</f>
         <v>Cirrascale 4-GPU POWER8/10 SERVER monthly</v>
       </c>
-      <c r="BW1" s="63"/>
-      <c r="BX1" s="64"/>
-      <c r="BY1" s="62" t="str">
+      <c r="BW1" s="70"/>
+      <c r="BX1" s="71"/>
+      <c r="BY1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$26</f>
         <v>Cirrascale 4-GPU POWER8/10 SERVER weekly</v>
       </c>
-      <c r="BZ1" s="63"/>
-      <c r="CA1" s="64"/>
-      <c r="CB1" s="62" t="str">
+      <c r="BZ1" s="70"/>
+      <c r="CA1" s="71"/>
+      <c r="CB1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$27</f>
         <v>Cirrascale 4-GPU POWER8/8 SERVER monthly</v>
       </c>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="64"/>
-      <c r="CE1" s="62" t="str">
+      <c r="CC1" s="70"/>
+      <c r="CD1" s="71"/>
+      <c r="CE1" s="69" t="str">
         <f>'cost-performance'!$A$13&amp;" "&amp;'cost-performance'!$C$28</f>
         <v>Cirrascale 4-GPU POWER8/8 SERVER weekly</v>
       </c>
-      <c r="CF1" s="63"/>
-      <c r="CG1" s="64"/>
-      <c r="CH1" s="62" t="str">
+      <c r="CF1" s="70"/>
+      <c r="CG1" s="71"/>
+      <c r="CH1" s="69" t="str">
         <f>'cost-performance'!$A$29&amp;" "&amp;'cost-performance'!$C$29</f>
         <v>Sakura Quad GPU model</v>
       </c>
-      <c r="CI1" s="63"/>
-      <c r="CJ1" s="64"/>
-      <c r="CK1" s="62" t="str">
+      <c r="CI1" s="70"/>
+      <c r="CJ1" s="71"/>
+      <c r="CK1" s="69" t="str">
         <f>'cost-performance'!$A$29&amp;" "&amp;'cost-performance'!$C$30</f>
         <v>Sakura Tesla model</v>
       </c>
-      <c r="CL1" s="63"/>
-      <c r="CM1" s="64"/>
+      <c r="CL1" s="70"/>
+      <c r="CM1" s="71"/>
     </row>
     <row r="2" spans="1:91" ht="20" thickTop="1" thickBot="1">
       <c r="A2" s="23"/>
@@ -13766,265 +15169,265 @@
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
       <c r="E2" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="J2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="K2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="M2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="N2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="Q2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="S2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="T2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="U2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="W2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="X2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="Y2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="Z2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AA2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AB2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AC2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AD2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AE2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AF2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AG2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AH2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AI2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AJ2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AK2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AL2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AM2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AN2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AO2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AP2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AQ2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AQ2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AR2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AS2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AT2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AU2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AV2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AW2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="AX2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AY2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="AZ2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BA2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BB2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BC2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BC2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BD2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BE2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BF2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BF2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BG2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BH2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BI2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BJ2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BK2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BL2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BL2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BM2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BN2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BO2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BO2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BP2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BQ2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BR2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BR2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BS2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BT2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BU2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BV2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BW2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="BX2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="BX2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="BY2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BZ2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="CA2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="CA2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="CB2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="CC2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="CD2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="CD2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="CE2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="CF2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="CG2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="CG2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="CH2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="CI2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="CJ2" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="CJ2" s="42" t="s">
-        <v>98</v>
-      </c>
       <c r="CK2" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="CL2" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="CM2" s="42" t="s">
         <v>97</v>
-      </c>
-      <c r="CM2" s="42" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:91" ht="19" thickTop="1">
@@ -36634,6 +38037,26 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="CB1:CD1"/>
+    <mergeCell ref="CE1:CG1"/>
+    <mergeCell ref="CH1:CJ1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="BM1:BO1"/>
+    <mergeCell ref="BP1:BR1"/>
+    <mergeCell ref="BS1:BU1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="BY1:CA1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="BD1:BF1"/>
+    <mergeCell ref="BG1:BI1"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="AL1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AU1:AW1"/>
+    <mergeCell ref="AR1:AT1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -36643,26 +38066,6 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="T1:V1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="AO1:AQ1"/>
-    <mergeCell ref="AU1:AW1"/>
-    <mergeCell ref="AR1:AT1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="BD1:BF1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="BJ1:BL1"/>
-    <mergeCell ref="CB1:CD1"/>
-    <mergeCell ref="CE1:CG1"/>
-    <mergeCell ref="CH1:CJ1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="BM1:BO1"/>
-    <mergeCell ref="BP1:BR1"/>
-    <mergeCell ref="BS1:BU1"/>
-    <mergeCell ref="BV1:BX1"/>
-    <mergeCell ref="BY1:CA1"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated offers and added legend and descriptions.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48920" windowHeight="17320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="48920" windowHeight="16360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,9 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-Cost includes One-time cost (初期費用) divided by 12 month (793 800 / 12 = 66 150 yen/month) Yen monthly price is 157 950. Used Yen to USD rate  104 yen/USD.</t>
+Cost includes One-time cost (初期費用) divided by 12 months (880 200 / 12 = 73 350 yen/month) Yen Monthly price is 100 440. 
+Total monthly cost: 100 440 + 73 350 = 173 790￥ （税込）
+Used Yen to USD rate  118 yen/USD. (Rate on 2016/12/16)</t>
         </r>
       </text>
     </comment>
@@ -543,7 +545,41 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-Cost includes One-time cost (初期費用) divided by 12 month 868 600 / 12 = 71 550 yen/month) Montly sum in Yen: 174 150. Yen to USD rate  104 yen/USD.</t>
+Cost includes One-time cost (初期費用) divided by 12 months
+945 000 / 12 = 78 750 yen/month) 
+Montly price: 104 760.
+Montly sum: 104 760 + 78 750 = 183 510￥　（税込）. 
+Yen to USD rate  118 yen/USD on 2016/12/16.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+Cost includes One-time cost (初期費用) divided by 12 months
+966 600 / 12 = 80 550 yen/month) 
+Montly price: 106 920.
+Montly sum: 106 920 + 80 550 = 187 470¥　（税込）. 
+Yen to USD rate  118 yen/USD on 2016/12/16.</t>
         </r>
       </text>
     </comment>
@@ -552,7 +588,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="220">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -765,10 +801,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>GeForce GTX TITAN X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>processors/shaders xN</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -831,10 +863,6 @@
     <t>https://www.sakura.ad.jp/koukaryoku/specification/</t>
   </si>
   <si>
-    <t>Tesla model</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>SSD</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1087,10 +1115,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>SK M40x1 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>per year USD</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1396,6 +1420,34 @@
   </si>
   <si>
     <t>CR P100x2 P8/8 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NVIDIA TITAN X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Tesla P40 model</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Tesla P100 model</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK P40x1 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Price includes one-time costs devided by 12 months.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK P100x1 m.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1793,7 +1845,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="604">
+  <cellStyleXfs count="609">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2397,6 +2449,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2509,6 +2566,15 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="594"/>
     <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="594" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="119" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="594" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2527,17 +2593,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="120" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="119" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="594" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="604">
+  <cellStyles count="609">
     <cellStyle name="Calculation" xfId="343" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="345" builtinId="23" hidden="1"/>
     <cellStyle name="comment" xfId="120"/>
@@ -2848,6 +2905,11 @@
     <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -3143,7 +3205,117 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3703,13 +3875,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EY32"/>
+  <dimension ref="A1:EY33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z16" sqref="Z16"/>
+      <selection pane="bottomRight" activeCell="Z34" sqref="Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3753,52 +3925,52 @@
     <row r="3" spans="1:155" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
       <c r="J3" s="25"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
       <c r="P3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="62"/>
       <c r="U3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="59" t="s">
+      <c r="V3" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
+      <c r="W3" s="62"/>
+      <c r="X3" s="62"/>
       <c r="Y3" s="34"/>
       <c r="Z3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AD3"/>
       <c r="AE3"/>
@@ -3937,13 +4109,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>21</v>
@@ -3952,7 +4124,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>4</v>
@@ -3964,7 +4136,7 @@
         <v>6</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>10</v>
@@ -3991,23 +4163,23 @@
         <v>15</v>
       </c>
       <c r="W4" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="X4" s="18" t="s">
         <v>24</v>
       </c>
       <c r="Y4" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Z4" s="18"/>
       <c r="AA4" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AB4" s="18" t="s">
         <v>47</v>
       </c>
       <c r="AC4" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:155" s="13" customFormat="1" ht="21" thickTop="1">
@@ -4040,7 +4212,7 @@
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L5" s="14">
         <v>64</v>
@@ -4071,7 +4243,7 @@
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AA5" s="26">
         <f>X5/(D5*F5)</f>
@@ -4088,7 +4260,7 @@
     </row>
     <row r="6" spans="1:155">
       <c r="A6" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>49</v>
@@ -4147,7 +4319,7 @@
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AA6" s="26">
         <f t="shared" ref="AA6:AA15" si="2">X6/(D6*F6)</f>
@@ -4220,7 +4392,7 @@
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AA7" s="26">
         <f t="shared" si="2"/>
@@ -4237,10 +4409,10 @@
     </row>
     <row r="8" spans="1:155">
       <c r="A8" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>25</v>
@@ -4293,7 +4465,7 @@
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AA8" s="26">
         <f t="shared" si="2"/>
@@ -4311,7 +4483,7 @@
     <row r="9" spans="1:155">
       <c r="A9" s="16"/>
       <c r="B9" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>17</v>
@@ -4383,7 +4555,7 @@
     <row r="10" spans="1:155">
       <c r="A10" s="16"/>
       <c r="B10" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>17</v>
@@ -4392,7 +4564,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -4401,10 +4573,10 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="5" t="s">
@@ -4455,7 +4627,7 @@
     <row r="11" spans="1:155">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>17</v>
@@ -4464,7 +4636,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -4473,10 +4645,10 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="5" t="s">
@@ -4560,7 +4732,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>30</v>
@@ -4626,7 +4798,7 @@
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AA13" s="26">
         <f>X13/(D13*F13)</f>
@@ -4643,13 +4815,13 @@
     </row>
     <row r="14" spans="1:155">
       <c r="A14" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -4671,7 +4843,7 @@
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L14" s="5">
         <v>2</v>
@@ -4689,7 +4861,7 @@
         <v>64</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R14" s="5">
         <v>1000</v>
@@ -4709,7 +4881,7 @@
       </c>
       <c r="Y14" s="26"/>
       <c r="Z14" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AA14" s="26">
         <f t="shared" si="2"/>
@@ -4727,16 +4899,16 @@
     <row r="15" spans="1:155">
       <c r="A15" s="16"/>
       <c r="B15" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F15" s="9">
         <v>9.65</v>
@@ -4745,14 +4917,14 @@
         <v>0.3</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L15" s="5">
         <v>2</v>
@@ -4770,7 +4942,7 @@
         <v>64</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R15" s="5">
         <v>1000</v>
@@ -4790,7 +4962,7 @@
       </c>
       <c r="Y15" s="26"/>
       <c r="Z15" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AA15" s="26">
         <f t="shared" si="2"/>
@@ -4849,7 +5021,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F17" s="9">
         <v>8.74</v>
@@ -4858,7 +5030,7 @@
         <v>2.91</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>22</v>
@@ -4895,7 +5067,7 @@
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA17" s="26">
         <f>X17/(D17*F17)</f>
@@ -4913,10 +5085,10 @@
     <row r="18" spans="1:155" s="13" customFormat="1" ht="20">
       <c r="A18" s="40"/>
       <c r="B18" s="41" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D18" s="29">
         <v>2</v>
@@ -4938,7 +5110,7 @@
       </c>
       <c r="J18" s="30"/>
       <c r="K18" s="42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L18" s="29">
         <v>2</v>
@@ -4968,7 +5140,7 @@
       </c>
       <c r="Y18" s="45"/>
       <c r="Z18" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA18" s="26">
         <f>X18/(D18*F18)</f>
@@ -5111,10 +5283,10 @@
     </row>
     <row r="19" spans="1:155">
       <c r="A19" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>37</v>
@@ -5168,7 +5340,7 @@
     </row>
     <row r="20" spans="1:155">
       <c r="A20" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="31"/>
@@ -5199,7 +5371,7 @@
     </row>
     <row r="21" spans="1:155">
       <c r="A21" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="31"/>
@@ -5261,7 +5433,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>17</v>
@@ -5343,10 +5515,10 @@
     </row>
     <row r="24" spans="1:155">
       <c r="A24" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>43</v>
@@ -5429,10 +5601,10 @@
     <row r="25" spans="1:155" s="13" customFormat="1">
       <c r="A25" s="2"/>
       <c r="B25" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>112</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>114</v>
       </c>
       <c r="D25" s="13">
         <v>8</v>
@@ -5472,13 +5644,13 @@
         <v>256</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R25" s="14">
         <v>1000</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="T25" s="14">
         <v>4000</v>
@@ -5512,10 +5684,10 @@
     <row r="26" spans="1:155" s="13" customFormat="1">
       <c r="A26" s="2"/>
       <c r="B26" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="31" t="s">
         <v>113</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>115</v>
       </c>
       <c r="D26" s="13">
         <v>8</v>
@@ -5537,7 +5709,7 @@
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L26" s="5">
         <v>2</v>
@@ -5555,13 +5727,13 @@
         <v>256</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R26" s="14">
         <v>1000</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T26" s="14">
         <v>4000</v>
@@ -5594,10 +5766,10 @@
     </row>
     <row r="27" spans="1:155">
       <c r="B27" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>94</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>96</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -5639,10 +5811,10 @@
         <v>1000</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R27" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
@@ -5659,7 +5831,7 @@
       </c>
       <c r="Y27" s="26"/>
       <c r="Z27" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AA27" s="26">
         <f t="shared" si="4"/>
@@ -5676,10 +5848,10 @@
     </row>
     <row r="28" spans="1:155">
       <c r="B28" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="31" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>97</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -5724,7 +5896,7 @@
         <v>33</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
@@ -5757,10 +5929,10 @@
     <row r="29" spans="1:155" s="13" customFormat="1">
       <c r="A29" s="48"/>
       <c r="B29" s="49" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D29" s="51">
         <v>2</v>
@@ -5784,7 +5956,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -5995,29 +6167,29 @@
         <v>52</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>53</v>
+        <v>213</v>
       </c>
       <c r="D31">
         <v>4</v>
       </c>
       <c r="E31" s="14">
-        <v>3072</v>
+        <v>3584</v>
       </c>
       <c r="F31" s="21">
-        <v>6.1440000000000001</v>
+        <v>10.157</v>
       </c>
       <c r="G31" s="21">
-        <v>0.192</v>
+        <v>0.317</v>
       </c>
       <c r="H31" s="14">
-        <v>12.3</v>
+        <v>12</v>
       </c>
       <c r="I31" s="14">
-        <v>336</v>
+        <v>480</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L31" s="5">
         <v>2</v>
@@ -6035,13 +6207,13 @@
         <v>128</v>
       </c>
       <c r="Q31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R31" s="5">
         <v>480</v>
       </c>
       <c r="S31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T31" s="5">
         <v>480</v>
@@ -6051,60 +6223,60 @@
       </c>
       <c r="V31" s="10" t="str">
         <f>USDOLLAR(X31/730,2)&amp;"?"</f>
-        <v>$2.08?</v>
+        <v>$2.02?</v>
       </c>
       <c r="W31" s="26"/>
       <c r="X31" s="26">
-        <v>1519</v>
+        <v>1472.8</v>
       </c>
       <c r="Y31" s="26"/>
       <c r="Z31" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA31" s="26">
         <f>X31/(D31*F31)</f>
-        <v>61.808268229166664</v>
+        <v>36.250861474844932</v>
       </c>
       <c r="AB31" s="5">
         <f>D31*F31*1000/X31</f>
-        <v>16.179065174456881</v>
+        <v>27.585551330798481</v>
       </c>
       <c r="AC31" s="26">
         <f>X31/(L31*N31)</f>
-        <v>5063.3333333333339</v>
+        <v>4909.333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:155">
       <c r="A32" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>70</v>
+        <v>214</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" s="14">
-        <v>3072</v>
-      </c>
-      <c r="F32" s="5">
-        <v>6.8440000000000003</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0.214</v>
-      </c>
-      <c r="H32" s="7">
-        <v>12.3</v>
-      </c>
-      <c r="I32" s="7">
-        <v>288</v>
+        <v>3840</v>
+      </c>
+      <c r="F32" s="21">
+        <v>11.757999999999999</v>
+      </c>
+      <c r="G32" s="21">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="H32" s="14">
+        <v>24.576000000000001</v>
+      </c>
+      <c r="I32" s="14">
+        <v>345.6</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L32" s="5">
         <v>2</v>
@@ -6122,7 +6294,7 @@
         <v>128</v>
       </c>
       <c r="Q32" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R32" s="5">
         <v>480</v>
@@ -6138,27 +6310,108 @@
       </c>
       <c r="V32" s="10" t="str">
         <f>USDOLLAR(X32/730,2)&amp;"?"</f>
-        <v>$2.29?</v>
+        <v>$2.13?</v>
       </c>
       <c r="W32" s="26"/>
       <c r="X32" s="26">
-        <v>1675</v>
+        <v>1555</v>
       </c>
       <c r="Y32" s="26"/>
       <c r="Z32" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA32" s="26">
         <f>X32/(D32*F32)</f>
-        <v>244.73991817650494</v>
+        <v>132.25038271814935</v>
       </c>
       <c r="AB32" s="5">
         <f>D32*F32*1000/X32</f>
-        <v>4.0859701492537317</v>
+        <v>7.5614147909967846</v>
       </c>
       <c r="AC32" s="26">
         <f>X32/(L32*N32)</f>
-        <v>5583.3333333333339</v>
+        <v>5183.3333333333339</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29">
+      <c r="B33" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="37">
+        <v>3584</v>
+      </c>
+      <c r="F33" s="50">
+        <v>9.5</v>
+      </c>
+      <c r="G33" s="50">
+        <v>4.7</v>
+      </c>
+      <c r="H33" s="50">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I33" s="50">
+        <v>720</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33" s="5">
+        <v>2</v>
+      </c>
+      <c r="M33" s="5">
+        <v>4</v>
+      </c>
+      <c r="N33" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="O33" s="5">
+        <v>1866</v>
+      </c>
+      <c r="P33" s="5">
+        <v>128</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R33" s="5">
+        <v>480</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T33" s="5">
+        <v>480</v>
+      </c>
+      <c r="U33" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="V33" s="10" t="str">
+        <f>USDOLLAR(X33/730,2)&amp;"?"</f>
+        <v>$2.18?</v>
+      </c>
+      <c r="X33" s="26">
+        <v>1588.7</v>
+      </c>
+      <c r="Z33" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA33" s="26">
+        <f>X33/(D33*F33)</f>
+        <v>167.23157894736843</v>
+      </c>
+      <c r="AB33" s="5">
+        <f>D33*F33*1000/X33</f>
+        <v>5.9797318562346575</v>
+      </c>
+      <c r="AC33" s="26">
+        <f>X33/(L33*N33)</f>
+        <v>5295.666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -6170,7 +6423,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AA31">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6182,7 +6435,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB31">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6193,8 +6446,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="AA32:AA33">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6205,8 +6458,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB32">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="AB32:AB33">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6217,8 +6470,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA32">
-    <cfRule type="colorScale" priority="21">
+  <conditionalFormatting sqref="AA32:AA33">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6229,8 +6482,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB32">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="AB32:AB33">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6241,13 +6494,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13:W13 Z13:XFD13 EZ18:XFD18 AA18:AC18 A19:XFD25 A30:XFD32 EZ29:XFD29 V29 V28:XFD28 S28:U29 R28 Q28:Q29 P28 O28:O29 N28 L26:M29 N26:XFD27 A26:K28 A5:XFD12 A14:XFD17">
-    <cfRule type="expression" dxfId="23" priority="14">
+  <conditionalFormatting sqref="A13:W13 Z13:XFD13 EZ18:XFD18 AA18:AC18 A19:XFD25 EZ29:XFD29 V29 V28:XFD28 S28:U29 R28 Q28:Q29 P28 O28:O29 N28 L26:M29 N26:XFD27 A26:K28 A5:XFD12 A14:XFD17 A30:XFD32 Z33:AC33 V33">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA30:AA32 AA5:AA28">
-    <cfRule type="colorScale" priority="69">
+  <conditionalFormatting sqref="AA5:AA28 AA30:AA33">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6258,8 +6511,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB30:AB32 AB5:AB28">
-    <cfRule type="colorScale" priority="71">
+  <conditionalFormatting sqref="AB5:AB28 AB30:AB33">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6271,7 +6524,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA30:AA31 AA5:AA28">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6283,7 +6536,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30:AB31 AB5:AB28">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6294,8 +6547,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC30:AC32 AC5:AC28">
-    <cfRule type="colorScale" priority="88">
+  <conditionalFormatting sqref="AC5:AC28 AC30:AC33">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6307,12 +6560,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA5:AA28">
-    <cfRule type="colorScale" priority="94">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6324,7 +6577,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB28">
-    <cfRule type="colorScale" priority="96">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6333,6 +6586,21 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K33:U33">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X33">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -6349,13 +6617,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -6383,148 +6651,148 @@
     <col min="23" max="23" width="7.33203125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="67" customFormat="1">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66" t="s">
+    <row r="1" spans="1:24" s="61" customFormat="1">
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="N1" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66" t="s">
+      <c r="O1" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="P1" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="N1" s="66" t="s">
+      <c r="Q1" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="O1" s="66" t="s">
+      <c r="R1" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="P1" s="66" t="s">
+      <c r="S1" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="Q1" s="66" t="s">
+      <c r="T1" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="R1" s="66" t="s">
+      <c r="U1" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="S1" s="66" t="s">
+      <c r="V1" s="60" t="s">
         <v>192</v>
-      </c>
-      <c r="T1" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="U1" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="V1" s="66" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="12" customFormat="1" ht="21" thickBot="1">
       <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L2" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="P2" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="M2" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="S2" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="T2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="U2" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="V2" s="36" t="s">
         <v>162</v>
-      </c>
-      <c r="T2" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="U2" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="V2" s="36" t="s">
-        <v>165</v>
       </c>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" thickTop="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>139</v>
+      <c r="B3" s="65" t="s">
+        <v>136</v>
       </c>
       <c r="C3" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>p2.16xlarge on-demand</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F3" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -6593,17 +6861,17 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="20" customHeight="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="24" t="str">
         <f t="shared" ref="C4:C14" ca="1" si="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>p2.8xlarge on-demand</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F4" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -6616,15 +6884,15 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="14">
-        <f t="shared" ref="J4:J30" ca="1" si="2">INDIRECT("Sheet1!N"&amp; INDIRECT("X"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("X"&amp;ROW()))</f>
+        <f t="shared" ref="J4:J31" ca="1" si="2">INDIRECT("Sheet1!N"&amp; INDIRECT("X"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("X"&amp;ROW()))</f>
         <v>0.35555555555555557</v>
       </c>
       <c r="K4" s="14">
-        <f t="shared" ref="K4:K30" ca="1" si="3">INDIRECT("Sheet1!F"&amp; INDIRECT("X"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("X"&amp;ROW()))</f>
+        <f t="shared" ref="K4:K31" ca="1" si="3">INDIRECT("Sheet1!F"&amp; INDIRECT("X"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("X"&amp;ROW()))</f>
         <v>69.92</v>
       </c>
       <c r="L4" s="14" t="str">
-        <f t="shared" ref="L4:T30" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
+        <f t="shared" ref="L4:T31" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="M4" s="14">
@@ -6672,17 +6940,17 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="20" customHeight="1">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>p2.xlarge on-demand</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F5" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -6751,17 +7019,17 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="20" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>p2 dedicated host On-demand</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F6" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -6830,17 +7098,17 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="20" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>p2 dedicated host 1 year no Upfront</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -6906,17 +7174,17 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="20" customHeight="1">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>p2 dedicated host 1 year 100% Upfront</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
@@ -6982,12 +7250,12 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="20" customHeight="1">
-      <c r="A9" s="61" t="str">
+      <c r="A9" s="64" t="str">
         <f>Sheet1!$A$13</f>
         <v>Softlayer</v>
       </c>
-      <c r="B9" s="62" t="s">
-        <v>140</v>
+      <c r="B9" s="65" t="s">
+        <v>137</v>
       </c>
       <c r="C9" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW())) &amp; " monthly"</f>
@@ -6995,7 +7263,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -7061,15 +7329,15 @@
       </c>
     </row>
     <row r="10" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="61"/>
-      <c r="B10" s="62"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW())) &amp; " hourly"</f>
         <v>NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4 hourly</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F10" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -7135,15 +7403,15 @@
       </c>
     </row>
     <row r="11" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="62"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -7209,15 +7477,15 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="20" customHeight="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="62"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
@@ -7288,7 +7556,7 @@
         <v>Nimbix</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C13" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7296,7 +7564,7 @@
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F13" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -7368,7 +7636,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F14" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -7429,12 +7697,12 @@
       </c>
     </row>
     <row r="15" spans="1:24" s="13" customFormat="1">
-      <c r="A15" s="63" t="str">
+      <c r="A15" s="66" t="str">
         <f>Sheet1!A23</f>
         <v>Cirrascale</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>142</v>
+      <c r="B15" s="67" t="s">
+        <v>139</v>
       </c>
       <c r="C15" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
@@ -7442,7 +7710,7 @@
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
@@ -7509,15 +7777,15 @@
       </c>
     </row>
     <row r="16" spans="1:24" s="13" customFormat="1" ht="19" customHeight="1">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " weekly"</f>
         <v>16-GPU x86 SERVER K80 weekly</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21">
@@ -7584,15 +7852,15 @@
       </c>
     </row>
     <row r="17" spans="1:24" ht="20" customHeight="1">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>8-GPU x86 SERVER M40 monthly</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
@@ -7659,15 +7927,15 @@
       </c>
     </row>
     <row r="18" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>8-GPU x86 SERVER M40 weekly</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21">
@@ -7734,15 +8002,15 @@
       </c>
     </row>
     <row r="19" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="63"/>
-      <c r="B19" s="64"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>8-GPU x86 SERVER P40 monthly</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -7809,15 +8077,15 @@
       </c>
     </row>
     <row r="20" spans="1:24" ht="20" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>8-GPU x86 SERVER P40 weekly</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21">
@@ -7884,15 +8152,15 @@
       </c>
     </row>
     <row r="21" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>8-GPU x86 SERVER P100 monthly</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -7946,11 +8214,11 @@
         <v>4000</v>
       </c>
       <c r="U21" s="14">
-        <f t="shared" ref="U21:U30" ca="1" si="7">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
+        <f t="shared" ref="U21:U31" ca="1" si="7">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="V21" s="16">
-        <f t="shared" ref="V21:V30" ca="1" si="8">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
+        <f t="shared" ref="V21:V31" ca="1" si="8">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="W21" s="16"/>
@@ -7959,15 +8227,15 @@
       </c>
     </row>
     <row r="22" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>8-GPU x86 SERVER P100 weekly</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21">
@@ -8034,15 +8302,15 @@
       </c>
     </row>
     <row r="23" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>4-GPU POWER8/10 SERVER monthly</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
@@ -8109,15 +8377,15 @@
       </c>
     </row>
     <row r="24" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="B24" s="64"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>4-GPU POWER8/10 SERVER weekly</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21">
@@ -8184,15 +8452,15 @@
       </c>
     </row>
     <row r="25" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="63"/>
-      <c r="B25" s="64"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>4-GPU POWER8/8 SERVER monthly</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -8259,15 +8527,15 @@
       </c>
     </row>
     <row r="26" spans="1:24" ht="20" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="B26" s="64"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>4-GPU POWER8/8 SERVER weekly</v>
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21">
@@ -8334,15 +8602,15 @@
       </c>
     </row>
     <row r="27" spans="1:24" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
         <v>2-GPU POWER8/8 SERVER monthly</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -8409,15 +8677,15 @@
       </c>
     </row>
     <row r="28" spans="1:24" ht="20" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="B28" s="64"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp;" weekly"</f>
         <v>2-GPU POWER8/8 SERVER weekly</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21">
@@ -8484,12 +8752,12 @@
       </c>
     </row>
     <row r="29" spans="1:24" ht="20" customHeight="1">
-      <c r="A29" s="61" t="str">
+      <c r="A29" s="64" t="str">
         <f>Sheet1!A31</f>
         <v>Sakura</v>
       </c>
-      <c r="B29" s="62" t="s">
-        <v>143</v>
+      <c r="B29" s="65" t="s">
+        <v>140</v>
       </c>
       <c r="C29" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -8497,13 +8765,13 @@
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
-        <v>1519</v>
+        <v>1472.8</v>
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="14">
@@ -8512,11 +8780,11 @@
       </c>
       <c r="K29" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>24.576000000000001</v>
+        <v>40.628</v>
       </c>
       <c r="L29" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>GeForce GTX TITAN X</v>
+        <v>NVIDIA TITAN X</v>
       </c>
       <c r="M29" s="14">
         <f t="shared" ca="1" si="4"/>
@@ -8564,21 +8832,21 @@
       </c>
     </row>
     <row r="30" spans="1:24" ht="20" customHeight="1">
-      <c r="A30" s="61"/>
-      <c r="B30" s="62"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
-        <v>Tesla model</v>
+        <v>Tesla P40 model</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="24" t="s">
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
-        <v>1675</v>
+        <v>1555</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="14">
@@ -8587,11 +8855,11 @@
       </c>
       <c r="K30" s="14">
         <f t="shared" ca="1" si="3"/>
-        <v>6.8440000000000003</v>
+        <v>11.757999999999999</v>
       </c>
       <c r="L30" s="14" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M40</v>
+        <v>P40</v>
       </c>
       <c r="M30" s="14">
         <f t="shared" ca="1" si="4"/>
@@ -8636,6 +8904,79 @@
       <c r="W30" s="16"/>
       <c r="X30" s="57">
         <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="C31" s="24" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
+        <v>Tesla P100 model</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
+        <v>1588.7</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="14">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="K31" s="14">
+        <f t="shared" ca="1" si="3"/>
+        <v>9.5</v>
+      </c>
+      <c r="L31" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>P100</v>
+      </c>
+      <c r="M31" s="14">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N31" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Xeon E5-2623 v3</v>
+      </c>
+      <c r="O31" s="14">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P31" s="14">
+        <f t="shared" ca="1" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="Q31" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>SSD</v>
+      </c>
+      <c r="R31" s="14">
+        <f t="shared" ca="1" si="4"/>
+        <v>480</v>
+      </c>
+      <c r="S31" s="14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>SSD</v>
+      </c>
+      <c r="T31" s="14">
+        <f t="shared" ca="1" si="4"/>
+        <v>480</v>
+      </c>
+      <c r="U31" s="14">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1</v>
+      </c>
+      <c r="V31" s="16" t="str">
+        <f t="shared" ca="1" si="8"/>
+        <v>Price includes one-time costs devided by 12 months.</v>
+      </c>
+      <c r="W31" s="16"/>
+      <c r="X31" s="57">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -8650,113 +8991,113 @@
     <mergeCell ref="B15:B28"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="I22 D24 I24 I26 D28 I28 D21:I21 D22:G22 F24:G24 D26:G26 F28:G28 C29:I30 H21:H30 C3:M14 Q13:Q14 J17:M30 C17:I20">
-    <cfRule type="expression" dxfId="21" priority="79">
+  <conditionalFormatting sqref="I22 D24 I24 I26 D28 I28 D21:I21 D22:G22 F24:G24 D26:G26 F28:G28 C29:I30 H21:H30 C3:M14 Q13:Q14 J17:M30 C17:I20 C31:M31">
+    <cfRule type="expression" dxfId="31" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 I23 F23:G23">
-    <cfRule type="expression" dxfId="20" priority="77">
+    <cfRule type="expression" dxfId="30" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:G25 I25">
-    <cfRule type="expression" dxfId="19" priority="76">
+    <cfRule type="expression" dxfId="29" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:G27 I27">
-    <cfRule type="expression" dxfId="18" priority="75">
+    <cfRule type="expression" dxfId="28" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="17" priority="66">
+    <cfRule type="expression" dxfId="27" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N14 N17:N30">
-    <cfRule type="expression" dxfId="16" priority="21">
+  <conditionalFormatting sqref="N3:N14 N17:N31">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P14 Q3:U3 R4:U12 R17:T30 P17:P30 V6:V30 R13:T14 U13:U30">
-    <cfRule type="expression" dxfId="15" priority="19">
+  <conditionalFormatting sqref="P3:P14 Q3:U3 R4:U12 R17:T30 V6:V30 R13:T14 U13:U30 P17:P31 R31:V31">
+    <cfRule type="expression" dxfId="25" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C22">
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C24">
-    <cfRule type="expression" dxfId="13" priority="27">
+    <cfRule type="expression" dxfId="23" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C28">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O14 O17:O30">
-    <cfRule type="expression" dxfId="10" priority="20">
+  <conditionalFormatting sqref="O3:O14 O17:O31">
+    <cfRule type="expression" dxfId="20" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q12">
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q30">
-    <cfRule type="expression" dxfId="8" priority="17">
+  <conditionalFormatting sqref="Q17:Q31">
+    <cfRule type="expression" dxfId="18" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15 C16:F16 H16:M16">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N16">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="16" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15:T16 P15:P16">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O16">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q15:Q16">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Corrected one short name (m-> w). Removed performance bar plot. New version of plotly. Draw vertical line on click point on Cost for rent period plot. Corrected calculation of per month cost (plot below Cost for rent period).
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -1099,343 +1099,339 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>CR P100x4 P8/10 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 P8/10 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK TitanXx4 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>per year USD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Provider link</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://aws.amazon.com</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.softlayer.com/gpu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.nimbix.net/nimbix-cloud-demand-pricing/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cirrascale.com/cloud/plans.aspx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.sakura.ad.jp/koukaryoku/specification/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Offer link</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22240</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22241</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22242</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/dedicated-hosts/pricing/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec3/dedicated-hosts/pricing/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec4/dedicated-hosts/pricing/</t>
+  </si>
+  <si>
+    <t>p2 dedicated host 1 year no Upfront</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>p2 dedicated host 1 year 100% Upfront</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>p2 dedicated host 3 years  100% Upfront</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GPU model</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CPU model</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CPUs</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Memory (GB)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>HDD prim.Type</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>HDD prim.GB</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>HDD sec.Type</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>HDD sec.GB</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Network</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CPU performance (TFlops)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GPU performance (TFlops singl.prec.)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>POWER8?</t>
+  </si>
+  <si>
+    <t>NGD4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 2496</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 12.3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NM K40x2 h.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>P100</t>
+  </si>
+  <si>
+    <t>POWER8</t>
+  </si>
+  <si>
+    <t>2-GPU POWER8/8 SERVER</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2630 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Q</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Outbound Traffic limited to 500GB.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Outbound Traffic limited to 500GB.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Outbound Traffic limited to 500GB.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SL K80x1 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SL K80x1 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SL M60x1 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SL K80x1 x86 h.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>CR K80x8 x86 m.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>CR P100x4 P8/10 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 P8/10 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SK TitanXx4 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>per year USD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Provider link</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://aws.amazon.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.softlayer.com/gpu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.nimbix.net/nimbix-cloud-demand-pricing/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.cirrascale.com/cloud/plans.aspx</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.sakura.ad.jp/koukaryoku/specification/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Offer link</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22240</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22241</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/pricing/on-demand/?refid=em_22242</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/dedicated-hosts/pricing/</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec3/dedicated-hosts/pricing/</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec4/dedicated-hosts/pricing/</t>
-  </si>
-  <si>
-    <t>p2 dedicated host 1 year no Upfront</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>p2 dedicated host 1 year 100% Upfront</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>p2 dedicated host 3 years  100% Upfront</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NVIDIA Tesla K80 Dual Intel Xeon E5-2690 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NVIDIA Tesla M60 Dual Intel Xeon E5-2690 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GPU model</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CPU model</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CPUs</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Memory (GB)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>HDD prim.Type</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>HDD prim.GB</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>HDD sec.Type</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>HDD sec.GB</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Network</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Notes</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Free Outbound Traffic = 1 GB/month. </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CPU performance (TFlops)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GPU performance (TFlops singl.prec.)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>POWER8?</t>
-  </si>
-  <si>
-    <t>NGD4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 2496</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 12.3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NM K40x2 h.</t>
+    <t>CR M40x8 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CRM40x8 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x8 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x8 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x8 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x8 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 P8/8 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 P8/8 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x2 P8/8 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x2 P8/8 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NVIDIA TITAN X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Tesla P40 model</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Tesla P100 model</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>P100</t>
-  </si>
-  <si>
-    <t>POWER8</t>
-  </si>
-  <si>
-    <t>2-GPU POWER8/8 SERVER</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2630 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>L</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>P</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Q</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Z</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NVIDIA Tesla K80 Dual Intel Xeon E5-2620 v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Outbound Traffic limited to 500GB.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Outbound Traffic limited to 500GB.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Outbound Traffic limited to 500GB.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SL K80x1 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SL K80x1 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SL M60x1 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SL K80x1 x86 h.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CRM40x8 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x8 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x8 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 P8/8 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 P8/8 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x2 P8/8 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x2 P8/8 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NVIDIA TITAN X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Tesla P40 model</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Tesla P100 model</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>P100</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1448,6 +1444,10 @@
   </si>
   <si>
     <t>SK P100x1 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86 w.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3205,7 +3205,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="27">
     <dxf>
       <font>
         <color auto="1"/>
@@ -3214,105 +3214,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3554,7 +3455,29 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4169,7 +4092,7 @@
         <v>24</v>
       </c>
       <c r="Y4" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Z4" s="18"/>
       <c r="AA4" s="18" t="s">
@@ -4243,7 +4166,7 @@
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA5" s="26">
         <f>X5/(D5*F5)</f>
@@ -4319,7 +4242,7 @@
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA6" s="26">
         <f t="shared" ref="AA6:AA15" si="2">X6/(D6*F6)</f>
@@ -4392,7 +4315,7 @@
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA7" s="26">
         <f t="shared" si="2"/>
@@ -4483,7 +4406,7 @@
     <row r="9" spans="1:155">
       <c r="A9" s="16"/>
       <c r="B9" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>17</v>
@@ -4555,7 +4478,7 @@
     <row r="10" spans="1:155">
       <c r="A10" s="16"/>
       <c r="B10" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>17</v>
@@ -4627,7 +4550,7 @@
     <row r="11" spans="1:155">
       <c r="A11" s="16"/>
       <c r="B11" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>17</v>
@@ -4732,7 +4655,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>30</v>
@@ -4798,7 +4721,7 @@
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA13" s="26">
         <f>X13/(D13*F13)</f>
@@ -4818,7 +4741,7 @@
         <v>122</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>55</v>
@@ -4881,7 +4804,7 @@
       </c>
       <c r="Y14" s="26"/>
       <c r="Z14" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AA14" s="26">
         <f t="shared" si="2"/>
@@ -4899,7 +4822,7 @@
     <row r="15" spans="1:155">
       <c r="A15" s="16"/>
       <c r="B15" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>84</v>
@@ -4962,7 +4885,7 @@
       </c>
       <c r="Y15" s="26"/>
       <c r="Z15" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AA15" s="26">
         <f t="shared" si="2"/>
@@ -5021,7 +4944,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F17" s="9">
         <v>8.74</v>
@@ -5030,7 +4953,7 @@
         <v>2.91</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>22</v>
@@ -5085,10 +5008,10 @@
     <row r="18" spans="1:155" s="13" customFormat="1" ht="20">
       <c r="A18" s="40"/>
       <c r="B18" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>169</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>170</v>
       </c>
       <c r="D18" s="29">
         <v>2</v>
@@ -5110,7 +5033,7 @@
       </c>
       <c r="J18" s="30"/>
       <c r="K18" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L18" s="29">
         <v>2</v>
@@ -5709,7 +5632,7 @@
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L26" s="5">
         <v>2</v>
@@ -5929,10 +5852,10 @@
     <row r="29" spans="1:155" s="13" customFormat="1">
       <c r="A29" s="48"/>
       <c r="B29" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="51">
         <v>2</v>
@@ -5956,7 +5879,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -6167,7 +6090,7 @@
         <v>52</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -6251,7 +6174,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>112</v>
@@ -6335,10 +6258,10 @@
     </row>
     <row r="33" spans="2:29">
       <c r="B33" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" t="s">
         <v>215</v>
-      </c>
-      <c r="C33" t="s">
-        <v>216</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -6399,7 +6322,7 @@
         <v>1588.7</v>
       </c>
       <c r="Z33" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA33" s="26">
         <f>X33/(D33*F33)</f>
@@ -6495,7 +6418,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:W13 Z13:XFD13 EZ18:XFD18 AA18:AC18 A19:XFD25 EZ29:XFD29 V29 V28:XFD28 S28:U29 R28 Q28:Q29 P28 O28:O29 N28 L26:M29 N26:XFD27 A26:K28 A5:XFD12 A14:XFD17 A30:XFD32 Z33:AC33 V33">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="26" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6560,7 +6483,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13">
-    <cfRule type="expression" dxfId="32" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6589,17 +6512,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:U33">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X33">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6620,10 +6543,10 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -6655,56 +6578,56 @@
       <c r="A1" s="59"/>
       <c r="B1" s="59"/>
       <c r="C1" s="60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="59"/>
       <c r="F1" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="60" t="s">
-        <v>181</v>
-      </c>
       <c r="H1" s="60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J1" s="60"/>
       <c r="K1" s="60"/>
       <c r="L1" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="N1" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="N1" s="60" t="s">
+      <c r="O1" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="O1" s="60" t="s">
+      <c r="P1" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="P1" s="60" t="s">
+      <c r="Q1" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="R1" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="S1" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="T1" s="60" t="s">
         <v>189</v>
       </c>
-      <c r="T1" s="60" t="s">
+      <c r="U1" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="V1" s="60" t="s">
         <v>191</v>
-      </c>
-      <c r="V1" s="60" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="12" customFormat="1" ht="21" thickBot="1">
@@ -6712,13 +6635,13 @@
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>121</v>
@@ -6736,43 +6659,43 @@
         <v>108</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="L2" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M2" s="33" t="s">
         <v>120</v>
       </c>
       <c r="N2" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="P2" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="Q2" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="S2" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="S2" s="36" t="s">
+      <c r="T2" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="U2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="V2" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="V2" s="36" t="s">
-        <v>162</v>
       </c>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
@@ -6782,14 +6705,14 @@
         <v>29</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
         <v>p2.16xlarge on-demand</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>126</v>
@@ -6868,7 +6791,7 @@
         <v>p2.8xlarge on-demand</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="24" t="s">
         <v>127</v>
@@ -6947,7 +6870,7 @@
         <v>p2.xlarge on-demand</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>128</v>
@@ -7026,7 +6949,7 @@
         <v>p2 dedicated host On-demand</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>123</v>
@@ -7105,7 +7028,7 @@
         <v>p2 dedicated host 1 year no Upfront</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>124</v>
@@ -7181,7 +7104,7 @@
         <v>p2 dedicated host 1 year 100% Upfront</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>125</v>
@@ -7255,7 +7178,7 @@
         <v>Softlayer</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW())) &amp; " monthly"</f>
@@ -7263,7 +7186,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -7337,7 +7260,7 @@
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F10" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -7411,7 +7334,7 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -7485,7 +7408,7 @@
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
@@ -7556,7 +7479,7 @@
         <v>Nimbix</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="24" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -7636,7 +7559,7 @@
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F14" s="21">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -7702,7 +7625,7 @@
         <v>Cirrascale</v>
       </c>
       <c r="B15" s="67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("X" &amp; ROW())) &amp; " monthly"</f>
@@ -7710,7 +7633,7 @@
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
@@ -7785,7 +7708,7 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24" t="s">
-        <v>130</v>
+        <v>219</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21">
@@ -7860,7 +7783,7 @@
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
@@ -7935,7 +7858,7 @@
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21">
@@ -8010,7 +7933,7 @@
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -8085,7 +8008,7 @@
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="21">
@@ -8160,7 +8083,7 @@
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -8235,7 +8158,7 @@
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21">
@@ -8310,7 +8233,7 @@
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
@@ -8385,7 +8308,7 @@
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21">
@@ -8460,7 +8383,7 @@
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -8535,7 +8458,7 @@
       </c>
       <c r="D26" s="24"/>
       <c r="E26" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="21">
@@ -8610,7 +8533,7 @@
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -8685,7 +8608,7 @@
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F28" s="21"/>
       <c r="G28" s="21">
@@ -8757,7 +8680,7 @@
         <v>Sakura</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" s="24" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("X"&amp;ROW()))</f>
@@ -8765,7 +8688,7 @@
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -8840,7 +8763,7 @@
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -8913,7 +8836,7 @@
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -8992,112 +8915,112 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="I22 D24 I24 I26 D28 I28 D21:I21 D22:G22 F24:G24 D26:G26 F28:G28 C29:I30 H21:H30 C3:M14 Q13:Q14 J17:M30 C17:I20 C31:M31">
-    <cfRule type="expression" dxfId="31" priority="79">
+    <cfRule type="expression" dxfId="21" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 I23 F23:G23">
-    <cfRule type="expression" dxfId="30" priority="77">
+    <cfRule type="expression" dxfId="20" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:G25 I25">
-    <cfRule type="expression" dxfId="29" priority="76">
+    <cfRule type="expression" dxfId="19" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:G27 I27">
-    <cfRule type="expression" dxfId="28" priority="75">
+    <cfRule type="expression" dxfId="18" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="27" priority="66">
+    <cfRule type="expression" dxfId="17" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N14 N17:N31">
-    <cfRule type="expression" dxfId="26" priority="21">
+    <cfRule type="expression" dxfId="16" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P14 Q3:U3 R4:U12 R17:T30 V6:V30 R13:T14 U13:U30 P17:P31 R31:V31">
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C22">
-    <cfRule type="expression" dxfId="24" priority="28">
+    <cfRule type="expression" dxfId="14" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C24">
-    <cfRule type="expression" dxfId="23" priority="27">
+    <cfRule type="expression" dxfId="13" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C26">
-    <cfRule type="expression" dxfId="22" priority="26">
+    <cfRule type="expression" dxfId="12" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C28">
-    <cfRule type="expression" dxfId="21" priority="25">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O14 O17:O31">
-    <cfRule type="expression" dxfId="20" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:Q12">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q31">
-    <cfRule type="expression" dxfId="18" priority="17">
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:M15 C16:F16 H16:M16">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N16">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R15:T16 P15:P16">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O16">
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q15:Q16">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added new offers from LeaderTelecom. Fixed filters independance.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="48920" windowHeight="15940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="48920" windowHeight="13320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,86 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-0.07 euro/min  = 4.2 euro/h
+0.02 euro/min  = 1.2 euro/h
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+0.03 euro/min * 60 min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+0.04 euro/min * 60 min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+0.07 euro/min * 60 min
 </t>
         </r>
       </text>
@@ -447,7 +526,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="282">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1383,16 +1462,6 @@
     <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 38.</t>
   </si>
   <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 €/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 €/Gb.</t>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 €/Gb.</t>
-  </si>
-  <si>
     <t>https://aws.amazon.com/ec2/dedicated-hosts/pricing/</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1401,63 +1470,163 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>LT 2GX1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 2GX1080 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 2GX1080 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 4GX1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 4GX1080 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 4GX1080 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>https://www.leadergpu.com</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>8 x GeForce GTX 1080 minute</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8 x GeForce GTX 1080 weekly</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8 x GeForce GTX 1080 monthly</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 8GX1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 8GX1080 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT 8GX1080 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>SL M60x1 2690v3 m.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>SL K80x1 2690v3 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x2 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x8 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x8 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x8 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Tesla P100</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>40/1</t>
+  </si>
+  <si>
+    <t>1 x Tesla P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Tesla P100 NVLink</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x Tesla P100 NVLink</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8 x Tesla P100 NVLink</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x FirePro S9300x2</t>
+  </si>
+  <si>
+    <t>2 x 4096</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 512</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2609 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FirePro S9300x2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x4 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x8 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 w.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1828,7 +1997,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="646">
+  <cellStyleXfs count="659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2487,8 +2656,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -2600,11 +2782,14 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="637"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="119" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="646">
+  <cellStyles count="659">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -2957,6 +3142,19 @@
     <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -3252,7 +3450,106 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3781,6 +4078,61 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -4076,13 +4428,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FE40"/>
+  <dimension ref="A1:FE45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF41" sqref="AF41"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -4098,8 +4450,8 @@
     <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" style="13" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="3.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
     <col min="14" max="14" width="4.83203125" style="13" customWidth="1"/>
     <col min="15" max="15" width="14.5" style="13" customWidth="1"/>
     <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -4135,47 +4487,47 @@
     <row r="3" spans="1:161" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
       <c r="R3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="59" t="s">
+      <c r="S3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59" t="s">
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="59"/>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59" t="s">
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
       <c r="AF3" s="1" t="s">
         <v>34</v>
       </c>
@@ -6163,13 +6515,13 @@
       <c r="Y27" s="5"/>
       <c r="Z27" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>$9.59?</v>
+        <v>$10.82?</v>
       </c>
       <c r="AA27" s="24">
-        <v>2049</v>
+        <v>2369</v>
       </c>
       <c r="AB27" s="24">
-        <v>6999</v>
+        <v>7899</v>
       </c>
       <c r="AC27" s="24"/>
       <c r="AD27" s="24"/>
@@ -6247,13 +6599,13 @@
       <c r="Y28" s="5"/>
       <c r="Z28" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>$11.78?</v>
+        <v>$10.82?</v>
       </c>
       <c r="AA28" s="24">
-        <v>2599</v>
+        <v>2369</v>
       </c>
       <c r="AB28" s="24">
-        <v>8599</v>
+        <v>7899</v>
       </c>
       <c r="AC28" s="24"/>
       <c r="AD28" s="24"/>
@@ -6727,7 +7079,7 @@
         <v>0.1</v>
       </c>
       <c r="Y33" s="14" t="str">
-        <f t="shared" ref="Y33:Y39" si="6">W33&amp;"/"&amp;X33</f>
+        <f t="shared" ref="Y33:Y43" si="6">W33&amp;"/"&amp;X33</f>
         <v>/0.1</v>
       </c>
       <c r="Z33" s="10"/>
@@ -6753,7 +7105,7 @@
       <c r="C34" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="14">
         <v>1</v>
       </c>
       <c r="E34" s="28">
@@ -6837,7 +7189,7 @@
       <c r="C35" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="14">
         <v>1</v>
       </c>
       <c r="E35" s="28">
@@ -6914,7 +7266,7 @@
     </row>
     <row r="36" spans="1:32">
       <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
@@ -6948,7 +7300,7 @@
       <c r="C37" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="14">
         <v>2</v>
       </c>
       <c r="E37" s="28">
@@ -7000,7 +7352,7 @@
       </c>
       <c r="U37" s="28"/>
       <c r="V37" s="28"/>
-      <c r="W37" s="28">
+      <c r="W37" s="14">
         <v>40</v>
       </c>
       <c r="X37" s="28">
@@ -7011,10 +7363,10 @@
         <v>40/1</v>
       </c>
       <c r="Z37" s="51">
-        <v>4.2</v>
+        <v>1.2</v>
       </c>
       <c r="AA37" s="51">
-        <v>398.5</v>
+        <v>199.25</v>
       </c>
       <c r="AB37" s="51">
         <v>797</v>
@@ -7023,7 +7375,7 @@
         <v>234</v>
       </c>
       <c r="AF37" s="16" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="24" customHeight="1">
@@ -7036,7 +7388,7 @@
       <c r="C38" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="14">
         <v>4</v>
       </c>
       <c r="E38" s="28">
@@ -7088,7 +7440,7 @@
       </c>
       <c r="U38" s="28"/>
       <c r="V38" s="28"/>
-      <c r="W38" s="28">
+      <c r="W38" s="14">
         <v>40</v>
       </c>
       <c r="X38" s="28">
@@ -7099,10 +7451,10 @@
         <v>40/1</v>
       </c>
       <c r="Z38" s="51">
-        <v>6</v>
+        <v>1.8</v>
       </c>
       <c r="AA38" s="51">
-        <v>529.1</v>
+        <v>264.58</v>
       </c>
       <c r="AB38" s="51">
         <v>1058.33</v>
@@ -7111,7 +7463,7 @@
         <v>234</v>
       </c>
       <c r="AF38" s="16" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="28" customHeight="1">
@@ -7121,7 +7473,7 @@
       <c r="C39" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="14">
         <v>8</v>
       </c>
       <c r="E39" s="28">
@@ -7169,11 +7521,11 @@
         <v>208</v>
       </c>
       <c r="T39" s="28">
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="U39" s="28"/>
       <c r="V39" s="28"/>
-      <c r="W39" s="28">
+      <c r="W39" s="14">
         <v>40</v>
       </c>
       <c r="X39" s="28">
@@ -7184,10 +7536,10 @@
         <v>40/1</v>
       </c>
       <c r="Z39" s="51">
-        <v>10.8</v>
+        <v>3</v>
       </c>
       <c r="AA39" s="51">
-        <v>1008.5</v>
+        <v>504.25</v>
       </c>
       <c r="AB39" s="51">
         <v>2017</v>
@@ -7196,33 +7548,514 @@
         <v>234</v>
       </c>
       <c r="AF39" s="16" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
+    <row r="40" spans="1:32" s="13" customFormat="1" ht="28" customHeight="1">
+      <c r="A40" s="2"/>
+      <c r="B40" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="14">
+        <v>1</v>
+      </c>
+      <c r="E40" s="31">
+        <v>3584</v>
+      </c>
+      <c r="F40" s="42">
+        <v>9.5</v>
+      </c>
+      <c r="G40" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="H40" s="42">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I40" s="42">
+        <v>720</v>
+      </c>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="L40" s="42">
+        <v>2</v>
+      </c>
+      <c r="M40" s="42">
+        <v>10</v>
+      </c>
+      <c r="N40" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O40" s="42">
+        <v>16</v>
+      </c>
+      <c r="P40" s="14">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="Q40" s="42">
+        <v>1866</v>
+      </c>
+      <c r="R40" s="42">
+        <v>32</v>
+      </c>
+      <c r="S40" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="T40" s="42">
+        <v>480</v>
+      </c>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="14">
+        <v>40</v>
+      </c>
+      <c r="X40" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z40" s="51">
+        <v>1.8</v>
+      </c>
+      <c r="AA40" s="51">
+        <v>322.18</v>
+      </c>
+      <c r="AB40" s="51">
+        <v>1288.7</v>
+      </c>
+      <c r="AE40" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF40" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" s="13" customFormat="1" ht="28" customHeight="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="C41" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="14">
+        <v>2</v>
+      </c>
+      <c r="E41" s="14">
+        <v>3584</v>
+      </c>
+      <c r="F41" s="42">
+        <v>9.5</v>
+      </c>
+      <c r="G41" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="H41" s="42">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I41" s="42">
+        <v>720</v>
+      </c>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="L41" s="42">
+        <v>2</v>
+      </c>
+      <c r="M41" s="42">
+        <v>10</v>
+      </c>
+      <c r="N41" s="42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O41" s="42">
+        <v>16</v>
+      </c>
+      <c r="P41" s="14">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="Q41" s="42">
+        <v>1866</v>
+      </c>
+      <c r="R41" s="42">
+        <v>32</v>
+      </c>
+      <c r="S41" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="T41" s="42">
+        <v>480</v>
+      </c>
+      <c r="U41" s="42"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="14">
+        <v>40</v>
+      </c>
+      <c r="X41" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z41" s="51">
+        <v>2.4</v>
+      </c>
+      <c r="AA41" s="51">
+        <v>439.68</v>
+      </c>
+      <c r="AB41" s="51">
+        <v>1758.7</v>
+      </c>
+      <c r="AE41" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF41" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32">
+      <c r="B42" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="14">
+        <v>2</v>
+      </c>
+      <c r="E42" s="14">
+        <v>3584</v>
+      </c>
+      <c r="F42" s="42">
+        <v>9.5</v>
+      </c>
+      <c r="G42" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="H42" s="42">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I42" s="42">
+        <v>720</v>
+      </c>
+      <c r="J42" s="28">
+        <v>1</v>
+      </c>
+      <c r="K42" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="L42" s="28">
+        <v>2</v>
+      </c>
+      <c r="M42" s="28">
+        <v>10</v>
+      </c>
+      <c r="N42" s="28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O42" s="28">
+        <v>16</v>
+      </c>
+      <c r="P42" s="14">
+        <f t="shared" ref="P42:P43" si="7">M42*N42*O42/1000</f>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>1866</v>
+      </c>
+      <c r="R42" s="28">
+        <v>64</v>
+      </c>
+      <c r="S42" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="T42" s="28">
+        <v>960</v>
+      </c>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="14">
+        <v>40</v>
+      </c>
+      <c r="X42" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v>40/1</v>
+      </c>
+      <c r="Z42" s="51">
+        <v>4.2</v>
+      </c>
+      <c r="AA42" s="51">
+        <v>786.25</v>
+      </c>
+      <c r="AB42" s="51">
+        <v>3145</v>
+      </c>
+      <c r="AE42" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF42" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32">
+      <c r="B43" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C43" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="14">
+        <v>4</v>
+      </c>
+      <c r="E43" s="14">
+        <v>3584</v>
+      </c>
+      <c r="F43" s="42">
+        <v>9.5</v>
+      </c>
+      <c r="G43" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="H43" s="42">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I43" s="42">
+        <v>720</v>
+      </c>
+      <c r="J43" s="28">
+        <v>1</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="L43" s="28">
+        <v>2</v>
+      </c>
+      <c r="M43" s="28">
+        <v>10</v>
+      </c>
+      <c r="N43" s="28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O43" s="28">
+        <v>16</v>
+      </c>
+      <c r="P43" s="14">
+        <f t="shared" si="7"/>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="Q43" s="28">
+        <v>1866</v>
+      </c>
+      <c r="R43" s="28">
+        <v>64</v>
+      </c>
+      <c r="S43" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="T43" s="28">
+        <v>1000</v>
+      </c>
+      <c r="U43" s="28"/>
+      <c r="V43" s="28"/>
+      <c r="W43" s="14">
+        <v>40</v>
+      </c>
+      <c r="X43" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="14" t="str">
+        <f t="shared" si="6"/>
+        <v>40/1</v>
+      </c>
+      <c r="Z43" s="51"/>
+      <c r="AA43" s="51"/>
+      <c r="AB43" s="51">
+        <v>4362</v>
+      </c>
+      <c r="AE43" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF43" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32">
+      <c r="B44" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="C44" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="14">
+        <v>8</v>
+      </c>
+      <c r="E44" s="14">
+        <v>3584</v>
+      </c>
+      <c r="F44" s="42">
+        <v>9.5</v>
+      </c>
+      <c r="G44" s="42">
+        <v>4.7</v>
+      </c>
+      <c r="H44" s="42">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I44" s="42">
+        <v>720</v>
+      </c>
+      <c r="J44" s="28">
+        <v>1</v>
+      </c>
+      <c r="K44" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="L44" s="28">
+        <v>2</v>
+      </c>
+      <c r="M44" s="28">
+        <v>10</v>
+      </c>
+      <c r="N44" s="28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O44" s="28">
+        <v>16</v>
+      </c>
+      <c r="P44" s="14">
+        <f>M44*N44*O44/1000</f>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="Q44" s="28">
+        <v>1866</v>
+      </c>
+      <c r="R44" s="28">
+        <v>128</v>
+      </c>
+      <c r="S44" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="T44" s="28">
+        <v>1000</v>
+      </c>
+      <c r="U44" s="28"/>
+      <c r="V44" s="28"/>
+      <c r="W44" s="14">
+        <v>40</v>
+      </c>
+      <c r="X44" s="28">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="14" t="str">
+        <f t="shared" ref="Y44:Y45" si="8">W44&amp;"/"&amp;X44</f>
+        <v>40/1</v>
+      </c>
+      <c r="Z44" s="51"/>
+      <c r="AA44" s="51"/>
+      <c r="AB44" s="51">
+        <v>7133</v>
+      </c>
+      <c r="AE44" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF44" s="16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32">
+      <c r="B45" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="D45" s="14">
+        <v>2</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="F45" s="14">
+        <v>13.9</v>
+      </c>
+      <c r="G45" s="14">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="J45" s="14"/>
+      <c r="K45" s="59" t="s">
+        <v>265</v>
+      </c>
+      <c r="L45" s="14">
+        <v>2</v>
+      </c>
+      <c r="M45" s="14">
+        <v>8</v>
+      </c>
+      <c r="N45" s="14">
+        <v>1.7</v>
+      </c>
+      <c r="O45" s="14">
+        <v>16</v>
+      </c>
+      <c r="P45" s="14">
+        <f>M45*N45*O45/1000</f>
+        <v>0.21759999999999999</v>
+      </c>
+      <c r="Q45" s="14">
+        <v>1866</v>
+      </c>
+      <c r="R45" s="14">
+        <v>32</v>
+      </c>
+      <c r="S45" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="T45" s="14">
+        <v>480</v>
+      </c>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14">
+        <v>40</v>
+      </c>
+      <c r="X45" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v>40/1</v>
+      </c>
+      <c r="Z45" s="51">
+        <v>2.4</v>
+      </c>
+      <c r="AA45" s="51">
+        <v>412.63</v>
+      </c>
+      <c r="AB45" s="51">
+        <v>1630.18</v>
+      </c>
+      <c r="AE45" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF45" s="16" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7234,6 +8067,30 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AG33">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH33">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG34:AG35">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -7245,7 +8102,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH33">
+  <conditionalFormatting sqref="AH34:AH35">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -7258,7 +8115,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG34:AG35">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7270,31 +8127,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AH35">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG34:AG35">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH34:AH35">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7306,32 +8139,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF19:XFD20 FF31:XFD31 Z31 U30:Y31 T30 S30:S31 R30 Q30:Q31 P30 L29:O31 A28:K30 Z35 A17 A18:I18 A21:Q21 S21:V21 K18:V18 A22:V22 Z18:AD22 W18:W22 A12:AD12 B8:AD8 A7:A8 A5:M6 B7:M7 B9:M9 A10:M11 N9:AD11 A23:AD25 A27:M27 L28:M28 N27:O28 A26:O26 P26:AD28 A32:AD32 A34:M34 N34:P35 AG32:XFD34 AG19:AI20 AG35:AI35 AG21:XFD30 AF32:AF35 AF18:AF30 AG5:XFD18 AE5:AF5 Q34:X34 AC34:AD34 AB35 A13:AA13 A14:AD16 P29:X29 Z29:AD30 A33:X33 Z33:AD33 Z34:AA34 N5:AD7 AE6:AE36 AF6:AF16">
-    <cfRule type="expression" dxfId="47" priority="39">
+    <cfRule type="expression" dxfId="61" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB13">
-    <cfRule type="expression" dxfId="46" priority="26">
+    <cfRule type="expression" dxfId="60" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="45" priority="25">
+    <cfRule type="expression" dxfId="59" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:M35 Q35:X35">
-    <cfRule type="expression" dxfId="44" priority="24">
+    <cfRule type="expression" dxfId="58" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34">
-    <cfRule type="expression" dxfId="43" priority="23">
+    <cfRule type="expression" dxfId="57" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG35 AG21:AG30 AG5:AG18">
-    <cfRule type="colorScale" priority="124">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7343,7 +8176,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AH35 AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="128">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7355,7 +8188,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG33 AG21:AG30 AG5:AG18">
-    <cfRule type="colorScale" priority="132">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7367,7 +8200,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AH33 AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="136">
+    <cfRule type="colorScale" priority="141">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7379,7 +8212,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32:AI35 AI21:AI30 AI5:AI18">
-    <cfRule type="colorScale" priority="140">
+    <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7391,7 +8224,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG21:AG30 AG5:AG18">
-    <cfRule type="colorScale" priority="144">
+    <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7403,7 +8236,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="147">
+    <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7415,68 +8248,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:Q20 S20:V20">
-    <cfRule type="expression" dxfId="42" priority="15">
+    <cfRule type="expression" dxfId="56" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG20">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG20">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG20">
@@ -7503,18 +8276,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="41" priority="6">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:D19 R20:R21 K19:V19">
-    <cfRule type="expression" dxfId="40" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG19">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="AG20">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7525,8 +8288,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="AH20">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7537,8 +8300,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG19">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="AI20">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7549,8 +8312,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="AG20">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH20">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7561,16 +8336,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="E19:I19">
+    <cfRule type="expression" dxfId="55" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:D19 R20:R21 K19:V19">
+    <cfRule type="expression" dxfId="54" priority="12">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG19">
@@ -7597,28 +8370,113 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AG19">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH19">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI19">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG19">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH19">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="53" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y17:Y22">
-    <cfRule type="expression" dxfId="38" priority="4">
+    <cfRule type="expression" dxfId="52" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y29">
-    <cfRule type="expression" dxfId="37" priority="3">
+    <cfRule type="expression" dxfId="51" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y33:Y35">
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="50" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y37:Y39">
-    <cfRule type="expression" dxfId="35" priority="1">
+    <cfRule type="expression" dxfId="49" priority="6">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P44">
+    <cfRule type="expression" dxfId="48" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y44:Y45">
+    <cfRule type="expression" dxfId="47" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P42:P43">
+    <cfRule type="expression" dxfId="46" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y42:Y43">
+    <cfRule type="expression" dxfId="45" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P45">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7636,13 +8494,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AC55"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7922,7 +8780,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19" t="str">
-        <f t="shared" ref="K4:K41" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="K4:K55" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L4" s="14">
@@ -8151,7 +9009,7 @@
         <v>p2 dedicated host 1 year no Upfront</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>113</v>
@@ -8238,7 +9096,7 @@
         <v>p2 dedicated host 1 year 100% Upfront</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>114</v>
@@ -8486,7 +9344,7 @@
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="22" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -8565,7 +9423,7 @@
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
@@ -9199,7 +10057,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>6999</v>
+        <v>7899</v>
       </c>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -9278,7 +10136,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>2049</v>
+        <v>2369</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -9359,7 +10217,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>8599</v>
+        <v>7899</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
@@ -9438,7 +10296,7 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>2599</v>
+        <v>2369</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -9816,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="X27" s="16">
-        <f t="shared" ref="X27:X41" ca="1" si="15">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="X27:X55" ca="1" si="15">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="Y27" s="16"/>
@@ -10242,34 +11100,34 @@
         <v>LeaderTelecom</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C33" s="22" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minute"</f>
-        <v>2 x GeForce GTX 1080 minute</v>
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>2 x GeForce GTX 1080 minutely</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F33" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>4.2</v>
+        <v>1.2</v>
       </c>
       <c r="K33" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>EUR</v>
       </c>
       <c r="L33" s="14">
-        <f t="shared" ref="L33:L41" ca="1" si="17">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L33:L55" ca="1" si="17">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.43519999999999998</v>
       </c>
       <c r="M33" s="14">
-        <f t="shared" ref="M33:M41" ca="1" si="18">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M33:M55" ca="1" si="18">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>16.456</v>
       </c>
       <c r="N33" s="14" t="str">
-        <f t="shared" ref="N33:W41" ca="1" si="19">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N33:W48" ca="1" si="19">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>GeForce GTX 1080</v>
       </c>
       <c r="O33" s="14">
@@ -10310,7 +11168,7 @@
       </c>
       <c r="X33" s="16" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC33" s="45">
         <v>37</v>
@@ -10322,11 +11180,11 @@
         <v>2 x GeForce GTX 1080 weekly</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G34" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>398.5</v>
+        <v>199.25</v>
       </c>
       <c r="K34" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10382,7 +11240,7 @@
       </c>
       <c r="X34" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC34" s="45">
         <v>37</v>
@@ -10394,7 +11252,7 @@
         <v>2 x GeForce GTX 1080 monthly</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H35" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -10454,7 +11312,7 @@
       </c>
       <c r="X35" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC35" s="45">
         <v>37</v>
@@ -10462,16 +11320,16 @@
     </row>
     <row r="36" spans="1:29">
       <c r="C36" s="22" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minute"</f>
-        <v>4 x GeForce GTX 1080 minute</v>
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>4 x GeForce GTX 1080 minutely</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F36" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>6</v>
+        <v>1.8</v>
       </c>
       <c r="H36" s="13"/>
       <c r="K36" s="19" t="str">
@@ -10528,7 +11386,7 @@
       </c>
       <c r="X36" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC36" s="45">
         <v>38</v>
@@ -10545,7 +11403,7 @@
       <c r="F37" s="13"/>
       <c r="G37" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>529.1</v>
+        <v>264.58</v>
       </c>
       <c r="H37" s="13"/>
       <c r="K37" s="19" t="str">
@@ -10602,7 +11460,7 @@
       </c>
       <c r="X37" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC37" s="45">
         <v>38</v>
@@ -10614,7 +11472,7 @@
         <v>4 x GeForce GTX 1080 monthly</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F38" s="13"/>
       <c r="H38" s="19">
@@ -10675,23 +11533,24 @@
       </c>
       <c r="X38" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC38" s="45">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:29">
-      <c r="C39" s="41" t="s">
-        <v>251</v>
+      <c r="C39" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>8 x GeForce GTX 1080 minutely</v>
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F39" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>10.8</v>
+        <v>3</v>
       </c>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
@@ -10735,7 +11594,7 @@
       </c>
       <c r="T39" s="14">
         <f t="shared" ca="1" si="19"/>
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="U39" s="14">
         <f t="shared" ca="1" si="19"/>
@@ -10751,24 +11610,25 @@
       </c>
       <c r="X39" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC39" s="45">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:29">
-      <c r="C40" s="41" t="s">
-        <v>252</v>
+      <c r="C40" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" weekly"</f>
+        <v>8 x GeForce GTX 1080 weekly</v>
       </c>
       <c r="D40" s="43"/>
       <c r="E40" s="41" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F40" s="43"/>
       <c r="G40" s="19">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>1008.5</v>
+        <v>504.25</v>
       </c>
       <c r="H40" s="43"/>
       <c r="I40" s="43"/>
@@ -10811,7 +11671,7 @@
       </c>
       <c r="T40" s="14">
         <f t="shared" ca="1" si="19"/>
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="U40" s="14">
         <f t="shared" ca="1" si="19"/>
@@ -10827,19 +11687,20 @@
       </c>
       <c r="X40" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC40" s="45">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:29">
-      <c r="C41" s="41" t="s">
-        <v>253</v>
+      <c r="C41" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" monthly"</f>
+        <v>8 x GeForce GTX 1080 monthly</v>
       </c>
       <c r="D41" s="43"/>
       <c r="E41" s="41" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
@@ -10887,7 +11748,7 @@
       </c>
       <c r="T41" s="14">
         <f t="shared" ca="1" si="19"/>
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="U41" s="14">
         <f t="shared" ca="1" si="19"/>
@@ -10903,185 +11764,1299 @@
       </c>
       <c r="X41" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 €/Gb.</v>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC41" s="45">
         <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
+      <c r="C42" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>1 x Tesla P100 minutely</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="F42" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>1.8</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="K42" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L42" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M42" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>9.5</v>
+      </c>
+      <c r="N42" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="P42" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S42" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V42" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W42" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X42" s="16" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
+      <c r="C43" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" weekly"</f>
+        <v>1 x Tesla P100 weekly</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>322.18</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="K43" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L43" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M43" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>9.5</v>
+      </c>
+      <c r="N43" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="P43" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S43" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V43" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X43" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
+      <c r="AC43" s="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
+      <c r="C44" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" monthly"</f>
+        <v>1 x Tesla P100 monthly</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="H44" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>1288.7</v>
+      </c>
+      <c r="K44" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L44" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M44" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>9.5</v>
+      </c>
+      <c r="N44" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="P44" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S44" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W44" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X44" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="13"/>
+      <c r="AC44" s="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
+      <c r="C45" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>2 x Tesla P100 minutely</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>2.4</v>
+      </c>
+      <c r="H45" s="13"/>
+      <c r="K45" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L45" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M45" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N45" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="P45" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S45" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W45" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X45" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
+      <c r="C46" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" weekly"</f>
+        <v>2 x Tesla P100 weekly</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>439.68</v>
+      </c>
+      <c r="H46" s="13"/>
+      <c r="K46" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L46" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M46" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N46" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="P46" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S46" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W46" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X46" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
+      <c r="C47" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" monthly"</f>
+        <v>2 x Tesla P100 monthly</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="H47" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>1758.7</v>
+      </c>
+      <c r="K47" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L47" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M47" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N47" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="P47" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>32</v>
+      </c>
+      <c r="S47" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="U47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V47" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W47" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X47" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AC47" s="45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
+      <c r="C48" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>2 x Tesla P100 NVLink minutely</v>
+      </c>
+      <c r="D48" s="41"/>
+      <c r="E48" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="F48" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>4.2</v>
+      </c>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L48" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M48" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N48" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>P100</v>
+      </c>
+      <c r="O48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="P48" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="R48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>64</v>
+      </c>
+      <c r="S48" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>SSD</v>
+      </c>
+      <c r="T48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>960</v>
+      </c>
+      <c r="U48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="V48" s="14">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="W48" s="14" t="str">
+        <f t="shared" ca="1" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="X48" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="3:29">
+      <c r="C49" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" weekly"</f>
+        <v>2 x Tesla P100 NVLink weekly</v>
+      </c>
+      <c r="D49" s="43"/>
+      <c r="E49" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="F49" s="43"/>
+      <c r="G49" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>786.25</v>
+      </c>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L49" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M49" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N49" s="14" t="str">
+        <f t="shared" ref="N49:W55" ca="1" si="20">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>P100</v>
+      </c>
+      <c r="O49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P49" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>64</v>
+      </c>
+      <c r="S49" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>960</v>
+      </c>
+      <c r="U49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V49" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W49" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X49" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="3:29">
+      <c r="C50" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" monthly"</f>
+        <v>2 x Tesla P100 NVLink monthly</v>
+      </c>
+      <c r="D50" s="43"/>
+      <c r="E50" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="19">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>3145</v>
+      </c>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L50" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M50" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N50" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>P100</v>
+      </c>
+      <c r="O50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P50" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>64</v>
+      </c>
+      <c r="S50" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>960</v>
+      </c>
+      <c r="U50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V50" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W50" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X50" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="3:29">
+      <c r="C51" s="22" t="str">
+        <f t="shared" ref="C51:C55" ca="1" si="21">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" monthly"</f>
+        <v>4 x Tesla P100 NVLink monthly</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="19">
+        <f t="shared" ref="H51" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>4362</v>
+      </c>
+      <c r="K51" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L51" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M51" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>38</v>
+      </c>
+      <c r="N51" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>P100</v>
+      </c>
+      <c r="O51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="P51" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>64</v>
+      </c>
+      <c r="S51" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>1000</v>
+      </c>
+      <c r="U51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V51" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W51" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X51" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="AC51" s="45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="3:29">
+      <c r="C52" s="22" t="str">
+        <f t="shared" ca="1" si="21"/>
+        <v>8 x Tesla P100 NVLink monthly</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="19">
+        <f t="shared" ref="H52" ca="1" si="23">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>7133</v>
+      </c>
+      <c r="K52" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L52" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="M52" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>76</v>
+      </c>
+      <c r="N52" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>P100</v>
+      </c>
+      <c r="O52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="P52" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2630 v4</v>
+      </c>
+      <c r="Q52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>128</v>
+      </c>
+      <c r="S52" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>1000</v>
+      </c>
+      <c r="U52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V52" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W52" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X52" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="AC52" s="45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="3:29">
+      <c r="C53" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;" minutely"</f>
+        <v>2 x FirePro S9300x2 minutely</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="F53" s="13">
+        <f t="shared" ref="F53" ca="1" si="24">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>2.4</v>
+      </c>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="K53" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L53" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.43519999999999998</v>
+      </c>
+      <c r="M53" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>27.8</v>
+      </c>
+      <c r="N53" s="14" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>FirePro S9300x2</v>
+      </c>
+      <c r="O53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P53" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2609 v4</v>
+      </c>
+      <c r="Q53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>32</v>
+      </c>
+      <c r="S53" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>480</v>
+      </c>
+      <c r="U53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V53" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W53" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X53" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="AC53" s="45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="3:29">
+      <c r="C54" s="22" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW())) &amp;"weekly"</f>
+        <v>2 x FirePro S9300x2weekly</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="F54" s="43"/>
+      <c r="G54" s="19">
+        <f t="shared" ref="G54" ca="1" si="25">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>412.63</v>
+      </c>
+      <c r="H54" s="43"/>
+      <c r="K54" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L54" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.43519999999999998</v>
+      </c>
+      <c r="M54" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>27.8</v>
+      </c>
+      <c r="N54" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>FirePro S9300x2</v>
+      </c>
+      <c r="O54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P54" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2609 v4</v>
+      </c>
+      <c r="Q54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>32</v>
+      </c>
+      <c r="S54" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>480</v>
+      </c>
+      <c r="U54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V54" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W54" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X54" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="AC54" s="45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="3:29">
+      <c r="C55" s="22" t="str">
+        <f t="shared" ca="1" si="21"/>
+        <v>2 x FirePro S9300x2 monthly</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="19">
+        <f t="shared" ref="H55" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>1630.18</v>
+      </c>
+      <c r="K55" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>EUR</v>
+      </c>
+      <c r="L55" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.43519999999999998</v>
+      </c>
+      <c r="M55" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>27.8</v>
+      </c>
+      <c r="N55" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>FirePro S9300x2</v>
+      </c>
+      <c r="O55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P55" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Xeon E5-2609 v4</v>
+      </c>
+      <c r="Q55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>32</v>
+      </c>
+      <c r="S55" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>SSD</v>
+      </c>
+      <c r="T55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>480</v>
+      </c>
+      <c r="U55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V55" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W55" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>40/1</v>
+      </c>
+      <c r="X55" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
+      </c>
+      <c r="AC55" s="45">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 F25:G25 F29:G29 H22:H31 S13:S15 E23:G23 E18:J22 C30:C32 E26:G28 D26:D33 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 K4:K35 E30:I32 M32:O41 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8">
-    <cfRule type="expression" dxfId="34" priority="97">
+  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 F25:G25 F29:G29 H22:H31 S13:S15 E23:G23 E18:J22 C30:C32 E26:G28 D26:D33 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 K4:K35 E30:I32 M32:O41 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8 L42:S55 T45:X55 K48:K55">
+    <cfRule type="expression" dxfId="43" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 I24:J24 F24:G24">
-    <cfRule type="expression" dxfId="33" priority="95">
+    <cfRule type="expression" dxfId="42" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:J26">
-    <cfRule type="expression" dxfId="32" priority="94">
+    <cfRule type="expression" dxfId="41" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:J28">
-    <cfRule type="expression" dxfId="31" priority="93">
+    <cfRule type="expression" dxfId="40" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="30" priority="84">
+    <cfRule type="expression" dxfId="39" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P15 P18:P41">
+    <cfRule type="expression" dxfId="38" priority="52">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:W3 T4:W12 T18:V31 T13:V15 W13:W31 R3:R15 R18:R41 X6:X41 T32:W38 U39:W41 T39:T44">
+    <cfRule type="expression" dxfId="37" priority="50">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C23">
+    <cfRule type="expression" dxfId="36" priority="59">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:C25">
+    <cfRule type="expression" dxfId="35" priority="58">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C27">
+    <cfRule type="expression" dxfId="34" priority="57">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C29">
+    <cfRule type="expression" dxfId="33" priority="56">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q15 Q18:Q41">
+    <cfRule type="expression" dxfId="32" priority="51">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S12">
+    <cfRule type="expression" dxfId="31" priority="49">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S18:S41">
+    <cfRule type="expression" dxfId="30" priority="48">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:J17 N17:O17">
     <cfRule type="expression" dxfId="29" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S3:W3 T4:W12 T18:V31 T13:V15 W13:W31 R3:R15 R18:R41 T32:W41 X6:X41">
-    <cfRule type="expression" dxfId="28" priority="37">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C23">
-    <cfRule type="expression" dxfId="27" priority="46">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:C25">
-    <cfRule type="expression" dxfId="26" priority="45">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
-    <cfRule type="expression" dxfId="25" priority="44">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C29">
-    <cfRule type="expression" dxfId="24" priority="43">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q15 Q18:Q41">
-    <cfRule type="expression" dxfId="23" priority="38">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S12">
-    <cfRule type="expression" dxfId="22" priority="36">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S18:S41">
-    <cfRule type="expression" dxfId="21" priority="35">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17:J17 N17:O17">
-    <cfRule type="expression" dxfId="20" priority="26">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="P16:P17">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="28" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:V17 R16:R17">
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16:Q17">
-    <cfRule type="expression" dxfId="17" priority="24">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17">
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="15" priority="21">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="14" priority="20">
+    <cfRule type="expression" dxfId="23" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="13" priority="19">
+    <cfRule type="expression" dxfId="22" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32:L41">
-    <cfRule type="expression" dxfId="12" priority="18">
+    <cfRule type="expression" dxfId="21" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="11" priority="17">
+    <cfRule type="expression" dxfId="20" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="10" priority="16">
+    <cfRule type="expression" dxfId="19" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="18" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
+    <cfRule type="expression" dxfId="17" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J30:J32">
+    <cfRule type="expression" dxfId="16" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36 K36:K47">
+    <cfRule type="expression" dxfId="15" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G37">
+    <cfRule type="expression" dxfId="14" priority="23">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
+    <cfRule type="expression" dxfId="13" priority="22">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="expression" dxfId="12" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="11" priority="16">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="expression" dxfId="10" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42">
     <cfRule type="expression" dxfId="8" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J32">
-    <cfRule type="expression" dxfId="7" priority="12">
+  <conditionalFormatting sqref="U42:X44">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36 K36:K41">
-    <cfRule type="expression" dxfId="6" priority="11">
+  <conditionalFormatting sqref="G43">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="expression" dxfId="5" priority="10">
+  <conditionalFormatting sqref="H44">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="4" priority="9">
+  <conditionalFormatting sqref="D45">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
+  <conditionalFormatting sqref="G46">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="H47">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
+  <conditionalFormatting sqref="H50:H52 H55">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
+  <conditionalFormatting sqref="G49 G54">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Corrected minute prices for LeaderTelecom
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="48920" windowHeight="13320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="30940" windowHeight="22580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-0.02 euro/min  = 1.2 euro/h
+euro/min  * 60  =  euro/h
 </t>
         </r>
       </text>
@@ -464,7 +464,7 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-0.03 euro/min * 60 min</t>
+euro/min * 60 = eur/h</t>
         </r>
       </text>
     </comment>
@@ -490,7 +490,7 @@
             <charset val="128"/>
           </rPr>
           <t xml:space="preserve">
-0.04 euro/min * 60 min</t>
+euro/min * 60 </t>
         </r>
       </text>
     </comment>
@@ -515,8 +515,7 @@
             <family val="2"/>
             <charset val="128"/>
           </rPr>
-          <t xml:space="preserve">
-0.07 euro/min * 60 min
+          <t xml:space="preserve"> euro/min * 60 min
 </t>
         </r>
       </text>
@@ -4431,10 +4430,10 @@
   <dimension ref="A1:FE45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="X20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7363,7 +7362,7 @@
         <v>40/1</v>
       </c>
       <c r="Z37" s="51">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="AA37" s="51">
         <v>199.25</v>
@@ -7451,7 +7450,7 @@
         <v>40/1</v>
       </c>
       <c r="Z38" s="51">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="AA38" s="51">
         <v>264.58</v>
@@ -7536,7 +7535,7 @@
         <v>40/1</v>
       </c>
       <c r="Z39" s="51">
-        <v>3</v>
+        <v>5.4</v>
       </c>
       <c r="AA39" s="51">
         <v>504.25</v>
@@ -7620,7 +7619,7 @@
         <v>256</v>
       </c>
       <c r="Z40" s="51">
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="AA40" s="51">
         <v>322.18</v>
@@ -7704,7 +7703,7 @@
         <v>256</v>
       </c>
       <c r="Z41" s="51">
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
       <c r="AA41" s="51">
         <v>439.68</v>
@@ -7791,7 +7790,7 @@
         <v>40/1</v>
       </c>
       <c r="Z42" s="51">
-        <v>4.2</v>
+        <v>9</v>
       </c>
       <c r="AA42" s="51">
         <v>786.25</v>
@@ -8497,10 +8496,10 @@
   <dimension ref="A1:AC55"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11112,7 +11111,7 @@
       </c>
       <c r="F33" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="K33" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11329,7 +11328,7 @@
       </c>
       <c r="F36" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="H36" s="13"/>
       <c r="K36" s="19" t="str">
@@ -11550,7 +11549,7 @@
       </c>
       <c r="F39" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>3</v>
+        <v>5.4</v>
       </c>
       <c r="G39" s="43"/>
       <c r="H39" s="43"/>
@@ -11780,7 +11779,7 @@
       </c>
       <c r="F42" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>1.8</v>
+        <v>3.6</v>
       </c>
       <c r="H42" s="13"/>
       <c r="K42" s="19" t="str">
@@ -12010,7 +12009,7 @@
       </c>
       <c r="F45" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
       <c r="H45" s="13"/>
       <c r="K45" s="19" t="str">
@@ -12240,7 +12239,7 @@
       </c>
       <c r="F48" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>4.2</v>
+        <v>9</v>
       </c>
       <c r="G48" s="43"/>
       <c r="H48" s="43"/>
@@ -13074,7 +13073,7 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="C22 C20" formula="1"/>
+    <ignoredError sqref="C21:C23 C20" formula="1"/>
     <ignoredError sqref="S13" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>

</xml_diff>

<commit_message>
Fixed Tokyo Univ. offers.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -599,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D58" authorId="0">
+    <comment ref="D55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -626,7 +626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB58" authorId="0">
+    <comment ref="AB55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -657,7 +657,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="328">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1723,22 +1723,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Reedbush-H Group 4 (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H Group 4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H Group 8 (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H Group 8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>per hour</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1755,26 +1739,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/index-e.html</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Max 128 nodes. Included 13824 node hours if 1 node is used, 6912 node hours if more than 1 node is used simultaneously.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Max 128 nodes. Included 27648 node hours if 2 nodes are used, 13824 node hours if more than 2 node are used simultaneously.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H Group 8 dedicated (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H Group 8 dedicated</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>https://www.nimbix.net/nimbix-cloud-demand-pricing/</t>
   </si>
   <si>
@@ -1782,10 +1746,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>TU gr.4 edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>MS Azure</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1924,14 +1884,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used simulateously.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included 13824 node hours if 1 node is used, 6912 node hours if more than 1 node is used simultaneously.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>AF</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1948,6 +1900,42 @@
   </si>
   <si>
     <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU gen edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev edu</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1962,7 +1950,7 @@
     <numFmt numFmtId="179" formatCode="[$¥-411]#,##0.00"/>
     <numFmt numFmtId="180" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2188,6 +2176,11 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Abadi MT Condensed Light"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -3032,7 +3025,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -3152,6 +3145,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="690">
     <cellStyle name="$Normal" xfId="356"/>
@@ -3845,7 +3839,40 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="78">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4671,17 +4698,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -4977,13 +4993,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FF61"/>
+  <dimension ref="A1:FF58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="V43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="Q42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5079,7 +5095,7 @@
       <c r="AD3" s="62"/>
       <c r="AE3" s="62"/>
       <c r="AF3" s="17" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="AG3" s="1" t="s">
         <v>32</v>
@@ -5287,16 +5303,16 @@
         <v>216</v>
       </c>
       <c r="Z4" s="17" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AA4" s="25" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AB4" s="17" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AC4" s="17" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="AD4" s="17" t="s">
         <v>201</v>
@@ -5377,7 +5393,7 @@
       </c>
       <c r="AF5" s="16"/>
       <c r="AG5" s="16" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:162">
@@ -5451,7 +5467,7 @@
       </c>
       <c r="AF6" s="16"/>
       <c r="AG6" s="16" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:162">
@@ -5525,7 +5541,7 @@
       </c>
       <c r="AF7" s="16"/>
       <c r="AG7" s="16" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:162">
@@ -6211,7 +6227,7 @@
     </row>
     <row r="18" spans="1:162" s="13" customFormat="1">
       <c r="A18" s="56" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>44</v>
@@ -7593,7 +7609,7 @@
         <v>49</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D33" s="28">
         <v>4</v>
@@ -7962,7 +7978,7 @@
     </row>
     <row r="38" spans="1:33" ht="24" customHeight="1">
       <c r="A38" s="16" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>187</v>
@@ -8545,7 +8561,7 @@
         <v>1</v>
       </c>
       <c r="Y44" s="14" t="str">
-        <f t="shared" ref="Y44:Y54" si="8">W44&amp;"/"&amp;X44</f>
+        <f t="shared" ref="Y44:Y53" si="8">W44&amp;"/"&amp;X44</f>
         <v>40/1</v>
       </c>
       <c r="Z44" s="51"/>
@@ -8564,10 +8580,10 @@
     <row r="45" spans="1:33" s="13" customFormat="1">
       <c r="A45" s="2"/>
       <c r="B45" s="59" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D45" s="14">
         <v>2</v>
@@ -8650,10 +8666,10 @@
     <row r="46" spans="1:33" s="13" customFormat="1">
       <c r="A46" s="2"/>
       <c r="B46" s="59" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D46" s="14">
         <v>4</v>
@@ -8675,7 +8691,7 @@
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="28" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="L46" s="28">
         <v>2</v>
@@ -8736,10 +8752,10 @@
     <row r="47" spans="1:33" s="13" customFormat="1">
       <c r="A47" s="2"/>
       <c r="B47" s="59" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D47" s="14">
         <v>8</v>
@@ -8988,15 +9004,15 @@
         <v>6912</v>
       </c>
       <c r="AG50" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:33">
       <c r="A51" s="16" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
       <c r="C51" s="57" t="s">
         <v>270</v>
@@ -9038,7 +9054,7 @@
         <v>16</v>
       </c>
       <c r="P51" s="14">
-        <f t="shared" ref="P51:P54" si="9">M51*N51*O51/1000</f>
+        <f t="shared" ref="P51:P53" si="9">M51*N51*O51/1000</f>
         <v>0.60480000000000012</v>
       </c>
       <c r="Q51" s="14">
@@ -9074,15 +9090,12 @@
         <v>13824</v>
       </c>
       <c r="AG51" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:33">
-      <c r="A52" s="16" t="s">
-        <v>330</v>
-      </c>
       <c r="B52" s="22" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="C52" s="57" t="s">
         <v>270</v>
@@ -9139,8 +9152,6 @@
       <c r="T52" s="14">
         <v>4000</v>
       </c>
-      <c r="U52" s="14"/>
-      <c r="V52" s="14"/>
       <c r="W52" s="14">
         <v>13.635</v>
       </c>
@@ -9149,20 +9160,23 @@
         <v>13.635/</v>
       </c>
       <c r="AC52" s="52">
-        <f>480000/1.08 /4</f>
-        <v>111111.11111111111</v>
+        <f>180000/1.08</f>
+        <v>166666.66666666666</v>
       </c>
       <c r="AE52" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="AF52" s="16"/>
-      <c r="AG52" s="16" t="s">
-        <v>281</v>
+      <c r="AF52" s="16">
+        <f>21600/2.5</f>
+        <v>8640</v>
+      </c>
+      <c r="AG52" s="63" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:33">
       <c r="B53" s="22" t="s">
-        <v>274</v>
+        <v>324</v>
       </c>
       <c r="C53" s="57" t="s">
         <v>270</v>
@@ -9217,7 +9231,7 @@
         <v>271</v>
       </c>
       <c r="T53" s="14">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="W53" s="14">
         <v>13.635</v>
@@ -9227,269 +9241,257 @@
         <v>13.635/</v>
       </c>
       <c r="AC53" s="52">
-        <f>700000/1.08 /8</f>
-        <v>81018.518518518511</v>
+        <f>216000/1.08</f>
+        <v>200000</v>
       </c>
       <c r="AE53" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="AF53" s="16"/>
-      <c r="AG53" s="16" t="s">
+      <c r="AF53" s="16">
+        <f>21600/2.5</f>
+        <v>8640</v>
+      </c>
+      <c r="AG53" s="63" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" ht="20">
+      <c r="A55" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" s="57" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="54" spans="1:33">
-      <c r="B54" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C54" s="57" t="s">
-        <v>270</v>
-      </c>
-      <c r="D54" s="14">
-        <v>2</v>
-      </c>
-      <c r="E54" s="14">
-        <v>3584</v>
-      </c>
-      <c r="F54" s="42">
-        <v>9.5</v>
-      </c>
-      <c r="G54" s="42">
-        <v>4.7</v>
-      </c>
-      <c r="H54" s="42">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="I54" s="42">
-        <v>720</v>
-      </c>
-      <c r="J54" s="28">
+      <c r="D55" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="14">
+        <v>8.74</v>
+      </c>
+      <c r="G55" s="14">
+        <v>2.91</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" s="14"/>
+      <c r="K55" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="L55" s="14">
         <v>1</v>
       </c>
-      <c r="K54" s="57" t="s">
-        <v>269</v>
-      </c>
-      <c r="L54" s="14">
-        <v>2</v>
-      </c>
-      <c r="M54" s="14">
-        <v>18</v>
-      </c>
-      <c r="N54" s="14">
-        <v>2.1</v>
-      </c>
-      <c r="O54" s="14">
-        <v>16</v>
-      </c>
-      <c r="P54" s="14">
-        <f t="shared" si="9"/>
-        <v>0.60480000000000012</v>
-      </c>
-      <c r="Q54" s="14">
-        <v>2400</v>
-      </c>
-      <c r="R54" s="14">
-        <v>256</v>
-      </c>
-      <c r="S54" s="57" t="s">
-        <v>271</v>
-      </c>
-      <c r="T54" s="14">
-        <v>8000</v>
-      </c>
-      <c r="W54" s="14">
-        <v>13.635</v>
-      </c>
-      <c r="Y54" s="14" t="str">
-        <f t="shared" si="8"/>
-        <v>13.635/</v>
-      </c>
-      <c r="AC54" s="52">
-        <f>840000/1.08 /8</f>
-        <v>97222.222222222219</v>
-      </c>
-      <c r="AE54" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="AF54" s="16"/>
-      <c r="AG54" s="16" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="55" spans="1:33">
-      <c r="B55" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C55" s="57" t="s">
-        <v>270</v>
-      </c>
-      <c r="D55" s="14">
-        <v>2</v>
-      </c>
-      <c r="E55" s="14">
-        <v>3584</v>
-      </c>
-      <c r="F55" s="42">
-        <v>9.5</v>
-      </c>
-      <c r="G55" s="42">
-        <v>4.7</v>
-      </c>
-      <c r="H55" s="42">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="I55" s="42">
-        <v>720</v>
-      </c>
-      <c r="J55" s="28">
-        <v>1</v>
-      </c>
-      <c r="K55" s="57" t="s">
-        <v>269</v>
-      </c>
-      <c r="L55" s="14">
-        <v>2</v>
-      </c>
       <c r="M55" s="14">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="N55" s="14">
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="O55" s="14">
         <v>16</v>
       </c>
       <c r="P55" s="14">
-        <f t="shared" ref="P55:P56" si="10">M55*N55*O55/1000</f>
-        <v>0.60480000000000012</v>
+        <f t="shared" ref="P55" si="10">M55*N55*O55/1000</f>
+        <v>0.24960000000000002</v>
       </c>
       <c r="Q55" s="14">
-        <v>2400</v>
+        <v>2133</v>
       </c>
       <c r="R55" s="14">
-        <v>256</v>
+        <v>56</v>
       </c>
       <c r="S55" s="57" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="T55" s="14">
-        <v>8000</v>
-      </c>
-      <c r="U55" s="13"/>
-      <c r="V55" s="13"/>
-      <c r="W55" s="14">
-        <v>13.635</v>
-      </c>
-      <c r="X55" s="13"/>
-      <c r="Y55" s="14" t="str">
-        <f t="shared" ref="Y55:Y56" si="11">W55&amp;"/"&amp;X55</f>
-        <v>13.635/</v>
-      </c>
-      <c r="AC55" s="52">
-        <f>1000000/1.08 /8</f>
-        <v>115740.74074074073</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="W55" s="14"/>
+      <c r="X55" s="14"/>
+      <c r="Y55" s="14"/>
+      <c r="Z55" s="24">
+        <v>1.08</v>
+      </c>
+      <c r="AB55" s="10">
+        <v>803.52</v>
+      </c>
+      <c r="AC55" s="58"/>
       <c r="AE55" s="16" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="AF55" s="16"/>
       <c r="AG55" s="16" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:33">
+      <c r="A56" s="16" t="s">
+        <v>303</v>
+      </c>
       <c r="B56" s="22" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C56" s="57" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D56" s="14">
-        <v>2</v>
-      </c>
-      <c r="E56" s="14">
-        <v>3584</v>
-      </c>
-      <c r="F56" s="42">
-        <v>9.5</v>
-      </c>
-      <c r="G56" s="42">
-        <v>4.7</v>
-      </c>
-      <c r="H56" s="42">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="I56" s="42">
-        <v>720</v>
-      </c>
-      <c r="J56" s="28">
         <v>1</v>
       </c>
+      <c r="E56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="14">
+        <v>8.74</v>
+      </c>
+      <c r="G56" s="14">
+        <v>2.91</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="14"/>
       <c r="K56" s="57" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="L56" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M56" s="14">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="N56" s="14">
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="O56" s="14">
         <v>16</v>
       </c>
       <c r="P56" s="14">
-        <f t="shared" si="10"/>
-        <v>0.60480000000000012</v>
+        <f t="shared" ref="P56:P58" si="11">M56*N56*O56/1000</f>
+        <v>0.49920000000000003</v>
       </c>
       <c r="Q56" s="14">
-        <v>2400</v>
+        <v>2133</v>
       </c>
       <c r="R56" s="14">
-        <v>256</v>
+        <v>112</v>
       </c>
       <c r="S56" s="57" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="T56" s="14">
-        <v>8000</v>
-      </c>
-      <c r="U56" s="13"/>
-      <c r="V56" s="13"/>
-      <c r="W56" s="14">
-        <v>13.635</v>
-      </c>
-      <c r="X56" s="13"/>
-      <c r="Y56" s="14" t="str">
+        <v>680</v>
+      </c>
+      <c r="W56" s="14"/>
+      <c r="X56" s="14"/>
+      <c r="Y56" s="14"/>
+      <c r="Z56" s="24">
+        <v>2.16</v>
+      </c>
+      <c r="AB56" s="10">
+        <v>1607.04</v>
+      </c>
+      <c r="AC56" s="58"/>
+      <c r="AE56" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AF56" s="16"/>
+    </row>
+    <row r="57" spans="1:33">
+      <c r="A57" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C57" s="57" t="s">
+        <v>282</v>
+      </c>
+      <c r="D57" s="14">
+        <v>2</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="14">
+        <v>8.74</v>
+      </c>
+      <c r="G57" s="14">
+        <v>2.91</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" s="14"/>
+      <c r="K57" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="L57" s="14">
+        <v>1</v>
+      </c>
+      <c r="M57" s="14">
+        <v>24</v>
+      </c>
+      <c r="N57" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="O57" s="14">
+        <v>16</v>
+      </c>
+      <c r="P57" s="14">
         <f t="shared" si="11"/>
-        <v>13.635/</v>
-      </c>
-      <c r="AC56" s="52">
-        <f>1200000/1.08 /8</f>
-        <v>138888.88888888888</v>
-      </c>
-      <c r="AE56" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="AF56" s="16"/>
-      <c r="AG56" s="16" t="s">
+        <v>0.99840000000000007</v>
+      </c>
+      <c r="Q57" s="14">
+        <v>2133</v>
+      </c>
+      <c r="R57" s="14">
+        <v>224</v>
+      </c>
+      <c r="S57" s="57" t="s">
+        <v>292</v>
+      </c>
+      <c r="T57" s="14">
+        <v>1440</v>
+      </c>
+      <c r="W57" s="14"/>
+      <c r="X57" s="14"/>
+      <c r="Y57" s="14"/>
+      <c r="Z57" s="24">
+        <v>4.32</v>
+      </c>
+      <c r="AB57" s="10">
+        <v>3214.08</v>
+      </c>
+      <c r="AC57" s="58"/>
+      <c r="AE57" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="AF57" s="16"/>
+    </row>
+    <row r="58" spans="1:33">
+      <c r="B58" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C58" s="57" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="58" spans="1:33" ht="20">
-      <c r="A58" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="C58" s="57" t="s">
-        <v>292</v>
-      </c>
       <c r="D58" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>17</v>
@@ -9508,13 +9510,13 @@
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="57" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="L58" s="14">
         <v>1</v>
       </c>
       <c r="M58" s="14">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="N58" s="14">
         <v>2.6</v>
@@ -9523,267 +9525,42 @@
         <v>16</v>
       </c>
       <c r="P58" s="14">
-        <f t="shared" ref="P58" si="12">M58*N58*O58/1000</f>
-        <v>0.24960000000000002</v>
+        <f t="shared" si="11"/>
+        <v>0.99840000000000007</v>
       </c>
       <c r="Q58" s="14">
         <v>2133</v>
       </c>
       <c r="R58" s="14">
-        <v>56</v>
+        <v>224</v>
       </c>
       <c r="S58" s="57" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="T58" s="14">
-        <v>380</v>
-      </c>
-      <c r="W58" s="14"/>
+        <v>1440</v>
+      </c>
+      <c r="W58" s="14" t="s">
+        <v>293</v>
+      </c>
       <c r="X58" s="14"/>
-      <c r="Y58" s="14"/>
+      <c r="Y58" s="14" t="str">
+        <f t="shared" ref="Y58" si="12">W58&amp;"/"&amp;X58</f>
+        <v>Infiniband/</v>
+      </c>
       <c r="Z58" s="24">
-        <v>1.08</v>
+        <v>4.7519999999999998</v>
       </c>
       <c r="AB58" s="10">
-        <v>803.52</v>
+        <v>3535.49</v>
       </c>
       <c r="AC58" s="58"/>
       <c r="AE58" s="16" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="AF58" s="16"/>
       <c r="AG58" s="16" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="59" spans="1:33">
-      <c r="A59" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="D59" s="14">
-        <v>1</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="14">
-        <v>8.74</v>
-      </c>
-      <c r="G59" s="14">
-        <v>2.91</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I59" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J59" s="14"/>
-      <c r="K59" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="L59" s="14">
-        <v>1</v>
-      </c>
-      <c r="M59" s="14">
-        <v>12</v>
-      </c>
-      <c r="N59" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="O59" s="14">
-        <v>16</v>
-      </c>
-      <c r="P59" s="14">
-        <f t="shared" ref="P59:P61" si="13">M59*N59*O59/1000</f>
-        <v>0.49920000000000003</v>
-      </c>
-      <c r="Q59" s="14">
-        <v>2133</v>
-      </c>
-      <c r="R59" s="14">
-        <v>112</v>
-      </c>
-      <c r="S59" s="57" t="s">
-        <v>302</v>
-      </c>
-      <c r="T59" s="14">
-        <v>680</v>
-      </c>
-      <c r="W59" s="14"/>
-      <c r="X59" s="14"/>
-      <c r="Y59" s="14"/>
-      <c r="Z59" s="24">
-        <v>2.16</v>
-      </c>
-      <c r="AB59" s="10">
-        <v>1607.04</v>
-      </c>
-      <c r="AC59" s="58"/>
-      <c r="AE59" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="AF59" s="16"/>
-    </row>
-    <row r="60" spans="1:33">
-      <c r="A60" s="16" t="s">
-        <v>294</v>
-      </c>
-      <c r="B60" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="C60" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="D60" s="14">
-        <v>2</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F60" s="14">
-        <v>8.74</v>
-      </c>
-      <c r="G60" s="14">
-        <v>2.91</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J60" s="14"/>
-      <c r="K60" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="L60" s="14">
-        <v>1</v>
-      </c>
-      <c r="M60" s="14">
-        <v>24</v>
-      </c>
-      <c r="N60" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="O60" s="14">
-        <v>16</v>
-      </c>
-      <c r="P60" s="14">
-        <f t="shared" si="13"/>
-        <v>0.99840000000000007</v>
-      </c>
-      <c r="Q60" s="14">
-        <v>2133</v>
-      </c>
-      <c r="R60" s="14">
-        <v>224</v>
-      </c>
-      <c r="S60" s="57" t="s">
-        <v>302</v>
-      </c>
-      <c r="T60" s="14">
-        <v>1440</v>
-      </c>
-      <c r="W60" s="14"/>
-      <c r="X60" s="14"/>
-      <c r="Y60" s="14"/>
-      <c r="Z60" s="24">
-        <v>4.32</v>
-      </c>
-      <c r="AB60" s="10">
-        <v>3214.08</v>
-      </c>
-      <c r="AC60" s="58"/>
-      <c r="AE60" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="AF60" s="16"/>
-    </row>
-    <row r="61" spans="1:33">
-      <c r="B61" s="22" t="s">
         <v>291</v>
-      </c>
-      <c r="C61" s="57" t="s">
-        <v>292</v>
-      </c>
-      <c r="D61" s="14">
-        <v>2</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="14">
-        <v>8.74</v>
-      </c>
-      <c r="G61" s="14">
-        <v>2.91</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J61" s="14"/>
-      <c r="K61" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="L61" s="14">
-        <v>1</v>
-      </c>
-      <c r="M61" s="14">
-        <v>24</v>
-      </c>
-      <c r="N61" s="14">
-        <v>2.6</v>
-      </c>
-      <c r="O61" s="14">
-        <v>16</v>
-      </c>
-      <c r="P61" s="14">
-        <f t="shared" si="13"/>
-        <v>0.99840000000000007</v>
-      </c>
-      <c r="Q61" s="14">
-        <v>2133</v>
-      </c>
-      <c r="R61" s="14">
-        <v>224</v>
-      </c>
-      <c r="S61" s="57" t="s">
-        <v>302</v>
-      </c>
-      <c r="T61" s="14">
-        <v>1440</v>
-      </c>
-      <c r="W61" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="X61" s="14"/>
-      <c r="Y61" s="14" t="str">
-        <f t="shared" ref="Y61" si="14">W61&amp;"/"&amp;X61</f>
-        <v>Infiniband/</v>
-      </c>
-      <c r="Z61" s="24">
-        <v>4.7519999999999998</v>
-      </c>
-      <c r="AB61" s="10">
-        <v>3535.49</v>
-      </c>
-      <c r="AC61" s="58"/>
-      <c r="AE61" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="AF61" s="16"/>
-      <c r="AG61" s="16" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -9796,7 +9573,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AH33">
-    <cfRule type="colorScale" priority="71">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9808,7 +9585,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33">
-    <cfRule type="colorScale" priority="70">
+    <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9820,7 +9597,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AH35">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9832,7 +9609,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9844,7 +9621,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AH35">
-    <cfRule type="colorScale" priority="64">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9856,7 +9633,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AI35">
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9867,33 +9644,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FG19:XFD20 FG31:XFD31 Z31 U30:Y31 T30 S30:S31 R30 Q30:Q31 P30 L29:O31 A28:K30 Z35 A17 B18:I18 A21:Q21 S21:V21 K18:V18 A22:V22 Z18:AD22 W18:W22 A12:AD12 A7:A8 A5:M6 B7:M7 B8:AD9 A23:AD25 A27:M27 L28:M28 N27:O28 A26:O26 P26:AD28 A32:AD32 A34:M34 N34:P35 AH32:XFD34 AH19:AJ20 AH35:AJ35 AH21:XFD30 AG32:AG35 AG18:AG30 AH5:XFD18 AE5:AG5 Q34:X34 AC34:AD34 AB35 A13:AA13 A14:AD16 P29:X29 Z29:AD30 A33:X33 Z33:AD33 Z34:AA34 N5:AD7 AE6:AF36 AG6:AG16 A10:AC11">
-    <cfRule type="expression" dxfId="75" priority="57">
+  <conditionalFormatting sqref="FG19:XFD20 FG31:XFD31 Z31 U30:Y31 T30 S30:S31 R30 Q30:Q31 P30 L29:O31 A28:K30 Z35 A17 B18:I18 A21:Q21 S21:V21 K18:V18 A22:V22 Z18:AD22 W18:W22 A12:AD12 A7:A8 A5:M6 B7:M7 B8:AD9 A23:AD25 A27:M27 L28:M28 N27:O28 A26:O26 P26:AD28 A32:AD32 A34:M34 N34:P35 AH32:XFD34 AH19:AJ20 AH35:AJ35 AH21:XFD30 AG32:AG35 AG18:AG30 AH5:XFD18 AE5:AG5 Q34:X34 AC34:AD34 AB35 A13:AA13 A14:AD16 P29:X29 Z29:AD30 A33:X33 Z33:AD33 Z34:AA34 N5:AD7 AE6:AF36 AG6:AG16 A10:AC11 P50:P53 Y50:Y53 AE50:AF52 AE53">
+    <cfRule type="expression" dxfId="76" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB13">
+    <cfRule type="expression" dxfId="75" priority="45">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
     <cfRule type="expression" dxfId="74" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
+  <conditionalFormatting sqref="K35:M35 Q35:X35">
     <cfRule type="expression" dxfId="73" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K35:M35 Q35:X35">
+  <conditionalFormatting sqref="AB34">
     <cfRule type="expression" dxfId="72" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB34">
-    <cfRule type="expression" dxfId="71" priority="41">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AH35 AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="142">
+    <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9905,7 +9682,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32:AI35 AI21:AI30 AI5:AI18">
-    <cfRule type="colorScale" priority="146">
+    <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9917,7 +9694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AH33 AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="150">
+    <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9929,7 +9706,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI32:AI33 AI21:AI30 AI5:AI18">
-    <cfRule type="colorScale" priority="154">
+    <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9941,7 +9718,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32:AJ35 AJ21:AJ30 AJ5:AJ18">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9953,7 +9730,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH21:AH30 AH5:AH18">
-    <cfRule type="colorScale" priority="162">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9965,7 +9742,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21:AI30 AI5:AI18">
-    <cfRule type="colorScale" priority="165">
+    <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9977,12 +9754,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:Q20 S20:V20">
-    <cfRule type="expression" dxfId="70" priority="33">
+    <cfRule type="expression" dxfId="71" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9994,7 +9771,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10006,7 +9783,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10018,7 +9795,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10030,7 +9807,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10042,7 +9819,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10054,7 +9831,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10066,17 +9843,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="69" priority="24">
+    <cfRule type="expression" dxfId="70" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 R20:R21 K19:V19">
-    <cfRule type="expression" dxfId="68" priority="25">
+    <cfRule type="expression" dxfId="69" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10088,7 +9865,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10100,7 +9877,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10112,7 +9889,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10124,7 +9901,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10136,7 +9913,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10148,7 +9925,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10160,128 +9937,108 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
+    <cfRule type="expression" dxfId="68" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y17:Y22">
     <cfRule type="expression" dxfId="67" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y17:Y22">
+  <conditionalFormatting sqref="Y29">
     <cfRule type="expression" dxfId="66" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y29">
+  <conditionalFormatting sqref="Y33:Y35">
     <cfRule type="expression" dxfId="65" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y33:Y35">
+  <conditionalFormatting sqref="Y37:Y39">
     <cfRule type="expression" dxfId="64" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y37:Y39">
+  <conditionalFormatting sqref="P44">
     <cfRule type="expression" dxfId="63" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P44">
+  <conditionalFormatting sqref="Y44:Y48">
     <cfRule type="expression" dxfId="62" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y44:Y48">
+  <conditionalFormatting sqref="P42:P43">
     <cfRule type="expression" dxfId="61" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P42:P43">
+  <conditionalFormatting sqref="Y42:Y43">
     <cfRule type="expression" dxfId="60" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y42:Y43">
+  <conditionalFormatting sqref="P48">
     <cfRule type="expression" dxfId="59" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P48">
-    <cfRule type="expression" dxfId="58" priority="14">
+  <conditionalFormatting sqref="M55:P55 N56:P58">
+    <cfRule type="expression" dxfId="57" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P50:P54">
-    <cfRule type="expression" dxfId="57" priority="13">
+  <conditionalFormatting sqref="Q55:Q58">
+    <cfRule type="expression" dxfId="55" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y50:Y54">
-    <cfRule type="expression" dxfId="56" priority="12">
+  <conditionalFormatting sqref="Y58">
+    <cfRule type="expression" dxfId="54" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE50:AF56">
-    <cfRule type="expression" dxfId="55" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P55:P56">
-    <cfRule type="expression" dxfId="54" priority="10">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y55:Y56">
-    <cfRule type="expression" dxfId="53" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M58:P58 N59:P61">
-    <cfRule type="expression" dxfId="52" priority="8">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q58:Q61">
-    <cfRule type="expression" dxfId="51" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y61">
-    <cfRule type="expression" dxfId="50" priority="6">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58:I61">
-    <cfRule type="expression" dxfId="49" priority="5">
+  <conditionalFormatting sqref="E55:I58">
+    <cfRule type="expression" dxfId="53" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C47">
-    <cfRule type="expression" dxfId="48" priority="4">
+    <cfRule type="expression" dxfId="52" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:I47">
-    <cfRule type="expression" dxfId="47" priority="3">
+    <cfRule type="expression" dxfId="51" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P45:P46">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="50" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P47">
-    <cfRule type="expression" dxfId="45" priority="1">
+    <cfRule type="expression" dxfId="49" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF53">
+    <cfRule type="expression" dxfId="48" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A18" r:id="rId1"/>
-    <hyperlink ref="A52" r:id="rId2"/>
+    <hyperlink ref="A51" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="56" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="Y50:Y54" emptyCellReference="1"/>
+    <ignoredError sqref="Y50:Y51 Y52:Y53" emptyCellReference="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId3"/>
   <extLst>
@@ -10295,13 +10052,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC67"/>
+  <dimension ref="A1:AC69"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="R46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomRight" activeCell="V63" sqref="V63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -10395,10 +10152,10 @@
         <v>217</v>
       </c>
       <c r="X1" s="48" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="Y1" s="48" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="12" customFormat="1" ht="21" thickBot="1">
@@ -10472,7 +10229,7 @@
         <v>137</v>
       </c>
       <c r="X2" s="30" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="Y2" s="30" t="s">
         <v>138</v>
@@ -10590,7 +10347,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19" t="str">
-        <f t="shared" ref="K4:K67" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="K4:K69" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L4" s="14">
@@ -12511,7 +12268,7 @@
       </c>
       <c r="X27" s="14"/>
       <c r="Y27" s="16">
-        <f t="shared" ref="Y27:Y67" ca="1" si="15">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="Y27:Y69" ca="1" si="15">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="Z27" s="16"/>
@@ -12963,11 +12720,11 @@
         <v>EUR</v>
       </c>
       <c r="L33" s="14">
-        <f t="shared" ref="L33:L67" ca="1" si="17">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L33:L69" ca="1" si="17">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.43519999999999998</v>
       </c>
       <c r="M33" s="14">
-        <f t="shared" ref="M33:M67" ca="1" si="18">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M33:M69" ca="1" si="18">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>16.456</v>
       </c>
       <c r="N33" s="14" t="str">
@@ -14192,7 +13949,7 @@
         <v>19</v>
       </c>
       <c r="N49" s="14" t="str">
-        <f t="shared" ref="N49:X64" ca="1" si="20">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N49:X66" ca="1" si="20">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>P100</v>
       </c>
       <c r="O49" s="14">
@@ -14478,7 +14235,7 @@
         <v>2 x Titan X minutely</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="F53" s="13">
         <f t="shared" ref="F53" ca="1" si="24">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14553,7 +14310,7 @@
         <v>2 x Titan X  monthly</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F54" s="43"/>
       <c r="G54" s="19">
@@ -14631,7 +14388,7 @@
         <v>4 x Titan X minutely</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="F55" s="43">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14706,7 +14463,7 @@
         <v>4 x Titan X monthly</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F56" s="43"/>
       <c r="G56" s="43"/>
@@ -14775,7 +14532,7 @@
         <v>8 x Titan X minutely</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="F57" s="43">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14848,14 +14605,14 @@
         <v>8 x Titan X monthly</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="H58">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>3408.81</v>
       </c>
       <c r="I58" s="19">
-        <f t="shared" ref="I58:I63" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="I58:I65" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K58" s="19" t="str">
@@ -15138,14 +14895,14 @@
         <v>The University of Tokyo</v>
       </c>
       <c r="B62" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="C62" s="22" t="str">
-        <f t="shared" ref="C62:C67" ca="1" si="27">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C62:C69" ca="1" si="27">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="I62" s="19">
         <f t="shared" ca="1" si="26"/>
@@ -15209,7 +14966,7 @@
       </c>
       <c r="Y62" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used simulateously.</v>
+        <v>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
       </c>
       <c r="AC62" s="45">
         <v>50</v>
@@ -15218,10 +14975,10 @@
     <row r="63" spans="1:29">
       <c r="C63" s="22" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>Reedbush-H Group 4 (educational)</v>
+        <v>Reedbush-H (educational)</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>287</v>
+        <v>325</v>
       </c>
       <c r="I63" s="19">
         <f t="shared" ca="1" si="26"/>
@@ -15285,168 +15042,182 @@
       </c>
       <c r="Y63" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Included 13824 node hours if 1 node is used, 6912 node hours if more than 1 node is used simultaneously.</v>
+        <v>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
       </c>
       <c r="AC63" s="45">
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="20">
-      <c r="A64" s="60" t="str">
+    <row r="64" spans="1:29" s="13" customFormat="1">
+      <c r="C64" s="22" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>Reedbush-H reviewed (educational)</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="I64" s="19">
+        <f t="shared" ca="1" si="26"/>
+        <v>166666.66666666666</v>
+      </c>
+      <c r="K64" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>JPY</v>
+      </c>
+      <c r="L64" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.2096000000000002</v>
+      </c>
+      <c r="M64" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N64" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>P100</v>
+      </c>
+      <c r="O64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P64" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v xml:space="preserve">Xeon E5-2695v4 </v>
+      </c>
+      <c r="Q64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>256</v>
+      </c>
+      <c r="S64" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>PFS</v>
+      </c>
+      <c r="T64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>4000</v>
+      </c>
+      <c r="U64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W64" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>13.635/</v>
+      </c>
+      <c r="X64" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>8640</v>
+      </c>
+      <c r="Y64" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+      </c>
+      <c r="AC64" s="45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" s="13" customFormat="1">
+      <c r="C65" s="22" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>Reedbush-H reviewed</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="I65" s="19">
+        <f t="shared" ca="1" si="26"/>
+        <v>200000</v>
+      </c>
+      <c r="K65" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>JPY</v>
+      </c>
+      <c r="L65" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.2096000000000002</v>
+      </c>
+      <c r="M65" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="N65" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>P100</v>
+      </c>
+      <c r="O65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="P65" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v xml:space="preserve">Xeon E5-2695v4 </v>
+      </c>
+      <c r="Q65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="R65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>256</v>
+      </c>
+      <c r="S65" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>PFS</v>
+      </c>
+      <c r="T65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>4000</v>
+      </c>
+      <c r="U65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="V65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="W65" s="14" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>13.635/</v>
+      </c>
+      <c r="X65" s="14">
+        <f t="shared" ca="1" si="20"/>
+        <v>8640</v>
+      </c>
+      <c r="Y65" s="16" t="str">
+        <f t="shared" ca="1" si="15"/>
+        <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+      </c>
+      <c r="AC65" s="45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" ht="20">
+      <c r="A66" s="60" t="str">
         <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>MS Azure</v>
       </c>
-      <c r="B64" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C64" s="22" t="str">
+      <c r="B66" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C66" s="22" t="str">
         <f t="shared" ca="1" si="27"/>
         <v>NC6</v>
       </c>
-      <c r="E64" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="F64" s="13">
-        <f t="shared" ref="F64:F67" ca="1" si="28">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+      <c r="E66" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="F66" s="13">
+        <f t="shared" ref="F66:F69" ca="1" si="28">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>1.08</v>
-      </c>
-      <c r="K64" s="19" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>USD</v>
-      </c>
-      <c r="L64" s="14">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.24960000000000002</v>
-      </c>
-      <c r="M64" s="14">
-        <f t="shared" ca="1" si="18"/>
-        <v>4.37</v>
-      </c>
-      <c r="N64" s="14" t="str">
-        <f t="shared" ref="N64:V67" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>K80</v>
-      </c>
-      <c r="O64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>0.5</v>
-      </c>
-      <c r="P64" s="61" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v>Xeon E5-2690v3</v>
-      </c>
-      <c r="Q64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="R64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>56</v>
-      </c>
-      <c r="S64" s="14" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v>SSD</v>
-      </c>
-      <c r="T64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>380</v>
-      </c>
-      <c r="U64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="V64" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="W64" s="14">
-        <f t="shared" ca="1" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="X64" s="14"/>
-      <c r="Y64" s="16" t="str">
-        <f t="shared" ca="1" si="15"/>
-        <v xml:space="preserve">1 GPU in specification is 1/2 of K80 </v>
-      </c>
-      <c r="AC64" s="45">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="65" spans="3:29">
-      <c r="C65" s="22" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>NC12</v>
-      </c>
-      <c r="E65" s="22" t="s">
-        <v>305</v>
-      </c>
-      <c r="F65" s="13">
-        <f t="shared" ca="1" si="28"/>
-        <v>2.16</v>
-      </c>
-      <c r="K65" s="19" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>USD</v>
-      </c>
-      <c r="L65" s="14">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.49920000000000003</v>
-      </c>
-      <c r="M65" s="14">
-        <f t="shared" ca="1" si="18"/>
-        <v>8.74</v>
-      </c>
-      <c r="N65" s="14" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v>K80</v>
-      </c>
-      <c r="O65" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="P65" s="61" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v>Xeon E5-2690v3</v>
-      </c>
-      <c r="Q65" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="R65" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>112</v>
-      </c>
-      <c r="S65" s="14" t="str">
-        <f t="shared" ca="1" si="29"/>
-        <v>SSD</v>
-      </c>
-      <c r="T65" s="14">
-        <f t="shared" ca="1" si="29"/>
-        <v>680</v>
-      </c>
-      <c r="W65" s="14">
-        <f t="shared" ref="W65:W67" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>0</v>
-      </c>
-      <c r="X65" s="14"/>
-      <c r="Y65" s="16">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="AC65" s="45">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" spans="3:29">
-      <c r="C66" s="22" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>NC24</v>
-      </c>
-      <c r="E66" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="F66" s="13">
-        <f t="shared" ca="1" si="28"/>
-        <v>4.32</v>
       </c>
       <c r="K66" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -15454,19 +15225,19 @@
       </c>
       <c r="L66" s="14">
         <f t="shared" ca="1" si="17"/>
-        <v>0.99840000000000007</v>
+        <v>0.24960000000000002</v>
       </c>
       <c r="M66" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>17.48</v>
+        <v>4.37</v>
       </c>
       <c r="N66" s="14" t="str">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ref="N66:V69" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O66" s="14">
         <f t="shared" ca="1" si="29"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="P66" s="61" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -15478,7 +15249,7 @@
       </c>
       <c r="R66" s="14">
         <f t="shared" ca="1" si="29"/>
-        <v>224</v>
+        <v>56</v>
       </c>
       <c r="S66" s="14" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -15486,32 +15257,40 @@
       </c>
       <c r="T66" s="14">
         <f t="shared" ca="1" si="29"/>
-        <v>1440</v>
+        <v>380</v>
+      </c>
+      <c r="U66" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="V66" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
       </c>
       <c r="W66" s="14">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0</v>
       </c>
       <c r="X66" s="14"/>
-      <c r="Y66" s="16">
+      <c r="Y66" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v xml:space="preserve">1 GPU in specification is 1/2 of K80 </v>
       </c>
       <c r="AC66" s="45">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="67" spans="3:29">
+    <row r="67" spans="1:29">
       <c r="C67" s="22" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>NC24r</v>
+        <v>NC12</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="F67" s="13">
         <f t="shared" ca="1" si="28"/>
-        <v>4.7519999999999998</v>
+        <v>2.16</v>
       </c>
       <c r="K67" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -15519,11 +15298,11 @@
       </c>
       <c r="L67" s="14">
         <f t="shared" ca="1" si="17"/>
-        <v>0.99840000000000007</v>
+        <v>0.49920000000000003</v>
       </c>
       <c r="M67" s="14">
         <f t="shared" ca="1" si="18"/>
-        <v>17.48</v>
+        <v>8.74</v>
       </c>
       <c r="N67" s="14" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -15531,7 +15310,7 @@
       </c>
       <c r="O67" s="14">
         <f t="shared" ca="1" si="29"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P67" s="61" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -15543,7 +15322,7 @@
       </c>
       <c r="R67" s="14">
         <f t="shared" ca="1" si="29"/>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="S67" s="14" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -15551,245 +15330,375 @@
       </c>
       <c r="T67" s="14">
         <f t="shared" ca="1" si="29"/>
+        <v>680</v>
+      </c>
+      <c r="W67" s="14">
+        <f t="shared" ref="W67:W69" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>0</v>
+      </c>
+      <c r="X67" s="14"/>
+      <c r="Y67" s="16">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC67" s="45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:29">
+      <c r="C68" s="22" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>NC24</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="F68" s="13">
+        <f t="shared" ca="1" si="28"/>
+        <v>4.32</v>
+      </c>
+      <c r="K68" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>USD</v>
+      </c>
+      <c r="L68" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.99840000000000007</v>
+      </c>
+      <c r="M68" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>17.48</v>
+      </c>
+      <c r="N68" s="14" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>K80</v>
+      </c>
+      <c r="O68" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="P68" s="61" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>Xeon E5-2690v3</v>
+      </c>
+      <c r="Q68" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="R68" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>224</v>
+      </c>
+      <c r="S68" s="14" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>SSD</v>
+      </c>
+      <c r="T68" s="14">
+        <f t="shared" ca="1" si="29"/>
         <v>1440</v>
       </c>
-      <c r="W67" s="14" t="str">
+      <c r="W68" s="14">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="X68" s="14"/>
+      <c r="Y68" s="16">
+        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC68" s="45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29">
+      <c r="C69" s="22" t="str">
+        <f t="shared" ca="1" si="27"/>
+        <v>NC24r</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="F69" s="13">
+        <f t="shared" ca="1" si="28"/>
+        <v>4.7519999999999998</v>
+      </c>
+      <c r="K69" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>USD</v>
+      </c>
+      <c r="L69" s="14">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.99840000000000007</v>
+      </c>
+      <c r="M69" s="14">
+        <f t="shared" ca="1" si="18"/>
+        <v>17.48</v>
+      </c>
+      <c r="N69" s="14" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>K80</v>
+      </c>
+      <c r="O69" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="P69" s="61" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>Xeon E5-2690v3</v>
+      </c>
+      <c r="Q69" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="R69" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>224</v>
+      </c>
+      <c r="S69" s="14" t="str">
+        <f t="shared" ca="1" si="29"/>
+        <v>SSD</v>
+      </c>
+      <c r="T69" s="14">
+        <f t="shared" ca="1" si="29"/>
+        <v>1440</v>
+      </c>
+      <c r="W69" s="14" t="str">
         <f t="shared" ca="1" si="30"/>
         <v>Infiniband/</v>
       </c>
-      <c r="X67" s="14"/>
-      <c r="Y67" s="16" t="str">
+      <c r="X69" s="14"/>
+      <c r="Y69" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
         <v>RDMA capable</v>
       </c>
-      <c r="AC67" s="45">
-        <v>61</v>
+      <c r="AC69" s="45">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 F25:G25 F29:G29 H22:H31 S13:S15 E23:G23 E18:J22 C30:C32 E26:G28 D26:D33 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 K4:K35 E30:I32 M32:O41 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8 I58:I63 H50:H52 L42:S61 T45:Y61 K48:K64 K65:T67 L64:V64 L62:Y63 W64:Y67">
-    <cfRule type="expression" dxfId="44" priority="113">
+  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 F25:G25 F29:G29 H22:H31 S13:S15 E23:G23 E18:J22 C30:C32 E26:G28 D26:D33 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 K4:K35 E30:I32 M32:O41 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8 H50:H52 L42:S61 T45:Y61 K67:T69 L66:V66 W66:Y69 I58:I65 K48:K66 L62:Y65">
+    <cfRule type="expression" dxfId="47" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 I24:J24 F24:G24">
-    <cfRule type="expression" dxfId="43" priority="111">
+    <cfRule type="expression" dxfId="46" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:J26">
-    <cfRule type="expression" dxfId="42" priority="110">
+    <cfRule type="expression" dxfId="45" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:J28">
-    <cfRule type="expression" dxfId="41" priority="109">
+    <cfRule type="expression" dxfId="44" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="40" priority="100">
+    <cfRule type="expression" dxfId="43" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P15 P18:P41">
-    <cfRule type="expression" dxfId="39" priority="55">
+    <cfRule type="expression" dxfId="42" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:X3 T4:X12 T18:V31 T13:V15 W13:X31 R3:R15 R18:R41 Y6:Y41 T32:X38 U39:X41 T39:T44">
-    <cfRule type="expression" dxfId="38" priority="53">
+    <cfRule type="expression" dxfId="41" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="expression" dxfId="37" priority="62">
+    <cfRule type="expression" dxfId="40" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C25">
-    <cfRule type="expression" dxfId="36" priority="61">
+    <cfRule type="expression" dxfId="39" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C27">
-    <cfRule type="expression" dxfId="35" priority="60">
+    <cfRule type="expression" dxfId="38" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="expression" dxfId="34" priority="59">
+    <cfRule type="expression" dxfId="37" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q15 Q18:Q41">
-    <cfRule type="expression" dxfId="33" priority="54">
+    <cfRule type="expression" dxfId="36" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S12">
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="35" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18:S41">
-    <cfRule type="expression" dxfId="31" priority="51">
+    <cfRule type="expression" dxfId="34" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:J17 N17:O17">
-    <cfRule type="expression" dxfId="30" priority="42">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P17">
-    <cfRule type="expression" dxfId="29" priority="41">
+    <cfRule type="expression" dxfId="32" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:V17 R16:R17">
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="31" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16:Q17">
-    <cfRule type="expression" dxfId="27" priority="40">
+    <cfRule type="expression" dxfId="30" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17">
-    <cfRule type="expression" dxfId="26" priority="38">
+    <cfRule type="expression" dxfId="29" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="25" priority="37">
+    <cfRule type="expression" dxfId="28" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="27" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="23" priority="35">
+    <cfRule type="expression" dxfId="26" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32:L41">
-    <cfRule type="expression" dxfId="22" priority="34">
+    <cfRule type="expression" dxfId="25" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="21" priority="33">
+    <cfRule type="expression" dxfId="24" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="23" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="expression" dxfId="19" priority="31">
+    <cfRule type="expression" dxfId="22" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="18" priority="29">
+    <cfRule type="expression" dxfId="21" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:J32">
-    <cfRule type="expression" dxfId="17" priority="28">
+    <cfRule type="expression" dxfId="20" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36 K36:K47">
-    <cfRule type="expression" dxfId="16" priority="27">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="expression" dxfId="15" priority="26">
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="12" priority="19">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="expression" dxfId="11" priority="18">
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="10" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U42:Y44">
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H57">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49 G54">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated MS NC offers. Added NV offers.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -652,12 +652,64 @@
         </r>
       </text>
     </comment>
+    <comment ref="E63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+http://images.nvidia.com/content/pdf/tesla/tesla-m60-product-brief.pdf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+https://en.wikipedia.org/wiki/List_of_Nvidia_graphics_processing_units</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="350">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1706,295 +1758,324 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
+  </si>
+  <si>
+    <t>NC6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2690v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>RDMA capable</t>
+  </si>
+  <si>
+    <t>Infiniband</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Titan X</t>
+  </si>
+  <si>
+    <t>4 x Titan X</t>
+  </si>
+  <si>
+    <t>8 x Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TITAN X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GeForce GTX Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2609 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC25r</t>
+  </si>
+  <si>
+    <t>MS NC24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.leadergpu.com</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx4 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx4 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx8 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx8 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Nodes*hours limit</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AF</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AG</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Max hours</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU gen edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Limited quantity available at this price</t>
+  </si>
+  <si>
+    <t>8-GPU x86 P40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 P40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Quadro P600</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-1650 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU POWER8/10 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x8 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x8 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>16-GPU x86 K80 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 M40 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86 ltd m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86 ltd w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR M40x8 ltd x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR M40x8 ltd x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LeaderTelecom</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x GeForce GTX 1080 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>http://venturebeat.com/2016/08/04/microsoft-azure-releases-n-series-gpu-instances-in-preview/</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
-  </si>
-  <si>
-    <t>NC6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2690v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>RDMA capable</t>
-  </si>
-  <si>
-    <t>SSD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Infiniband</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x Titan X</t>
-  </si>
-  <si>
-    <t>4 x Titan X</t>
-  </si>
-  <si>
-    <t>8 x Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TITAN X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GeForce GTX Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2609 v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC25r</t>
-  </si>
-  <si>
-    <t>MS NC24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.leadergpu.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx2 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx2 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx4 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx4 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx8 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx8 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Nodes*hours limit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AF</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AG</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Max hours</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H reviewed (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H reviewed</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU gen edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU rev</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU rev edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Limited quantity available at this price</t>
-  </si>
-  <si>
-    <t>8-GPU x86 P40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 Quadro P6000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 P40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 Quadro P6000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Quadro P600</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-1650 v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU POWER8/10 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x8 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>16-GPU x86 K80 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 M40 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86 ltd m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86 ltd w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 ltd x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 ltd x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LeaderTelecom</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4 x GeForce GTX 1080 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SATA</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV24</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2380,7 +2461,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="706">
+  <cellStyleXfs count="708">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3031,6 +3112,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3222,7 +3305,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="706">
+  <cellStyles count="708">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3635,6 +3718,8 @@
     <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -3930,7 +4015,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="79">
+  <dxfs count="80">
     <dxf>
       <font>
         <color auto="1"/>
@@ -4800,6 +4885,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -5095,13 +5191,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FF62"/>
+  <dimension ref="A1:FF65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="L24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5197,7 +5293,7 @@
       <c r="AD3" s="63"/>
       <c r="AE3" s="63"/>
       <c r="AF3" s="17" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AG3" s="1" t="s">
         <v>32</v>
@@ -5495,7 +5591,7 @@
       </c>
       <c r="AF5" s="16"/>
       <c r="AG5" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:162">
@@ -5569,7 +5665,7 @@
       </c>
       <c r="AF6" s="16"/>
       <c r="AG6" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:162">
@@ -5643,7 +5739,7 @@
       </c>
       <c r="AF7" s="16"/>
       <c r="AG7" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:162">
@@ -6968,7 +7064,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>16</v>
@@ -7049,7 +7145,7 @@
       </c>
       <c r="AF25" s="16"/>
       <c r="AG25" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:162">
@@ -7057,7 +7153,7 @@
         <v>62</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>41</v>
@@ -7138,13 +7234,13 @@
       </c>
       <c r="AF26" s="16"/>
       <c r="AG26" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:162" s="13" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>93</v>
@@ -7229,7 +7325,7 @@
     <row r="28" spans="1:162" s="13" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>94</v>
@@ -7314,10 +7410,10 @@
     <row r="29" spans="1:162" s="13" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D29" s="13">
         <v>8</v>
@@ -7396,7 +7492,7 @@
     <row r="30" spans="1:162" s="13" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="22" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>93</v>
@@ -7421,7 +7517,7 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L30" s="5">
         <v>1</v>
@@ -7478,7 +7574,7 @@
     <row r="31" spans="1:162" s="13" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>35</v>
@@ -7503,7 +7599,7 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L31" s="5">
         <v>1</v>
@@ -7560,10 +7656,10 @@
     <row r="32" spans="1:162" s="13" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D32" s="13">
         <v>4</v>
@@ -7585,7 +7681,7 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="L32" s="5">
         <v>1</v>
@@ -7641,7 +7737,7 @@
     </row>
     <row r="33" spans="1:162">
       <c r="B33" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>78</v>
@@ -7725,7 +7821,7 @@
     </row>
     <row r="34" spans="1:162">
       <c r="B34" s="22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>79</v>
@@ -7802,7 +7898,7 @@
     <row r="35" spans="1:162" s="13" customFormat="1">
       <c r="A35" s="40"/>
       <c r="B35" s="41" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>138</v>
@@ -8045,7 +8141,7 @@
         <v>49</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D37" s="28">
         <v>4</v>
@@ -8325,7 +8421,7 @@
     </row>
     <row r="41" spans="1:162" ht="23" customHeight="1">
       <c r="A41" s="21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>176</v>
@@ -8415,10 +8511,10 @@
     </row>
     <row r="42" spans="1:162" ht="24" customHeight="1">
       <c r="A42" s="16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C42" s="28" t="s">
         <v>178</v>
@@ -9018,10 +9114,10 @@
     <row r="49" spans="1:33" s="13" customFormat="1">
       <c r="A49" s="2"/>
       <c r="B49" s="59" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D49" s="14">
         <v>2</v>
@@ -9104,10 +9200,10 @@
     <row r="50" spans="1:33" s="13" customFormat="1">
       <c r="A50" s="2"/>
       <c r="B50" s="59" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D50" s="14">
         <v>4</v>
@@ -9129,7 +9225,7 @@
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L50" s="28">
         <v>2</v>
@@ -9190,10 +9286,10 @@
     <row r="51" spans="1:33" s="13" customFormat="1">
       <c r="A51" s="2"/>
       <c r="B51" s="59" t="s">
+        <v>281</v>
+      </c>
+      <c r="C51" s="28" t="s">
         <v>283</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>285</v>
       </c>
       <c r="D51" s="14">
         <v>8</v>
@@ -9442,15 +9538,15 @@
         <v>6912</v>
       </c>
       <c r="AG54" s="16" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:33">
       <c r="A55" s="16" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C55" s="57" t="s">
         <v>254</v>
@@ -9528,12 +9624,12 @@
         <v>13824</v>
       </c>
       <c r="AG55" s="16" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:33">
       <c r="B56" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C56" s="57" t="s">
         <v>254</v>
@@ -9609,12 +9705,12 @@
         <v>8640</v>
       </c>
       <c r="AG56" s="62" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:33">
       <c r="B57" s="22" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C57" s="57" t="s">
         <v>254</v>
@@ -9690,7 +9786,7 @@
         <v>8640</v>
       </c>
       <c r="AG57" s="62" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:33" ht="20">
@@ -9698,7 +9794,7 @@
         <v>262</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C59" s="57" t="s">
         <v>266</v>
@@ -9723,7 +9819,7 @@
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L59" s="14">
         <v>1</v>
@@ -9748,7 +9844,7 @@
         <v>56</v>
       </c>
       <c r="S59" s="57" t="s">
-        <v>276</v>
+        <v>346</v>
       </c>
       <c r="T59" s="14">
         <v>380</v>
@@ -9757,10 +9853,11 @@
       <c r="X59" s="14"/>
       <c r="Y59" s="14"/>
       <c r="Z59" s="24">
-        <v>1.08</v>
+        <v>0.9</v>
       </c>
       <c r="AB59" s="10">
-        <v>803.52</v>
+        <f>Z59*24*31</f>
+        <v>669.6</v>
       </c>
       <c r="AC59" s="58"/>
       <c r="AE59" s="16" t="s">
@@ -9768,12 +9865,12 @@
       </c>
       <c r="AF59" s="16"/>
       <c r="AG59" s="16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:33">
       <c r="A60" s="16" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="B60" s="22" t="s">
         <v>263</v>
@@ -9801,7 +9898,7 @@
       </c>
       <c r="J60" s="14"/>
       <c r="K60" s="57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L60" s="14">
         <v>1</v>
@@ -9826,7 +9923,7 @@
         <v>112</v>
       </c>
       <c r="S60" s="57" t="s">
-        <v>276</v>
+        <v>346</v>
       </c>
       <c r="T60" s="14">
         <v>680</v>
@@ -9835,10 +9932,11 @@
       <c r="X60" s="14"/>
       <c r="Y60" s="14"/>
       <c r="Z60" s="24">
-        <v>2.16</v>
+        <v>1.8</v>
       </c>
       <c r="AB60" s="10">
-        <v>1607.04</v>
+        <f t="shared" ref="AB60:AB62" si="14">Z60*24*31</f>
+        <v>1339.2</v>
       </c>
       <c r="AC60" s="58"/>
       <c r="AE60" s="16" t="s">
@@ -9848,7 +9946,7 @@
     </row>
     <row r="61" spans="1:33">
       <c r="A61" s="16" t="s">
-        <v>268</v>
+        <v>344</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>264</v>
@@ -9876,7 +9974,7 @@
       </c>
       <c r="J61" s="14"/>
       <c r="K61" s="57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L61" s="14">
         <v>1</v>
@@ -9901,7 +9999,7 @@
         <v>224</v>
       </c>
       <c r="S61" s="57" t="s">
-        <v>276</v>
+        <v>346</v>
       </c>
       <c r="T61" s="14">
         <v>1440</v>
@@ -9910,10 +10008,11 @@
       <c r="X61" s="14"/>
       <c r="Y61" s="14"/>
       <c r="Z61" s="24">
-        <v>4.32</v>
+        <v>3.6</v>
       </c>
       <c r="AB61" s="10">
-        <v>3214.08</v>
+        <f t="shared" si="14"/>
+        <v>2678.4</v>
       </c>
       <c r="AC61" s="58"/>
       <c r="AE61" s="16" t="s">
@@ -9948,7 +10047,7 @@
       </c>
       <c r="J62" s="14"/>
       <c r="K62" s="57" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L62" s="14">
         <v>1</v>
@@ -9973,24 +10072,25 @@
         <v>224</v>
       </c>
       <c r="S62" s="57" t="s">
-        <v>276</v>
+        <v>346</v>
       </c>
       <c r="T62" s="14">
         <v>1440</v>
       </c>
       <c r="W62" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="X62" s="14"/>
       <c r="Y62" s="14" t="str">
-        <f t="shared" ref="Y62" si="14">W62&amp;"/"&amp;X62</f>
+        <f t="shared" ref="Y62" si="15">W62&amp;"/"&amp;X62</f>
         <v>Infiniband/</v>
       </c>
       <c r="Z62" s="24">
-        <v>4.7519999999999998</v>
+        <v>3.96</v>
       </c>
       <c r="AB62" s="10">
-        <v>3535.49</v>
+        <f t="shared" si="14"/>
+        <v>2946.24</v>
       </c>
       <c r="AC62" s="58"/>
       <c r="AE62" s="16" t="s">
@@ -9998,7 +10098,196 @@
       </c>
       <c r="AF62" s="16"/>
       <c r="AG62" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33">
+      <c r="B63" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="C63" t="s">
+        <v>343</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F63" s="9">
+        <v>9.65</v>
+      </c>
+      <c r="G63" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K63" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="L63" s="14">
+        <v>1</v>
+      </c>
+      <c r="M63" s="14">
+        <v>6</v>
+      </c>
+      <c r="N63" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="O63" s="14">
+        <v>16</v>
+      </c>
+      <c r="P63" s="14">
+        <f t="shared" ref="P63:P65" si="16">M63*N63*O63/1000</f>
+        <v>0.24960000000000002</v>
+      </c>
+      <c r="Q63" s="14">
+        <v>2133</v>
+      </c>
+      <c r="R63">
+        <v>56</v>
+      </c>
+      <c r="S63" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="T63">
+        <v>340</v>
+      </c>
+      <c r="Z63" s="24">
+        <v>1.24</v>
+      </c>
+      <c r="AE63" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33">
+      <c r="B64" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F64" s="9">
+        <v>9.65</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K64" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="L64" s="14">
+        <v>1</v>
+      </c>
+      <c r="M64" s="14">
+        <v>12</v>
+      </c>
+      <c r="N64" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="O64" s="14">
+        <v>16</v>
+      </c>
+      <c r="P64" s="14">
+        <f t="shared" si="16"/>
+        <v>0.49920000000000003</v>
+      </c>
+      <c r="Q64" s="14">
+        <v>2133</v>
+      </c>
+      <c r="R64">
+        <v>112</v>
+      </c>
+      <c r="S64" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="T64">
+        <v>680</v>
+      </c>
+      <c r="Z64" s="24">
+        <v>2.48</v>
+      </c>
+      <c r="AE64" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="65" spans="2:31">
+      <c r="B65" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" s="9">
+        <v>9.65</v>
+      </c>
+      <c r="G65" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K65" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="L65" s="14">
+        <v>1</v>
+      </c>
+      <c r="M65" s="14">
+        <v>24</v>
+      </c>
+      <c r="N65" s="14">
+        <v>2.6</v>
+      </c>
+      <c r="O65" s="14">
+        <v>16</v>
+      </c>
+      <c r="P65" s="14">
+        <f t="shared" si="16"/>
+        <v>0.99840000000000007</v>
+      </c>
+      <c r="Q65" s="14">
+        <v>2133</v>
+      </c>
+      <c r="R65">
+        <v>224</v>
+      </c>
+      <c r="S65" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="T65">
+        <v>1440</v>
+      </c>
+      <c r="Z65" s="24">
+        <v>4.97</v>
+      </c>
+      <c r="AE65" s="16" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -10011,7 +10300,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AH37">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10023,7 +10312,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI37">
-    <cfRule type="colorScale" priority="72">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10035,7 +10324,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH38:AH39">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10047,7 +10336,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10059,7 +10348,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH38:AH39">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10071,7 +10360,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10083,32 +10372,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG19:XFD20 FG35:XFD35 Z35 U34:Y35 T34 S34:S35 R34 Q34:Q35 P34 Z39 A17 B18:I18 A21:Q21 S21:V21 K18:V18 A22:V22 Z18:AD22 W18:W22 A12:AD12 A7:A8 A5:M6 B7:M7 B8:AD9 A36:AD36 A38:M38 N38:P39 AH36:XFD38 AH19:AJ20 AH39:AJ39 AH21:XFD34 AG36:AG39 AG18:AG24 AH5:XFD18 AE5:AG5 Q38:X38 AC38:AD38 AB39 A13:AA13 A14:AD16 P33:X33 Z33:AD34 A37:X37 Z37:AD37 Z38:AA38 N5:AD7 AG6:AG16 A10:AC11 P54:P57 Y54:Y57 AE54:AF56 AE57 AG27:AG34 L33:O35 A33:K34 A23:AD29 A30:B32 J30:AD32 AE6:AF40">
-    <cfRule type="expression" dxfId="78" priority="59">
+    <cfRule type="expression" dxfId="79" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB13">
+    <cfRule type="expression" dxfId="78" priority="47">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="expression" dxfId="77" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
+  <conditionalFormatting sqref="K39:M39 Q39:X39">
     <cfRule type="expression" dxfId="76" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K39:M39 Q39:X39">
+  <conditionalFormatting sqref="AB38">
     <cfRule type="expression" dxfId="75" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB38">
-    <cfRule type="expression" dxfId="74" priority="43">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AH36:AH39 AH21:AH34 AH5:AH18">
-    <cfRule type="colorScale" priority="144">
+    <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10120,7 +10409,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI39 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="148">
+    <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10132,7 +10421,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH36:AH37 AH21:AH34 AH5:AH18">
-    <cfRule type="colorScale" priority="152">
+    <cfRule type="colorScale" priority="153">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10144,7 +10433,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI37 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="156">
+    <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10156,7 +10445,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ39 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="160">
+    <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10168,7 +10457,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH21:AH34 AH5:AH18">
-    <cfRule type="colorScale" priority="164">
+    <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10180,7 +10469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="167">
+    <cfRule type="colorScale" priority="168">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10192,12 +10481,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:Q20 S20:V20">
-    <cfRule type="expression" dxfId="73" priority="35">
+    <cfRule type="expression" dxfId="74" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10209,7 +10498,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10221,7 +10510,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10233,7 +10522,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10245,7 +10534,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10257,7 +10546,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH20">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10269,7 +10558,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10281,17 +10570,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="72" priority="26">
+    <cfRule type="expression" dxfId="73" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 R20:R21 K19:V19">
-    <cfRule type="expression" dxfId="71" priority="27">
+    <cfRule type="expression" dxfId="72" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10303,7 +10592,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10315,7 +10604,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10327,7 +10616,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10339,7 +10628,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10351,7 +10640,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH19">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10363,7 +10652,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10375,101 +10664,106 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P41:P43">
+    <cfRule type="expression" dxfId="71" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y17:Y22">
     <cfRule type="expression" dxfId="70" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y17:Y22">
+  <conditionalFormatting sqref="Y33">
     <cfRule type="expression" dxfId="69" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y33">
+  <conditionalFormatting sqref="Y37:Y39">
     <cfRule type="expression" dxfId="68" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y37:Y39">
+  <conditionalFormatting sqref="Y41:Y43">
     <cfRule type="expression" dxfId="67" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y41:Y43">
+  <conditionalFormatting sqref="P48">
     <cfRule type="expression" dxfId="66" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P48">
+  <conditionalFormatting sqref="Y48:Y52">
     <cfRule type="expression" dxfId="65" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y48:Y52">
+  <conditionalFormatting sqref="P46:P47">
     <cfRule type="expression" dxfId="64" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P46:P47">
+  <conditionalFormatting sqref="Y46:Y47">
     <cfRule type="expression" dxfId="63" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y46:Y47">
+  <conditionalFormatting sqref="P52">
     <cfRule type="expression" dxfId="62" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P52">
-    <cfRule type="expression" dxfId="61" priority="16">
+  <conditionalFormatting sqref="M59:P59 N60:P65">
+    <cfRule type="expression" dxfId="61" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M59:P59 N60:P62">
+  <conditionalFormatting sqref="Q59:Q65">
     <cfRule type="expression" dxfId="60" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q59:Q62">
+  <conditionalFormatting sqref="Y62">
     <cfRule type="expression" dxfId="59" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y62">
+  <conditionalFormatting sqref="E59:I62">
     <cfRule type="expression" dxfId="58" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59:I62">
+  <conditionalFormatting sqref="C49:C51">
     <cfRule type="expression" dxfId="57" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C51">
+  <conditionalFormatting sqref="E49:I51">
     <cfRule type="expression" dxfId="56" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:I51">
+  <conditionalFormatting sqref="P49:P50">
     <cfRule type="expression" dxfId="55" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P49:P50">
+  <conditionalFormatting sqref="P51">
     <cfRule type="expression" dxfId="54" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P51">
+  <conditionalFormatting sqref="AF57">
     <cfRule type="expression" dxfId="53" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF57">
+  <conditionalFormatting sqref="C30:I32">
     <cfRule type="expression" dxfId="52" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:I32">
+  <conditionalFormatting sqref="E63:I65">
     <cfRule type="expression" dxfId="51" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -10495,13 +10789,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC77"/>
+  <dimension ref="A1:AC80"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
+      <selection pane="bottomRight" activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -10595,10 +10889,10 @@
         <v>204</v>
       </c>
       <c r="X1" s="48" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="Y1" s="48" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="12" customFormat="1" ht="21" thickBot="1">
@@ -10672,7 +10966,7 @@
         <v>131</v>
       </c>
       <c r="X2" s="30" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="Y2" s="30" t="s">
         <v>132</v>
@@ -10790,7 +11084,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19" t="str">
-        <f t="shared" ref="K4:K77" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="K4:K78" ca="1" si="3">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L4" s="14">
@@ -11756,7 +12050,7 @@
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="22" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -11837,7 +12131,7 @@
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19">
@@ -11918,7 +12212,7 @@
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
@@ -11999,7 +12293,7 @@
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F19" s="19"/>
       <c r="G19" s="19">
@@ -12404,7 +12698,7 @@
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -12485,7 +12779,7 @@
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19">
@@ -12566,7 +12860,7 @@
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -12647,7 +12941,7 @@
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19">
@@ -12728,7 +13022,7 @@
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
@@ -12809,7 +13103,7 @@
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19">
@@ -12896,7 +13190,7 @@
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -12980,7 +13274,7 @@
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19">
@@ -13811,11 +14105,11 @@
         <v>EUR</v>
       </c>
       <c r="L41" s="14">
-        <f t="shared" ref="L41:L77" ca="1" si="21">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L41:L80" ca="1" si="21">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.43519999999999998</v>
       </c>
       <c r="M41" s="14">
-        <f t="shared" ref="M41:M77" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M41:M80" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>16.456</v>
       </c>
       <c r="N41" s="14" t="str">
@@ -14020,7 +14314,7 @@
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="22" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F44" s="13">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14094,7 +14388,7 @@
         <v>4 x GeForce GTX 1080 ltd. weekly</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F45" s="13"/>
       <c r="G45" s="19">
@@ -14169,7 +14463,7 @@
         <v>4 x GeForce GTX 1080 ltd. monthly</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F46" s="13"/>
       <c r="H46" s="19">
@@ -15326,7 +15620,7 @@
         <v>2 x Titan X minutely</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F61" s="13">
         <f t="shared" ref="F61" ca="1" si="28">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15401,7 +15695,7 @@
         <v>2 x Titan X  monthly</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F62" s="43"/>
       <c r="G62" s="19">
@@ -15479,7 +15773,7 @@
         <v>4 x Titan X minutely</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F63" s="43">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15554,7 +15848,7 @@
         <v>4 x Titan X monthly</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F64" s="43"/>
       <c r="G64" s="43"/>
@@ -15623,7 +15917,7 @@
         <v>8 x Titan X minutely</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F65" s="43">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15696,7 +15990,7 @@
         <v>8 x Titan X monthly</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H66">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15986,10 +16280,10 @@
         <v>The University of Tokyo</v>
       </c>
       <c r="B70" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C70" s="22" t="str">
-        <f t="shared" ref="C70:C77" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C70:C80" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="E70" s="22" t="s">
@@ -16069,7 +16363,7 @@
         <v>Reedbush-H (educational)</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I71" s="19">
         <f t="shared" ca="1" si="30"/>
@@ -16145,7 +16439,7 @@
         <v>Reedbush-H reviewed (educational)</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I72" s="19">
         <f t="shared" ca="1" si="30"/>
@@ -16221,7 +16515,7 @@
         <v>Reedbush-H reviewed</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I73" s="19">
         <f t="shared" ca="1" si="30"/>
@@ -16297,18 +16591,18 @@
         <v>MS Azure</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C74" s="22" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>NC6</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F74" s="13">
-        <f t="shared" ref="F74:F77" ca="1" si="32">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>1.08</v>
+        <f t="shared" ref="F74:F80" ca="1" si="32">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>0.9</v>
       </c>
       <c r="K74" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -16323,7 +16617,7 @@
         <v>4.37</v>
       </c>
       <c r="N74" s="14" t="str">
-        <f t="shared" ref="N74:V77" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N74:V80" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O74" s="14">
@@ -16344,7 +16638,7 @@
       </c>
       <c r="S74" s="14" t="str">
         <f t="shared" ca="1" si="33"/>
-        <v>SSD</v>
+        <v>SATA</v>
       </c>
       <c r="T74" s="14">
         <f t="shared" ca="1" si="33"/>
@@ -16377,11 +16671,11 @@
         <v>NC12</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F75" s="13">
         <f t="shared" ca="1" si="32"/>
-        <v>2.16</v>
+        <v>1.8</v>
       </c>
       <c r="K75" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -16417,7 +16711,7 @@
       </c>
       <c r="S75" s="14" t="str">
         <f t="shared" ca="1" si="33"/>
-        <v>SSD</v>
+        <v>SATA</v>
       </c>
       <c r="T75" s="14">
         <f t="shared" ca="1" si="33"/>
@@ -16442,11 +16736,11 @@
         <v>NC24</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F76" s="13">
         <f t="shared" ca="1" si="32"/>
-        <v>4.32</v>
+        <v>3.6</v>
       </c>
       <c r="K76" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -16482,7 +16776,7 @@
       </c>
       <c r="S76" s="14" t="str">
         <f t="shared" ca="1" si="33"/>
-        <v>SSD</v>
+        <v>SATA</v>
       </c>
       <c r="T76" s="14">
         <f t="shared" ca="1" si="33"/>
@@ -16507,11 +16801,11 @@
         <v>NC24r</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F77" s="13">
         <f t="shared" ca="1" si="32"/>
-        <v>4.7519999999999998</v>
+        <v>3.96</v>
       </c>
       <c r="K77" s="19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -16547,7 +16841,7 @@
       </c>
       <c r="S77" s="14" t="str">
         <f t="shared" ca="1" si="33"/>
-        <v>SSD</v>
+        <v>SATA</v>
       </c>
       <c r="T77" s="14">
         <f t="shared" ca="1" si="33"/>
@@ -16566,9 +16860,180 @@
         <v>62</v>
       </c>
     </row>
+    <row r="78" spans="1:29">
+      <c r="C78" s="22" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>NV6</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="F78" s="13">
+        <f t="shared" ca="1" si="32"/>
+        <v>1.24</v>
+      </c>
+      <c r="H78" s="13"/>
+      <c r="K78" s="19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>USD</v>
+      </c>
+      <c r="L78" s="14">
+        <f t="shared" ca="1" si="21"/>
+        <v>0.24960000000000002</v>
+      </c>
+      <c r="M78" s="14">
+        <f t="shared" ca="1" si="22"/>
+        <v>9.65</v>
+      </c>
+      <c r="N78" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>M60</v>
+      </c>
+      <c r="O78" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="P78" s="61" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>Xeon E5-2690v3</v>
+      </c>
+      <c r="Q78" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="R78" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>56</v>
+      </c>
+      <c r="S78" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>SATA</v>
+      </c>
+      <c r="T78" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>340</v>
+      </c>
+      <c r="AC78" s="45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29">
+      <c r="C79" s="22" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>NV12</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="F79" s="13">
+        <f t="shared" ca="1" si="32"/>
+        <v>2.48</v>
+      </c>
+      <c r="H79" s="13"/>
+      <c r="K79" s="19" t="str">
+        <f t="shared" ref="K79:K80" ca="1" si="35">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>USD</v>
+      </c>
+      <c r="L79" s="14">
+        <f t="shared" ca="1" si="21"/>
+        <v>0.49920000000000003</v>
+      </c>
+      <c r="M79" s="14">
+        <f t="shared" ca="1" si="22"/>
+        <v>19.3</v>
+      </c>
+      <c r="N79" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>M60</v>
+      </c>
+      <c r="O79" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="P79" s="61" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>Xeon E5-2690v3</v>
+      </c>
+      <c r="Q79" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="R79" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>112</v>
+      </c>
+      <c r="S79" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>SATA</v>
+      </c>
+      <c r="T79" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>680</v>
+      </c>
+      <c r="AC79" s="45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29">
+      <c r="C80" s="22" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>NV24</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="F80" s="13">
+        <f t="shared" ca="1" si="32"/>
+        <v>4.97</v>
+      </c>
+      <c r="H80" s="13"/>
+      <c r="K80" s="19" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>USD</v>
+      </c>
+      <c r="L80" s="14">
+        <f t="shared" ca="1" si="21"/>
+        <v>0.99840000000000007</v>
+      </c>
+      <c r="M80" s="14">
+        <f t="shared" ca="1" si="22"/>
+        <v>38.6</v>
+      </c>
+      <c r="N80" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>M60</v>
+      </c>
+      <c r="O80" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="P80" s="61" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>Xeon E5-2690v3</v>
+      </c>
+      <c r="Q80" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>1</v>
+      </c>
+      <c r="R80" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>224</v>
+      </c>
+      <c r="S80" s="14" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>SATA</v>
+      </c>
+      <c r="T80" s="14">
+        <f t="shared" ca="1" si="33"/>
+        <v>1440</v>
+      </c>
+      <c r="AC80" s="45">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 S13:S15 E23:G23 E18:J22 D26:D41 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8 H58:H60 L50:S69 T53:Y69 K75:T77 L74:V74 W74:Y77 I66:I73 K56:K74 L70:Y73 F25:G29 E34:E36 H22:H30 F30:I30 I31 F36:G36 I36 E39:G40 I39:I40 E38 F31:G31 F32:I35 F37:I37 K4:K43 M32:O49 C30:C40">
+  <conditionalFormatting sqref="I23:J23 I25:J25 I27:J27 I29:J29 S13:S15 E23:G23 E18:J22 D26:D41 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:J16 E4:J6 N16:O16 L30:O31 E3:O3 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 J8 H58:H60 L50:S69 T53:Y69 L74:V74 W74:Y77 I66:I73 K56:K74 L70:Y73 F25:G29 E34:E36 H22:H30 F30:I30 I31 F36:G36 I36 E39:G40 I39:I40 E38 F31:G31 F32:I35 F37:I37 K4:K43 M32:O49 C30:C40 K75:T80">
     <cfRule type="expression" dxfId="50" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed MS vCPU performance calculation (1 CPU TFlops on Sheet1 made constant). Added 5 Google offers.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="48820" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="48820" windowHeight="16540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,12 +668,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="L67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+CPU performance note:
+For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).
+Assumption:
+CPUS considered to have 2 hyper threads per physical core.
+2.6 GHz Sandy Bridge
+2.6 * 1/2 * 8 (Flops/cycle DP) = 10.4 GFlops DP, 20.8 GFlops SP
+2.5 GHz Ivy Bridge   10   GFlops DP, 20   GFlops SP
+2.3 GHz Haswell    18.4   36.8
+2.2 Ghz Broadwell   17.6   35.2
+Mean values:    14.1   28.2
+0.0282TFlops per vCPU is used</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q67" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+CPU performance note:
+For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).
+Assumption:
+CPUS considered to have 2 hyper threads per physical core.
+2.6 GHz Sandy Bridge
+2.6 * 1/2 * 8 (Flops/cycle DP) = 10.4 GFlops DP, 20.8 GFlops SP
+2.5 GHz Ivy Bridge   10   GFlops DP, 20   GFlops SP
+2.3 GHz Haswell    18.4   36.8
+2.2 Ghz Broadwell   17.6   35.2
+Mean values:    14.1   28.2
+0.0282TFlops per vCPU is used</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="367">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1487,198 +1559,617 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FirePro S9300x2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x4 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x8 NVL m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 NVL w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT S9300x2 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x1 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>The University of Tokyo</t>
+  </si>
+  <si>
+    <t>Reedbush-H Personal (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2630 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>PFS</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>per hour</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>per week</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>per month (30 days)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>per year</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU personal</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS Azure</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NC12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NC24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NC24r</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K80</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>USD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
+  </si>
+  <si>
+    <t>NC6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>RDMA capable</t>
+  </si>
+  <si>
+    <t>Infiniband</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Titan X</t>
+  </si>
+  <si>
+    <t>4 x Titan X</t>
+  </si>
+  <si>
+    <t>8 x Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TITAN X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GeForce GTX Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Xeon E5-2609 v4</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>MS NC25r</t>
+  </si>
+  <si>
+    <t>MS NC24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.leadergpu.com</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx2 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx2 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx4 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx4 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx8 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTXx8 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Nodes*hours limit</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Max hours</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+  </si>
+  <si>
+    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H reviewed</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU gen edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU rev edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Limited quantity available at this price</t>
+  </si>
+  <si>
+    <t>8-GPU x86 P40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 P40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4-GPU x86 Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Quadro P600</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-1650 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU POWER8/10 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x4 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x4 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x8 x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x8 x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>16-GPU x86 K80 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8-GPU x86 M40 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86 ltd m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86 ltd w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR M40x8 ltd x86 m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR M40x8 ltd x86 w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LeaderTelecom</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x GeForce GTX 1080 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd w.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd m.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://venturebeat.com/2016/08/04/microsoft-azure-releases-n-series-gpu-instances-in-preview/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SATA</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV6</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NV24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</t>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SP Flops/sycle</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DP FLOPs/cycle</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Perf. Tflops (SP)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Q</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CPU performance (Tflops SP)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AF</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AB</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AA</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AG</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AH</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AE</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www-01.ibm.com/common/ssi/cgi-bin/ssialias?htmlfid=POD03117USEN</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>www.nimbix.net/nimbix-cloud-demand-pricing</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 12.3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AZ p2 dedicated h.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AZ p2 dedicated y.0Up</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AZ p2 dedicated y.100Up</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://en.wikichip.org/wiki/intel/xeon_e5/e5-2686_v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Google</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://cloud.google.com/compute/docs/machine-types</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/products/calculator/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/instance-types/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>6c39m1g</t>
+  </si>
+  <si>
+    <t>6c39m1g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>SSD</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>LT P100x1 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x1 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT S9300x2 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>FirePro S9300x2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT S9300x2 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 NVL min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 NVL m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x4 NVL m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x8 NVL m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 NVL w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT S9300x2 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x1 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>The University of Tokyo</t>
-  </si>
-  <si>
-    <t>Reedbush-H Personal (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2630 v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Xeon E5-2695v4 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>PFS</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>per hour</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>per week</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>per month (30 days)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>per year</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU personal</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS Azure</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NC12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NC24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NC24r</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K80</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>USD</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
-  </si>
-  <si>
-    <t>NC6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2690v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>RDMA capable</t>
-  </si>
-  <si>
-    <t>Infiniband</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x Titan X</t>
-  </si>
-  <si>
-    <t>4 x Titan X</t>
-  </si>
-  <si>
-    <t>8 x Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TITAN X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GeForce GTX Titan X</t>
+    <t>12c78m2g</t>
+  </si>
+  <si>
+    <t>12c78m2g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>24c156m4g</t>
+  </si>
+  <si>
+    <t>24c156m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32c208m4g</t>
+  </si>
+  <si>
+    <t>32c208m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>64c416m8g</t>
+  </si>
+  <si>
+    <t>64c416m8g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;
+Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;
+Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;
+In vCPU performance used SP value: 0.0282TFlops per vCPU.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://cloudplatform.googleblog.com/2017/02/GPUs-are-now-available-for-Google-Compute-Engine-and-Cloud-Machine-Learning.html</t>
+  </si>
+  <si>
+    <t>Xeon E5-2690 v3</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1686,363 +2177,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>MS NC25r</t>
-  </si>
-  <si>
-    <t>MS NC24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.leadergpu.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx2 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx2 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx4 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx4 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx8 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTXx8 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Nodes*hours limit</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Max hours</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
-  </si>
-  <si>
-    <t>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H reviewed (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H reviewed</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU gen edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU rev</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU rev edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Limited quantity available at this price</t>
-  </si>
-  <si>
-    <t>8-GPU x86 P40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 Quadro P6000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 P40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4-GPU x86 Quadro P6000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Quadro P600</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-1650 v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU POWER8/10 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x4 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x4 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x8 x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x8 x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>16-GPU x86 K80 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8-GPU x86 M40 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86 ltd m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86 ltd w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 ltd x86 m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 ltd x86 w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LeaderTelecom</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4 x GeForce GTX 1080 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd w.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd m.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NV6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NV12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NV24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://venturebeat.com/2016/08/04/microsoft-azure-releases-n-series-gpu-instances-in-preview/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SATA</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NV6</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NV12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NV24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</t>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SP Flops/sycle</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>DP FLOPs/cycle</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Perf. Tflops (SP)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Q</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CPU performance (Tflops SP)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AF</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AC</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AB</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AA</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>T</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AG</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AH</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Z</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AE</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www-01.ibm.com/common/ssi/cgi-bin/ssialias?htmlfid=POD03117USEN</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>www.nimbix.net/nimbix-cloud-demand-pricing</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 12.3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AZ p2 dedicated h.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AZ p2 dedicated y.0Up</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AZ p2 dedicated y.100Up</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://en.wikichip.org/wiki/intel/xeon_e5/e5-2686_v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec2/instance-types/</t>
+    <t>Xeon E5-2695 v4</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2428,7 +2563,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="715">
+  <cellStyleXfs count="743">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3155,6 +3290,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="61">
@@ -3262,15 +3425,15 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="119" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="120" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="715">
+  <cellStyles count="743">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3693,6 +3856,20 @@
     <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -3976,6 +4153,20 @@
     <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -3987,7 +4178,293 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="110">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -5207,13 +5684,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FG65"/>
+  <dimension ref="A1:FG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomRight" activeCell="K54" sqref="K54:K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5267,50 +5744,50 @@
     <row r="3" spans="1:163" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="60" t="s">
+      <c r="K3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
       <c r="S3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="60" t="s">
+      <c r="T3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60" t="s">
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="60"/>
-      <c r="AA3" s="60" t="s">
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="60"/>
-      <c r="AF3" s="60"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
       <c r="AG3" s="16" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>32</v>
@@ -5485,13 +5962,13 @@
         <v>171</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>10</v>
@@ -5521,16 +5998,16 @@
         <v>182</v>
       </c>
       <c r="AA4" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB4" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC4" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="AB4" s="24" t="s">
+      <c r="AD4" s="16" t="s">
         <v>232</v>
-      </c>
-      <c r="AC4" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="AD4" s="16" t="s">
-        <v>234</v>
       </c>
       <c r="AE4" s="16" t="s">
         <v>177</v>
@@ -5563,7 +6040,7 @@
         <v>2.91</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>21</v>
@@ -5615,7 +6092,7 @@
       </c>
       <c r="AG5" s="15"/>
       <c r="AH5" s="15" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:163">
@@ -5693,7 +6170,7 @@
       </c>
       <c r="AG6" s="15"/>
       <c r="AH6" s="15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:163">
@@ -5771,12 +6248,12 @@
       </c>
       <c r="AG7" s="15"/>
       <c r="AH7" s="15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:163">
       <c r="A8" s="15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>80</v>
@@ -5848,7 +6325,7 @@
     </row>
     <row r="9" spans="1:163">
       <c r="A9" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>112</v>
@@ -6491,7 +6968,7 @@
     </row>
     <row r="18" spans="1:163" s="12" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>43</v>
@@ -7072,7 +7549,7 @@
     </row>
     <row r="22" spans="1:163">
       <c r="A22" s="15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="27"/>
@@ -7185,7 +7662,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>16</v>
@@ -7269,7 +7746,7 @@
       </c>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:163">
@@ -7277,7 +7754,7 @@
         <v>59</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>40</v>
@@ -7361,13 +7838,13 @@
       </c>
       <c r="AG26" s="15"/>
       <c r="AH26" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:163" s="12" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="21" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>90</v>
@@ -7455,7 +7932,7 @@
     <row r="28" spans="1:163" s="12" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>91</v>
@@ -7543,10 +8020,10 @@
     <row r="29" spans="1:163" s="12" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D29" s="12">
         <v>8</v>
@@ -7628,7 +8105,7 @@
     <row r="30" spans="1:163" s="12" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>90</v>
@@ -7653,7 +8130,7 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="L30" s="5">
         <v>1</v>
@@ -7713,7 +8190,7 @@
     <row r="31" spans="1:163" s="12" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="21" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>34</v>
@@ -7738,7 +8215,7 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="L31" s="5">
         <v>1</v>
@@ -7798,10 +8275,10 @@
     <row r="32" spans="1:163" s="12" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D32" s="12">
         <v>4</v>
@@ -7823,7 +8300,7 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="L32" s="5">
         <v>1</v>
@@ -7882,7 +8359,7 @@
     </row>
     <row r="33" spans="1:163">
       <c r="B33" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>75</v>
@@ -7974,7 +8451,7 @@
     </row>
     <row r="34" spans="1:163">
       <c r="B34" s="21" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>76</v>
@@ -8059,7 +8536,7 @@
     <row r="35" spans="1:163" s="12" customFormat="1">
       <c r="A35" s="38"/>
       <c r="B35" s="39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C35" s="40" t="s">
         <v>131</v>
@@ -8311,7 +8788,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D37" s="27">
         <v>4</v>
@@ -8601,7 +9078,7 @@
     </row>
     <row r="41" spans="1:163" ht="23" customHeight="1">
       <c r="A41" s="20" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>167</v>
@@ -8694,10 +9171,10 @@
     </row>
     <row r="42" spans="1:163" ht="24" customHeight="1">
       <c r="A42" s="15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>169</v>
@@ -9259,7 +9736,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L48" s="27">
         <v>2</v>
@@ -9320,10 +9797,10 @@
     <row r="49" spans="1:34" s="12" customFormat="1">
       <c r="A49" s="2"/>
       <c r="B49" s="56" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D49" s="13">
         <v>2</v>
@@ -9409,10 +9886,10 @@
     <row r="50" spans="1:34" s="12" customFormat="1">
       <c r="A50" s="2"/>
       <c r="B50" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="C50" s="27" t="s">
         <v>254</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>257</v>
       </c>
       <c r="D50" s="13">
         <v>4</v>
@@ -9434,7 +9911,7 @@
       </c>
       <c r="J50" s="27"/>
       <c r="K50" s="27" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L50" s="27">
         <v>2</v>
@@ -9498,10 +9975,10 @@
     <row r="51" spans="1:34" s="12" customFormat="1">
       <c r="A51" s="2"/>
       <c r="B51" s="56" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D51" s="13">
         <v>8</v>
@@ -9523,7 +10000,7 @@
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L51" s="27">
         <v>2</v>
@@ -9589,7 +10066,7 @@
         <v>204</v>
       </c>
       <c r="C52" s="54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D52" s="13">
         <v>2</v>
@@ -9611,7 +10088,7 @@
       </c>
       <c r="J52" s="13"/>
       <c r="K52" s="54" t="s">
-        <v>208</v>
+        <v>365</v>
       </c>
       <c r="L52" s="13">
         <v>2</v>
@@ -9639,7 +10116,7 @@
         <v>32</v>
       </c>
       <c r="T52" s="54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U52" s="13">
         <v>480</v>
@@ -9678,13 +10155,13 @@
     </row>
     <row r="54" spans="1:34" ht="20">
       <c r="A54" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="B54" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>226</v>
-      </c>
       <c r="C54" s="54" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D54" s="13">
         <v>2</v>
@@ -9708,7 +10185,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="54" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="L54" s="13">
         <v>2</v>
@@ -9736,7 +10213,7 @@
         <v>256</v>
       </c>
       <c r="T54" s="54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U54" s="13">
         <v>1000</v>
@@ -9762,18 +10239,18 @@
         <v>6912</v>
       </c>
       <c r="AH54" s="15" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:34">
       <c r="A55" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C55" s="54" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D55" s="13">
         <v>2</v>
@@ -9797,7 +10274,7 @@
         <v>1</v>
       </c>
       <c r="K55" s="54" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="L55" s="13">
         <v>2</v>
@@ -9825,7 +10302,7 @@
         <v>256</v>
       </c>
       <c r="T55" s="54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U55" s="13">
         <v>4000</v>
@@ -9851,15 +10328,15 @@
         <v>13824</v>
       </c>
       <c r="AH55" s="15" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:34">
       <c r="B56" s="21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D56" s="13">
         <v>2</v>
@@ -9883,7 +10360,7 @@
         <v>1</v>
       </c>
       <c r="K56" s="54" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="L56" s="13">
         <v>2</v>
@@ -9911,7 +10388,7 @@
         <v>256</v>
       </c>
       <c r="T56" s="54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U56" s="13">
         <v>4000</v>
@@ -9934,16 +10411,16 @@
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
-      <c r="AH56" s="59" t="s">
-        <v>273</v>
+      <c r="AH56" s="58" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:34">
       <c r="B57" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C57" s="54" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D57" s="13">
         <v>2</v>
@@ -9967,7 +10444,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="54" t="s">
-        <v>228</v>
+        <v>366</v>
       </c>
       <c r="L57" s="13">
         <v>2</v>
@@ -9995,7 +10472,7 @@
         <v>256</v>
       </c>
       <c r="T57" s="54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U57" s="13">
         <v>4000</v>
@@ -10018,8 +10495,8 @@
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
-      <c r="AH57" s="59" t="s">
-        <v>273</v>
+      <c r="AH57" s="58" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:34">
@@ -10027,13 +10504,13 @@
     </row>
     <row r="59" spans="1:34" ht="20">
       <c r="A59" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C59" s="54" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D59" s="13">
         <v>0.5</v>
@@ -10055,13 +10532,13 @@
       </c>
       <c r="J59" s="13"/>
       <c r="K59" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L59" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M59" s="13">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N59" s="13">
         <v>2.6</v>
@@ -10074,7 +10551,7 @@
       </c>
       <c r="Q59" s="13">
         <f t="shared" si="10"/>
-        <v>0.49920000000000003</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="R59" s="13">
         <v>2133</v>
@@ -10083,7 +10560,7 @@
         <v>56</v>
       </c>
       <c r="T59" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U59" s="13">
         <v>380</v>
@@ -10100,22 +10577,22 @@
       </c>
       <c r="AD59" s="55"/>
       <c r="AF59" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AG59" s="15"/>
       <c r="AH59" s="15" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:34">
       <c r="A60" s="15" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D60" s="13">
         <v>1</v>
@@ -10137,7 +10614,7 @@
       </c>
       <c r="J60" s="13"/>
       <c r="K60" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L60" s="13">
         <v>1</v>
@@ -10165,7 +10642,7 @@
         <v>112</v>
       </c>
       <c r="T60" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U60" s="13">
         <v>680</v>
@@ -10182,19 +10659,19 @@
       </c>
       <c r="AD60" s="55"/>
       <c r="AF60" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AG60" s="15"/>
     </row>
     <row r="61" spans="1:34">
       <c r="A61" s="15" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B61" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="C61" s="54" t="s">
         <v>238</v>
-      </c>
-      <c r="C61" s="54" t="s">
-        <v>240</v>
       </c>
       <c r="D61" s="13">
         <v>2</v>
@@ -10216,13 +10693,13 @@
       </c>
       <c r="J61" s="13"/>
       <c r="K61" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L61" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M61" s="13">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="N61" s="13">
         <v>2.6</v>
@@ -10235,7 +10712,7 @@
       </c>
       <c r="Q61" s="13">
         <f t="shared" si="10"/>
-        <v>1.9968000000000001</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="R61" s="13">
         <v>2133</v>
@@ -10244,7 +10721,7 @@
         <v>224</v>
       </c>
       <c r="T61" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U61" s="13">
         <v>1440</v>
@@ -10261,16 +10738,16 @@
       </c>
       <c r="AD61" s="55"/>
       <c r="AF61" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AG61" s="15"/>
     </row>
     <row r="62" spans="1:34">
       <c r="B62" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C62" s="54" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D62" s="13">
         <v>2</v>
@@ -10292,13 +10769,13 @@
       </c>
       <c r="J62" s="13"/>
       <c r="K62" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L62" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M62" s="13">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="N62" s="13">
         <v>2.6</v>
@@ -10311,7 +10788,7 @@
       </c>
       <c r="Q62" s="13">
         <f t="shared" si="10"/>
-        <v>1.9968000000000001</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="R62" s="13">
         <v>2133</v>
@@ -10320,13 +10797,13 @@
         <v>224</v>
       </c>
       <c r="T62" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U62" s="13">
         <v>1440</v>
       </c>
       <c r="X62" s="13" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="Y62" s="13"/>
       <c r="Z62" s="13" t="str">
@@ -10342,21 +10819,21 @@
       </c>
       <c r="AD62" s="55"/>
       <c r="AF62" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AG62" s="15"/>
       <c r="AH62" s="15" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:34">
       <c r="B63" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C63" t="s">
         <v>311</v>
       </c>
-      <c r="C63" t="s">
-        <v>314</v>
-      </c>
-      <c r="D63">
+      <c r="D63" s="13">
         <v>1</v>
       </c>
       <c r="E63" s="13" t="s">
@@ -10375,13 +10852,13 @@
         <v>71</v>
       </c>
       <c r="K63" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L63" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M63" s="13">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N63" s="13">
         <v>2.6</v>
@@ -10394,7 +10871,7 @@
       </c>
       <c r="Q63" s="13">
         <f t="shared" si="10"/>
-        <v>0.49920000000000003</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="R63" s="13">
         <v>2133</v>
@@ -10403,7 +10880,7 @@
         <v>56</v>
       </c>
       <c r="T63" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U63">
         <v>340</v>
@@ -10412,17 +10889,17 @@
         <v>1.24</v>
       </c>
       <c r="AF63" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:34">
       <c r="B64" s="21" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="D64">
+        <v>311</v>
+      </c>
+      <c r="D64" s="13">
         <v>2</v>
       </c>
       <c r="E64" s="13" t="s">
@@ -10441,7 +10918,7 @@
         <v>71</v>
       </c>
       <c r="K64" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L64" s="13">
         <v>1</v>
@@ -10469,7 +10946,7 @@
         <v>112</v>
       </c>
       <c r="T64" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U64">
         <v>680</v>
@@ -10478,17 +10955,17 @@
         <v>2.48</v>
       </c>
       <c r="AF64" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
-    <row r="65" spans="2:32">
+    <row r="65" spans="1:34">
       <c r="B65" s="21" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="D65">
+        <v>311</v>
+      </c>
+      <c r="D65" s="13">
         <v>4</v>
       </c>
       <c r="E65" s="13" t="s">
@@ -10507,13 +10984,13 @@
         <v>71</v>
       </c>
       <c r="K65" s="54" t="s">
-        <v>244</v>
+        <v>364</v>
       </c>
       <c r="L65" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M65" s="13">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="N65" s="13">
         <v>2.6</v>
@@ -10526,7 +11003,7 @@
       </c>
       <c r="Q65" s="13">
         <f t="shared" si="10"/>
-        <v>1.9968000000000001</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="R65" s="13">
         <v>2133</v>
@@ -10535,7 +11012,7 @@
         <v>224</v>
       </c>
       <c r="T65" s="54" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U65">
         <v>1440</v>
@@ -10544,7 +11021,315 @@
         <v>4.97</v>
       </c>
       <c r="AF65" s="15" t="s">
-        <v>241</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34">
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:34" ht="20" customHeight="1">
+      <c r="A67" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="C67" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="G67" s="13">
+        <v>2.91</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13">
+        <v>6</v>
+      </c>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13"/>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+      <c r="Q67" s="13">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="S67">
+        <v>39</v>
+      </c>
+      <c r="T67" t="s">
+        <v>352</v>
+      </c>
+      <c r="U67">
+        <v>375</v>
+      </c>
+      <c r="AA67" s="23">
+        <v>1.073</v>
+      </c>
+      <c r="AF67" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH67" s="60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" ht="20" customHeight="1">
+      <c r="A68" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C68" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" s="13">
+        <v>1</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="G68" s="13">
+        <v>2.91</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13">
+        <v>12</v>
+      </c>
+      <c r="M68" s="13"/>
+      <c r="N68" s="13"/>
+      <c r="O68" s="13"/>
+      <c r="P68" s="13"/>
+      <c r="Q68" s="13">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="R68" s="12"/>
+      <c r="S68" s="12">
+        <v>39</v>
+      </c>
+      <c r="T68" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="U68" s="12">
+        <v>375</v>
+      </c>
+      <c r="V68" s="12"/>
+      <c r="W68" s="12"/>
+      <c r="Y68" s="12"/>
+      <c r="AA68" s="23">
+        <v>2.0339999999999998</v>
+      </c>
+      <c r="AF68" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH68" s="60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" ht="20" customHeight="1">
+      <c r="A69" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="C69" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D69" s="13">
+        <v>2</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="G69" s="13">
+        <v>2.91</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13">
+        <v>24</v>
+      </c>
+      <c r="M69" s="13"/>
+      <c r="N69" s="13"/>
+      <c r="O69" s="13"/>
+      <c r="P69" s="13"/>
+      <c r="Q69" s="13">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="R69" s="12"/>
+      <c r="S69" s="12">
+        <v>39</v>
+      </c>
+      <c r="T69" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="U69" s="12">
+        <v>375</v>
+      </c>
+      <c r="V69" s="12"/>
+      <c r="W69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="AA69" s="23">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="AF69" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH69" s="60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:34" ht="20" customHeight="1">
+      <c r="B70" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="C70" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D70" s="13">
+        <v>2</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="G70" s="13">
+        <v>2.91</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13">
+        <v>32</v>
+      </c>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="R70" s="12"/>
+      <c r="S70" s="12">
+        <v>39</v>
+      </c>
+      <c r="T70" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="U70" s="12">
+        <v>375</v>
+      </c>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="AA70" s="23">
+        <v>4.3029999999999999</v>
+      </c>
+      <c r="AF70" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH70" s="60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" ht="20" customHeight="1">
+      <c r="B71" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="C71" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="D71" s="13">
+        <v>4</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="13">
+        <v>8.74</v>
+      </c>
+      <c r="G71" s="13">
+        <v>2.91</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13">
+        <v>64</v>
+      </c>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="R71" s="12"/>
+      <c r="S71" s="12">
+        <v>39</v>
+      </c>
+      <c r="T71" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="U71" s="12">
+        <v>375</v>
+      </c>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="AA71" s="23">
+        <v>8.4930000000000003</v>
+      </c>
+      <c r="AF71" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH71" s="60" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -10557,7 +11342,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AI37">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10569,7 +11354,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ37">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10581,7 +11366,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10593,7 +11378,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10605,7 +11390,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10617,7 +11402,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="77">
+    <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10629,32 +11414,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 AA39 A17 B18:I18 A21:J21 T21:W21 A22:W22 AA18:AE22 X18:X22 A12:AE12 A5:M8 A36:AE36 A38:M38 N38:O39 AI36:XFD38 AI19:AK20 AI39:AK39 AI21:XFD34 AH36:AH39 AH18:AH24 AI5:XFD18 R38:Y38 AD38:AE38 AC39 A13:AB13 R33:Y33 AA33:AE34 A37:O37 AA37:AE37 AA38:AB38 AH6:AH16 A10:C11 Z54:Z57 AF54:AG56 AF57 AH27:AH34 A23:AE25 A30:B32 J30:O32 AF6:AG40 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 Q37:Y37 Q37:Q39 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11">
-    <cfRule type="expression" dxfId="83" priority="71">
+    <cfRule type="expression" dxfId="109" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC13">
-    <cfRule type="expression" dxfId="82" priority="58">
+    <cfRule type="expression" dxfId="108" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="81" priority="57">
+    <cfRule type="expression" dxfId="107" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:M39 R39:Y39">
-    <cfRule type="expression" dxfId="80" priority="56">
+    <cfRule type="expression" dxfId="106" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC38">
-    <cfRule type="expression" dxfId="79" priority="55">
+    <cfRule type="expression" dxfId="105" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI39 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="156">
+    <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10666,7 +11451,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ39 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="160">
+    <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10678,7 +11463,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI37 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="164">
+    <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10690,7 +11475,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="168">
+    <cfRule type="colorScale" priority="169">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10702,7 +11487,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK36:AK39 AK21:AK34 AK5:AK18">
-    <cfRule type="colorScale" priority="172">
+    <cfRule type="colorScale" priority="173">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10714,7 +11499,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="176">
+    <cfRule type="colorScale" priority="177">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10726,7 +11511,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="179">
+    <cfRule type="colorScale" priority="180">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10738,12 +11523,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20 T20:W20">
-    <cfRule type="expression" dxfId="78" priority="47">
+    <cfRule type="expression" dxfId="104" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10755,7 +11540,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10767,7 +11552,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10779,7 +11564,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10791,7 +11576,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10803,7 +11588,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10815,7 +11600,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10827,17 +11612,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="77" priority="38">
+    <cfRule type="expression" dxfId="103" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 S20:S21 S19:W19">
-    <cfRule type="expression" dxfId="76" priority="39">
+    <cfRule type="expression" dxfId="102" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10849,7 +11634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10861,7 +11646,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10873,7 +11658,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10885,7 +11670,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK19">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10897,7 +11682,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10909,7 +11694,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10921,132 +11706,137 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41:Q65">
-    <cfRule type="expression" dxfId="75" priority="37">
+    <cfRule type="expression" dxfId="101" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z22">
-    <cfRule type="expression" dxfId="74" priority="36">
+    <cfRule type="expression" dxfId="100" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="expression" dxfId="73" priority="35">
+    <cfRule type="expression" dxfId="99" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z37:Z39">
-    <cfRule type="expression" dxfId="72" priority="34">
+    <cfRule type="expression" dxfId="98" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z41:Z43">
-    <cfRule type="expression" dxfId="71" priority="33">
+    <cfRule type="expression" dxfId="97" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z48:Z52">
-    <cfRule type="expression" dxfId="70" priority="31">
+    <cfRule type="expression" dxfId="96" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z47">
-    <cfRule type="expression" dxfId="69" priority="29">
+    <cfRule type="expression" dxfId="95" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M59:O59 N60:O65">
-    <cfRule type="expression" dxfId="68" priority="22">
+    <cfRule type="expression" dxfId="94" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R59:R65">
-    <cfRule type="expression" dxfId="67" priority="21">
+    <cfRule type="expression" dxfId="93" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z62">
-    <cfRule type="expression" dxfId="66" priority="20">
+    <cfRule type="expression" dxfId="92" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:I62">
-    <cfRule type="expression" dxfId="65" priority="19">
+    <cfRule type="expression" dxfId="91" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C51">
-    <cfRule type="expression" dxfId="64" priority="18">
+    <cfRule type="expression" dxfId="90" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:I51">
-    <cfRule type="expression" dxfId="63" priority="17">
+    <cfRule type="expression" dxfId="89" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG57">
-    <cfRule type="expression" dxfId="62" priority="14">
+    <cfRule type="expression" dxfId="88" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I32">
-    <cfRule type="expression" dxfId="61" priority="13">
+    <cfRule type="expression" dxfId="87" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:I65">
-    <cfRule type="expression" dxfId="60" priority="12">
+    <cfRule type="expression" dxfId="86" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q21">
-    <cfRule type="expression" dxfId="59" priority="11">
+    <cfRule type="expression" dxfId="85" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="58" priority="10">
+    <cfRule type="expression" dxfId="84" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K21">
-    <cfRule type="expression" dxfId="57" priority="9">
+    <cfRule type="expression" dxfId="83" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
-    <cfRule type="expression" dxfId="56" priority="8">
+    <cfRule type="expression" dxfId="82" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44:P48">
-    <cfRule type="expression" dxfId="55" priority="7">
+    <cfRule type="expression" dxfId="81" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49:P52">
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="80" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54">
-    <cfRule type="expression" dxfId="53" priority="5">
+    <cfRule type="expression" dxfId="79" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P57">
-    <cfRule type="expression" dxfId="52" priority="4">
+    <cfRule type="expression" dxfId="78" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P59:P62">
-    <cfRule type="expression" dxfId="51" priority="3">
+    <cfRule type="expression" dxfId="77" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P63:P65">
-    <cfRule type="expression" dxfId="50" priority="2">
+    <cfRule type="expression" dxfId="76" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67:I71">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11067,13 +11857,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC80"/>
+  <dimension ref="A1:AC86"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="N67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="P70" sqref="P70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11113,25 +11903,25 @@
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
       <c r="F1" s="46" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G1" s="46" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H1" s="46" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="L1" s="46" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M1" s="46" t="s">
         <v>165</v>
@@ -11149,28 +11939,28 @@
         <v>136</v>
       </c>
       <c r="R1" s="46" t="s">
+        <v>329</v>
+      </c>
+      <c r="S1" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="T1" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="U1" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="V1" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="W1" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="X1" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="Y1" s="46" t="s">
         <v>335</v>
-      </c>
-      <c r="U1" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="V1" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="W1" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="X1" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="Y1" s="46" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" ht="21" thickBot="1">
@@ -11208,7 +11998,7 @@
         <v>181</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>183</v>
@@ -11244,7 +12034,7 @@
         <v>125</v>
       </c>
       <c r="X2" s="29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="Y2" s="29" t="s">
         <v>126</v>
@@ -11524,7 +12314,7 @@
         <v>111</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F6" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11609,7 +12399,7 @@
         <v>186</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -11697,7 +12487,7 @@
         <v>187</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -12361,7 +13151,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -12445,7 +13235,7 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18">
@@ -12529,7 +13319,7 @@
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
@@ -12613,7 +13403,7 @@
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18">
@@ -13033,7 +13823,7 @@
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -13117,7 +13907,7 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18">
@@ -13201,7 +13991,7 @@
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -13285,7 +14075,7 @@
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18">
@@ -13369,7 +14159,7 @@
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -13453,7 +14243,7 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18">
@@ -13543,7 +14333,7 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -13627,7 +14417,7 @@
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="18">
@@ -14486,7 +15276,7 @@
         <v>EUR</v>
       </c>
       <c r="L41" s="13">
-        <f t="shared" ref="L41:L80" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L41:L86" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.87039999999999995</v>
       </c>
       <c r="M41" s="13">
@@ -14703,7 +15493,7 @@
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="21" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F44" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14781,7 +15571,7 @@
         <v>4 x GeForce GTX 1080 ltd. weekly</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="18">
@@ -14860,7 +15650,7 @@
         <v>4 x GeForce GTX 1080 ltd. monthly</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F46" s="12"/>
       <c r="H46" s="18">
@@ -15181,7 +15971,7 @@
         <v>1 x Tesla P100 minutely</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F50" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15261,7 +16051,7 @@
         <v>1 x Tesla P100 weekly</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="18">
@@ -15342,7 +16132,7 @@
         <v>1 x Tesla P100 monthly</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F52" s="12"/>
       <c r="H52" s="18">
@@ -15423,7 +16213,7 @@
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F53" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15503,7 +16293,7 @@
         <v>2 x Tesla P100 weekly</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="18">
@@ -15584,7 +16374,7 @@
         <v>2 x Tesla P100 monthly</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F55" s="12"/>
       <c r="H55" s="18">
@@ -15665,7 +16455,7 @@
       </c>
       <c r="D56" s="39"/>
       <c r="E56" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F56" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -15748,7 +16538,7 @@
       </c>
       <c r="D57" s="41"/>
       <c r="E57" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F57" s="41"/>
       <c r="G57" s="18">
@@ -15831,7 +16621,7 @@
       </c>
       <c r="D58" s="41"/>
       <c r="E58" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F58" s="41"/>
       <c r="G58" s="41"/>
@@ -15913,7 +16703,7 @@
         <v>4 x Tesla P100 NVLink monthly</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F59" s="41"/>
       <c r="G59" s="41"/>
@@ -15992,7 +16782,7 @@
         <v>8 x Tesla P100 NVLink monthly</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F60" s="41"/>
       <c r="G60" s="41"/>
@@ -16071,7 +16861,7 @@
         <v>2 x Titan X minutely</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F61" s="12">
         <f t="shared" ref="F61" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16150,7 +16940,7 @@
         <v>2 x Titan X  monthly</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F62" s="41"/>
       <c r="G62" s="18">
@@ -16232,7 +17022,7 @@
         <v>4 x Titan X minutely</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F63" s="41">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16311,7 +17101,7 @@
         <v>4 x Titan X monthly</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F64" s="41"/>
       <c r="G64" s="41"/>
@@ -16384,7 +17174,7 @@
         <v>8 x Titan X minutely</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F65" s="41">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16461,7 +17251,7 @@
         <v>8 x Titan X monthly</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H66">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16542,7 +17332,7 @@
         <v>2 x FirePro S9300x2 minutely</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F67">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16623,7 +17413,7 @@
         <v>2 x FirePro S9300x2 weekly</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G68" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16695,7 +17485,7 @@
         <v>2 x FirePro S9300x2 monthly</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H69" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -16767,17 +17557,17 @@
         <v>The University of Tokyo</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C70" s="21" t="str">
-        <f t="shared" ref="C70:C80" ca="1" si="32">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C70:E85" ca="1" si="32">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I70" s="18">
         <f t="shared" ca="1" si="31"/>
@@ -16809,7 +17599,7 @@
       </c>
       <c r="P70" s="13" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v xml:space="preserve">Xeon E5-2695v4 </v>
+        <v>Xeon E5-2695 v4</v>
       </c>
       <c r="Q70" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -16857,10 +17647,10 @@
         <v>Reedbush-H (educational)</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="I71" s="18">
         <f t="shared" ca="1" si="31"/>
@@ -16892,7 +17682,7 @@
       </c>
       <c r="P71" s="13" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v xml:space="preserve">Xeon E5-2695v4 </v>
+        <v>Xeon E5-2695 v4</v>
       </c>
       <c r="Q71" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -16940,10 +17730,10 @@
         <v>Reedbush-H reviewed (educational)</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I72" s="18">
         <f t="shared" ca="1" si="31"/>
@@ -16975,7 +17765,7 @@
       </c>
       <c r="P72" s="13" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v xml:space="preserve">Xeon E5-2695v4 </v>
+        <v>Xeon E5-2695 v4</v>
       </c>
       <c r="Q72" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -17023,10 +17813,10 @@
         <v>Reedbush-H reviewed</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="I73" s="18">
         <f t="shared" ca="1" si="31"/>
@@ -17058,7 +17848,7 @@
       </c>
       <c r="P73" s="13" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v xml:space="preserve">Xeon E5-2695v4 </v>
+        <v>Xeon E5-2695 v4</v>
       </c>
       <c r="Q73" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -17106,14 +17896,14 @@
         <v>MS Azure</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C74" s="21" t="str">
         <f t="shared" ca="1" si="32"/>
         <v>NC6</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F74" s="12">
         <f t="shared" ref="F74:F80" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -17140,20 +17930,20 @@
         <v>4.37</v>
       </c>
       <c r="N74" s="13" t="str">
-        <f t="shared" ref="N74:V80" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N74:V86" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O74" s="13">
         <f t="shared" ca="1" si="34"/>
         <v>0.5</v>
       </c>
-      <c r="P74" s="58" t="str">
+      <c r="P74" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q74" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R74" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17194,7 +17984,7 @@
         <v>NC12</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F75" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17228,9 +18018,9 @@
         <f t="shared" ca="1" si="34"/>
         <v>1</v>
       </c>
-      <c r="P75" s="58" t="str">
+      <c r="P75" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q75" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17267,7 +18057,7 @@
         <v>NC24</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F76" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17278,7 +18068,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="18">
-        <f t="shared" ref="J76:J80" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="J76:K86" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K76" s="18" t="str">
@@ -17301,13 +18091,13 @@
         <f t="shared" ca="1" si="34"/>
         <v>2</v>
       </c>
-      <c r="P76" s="58" t="str">
+      <c r="P76" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q76" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R76" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17340,7 +18130,7 @@
         <v>NC24r</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F77" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17374,13 +18164,13 @@
         <f t="shared" ca="1" si="34"/>
         <v>2</v>
       </c>
-      <c r="P77" s="58" t="str">
+      <c r="P77" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q77" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R77" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17413,7 +18203,7 @@
         <v>NV6</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F78" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17448,13 +18238,13 @@
         <f t="shared" ca="1" si="34"/>
         <v>1</v>
       </c>
-      <c r="P78" s="58" t="str">
+      <c r="P78" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q78" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R78" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17478,7 +18268,7 @@
         <v>NV12</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F79" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17513,9 +18303,9 @@
         <f t="shared" ca="1" si="34"/>
         <v>2</v>
       </c>
-      <c r="P79" s="58" t="str">
+      <c r="P79" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q79" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17543,7 +18333,7 @@
         <v>NV24</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F80" s="12">
         <f t="shared" ca="1" si="33"/>
@@ -17578,13 +18368,13 @@
         <f t="shared" ca="1" si="34"/>
         <v>4</v>
       </c>
-      <c r="P80" s="58" t="str">
+      <c r="P80" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
-        <v>Xeon E5-2690v3</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="Q80" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R80" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -17601,250 +18391,649 @@
       <c r="AC80" s="43">
         <v>65</v>
       </c>
+    </row>
+    <row r="81" spans="1:29" ht="20">
+      <c r="A81" s="57" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>Google</v>
+      </c>
+      <c r="B81" t="s">
+        <v>363</v>
+      </c>
+      <c r="C81" s="21" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>6c39m1g</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="F81" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>1.073</v>
+      </c>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K81" s="18" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>USD</v>
+      </c>
+      <c r="L81" s="13">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.16919999999999999</v>
+      </c>
+      <c r="M81" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>4.37</v>
+      </c>
+      <c r="N81" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>K80</v>
+      </c>
+      <c r="O81" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q81" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>6</v>
+      </c>
+      <c r="R81" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="S81" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>SSD</v>
+      </c>
+      <c r="T81" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>375</v>
+      </c>
+      <c r="Y81" s="15" t="str">
+        <f t="shared" ref="Y81:Y85" ca="1" si="38">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC81" s="43">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29">
+      <c r="C82" s="21" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>12c78m2g</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="F82" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>2.0339999999999998</v>
+      </c>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K82" s="18" t="str">
+        <f t="shared" ca="1" si="36"/>
+        <v>USD</v>
+      </c>
+      <c r="L82" s="13">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.33839999999999998</v>
+      </c>
+      <c r="M82" s="13">
+        <f t="shared" ref="M82" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>8.74</v>
+      </c>
+      <c r="N82" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>K80</v>
+      </c>
+      <c r="O82" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="Q82" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>12</v>
+      </c>
+      <c r="R82" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="S82" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>SSD</v>
+      </c>
+      <c r="T82" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>375</v>
+      </c>
+      <c r="Y82" s="15" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC82" s="43">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:29">
+      <c r="C83" s="21" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>24c156m4g</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="F83" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K83" s="18" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>USD</v>
+      </c>
+      <c r="L83" s="13">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.67679999999999996</v>
+      </c>
+      <c r="M83" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>17.48</v>
+      </c>
+      <c r="N83" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>K80</v>
+      </c>
+      <c r="O83" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="Q83" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>24</v>
+      </c>
+      <c r="R83" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="S83" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>SSD</v>
+      </c>
+      <c r="T83" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>375</v>
+      </c>
+      <c r="Y83" s="15" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC83" s="43">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:29">
+      <c r="C84" s="21" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>32c208m4g</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="F84" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>4.3029999999999999</v>
+      </c>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K84" s="18" t="str">
+        <f t="shared" ca="1" si="36"/>
+        <v>USD</v>
+      </c>
+      <c r="L84" s="13">
+        <f t="shared" ca="1" si="22"/>
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="M84" s="13">
+        <f t="shared" ref="M84" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>17.48</v>
+      </c>
+      <c r="N84" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>K80</v>
+      </c>
+      <c r="O84" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="Q84" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>32</v>
+      </c>
+      <c r="R84" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="S84" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>SSD</v>
+      </c>
+      <c r="T84" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>375</v>
+      </c>
+      <c r="Y84" s="15" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC84" s="43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29">
+      <c r="C85" s="21" t="str">
+        <f t="shared" ca="1" si="32"/>
+        <v>64c416m8g</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="F85" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>8.4930000000000003</v>
+      </c>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K85" s="18" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>USD</v>
+      </c>
+      <c r="L85" s="13">
+        <f t="shared" ca="1" si="22"/>
+        <v>1.8048</v>
+      </c>
+      <c r="M85" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>34.96</v>
+      </c>
+      <c r="N85" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>K80</v>
+      </c>
+      <c r="O85" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="Q85" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>64</v>
+      </c>
+      <c r="R85" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>39</v>
+      </c>
+      <c r="S85" s="13" t="str">
+        <f t="shared" ca="1" si="34"/>
+        <v>SSD</v>
+      </c>
+      <c r="T85" s="13">
+        <f t="shared" ca="1" si="34"/>
+        <v>375</v>
+      </c>
+      <c r="Y85" s="15" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC85" s="43">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29">
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="I23 I25 I27 I29 S13:S15 E23:G23 E18:I22 D26:D41 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:I16 N16:O16 L30:O31 E3:I6 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 H58:H60 L50:S69 T53:Y69 L74:V74 W74:Y77 K56:K74 L70:Y73 F25:G29 E34:E36 H22:H30 F30:I30 I31 F36:G36 I36 E39:G40 I39:I40 E38 F31:G31 F32:I35 F37:I37 K4:K43 M32:O49 C30:C40 K75:T80 I66:I80 K3:O3 J3:J80">
-    <cfRule type="expression" dxfId="49" priority="119">
+    <cfRule type="expression" dxfId="75" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 I24 F24:G24">
-    <cfRule type="expression" dxfId="48" priority="117">
+    <cfRule type="expression" dxfId="74" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="47" priority="116">
+    <cfRule type="expression" dxfId="73" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="46" priority="115">
+    <cfRule type="expression" dxfId="72" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="45" priority="106">
+    <cfRule type="expression" dxfId="71" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P15 P18:P49">
-    <cfRule type="expression" dxfId="44" priority="61">
+    <cfRule type="expression" dxfId="70" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:X3 T4:X12 T18:V31 T13:V15 W13:X31 R3:R15 U47:X49 T47:T52 R18:R49 Y6:Y49 T32:X46">
-    <cfRule type="expression" dxfId="43" priority="59">
+    <cfRule type="expression" dxfId="69" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="expression" dxfId="42" priority="68">
+    <cfRule type="expression" dxfId="68" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C25">
-    <cfRule type="expression" dxfId="41" priority="67">
+    <cfRule type="expression" dxfId="67" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C27">
-    <cfRule type="expression" dxfId="40" priority="66">
+    <cfRule type="expression" dxfId="66" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="expression" dxfId="39" priority="65">
+    <cfRule type="expression" dxfId="65" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q15 Q18:Q49">
-    <cfRule type="expression" dxfId="38" priority="60">
+    <cfRule type="expression" dxfId="64" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S12">
-    <cfRule type="expression" dxfId="37" priority="58">
+    <cfRule type="expression" dxfId="63" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18:S49">
-    <cfRule type="expression" dxfId="36" priority="57">
+    <cfRule type="expression" dxfId="62" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:I17 N17:O17">
-    <cfRule type="expression" dxfId="35" priority="48">
+    <cfRule type="expression" dxfId="61" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P17">
-    <cfRule type="expression" dxfId="34" priority="47">
+    <cfRule type="expression" dxfId="60" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:V17 R16:R17">
-    <cfRule type="expression" dxfId="33" priority="45">
+    <cfRule type="expression" dxfId="59" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16:Q17">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="58" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17">
-    <cfRule type="expression" dxfId="31" priority="44">
+    <cfRule type="expression" dxfId="57" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="30" priority="43">
+    <cfRule type="expression" dxfId="56" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="29" priority="42">
+    <cfRule type="expression" dxfId="55" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="28" priority="41">
+    <cfRule type="expression" dxfId="54" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32:L49">
-    <cfRule type="expression" dxfId="27" priority="40">
+    <cfRule type="expression" dxfId="53" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="expression" dxfId="26" priority="39">
+    <cfRule type="expression" dxfId="52" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="25" priority="38">
+    <cfRule type="expression" dxfId="51" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="50" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44 K44:K55">
-    <cfRule type="expression" dxfId="23" priority="33">
+    <cfRule type="expression" dxfId="49" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="22" priority="32">
+    <cfRule type="expression" dxfId="48" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="expression" dxfId="21" priority="31">
+    <cfRule type="expression" dxfId="47" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="20" priority="26">
+    <cfRule type="expression" dxfId="46" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="45" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="18" priority="24">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="43" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="42" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U50:Y52">
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="41" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="38" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="37" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63:H65">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="35" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57 G62">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="33" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E29">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:H40">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="29" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
+    <cfRule type="expression" dxfId="27" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F81:O82">
+    <cfRule type="expression" dxfId="22" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83:O84">
+    <cfRule type="expression" dxfId="20" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F85:O86">
+    <cfRule type="expression" dxfId="18" priority="8">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T81:T84 R81:R84">
+    <cfRule type="expression" dxfId="13" priority="6">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q81:Q84">
+    <cfRule type="expression" dxfId="11" priority="7">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S81:S84">
+    <cfRule type="expression" dxfId="9" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T85 R85">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q85">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S85">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y81:Y85">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fixed Google memory sizes.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -2117,9 +2117,6 @@
   </si>
   <si>
     <t>6c39m1g</t>
-  </si>
-  <si>
-    <t>6c39m1g</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -2132,27 +2129,15 @@
   </si>
   <si>
     <t>12c78m2g</t>
-  </si>
-  <si>
-    <t>12c78m2g</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>24c156m4g</t>
-  </si>
-  <si>
-    <t>24c156m4g</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>32c208m4g</t>
-  </si>
-  <si>
-    <t>32c208m4g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>64c416m8g</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>64c416m8g</t>
@@ -2178,6 +2163,26 @@
   </si>
   <si>
     <t>Xeon E5-2695 v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GL 6c39m1g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GL 12c78m2g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GL 24c156m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GL 32c208m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GL 64c416m8g</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3426,11 +3431,11 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="120" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="120" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="743">
@@ -4178,7 +4183,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="94">
     <dxf>
       <font>
         <color auto="1"/>
@@ -4286,193 +4291,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5389,6 +5207,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -5687,10 +5516,10 @@
   <dimension ref="A1:FG71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K54" sqref="K54:K57"/>
+      <selection pane="bottomRight" activeCell="S74" sqref="S74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5744,48 +5573,48 @@
     <row r="3" spans="1:163" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
       <c r="S3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="59" t="s">
+      <c r="T3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59" t="s">
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59" t="s">
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
-      <c r="AF3" s="59"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
       <c r="AG3" s="16" t="s">
         <v>265</v>
       </c>
@@ -10088,7 +9917,7 @@
       </c>
       <c r="J52" s="13"/>
       <c r="K52" s="54" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="L52" s="13">
         <v>2</v>
@@ -10185,7 +10014,7 @@
         <v>1</v>
       </c>
       <c r="K54" s="54" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L54" s="13">
         <v>2</v>
@@ -10274,7 +10103,7 @@
         <v>1</v>
       </c>
       <c r="K55" s="54" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L55" s="13">
         <v>2</v>
@@ -10360,7 +10189,7 @@
         <v>1</v>
       </c>
       <c r="K56" s="54" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L56" s="13">
         <v>2</v>
@@ -10444,7 +10273,7 @@
         <v>1</v>
       </c>
       <c r="K57" s="54" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L57" s="13">
         <v>2</v>
@@ -10532,7 +10361,7 @@
       </c>
       <c r="J59" s="13"/>
       <c r="K59" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L59" s="13">
         <v>0.5</v>
@@ -10614,7 +10443,7 @@
       </c>
       <c r="J60" s="13"/>
       <c r="K60" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L60" s="13">
         <v>1</v>
@@ -10693,7 +10522,7 @@
       </c>
       <c r="J61" s="13"/>
       <c r="K61" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L61" s="13">
         <v>2</v>
@@ -10769,7 +10598,7 @@
       </c>
       <c r="J62" s="13"/>
       <c r="K62" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L62" s="13">
         <v>2</v>
@@ -10852,7 +10681,7 @@
         <v>71</v>
       </c>
       <c r="K63" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L63" s="13">
         <v>0.5</v>
@@ -10918,7 +10747,7 @@
         <v>71</v>
       </c>
       <c r="K64" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L64" s="13">
         <v>1</v>
@@ -10984,7 +10813,7 @@
         <v>71</v>
       </c>
       <c r="K65" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="L65" s="13">
         <v>2</v>
@@ -11032,7 +10861,7 @@
         <v>345</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C67" s="54" t="s">
         <v>238</v>
@@ -11071,7 +10900,7 @@
         <v>39</v>
       </c>
       <c r="T67" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U67">
         <v>375</v>
@@ -11080,10 +10909,10 @@
         <v>1.073</v>
       </c>
       <c r="AF67" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="AH67" s="60" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="AH67" s="59" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="68" spans="1:34" ht="20" customHeight="1">
@@ -11091,7 +10920,7 @@
         <v>346</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C68" s="54" t="s">
         <v>238</v>
@@ -11128,10 +10957,10 @@
       </c>
       <c r="R68" s="12"/>
       <c r="S68" s="12">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="T68" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U68" s="12">
         <v>375</v>
@@ -11143,10 +10972,10 @@
         <v>2.0339999999999998</v>
       </c>
       <c r="AF68" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="AH68" s="60" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="AH68" s="59" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:34" ht="20" customHeight="1">
@@ -11154,7 +10983,7 @@
         <v>347</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C69" s="54" t="s">
         <v>238</v>
@@ -11191,10 +11020,10 @@
       </c>
       <c r="R69" s="12"/>
       <c r="S69" s="12">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="T69" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U69" s="12">
         <v>375</v>
@@ -11206,15 +11035,15 @@
         <v>3.9550000000000001</v>
       </c>
       <c r="AF69" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="AH69" s="60" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="AH69" s="59" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:34" ht="20" customHeight="1">
       <c r="B70" s="21" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C70" s="54" t="s">
         <v>238</v>
@@ -11251,10 +11080,10 @@
       </c>
       <c r="R70" s="12"/>
       <c r="S70" s="12">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="T70" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U70" s="12">
         <v>375</v>
@@ -11266,15 +11095,15 @@
         <v>4.3029999999999999</v>
       </c>
       <c r="AF70" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="AH70" s="60" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="AH70" s="59" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="71" spans="1:34" ht="20" customHeight="1">
       <c r="B71" s="21" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C71" s="54" t="s">
         <v>238</v>
@@ -11311,10 +11140,10 @@
       </c>
       <c r="R71" s="12"/>
       <c r="S71" s="12">
-        <v>39</v>
+        <v>416</v>
       </c>
       <c r="T71" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U71" s="12">
         <v>375</v>
@@ -11326,10 +11155,10 @@
         <v>8.4930000000000003</v>
       </c>
       <c r="AF71" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="AH71" s="60" t="s">
-        <v>362</v>
+        <v>352</v>
+      </c>
+      <c r="AH71" s="59" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -11414,27 +11243,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 AA39 A17 B18:I18 A21:J21 T21:W21 A22:W22 AA18:AE22 X18:X22 A12:AE12 A5:M8 A36:AE36 A38:M38 N38:O39 AI36:XFD38 AI19:AK20 AI39:AK39 AI21:XFD34 AH36:AH39 AH18:AH24 AI5:XFD18 R38:Y38 AD38:AE38 AC39 A13:AB13 R33:Y33 AA33:AE34 A37:O37 AA37:AE37 AA38:AB38 AH6:AH16 A10:C11 Z54:Z57 AF54:AG56 AF57 AH27:AH34 A23:AE25 A30:B32 J30:O32 AF6:AG40 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 Q37:Y37 Q37:Q39 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11">
-    <cfRule type="expression" dxfId="109" priority="72">
+    <cfRule type="expression" dxfId="93" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC13">
-    <cfRule type="expression" dxfId="108" priority="59">
+    <cfRule type="expression" dxfId="92" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="107" priority="58">
+    <cfRule type="expression" dxfId="91" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:M39 R39:Y39">
-    <cfRule type="expression" dxfId="106" priority="57">
+    <cfRule type="expression" dxfId="90" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC38">
-    <cfRule type="expression" dxfId="105" priority="56">
+    <cfRule type="expression" dxfId="89" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11523,7 +11352,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20 T20:W20">
-    <cfRule type="expression" dxfId="104" priority="48">
+    <cfRule type="expression" dxfId="88" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11612,12 +11441,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="103" priority="39">
+    <cfRule type="expression" dxfId="87" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 S20:S21 S19:W19">
-    <cfRule type="expression" dxfId="102" priority="40">
+    <cfRule type="expression" dxfId="86" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11706,137 +11535,137 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41:Q65">
-    <cfRule type="expression" dxfId="101" priority="38">
+    <cfRule type="expression" dxfId="85" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z22">
-    <cfRule type="expression" dxfId="100" priority="37">
+    <cfRule type="expression" dxfId="84" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="expression" dxfId="99" priority="36">
+    <cfRule type="expression" dxfId="83" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z37:Z39">
-    <cfRule type="expression" dxfId="98" priority="35">
+    <cfRule type="expression" dxfId="82" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z41:Z43">
-    <cfRule type="expression" dxfId="97" priority="34">
+    <cfRule type="expression" dxfId="81" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z48:Z52">
-    <cfRule type="expression" dxfId="96" priority="32">
+    <cfRule type="expression" dxfId="80" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z47">
-    <cfRule type="expression" dxfId="95" priority="30">
+    <cfRule type="expression" dxfId="79" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M59:O59 N60:O65">
-    <cfRule type="expression" dxfId="94" priority="23">
+    <cfRule type="expression" dxfId="78" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R59:R65">
-    <cfRule type="expression" dxfId="93" priority="22">
+    <cfRule type="expression" dxfId="77" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z62">
-    <cfRule type="expression" dxfId="92" priority="21">
+    <cfRule type="expression" dxfId="76" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:I62">
-    <cfRule type="expression" dxfId="91" priority="20">
+    <cfRule type="expression" dxfId="75" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C51">
-    <cfRule type="expression" dxfId="90" priority="19">
+    <cfRule type="expression" dxfId="74" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:I51">
-    <cfRule type="expression" dxfId="89" priority="18">
+    <cfRule type="expression" dxfId="73" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG57">
-    <cfRule type="expression" dxfId="88" priority="15">
+    <cfRule type="expression" dxfId="72" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I32">
-    <cfRule type="expression" dxfId="87" priority="14">
+    <cfRule type="expression" dxfId="71" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:I65">
-    <cfRule type="expression" dxfId="86" priority="13">
+    <cfRule type="expression" dxfId="70" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q21">
-    <cfRule type="expression" dxfId="85" priority="12">
+    <cfRule type="expression" dxfId="69" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="84" priority="11">
+    <cfRule type="expression" dxfId="68" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K21">
-    <cfRule type="expression" dxfId="83" priority="10">
+    <cfRule type="expression" dxfId="67" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
-    <cfRule type="expression" dxfId="82" priority="9">
+    <cfRule type="expression" dxfId="66" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44:P48">
-    <cfRule type="expression" dxfId="81" priority="8">
+    <cfRule type="expression" dxfId="65" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49:P52">
-    <cfRule type="expression" dxfId="80" priority="7">
+    <cfRule type="expression" dxfId="64" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54">
-    <cfRule type="expression" dxfId="79" priority="6">
+    <cfRule type="expression" dxfId="63" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P57">
-    <cfRule type="expression" dxfId="78" priority="5">
+    <cfRule type="expression" dxfId="62" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P59:P62">
-    <cfRule type="expression" dxfId="77" priority="4">
+    <cfRule type="expression" dxfId="61" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P63:P65">
-    <cfRule type="expression" dxfId="76" priority="3">
+    <cfRule type="expression" dxfId="60" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67:I71">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="59" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11860,10 +11689,10 @@
   <dimension ref="A1:AC86"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="N67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P70" sqref="P70"/>
+      <selection pane="bottomRight" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -15276,7 +15105,7 @@
         <v>EUR</v>
       </c>
       <c r="L41" s="13">
-        <f t="shared" ref="L41:L86" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L41:L85" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.87039999999999995</v>
       </c>
       <c r="M41" s="13">
@@ -17560,7 +17389,7 @@
         <v>318</v>
       </c>
       <c r="C70" s="21" t="str">
-        <f t="shared" ref="C70:E85" ca="1" si="32">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C70:C85" ca="1" si="32">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D70" s="15" t="s">
@@ -17930,7 +17759,7 @@
         <v>4.37</v>
       </c>
       <c r="N74" s="13" t="str">
-        <f t="shared" ref="N74:V86" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N74:V85" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O74" s="13">
@@ -18068,7 +17897,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="18">
-        <f t="shared" ref="J76:K86" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="J76:K85" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K76" s="18" t="str">
@@ -18398,7 +18227,7 @@
         <v>Google</v>
       </c>
       <c r="B81" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C81" s="21" t="str">
         <f t="shared" ca="1" si="32"/>
@@ -18408,7 +18237,7 @@
         <v>347</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="F81" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -18474,7 +18303,7 @@
         <v>347</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="F82" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -18513,7 +18342,7 @@
       </c>
       <c r="R82" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="S82" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -18540,7 +18369,7 @@
         <v>347</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="F83" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -18579,7 +18408,7 @@
       </c>
       <c r="R83" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="S83" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -18606,7 +18435,7 @@
         <v>347</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="F84" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -18645,7 +18474,7 @@
       </c>
       <c r="R84" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="S84" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -18672,7 +18501,7 @@
         <v>347</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="F85" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -18711,7 +18540,7 @@
       </c>
       <c r="R85" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>39</v>
+        <v>416</v>
       </c>
       <c r="S85" s="13" t="str">
         <f t="shared" ca="1" si="34"/>
@@ -18744,297 +18573,297 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="I23 I25 I27 I29 S13:S15 E23:G23 E18:I22 D26:D41 E17:F17 D10:D24 D3:D8 C3:C21 E7:G7 E9:I16 N16:O16 L30:O31 E3:I6 L4:O15 M16:M17 L16:L29 M18:O29 E8:H8 H58:H60 L50:S69 T53:Y69 L74:V74 W74:Y77 K56:K74 L70:Y73 F25:G29 E34:E36 H22:H30 F30:I30 I31 F36:G36 I36 E39:G40 I39:I40 E38 F31:G31 F32:I35 F37:I37 K4:K43 M32:O49 C30:C40 K75:T80 I66:I80 K3:O3 J3:J80">
-    <cfRule type="expression" dxfId="75" priority="129">
+    <cfRule type="expression" dxfId="58" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25 I24 F24:G24">
-    <cfRule type="expression" dxfId="74" priority="127">
+    <cfRule type="expression" dxfId="57" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="expression" dxfId="73" priority="126">
+    <cfRule type="expression" dxfId="56" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="72" priority="125">
+    <cfRule type="expression" dxfId="55" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="71" priority="116">
+    <cfRule type="expression" dxfId="54" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P15 P18:P49">
-    <cfRule type="expression" dxfId="70" priority="71">
+    <cfRule type="expression" dxfId="53" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:X3 T4:X12 T18:V31 T13:V15 W13:X31 R3:R15 U47:X49 T47:T52 R18:R49 Y6:Y49 T32:X46">
-    <cfRule type="expression" dxfId="69" priority="69">
+    <cfRule type="expression" dxfId="52" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C23">
-    <cfRule type="expression" dxfId="68" priority="78">
+    <cfRule type="expression" dxfId="51" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C25">
-    <cfRule type="expression" dxfId="67" priority="77">
+    <cfRule type="expression" dxfId="50" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C27">
-    <cfRule type="expression" dxfId="66" priority="76">
+    <cfRule type="expression" dxfId="49" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C29">
-    <cfRule type="expression" dxfId="65" priority="75">
+    <cfRule type="expression" dxfId="48" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q15 Q18:Q49">
-    <cfRule type="expression" dxfId="64" priority="70">
+    <cfRule type="expression" dxfId="47" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S12">
-    <cfRule type="expression" dxfId="63" priority="68">
+    <cfRule type="expression" dxfId="46" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S18:S49">
-    <cfRule type="expression" dxfId="62" priority="67">
+    <cfRule type="expression" dxfId="45" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:I17 N17:O17">
-    <cfRule type="expression" dxfId="61" priority="58">
+    <cfRule type="expression" dxfId="44" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P16:P17">
-    <cfRule type="expression" dxfId="60" priority="57">
+    <cfRule type="expression" dxfId="43" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:V17 R16:R17">
-    <cfRule type="expression" dxfId="59" priority="55">
+    <cfRule type="expression" dxfId="42" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16:Q17">
-    <cfRule type="expression" dxfId="58" priority="56">
+    <cfRule type="expression" dxfId="41" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:S17">
-    <cfRule type="expression" dxfId="57" priority="54">
+    <cfRule type="expression" dxfId="40" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="56" priority="53">
+    <cfRule type="expression" dxfId="39" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="55" priority="52">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="54" priority="51">
+    <cfRule type="expression" dxfId="37" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32:L49">
-    <cfRule type="expression" dxfId="53" priority="50">
+    <cfRule type="expression" dxfId="36" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="expression" dxfId="52" priority="49">
+    <cfRule type="expression" dxfId="35" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="51" priority="48">
+    <cfRule type="expression" dxfId="34" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="50" priority="45">
+    <cfRule type="expression" dxfId="33" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44 K44:K55">
-    <cfRule type="expression" dxfId="49" priority="43">
+    <cfRule type="expression" dxfId="32" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="48" priority="42">
+    <cfRule type="expression" dxfId="31" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="expression" dxfId="47" priority="41">
+    <cfRule type="expression" dxfId="30" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="46" priority="36">
+    <cfRule type="expression" dxfId="29" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="45" priority="35">
+    <cfRule type="expression" dxfId="28" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="44" priority="34">
+    <cfRule type="expression" dxfId="27" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48">
-    <cfRule type="expression" dxfId="43" priority="33">
+    <cfRule type="expression" dxfId="26" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="42" priority="32">
+    <cfRule type="expression" dxfId="25" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U50:Y52">
-    <cfRule type="expression" dxfId="41" priority="29">
+    <cfRule type="expression" dxfId="24" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="39" priority="25">
+    <cfRule type="expression" dxfId="22" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="38" priority="24">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="36" priority="22">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63:H65">
-    <cfRule type="expression" dxfId="35" priority="21">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57 G62">
-    <cfRule type="expression" dxfId="34" priority="20">
+    <cfRule type="expression" dxfId="17" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="expression" dxfId="33" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E29">
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" dxfId="31" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:H40">
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F81:O82">
-    <cfRule type="expression" dxfId="22" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83:O84">
-    <cfRule type="expression" dxfId="20" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F85:O86">
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T81:T84 R81:R84">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q81:Q84">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S81:S84">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T85 R85">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q85">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S85">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y81:Y85">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
TU, MS and Google offers links fixed.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="313">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1916,6 +1916,10 @@
   </si>
   <si>
     <t>2 x 240</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -10335,7 +10339,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="N22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -13421,6 +13425,9 @@
         <f t="shared" ca="1" si="31"/>
         <v>Reedbush-H reviewed</v>
       </c>
+      <c r="D37" s="15" t="s">
+        <v>312</v>
+      </c>
       <c r="E37" s="21" t="s">
         <v>204</v>
       </c>
@@ -13734,7 +13741,7 @@
     </row>
     <row r="41" spans="1:29" ht="20">
       <c r="A41" s="55">
-        <f t="shared" ref="A39:A45" ca="1" si="38">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="A41:A45" ca="1" si="38">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>0</v>
       </c>
       <c r="C41" s="21" t="str">
@@ -13955,9 +13962,6 @@
       <c r="C44" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>NV24</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>258</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>229</v>
@@ -14294,6 +14298,9 @@
       <c r="C49" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>64c416m8g</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>258</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>276</v>

</xml_diff>

<commit_message>
Added new LT offer.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33960" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="317">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1439,10 +1439,6 @@
   </si>
   <si>
     <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TITAN X</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1920,6 +1916,26 @@
   </si>
   <si>
     <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GTX Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Titan X min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTitanx2</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2289,7 +2305,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="793">
+  <cellStyleXfs count="803">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3016,6 +3032,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3207,7 +3233,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="793">
+  <cellStyles count="803">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3669,6 +3695,11 @@
     <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -3991,6 +4022,11 @@
     <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -4002,7 +4038,29 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4685,6 +4743,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -4983,10 +5052,10 @@
   <dimension ref="A1:FG62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="O32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="N25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AH42" sqref="AH42"/>
+      <selection pane="bottomRight" activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5083,7 +5152,7 @@
       <c r="AE3" s="58"/>
       <c r="AF3" s="58"/>
       <c r="AG3" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>32</v>
@@ -5258,13 +5327,13 @@
         <v>149</v>
       </c>
       <c r="O4" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>233</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>234</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>10</v>
@@ -5336,7 +5405,7 @@
         <v>2.91</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>21</v>
@@ -5549,7 +5618,7 @@
     </row>
     <row r="8" spans="1:163">
       <c r="A8" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>80</v>
@@ -5621,7 +5690,7 @@
     </row>
     <row r="9" spans="1:163">
       <c r="A9" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>106</v>
@@ -5718,7 +5787,7 @@
         <v>82</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="5" t="s">
@@ -5787,7 +5856,7 @@
         <v>84</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="5" t="s">
@@ -6265,7 +6334,7 @@
     </row>
     <row r="18" spans="1:163" s="12" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>43</v>
@@ -6775,7 +6844,7 @@
     </row>
     <row r="21" spans="1:163">
       <c r="A21" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>141</v>
@@ -6856,7 +6925,7 @@
       </c>
       <c r="AG21" s="15"/>
       <c r="AH21" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:163">
@@ -6963,7 +7032,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>16</v>
@@ -7047,7 +7116,7 @@
       </c>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:163">
@@ -7055,7 +7124,7 @@
         <v>59</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>40</v>
@@ -7139,13 +7208,13 @@
       </c>
       <c r="AG26" s="15"/>
       <c r="AH26" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:163" s="12" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>87</v>
@@ -7233,7 +7302,7 @@
     <row r="28" spans="1:163" s="12" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>88</v>
@@ -7321,10 +7390,10 @@
     <row r="29" spans="1:163" s="12" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" s="12">
         <v>8</v>
@@ -7406,7 +7475,7 @@
     <row r="30" spans="1:163" s="12" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>87</v>
@@ -7431,7 +7500,7 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L30" s="5">
         <v>1</v>
@@ -7491,7 +7560,7 @@
     <row r="31" spans="1:163" s="12" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>34</v>
@@ -7516,7 +7585,7 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L31" s="5">
         <v>1</v>
@@ -7576,10 +7645,10 @@
     <row r="32" spans="1:163" s="12" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="26" t="s">
         <v>212</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>213</v>
       </c>
       <c r="D32" s="12">
         <v>4</v>
@@ -7601,7 +7670,7 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L32" s="5">
         <v>1</v>
@@ -7660,7 +7729,7 @@
     </row>
     <row r="33" spans="1:163">
       <c r="B33" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>75</v>
@@ -7753,7 +7822,7 @@
     </row>
     <row r="34" spans="1:163">
       <c r="B34" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>76</v>
@@ -7838,7 +7907,7 @@
     <row r="35" spans="1:163" s="12" customFormat="1">
       <c r="A35" s="37"/>
       <c r="B35" s="38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C35" s="39" t="s">
         <v>125</v>
@@ -8090,7 +8159,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>191</v>
+        <v>312</v>
       </c>
       <c r="D37" s="26">
         <v>4</v>
@@ -8380,10 +8449,10 @@
     </row>
     <row r="41" spans="1:163" ht="23" customHeight="1">
       <c r="A41" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>146</v>
@@ -8469,15 +8538,15 @@
       </c>
       <c r="AG41" s="15"/>
       <c r="AH41" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:163" ht="24" customHeight="1">
       <c r="A42" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>147</v>
@@ -8538,7 +8607,7 @@
       <c r="V42" s="26"/>
       <c r="W42" s="26"/>
       <c r="X42" s="13">
-        <f t="shared" ref="X42:X43" si="12">40/8</f>
+        <f t="shared" ref="X42:X44" si="12">40/8</f>
         <v>5</v>
       </c>
       <c r="Y42" s="26">
@@ -8563,12 +8632,12 @@
       </c>
       <c r="AG42" s="15"/>
       <c r="AH42" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:163" ht="28" customHeight="1">
       <c r="B43" s="21" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>147</v>
@@ -8628,7 +8697,7 @@
       </c>
       <c r="V43" s="26"/>
       <c r="W43" s="26"/>
-      <c r="X43" s="13">
+      <c r="X43" s="26">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
@@ -8654,11 +8723,95 @@
       </c>
       <c r="AG43" s="15"/>
       <c r="AH43" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:163">
-      <c r="Q44" s="13"/>
+      <c r="B44" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="D44" s="13">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>3072</v>
+      </c>
+      <c r="F44">
+        <v>6.1660000000000004</v>
+      </c>
+      <c r="G44">
+        <v>0.192</v>
+      </c>
+      <c r="H44">
+        <v>12.288</v>
+      </c>
+      <c r="I44">
+        <v>336</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="L44" s="26">
+        <v>2</v>
+      </c>
+      <c r="M44" s="26">
+        <v>8</v>
+      </c>
+      <c r="N44" s="26">
+        <v>1.7</v>
+      </c>
+      <c r="O44" s="26">
+        <v>16</v>
+      </c>
+      <c r="P44" s="26">
+        <v>32</v>
+      </c>
+      <c r="Q44" s="26">
+        <f>M44*N44*P44/1000</f>
+        <v>0.43519999999999998</v>
+      </c>
+      <c r="R44" s="26">
+        <v>1866</v>
+      </c>
+      <c r="S44" s="26">
+        <v>32</v>
+      </c>
+      <c r="T44" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="U44" s="26">
+        <v>480</v>
+      </c>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="Y44" s="26">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="13" t="str">
+        <f t="shared" ref="Z44" si="13">X44&amp;"/"&amp;Y44</f>
+        <v>5/1</v>
+      </c>
+      <c r="AA44" s="48">
+        <f>0.03*60</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="AB44" s="48"/>
+      <c r="AC44" s="48">
+        <v>799</v>
+      </c>
+      <c r="AF44" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH44" s="15" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="45" spans="1:163" ht="20">
       <c r="A45" s="20" t="s">
@@ -8667,7 +8820,7 @@
       <c r="B45" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D45" s="13">
@@ -8692,7 +8845,7 @@
         <v>1</v>
       </c>
       <c r="K45" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L45" s="13">
         <v>2</v>
@@ -8732,7 +8885,7 @@
         <v>13.64</v>
       </c>
       <c r="Z45" s="13" t="str">
-        <f t="shared" ref="Z45:Z48" si="13">X45&amp;"/"&amp;Y45</f>
+        <f t="shared" ref="Z45:Z48" si="14">X45&amp;"/"&amp;Y45</f>
         <v>13.64/</v>
       </c>
       <c r="AD45" s="49">
@@ -8747,17 +8900,17 @@
         <v>6912</v>
       </c>
       <c r="AH45" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:163">
       <c r="A46" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D46" s="13">
@@ -8782,7 +8935,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L46" s="13">
         <v>2</v>
@@ -8818,11 +8971,11 @@
       <c r="V46" s="13"/>
       <c r="W46" s="13"/>
       <c r="X46" s="13">
-        <f t="shared" ref="X46:X48" si="14">13.64*4*2/8</f>
+        <f t="shared" ref="X46:X48" si="15">13.64*4*2/8</f>
         <v>13.64</v>
       </c>
       <c r="Z46" s="13" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13.64/</v>
       </c>
       <c r="AD46" s="49">
@@ -8837,14 +8990,14 @@
         <v>13824</v>
       </c>
       <c r="AH46" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:163">
       <c r="B47" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C47" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D47" s="13">
@@ -8869,7 +9022,7 @@
         <v>1</v>
       </c>
       <c r="K47" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L47" s="13">
         <v>2</v>
@@ -8903,11 +9056,11 @@
         <v>4000</v>
       </c>
       <c r="X47" s="13">
+        <f t="shared" si="15"/>
+        <v>13.64</v>
+      </c>
+      <c r="Z47" s="13" t="str">
         <f t="shared" si="14"/>
-        <v>13.64</v>
-      </c>
-      <c r="Z47" s="13" t="str">
-        <f t="shared" si="13"/>
         <v>13.64/</v>
       </c>
       <c r="AD47" s="49">
@@ -8922,14 +9075,14 @@
         <v>8640</v>
       </c>
       <c r="AH47" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:163">
       <c r="B48" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C48" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D48" s="13">
@@ -8954,7 +9107,7 @@
         <v>1</v>
       </c>
       <c r="K48" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L48" s="13">
         <v>2</v>
@@ -8988,11 +9141,11 @@
         <v>4000</v>
       </c>
       <c r="X48" s="13">
+        <f t="shared" si="15"/>
+        <v>13.64</v>
+      </c>
+      <c r="Z48" s="13" t="str">
         <f t="shared" si="14"/>
-        <v>13.64</v>
-      </c>
-      <c r="Z48" s="13" t="str">
-        <f t="shared" si="13"/>
         <v>13.64/</v>
       </c>
       <c r="AD48" s="49">
@@ -9007,10 +9160,11 @@
         <v>8640</v>
       </c>
       <c r="AH48" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:34">
+      <c r="C49" s="26"/>
       <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="1:34" ht="20">
@@ -9020,7 +9174,7 @@
       <c r="B50" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C50" s="53" t="s">
+      <c r="C50" s="26" t="s">
         <v>179</v>
       </c>
       <c r="D50" s="13">
@@ -9043,7 +9197,7 @@
       </c>
       <c r="J50" s="13"/>
       <c r="K50" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L50" s="13">
         <v>0.5</v>
@@ -9071,7 +9225,7 @@
         <v>56</v>
       </c>
       <c r="T50" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U50" s="13">
         <v>380</v>
@@ -9097,12 +9251,12 @@
     </row>
     <row r="51" spans="1:34">
       <c r="A51" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B51" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="53" t="s">
+      <c r="C51" s="26" t="s">
         <v>179</v>
       </c>
       <c r="D51" s="13">
@@ -9125,7 +9279,7 @@
       </c>
       <c r="J51" s="13"/>
       <c r="K51" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L51" s="13">
         <v>1</v>
@@ -9153,7 +9307,7 @@
         <v>112</v>
       </c>
       <c r="T51" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U51" s="13">
         <v>680</v>
@@ -9165,7 +9319,7 @@
         <v>1.8</v>
       </c>
       <c r="AC51" s="10">
-        <f t="shared" ref="AC51:AC53" si="15">AA51*24*31</f>
+        <f t="shared" ref="AC51:AC53" si="16">AA51*24*31</f>
         <v>1339.2</v>
       </c>
       <c r="AD51" s="54"/>
@@ -9176,12 +9330,12 @@
     </row>
     <row r="52" spans="1:34">
       <c r="A52" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B52" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C52" s="53" t="s">
+      <c r="C52" s="26" t="s">
         <v>179</v>
       </c>
       <c r="D52" s="13">
@@ -9204,7 +9358,7 @@
       </c>
       <c r="J52" s="13"/>
       <c r="K52" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L52" s="13">
         <v>2</v>
@@ -9232,7 +9386,7 @@
         <v>224</v>
       </c>
       <c r="T52" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U52" s="13">
         <v>1440</v>
@@ -9244,7 +9398,7 @@
         <v>3.6</v>
       </c>
       <c r="AC52" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2678.4</v>
       </c>
       <c r="AD52" s="54"/>
@@ -9257,7 +9411,7 @@
       <c r="B53" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="53" t="s">
+      <c r="C53" s="26" t="s">
         <v>179</v>
       </c>
       <c r="D53" s="13">
@@ -9280,7 +9434,7 @@
       </c>
       <c r="J53" s="13"/>
       <c r="K53" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L53" s="13">
         <v>2</v>
@@ -9308,7 +9462,7 @@
         <v>224</v>
       </c>
       <c r="T53" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U53" s="13">
         <v>1440</v>
@@ -9318,14 +9472,14 @@
       </c>
       <c r="Y53" s="13"/>
       <c r="Z53" s="13" t="str">
-        <f t="shared" ref="Z53" si="16">X53&amp;"/"&amp;Y53</f>
+        <f t="shared" ref="Z53" si="17">X53&amp;"/"&amp;Y53</f>
         <v>Infiniband/</v>
       </c>
       <c r="AA53" s="23">
         <v>3.96</v>
       </c>
       <c r="AC53" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2946.24</v>
       </c>
       <c r="AD53" s="54"/>
@@ -9339,10 +9493,10 @@
     </row>
     <row r="54" spans="1:34">
       <c r="B54" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D54" s="13">
         <v>1</v>
@@ -9363,7 +9517,7 @@
         <v>71</v>
       </c>
       <c r="K54" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L54" s="13">
         <v>0.5</v>
@@ -9391,7 +9545,7 @@
         <v>56</v>
       </c>
       <c r="T54" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U54">
         <v>340</v>
@@ -9405,10 +9559,10 @@
     </row>
     <row r="55" spans="1:34">
       <c r="B55" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D55" s="13">
         <v>2</v>
@@ -9429,7 +9583,7 @@
         <v>71</v>
       </c>
       <c r="K55" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L55" s="13">
         <v>1</v>
@@ -9457,7 +9611,7 @@
         <v>112</v>
       </c>
       <c r="T55" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U55">
         <v>680</v>
@@ -9471,10 +9625,10 @@
     </row>
     <row r="56" spans="1:34">
       <c r="B56" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>223</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>224</v>
       </c>
       <c r="D56" s="13">
         <v>4</v>
@@ -9495,7 +9649,7 @@
         <v>71</v>
       </c>
       <c r="K56" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L56" s="13">
         <v>2</v>
@@ -9523,7 +9677,7 @@
         <v>224</v>
       </c>
       <c r="T56" s="53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U56">
         <v>1440</v>
@@ -9540,10 +9694,10 @@
     </row>
     <row r="58" spans="1:34" ht="20" customHeight="1">
       <c r="A58" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C58" s="53" t="s">
         <v>179</v>
@@ -9582,7 +9736,7 @@
         <v>39</v>
       </c>
       <c r="T58" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U58">
         <v>375</v>
@@ -9591,18 +9745,18 @@
         <v>1.073</v>
       </c>
       <c r="AF58" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AH58" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:34" ht="20" customHeight="1">
       <c r="A59" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C59" s="53" t="s">
         <v>179</v>
@@ -9642,7 +9796,7 @@
         <v>78</v>
       </c>
       <c r="T59" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U59" s="12">
         <v>375</v>
@@ -9654,18 +9808,18 @@
         <v>2.0339999999999998</v>
       </c>
       <c r="AF59" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AH59" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:34" ht="20" customHeight="1">
       <c r="A60" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C60" s="53" t="s">
         <v>179</v>
@@ -9705,7 +9859,7 @@
         <v>156</v>
       </c>
       <c r="T60" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U60" s="12">
         <v>375</v>
@@ -9717,15 +9871,15 @@
         <v>3.9550000000000001</v>
       </c>
       <c r="AF60" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AH60" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:34" ht="20" customHeight="1">
       <c r="B61" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C61" s="53" t="s">
         <v>179</v>
@@ -9765,7 +9919,7 @@
         <v>208</v>
       </c>
       <c r="T61" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U61" s="12">
         <v>375</v>
@@ -9777,15 +9931,15 @@
         <v>4.3029999999999999</v>
       </c>
       <c r="AF61" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AH61" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:34" ht="20" customHeight="1">
       <c r="B62" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C62" s="53" t="s">
         <v>179</v>
@@ -9825,7 +9979,7 @@
         <v>416</v>
       </c>
       <c r="T62" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U62" s="12">
         <v>375</v>
@@ -9837,10 +9991,10 @@
         <v>8.4930000000000003</v>
       </c>
       <c r="AF62" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AH62" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -9853,7 +10007,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AI37">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9865,7 +10019,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ37">
-    <cfRule type="colorScale" priority="85">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9877,7 +10031,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="81">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9889,7 +10043,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9901,7 +10055,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9913,7 +10067,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9924,33 +10078,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 AA39 A17 B18:I18 T21:W21 AA18:AE22 A12:AE12 A5:M8 A36:AE36 A38:M38 N38:O39 AI36:XFD38 AI19:AK20 AI39:AK39 AI21:XFD34 AH36:AH39 AH18:AH24 AI5:XFD18 R38:Y38 AD38:AE38 AC39 A13:AB13 R33:Y33 AA33:AE34 A37:O37 AA37:AE37 AA38:AB38 AH6:AH16 A10:C11 Z45:Z48 AF45:AG47 AF48 AH27:AH34 A23:AE25 A30:B32 J30:O32 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 Q37:Y37 Q37:Q39 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11 AF6:AG40 A21:J21 A22:W22 Q41:Q56">
-    <cfRule type="expression" dxfId="61" priority="72">
+  <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 AA39 A17 B18:I18 T21:W21 AA18:AE22 A12:AE12 A5:M8 A36:AE36 A38:M38 N38:O39 AI36:XFD38 AI19:AK20 AI39:AK39 AI21:XFD34 AH36:AH39 AH18:AH24 AI5:XFD18 R38:Y38 AD38:AE38 AC39 A13:AB13 R33:Y33 AA33:AE34 A37:O37 AA37:AE37 AA38:AB38 AH6:AH16 A10:C11 Z45:Z48 AF45:AG47 AF48 AH27:AH34 A23:AE25 A30:B32 J30:O32 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 Q37:Y37 Q37:Q39 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11 AF6:AG40 A21:J21 A22:W22 Q41:Q43 Q45:Q56">
+    <cfRule type="expression" dxfId="64" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC13">
-    <cfRule type="expression" dxfId="60" priority="59">
+    <cfRule type="expression" dxfId="63" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="59" priority="58">
+    <cfRule type="expression" dxfId="62" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:M39 R39:Y39">
-    <cfRule type="expression" dxfId="58" priority="57">
+    <cfRule type="expression" dxfId="61" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC38">
-    <cfRule type="expression" dxfId="57" priority="56">
+    <cfRule type="expression" dxfId="60" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI39 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="157">
+    <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9962,7 +10116,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ39 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="161">
+    <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9974,7 +10128,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI37 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="165">
+    <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9986,7 +10140,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="169">
+    <cfRule type="colorScale" priority="170">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -9998,7 +10152,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK36:AK39 AK21:AK34 AK5:AK18">
-    <cfRule type="colorScale" priority="173">
+    <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10010,7 +10164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="177">
+    <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10022,7 +10176,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="180">
+    <cfRule type="colorScale" priority="181">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10034,12 +10188,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20 T20:W20">
-    <cfRule type="expression" dxfId="56" priority="48">
+    <cfRule type="expression" dxfId="59" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10051,7 +10205,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10063,7 +10217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10075,7 +10229,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10087,7 +10241,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10099,7 +10253,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10111,7 +10265,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10123,17 +10277,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="55" priority="39">
+    <cfRule type="expression" dxfId="58" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 S20:S21 S19:W19">
-    <cfRule type="expression" dxfId="54" priority="40">
+    <cfRule type="expression" dxfId="57" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10145,7 +10299,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10157,7 +10311,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10169,7 +10323,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10181,7 +10335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK19">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10193,7 +10347,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10205,7 +10359,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10217,102 +10371,107 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z22">
-    <cfRule type="expression" dxfId="53" priority="37">
+    <cfRule type="expression" dxfId="56" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="expression" dxfId="52" priority="36">
+    <cfRule type="expression" dxfId="55" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z37:Z39">
-    <cfRule type="expression" dxfId="51" priority="35">
+    <cfRule type="expression" dxfId="54" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z41:Z43">
-    <cfRule type="expression" dxfId="50" priority="34">
+  <conditionalFormatting sqref="Z41:Z44">
+    <cfRule type="expression" dxfId="53" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50:O50 N51:O56">
-    <cfRule type="expression" dxfId="49" priority="23">
+    <cfRule type="expression" dxfId="52" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R50:R56">
-    <cfRule type="expression" dxfId="48" priority="22">
+    <cfRule type="expression" dxfId="51" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z53">
-    <cfRule type="expression" dxfId="47" priority="21">
+    <cfRule type="expression" dxfId="50" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:I53">
-    <cfRule type="expression" dxfId="46" priority="20">
+    <cfRule type="expression" dxfId="49" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG48">
-    <cfRule type="expression" dxfId="45" priority="15">
+    <cfRule type="expression" dxfId="48" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I32">
-    <cfRule type="expression" dxfId="44" priority="14">
+    <cfRule type="expression" dxfId="47" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:I56">
-    <cfRule type="expression" dxfId="43" priority="13">
+    <cfRule type="expression" dxfId="46" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q21">
-    <cfRule type="expression" dxfId="42" priority="12">
+    <cfRule type="expression" dxfId="45" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="41" priority="11">
+    <cfRule type="expression" dxfId="44" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K21">
-    <cfRule type="expression" dxfId="40" priority="10">
+    <cfRule type="expression" dxfId="43" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
-    <cfRule type="expression" dxfId="39" priority="9">
+    <cfRule type="expression" dxfId="42" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P45">
-    <cfRule type="expression" dxfId="38" priority="6">
+    <cfRule type="expression" dxfId="41" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P46:P48">
-    <cfRule type="expression" dxfId="37" priority="5">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P50:P53">
-    <cfRule type="expression" dxfId="36" priority="4">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54:P56">
-    <cfRule type="expression" dxfId="35" priority="3">
+    <cfRule type="expression" dxfId="38" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:I62">
-    <cfRule type="expression" dxfId="34" priority="1">
+    <cfRule type="expression" dxfId="37" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q44">
+    <cfRule type="expression" dxfId="36" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10333,13 +10492,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AC50"/>
+  <dimension ref="A1:AC51"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="N22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -10379,25 +10538,25 @@
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
       <c r="F1" s="45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L1" s="45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M1" s="45" t="s">
         <v>145</v>
@@ -10415,28 +10574,28 @@
         <v>130</v>
       </c>
       <c r="R1" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="S1" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="T1" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="V1" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="V1" s="45" t="s">
+      <c r="W1" s="45" t="s">
+        <v>248</v>
+      </c>
+      <c r="X1" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="W1" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="X1" s="45" t="s">
+      <c r="Y1" s="45" t="s">
         <v>247</v>
-      </c>
-      <c r="Y1" s="45" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" ht="21" thickBot="1">
@@ -10474,7 +10633,7 @@
         <v>159</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>161</v>
@@ -10510,7 +10669,7 @@
         <v>119</v>
       </c>
       <c r="X2" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Y2" s="28" t="s">
         <v>120</v>
@@ -10634,7 +10793,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="18" t="str">
-        <f t="shared" ref="K4:K42" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="K4:K43" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L4" s="13">
@@ -10790,7 +10949,7 @@
         <v>105</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F6" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -10875,7 +11034,7 @@
         <v>164</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -10963,7 +11122,7 @@
         <v>165</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -11052,7 +11211,7 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11138,7 +11297,7 @@
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -11221,7 +11380,7 @@
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -11394,7 +11553,7 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11404,7 +11563,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18">
-        <f t="shared" ref="J13:J36" ca="1" si="10">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="J13:J37" ca="1" si="10">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K13" s="18" t="str">
@@ -11475,7 +11634,7 @@
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F14" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11541,7 +11700,7 @@
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" ref="F15:F16" ca="1" si="11">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11607,7 +11766,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F16" s="18">
         <f t="shared" ca="1" si="11"/>
@@ -11679,7 +11838,7 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18">
@@ -11766,7 +11925,7 @@
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18">
@@ -11853,7 +12012,7 @@
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18">
@@ -11940,7 +12099,7 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18">
@@ -12027,7 +12186,7 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18">
@@ -12114,7 +12273,7 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18">
@@ -12201,7 +12360,7 @@
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18">
@@ -12271,7 +12430,7 @@
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="15">
-        <f t="shared" ref="Y23:Y41" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="Y23:Y42" ca="1" si="22">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="Z23" s="15"/>
@@ -12294,7 +12453,7 @@
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18">
@@ -12379,7 +12538,7 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18">
@@ -12464,7 +12623,7 @@
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18">
@@ -12549,7 +12708,7 @@
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18">
@@ -12642,7 +12801,7 @@
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F28" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -12678,7 +12837,7 @@
       </c>
       <c r="N28" s="13" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>TITAN X</v>
+        <v>Titan X</v>
       </c>
       <c r="O28" s="13">
         <f t="shared" ca="1" si="18"/>
@@ -12733,7 +12892,7 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
@@ -12815,7 +12974,7 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
@@ -12904,7 +13063,7 @@
         <v>2 x GeForce GTX 1080 min.</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F31" s="12">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -12927,15 +13086,15 @@
         <v>EUR</v>
       </c>
       <c r="L31" s="13">
-        <f t="shared" ref="L31:L49" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L31:L50" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.87039999999999995</v>
       </c>
       <c r="M31" s="13">
-        <f t="shared" ref="M31:M44" ca="1" si="27">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M31:M45" ca="1" si="27">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>16.456</v>
       </c>
       <c r="N31" s="13" t="str">
-        <f t="shared" ref="N31:W33" ca="1" si="28">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N31:W34" ca="1" si="28">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>GeForce GTX 1080</v>
       </c>
       <c r="O31" s="13">
@@ -12989,10 +13148,10 @@
         <v>4 x GeForce GTX 1080 ltd. min.</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F32" s="12">
-        <f t="shared" ref="F32:H33" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="F32:H34" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>1.7999999999999998</v>
       </c>
       <c r="G32" s="18">
@@ -13075,7 +13234,7 @@
       </c>
       <c r="D33" s="40"/>
       <c r="E33" s="38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F33" s="12">
         <f t="shared" ca="1" si="29"/>
@@ -13155,111 +13314,108 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="20">
-      <c r="A34" s="55" t="str">
-        <f t="shared" ref="A34:A37" ca="1" si="30">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>The University of Tokyo</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>231</v>
-      </c>
+    <row r="34" spans="1:29" s="12" customFormat="1">
       <c r="C34" s="21" t="str">
-        <f t="shared" ref="C34:C49" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>Reedbush-H Personal (educational)</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="I34" s="18">
-        <f t="shared" ref="I34:J44" ca="1" si="32">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>138888.88888888888</v>
-      </c>
-      <c r="J34" s="18">
-        <f t="shared" ca="1" si="10"/>
-        <v>0</v>
-      </c>
+        <f ca="1">INDIRECT("Sheet1!B" &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>2 x Titan X min.</v>
+      </c>
+      <c r="D34" s="40"/>
+      <c r="E34" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" ca="1" si="29"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18">
+        <f t="shared" ca="1" si="29"/>
+        <v>799</v>
+      </c>
+      <c r="I34" s="40"/>
+      <c r="J34" s="18"/>
       <c r="K34" s="18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="L34" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>2.4192000000000005</v>
+        <v>0.87039999999999995</v>
       </c>
       <c r="M34" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>19</v>
+        <v>12.332000000000001</v>
       </c>
       <c r="N34" s="13" t="str">
-        <f t="shared" ref="N34:X38" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>P100</v>
+        <f t="shared" ca="1" si="28"/>
+        <v>GTX Titan X</v>
       </c>
       <c r="O34" s="13">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="28"/>
         <v>2</v>
       </c>
       <c r="P34" s="13" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v>Xeon E5-2695 v4</v>
+        <f t="shared" ca="1" si="28"/>
+        <v>Xeon E5-2609 v4</v>
       </c>
       <c r="Q34" s="13">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="28"/>
         <v>2</v>
       </c>
       <c r="R34" s="13">
-        <f t="shared" ca="1" si="33"/>
-        <v>256</v>
+        <f t="shared" ca="1" si="28"/>
+        <v>32</v>
       </c>
       <c r="S34" s="13" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v>PFS</v>
+        <f t="shared" ca="1" si="28"/>
+        <v>SSD</v>
       </c>
       <c r="T34" s="13">
-        <f t="shared" ca="1" si="33"/>
-        <v>1000</v>
+        <f t="shared" ca="1" si="28"/>
+        <v>480</v>
       </c>
       <c r="U34" s="13">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="28"/>
         <v>0</v>
       </c>
       <c r="V34" s="13">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="28"/>
         <v>0</v>
       </c>
       <c r="W34" s="13" t="str">
-        <f t="shared" ca="1" si="33"/>
-        <v>13.64/</v>
-      </c>
-      <c r="X34" s="13">
-        <f t="shared" ca="1" si="33"/>
-        <v>6912</v>
-      </c>
+        <f t="shared" ca="1" si="28"/>
+        <v>5/1</v>
+      </c>
+      <c r="X34" s="13"/>
       <c r="Y34" s="15" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
+        <v>Hourly plan charged minutely. Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
       <c r="AC34" s="42">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="20">
-      <c r="A35" s="55"/>
+      <c r="A35" s="55" t="str">
+        <f t="shared" ref="A35:A38" ca="1" si="30">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>The University of Tokyo</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>230</v>
+      </c>
       <c r="C35" s="21" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>Reedbush-H (educational)</v>
+        <f t="shared" ref="C35:C50" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="I35" s="18">
-        <f t="shared" ca="1" si="32"/>
-        <v>277777.77777777775</v>
+        <f t="shared" ref="I35:J45" ca="1" si="32">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>138888.88888888888</v>
       </c>
       <c r="J35" s="18">
         <f t="shared" ca="1" si="10"/>
@@ -13278,7 +13434,7 @@
         <v>19</v>
       </c>
       <c r="N35" s="13" t="str">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ref="N35:X39" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>P100</v>
       </c>
       <c r="O35" s="13">
@@ -13303,7 +13459,7 @@
       </c>
       <c r="T35" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="U35" s="13">
         <f t="shared" ca="1" si="33"/>
@@ -13319,34 +13475,31 @@
       </c>
       <c r="X35" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>13824</v>
+        <v>6912</v>
       </c>
       <c r="Y35" s="15" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
+        <v>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
       </c>
       <c r="AC35" s="42">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="12" customFormat="1" ht="20">
-      <c r="A36" s="55">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
+    <row r="36" spans="1:29" ht="20">
+      <c r="A36" s="55"/>
       <c r="C36" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>Reedbush-H reviewed (educational)</v>
+        <v>Reedbush-H (educational)</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I36" s="18">
         <f t="shared" ca="1" si="32"/>
-        <v>166666.66666666666</v>
+        <v>277777.77777777775</v>
       </c>
       <c r="J36" s="18">
         <f t="shared" ca="1" si="10"/>
@@ -13406,14 +13559,14 @@
       </c>
       <c r="X36" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>8640</v>
+        <v>13824</v>
       </c>
       <c r="Y36" s="15" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+        <v>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
       </c>
       <c r="AC36" s="42">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:29" s="12" customFormat="1" ht="20">
@@ -13423,20 +13576,20 @@
       </c>
       <c r="C37" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>Reedbush-H reviewed</v>
+        <v>Reedbush-H reviewed (educational)</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>312</v>
+        <v>195</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>204</v>
       </c>
       <c r="I37" s="18">
         <f t="shared" ca="1" si="32"/>
-        <v>200000</v>
+        <v>166666.66666666666</v>
       </c>
       <c r="J37" s="18">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="10"/>
         <v>0</v>
       </c>
       <c r="K37" s="18" t="str">
@@ -13500,116 +13653,121 @@
         <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
       <c r="AC37" s="42">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" s="12" customFormat="1" ht="20">
+      <c r="A38" s="55">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="C38" s="21" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>Reedbush-H reviewed</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="I38" s="18">
+        <f t="shared" ca="1" si="32"/>
+        <v>200000</v>
+      </c>
+      <c r="J38" s="18">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="18" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>JPY</v>
+      </c>
+      <c r="L38" s="13">
+        <f t="shared" ca="1" si="26"/>
+        <v>2.4192000000000005</v>
+      </c>
+      <c r="M38" s="13">
+        <f t="shared" ca="1" si="27"/>
+        <v>19</v>
+      </c>
+      <c r="N38" s="13" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>P100</v>
+      </c>
+      <c r="O38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="P38" s="13" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>Xeon E5-2695 v4</v>
+      </c>
+      <c r="Q38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="R38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>256</v>
+      </c>
+      <c r="S38" s="13" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>PFS</v>
+      </c>
+      <c r="T38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>4000</v>
+      </c>
+      <c r="U38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="13" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>13.64/</v>
+      </c>
+      <c r="X38" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>8640</v>
+      </c>
+      <c r="Y38" s="15" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+      </c>
+      <c r="AC38" s="42">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:29" ht="20">
-      <c r="A38" s="55" t="str">
+    <row r="39" spans="1:29" ht="20">
+      <c r="A39" s="55" t="str">
         <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>MS Azure</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C38" s="21" t="str">
+      <c r="C39" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>NC6</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E39" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="F38" s="12">
-        <f t="shared" ref="F38:F44" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+      <c r="F39" s="12">
+        <f t="shared" ref="F39:F45" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0.9</v>
-      </c>
-      <c r="I38" s="18">
-        <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="18">
-        <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>USD</v>
-      </c>
-      <c r="L38" s="13">
-        <f t="shared" ca="1" si="26"/>
-        <v>0.49920000000000003</v>
-      </c>
-      <c r="M38" s="13">
-        <f t="shared" ca="1" si="27"/>
-        <v>4.37</v>
-      </c>
-      <c r="N38" s="13" t="str">
-        <f t="shared" ref="N38:V49" ca="1" si="35">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>K80</v>
-      </c>
-      <c r="O38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="P38" s="13" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v>Xeon E5-2690 v3</v>
-      </c>
-      <c r="Q38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="R38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>56</v>
-      </c>
-      <c r="S38" s="13" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v>SATA</v>
-      </c>
-      <c r="T38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>380</v>
-      </c>
-      <c r="U38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="V38" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="W38" s="13">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="X38" s="13"/>
-      <c r="Y38" s="15" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v xml:space="preserve">1 GPU in specification is 1/2 of K80 </v>
-      </c>
-      <c r="AC38" s="42">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" ht="20">
-      <c r="A39" s="55"/>
-      <c r="C39" s="21" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>NC12</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" s="12">
-        <f t="shared" ca="1" si="34"/>
-        <v>1.8</v>
       </c>
       <c r="I39" s="18">
         <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J39" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="K39" s="18" t="str">
@@ -13618,19 +13776,19 @@
       </c>
       <c r="L39" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.99840000000000007</v>
+        <v>0.49920000000000003</v>
       </c>
       <c r="M39" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>8.74</v>
+        <v>4.37</v>
       </c>
       <c r="N39" s="13" t="str">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ref="N39:V50" ca="1" si="35">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O39" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P39" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13638,11 +13796,11 @@
       </c>
       <c r="Q39" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R39" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="S39" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13650,40 +13808,48 @@
       </c>
       <c r="T39" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>680</v>
+        <v>380</v>
+      </c>
+      <c r="U39" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
       </c>
       <c r="W39" s="13">
-        <f t="shared" ref="W39:W41" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="X39" s="13"/>
-      <c r="Y39" s="15">
+      <c r="Y39" s="15" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>0</v>
+        <v xml:space="preserve">1 GPU in specification is 1/2 of K80 </v>
       </c>
       <c r="AC39" s="42">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="20">
       <c r="A40" s="55"/>
       <c r="C40" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>NC24</v>
+        <v>NC12</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F40" s="12">
         <f t="shared" ca="1" si="34"/>
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
       <c r="I40" s="18">
         <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J40" s="18">
-        <f t="shared" ref="J40:K49" ca="1" si="37">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K40" s="18" t="str">
@@ -13692,11 +13858,11 @@
       </c>
       <c r="L40" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>1.9968000000000001</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="M40" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>17.48</v>
+        <v>8.74</v>
       </c>
       <c r="N40" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13704,7 +13870,7 @@
       </c>
       <c r="O40" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P40" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13712,11 +13878,11 @@
       </c>
       <c r="Q40" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R40" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="S40" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13724,10 +13890,10 @@
       </c>
       <c r="T40" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1440</v>
+        <v>680</v>
       </c>
       <c r="W40" s="13">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ref="W40:W42" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="X40" s="13"/>
@@ -13736,31 +13902,28 @@
         <v>0</v>
       </c>
       <c r="AC40" s="42">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="20">
-      <c r="A41" s="55">
-        <f t="shared" ref="A41:A45" ca="1" si="38">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>0</v>
-      </c>
+      <c r="A41" s="55"/>
       <c r="C41" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>NC24r</v>
+        <v>NC24</v>
       </c>
       <c r="E41" s="21" t="s">
         <v>192</v>
       </c>
       <c r="F41" s="12">
         <f t="shared" ca="1" si="34"/>
-        <v>3.96</v>
+        <v>3.6</v>
       </c>
       <c r="I41" s="18">
         <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="J41" s="18">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ref="J41:K50" ca="1" si="37">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K41" s="18" t="str">
@@ -13803,36 +13966,35 @@
         <f t="shared" ca="1" si="35"/>
         <v>1440</v>
       </c>
-      <c r="W41" s="13" t="str">
+      <c r="W41" s="13">
         <f t="shared" ca="1" si="36"/>
-        <v>Infiniband/</v>
+        <v>0</v>
       </c>
       <c r="X41" s="13"/>
-      <c r="Y41" s="15" t="str">
+      <c r="Y41" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>RDMA capable</v>
+        <v>0</v>
       </c>
       <c r="AC41" s="42">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="20">
       <c r="A42" s="55">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ref="A42:A46" ca="1" si="38">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>0</v>
       </c>
       <c r="C42" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>NV6</v>
+        <v>NC24r</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="F42" s="12">
         <f t="shared" ca="1" si="34"/>
-        <v>1.24</v>
-      </c>
-      <c r="H42" s="12"/>
+        <v>3.96</v>
+      </c>
       <c r="I42" s="18">
         <f t="shared" ca="1" si="32"/>
         <v>0</v>
@@ -13847,19 +14009,19 @@
       </c>
       <c r="L42" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.49920000000000003</v>
+        <v>1.9968000000000001</v>
       </c>
       <c r="M42" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>9.65</v>
+        <v>17.48</v>
       </c>
       <c r="N42" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
-        <v>M60</v>
+        <v>K80</v>
       </c>
       <c r="O42" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P42" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13867,11 +14029,11 @@
       </c>
       <c r="Q42" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R42" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>56</v>
+        <v>224</v>
       </c>
       <c r="S42" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13879,10 +14041,19 @@
       </c>
       <c r="T42" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>340</v>
+        <v>1440</v>
+      </c>
+      <c r="W42" s="13" t="str">
+        <f t="shared" ca="1" si="36"/>
+        <v>Infiniband/</v>
+      </c>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="15" t="str">
+        <f t="shared" ca="1" si="22"/>
+        <v>RDMA capable</v>
       </c>
       <c r="AC42" s="42">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="20">
@@ -13892,14 +14063,14 @@
       </c>
       <c r="C43" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>NV12</v>
+        <v>NV6</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F43" s="12">
         <f t="shared" ca="1" si="34"/>
-        <v>2.48</v>
+        <v>1.24</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="18">
@@ -13911,16 +14082,16 @@
         <v>0</v>
       </c>
       <c r="K43" s="18" t="str">
-        <f t="shared" ref="K43:K44" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>USD</v>
       </c>
       <c r="L43" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.99840000000000007</v>
+        <v>0.49920000000000003</v>
       </c>
       <c r="M43" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>19.3</v>
+        <v>9.65</v>
       </c>
       <c r="N43" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13928,7 +14099,7 @@
       </c>
       <c r="O43" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P43" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13936,11 +14107,11 @@
       </c>
       <c r="Q43" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R43" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="S43" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13948,10 +14119,10 @@
       </c>
       <c r="T43" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="AC43" s="42">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="20">
@@ -13961,14 +14132,14 @@
       </c>
       <c r="C44" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>NV24</v>
+        <v>NV12</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F44" s="12">
         <f t="shared" ca="1" si="34"/>
-        <v>4.97</v>
+        <v>2.48</v>
       </c>
       <c r="H44" s="12"/>
       <c r="I44" s="18">
@@ -13980,16 +14151,16 @@
         <v>0</v>
       </c>
       <c r="K44" s="18" t="str">
-        <f t="shared" ca="1" si="39"/>
+        <f t="shared" ref="K44:K45" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L44" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>1.9968000000000001</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="M44" s="13">
         <f t="shared" ca="1" si="27"/>
-        <v>38.6</v>
+        <v>19.3</v>
       </c>
       <c r="N44" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -13997,7 +14168,7 @@
       </c>
       <c r="O44" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P44" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14005,11 +14176,11 @@
       </c>
       <c r="Q44" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R44" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="S44" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14017,99 +14188,102 @@
       </c>
       <c r="T44" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1440</v>
+        <v>680</v>
       </c>
       <c r="AC44" s="42">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="20">
-      <c r="A45" s="55" t="str">
+      <c r="A45" s="55">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="21" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>NV24</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" ca="1" si="34"/>
+        <v>4.97</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="18">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="18">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="18" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>USD</v>
+      </c>
+      <c r="L45" s="13">
+        <f t="shared" ca="1" si="26"/>
+        <v>1.9968000000000001</v>
+      </c>
+      <c r="M45" s="13">
+        <f t="shared" ca="1" si="27"/>
+        <v>38.6</v>
+      </c>
+      <c r="N45" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>M60</v>
+      </c>
+      <c r="O45" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="P45" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>Xeon E5-2690 v3</v>
+      </c>
+      <c r="Q45" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="R45" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>224</v>
+      </c>
+      <c r="S45" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>SATA</v>
+      </c>
+      <c r="T45" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>1440</v>
+      </c>
+      <c r="AC45" s="42">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="20">
+      <c r="A46" s="55" t="str">
         <f t="shared" ca="1" si="38"/>
         <v>Google</v>
       </c>
-      <c r="B45" t="s">
-        <v>269</v>
-      </c>
-      <c r="C45" s="21" t="str">
+      <c r="B46" t="s">
+        <v>268</v>
+      </c>
+      <c r="C46" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>6c39m1g</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="F45" s="18">
+      <c r="D46" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="F46" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>1.073</v>
-      </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18">
-        <f t="shared" ca="1" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="18" t="str">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>USD</v>
-      </c>
-      <c r="L45" s="13">
-        <f t="shared" ca="1" si="26"/>
-        <v>0.16919999999999999</v>
-      </c>
-      <c r="M45" s="13">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
-        <v>4.37</v>
-      </c>
-      <c r="N45" s="13" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v>K80</v>
-      </c>
-      <c r="O45" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q45" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>6</v>
-      </c>
-      <c r="R45" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>39</v>
-      </c>
-      <c r="S45" s="13" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v>SSD</v>
-      </c>
-      <c r="T45" s="13">
-        <f t="shared" ca="1" si="35"/>
-        <v>375</v>
-      </c>
-      <c r="Y45" s="15" t="str">
-        <f t="shared" ref="Y45:Y49" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
-      </c>
-      <c r="AC45" s="42">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:29">
-      <c r="C46" s="21" t="str">
-        <f t="shared" ca="1" si="31"/>
-        <v>12c78m2g</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>273</v>
-      </c>
-      <c r="F46" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>2.0339999999999998</v>
       </c>
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
@@ -14119,16 +14293,16 @@
         <v>0</v>
       </c>
       <c r="K46" s="18" t="str">
-        <f t="shared" ca="1" si="37"/>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L46" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.33839999999999998</v>
+        <v>0.16919999999999999</v>
       </c>
       <c r="M46" s="13">
-        <f t="shared" ref="M46" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
-        <v>8.74</v>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>4.37</v>
       </c>
       <c r="N46" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14136,15 +14310,15 @@
       </c>
       <c r="O46" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q46" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="R46" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="S46" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14155,27 +14329,27 @@
         <v>375</v>
       </c>
       <c r="Y46" s="15" t="str">
-        <f t="shared" ca="1" si="40"/>
+        <f t="shared" ref="Y46:Y50" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC46" s="42">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:29">
       <c r="C47" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>24c156m4g</v>
+        <v>12c78m2g</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F47" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>3.9550000000000001</v>
+        <v>2.0339999999999998</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
@@ -14185,16 +14359,16 @@
         <v>0</v>
       </c>
       <c r="K47" s="18" t="str">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="37"/>
         <v>USD</v>
       </c>
       <c r="L47" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.67679999999999996</v>
+        <v>0.33839999999999998</v>
       </c>
       <c r="M47" s="13">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
-        <v>17.48</v>
+        <f t="shared" ref="M47" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>8.74</v>
       </c>
       <c r="N47" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14202,15 +14376,15 @@
       </c>
       <c r="O47" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q47" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="R47" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="S47" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14225,23 +14399,23 @@
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC47" s="42">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:29">
       <c r="C48" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>32c208m4g</v>
+        <v>24c156m4g</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F48" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>4.3029999999999999</v>
+        <v>3.9550000000000001</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -14251,15 +14425,15 @@
         <v>0</v>
       </c>
       <c r="K48" s="18" t="str">
-        <f t="shared" ca="1" si="37"/>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="L48" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>0.90239999999999998</v>
+        <v>0.67679999999999996</v>
       </c>
       <c r="M48" s="13">
-        <f t="shared" ref="M48" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>17.48</v>
       </c>
       <c r="N48" s="13" t="str">
@@ -14272,11 +14446,11 @@
       </c>
       <c r="Q48" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="R48" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="S48" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14291,23 +14465,23 @@
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC48" s="42">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="3:29">
       <c r="C49" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>64c416m8g</v>
+        <v>32c208m4g</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F49" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>8.4930000000000003</v>
+        <v>4.3029999999999999</v>
       </c>
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
@@ -14317,16 +14491,16 @@
         <v>0</v>
       </c>
       <c r="K49" s="18" t="str">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="37"/>
         <v>USD</v>
       </c>
       <c r="L49" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>1.8048</v>
+        <v>0.90239999999999998</v>
       </c>
       <c r="M49" s="13">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
-        <v>34.96</v>
+        <f t="shared" ref="M49" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>17.48</v>
       </c>
       <c r="N49" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14334,15 +14508,15 @@
       </c>
       <c r="O49" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q49" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="R49" s="13">
         <f t="shared" ca="1" si="35"/>
-        <v>416</v>
+        <v>208</v>
       </c>
       <c r="S49" s="13" t="str">
         <f t="shared" ca="1" si="35"/>
@@ -14357,190 +14531,266 @@
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC49" s="42">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="3:29">
-      <c r="F50" s="18"/>
+      <c r="C50" s="21" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>64c416m8g</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="F50" s="18">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>8.4930000000000003</v>
+      </c>
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
       <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
+      <c r="J50" s="18">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K50" s="18" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>USD</v>
+      </c>
+      <c r="L50" s="13">
+        <f t="shared" ca="1" si="26"/>
+        <v>1.8048</v>
+      </c>
+      <c r="M50" s="13">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>34.96</v>
+      </c>
+      <c r="N50" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>K80</v>
+      </c>
+      <c r="O50" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="Q50" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>64</v>
+      </c>
+      <c r="R50" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>416</v>
+      </c>
+      <c r="S50" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>SSD</v>
+      </c>
+      <c r="T50" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>375</v>
+      </c>
+      <c r="Y50" s="15" t="str">
+        <f t="shared" ca="1" si="40"/>
+        <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
+      </c>
+      <c r="AC50" s="42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="3:29">
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="D3:D8 E7:G7 E3:I6 E8:H8 L38:V38 W38:Y41 L34:Y37 I27 E29:G30 I29:I30 K39:T44 E9:I14 T4:X11 S4:S14 E17:F17 H17:I17 E26:E28 H24:I26 E22:E23 F22:G27 D22:D30 H20:H24 D10:D14 E18:I20 W12:X14 T18:V24 T25:X32 Y6:Y14 P18:S33 T33 C3:C14 J3:R14 C17:C33 Y17:Y33 L17:O33 W17:X24 D17:D20 I34:I44 K17:K38 J17:J44">
+  <conditionalFormatting sqref="D3:D8 E7:G7 E3:I6 E8:H8 L39:V39 W39:Y42 L35:Y38 I27 E29:G30 I29:I30 K40:T45 E9:I14 T4:X11 S4:S14 E17:F17 H17:I17 E26:E28 H24:I26 E22:E23 F22:G27 D22:D30 H20:H24 D10:D14 E18:I20 W12:X14 T18:V24 T25:X32 Y6:Y14 P18:S33 T33 C3:C14 J3:R14 L17:O33 W17:X24 D17:D20 I35:I45 J17:J45 C17:C34 K17:K39 Y17:Y34 L34:T34">
+    <cfRule type="expression" dxfId="35" priority="138">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21 I21 F21">
+    <cfRule type="expression" dxfId="34" priority="136">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
     <cfRule type="expression" dxfId="33" priority="135">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21 I21 F21">
-    <cfRule type="expression" dxfId="32" priority="133">
+  <conditionalFormatting sqref="I23">
+    <cfRule type="expression" dxfId="32" priority="134">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="31" priority="132">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="30" priority="131">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:X3 T12:V14 U33:X33">
-    <cfRule type="expression" dxfId="29" priority="75">
+  <conditionalFormatting sqref="S3:X3 T12:V14 U33:X34">
+    <cfRule type="expression" dxfId="31" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="expression" dxfId="28" priority="63">
+    <cfRule type="expression" dxfId="30" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17:V17 R17">
-    <cfRule type="expression" dxfId="27" priority="61">
+    <cfRule type="expression" dxfId="29" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="expression" dxfId="26" priority="62">
+    <cfRule type="expression" dxfId="28" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17">
-    <cfRule type="expression" dxfId="25" priority="60">
+    <cfRule type="expression" dxfId="27" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="24" priority="57">
+    <cfRule type="expression" dxfId="26" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="23" priority="51">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="22" priority="42">
+    <cfRule type="expression" dxfId="24" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="21" priority="41">
+    <cfRule type="expression" dxfId="23" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:H30">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45:O46">
-    <cfRule type="expression" dxfId="15" priority="16">
+  <conditionalFormatting sqref="F46:O47">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:O48">
+  <conditionalFormatting sqref="F48:O49">
+    <cfRule type="expression" dxfId="16" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50:O51">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T46:T49 R46:R49">
     <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49:O50">
-    <cfRule type="expression" dxfId="13" priority="14">
+  <conditionalFormatting sqref="Q46:Q49">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T45:T48 R45:R48">
-    <cfRule type="expression" dxfId="12" priority="12">
+  <conditionalFormatting sqref="S46:S49">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q45:Q48">
-    <cfRule type="expression" dxfId="11" priority="13">
+  <conditionalFormatting sqref="T50 R50">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S45:S48">
-    <cfRule type="expression" dxfId="10" priority="11">
+  <conditionalFormatting sqref="Q50">
+    <cfRule type="expression" dxfId="10" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T49 R49">
-    <cfRule type="expression" dxfId="9" priority="9">
+  <conditionalFormatting sqref="S50">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q49">
+  <conditionalFormatting sqref="Y46:Y50">
     <cfRule type="expression" dxfId="8" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S49">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y45:Y49">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G33">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H33">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:S16 W15:Y16">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15:V16">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G34">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added K CPU performance and cost.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="325">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1936,6 +1936,35 @@
   </si>
   <si>
     <t>LT GTXTitanx2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K computer</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.aics.riken.jp/jp/k/system.html</t>
+  </si>
+  <si>
+    <t>SPARC64TM VIIIfx</t>
+  </si>
+  <si>
+    <t>K (1node)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JPY</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K 1node</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.hpci-office.jp/pages/shinsei_hpci_fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2305,7 +2334,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="803">
+  <cellStyleXfs count="815">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3032,6 +3061,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3233,7 +3274,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="803">
+  <cellStyles count="815">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3700,6 +3741,12 @@
     <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="814" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -4027,6 +4074,12 @@
     <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -4038,7 +4091,29 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4754,6 +4829,17 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -5049,13 +5135,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FG62"/>
+  <dimension ref="A1:FG66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="N25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Y43" sqref="Y43"/>
+      <selection pane="bottomRight" activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9997,6 +10083,50 @@
         <v>267</v>
       </c>
     </row>
+    <row r="65" spans="1:32" ht="20">
+      <c r="A65" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="K65" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="L65">
+        <v>8</v>
+      </c>
+      <c r="M65">
+        <v>8</v>
+      </c>
+      <c r="N65" s="12">
+        <v>2</v>
+      </c>
+      <c r="O65" s="12">
+        <v>8</v>
+      </c>
+      <c r="P65" s="12">
+        <v>8</v>
+      </c>
+      <c r="Q65" s="13">
+        <f t="shared" ref="Q65" si="18">M65*N65*P65/1000</f>
+        <v>0.128</v>
+      </c>
+      <c r="S65">
+        <v>16</v>
+      </c>
+      <c r="AA65">
+        <v>14.53</v>
+      </c>
+      <c r="AF65" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="66" spans="1:32">
+      <c r="A66" s="15" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C3:I3"/>
@@ -10007,7 +10137,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AI37">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10019,7 +10149,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ37">
-    <cfRule type="colorScale" priority="86">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10031,7 +10161,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="82">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10043,7 +10173,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="81">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10055,7 +10185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI38:AI39">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10067,7 +10197,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ38:AJ39">
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10079,32 +10209,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 AA39 A17 B18:I18 T21:W21 AA18:AE22 A12:AE12 A5:M8 A36:AE36 A38:M38 N38:O39 AI36:XFD38 AI19:AK20 AI39:AK39 AI21:XFD34 AH36:AH39 AH18:AH24 AI5:XFD18 R38:Y38 AD38:AE38 AC39 A13:AB13 R33:Y33 AA33:AE34 A37:O37 AA37:AE37 AA38:AB38 AH6:AH16 A10:C11 Z45:Z48 AF45:AG47 AF48 AH27:AH34 A23:AE25 A30:B32 J30:O32 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 Q37:Y37 Q37:Q39 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11 AF6:AG40 A21:J21 A22:W22 Q41:Q43 Q45:Q56">
-    <cfRule type="expression" dxfId="64" priority="73">
+    <cfRule type="expression" dxfId="67" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC13">
-    <cfRule type="expression" dxfId="63" priority="60">
+    <cfRule type="expression" dxfId="66" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="62" priority="59">
+    <cfRule type="expression" dxfId="65" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:M39 R39:Y39">
-    <cfRule type="expression" dxfId="61" priority="58">
+    <cfRule type="expression" dxfId="64" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC38">
-    <cfRule type="expression" dxfId="60" priority="57">
+    <cfRule type="expression" dxfId="63" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI39 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10116,7 +10246,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ39 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="162">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10128,7 +10258,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI36:AI37 AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="166">
+    <cfRule type="colorScale" priority="167">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10140,7 +10270,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ36:AJ37 AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="170">
+    <cfRule type="colorScale" priority="171">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10152,7 +10282,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK36:AK39 AK21:AK34 AK5:AK18">
-    <cfRule type="colorScale" priority="174">
+    <cfRule type="colorScale" priority="175">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10164,7 +10294,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI21:AI34 AI5:AI18">
-    <cfRule type="colorScale" priority="178">
+    <cfRule type="colorScale" priority="179">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10176,7 +10306,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ21:AJ34 AJ5:AJ18">
-    <cfRule type="colorScale" priority="181">
+    <cfRule type="colorScale" priority="182">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10188,12 +10318,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20 T20:W20">
-    <cfRule type="expression" dxfId="59" priority="49">
+    <cfRule type="expression" dxfId="62" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10205,7 +10335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10217,7 +10347,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10229,7 +10359,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="53">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10241,7 +10371,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10253,7 +10383,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI20">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10265,7 +10395,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ20">
-    <cfRule type="colorScale" priority="56">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10277,17 +10407,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="58" priority="40">
+    <cfRule type="expression" dxfId="61" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 S20:S21 S19:W19">
-    <cfRule type="expression" dxfId="57" priority="41">
+    <cfRule type="expression" dxfId="60" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10299,7 +10429,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10311,7 +10441,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10323,7 +10453,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10335,7 +10465,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK19">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10347,7 +10477,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI19">
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10359,7 +10489,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -10371,107 +10501,112 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z22">
-    <cfRule type="expression" dxfId="56" priority="38">
+    <cfRule type="expression" dxfId="59" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="expression" dxfId="55" priority="37">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z37:Z39">
-    <cfRule type="expression" dxfId="54" priority="36">
+    <cfRule type="expression" dxfId="57" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z41:Z44">
-    <cfRule type="expression" dxfId="53" priority="35">
+    <cfRule type="expression" dxfId="56" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50:O50 N51:O56">
-    <cfRule type="expression" dxfId="52" priority="24">
+    <cfRule type="expression" dxfId="55" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R50:R56">
-    <cfRule type="expression" dxfId="51" priority="23">
+    <cfRule type="expression" dxfId="54" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z53">
-    <cfRule type="expression" dxfId="50" priority="22">
+    <cfRule type="expression" dxfId="53" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:I53">
-    <cfRule type="expression" dxfId="49" priority="21">
+    <cfRule type="expression" dxfId="52" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG48">
-    <cfRule type="expression" dxfId="48" priority="16">
+    <cfRule type="expression" dxfId="51" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I32">
-    <cfRule type="expression" dxfId="47" priority="15">
+    <cfRule type="expression" dxfId="50" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:I56">
-    <cfRule type="expression" dxfId="46" priority="14">
+    <cfRule type="expression" dxfId="49" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q21">
-    <cfRule type="expression" dxfId="45" priority="13">
+    <cfRule type="expression" dxfId="48" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="44" priority="12">
+    <cfRule type="expression" dxfId="47" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K21">
-    <cfRule type="expression" dxfId="43" priority="11">
+    <cfRule type="expression" dxfId="46" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:P39">
-    <cfRule type="expression" dxfId="42" priority="10">
+    <cfRule type="expression" dxfId="45" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P45">
-    <cfRule type="expression" dxfId="41" priority="7">
+    <cfRule type="expression" dxfId="44" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P46:P48">
-    <cfRule type="expression" dxfId="40" priority="6">
+    <cfRule type="expression" dxfId="43" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P50:P53">
-    <cfRule type="expression" dxfId="39" priority="5">
+    <cfRule type="expression" dxfId="42" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54:P56">
-    <cfRule type="expression" dxfId="38" priority="4">
+    <cfRule type="expression" dxfId="41" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:I62">
-    <cfRule type="expression" dxfId="37" priority="2">
+    <cfRule type="expression" dxfId="40" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="expression" dxfId="36" priority="1">
+    <cfRule type="expression" dxfId="39" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q65">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10494,11 +10629,11 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC51"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="M23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomRight" activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -13086,7 +13221,7 @@
         <v>EUR</v>
       </c>
       <c r="L31" s="13">
-        <f t="shared" ref="L31:L50" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L31:L51" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.87039999999999995</v>
       </c>
       <c r="M31" s="13">
@@ -13404,7 +13539,7 @@
         <v>230</v>
       </c>
       <c r="C35" s="21" t="str">
-        <f t="shared" ref="C35:C50" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C35:C51" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D35" s="15" t="s">
@@ -13783,7 +13918,7 @@
         <v>4.37</v>
       </c>
       <c r="N39" s="13" t="str">
-        <f t="shared" ref="N39:V50" ca="1" si="35">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N39:V51" ca="1" si="35">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="O39" s="13">
@@ -13923,7 +14058,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="18">
-        <f t="shared" ref="J41:K50" ca="1" si="37">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="J41:K51" ca="1" si="37">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K41" s="18" t="str">
@@ -14282,7 +14417,7 @@
         <v>271</v>
       </c>
       <c r="F46" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="F46:F51" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>1.073</v>
       </c>
       <c r="G46" s="18"/>
@@ -14329,7 +14464,7 @@
         <v>375</v>
       </c>
       <c r="Y46" s="15" t="str">
-        <f t="shared" ref="Y46:Y50" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="Y46:Y51" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC46" s="42">
@@ -14348,7 +14483,7 @@
         <v>272</v>
       </c>
       <c r="F47" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="40"/>
         <v>2.0339999999999998</v>
       </c>
       <c r="G47" s="18"/>
@@ -14367,7 +14502,7 @@
         <v>0.33839999999999998</v>
       </c>
       <c r="M47" s="13">
-        <f t="shared" ref="M47" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M47" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>8.74</v>
       </c>
       <c r="N47" s="13" t="str">
@@ -14395,7 +14530,7 @@
         <v>375</v>
       </c>
       <c r="Y47" s="15" t="str">
-        <f t="shared" ca="1" si="40"/>
+        <f t="shared" ca="1" si="41"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC47" s="42">
@@ -14414,7 +14549,7 @@
         <v>273</v>
       </c>
       <c r="F48" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="40"/>
         <v>3.9550000000000001</v>
       </c>
       <c r="G48" s="18"/>
@@ -14461,14 +14596,14 @@
         <v>375</v>
       </c>
       <c r="Y48" s="15" t="str">
-        <f t="shared" ca="1" si="40"/>
+        <f t="shared" ca="1" si="41"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC48" s="42">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="3:29">
+    <row r="49" spans="1:29">
       <c r="C49" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>32c208m4g</v>
@@ -14480,7 +14615,7 @@
         <v>274</v>
       </c>
       <c r="F49" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="40"/>
         <v>4.3029999999999999</v>
       </c>
       <c r="G49" s="18"/>
@@ -14499,7 +14634,7 @@
         <v>0.90239999999999998</v>
       </c>
       <c r="M49" s="13">
-        <f t="shared" ref="M49" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M49" ca="1" si="43">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>17.48</v>
       </c>
       <c r="N49" s="13" t="str">
@@ -14527,14 +14662,14 @@
         <v>375</v>
       </c>
       <c r="Y49" s="15" t="str">
-        <f t="shared" ca="1" si="40"/>
+        <f t="shared" ca="1" si="41"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC49" s="42">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="3:29">
+    <row r="50" spans="1:29">
       <c r="C50" s="21" t="str">
         <f t="shared" ca="1" si="31"/>
         <v>64c416m8g</v>
@@ -14546,7 +14681,7 @@
         <v>275</v>
       </c>
       <c r="F50" s="18">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="40"/>
         <v>8.4930000000000003</v>
       </c>
       <c r="G50" s="18"/>
@@ -14593,204 +14728,274 @@
         <v>375</v>
       </c>
       <c r="Y50" s="15" t="str">
-        <f t="shared" ca="1" si="40"/>
+        <f t="shared" ca="1" si="41"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC50" s="42">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="3:29">
-      <c r="F51" s="18"/>
+    <row r="51" spans="1:29" ht="20">
+      <c r="A51" s="55" t="str">
+        <f t="shared" ref="A51" ca="1" si="44">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>K computer</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C51" s="21" t="str">
+        <f t="shared" ca="1" si="31"/>
+        <v>K (1node)</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F51" s="18">
+        <f t="shared" ca="1" si="40"/>
+        <v>14.53</v>
+      </c>
       <c r="G51" s="18"/>
       <c r="H51" s="18"/>
       <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
+      <c r="J51" s="18">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="K51" s="18" t="str">
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>JPY</v>
+      </c>
+      <c r="L51" s="13">
+        <f t="shared" ca="1" si="26"/>
+        <v>1.024</v>
+      </c>
+      <c r="M51" s="13">
+        <v>0</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="O51" s="13">
+        <v>0</v>
+      </c>
+      <c r="P51" s="13" t="str">
+        <f t="shared" ca="1" si="35"/>
+        <v>SPARC64TM VIIIfx</v>
+      </c>
+      <c r="Q51" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>8</v>
+      </c>
+      <c r="R51" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>16</v>
+      </c>
+      <c r="S51" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="13">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="U51" s="12"/>
+      <c r="V51" s="12"/>
+      <c r="W51" s="12"/>
+      <c r="Y51" s="15">
+        <f t="shared" ca="1" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AC51" s="42">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D3:D8 E7:G7 E3:I6 E8:H8 L39:V39 W39:Y42 L35:Y38 I27 E29:G30 I29:I30 K40:T45 E9:I14 T4:X11 S4:S14 E17:F17 H17:I17 E26:E28 H24:I26 E22:E23 F22:G27 D22:D30 H20:H24 D10:D14 E18:I20 W12:X14 T18:V24 T25:X32 Y6:Y14 P18:S33 T33 C3:C14 J3:R14 L17:O33 W17:X24 D17:D20 I35:I45 J17:J45 C17:C34 K17:K39 Y17:Y34 L34:T34">
-    <cfRule type="expression" dxfId="35" priority="138">
+    <cfRule type="expression" dxfId="37" priority="139">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21 I21 F21">
-    <cfRule type="expression" dxfId="34" priority="136">
+    <cfRule type="expression" dxfId="36" priority="137">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="33" priority="135">
+    <cfRule type="expression" dxfId="35" priority="136">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="expression" dxfId="32" priority="134">
+    <cfRule type="expression" dxfId="34" priority="135">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:X3 T12:V14 U33:X34">
-    <cfRule type="expression" dxfId="31" priority="78">
+    <cfRule type="expression" dxfId="33" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
+    <cfRule type="expression" dxfId="32" priority="67">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17:V17 R17">
+    <cfRule type="expression" dxfId="31" priority="65">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
     <cfRule type="expression" dxfId="30" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T17:V17 R17">
+  <conditionalFormatting sqref="S17">
     <cfRule type="expression" dxfId="29" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
-    <cfRule type="expression" dxfId="28" priority="65">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="expression" dxfId="27" priority="63">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="26" priority="60">
+    <cfRule type="expression" dxfId="28" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="25" priority="54">
+    <cfRule type="expression" dxfId="27" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="24" priority="45">
+    <cfRule type="expression" dxfId="26" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="23" priority="44">
+    <cfRule type="expression" dxfId="25" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="22" priority="24">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28:H30">
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="expression" dxfId="20" priority="22">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:O47">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48:O49">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50:O51">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T46:T49 R46:R49">
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q46:Q49">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T46:T49 R46:R49">
+  <conditionalFormatting sqref="S46:S49">
     <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q46:Q49">
-    <cfRule type="expression" dxfId="13" priority="16">
+  <conditionalFormatting sqref="T50:T51 R50:R51">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S46:S49">
+  <conditionalFormatting sqref="Q50:Q51">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T50 R50">
+  <conditionalFormatting sqref="S50:S51">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q50">
-    <cfRule type="expression" dxfId="10" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S50">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y46:Y50">
-    <cfRule type="expression" dxfId="8" priority="10">
+  <conditionalFormatting sqref="Y46:Y51">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G33">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H33">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:S16 W15:Y16">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15:V16">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P51">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Quardo P600 -> P6000
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="326">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -925,10 +925,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>http://www.cirrascale.com/cloud/plans.aspx</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>https://www.sakura.ad.jp/koukaryoku/specification/</t>
   </si>
   <si>
@@ -1501,10 +1497,6 @@
   </si>
   <si>
     <t>4-GPU x86 Quadro P6000</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Quadro P600</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1799,176 +1791,188 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>CR P100x4 P8/10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 P8/8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x2 P8/8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK P40x1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK P100x1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">LT GTX1080x8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT GTX1080x4 ltd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NM P100 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">NM K80x4 </t>
+  </si>
+  <si>
+    <t>AZ p2 dedicated y.0Up</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AZ p2 dedicated</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NM M40x4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NM P100x4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Provider web site states 128 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU. </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x GeForce GTX 1080 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Hourly plan charged minutely. Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Limited offer till the end of April 2017. Hourly plan charged minutely. Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8 x GeForce GTX 1080 min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x GeForce GTX 1080 ltd. min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.leadergpu.com</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 240</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 240</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GTX Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x Titan X min.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Quad GPU Pascal</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GTX Titan X</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SK TitanX x4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTXTitanX x2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Reedbush-H (educational)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MS NC24r</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Quad GPU Maxwell </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Quad GPU Pascal </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Tesla P40 model </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Tesla P100 model </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SK TitanX x4 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SK P40x1 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SK P100x1 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SK GTXTitanX x4 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cirrascale.com/cloud/plans.aspx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Quadro P6000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>CR P6000x4 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 P8/10</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x4 P8/8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x2 P8/8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SK P40x1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SK P100x1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">LT GTX1080x8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT GTX1080x4 ltd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NM P100 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">NM K80x4 </t>
-  </si>
-  <si>
-    <t>AZ p2 dedicated y.0Up</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>AZ p2 dedicated</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NM M40x4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NM P100x4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Provider web site states 128 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU. </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x GeForce GTX 1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Hourly plan charged minutely. Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Limited offer till the end of April 2017. Hourly plan charged minutely. Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8 x GeForce GTX 1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4 x GeForce GTX 1080 ltd. min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.leadergpu.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 240</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 240</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GTX Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SSD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x Titan X min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Quad GPU Pascal</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GTX Titan X</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SK TitanX x4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTXTitanX x2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.cc.u-tokyo.ac.jp/support/application/kitei/hyou5.pdf</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Reedbush-H (educational)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TU edu</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>MS NC24r</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Quad GPU Maxwell </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Quad GPU Pascal </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Tesla P40 model </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Tesla P100 model </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SK TitanX x4 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SK P40x1 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SK P100x1 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SK GTXTitanX x4 </t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2338,7 +2342,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="823">
+  <cellStyleXfs count="825">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3173,6 +3177,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="59">
@@ -3286,7 +3292,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="823">
+  <cellStyles count="825">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3765,6 +3771,7 @@
     <cellStyle name="Followed Hyperlink" xfId="820" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="821" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="824" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -4100,6 +4107,7 @@
     <cellStyle name="Hyperlink" xfId="813" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="815" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="823" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -4111,7 +4119,29 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4993,10 +5023,10 @@
   <dimension ref="A1:FG66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5093,7 +5123,7 @@
       <c r="AE3" s="58"/>
       <c r="AF3" s="58"/>
       <c r="AG3" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AH3" s="1" t="s">
         <v>32</v>
@@ -5253,7 +5283,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>4</v>
@@ -5265,16 +5295,16 @@
         <v>6</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P4" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>226</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>228</v>
       </c>
       <c r="R4" s="16" t="s">
         <v>10</v>
@@ -5295,31 +5325,31 @@
         <v>9</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y4" s="16" t="s">
         <v>13</v>
       </c>
       <c r="Z4" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AA4" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB4" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="AB4" s="16" t="s">
+      <c r="AC4" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="AC4" s="16" t="s">
+      <c r="AD4" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="AD4" s="16" t="s">
-        <v>171</v>
-      </c>
       <c r="AE4" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF4" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AH4" s="16"/>
     </row>
@@ -5346,14 +5376,14 @@
         <v>2.91</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L5" s="13">
         <f>1/36*64</f>
@@ -5394,16 +5424,16 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG5" s="15"/>
       <c r="AH5" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:163">
       <c r="A6" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>45</v>
@@ -5472,16 +5502,16 @@
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
       <c r="AF6" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG6" s="15"/>
       <c r="AH6" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:163">
       <c r="A7" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>46</v>
@@ -5550,19 +5580,19 @@
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
       <c r="AF7" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG7" s="15"/>
       <c r="AH7" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:163">
       <c r="A8" s="15" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>23</v>
@@ -5625,16 +5655,16 @@
       <c r="AD8" s="10"/>
       <c r="AE8" s="10"/>
       <c r="AF8" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG8" s="15"/>
     </row>
     <row r="9" spans="1:163">
       <c r="A9" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>16</v>
@@ -5697,17 +5727,17 @@
       <c r="AD9" s="23"/>
       <c r="AE9" s="23"/>
       <c r="AF9" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG9" s="15"/>
       <c r="AH9" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:163">
       <c r="A10" s="15"/>
       <c r="B10" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>16</v>
@@ -5716,7 +5746,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -5725,10 +5755,10 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="5" t="s">
@@ -5769,14 +5799,14 @@
         <v>88389</v>
       </c>
       <c r="AF10" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG10" s="15"/>
     </row>
     <row r="11" spans="1:163">
       <c r="A11" s="15"/>
       <c r="B11" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>16</v>
@@ -5785,7 +5815,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -5794,10 +5824,10 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="5" t="s">
@@ -5838,7 +5868,7 @@
         <v>184780</v>
       </c>
       <c r="AF11" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG11" s="15"/>
     </row>
@@ -5881,7 +5911,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>28</v>
@@ -5963,19 +5993,19 @@
       <c r="AD13" s="10"/>
       <c r="AE13" s="10"/>
       <c r="AF13" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG13" s="15"/>
       <c r="AH13" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:163">
       <c r="A14" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>50</v>
@@ -6054,26 +6084,26 @@
       <c r="AD14" s="23"/>
       <c r="AE14" s="23"/>
       <c r="AF14" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG14" s="15"/>
       <c r="AH14" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:163">
       <c r="A15" s="15"/>
       <c r="B15" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" s="9">
         <v>9.65</v>
@@ -6082,14 +6112,14 @@
         <v>0.3</v>
       </c>
       <c r="H15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L15" s="5">
         <v>2</v>
@@ -6117,7 +6147,7 @@
         <v>64</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U15" s="5">
         <v>1000</v>
@@ -6143,11 +6173,11 @@
       <c r="AD15" s="23"/>
       <c r="AE15" s="23"/>
       <c r="AF15" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG15" s="15"/>
       <c r="AH15" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:163">
@@ -6189,10 +6219,10 @@
         <v>41</v>
       </c>
       <c r="B17" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>119</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>120</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
@@ -6266,7 +6296,7 @@
       <c r="AD17" s="35"/>
       <c r="AE17" s="35"/>
       <c r="AF17" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG17" s="15"/>
       <c r="AH17" s="15" t="s">
@@ -6275,7 +6305,7 @@
     </row>
     <row r="18" spans="1:163" s="12" customFormat="1">
       <c r="A18" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>43</v>
@@ -6287,7 +6317,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="9">
         <v>8.74</v>
@@ -6296,7 +6326,7 @@
         <v>2.91</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>21</v>
@@ -6355,7 +6385,7 @@
       <c r="AD18" s="10"/>
       <c r="AE18" s="10"/>
       <c r="AF18" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG18" s="15"/>
       <c r="AH18" s="15" t="s">
@@ -6365,10 +6395,10 @@
     <row r="19" spans="1:163" s="12" customFormat="1" ht="20">
       <c r="A19" s="31"/>
       <c r="B19" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" s="5">
         <v>4</v>
@@ -6442,7 +6472,7 @@
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
       <c r="AF19" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG19" s="15"/>
       <c r="AH19" s="15" t="s">
@@ -6578,7 +6608,7 @@
     <row r="20" spans="1:163" s="12" customFormat="1" ht="20">
       <c r="A20" s="31"/>
       <c r="B20" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>34</v>
@@ -6652,7 +6682,7 @@
       <c r="AD20" s="23"/>
       <c r="AE20" s="23"/>
       <c r="AF20" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG20" s="15"/>
       <c r="AH20" s="15"/>
@@ -6785,10 +6815,10 @@
     </row>
     <row r="21" spans="1:163">
       <c r="A21" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>34</v>
@@ -6862,11 +6892,11 @@
       <c r="AD21" s="23"/>
       <c r="AE21" s="23"/>
       <c r="AF21" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG21" s="15"/>
       <c r="AH21" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:163">
@@ -6973,7 +7003,7 @@
         <v>42</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>16</v>
@@ -7053,19 +7083,19 @@
       <c r="AD25" s="23"/>
       <c r="AE25" s="23"/>
       <c r="AF25" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG25" s="15"/>
       <c r="AH25" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:163">
       <c r="A26" s="15" t="s">
-        <v>58</v>
+        <v>322</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>40</v>
@@ -7145,20 +7175,20 @@
       <c r="AD26" s="23"/>
       <c r="AE26" s="23"/>
       <c r="AF26" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG26" s="15"/>
       <c r="AH26" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:163" s="12" customFormat="1">
       <c r="A27" s="2"/>
       <c r="B27" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" s="12">
         <v>8</v>
@@ -7208,13 +7238,13 @@
         <v>256</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U27" s="13">
         <v>1000</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W27" s="13">
         <v>4000</v>
@@ -7235,7 +7265,7 @@
       <c r="AD27" s="23"/>
       <c r="AE27" s="23"/>
       <c r="AF27" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG27" s="15"/>
       <c r="AH27" s="15"/>
@@ -7243,10 +7273,10 @@
     <row r="28" spans="1:163" s="12" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D28" s="12">
         <v>8</v>
@@ -7268,7 +7298,7 @@
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L28" s="5">
         <v>2</v>
@@ -7296,13 +7326,13 @@
         <v>256</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U28" s="13">
         <v>1000</v>
       </c>
       <c r="V28" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W28" s="13">
         <v>4000</v>
@@ -7323,7 +7353,7 @@
       <c r="AD28" s="23"/>
       <c r="AE28" s="23"/>
       <c r="AF28" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG28" s="15"/>
       <c r="AH28" s="15"/>
@@ -7331,10 +7361,10 @@
     <row r="29" spans="1:163" s="12" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>207</v>
+        <v>323</v>
       </c>
       <c r="D29" s="12">
         <v>8</v>
@@ -7356,7 +7386,7 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -7384,13 +7414,13 @@
         <v>256</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U29" s="13">
         <v>1000</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W29" s="13">
         <v>4000</v>
@@ -7408,7 +7438,7 @@
       <c r="AD29" s="23"/>
       <c r="AE29" s="23"/>
       <c r="AF29" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG29" s="15"/>
       <c r="AH29" s="15"/>
@@ -7416,10 +7446,10 @@
     <row r="30" spans="1:163" s="12" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D30" s="12">
         <v>4</v>
@@ -7441,7 +7471,7 @@
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L30" s="5">
         <v>1</v>
@@ -7469,13 +7499,13 @@
         <v>128</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U30" s="13">
         <v>1000</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W30" s="13">
         <v>4000</v>
@@ -7493,7 +7523,7 @@
       <c r="AD30" s="23"/>
       <c r="AE30" s="23"/>
       <c r="AF30" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG30" s="15"/>
       <c r="AH30" s="15"/>
@@ -7501,7 +7531,7 @@
     <row r="31" spans="1:163" s="12" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>34</v>
@@ -7526,7 +7556,7 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L31" s="5">
         <v>1</v>
@@ -7554,13 +7584,13 @@
         <v>128</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U31" s="13">
         <v>1000</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W31" s="13">
         <v>4000</v>
@@ -7578,7 +7608,7 @@
       <c r="AD31" s="23"/>
       <c r="AE31" s="23"/>
       <c r="AF31" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG31" s="15"/>
       <c r="AH31" s="15"/>
@@ -7586,10 +7616,10 @@
     <row r="32" spans="1:163" s="12" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>207</v>
+        <v>324</v>
       </c>
       <c r="D32" s="12">
         <v>4</v>
@@ -7611,7 +7641,7 @@
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L32" s="5">
         <v>1</v>
@@ -7639,13 +7669,13 @@
         <v>128</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U32" s="13">
         <v>1000</v>
       </c>
       <c r="V32" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W32" s="13">
         <v>4000</v>
@@ -7663,17 +7693,17 @@
       <c r="AD32" s="23"/>
       <c r="AE32" s="23"/>
       <c r="AF32" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG32" s="15"/>
       <c r="AH32" s="15"/>
     </row>
     <row r="33" spans="1:163">
       <c r="B33" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -7725,10 +7755,10 @@
         <v>1000</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U33" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V33" s="13"/>
       <c r="W33" s="13"/>
@@ -7754,19 +7784,19 @@
       <c r="AD33" s="23"/>
       <c r="AE33" s="23"/>
       <c r="AF33" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG33" s="15"/>
       <c r="AH33" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:163">
       <c r="B34" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -7821,7 +7851,7 @@
         <v>31</v>
       </c>
       <c r="U34" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V34" s="13"/>
       <c r="W34" s="13"/>
@@ -7841,17 +7871,17 @@
       <c r="AD34" s="23"/>
       <c r="AE34" s="23"/>
       <c r="AF34" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG34" s="15"/>
     </row>
     <row r="35" spans="1:163" s="12" customFormat="1">
       <c r="A35" s="37"/>
       <c r="B35" s="38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D35" s="40">
         <v>2</v>
@@ -7926,7 +7956,7 @@
       <c r="AD35" s="41"/>
       <c r="AE35" s="41"/>
       <c r="AF35" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG35" s="15"/>
       <c r="AH35" s="15"/>
@@ -8088,7 +8118,7 @@
       <c r="AD36" s="23"/>
       <c r="AE36" s="23"/>
       <c r="AF36" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AG36" s="15"/>
     </row>
@@ -8097,10 +8127,10 @@
         <v>47</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D37" s="26">
         <v>4</v>
@@ -8179,19 +8209,19 @@
       <c r="AD37" s="23"/>
       <c r="AE37" s="49"/>
       <c r="AF37" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG37" s="15"/>
     </row>
     <row r="38" spans="1:163" s="12" customFormat="1">
       <c r="A38" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D38" s="26">
         <v>4</v>
@@ -8270,17 +8300,17 @@
       <c r="AD38" s="23"/>
       <c r="AE38" s="49"/>
       <c r="AF38" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG38" s="15"/>
       <c r="AH38" s="15"/>
     </row>
     <row r="39" spans="1:163" s="12" customFormat="1">
       <c r="B39" s="21" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="13">
         <v>1</v>
@@ -8330,7 +8360,7 @@
         <v>128</v>
       </c>
       <c r="T39" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U39" s="26">
         <v>480</v>
@@ -8359,17 +8389,17 @@
       <c r="AD39" s="23"/>
       <c r="AE39" s="49"/>
       <c r="AF39" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG39" s="15"/>
       <c r="AH39" s="15"/>
     </row>
     <row r="40" spans="1:163">
       <c r="B40" s="21" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D40" s="13">
         <v>1</v>
@@ -8446,16 +8476,16 @@
       <c r="AC40" s="49"/>
       <c r="AE40" s="49"/>
       <c r="AF40" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG40" s="15"/>
     </row>
     <row r="41" spans="1:163">
       <c r="B41" s="21" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D41" s="26">
         <v>4</v>
@@ -8536,17 +8566,17 @@
         <v>815000</v>
       </c>
       <c r="AF41" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG41" s="15"/>
     </row>
     <row r="42" spans="1:163" s="12" customFormat="1">
       <c r="A42" s="2"/>
       <c r="B42" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" s="13">
         <v>1</v>
@@ -8627,7 +8657,7 @@
         <v>875000</v>
       </c>
       <c r="AF42" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG42" s="15"/>
       <c r="AH42" s="15"/>
@@ -8635,7 +8665,7 @@
     <row r="43" spans="1:163" s="12" customFormat="1">
       <c r="A43" s="2"/>
       <c r="B43" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>34</v>
@@ -8717,7 +8747,7 @@
         <v>895000</v>
       </c>
       <c r="AF43" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG43" s="15"/>
       <c r="AH43" s="15"/>
@@ -8758,13 +8788,13 @@
     </row>
     <row r="45" spans="1:163" ht="23" customHeight="1">
       <c r="A45" s="20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D45" s="13">
         <v>2</v>
@@ -8786,7 +8816,7 @@
       </c>
       <c r="J45" s="26"/>
       <c r="K45" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L45" s="26">
         <v>2</v>
@@ -8814,7 +8844,7 @@
         <v>32</v>
       </c>
       <c r="T45" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U45" s="26">
         <v>480</v>
@@ -8843,22 +8873,22 @@
         <v>364.45</v>
       </c>
       <c r="AF45" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG45" s="15"/>
       <c r="AH45" s="15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:163" ht="24" customHeight="1">
       <c r="A46" s="15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D46" s="13">
         <v>4</v>
@@ -8880,7 +8910,7 @@
       </c>
       <c r="J46" s="26"/>
       <c r="K46" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L46" s="26">
         <v>2</v>
@@ -8908,7 +8938,7 @@
         <v>64</v>
       </c>
       <c r="T46" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U46" s="26">
         <v>480</v>
@@ -8937,19 +8967,19 @@
         <v>799</v>
       </c>
       <c r="AF46" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG46" s="15"/>
       <c r="AH46" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:163" ht="28" customHeight="1">
       <c r="B47" s="21" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" s="13">
         <v>8</v>
@@ -8971,7 +9001,7 @@
       </c>
       <c r="J47" s="26"/>
       <c r="K47" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L47" s="26">
         <v>2</v>
@@ -8999,7 +9029,7 @@
         <v>128</v>
       </c>
       <c r="T47" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U47" s="26">
         <v>960</v>
@@ -9028,19 +9058,19 @@
         <v>2017</v>
       </c>
       <c r="AF47" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AG47" s="15"/>
       <c r="AH47" s="15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48" spans="1:163">
       <c r="B48" s="21" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D48" s="13">
         <v>2</v>
@@ -9062,7 +9092,7 @@
       </c>
       <c r="J48" s="26"/>
       <c r="K48" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L48" s="26">
         <v>2</v>
@@ -9090,7 +9120,7 @@
         <v>32</v>
       </c>
       <c r="T48" s="26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="U48" s="26">
         <v>480</v>
@@ -9117,21 +9147,21 @@
         <v>799</v>
       </c>
       <c r="AF48" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AH48" s="15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="1:34" ht="20">
       <c r="A49" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="C49" s="26" t="s">
         <v>165</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>166</v>
       </c>
       <c r="D49" s="13">
         <v>2</v>
@@ -9155,7 +9185,7 @@
         <v>1</v>
       </c>
       <c r="K49" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L49" s="13">
         <v>2</v>
@@ -9183,7 +9213,7 @@
         <v>256</v>
       </c>
       <c r="T49" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U49" s="13">
         <v>1000</v>
@@ -9203,25 +9233,25 @@
         <v>138888.88888888888</v>
       </c>
       <c r="AF49" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG49" s="15">
         <f>17280/2.5</f>
         <v>6912</v>
       </c>
       <c r="AH49" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:34">
       <c r="A50" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D50" s="13">
         <v>2</v>
@@ -9245,7 +9275,7 @@
         <v>1</v>
       </c>
       <c r="K50" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L50" s="13">
         <v>2</v>
@@ -9273,7 +9303,7 @@
         <v>256</v>
       </c>
       <c r="T50" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U50" s="13">
         <v>4000</v>
@@ -9293,22 +9323,22 @@
         <v>277777.77777777775</v>
       </c>
       <c r="AF50" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG50" s="15">
         <f>34560/2.5</f>
         <v>13824</v>
       </c>
       <c r="AH50" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:34">
       <c r="B51" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D51" s="13">
         <v>2</v>
@@ -9332,7 +9362,7 @@
         <v>1</v>
       </c>
       <c r="K51" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L51" s="13">
         <v>2</v>
@@ -9360,7 +9390,7 @@
         <v>256</v>
       </c>
       <c r="T51" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U51" s="13">
         <v>4000</v>
@@ -9378,22 +9408,22 @@
         <v>166666.66666666666</v>
       </c>
       <c r="AF51" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG51" s="15">
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
       <c r="AH51" s="56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:34">
       <c r="B52" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D52" s="13">
         <v>2</v>
@@ -9417,7 +9447,7 @@
         <v>1</v>
       </c>
       <c r="K52" s="53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L52" s="13">
         <v>2</v>
@@ -9445,7 +9475,7 @@
         <v>256</v>
       </c>
       <c r="T52" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U52" s="13">
         <v>4000</v>
@@ -9463,14 +9493,14 @@
         <v>200000</v>
       </c>
       <c r="AF52" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG52" s="15">
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
       <c r="AH52" s="56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:34">
@@ -9479,13 +9509,13 @@
     </row>
     <row r="54" spans="1:34" ht="20">
       <c r="A54" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D54" s="13">
         <v>0.5</v>
@@ -9507,7 +9537,7 @@
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L54" s="13">
         <v>0.5</v>
@@ -9535,7 +9565,7 @@
         <v>56</v>
       </c>
       <c r="T54" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U54" s="13">
         <v>380</v>
@@ -9552,22 +9582,22 @@
       </c>
       <c r="AD54" s="54"/>
       <c r="AF54" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG54" s="15"/>
       <c r="AH54" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:34">
       <c r="A55" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D55" s="13">
         <v>1</v>
@@ -9589,7 +9619,7 @@
       </c>
       <c r="J55" s="13"/>
       <c r="K55" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L55" s="13">
         <v>1</v>
@@ -9617,7 +9647,7 @@
         <v>112</v>
       </c>
       <c r="T55" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U55" s="13">
         <v>680</v>
@@ -9634,19 +9664,19 @@
       </c>
       <c r="AD55" s="54"/>
       <c r="AF55" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG55" s="15"/>
     </row>
     <row r="56" spans="1:34">
       <c r="A56" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" s="13">
         <v>2</v>
@@ -9668,7 +9698,7 @@
       </c>
       <c r="J56" s="13"/>
       <c r="K56" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L56" s="13">
         <v>2</v>
@@ -9696,7 +9726,7 @@
         <v>224</v>
       </c>
       <c r="T56" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U56" s="13">
         <v>1440</v>
@@ -9713,16 +9743,16 @@
       </c>
       <c r="AD56" s="54"/>
       <c r="AF56" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG56" s="15"/>
     </row>
     <row r="57" spans="1:34">
       <c r="B57" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C57" s="26" t="s">
         <v>176</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>177</v>
       </c>
       <c r="D57" s="13">
         <v>2</v>
@@ -9744,7 +9774,7 @@
       </c>
       <c r="J57" s="13"/>
       <c r="K57" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L57" s="13">
         <v>2</v>
@@ -9772,13 +9802,13 @@
         <v>224</v>
       </c>
       <c r="T57" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U57" s="13">
         <v>1440</v>
       </c>
       <c r="X57" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Y57" s="13"/>
       <c r="Z57" s="13" t="str">
@@ -9794,25 +9824,25 @@
       </c>
       <c r="AD57" s="54"/>
       <c r="AF57" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG57" s="15"/>
       <c r="AH57" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:34">
       <c r="B58" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D58" s="13">
         <v>1</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F58" s="9">
         <v>9.65</v>
@@ -9821,13 +9851,13 @@
         <v>0.3</v>
       </c>
       <c r="H58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I58" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I58" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="K58" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L58" s="13">
         <v>0.5</v>
@@ -9855,7 +9885,7 @@
         <v>56</v>
       </c>
       <c r="T58" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U58">
         <v>340</v>
@@ -9864,21 +9894,21 @@
         <v>1.24</v>
       </c>
       <c r="AF58" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:34">
       <c r="B59" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>216</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>218</v>
       </c>
       <c r="D59" s="13">
         <v>2</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F59" s="9">
         <v>9.65</v>
@@ -9887,13 +9917,13 @@
         <v>0.3</v>
       </c>
       <c r="H59" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I59" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I59" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="K59" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L59" s="13">
         <v>1</v>
@@ -9921,7 +9951,7 @@
         <v>112</v>
       </c>
       <c r="T59" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U59">
         <v>680</v>
@@ -9930,21 +9960,21 @@
         <v>2.48</v>
       </c>
       <c r="AF59" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:34">
       <c r="B60" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D60" s="13">
         <v>4</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F60" s="9">
         <v>9.65</v>
@@ -9953,13 +9983,13 @@
         <v>0.3</v>
       </c>
       <c r="H60" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I60" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I60" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="K60" s="53" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L60" s="13">
         <v>2</v>
@@ -9987,7 +10017,7 @@
         <v>224</v>
       </c>
       <c r="T60" s="53" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U60">
         <v>1440</v>
@@ -9996,7 +10026,7 @@
         <v>4.97</v>
       </c>
       <c r="AF60" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:34">
@@ -10004,13 +10034,13 @@
     </row>
     <row r="62" spans="1:34" ht="20" customHeight="1">
       <c r="A62" s="20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C62" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D62" s="13">
         <v>0.5</v>
@@ -10046,7 +10076,7 @@
         <v>39</v>
       </c>
       <c r="T62" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U62">
         <v>375</v>
@@ -10055,21 +10085,21 @@
         <v>1.073</v>
       </c>
       <c r="AF62" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AH62" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:34" ht="20" customHeight="1">
       <c r="A63" s="15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C63" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D63" s="13">
         <v>1</v>
@@ -10106,7 +10136,7 @@
         <v>78</v>
       </c>
       <c r="T63" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U63" s="12">
         <v>375</v>
@@ -10118,21 +10148,21 @@
         <v>2.0339999999999998</v>
       </c>
       <c r="AF63" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AH63" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:34" ht="20" customHeight="1">
       <c r="A64" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C64" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="13">
         <v>2</v>
@@ -10169,7 +10199,7 @@
         <v>156</v>
       </c>
       <c r="T64" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U64" s="12">
         <v>375</v>
@@ -10181,18 +10211,18 @@
         <v>3.9550000000000001</v>
       </c>
       <c r="AF64" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AH64" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="2:34" ht="20" customHeight="1">
       <c r="B65" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="13">
         <v>2</v>
@@ -10229,7 +10259,7 @@
         <v>208</v>
       </c>
       <c r="T65" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U65" s="12">
         <v>375</v>
@@ -10241,18 +10271,18 @@
         <v>4.3029999999999999</v>
       </c>
       <c r="AF65" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AH65" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="2:34" ht="20" customHeight="1">
       <c r="B66" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C66" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D66" s="13">
         <v>4</v>
@@ -10289,7 +10319,7 @@
         <v>416</v>
       </c>
       <c r="T66" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U66" s="12">
         <v>375</v>
@@ -10301,10 +10331,10 @@
         <v>8.4930000000000003</v>
       </c>
       <c r="AF66" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AH66" s="57" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -10389,17 +10419,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH19:XFD20 FH35:XFD35 AA35 V34:Z35 U34 T34:T35 S34 R34:R35 A17 B18:I18 T21:W21 AA18:AE22 A12:AE12 A5:M8 A36:AE36 AI36:XFD40 AI19:AK20 AI41:AK44 AI21:XFD34 AH36:AH44 AH18:AH24 AI5:XFD18 AD39:AE39 A13:AB13 R33:Y33 AA33:AE34 AH6:AH16 A10:C11 Z49:Z52 AF49:AG51 AF52 AH27:AH34 A23:AE25 A30:B32 J30:O32 R10:AD11 Q8:AE8 R9:AE9 Q9:Q11 A14:AE16 S18:W18 A26:O29 P26:AE32 A33:K34 L33:Q35 B9:C9 D9:M11 R6:AE7 R5:AH5 Q5:Q7 N5:P11 A21:J21 A22:W22 Q49:Q60 D37:J37 AF6:AG36 A37:B37 AC44 AC40 Q44:Q47 AF44:AG44 AF39:AF40 B44 B40 K44:P44 R44:AA44 B39:J39 A38:J38 AG39:AG43 L37:AG37 L38:T40 V38:AG38 V39:AB39 V40:AA40 U38:U43">
-    <cfRule type="expression" dxfId="52" priority="76">
+    <cfRule type="expression" dxfId="54" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC13">
-    <cfRule type="expression" dxfId="51" priority="63">
+    <cfRule type="expression" dxfId="53" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC39">
-    <cfRule type="expression" dxfId="50" priority="60">
+    <cfRule type="expression" dxfId="52" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10488,7 +10518,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:J20 T20:W20">
-    <cfRule type="expression" dxfId="49" priority="52">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10577,12 +10607,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:I19">
-    <cfRule type="expression" dxfId="48" priority="43">
+    <cfRule type="expression" dxfId="50" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:D19 S20:S21 S19:W19">
-    <cfRule type="expression" dxfId="47" priority="44">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10671,112 +10701,112 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z22">
-    <cfRule type="expression" dxfId="46" priority="41">
+    <cfRule type="expression" dxfId="48" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33">
-    <cfRule type="expression" dxfId="45" priority="40">
+    <cfRule type="expression" dxfId="47" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:Z48">
-    <cfRule type="expression" dxfId="44" priority="38">
+    <cfRule type="expression" dxfId="46" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:O54 N55:O60">
-    <cfRule type="expression" dxfId="43" priority="27">
+    <cfRule type="expression" dxfId="45" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R54:R60">
-    <cfRule type="expression" dxfId="42" priority="26">
+    <cfRule type="expression" dxfId="44" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z57">
-    <cfRule type="expression" dxfId="41" priority="25">
+    <cfRule type="expression" dxfId="43" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:I57">
-    <cfRule type="expression" dxfId="40" priority="24">
+    <cfRule type="expression" dxfId="42" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG52">
-    <cfRule type="expression" dxfId="39" priority="19">
+    <cfRule type="expression" dxfId="41" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:I32">
-    <cfRule type="expression" dxfId="38" priority="18">
+    <cfRule type="expression" dxfId="40" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:I60">
-    <cfRule type="expression" dxfId="37" priority="17">
+    <cfRule type="expression" dxfId="39" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Q21">
-    <cfRule type="expression" dxfId="36" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="expression" dxfId="35" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:K21">
-    <cfRule type="expression" dxfId="34" priority="14">
+    <cfRule type="expression" dxfId="36" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P49">
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="35" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P50:P52">
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P54:P57">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="33" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P58:P60">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="32" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:I66">
-    <cfRule type="expression" dxfId="29" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q48">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:K43">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD42:AE42 AC43 AF42:AF43 B43 B41:J42 L41:T43 V42:AB42 V41:AF41 V43:AA43">
-    <cfRule type="expression" dxfId="26" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC42">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10800,10 +10830,10 @@
   <dimension ref="A1:AC54"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -10834,150 +10864,150 @@
   <sheetData>
     <row r="1" spans="1:29" s="46" customFormat="1">
       <c r="A1" s="45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="44"/>
       <c r="E1" s="44"/>
       <c r="F1" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="S1" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="G1" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="H1" s="45" t="s">
-        <v>233</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>231</v>
-      </c>
-      <c r="L1" s="45" t="s">
-        <v>229</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" s="45" t="s">
+      <c r="T1" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="U1" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="V1" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="W1" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="X1" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="V1" s="45" t="s">
+      <c r="Y1" s="45" t="s">
         <v>240</v>
-      </c>
-      <c r="W1" s="45" t="s">
-        <v>243</v>
-      </c>
-      <c r="X1" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y1" s="45" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="11" customFormat="1" ht="21" thickBot="1">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="P2" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="O2" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="27" t="s">
+      <c r="Q2" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="Q2" s="27" t="s">
+      <c r="R2" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="S2" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="T2" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="T2" s="27" t="s">
+      <c r="U2" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="W2" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="X2" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y2" s="28" t="s">
         <v>117</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="Y2" s="28" t="s">
-        <v>118</v>
       </c>
       <c r="Z2" s="12"/>
       <c r="AC2" s="12"/>
@@ -10996,10 +11026,10 @@
         <v>p2.16xlarge on-demand</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11084,10 +11114,10 @@
         <v>p2.8xlarge on-demand</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11172,10 +11202,10 @@
         <v>p2.xlarge on-demand</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11260,10 +11290,10 @@
         <v>p2 dedicated host On-demand</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F6" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11348,10 +11378,10 @@
         <v>p2 dedicated host 1 year no Upfront</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -11439,10 +11469,10 @@
         <v>p2 dedicated host 1 year 100% Upfront</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -11534,7 +11564,7 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="21" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F9" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11623,7 +11653,7 @@
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -11709,7 +11739,7 @@
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -11801,7 +11831,7 @@
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F12" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11888,7 +11918,7 @@
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F13" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -11975,7 +12005,7 @@
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F14" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -12059,7 +12089,7 @@
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" ref="F15:F16" ca="1" si="12">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -12143,7 +12173,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F16" s="18">
         <f t="shared" ca="1" si="12"/>
@@ -12233,7 +12263,7 @@
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18">
@@ -12323,7 +12353,7 @@
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18">
@@ -12413,7 +12443,7 @@
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="18">
@@ -12503,7 +12533,7 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F20" s="18"/>
       <c r="G20" s="18">
@@ -12593,7 +12623,7 @@
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="18">
@@ -12626,7 +12656,7 @@
       </c>
       <c r="N21" s="13" t="str">
         <f t="shared" ref="N21:R28" ca="1" si="19">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Quadro P600</v>
+        <v>Quadro P6000</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" ca="1" si="19"/>
@@ -12683,7 +12713,7 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F22" s="18"/>
       <c r="G22" s="18">
@@ -12773,7 +12803,7 @@
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F23" s="18"/>
       <c r="G23" s="18">
@@ -12869,7 +12899,7 @@
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18">
@@ -12902,7 +12932,7 @@
       </c>
       <c r="N24" s="13" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>Quadro P600</v>
+        <v>Quadro P6000</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" ca="1" si="19"/>
@@ -12957,7 +12987,7 @@
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F25" s="18"/>
       <c r="G25" s="18">
@@ -13045,7 +13075,7 @@
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18">
@@ -13133,7 +13163,7 @@
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="21" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18">
@@ -13229,7 +13259,7 @@
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F28" s="18">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -13320,7 +13350,7 @@
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" ref="F29:F44" ca="1" si="25">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -13411,7 +13441,7 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="21" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" ca="1" si="25"/>
@@ -13499,7 +13529,7 @@
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="21" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F31" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -13597,7 +13627,7 @@
         <v>Quad GPU Pascal</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F32" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -13686,7 +13716,7 @@
         <v>Tesla P40 model</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F33" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -13776,7 +13806,7 @@
       </c>
       <c r="D34" s="40"/>
       <c r="E34" s="21" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F34" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -13870,7 +13900,7 @@
       </c>
       <c r="D35" s="40"/>
       <c r="E35" s="21" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F35" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -13960,7 +13990,7 @@
         <v>4 x GeForce GTX 1080 ltd. min.</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F36" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14053,7 +14083,7 @@
         <v>8 x GeForce GTX 1080 min.</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F37" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14149,7 +14179,7 @@
         <v>2 x Titan X min.</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F38" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14241,17 +14271,17 @@
         <v>The University of Tokyo</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C39" s="21" t="str">
         <f t="shared" ca="1" si="30"/>
         <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F39" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14343,10 +14373,10 @@
         <v>Reedbush-H (educational)</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F40" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14442,10 +14472,10 @@
         <v>Reedbush-H reviewed (educational)</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F41" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14538,10 +14568,10 @@
         <v>Reedbush-H reviewed</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F42" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14633,7 +14663,7 @@
         <v>MS Azure</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C43" s="21" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -14641,7 +14671,7 @@
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F43" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14733,7 +14763,7 @@
         <v>NC12</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F44" s="13">
         <f t="shared" ca="1" si="25"/>
@@ -14825,7 +14855,7 @@
         <v>NC24</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F45" s="13">
         <f t="shared" ref="F45:F54" ca="1" si="37">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
@@ -14921,7 +14951,7 @@
         <v>NC24r</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F46" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15017,7 +15047,7 @@
         <v>NV6</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F47" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15113,7 +15143,7 @@
         <v>NV12</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F48" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15205,7 +15235,7 @@
         <v>NV24</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F49" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15297,17 +15327,17 @@
         <v>Google</v>
       </c>
       <c r="B50" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C50" s="21" t="str">
         <f t="shared" ca="1" si="30"/>
         <v>6c39m1g</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F50" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15399,10 +15429,10 @@
         <v>12c78m2g</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F51" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15494,10 +15524,10 @@
         <v>24c156m4g</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F52" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15589,10 +15619,10 @@
         <v>32c208m4g</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F53" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15684,10 +15714,10 @@
         <v>64c416m8g</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F54" s="13">
         <f t="shared" ca="1" si="37"/>
@@ -15776,127 +15806,132 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="D3:D8 E7:G7 E3:I6 E8:H14 T9:X9 E17:F17 H17 E22:E23 F22:G27 D22:D31 H20:H26 D10:D14 E18:H20 T18:V24 T25:X29 Y6:Y14 P18:S29 T34 C3:C14 L17:O29 X17:X24 D17:D20 Y17:Y35 J17:K34 L31:S34 T31:X33 L30:X30 C17:C35 E30:E31 E26:E28 Q48:T50 W36:Y54 X14 W14:W24 W10:X13 S9:S16 T10:V16 J3:R14 P48:P54 G28:G54 K50:O50 K35:T47 J35:J54 I39:I54">
-    <cfRule type="expression" dxfId="24" priority="142">
+    <cfRule type="expression" dxfId="26" priority="143">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21 F21">
-    <cfRule type="expression" dxfId="23" priority="140">
+    <cfRule type="expression" dxfId="25" priority="141">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U34:X34 W35:X35 U35:V54 S3:W8">
-    <cfRule type="expression" dxfId="22" priority="82">
+    <cfRule type="expression" dxfId="24" priority="83">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
+    <cfRule type="expression" dxfId="23" priority="71">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17:V17 R17">
+    <cfRule type="expression" dxfId="22" priority="69">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
     <cfRule type="expression" dxfId="21" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T17:V17 R17">
+  <conditionalFormatting sqref="S17">
     <cfRule type="expression" dxfId="20" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
-    <cfRule type="expression" dxfId="19" priority="69">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="expression" dxfId="18" priority="67">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="17" priority="64">
+    <cfRule type="expression" dxfId="19" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="16" priority="58">
+    <cfRule type="expression" dxfId="18" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I38">
-    <cfRule type="expression" dxfId="15" priority="49">
+    <cfRule type="expression" dxfId="17" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="14" priority="48">
+    <cfRule type="expression" dxfId="16" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27:H54">
-    <cfRule type="expression" dxfId="13" priority="28">
+    <cfRule type="expression" dxfId="15" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F54">
-    <cfRule type="expression" dxfId="12" priority="24">
+    <cfRule type="expression" dxfId="14" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:O49">
-    <cfRule type="expression" dxfId="11" priority="23">
+    <cfRule type="expression" dxfId="13" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:O54">
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="12" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T51:T54 R51:R54">
+    <cfRule type="expression" dxfId="11" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q51:Q54">
+    <cfRule type="expression" dxfId="10" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S51:S54">
     <cfRule type="expression" dxfId="9" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q51:Q54">
-    <cfRule type="expression" dxfId="8" priority="17">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S51:S54">
-    <cfRule type="expression" dxfId="7" priority="15">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="8" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:H16 X15:Y16 J15:R16">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:E34">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X8">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
LeaderTelecom limited price for 4xGTX1080
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1953,10 +1953,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>4 x GeForce GTX 1080 min.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>2 x P100 min.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1988,6 +1984,10 @@
   </si>
   <si>
     <t>AZ p2 dedicated 3y.100Up</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x GeForce GTX 1080 min. ltd.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -4158,7 +4158,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="54">
     <dxf>
       <font>
         <color auto="1"/>
@@ -4442,127 +4442,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5171,11 +5050,11 @@
   </sheetPr>
   <dimension ref="A1:FG67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomRight" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5955,7 +5834,7 @@
     <row r="11" spans="1:163" s="12" customFormat="1">
       <c r="A11" s="15"/>
       <c r="B11" s="21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>16</v>
@@ -9106,7 +8985,7 @@
         <v>296</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>144</v>
@@ -9178,21 +9057,21 @@
         <v>5/1</v>
       </c>
       <c r="AA47" s="48">
-        <f>0.04*60</f>
-        <v>2.4</v>
+        <f>0.03*60</f>
+        <v>1.7999999999999998</v>
       </c>
       <c r="AB47" s="48">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="AC47" s="48">
-        <v>1058.33</v>
+        <v>848.65</v>
       </c>
       <c r="AF47" s="15" t="s">
         <v>160</v>
       </c>
       <c r="AG47" s="15"/>
       <c r="AH47" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="48" spans="1:163" ht="28" customHeight="1">
@@ -9288,7 +9167,7 @@
     </row>
     <row r="49" spans="1:34">
       <c r="B49" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>165</v>
@@ -10642,17 +10521,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH20:XFD21 FH36:XFD36 AA36 V35:Z36 U35 T35:T36 S35 R35:R36 A18 B19:I19 T22:W22 AA19:AE23 A13:AE13 A5:M8 A37:AE37 AI37:XFD41 AI20:AK21 AI42:AK45 AI22:XFD35 AH37:AH45 AH19:AH25 AI5:XFD19 AD40:AE40 A14:AB14 R34:Y34 AA34:AE35 Z50:Z53 AF50:AG52 AF53 AH28:AH35 A24:AE26 A31:B33 J31:O33 Q8:AE8 R9:AE9 Q9:Q10 A15:AE17 S19:W19 A27:O30 P27:AE33 A34:K35 L34:Q36 B9:C9 D9:M10 R6:AE7 R5:AH5 Q5:Q7 N5:P10 A22:J22 A23:W23 Q50:Q61 D38:J38 A38:B38 AC45 AC41 Q45:Q48 AF45:AG45 AF40:AF41 B45 B41 K45:P45 R45:AA45 B40:J40 A39:J39 AG40:AG44 L38:AG38 L39:T41 V39:AG39 V40:AB40 V41:AA41 U39:U44 R10:AD12 A10:C10 AF6:AG37 AH6:AH17 A11:Q12">
-    <cfRule type="expression" dxfId="59" priority="77">
+    <cfRule type="expression" dxfId="53" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC14">
-    <cfRule type="expression" dxfId="58" priority="64">
+    <cfRule type="expression" dxfId="52" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC40">
-    <cfRule type="expression" dxfId="57" priority="61">
+    <cfRule type="expression" dxfId="51" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10741,7 +10620,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:J21 T21:W21">
-    <cfRule type="expression" dxfId="56" priority="53">
+    <cfRule type="expression" dxfId="50" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10830,12 +10709,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:I20">
-    <cfRule type="expression" dxfId="55" priority="44">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:D20 S21:S22 S20:W20">
-    <cfRule type="expression" dxfId="54" priority="45">
+    <cfRule type="expression" dxfId="48" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10924,112 +10803,112 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z18:Z23">
-    <cfRule type="expression" dxfId="53" priority="42">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="52" priority="41">
+    <cfRule type="expression" dxfId="46" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="51" priority="39">
+    <cfRule type="expression" dxfId="45" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M55:O55 N56:O61">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="44" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R55:R61">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="43" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z58">
-    <cfRule type="expression" dxfId="48" priority="26">
+    <cfRule type="expression" dxfId="42" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:I58">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG53">
-    <cfRule type="expression" dxfId="46" priority="20">
+    <cfRule type="expression" dxfId="40" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:I33">
-    <cfRule type="expression" dxfId="45" priority="19">
+    <cfRule type="expression" dxfId="39" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:I61">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="38" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18:Q22">
-    <cfRule type="expression" dxfId="43" priority="17">
+    <cfRule type="expression" dxfId="37" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="expression" dxfId="42" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K22">
-    <cfRule type="expression" dxfId="41" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P50">
-    <cfRule type="expression" dxfId="40" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P51:P53">
-    <cfRule type="expression" dxfId="39" priority="10">
+    <cfRule type="expression" dxfId="33" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P58">
-    <cfRule type="expression" dxfId="38" priority="9">
+    <cfRule type="expression" dxfId="32" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P59:P61">
-    <cfRule type="expression" dxfId="37" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:I67">
-    <cfRule type="expression" dxfId="36" priority="6">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K44">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD43:AE43 AC44 AF43:AF44 B44 B42:J43 L42:T44 V43:AB43 V42:AF42 V44:AA44">
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="28" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC43">
-    <cfRule type="expression" dxfId="33" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11052,8 +10931,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Y9" sqref="Y9"/>
@@ -11783,10 +11662,10 @@
         <v>p2 dedicated host 3 years no Upfront</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
@@ -11850,10 +11729,10 @@
         <v>p2 dedicated host 3 years  100% Upfront</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
@@ -14347,22 +14226,22 @@
       <c r="A38" s="55"/>
       <c r="C38" s="21" t="str">
         <f t="shared" ref="C38:C56" ca="1" si="31">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>4 x GeForce GTX 1080 min.</v>
+        <v>4 x GeForce GTX 1080 min. ltd.</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F38" s="13">
         <f t="shared" ca="1" si="26"/>
-        <v>2.4</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="G38" s="18">
         <f t="shared" ca="1" si="21"/>
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="H38" s="18">
         <f t="shared" ca="1" si="22"/>
-        <v>1058.33</v>
+        <v>848.65</v>
       </c>
       <c r="I38" s="18">
         <f t="shared" ca="1" si="8"/>
@@ -14539,7 +14418,7 @@
         <v>2 x P100 min.</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F40" s="13">
         <f t="shared" ca="1" si="26"/>
@@ -16166,132 +16045,132 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="E3:I6 T11:X11 E19:F19 H19 E24:E25 F24:G29 D24:D33 H22:H28 D12:D16 E20:H22 T20:V26 T27:X31 P20:S31 T36 L19:O31 X19:X26 D19:D22 Y19:Y37 J19:K36 L33:S36 T33:X35 L32:X32 C19:C37 E32:E33 E28:E30 Q50:T52 W38:Y56 X16 W16:W26 W12:X15 S11:S18 T12:V18 P50:P56 G30:G56 K52:O52 K37:T49 J37:J56 I41:I56 C11:C16 E11:H16 C3:D10 E7:G10 J3:R16 Y6:Y16">
-    <cfRule type="expression" dxfId="31" priority="143">
+    <cfRule type="expression" dxfId="25" priority="143">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 F23">
-    <cfRule type="expression" dxfId="30" priority="141">
+    <cfRule type="expression" dxfId="24" priority="141">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U36:X36 W37:X37 U37:V56 S3:W10">
-    <cfRule type="expression" dxfId="29" priority="83">
+    <cfRule type="expression" dxfId="23" priority="83">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19">
-    <cfRule type="expression" dxfId="28" priority="71">
+    <cfRule type="expression" dxfId="22" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T19:V19 R19">
-    <cfRule type="expression" dxfId="27" priority="69">
+    <cfRule type="expression" dxfId="21" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q19">
-    <cfRule type="expression" dxfId="26" priority="70">
+    <cfRule type="expression" dxfId="20" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19">
-    <cfRule type="expression" dxfId="25" priority="68">
+    <cfRule type="expression" dxfId="19" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="expression" dxfId="24" priority="65">
+    <cfRule type="expression" dxfId="18" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H10">
-    <cfRule type="expression" dxfId="23" priority="59">
+    <cfRule type="expression" dxfId="17" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I40">
-    <cfRule type="expression" dxfId="22" priority="50">
+    <cfRule type="expression" dxfId="16" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I10">
-    <cfRule type="expression" dxfId="21" priority="49">
+    <cfRule type="expression" dxfId="15" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H56">
-    <cfRule type="expression" dxfId="20" priority="29">
+    <cfRule type="expression" dxfId="14" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:F56">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="13" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:O51">
-    <cfRule type="expression" dxfId="18" priority="24">
+    <cfRule type="expression" dxfId="12" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:O56">
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="11" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T53:T56 R53:R56">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q53:Q56">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S53:S56">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="7" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:H18 X17:Y18 J17:R18">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E36">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:X10">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Tsubame2.5 offers. Continuous offers with time limit (nodes:hours limit) charged in periods equal to the time limit.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35760" windowHeight="18120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33560" windowHeight="14800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,12 +687,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="L85" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Peter Bryzgalov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="2"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+Limited to 4 cores</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="377">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -2021,44 +2047,148 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</t>
+  </si>
+  <si>
+    <t>2 x GeForce GTX 1080</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4 x GeForce GTX 1080 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>8 x GeForce GTX 1080</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb.</t>
+  </si>
+  <si>
+    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</t>
+  </si>
+  <si>
+    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,12 &amp;euro;/Gb.</t>
+  </si>
+  <si>
+    <t>Tsubame 2.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>G open</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S open</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S96</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S96 open</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>L256</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>L256 open</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K20</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon X5670</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;2 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;3 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;4 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;5 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;6 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;7 day.</t>
+  </si>
+  <si>
+    <t>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;8 day.</t>
+  </si>
+  <si>
+    <t>S1070</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4x98.5</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>4x4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon X7550</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://tsubame.gsic.titech.ac.jp/en/paid-services</t>
+  </si>
+  <si>
     <t>AJ</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</t>
-  </si>
-  <si>
-    <t>2 x GeForce GTX 1080</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4 x GeForce GTX 1080 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>8 x GeForce GTX 1080</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb.</t>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</t>
-  </si>
-  <si>
-    <t>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,12 &amp;euro;/Gb.</t>
+    <t>AK</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Continuous</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -2427,7 +2557,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="887">
+  <cellStyleXfs count="919">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3327,8 +3457,40 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -3439,10 +3601,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="263" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="887">
+  <cellStyles count="919">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -3953,6 +4121,22 @@
     <cellStyle name="Followed Hyperlink" xfId="882" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="884" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="918" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -4320,6 +4504,22 @@
     <cellStyle name="Hyperlink" xfId="881" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="883" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="917" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -4331,7 +4531,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="81">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5091,6 +5291,138 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -5386,13 +5718,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:FI76"/>
+  <dimension ref="A1:FJ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AC42" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="AC79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AJ45" sqref="AJ45"/>
+      <selection pane="bottomRight" activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5429,79 +5761,83 @@
     <col min="32" max="32" width="12.6640625" style="12" customWidth="1"/>
     <col min="33" max="33" width="14.1640625" style="12" customWidth="1"/>
     <col min="34" max="34" width="8.83203125" style="12" customWidth="1"/>
-    <col min="35" max="35" width="10.6640625" style="12" customWidth="1"/>
-    <col min="36" max="36" width="93.6640625" style="15" customWidth="1"/>
-    <col min="37" max="37" width="22.1640625" style="12" customWidth="1"/>
-    <col min="38" max="38" width="28.1640625" style="12" customWidth="1"/>
-    <col min="39" max="39" width="21.5" style="12" customWidth="1"/>
+    <col min="35" max="36" width="10.6640625" style="13" customWidth="1"/>
+    <col min="37" max="37" width="93.6640625" style="15" customWidth="1"/>
+    <col min="38" max="38" width="22.1640625" style="12" customWidth="1"/>
+    <col min="39" max="39" width="28.1640625" style="12" customWidth="1"/>
+    <col min="40" max="40" width="21.5" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" s="4" customFormat="1" ht="26">
+    <row r="1" spans="1:166" s="4" customFormat="1" ht="26">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="12"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="15"/>
       <c r="AL1" s="12"/>
       <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
     </row>
-    <row r="3" spans="1:165" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
+    <row r="3" spans="1:166" s="6" customFormat="1" ht="46" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
       <c r="S3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="59" t="s">
+      <c r="T3" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59" t="s">
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
       <c r="AA3" s="58"/>
-      <c r="AB3" s="59" t="s">
+      <c r="AB3" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
-      <c r="AF3" s="59"/>
-      <c r="AG3" s="59"/>
-      <c r="AH3" s="59"/>
-      <c r="AI3" s="1" t="s">
+      <c r="AC3" s="61"/>
+      <c r="AD3" s="61"/>
+      <c r="AE3" s="61"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="61"/>
+      <c r="AH3" s="61"/>
+      <c r="AI3" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK3" s="12"/>
       <c r="AL3" s="12"/>
       <c r="AM3" s="12"/>
-      <c r="AN3"/>
+      <c r="AN3" s="12"/>
       <c r="AO3"/>
       <c r="AP3"/>
       <c r="AQ3"/>
@@ -5627,8 +5963,9 @@
       <c r="FG3"/>
       <c r="FH3"/>
       <c r="FI3"/>
+      <c r="FJ3"/>
     </row>
-    <row r="4" spans="1:165" s="12" customFormat="1" ht="42" customHeight="1" thickTop="1" thickBot="1">
+    <row r="4" spans="1:166" s="12" customFormat="1" ht="42" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16" t="s">
@@ -5727,10 +6064,11 @@
       <c r="AH4" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
+      <c r="AI4" s="60"/>
+      <c r="AJ4" s="60"/>
+      <c r="AK4" s="16"/>
     </row>
-    <row r="5" spans="1:165" s="12" customFormat="1" ht="21" thickTop="1">
+    <row r="5" spans="1:166" s="12" customFormat="1" ht="21" thickTop="1">
       <c r="A5" s="20" t="s">
         <v>27</v>
       </c>
@@ -5805,12 +6143,13 @@
       <c r="AH5" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15" t="s">
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:165">
+    <row r="6" spans="1:166">
       <c r="A6" s="14" t="s">
         <v>99</v>
       </c>
@@ -5885,12 +6224,11 @@
       <c r="AH6" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15" t="s">
+      <c r="AK6" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:165">
+    <row r="7" spans="1:166">
       <c r="A7" s="15" t="s">
         <v>76</v>
       </c>
@@ -5965,12 +6303,11 @@
       <c r="AH7" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="15" t="s">
+      <c r="AK7" s="15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:165">
+    <row r="8" spans="1:166">
       <c r="A8" s="15" t="s">
         <v>244</v>
       </c>
@@ -6042,9 +6379,8 @@
       <c r="AH8" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI8" s="15"/>
     </row>
-    <row r="9" spans="1:165">
+    <row r="9" spans="1:166">
       <c r="A9" s="15" t="s">
         <v>248</v>
       </c>
@@ -6116,12 +6452,11 @@
       <c r="AH9" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="15" t="s">
+      <c r="AK9" s="15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:165">
+    <row r="10" spans="1:166">
       <c r="A10" s="15"/>
       <c r="B10" s="21" t="s">
         <v>104</v>
@@ -6190,9 +6525,8 @@
       <c r="AH10" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI10" s="15"/>
     </row>
-    <row r="11" spans="1:165" s="12" customFormat="1">
+    <row r="11" spans="1:166" s="12" customFormat="1">
       <c r="A11" s="15"/>
       <c r="B11" s="21" t="s">
         <v>316</v>
@@ -6261,12 +6595,13 @@
       <c r="AH11" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15" t="s">
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="15" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:165">
+    <row r="12" spans="1:166">
       <c r="A12" s="15"/>
       <c r="B12" s="21" t="s">
         <v>105</v>
@@ -6335,9 +6670,8 @@
       <c r="AH12" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI12" s="15"/>
     </row>
-    <row r="13" spans="1:165">
+    <row r="13" spans="1:166">
       <c r="B13" s="21"/>
       <c r="C13" s="26"/>
       <c r="D13" s="5"/>
@@ -6371,9 +6705,8 @@
       <c r="AF13" s="23"/>
       <c r="AG13" s="23"/>
       <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
     </row>
-    <row r="14" spans="1:165" ht="20">
+    <row r="14" spans="1:166" ht="20">
       <c r="A14" s="20" t="s">
         <v>26</v>
       </c>
@@ -6464,12 +6797,11 @@
       <c r="AH14" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="15" t="s">
+      <c r="AK14" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:165">
+    <row r="15" spans="1:166">
       <c r="A15" s="15" t="s">
         <v>93</v>
       </c>
@@ -6557,12 +6889,11 @@
       <c r="AH15" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15" t="s">
+      <c r="AK15" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:165">
+    <row r="16" spans="1:166">
       <c r="A16" s="15"/>
       <c r="B16" s="21" t="s">
         <v>107</v>
@@ -6648,12 +6979,11 @@
       <c r="AH16" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="15" t="s">
+      <c r="AK16" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:165">
+    <row r="17" spans="1:166">
       <c r="B17" s="21"/>
       <c r="C17" s="26"/>
       <c r="D17" s="5"/>
@@ -6687,9 +7017,8 @@
       <c r="AF17" s="23"/>
       <c r="AG17" s="23"/>
       <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
     </row>
-    <row r="18" spans="1:165" ht="20">
+    <row r="18" spans="1:166" ht="20">
       <c r="A18" s="20" t="s">
         <v>41</v>
       </c>
@@ -6775,12 +7104,11 @@
       <c r="AH18" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15" t="s">
+      <c r="AK18" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:165" s="12" customFormat="1">
+    <row r="19" spans="1:166" s="12" customFormat="1">
       <c r="A19" s="15" t="s">
         <v>241</v>
       </c>
@@ -6866,12 +7194,13 @@
       <c r="AH19" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15" t="s">
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
+      <c r="AK19" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:165" s="12" customFormat="1" ht="20">
+    <row r="20" spans="1:166" s="12" customFormat="1" ht="20">
       <c r="A20" s="31"/>
       <c r="B20" s="21" t="s">
         <v>137</v>
@@ -6955,11 +7284,11 @@
       <c r="AH20" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="15" t="s">
+      <c r="AI20" s="13"/>
+      <c r="AJ20" s="13"/>
+      <c r="AK20" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AN20" s="36"/>
       <c r="AO20" s="36"/>
       <c r="AP20" s="36"/>
       <c r="AQ20" s="36"/>
@@ -7085,8 +7414,9 @@
       <c r="FG20" s="36"/>
       <c r="FH20" s="36"/>
       <c r="FI20" s="36"/>
+      <c r="FJ20" s="36"/>
     </row>
-    <row r="21" spans="1:165" s="12" customFormat="1" ht="20">
+    <row r="21" spans="1:166" s="12" customFormat="1" ht="20">
       <c r="A21" s="31"/>
       <c r="B21" s="21" t="s">
         <v>136</v>
@@ -7167,9 +7497,9 @@
       <c r="AH21" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-      <c r="AN21" s="36"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="15"/>
       <c r="AO21" s="36"/>
       <c r="AP21" s="36"/>
       <c r="AQ21" s="36"/>
@@ -7295,8 +7625,9 @@
       <c r="FG21" s="36"/>
       <c r="FH21" s="36"/>
       <c r="FI21" s="36"/>
+      <c r="FJ21" s="36"/>
     </row>
-    <row r="22" spans="1:165">
+    <row r="22" spans="1:166">
       <c r="A22" s="15" t="s">
         <v>240</v>
       </c>
@@ -7379,12 +7710,11 @@
       <c r="AH22" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI22" s="15"/>
-      <c r="AJ22" s="15" t="s">
+      <c r="AK22" s="15" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:165">
+    <row r="23" spans="1:166">
       <c r="A23" s="15" t="s">
         <v>57</v>
       </c>
@@ -7418,9 +7748,8 @@
       <c r="AF23" s="23"/>
       <c r="AG23" s="23"/>
       <c r="AH23" s="15"/>
-      <c r="AI23" s="15"/>
     </row>
-    <row r="24" spans="1:165">
+    <row r="24" spans="1:166">
       <c r="A24" s="15"/>
       <c r="B24" s="21"/>
       <c r="C24" s="26"/>
@@ -7453,9 +7782,8 @@
       <c r="AF24" s="23"/>
       <c r="AG24" s="23"/>
       <c r="AH24" s="15"/>
-      <c r="AI24" s="15"/>
     </row>
-    <row r="25" spans="1:165">
+    <row r="25" spans="1:166">
       <c r="B25" s="21"/>
       <c r="C25" s="26"/>
       <c r="E25" s="13"/>
@@ -7487,9 +7815,8 @@
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
       <c r="AH25" s="15"/>
-      <c r="AI25" s="15"/>
     </row>
-    <row r="26" spans="1:165" ht="20">
+    <row r="26" spans="1:166" ht="20">
       <c r="A26" s="20" t="s">
         <v>42</v>
       </c>
@@ -7578,12 +7905,11 @@
       <c r="AH26" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI26" s="15"/>
-      <c r="AJ26" s="15" t="s">
+      <c r="AK26" s="15" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="1:165">
+    <row r="27" spans="1:166">
       <c r="A27" s="15" t="s">
         <v>310</v>
       </c>
@@ -7672,12 +7998,11 @@
       <c r="AH27" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI27" s="15"/>
-      <c r="AJ27" s="15" t="s">
+      <c r="AK27" s="15" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:165" s="12" customFormat="1">
+    <row r="28" spans="1:166" s="12" customFormat="1">
       <c r="A28" s="2"/>
       <c r="B28" s="21" t="s">
         <v>200</v>
@@ -7764,10 +8089,11 @@
       <c r="AH28" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI28" s="15"/>
-      <c r="AJ28" s="15"/>
+      <c r="AI28" s="13"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="15"/>
     </row>
-    <row r="29" spans="1:165" s="12" customFormat="1">
+    <row r="29" spans="1:166" s="12" customFormat="1">
       <c r="A29" s="2"/>
       <c r="B29" s="21" t="s">
         <v>201</v>
@@ -7854,10 +8180,11 @@
       <c r="AH29" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI29" s="15"/>
-      <c r="AJ29" s="15"/>
+      <c r="AI29" s="13"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="15"/>
     </row>
-    <row r="30" spans="1:165" s="12" customFormat="1">
+    <row r="30" spans="1:166" s="12" customFormat="1">
       <c r="A30" s="2"/>
       <c r="B30" s="21" t="s">
         <v>202</v>
@@ -7941,10 +8268,11 @@
       <c r="AH30" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI30" s="15"/>
-      <c r="AJ30" s="15"/>
+      <c r="AI30" s="13"/>
+      <c r="AJ30" s="13"/>
+      <c r="AK30" s="15"/>
     </row>
-    <row r="31" spans="1:165" s="12" customFormat="1">
+    <row r="31" spans="1:166" s="12" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="21" t="s">
         <v>203</v>
@@ -8028,10 +8356,11 @@
       <c r="AH31" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI31" s="15"/>
-      <c r="AJ31" s="15"/>
+      <c r="AI31" s="13"/>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="15"/>
     </row>
-    <row r="32" spans="1:165" s="12" customFormat="1">
+    <row r="32" spans="1:166" s="12" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="21" t="s">
         <v>204</v>
@@ -8115,10 +8444,11 @@
       <c r="AH32" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI32" s="15"/>
-      <c r="AJ32" s="15"/>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="13"/>
+      <c r="AK32" s="15"/>
     </row>
-    <row r="33" spans="1:165" s="12" customFormat="1">
+    <row r="33" spans="1:166" s="12" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="21" t="s">
         <v>205</v>
@@ -8202,10 +8532,11 @@
       <c r="AH33" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI33" s="15"/>
-      <c r="AJ33" s="15"/>
+      <c r="AI33" s="13"/>
+      <c r="AJ33" s="13"/>
+      <c r="AK33" s="15"/>
     </row>
-    <row r="34" spans="1:165">
+    <row r="34" spans="1:166">
       <c r="B34" s="21" t="s">
         <v>207</v>
       </c>
@@ -8295,12 +8626,11 @@
       <c r="AH34" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI34" s="15"/>
-      <c r="AJ34" s="15" t="s">
+      <c r="AK34" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:165">
+    <row r="35" spans="1:166">
       <c r="B35" s="21" t="s">
         <v>208</v>
       </c>
@@ -8384,9 +8714,8 @@
       <c r="AH35" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI35" s="15"/>
     </row>
-    <row r="36" spans="1:165" s="12" customFormat="1">
+    <row r="36" spans="1:166" s="12" customFormat="1">
       <c r="A36" s="37"/>
       <c r="B36" s="38" t="s">
         <v>209</v>
@@ -8471,9 +8800,9 @@
       <c r="AH36" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI36" s="15"/>
-      <c r="AJ36" s="15"/>
-      <c r="AN36" s="40"/>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="15"/>
       <c r="AO36" s="40"/>
       <c r="AP36" s="40"/>
       <c r="AQ36" s="40"/>
@@ -8599,8 +8928,9 @@
       <c r="FG36" s="40"/>
       <c r="FH36" s="40"/>
       <c r="FI36" s="40"/>
+      <c r="FJ36" s="40"/>
     </row>
-    <row r="37" spans="1:165">
+    <row r="37" spans="1:166">
       <c r="B37" s="21"/>
       <c r="C37" s="26"/>
       <c r="E37" s="13"/>
@@ -8635,9 +8965,8 @@
       <c r="AH37" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="AI37" s="15"/>
     </row>
-    <row r="38" spans="1:165" ht="20">
+    <row r="38" spans="1:166" ht="20">
       <c r="A38" s="20" t="s">
         <v>47</v>
       </c>
@@ -8730,9 +9059,8 @@
       <c r="AH38" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI38" s="15"/>
     </row>
-    <row r="39" spans="1:165" s="12" customFormat="1">
+    <row r="39" spans="1:166" s="12" customFormat="1">
       <c r="A39" s="15" t="s">
         <v>58</v>
       </c>
@@ -8825,10 +9153,11 @@
       <c r="AH39" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI39" s="15"/>
-      <c r="AJ39" s="15"/>
+      <c r="AI39" s="13"/>
+      <c r="AJ39" s="13"/>
+      <c r="AK39" s="15"/>
     </row>
-    <row r="40" spans="1:165" s="12" customFormat="1">
+    <row r="40" spans="1:166" s="12" customFormat="1">
       <c r="B40" s="21" t="s">
         <v>304</v>
       </c>
@@ -8918,10 +9247,11 @@
       <c r="AH40" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI40" s="15"/>
-      <c r="AJ40" s="15"/>
+      <c r="AI40" s="13"/>
+      <c r="AJ40" s="13"/>
+      <c r="AK40" s="15"/>
     </row>
-    <row r="41" spans="1:165">
+    <row r="41" spans="1:166">
       <c r="B41" s="21" t="s">
         <v>305</v>
       </c>
@@ -9008,9 +9338,8 @@
       <c r="AH41" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI41" s="15"/>
     </row>
-    <row r="42" spans="1:165">
+    <row r="42" spans="1:166">
       <c r="B42" s="21" t="s">
         <v>295</v>
       </c>
@@ -9102,9 +9431,8 @@
       <c r="AH42" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI42" s="15"/>
     </row>
-    <row r="43" spans="1:165" s="12" customFormat="1">
+    <row r="43" spans="1:166" s="12" customFormat="1">
       <c r="A43" s="2"/>
       <c r="B43" s="21" t="s">
         <v>133</v>
@@ -9197,10 +9525,11 @@
       <c r="AH43" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI43" s="15"/>
-      <c r="AJ43" s="15"/>
+      <c r="AI43" s="13"/>
+      <c r="AJ43" s="13"/>
+      <c r="AK43" s="15"/>
     </row>
-    <row r="44" spans="1:165" s="12" customFormat="1">
+    <row r="44" spans="1:166" s="12" customFormat="1">
       <c r="A44" s="2"/>
       <c r="B44" s="21" t="s">
         <v>134</v>
@@ -9290,10 +9619,11 @@
       <c r="AH44" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI44" s="15"/>
-      <c r="AJ44" s="15"/>
+      <c r="AI44" s="13"/>
+      <c r="AJ44" s="13"/>
+      <c r="AK44" s="15"/>
     </row>
-    <row r="45" spans="1:165" s="12" customFormat="1">
+    <row r="45" spans="1:166" s="12" customFormat="1">
       <c r="A45" s="2"/>
       <c r="B45" s="21"/>
       <c r="C45" s="26"/>
@@ -9325,15 +9655,16 @@
       <c r="AD45" s="49"/>
       <c r="AG45" s="49"/>
       <c r="AH45" s="15"/>
-      <c r="AI45" s="15"/>
-      <c r="AJ45" s="15"/>
+      <c r="AI45" s="13"/>
+      <c r="AJ45" s="13"/>
+      <c r="AK45" s="15"/>
     </row>
-    <row r="46" spans="1:165" ht="23" customHeight="1">
+    <row r="46" spans="1:166" ht="23" customHeight="1">
       <c r="A46" s="20" t="s">
         <v>212</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>143</v>
@@ -9417,17 +9748,16 @@
       <c r="AH46" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="AI46" s="15"/>
-      <c r="AJ46" s="15" t="s">
-        <v>345</v>
+      <c r="AK46" s="15" t="s">
+        <v>344</v>
       </c>
     </row>
-    <row r="47" spans="1:165" ht="24" customHeight="1">
+    <row r="47" spans="1:166" ht="24" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>290</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>144</v>
@@ -9511,14 +9841,13 @@
       <c r="AH47" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="AI47" s="15"/>
-      <c r="AJ47" s="15" t="s">
-        <v>346</v>
+      <c r="AK47" s="15" t="s">
+        <v>345</v>
       </c>
     </row>
-    <row r="48" spans="1:165" ht="28" customHeight="1">
+    <row r="48" spans="1:166" ht="28" customHeight="1">
       <c r="B48" s="21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C48" s="26" t="s">
         <v>144</v>
@@ -9602,14 +9931,13 @@
       <c r="AH48" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="AI48" s="15"/>
-      <c r="AJ48" s="15" t="s">
-        <v>347</v>
+      <c r="AK48" s="15" t="s">
+        <v>346</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:37">
       <c r="B49" s="21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>165</v>
@@ -9693,11 +10021,11 @@
       <c r="AH49" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="AJ49" s="15" t="s">
-        <v>348</v>
+      <c r="AK49" s="15" t="s">
+        <v>347</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="20">
+    <row r="50" spans="1:37" ht="20">
       <c r="A50" s="20" t="s">
         <v>163</v>
       </c>
@@ -9781,15 +10109,15 @@
       <c r="AH50" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI50" s="15">
+      <c r="AI50" s="13">
         <f>17280/2.5</f>
         <v>6912</v>
       </c>
-      <c r="AJ50" s="15" t="s">
+      <c r="AK50" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:37">
       <c r="A51" s="15" t="s">
         <v>222</v>
       </c>
@@ -9873,15 +10201,15 @@
       <c r="AH51" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI51" s="15">
+      <c r="AI51" s="13">
         <f>34560/2.5</f>
         <v>13824</v>
       </c>
-      <c r="AJ51" s="15" t="s">
+      <c r="AK51" s="15" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:37">
       <c r="B52" s="21" t="s">
         <v>195</v>
       </c>
@@ -9960,15 +10288,15 @@
       <c r="AH52" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI52" s="15">
+      <c r="AI52" s="13">
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
-      <c r="AJ52" s="56" t="s">
+      <c r="AK52" s="56" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:37">
       <c r="B53" s="21" t="s">
         <v>196</v>
       </c>
@@ -10047,19 +10375,19 @@
       <c r="AH53" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AI53" s="15">
+      <c r="AI53" s="13">
         <f>21600/2.5</f>
         <v>8640</v>
       </c>
-      <c r="AJ53" s="56" t="s">
+      <c r="AK53" s="56" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:37">
       <c r="C54" s="26"/>
       <c r="Q54" s="13"/>
     </row>
-    <row r="55" spans="1:36" ht="20">
+    <row r="55" spans="1:37" ht="20">
       <c r="A55" s="20" t="s">
         <v>172</v>
       </c>
@@ -10138,12 +10466,11 @@
       <c r="AH55" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AI55" s="15"/>
-      <c r="AJ55" s="15" t="s">
+      <c r="AK55" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:37">
       <c r="A56" s="15" t="s">
         <v>249</v>
       </c>
@@ -10222,9 +10549,8 @@
       <c r="AH56" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AI56" s="15"/>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:37">
       <c r="A57" s="15" t="s">
         <v>217</v>
       </c>
@@ -10303,9 +10629,8 @@
       <c r="AH57" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AI57" s="15"/>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:37">
       <c r="B58" s="21" t="s">
         <v>175</v>
       </c>
@@ -10386,12 +10711,11 @@
       <c r="AH58" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="AI58" s="15"/>
-      <c r="AJ58" s="15" t="s">
+      <c r="AK58" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:37">
       <c r="B59" s="21" t="s">
         <v>213</v>
       </c>
@@ -10457,7 +10781,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:37">
       <c r="B60" s="21" t="s">
         <v>214</v>
       </c>
@@ -10523,7 +10847,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:37">
       <c r="B61" s="21" t="s">
         <v>215</v>
       </c>
@@ -10589,10 +10913,10 @@
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:37">
       <c r="D62" s="13"/>
     </row>
-    <row r="63" spans="1:36" ht="20" customHeight="1">
+    <row r="63" spans="1:37" ht="20" customHeight="1">
       <c r="A63" s="20" t="s">
         <v>245</v>
       </c>
@@ -10647,11 +10971,11 @@
       <c r="AH63" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="AJ63" s="57" t="s">
+      <c r="AK63" s="57" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="20" customHeight="1">
+    <row r="64" spans="1:37" ht="20" customHeight="1">
       <c r="A64" s="15" t="s">
         <v>246</v>
       </c>
@@ -10710,11 +11034,11 @@
       <c r="AH64" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="AJ64" s="57" t="s">
+      <c r="AK64" s="57" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="20" customHeight="1">
+    <row r="65" spans="1:37" ht="20" customHeight="1">
       <c r="A65" s="15" t="s">
         <v>247</v>
       </c>
@@ -10773,11 +11097,11 @@
       <c r="AH65" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="AJ65" s="57" t="s">
+      <c r="AK65" s="57" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="20" customHeight="1">
+    <row r="66" spans="1:37" ht="20" customHeight="1">
       <c r="B66" s="21" t="s">
         <v>255</v>
       </c>
@@ -10833,11 +11157,11 @@
       <c r="AH66" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="AJ66" s="57" t="s">
+      <c r="AK66" s="57" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="20" customHeight="1">
+    <row r="67" spans="1:37" ht="20" customHeight="1">
       <c r="B67" s="21" t="s">
         <v>256</v>
       </c>
@@ -10893,11 +11217,11 @@
       <c r="AH67" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="AJ67" s="57" t="s">
+      <c r="AK67" s="57" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="20">
+    <row r="75" spans="1:37" ht="20">
       <c r="A75" s="20" t="s">
         <v>321</v>
       </c>
@@ -10963,24 +11287,24 @@
         <f>5/8</f>
         <v>0.625</v>
       </c>
-      <c r="AB75" s="13">
+      <c r="AB75" s="49">
         <v>440</v>
       </c>
-      <c r="AC75" s="13"/>
-      <c r="AD75" s="13"/>
-      <c r="AE75" s="13"/>
-      <c r="AF75" s="13">
+      <c r="AC75" s="49"/>
+      <c r="AD75" s="49"/>
+      <c r="AE75" s="49"/>
+      <c r="AF75" s="49">
         <v>220000</v>
       </c>
-      <c r="AG75" s="13"/>
+      <c r="AG75" s="49"/>
       <c r="AH75" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AJ75" s="15" t="s">
-        <v>339</v>
+      <c r="AK75" s="15" t="s">
+        <v>338</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:37">
       <c r="A76" s="15" t="s">
         <v>322</v>
       </c>
@@ -11046,21 +11370,758 @@
         <f>5/8</f>
         <v>0.625</v>
       </c>
-      <c r="AB76" s="13">
+      <c r="AB76" s="49">
         <v>400</v>
       </c>
-      <c r="AC76" s="13"/>
-      <c r="AD76" s="13"/>
-      <c r="AE76" s="13"/>
-      <c r="AF76" s="13">
+      <c r="AC76" s="49"/>
+      <c r="AD76" s="49"/>
+      <c r="AE76" s="49"/>
+      <c r="AF76" s="49">
         <v>198000</v>
       </c>
-      <c r="AG76" s="13"/>
+      <c r="AG76" s="49"/>
       <c r="AH76" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="AJ76" s="15" t="s">
-        <v>340</v>
+      <c r="AK76" s="15" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="C77" s="53"/>
+      <c r="D77" s="13"/>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="C78" s="53"/>
+      <c r="D78" s="13"/>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="C79" s="53"/>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="C80" s="53"/>
+      <c r="D80" s="13"/>
+    </row>
+    <row r="81" spans="1:37" ht="20">
+      <c r="A81" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C81" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D81" s="13">
+        <v>3</v>
+      </c>
+      <c r="E81" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F81" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G81" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H81" s="13">
+        <v>5</v>
+      </c>
+      <c r="I81" s="13">
+        <v>208</v>
+      </c>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L81" s="13">
+        <v>2</v>
+      </c>
+      <c r="M81" s="13">
+        <v>6</v>
+      </c>
+      <c r="N81" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O81" s="13">
+        <v>4</v>
+      </c>
+      <c r="P81" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q81" s="13">
+        <f t="shared" ref="Q81" si="28">M81*N81*P81/1000</f>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R81" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S81" s="13">
+        <v>54</v>
+      </c>
+      <c r="T81" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U81" s="13">
+        <v>50</v>
+      </c>
+      <c r="V81" s="13"/>
+      <c r="W81" s="13"/>
+      <c r="X81" s="13">
+        <v>80</v>
+      </c>
+      <c r="Z81" s="13" t="str">
+        <f t="shared" ref="Z81" si="29">X81&amp;"/"&amp;Y81</f>
+        <v>80/</v>
+      </c>
+      <c r="AA81" s="49"/>
+      <c r="AB81" s="49"/>
+      <c r="AC81" s="49"/>
+      <c r="AD81" s="49"/>
+      <c r="AE81" s="49">
+        <v>480000</v>
+      </c>
+      <c r="AH81" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI81" s="13">
+        <v>3000</v>
+      </c>
+      <c r="AJ81" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK81" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="C82" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D82" s="13">
+        <v>3</v>
+      </c>
+      <c r="E82" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F82" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G82" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H82" s="13">
+        <v>5</v>
+      </c>
+      <c r="I82" s="13">
+        <v>208</v>
+      </c>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L82" s="13">
+        <v>2</v>
+      </c>
+      <c r="M82" s="13">
+        <v>6</v>
+      </c>
+      <c r="N82" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O82" s="13">
+        <v>4</v>
+      </c>
+      <c r="P82" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q82" s="13">
+        <f t="shared" ref="Q82:Q84" si="30">M82*N82*P82/1000</f>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R82" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S82" s="13">
+        <v>54</v>
+      </c>
+      <c r="T82" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U82" s="13">
+        <v>50</v>
+      </c>
+      <c r="V82" s="13"/>
+      <c r="W82" s="13"/>
+      <c r="X82" s="13">
+        <v>80</v>
+      </c>
+      <c r="Y82" s="12"/>
+      <c r="Z82" s="13" t="str">
+        <f t="shared" ref="Z82:Z84" si="31">X82&amp;"/"&amp;Y82</f>
+        <v>80/</v>
+      </c>
+      <c r="AA82" s="49"/>
+      <c r="AB82" s="49"/>
+      <c r="AC82" s="49"/>
+      <c r="AD82" s="49"/>
+      <c r="AE82" s="49">
+        <v>120000</v>
+      </c>
+      <c r="AH82" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI82" s="13">
+        <v>3000</v>
+      </c>
+      <c r="AJ82" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK82" s="15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37" s="12" customFormat="1">
+      <c r="A83" s="2"/>
+      <c r="B83" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="C83" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D83" s="13">
+        <v>3</v>
+      </c>
+      <c r="E83" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F83" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G83" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H83" s="13">
+        <v>5</v>
+      </c>
+      <c r="I83" s="13">
+        <v>208</v>
+      </c>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L83" s="13">
+        <v>2</v>
+      </c>
+      <c r="M83" s="13">
+        <v>6</v>
+      </c>
+      <c r="N83" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O83" s="13">
+        <v>4</v>
+      </c>
+      <c r="P83" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q83" s="13">
+        <f t="shared" si="30"/>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R83" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S83" s="13">
+        <v>96</v>
+      </c>
+      <c r="T83" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U83" s="13">
+        <v>50</v>
+      </c>
+      <c r="V83" s="13"/>
+      <c r="W83" s="13"/>
+      <c r="X83" s="13">
+        <v>80</v>
+      </c>
+      <c r="Z83" s="13" t="str">
+        <f t="shared" si="31"/>
+        <v>80/</v>
+      </c>
+      <c r="AA83" s="49"/>
+      <c r="AB83" s="49"/>
+      <c r="AC83" s="49"/>
+      <c r="AD83" s="49"/>
+      <c r="AE83" s="49">
+        <v>480000</v>
+      </c>
+      <c r="AH83" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI83" s="13">
+        <f>AI81/1.2</f>
+        <v>2500</v>
+      </c>
+      <c r="AJ83" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK83" s="15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37" s="12" customFormat="1">
+      <c r="A84" s="2"/>
+      <c r="B84" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="C84" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D84" s="13">
+        <v>3</v>
+      </c>
+      <c r="E84" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F84" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G84" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H84" s="13">
+        <v>5</v>
+      </c>
+      <c r="I84" s="13">
+        <v>208</v>
+      </c>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L84" s="13">
+        <v>2</v>
+      </c>
+      <c r="M84" s="13">
+        <v>6</v>
+      </c>
+      <c r="N84" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O84" s="13">
+        <v>4</v>
+      </c>
+      <c r="P84" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q84" s="13">
+        <f t="shared" si="30"/>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R84" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S84" s="13">
+        <v>96</v>
+      </c>
+      <c r="T84" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U84" s="13">
+        <v>50</v>
+      </c>
+      <c r="V84" s="13"/>
+      <c r="W84" s="13"/>
+      <c r="X84" s="13">
+        <v>80</v>
+      </c>
+      <c r="Z84" s="13" t="str">
+        <f t="shared" si="31"/>
+        <v>80/</v>
+      </c>
+      <c r="AA84" s="49"/>
+      <c r="AB84" s="49"/>
+      <c r="AC84" s="49"/>
+      <c r="AD84" s="49"/>
+      <c r="AE84" s="49">
+        <v>120000</v>
+      </c>
+      <c r="AH84" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI84" s="13">
+        <f>AI81/1.2</f>
+        <v>2500</v>
+      </c>
+      <c r="AJ84" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK84" s="15" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="B85" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="C85" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D85" s="13">
+        <v>3</v>
+      </c>
+      <c r="E85" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F85" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G85" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H85" s="13">
+        <v>5</v>
+      </c>
+      <c r="I85" s="13">
+        <v>208</v>
+      </c>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L85" s="13">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M85" s="13">
+        <v>6</v>
+      </c>
+      <c r="N85" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O85" s="13">
+        <v>4</v>
+      </c>
+      <c r="P85" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q85" s="13">
+        <f t="shared" ref="Q85:Q87" si="32">M85*N85*P85/1000</f>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R85" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S85" s="13">
+        <v>25</v>
+      </c>
+      <c r="T85" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U85" s="13">
+        <v>30</v>
+      </c>
+      <c r="V85" s="13"/>
+      <c r="W85" s="13"/>
+      <c r="X85" s="13">
+        <v>80</v>
+      </c>
+      <c r="Y85" s="12"/>
+      <c r="Z85" s="13" t="str">
+        <f t="shared" ref="Z85:Z88" si="33">X85&amp;"/"&amp;Y85</f>
+        <v>80/</v>
+      </c>
+      <c r="AA85" s="49"/>
+      <c r="AB85" s="49"/>
+      <c r="AC85" s="49"/>
+      <c r="AD85" s="49"/>
+      <c r="AE85" s="49">
+        <v>480000</v>
+      </c>
+      <c r="AH85" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI85" s="13">
+        <f>AI81*2</f>
+        <v>6000</v>
+      </c>
+      <c r="AJ85" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK85" s="15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="B86" s="21" t="s">
+        <v>351</v>
+      </c>
+      <c r="C86" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D86" s="13">
+        <v>3</v>
+      </c>
+      <c r="E86" s="13">
+        <v>2496</v>
+      </c>
+      <c r="F86" s="13">
+        <v>3.524</v>
+      </c>
+      <c r="G86" s="13">
+        <v>1.175</v>
+      </c>
+      <c r="H86" s="13">
+        <v>5</v>
+      </c>
+      <c r="I86" s="13">
+        <v>208</v>
+      </c>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="L86" s="13">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M86" s="13">
+        <v>6</v>
+      </c>
+      <c r="N86" s="13">
+        <v>2.93</v>
+      </c>
+      <c r="O86" s="13">
+        <v>4</v>
+      </c>
+      <c r="P86" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q86" s="13">
+        <f t="shared" si="32"/>
+        <v>0.14064000000000002</v>
+      </c>
+      <c r="R86" s="13">
+        <v>1333</v>
+      </c>
+      <c r="S86" s="13">
+        <v>25</v>
+      </c>
+      <c r="T86" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U86" s="13">
+        <v>30</v>
+      </c>
+      <c r="V86" s="13"/>
+      <c r="W86" s="13"/>
+      <c r="X86" s="13">
+        <v>80</v>
+      </c>
+      <c r="Y86" s="12"/>
+      <c r="Z86" s="13" t="str">
+        <f t="shared" si="33"/>
+        <v>80/</v>
+      </c>
+      <c r="AA86" s="49"/>
+      <c r="AB86" s="49"/>
+      <c r="AC86" s="49"/>
+      <c r="AD86" s="49"/>
+      <c r="AE86" s="49">
+        <v>120000</v>
+      </c>
+      <c r="AH86" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI86" s="13">
+        <f>AI82*2</f>
+        <v>6000</v>
+      </c>
+      <c r="AJ86" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK86" s="15" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="B87" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C87" s="53" t="s">
+        <v>368</v>
+      </c>
+      <c r="D87" s="13">
+        <v>1</v>
+      </c>
+      <c r="E87" s="13">
+        <v>960</v>
+      </c>
+      <c r="F87" s="13">
+        <v>2.4883000000000002</v>
+      </c>
+      <c r="G87" s="13">
+        <v>311</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="I87" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="L87" s="13">
+        <v>4</v>
+      </c>
+      <c r="M87" s="13">
+        <v>8</v>
+      </c>
+      <c r="N87" s="13">
+        <v>2</v>
+      </c>
+      <c r="O87" s="13">
+        <v>4</v>
+      </c>
+      <c r="P87" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q87" s="13">
+        <f t="shared" si="32"/>
+        <v>0.128</v>
+      </c>
+      <c r="R87" s="13">
+        <v>1066</v>
+      </c>
+      <c r="S87" s="13">
+        <v>252</v>
+      </c>
+      <c r="T87" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="U87" s="13">
+        <v>500</v>
+      </c>
+      <c r="X87" s="13">
+        <v>40</v>
+      </c>
+      <c r="Z87" s="13" t="str">
+        <f t="shared" si="33"/>
+        <v>40/</v>
+      </c>
+      <c r="AE87" s="49">
+        <v>480000</v>
+      </c>
+      <c r="AH87" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI87" s="13">
+        <f>AI81/4</f>
+        <v>750</v>
+      </c>
+      <c r="AJ87" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK87" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="B88" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="C88" s="53" t="s">
+        <v>368</v>
+      </c>
+      <c r="D88" s="13">
+        <v>1</v>
+      </c>
+      <c r="E88" s="13">
+        <v>960</v>
+      </c>
+      <c r="F88" s="13">
+        <v>2.4883000000000002</v>
+      </c>
+      <c r="G88" s="13">
+        <v>311</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="I88" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="L88" s="13">
+        <v>4</v>
+      </c>
+      <c r="M88" s="13">
+        <v>8</v>
+      </c>
+      <c r="N88" s="13">
+        <v>2</v>
+      </c>
+      <c r="O88" s="13">
+        <v>4</v>
+      </c>
+      <c r="P88" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q88" s="13">
+        <f t="shared" ref="Q88" si="34">M88*N88*P88/1000</f>
+        <v>0.128</v>
+      </c>
+      <c r="R88" s="13">
+        <v>1066</v>
+      </c>
+      <c r="S88" s="13">
+        <v>252</v>
+      </c>
+      <c r="T88" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="U88" s="13">
+        <v>500</v>
+      </c>
+      <c r="V88" s="12"/>
+      <c r="W88" s="12"/>
+      <c r="X88" s="13">
+        <v>40</v>
+      </c>
+      <c r="Z88" s="13" t="str">
+        <f t="shared" si="33"/>
+        <v>40/</v>
+      </c>
+      <c r="AE88" s="49">
+        <v>120000</v>
+      </c>
+      <c r="AH88" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI88" s="13">
+        <f>AI82/4</f>
+        <v>750</v>
+      </c>
+      <c r="AJ88" s="13">
+        <v>1</v>
+      </c>
+      <c r="AK88" s="15" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -11072,8 +12133,8 @@
     <mergeCell ref="X3:Z3"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="AK38:AK40">
-    <cfRule type="colorScale" priority="104">
+  <conditionalFormatting sqref="AL38:AL40">
+    <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11084,8 +12145,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL38:AL40">
-    <cfRule type="colorScale" priority="103">
+  <conditionalFormatting sqref="AM38:AM40">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11096,8 +12157,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK41:AK45">
-    <cfRule type="colorScale" priority="99">
+  <conditionalFormatting sqref="AL41:AL45">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11108,8 +12169,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL41:AL45">
-    <cfRule type="colorScale" priority="98">
+  <conditionalFormatting sqref="AM41:AM45">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11120,8 +12181,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK41:AK45">
-    <cfRule type="colorScale" priority="97">
+  <conditionalFormatting sqref="AL41:AL45">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11132,8 +12193,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL41:AL45">
-    <cfRule type="colorScale" priority="96">
+  <conditionalFormatting sqref="AM41:AM45">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11144,23 +12205,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FJ20:XFD21 FJ36:XFD36 AB36 V35:AA36 U35 T35:T36 S35 R35:R36 A18 B19:I19 T22:W22 AB19:AG23 A13:AG13 A5:M8 A37:AG37 AK37:XFD41 AK20:AM21 AK42:AM45 AK22:XFD35 AJ37:AJ45 AJ19:AJ25 AK5:XFD19 AE40:AG40 A14:AC14 R34:Y34 AB34:AG35 Z50:AA53 AH50:AI52 AH53 AJ28:AJ35 A24:AG26 A31:B33 J31:O33 Q8:AG8 R9:AG9 Q9:Q10 A15:AG17 S19:W19 A27:O30 P27:AG33 A34:K35 L34:Q36 B9:C9 D9:M10 R6:AG7 R5:AJ5 Q5:Q7 N5:P10 A22:J22 A23:W23 Q50:Q61 D38:J38 A38:B38 AD45 AD41 Q45:Q48 AH45:AI45 AH40:AH41 B45 B41 K45:P45 R45:AB45 B40:J40 A39:J39 AI40:AI44 L38:AI38 L39:T41 V39:W41 U39:U44 R10:AF12 A10:C10 AH6:AI37 AJ6:AJ17 A11:Q12 Z41:AB41 Z40:AC40 Z39:AI39 X39:Y44">
-    <cfRule type="expression" dxfId="68" priority="90">
+  <conditionalFormatting sqref="FK20:XFD21 FK36:XFD36 AB36 V35:AA36 U35 T35:T36 S35 R35:R36 A18 B19:I19 T22:W22 AB19:AG23 A13:AG13 A5:M8 A37:AG37 AL37:XFD41 AL20:AN21 AL42:AN45 AL22:XFD35 AK37:AK45 AK19:AK25 AL5:XFD19 AE40:AG40 A14:AC14 R34:Y34 AB34:AG35 Z50:AA53 AH50:AJ52 AH53 AK28:AK35 A24:AG26 A31:B33 J31:O33 Q8:AG8 R9:AG9 Q9:Q10 A15:AG17 S19:W19 A27:O30 P27:AG33 A34:K35 L34:Q36 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A22:J22 A23:W23 Q50:Q61 D38:J38 A38:B38 AD45 AD41 Q45:Q48 AH45:AJ45 AH40:AH41 B45 B41 K45:P45 R45:AB45 B40:J40 A39:J39 AI40:AJ44 L38:AJ38 L39:T41 V39:W41 U39:U44 R10:AF12 A10:C10 AH6:AJ37 AK6:AK17 A11:Q12 Z41:AB41 Z40:AC40 Z39:AJ39 X39:Y44">
+    <cfRule type="expression" dxfId="80" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD14">
-    <cfRule type="expression" dxfId="67" priority="77">
+    <cfRule type="expression" dxfId="79" priority="89">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD40">
-    <cfRule type="expression" dxfId="66" priority="74">
+    <cfRule type="expression" dxfId="78" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK37:AK45 AK22:AK35 AK5:AK19">
-    <cfRule type="colorScale" priority="175">
+  <conditionalFormatting sqref="AL37:AL45 AL22:AL35 AL5:AL19">
+    <cfRule type="colorScale" priority="187">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11171,8 +12232,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL37:AL45 AL22:AL35 AL5:AL19">
-    <cfRule type="colorScale" priority="179">
+  <conditionalFormatting sqref="AM37:AM45 AM22:AM35 AM5:AM19">
+    <cfRule type="colorScale" priority="191">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11183,43 +12244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK37:AK40 AK22:AK35 AK5:AK19">
-    <cfRule type="colorScale" priority="183">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AL37:AL40 AL22:AL35 AL5:AL19">
-    <cfRule type="colorScale" priority="187">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM37:AM45 AM22:AM35 AM5:AM19">
-    <cfRule type="colorScale" priority="191">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK22:AK35 AK5:AK19">
     <cfRule type="colorScale" priority="195">
       <colorScale>
         <cfvo type="min"/>
@@ -11231,8 +12256,44 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AM37:AM40 AM22:AM35 AM5:AM19">
+    <cfRule type="colorScale" priority="199">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN37:AN45 AN22:AN35 AN5:AN19">
+    <cfRule type="colorScale" priority="203">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AL22:AL35 AL5:AL19">
-    <cfRule type="colorScale" priority="198">
+    <cfRule type="colorScale" priority="207">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM22:AM35 AM5:AM19">
+    <cfRule type="colorScale" priority="210">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11244,12 +12305,60 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:J21 T21:W21">
-    <cfRule type="expression" dxfId="65" priority="66">
+    <cfRule type="expression" dxfId="77" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK21">
-    <cfRule type="colorScale" priority="67">
+  <conditionalFormatting sqref="AL21">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM21">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL21">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM21">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN21">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11261,7 +12370,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL21">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM21">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11272,31 +12393,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK21">
-    <cfRule type="colorScale" priority="69">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="E20:I20">
+    <cfRule type="expression" dxfId="76" priority="69">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL21">
-    <cfRule type="colorScale" priority="70">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="B20:D20 S21:S22 S20:W20">
+    <cfRule type="expression" dxfId="75" priority="70">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM21">
+  <conditionalFormatting sqref="AL20">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -11308,8 +12415,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK21">
+  <conditionalFormatting sqref="AM20">
     <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL20">
+    <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11320,8 +12439,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL21">
-    <cfRule type="colorScale" priority="73">
+  <conditionalFormatting sqref="AM20">
+    <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11332,18 +12451,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:I20">
-    <cfRule type="expression" dxfId="64" priority="57">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:D20 S21:S22 S20:W20">
-    <cfRule type="expression" dxfId="63" priority="58">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="59">
+  <conditionalFormatting sqref="AN20">
+    <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11355,19 +12464,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL20">
-    <cfRule type="colorScale" priority="60">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11378,44 +12475,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL20">
-    <cfRule type="colorScale" priority="62">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AM20">
-    <cfRule type="colorScale" priority="63">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK20">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL20">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -11427,176 +12488,236 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z18:AA23">
-    <cfRule type="expression" dxfId="62" priority="55">
+    <cfRule type="expression" dxfId="74" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34:AA34">
-    <cfRule type="expression" dxfId="61" priority="54">
+    <cfRule type="expression" dxfId="73" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:AA49">
-    <cfRule type="expression" dxfId="60" priority="52">
+    <cfRule type="expression" dxfId="72" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M55:O55 N56:O61">
-    <cfRule type="expression" dxfId="59" priority="41">
+    <cfRule type="expression" dxfId="71" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R55:R61">
-    <cfRule type="expression" dxfId="58" priority="40">
+    <cfRule type="expression" dxfId="70" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z58:AA58">
-    <cfRule type="expression" dxfId="57" priority="39">
+    <cfRule type="expression" dxfId="69" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:I58">
-    <cfRule type="expression" dxfId="56" priority="38">
+    <cfRule type="expression" dxfId="68" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI53">
-    <cfRule type="expression" dxfId="55" priority="33">
+  <conditionalFormatting sqref="AI53:AJ53">
+    <cfRule type="expression" dxfId="67" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:I33">
-    <cfRule type="expression" dxfId="54" priority="32">
+    <cfRule type="expression" dxfId="66" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:I61">
-    <cfRule type="expression" dxfId="53" priority="31">
+    <cfRule type="expression" dxfId="65" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18:Q22">
-    <cfRule type="expression" dxfId="52" priority="30">
+    <cfRule type="expression" dxfId="64" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="expression" dxfId="51" priority="29">
+    <cfRule type="expression" dxfId="63" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18:K22">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="62" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P50">
-    <cfRule type="expression" dxfId="49" priority="24">
+    <cfRule type="expression" dxfId="61" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P51:P53">
-    <cfRule type="expression" dxfId="48" priority="23">
+    <cfRule type="expression" dxfId="60" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P58">
-    <cfRule type="expression" dxfId="47" priority="22">
+    <cfRule type="expression" dxfId="59" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P59:P61">
-    <cfRule type="expression" dxfId="46" priority="21">
+    <cfRule type="expression" dxfId="58" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:I67">
-    <cfRule type="expression" dxfId="45" priority="19">
+    <cfRule type="expression" dxfId="57" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:K44">
-    <cfRule type="expression" dxfId="44" priority="15">
+    <cfRule type="expression" dxfId="56" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE43:AG43 AD44 AH43:AH44 B44 B42:J43 L42:T44 V42:W44 Z44:AB44 Z42:AH42 Z43:AC43">
-    <cfRule type="expression" dxfId="43" priority="17">
+    <cfRule type="expression" dxfId="55" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD43">
-    <cfRule type="expression" dxfId="42" priority="16">
+    <cfRule type="expression" dxfId="54" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49">
+    <cfRule type="expression" dxfId="53" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E76:I76">
+    <cfRule type="expression" dxfId="52" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q75:Q76">
+    <cfRule type="expression" dxfId="51" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O76">
+    <cfRule type="expression" dxfId="50" priority="23">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P76">
+    <cfRule type="expression" dxfId="49" priority="22">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N76">
+    <cfRule type="expression" dxfId="48" priority="21">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L76">
+    <cfRule type="expression" dxfId="47" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M76">
+    <cfRule type="expression" dxfId="46" priority="19">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U76">
+    <cfRule type="expression" dxfId="45" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S76">
+    <cfRule type="expression" dxfId="44" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T76">
+    <cfRule type="expression" dxfId="43" priority="16">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X76">
+    <cfRule type="expression" dxfId="42" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH75">
     <cfRule type="expression" dxfId="41" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76:I76">
+  <conditionalFormatting sqref="AH76">
     <cfRule type="expression" dxfId="40" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q75:Q76">
+  <conditionalFormatting sqref="Q81:Q86">
     <cfRule type="expression" dxfId="39" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O76">
+  <conditionalFormatting sqref="Z81:Z86">
     <cfRule type="expression" dxfId="38" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P76">
+  <conditionalFormatting sqref="Q87:Q88">
     <cfRule type="expression" dxfId="37" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N76">
+  <conditionalFormatting sqref="Z87:Z88">
     <cfRule type="expression" dxfId="36" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L76">
+  <conditionalFormatting sqref="AH81">
     <cfRule type="expression" dxfId="35" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M76">
+  <conditionalFormatting sqref="AH82">
     <cfRule type="expression" dxfId="34" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U76">
+  <conditionalFormatting sqref="AH83">
     <cfRule type="expression" dxfId="33" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S76">
+  <conditionalFormatting sqref="AH84">
     <cfRule type="expression" dxfId="32" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T76">
+  <conditionalFormatting sqref="AH85">
     <cfRule type="expression" dxfId="31" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X76">
+  <conditionalFormatting sqref="AH86">
     <cfRule type="expression" dxfId="30" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH75">
+  <conditionalFormatting sqref="AH87">
     <cfRule type="expression" dxfId="29" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH76">
+  <conditionalFormatting sqref="AH88">
     <cfRule type="expression" dxfId="28" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -11618,13 +12739,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AE58"/>
+  <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="X27" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="P51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA37" sqref="AA37"/>
+      <selection pane="bottomRight" activeCell="E59" sqref="E59:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -11649,9 +12770,8 @@
     <col min="22" max="22" width="15" customWidth="1"/>
     <col min="23" max="23" width="15.6640625" customWidth="1"/>
     <col min="24" max="24" width="14.1640625" customWidth="1"/>
-    <col min="26" max="26" width="12" style="12" customWidth="1"/>
-    <col min="27" max="27" width="93.1640625" customWidth="1"/>
-    <col min="28" max="28" width="7.33203125" style="12" customWidth="1"/>
+    <col min="26" max="27" width="12" style="12" customWidth="1"/>
+    <col min="28" max="28" width="93.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="46" customFormat="1">
@@ -11728,7 +12848,10 @@
         <v>337</v>
       </c>
       <c r="AA1" s="45" t="s">
-        <v>338</v>
+        <v>374</v>
+      </c>
+      <c r="AB1" s="45" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="11" customFormat="1" ht="21" thickBot="1">
@@ -11811,9 +12934,11 @@
         <v>190</v>
       </c>
       <c r="AA2" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="AB2" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="AB2" s="12"/>
       <c r="AE2" s="12"/>
     </row>
     <row r="3" spans="1:31" ht="21" customHeight="1" thickTop="1">
@@ -11873,7 +12998,7 @@
         <v>69.92</v>
       </c>
       <c r="P3" s="13" t="str">
-        <f t="shared" ref="P3:AA18" ca="1" si="2">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="P3:AB18" ca="1" si="2">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>K80</v>
       </c>
       <c r="Q3" s="13">
@@ -11916,7 +13041,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA3" s="15" t="str">
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="15" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</v>
       </c>
@@ -11938,7 +13064,7 @@
         <v>95</v>
       </c>
       <c r="F4" s="18">
-        <f t="shared" ref="F4:F58" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="F4:F66" ca="1" si="4">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="G4" s="18">
@@ -12012,7 +13138,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA4" s="15" t="str">
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="15" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</v>
       </c>
@@ -12108,7 +13235,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA5" s="15" t="str">
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="15" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>Free Outbound Traffic = 1 GB/month.  One virtual CPU performance is calculated as one real Xeon E5-2686 v4 performance devided by 18 cores * 2 Hyper-threads = 36.</v>
       </c>
@@ -12204,8 +13332,9 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="15">
-        <f t="shared" ref="AA6:AA15" ca="1" si="8">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="15">
+        <f t="shared" ref="AB6:AB15" ca="1" si="8">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="AC6" s="42">
@@ -12303,7 +13432,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="15" t="str">
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>This is the average monthly payment over the course of the Dedicated Host Reservation term. For each month, the actual monthly payment will equal the actual number of hours in that month multiplied by the hourly usage rate. The hourly usage rate is equivalent to the total average monthly payments over the term divided by the total number of hours (based on a 365 day year) over the term.</v>
       </c>
@@ -12402,7 +13532,8 @@
         <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="15">
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="15">
         <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
@@ -12477,7 +13608,8 @@
       <c r="X9" s="13"/>
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
-      <c r="AA9" s="15" t="str">
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>This is the average monthly payment over the course of the Dedicated Host Reservation term. For each month, the actual monthly payment will equal the actual number of hours in that month multiplied by the hourly usage rate. The hourly usage rate is equivalent to the total average monthly payments over the term divided by the total number of hours (based on a 365 day year) over the term.</v>
       </c>
@@ -12552,7 +13684,8 @@
       <c r="X10" s="13"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
-      <c r="AA10" s="15">
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="15">
         <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
@@ -12655,7 +13788,8 @@
         <v>/0.1</v>
       </c>
       <c r="Z11" s="13"/>
-      <c r="AA11" s="15" t="str">
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>Outbound Traffic limited to 500GB.</v>
       </c>
@@ -12749,7 +13883,8 @@
         <v>/10</v>
       </c>
       <c r="Z12" s="13"/>
-      <c r="AA12" s="15" t="str">
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>Outbound Traffic limited to 500GB.</v>
       </c>
@@ -12843,7 +13978,8 @@
         <v>/10</v>
       </c>
       <c r="Z13" s="13"/>
-      <c r="AA13" s="15" t="str">
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>Outbound Traffic limited to 500GB.</v>
       </c>
@@ -12943,11 +14079,11 @@
         <v>7/</v>
       </c>
       <c r="Z14" s="13"/>
-      <c r="AA14" s="15" t="str">
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve"> http://www-01.ibm.com/common/ssi/cgi-bin/ssialias?htmlfid=POB03046USEN</v>
       </c>
-      <c r="AB14" s="15"/>
       <c r="AC14" s="42">
         <v>18</v>
       </c>
@@ -12982,7 +14118,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="18">
-        <f t="shared" ref="L15:L58" ca="1" si="14">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L15:L66" ca="1" si="14">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="M15" s="18" t="str">
@@ -13038,11 +14174,11 @@
         <v>7/</v>
       </c>
       <c r="Z15" s="13"/>
-      <c r="AA15" s="15" t="str">
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="15" t="str">
         <f t="shared" ca="1" si="8"/>
         <v xml:space="preserve"> http://www-01.ibm.com/common/ssi/cgi-bin/ssialias?htmlfid=POB03046USEN</v>
       </c>
-      <c r="AB15" s="15"/>
       <c r="AC15" s="42">
         <v>19</v>
       </c>
@@ -13133,7 +14269,7 @@
         <v>7/</v>
       </c>
       <c r="Z16" s="13"/>
-      <c r="AA16" s="15"/>
+      <c r="AA16" s="13"/>
       <c r="AB16" s="15"/>
       <c r="AC16" s="42">
         <v>20</v>
@@ -13225,7 +14361,7 @@
         <v>7/</v>
       </c>
       <c r="Z17" s="13"/>
-      <c r="AA17" s="15"/>
+      <c r="AA17" s="13"/>
       <c r="AB17" s="15"/>
       <c r="AC17" s="42">
         <v>21</v>
@@ -13317,7 +14453,7 @@
         <v>7/</v>
       </c>
       <c r="Z18" s="13"/>
-      <c r="AA18" s="15"/>
+      <c r="AA18" s="13"/>
       <c r="AB18" s="15"/>
       <c r="AC18" s="42">
         <v>22</v>
@@ -13398,7 +14534,7 @@
         <v>512</v>
       </c>
       <c r="U19" s="13" t="str">
-        <f t="shared" ref="U19:AA24" ca="1" si="19">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="U19:AB24" ca="1" si="19">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>SSD</v>
       </c>
       <c r="V19" s="13">
@@ -13418,11 +14554,11 @@
         <v>0</v>
       </c>
       <c r="Z19" s="13"/>
-      <c r="AA19" s="15" t="str">
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="15" t="str">
         <f t="shared" ca="1" si="19"/>
         <v>Limited quantity available at this price</v>
       </c>
-      <c r="AB19" s="15"/>
       <c r="AC19" s="42">
         <v>26</v>
       </c>
@@ -13516,11 +14652,11 @@
         <v>0</v>
       </c>
       <c r="Z20" s="13"/>
-      <c r="AA20" s="15" t="str">
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="15" t="str">
         <f t="shared" ca="1" si="19"/>
         <v>Limited quantity available at this price</v>
       </c>
-      <c r="AB20" s="15"/>
       <c r="AC20" s="42">
         <v>27</v>
       </c>
@@ -13614,11 +14750,11 @@
         <v>0</v>
       </c>
       <c r="Z21" s="13"/>
-      <c r="AA21" s="15">
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="15">
         <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
-      <c r="AB21" s="15"/>
       <c r="AC21" s="42">
         <v>28</v>
       </c>
@@ -13712,11 +14848,11 @@
         <v>0</v>
       </c>
       <c r="Z22" s="13"/>
-      <c r="AA22" s="15">
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="15">
         <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
-      <c r="AB22" s="15"/>
       <c r="AC22" s="42">
         <v>29</v>
       </c>
@@ -13810,11 +14946,11 @@
         <v>0</v>
       </c>
       <c r="Z23" s="13"/>
-      <c r="AA23" s="15">
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="15">
         <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
-      <c r="AB23" s="15"/>
       <c r="AC23" s="42">
         <v>30</v>
       </c>
@@ -13908,11 +15044,11 @@
         <v>0</v>
       </c>
       <c r="Z24" s="13"/>
-      <c r="AA24" s="15">
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="15">
         <f t="shared" ca="1" si="19"/>
         <v>0</v>
       </c>
-      <c r="AB24" s="15"/>
       <c r="AC24" s="42">
         <v>31</v>
       </c>
@@ -14006,11 +15142,11 @@
         <v>0</v>
       </c>
       <c r="Z25" s="13"/>
-      <c r="AA25" s="15">
-        <f t="shared" ref="AA25:AA51" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>0</v>
-      </c>
-      <c r="AB25" s="15"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="15">
+        <f t="shared" ref="AB25:AB51" ca="1" si="26">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>0</v>
+      </c>
       <c r="AC25" s="42">
         <v>32</v>
       </c>
@@ -14110,11 +15246,11 @@
         <v>0</v>
       </c>
       <c r="Z26" s="13"/>
-      <c r="AA26" s="15">
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="15"/>
       <c r="AC26" s="42">
         <v>33</v>
       </c>
@@ -14206,11 +15342,11 @@
         <v>3.03/</v>
       </c>
       <c r="Z27" s="13"/>
-      <c r="AA27" s="15" t="str">
+      <c r="AA27" s="13"/>
+      <c r="AB27" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Infiniband EDR (24.24Gb/s)</v>
       </c>
-      <c r="AB27" s="15"/>
       <c r="AC27" s="42">
         <v>34</v>
       </c>
@@ -14302,11 +15438,11 @@
         <v>0</v>
       </c>
       <c r="Z28" s="13"/>
-      <c r="AA28" s="15">
+      <c r="AA28" s="13"/>
+      <c r="AB28" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="15"/>
       <c r="AC28" s="42">
         <v>35</v>
       </c>
@@ -14398,11 +15534,11 @@
         <v>0</v>
       </c>
       <c r="Z29" s="13"/>
-      <c r="AA29" s="15">
+      <c r="AA29" s="13"/>
+      <c r="AB29" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="15"/>
       <c r="AC29" s="42">
         <v>36</v>
       </c>
@@ -14505,11 +15641,11 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z30" s="13"/>
-      <c r="AA30" s="15">
+      <c r="AA30" s="13"/>
+      <c r="AB30" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="15"/>
       <c r="AC30" s="42">
         <v>38</v>
       </c>
@@ -14604,11 +15740,11 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z31" s="13"/>
-      <c r="AA31" s="15">
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB31" s="15"/>
       <c r="AC31" s="42">
         <v>39</v>
       </c>
@@ -14703,7 +15839,7 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z32" s="13"/>
-      <c r="AA32" s="15"/>
+      <c r="AA32" s="13"/>
       <c r="AB32" s="15"/>
       <c r="AC32" s="42">
         <v>40</v>
@@ -14799,11 +15935,11 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z33" s="13"/>
-      <c r="AA33" s="15">
+      <c r="AA33" s="13"/>
+      <c r="AB33" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
-      <c r="AB33" s="15"/>
       <c r="AC33" s="42">
         <v>41</v>
       </c>
@@ -14857,7 +15993,7 @@
         <v>JPY</v>
       </c>
       <c r="N34" s="13">
-        <f t="shared" ref="N34:N58" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N34:N66" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.76800000000000002</v>
       </c>
       <c r="O34" s="13">
@@ -14905,7 +16041,8 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z34" s="13"/>
-      <c r="AA34" s="15">
+      <c r="AA34" s="13"/>
+      <c r="AB34" s="15">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
@@ -15002,7 +16139,8 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z35" s="13"/>
-      <c r="AA35" s="15">
+      <c r="AA35" s="13"/>
+      <c r="AB35" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -15100,7 +16238,8 @@
         <v>1.25/0.0125</v>
       </c>
       <c r="Z36" s="13"/>
-      <c r="AA36" s="15">
+      <c r="AA36" s="13"/>
+      <c r="AB36" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -15202,7 +16341,8 @@
         <v>5/1</v>
       </c>
       <c r="Z37" s="13"/>
-      <c r="AA37" s="15" t="str">
+      <c r="AA37" s="13"/>
+      <c r="AB37" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</v>
       </c>
@@ -15213,7 +16353,7 @@
     <row r="38" spans="1:29" ht="20">
       <c r="A38" s="55"/>
       <c r="C38" s="21" t="str">
-        <f t="shared" ref="C38:C58" ca="1" si="33">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <f t="shared" ref="C38:C66" ca="1" si="33">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>4 x GeForce GTX 1080 ltd.</v>
       </c>
       <c r="E38" s="21" t="s">
@@ -15303,7 +16443,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA38" s="15" t="str">
+      <c r="AA38" s="13"/>
+      <c r="AB38" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb.</v>
       </c>
@@ -15404,7 +16545,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA39" s="15" t="str">
+      <c r="AA39" s="13"/>
+      <c r="AB39" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</v>
       </c>
@@ -15508,7 +16650,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA40" s="15" t="str">
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included internet traffic (monthly based payments): 10 Tb/month. Included internet traffic (weekly based payments): 2.5 Tb/week. Included internet traffic (minute/hourly based payments): 0 Gb. Additional 1Gb (not included): 0,12 &amp;euro;/Gb.</v>
       </c>
@@ -15618,7 +16761,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>6912</v>
       </c>
-      <c r="AA41" s="15" t="str">
+      <c r="AA41" s="13"/>
+      <c r="AB41" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
       </c>
@@ -15721,7 +16865,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>13824</v>
       </c>
-      <c r="AA42" s="15" t="str">
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
       </c>
@@ -15785,7 +16930,7 @@
         <v>19</v>
       </c>
       <c r="P43" s="13" t="str">
-        <f t="shared" ref="P43:X58" ca="1" si="38">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="P43:X59" ca="1" si="38">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>P100</v>
       </c>
       <c r="Q43" s="13">
@@ -15828,7 +16973,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>8640</v>
       </c>
-      <c r="AA43" s="15" t="str">
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
@@ -15925,14 +17071,15 @@
         <v>0</v>
       </c>
       <c r="Y44" s="13" t="str">
-        <f t="shared" ref="Y44:Z58" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="Y44:AA60" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>13.64/</v>
       </c>
       <c r="Z44" s="13">
         <f t="shared" ca="1" si="34"/>
         <v>8640</v>
       </c>
-      <c r="AA44" s="15" t="str">
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
@@ -16040,7 +17187,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA45" s="15" t="str">
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v xml:space="preserve">1 GPU in specification is 1/2 of K80 </v>
       </c>
@@ -16140,7 +17288,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA46" s="15">
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -16161,7 +17310,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="13">
-        <f t="shared" ref="G47:G58" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="G47:G66" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>3.6</v>
       </c>
       <c r="H47" s="18">
@@ -16240,7 +17389,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA47" s="15">
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -16344,7 +17494,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA48" s="15" t="str">
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="15" t="str">
         <f t="shared" ca="1" si="26"/>
         <v>RDMA capable</v>
       </c>
@@ -16448,7 +17599,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA49" s="15">
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -16552,7 +17704,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA50" s="15">
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -16577,7 +17730,7 @@
         <v>4.97</v>
       </c>
       <c r="H51" s="18">
-        <f t="shared" ref="H51:K58" ca="1" si="43">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="H51:K66" ca="1" si="43">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="I51" s="18">
@@ -16597,7 +17750,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="18" t="str">
-        <f t="shared" ref="M51:M58" ca="1" si="44">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M51:M66" ca="1" si="44">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>USD</v>
       </c>
       <c r="N51" s="13">
@@ -16652,7 +17805,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA51" s="15">
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="15">
         <f t="shared" ca="1" si="26"/>
         <v>0</v>
       </c>
@@ -16762,8 +17916,9 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA52" s="15" t="str">
-        <f t="shared" ref="AA52:AA58" ca="1" si="47">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+      <c r="AA52" s="13"/>
+      <c r="AB52" s="15" t="str">
+        <f t="shared" ref="AB52:AB66" ca="1" si="47">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
       <c r="AC52" s="42">
@@ -16865,7 +18020,8 @@
         <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
-      <c r="AA53" s="15" t="str">
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
@@ -16921,7 +18077,7 @@
         <v>0.67679999999999996</v>
       </c>
       <c r="O54" s="13">
-        <f t="shared" ref="O54:O58" ca="1" si="48">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="O54:O66" ca="1" si="48">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>17.48</v>
       </c>
       <c r="P54" s="13" t="str">
@@ -16968,7 +18124,8 @@
         <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
-      <c r="AA54" s="15" t="str">
+      <c r="AA54" s="13"/>
+      <c r="AB54" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
@@ -17071,7 +18228,8 @@
         <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
-      <c r="AA55" s="15" t="str">
+      <c r="AA55" s="13"/>
+      <c r="AB55" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
@@ -17174,7 +18332,8 @@
         <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
-      <c r="AA56" s="15" t="str">
+      <c r="AA56" s="13"/>
+      <c r="AB56" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>For the n1 series of machine types, a virtual CPU is implemented as a single hardware hyper-thread on a 2.6 GHz Intel Xeon E5 (Sandy Bridge), 2.5 GHz Intel Xeon E5 v2 (Ivy Bridge), 2.3 GHz Intel Xeon E5 v3 (Haswell), or 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;_x000D_Assumption: CPUS considered to have 2 hyper threads per physical core.&lt;br&gt;_x000D_Mean values for DP and SP: 14.1GFlops and 28.2GFlops&lt;br&gt;_x000D_In vCPU performance used SP value: 0.0282TFlops per vCPU.</v>
       </c>
@@ -17281,7 +18440,8 @@
         <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
-      <c r="AA57" s="15" t="str">
+      <c r="AA57" s="13"/>
+      <c r="AB57" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</v>
       </c>
@@ -17381,17 +18541,865 @@
         <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
-      <c r="AA58" s="15" t="str">
+      <c r="AA58" s="13"/>
+      <c r="AB58" s="15" t="str">
         <f t="shared" ca="1" si="47"/>
         <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</v>
       </c>
       <c r="AC58" s="42">
         <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" ht="20">
+      <c r="A59" s="55" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>Tsubame 2.5</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="C59" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>S</v>
+      </c>
+      <c r="E59" s="21" t="str">
+        <f ca="1">"Tsub." &amp; C59</f>
+        <v>Tsub.S</v>
+      </c>
+      <c r="F59" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G59" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I59" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>480000</v>
+      </c>
+      <c r="K59" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L59" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M59" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N59" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.28128000000000003</v>
+      </c>
+      <c r="O59" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P59" s="13" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>K20</v>
+      </c>
+      <c r="Q59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="R59" s="13" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="T59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>54</v>
+      </c>
+      <c r="U59" s="13" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>SSD</v>
+      </c>
+      <c r="V59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>50</v>
+      </c>
+      <c r="W59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="X59" s="13">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="Y59" s="13" t="str">
+        <f t="shared" ca="1" si="39"/>
+        <v>80/</v>
+      </c>
+      <c r="Z59" s="13">
+        <f t="shared" ca="1" si="39"/>
+        <v>3000</v>
+      </c>
+      <c r="AA59" s="13">
+        <f t="shared" ca="1" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="AB59" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+      </c>
+      <c r="AC59" s="42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29">
+      <c r="C60" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>S open</v>
+      </c>
+      <c r="E60" s="21" t="str">
+        <f t="shared" ref="E60:E66" ca="1" si="49">"Tsub." &amp; C60</f>
+        <v>Tsub.S open</v>
+      </c>
+      <c r="F60" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G60" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H60" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I60" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>120000</v>
+      </c>
+      <c r="K60" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L60" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M60" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N60" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.28128000000000003</v>
+      </c>
+      <c r="O60" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P60" s="13" t="str">
+        <f t="shared" ref="P60:AA66" ca="1" si="50">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>K20</v>
+      </c>
+      <c r="Q60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="R60" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="T60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>54</v>
+      </c>
+      <c r="U60" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>50</v>
+      </c>
+      <c r="W60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y60" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>80/</v>
+      </c>
+      <c r="Z60" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3000</v>
+      </c>
+      <c r="AA60" s="13">
+        <f t="shared" ca="1" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="AB60" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;2 day.</v>
+      </c>
+      <c r="AC60" s="42">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29">
+      <c r="C61" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>S96</v>
+      </c>
+      <c r="E61" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.S96</v>
+      </c>
+      <c r="F61" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H61" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I61" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>480000</v>
+      </c>
+      <c r="K61" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L61" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M61" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N61" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.28128000000000003</v>
+      </c>
+      <c r="O61" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P61" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>K20</v>
+      </c>
+      <c r="Q61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="R61" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="T61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>96</v>
+      </c>
+      <c r="U61" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>50</v>
+      </c>
+      <c r="W61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>80/</v>
+      </c>
+      <c r="Z61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>2500</v>
+      </c>
+      <c r="AA61" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB61" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;3 day.</v>
+      </c>
+      <c r="AC61" s="42">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29">
+      <c r="C62" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>S96 open</v>
+      </c>
+      <c r="E62" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.S96 open</v>
+      </c>
+      <c r="F62" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>120000</v>
+      </c>
+      <c r="K62" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N62" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.28128000000000003</v>
+      </c>
+      <c r="O62" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P62" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>K20</v>
+      </c>
+      <c r="Q62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="R62" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="T62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>96</v>
+      </c>
+      <c r="U62" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>50</v>
+      </c>
+      <c r="W62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>80/</v>
+      </c>
+      <c r="Z62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>2500</v>
+      </c>
+      <c r="AA62" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB62" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;4 day.</v>
+      </c>
+      <c r="AC62" s="42">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29">
+      <c r="C63" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>G</v>
+      </c>
+      <c r="E63" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.G</v>
+      </c>
+      <c r="F63" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H63" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I63" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>480000</v>
+      </c>
+      <c r="K63" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N63" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>9.376000000000001E-2</v>
+      </c>
+      <c r="O63" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P63" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>K20</v>
+      </c>
+      <c r="Q63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="R63" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>25</v>
+      </c>
+      <c r="U63" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>30</v>
+      </c>
+      <c r="W63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>80/</v>
+      </c>
+      <c r="Z63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>6000</v>
+      </c>
+      <c r="AA63" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB63" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;5 day.</v>
+      </c>
+      <c r="AC63" s="42">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29">
+      <c r="C64" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>G open</v>
+      </c>
+      <c r="E64" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.G open</v>
+      </c>
+      <c r="F64" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H64" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I64" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>120000</v>
+      </c>
+      <c r="K64" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L64" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M64" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N64" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>9.376000000000001E-2</v>
+      </c>
+      <c r="O64" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P64" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>K20</v>
+      </c>
+      <c r="Q64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>3</v>
+      </c>
+      <c r="R64" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>25</v>
+      </c>
+      <c r="U64" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>30</v>
+      </c>
+      <c r="W64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y64" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>80/</v>
+      </c>
+      <c r="Z64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>6000</v>
+      </c>
+      <c r="AA64" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB64" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;6 day.</v>
+      </c>
+      <c r="AC64" s="42">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="3:29">
+      <c r="C65" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>L256</v>
+      </c>
+      <c r="E65" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.L256</v>
+      </c>
+      <c r="F65" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H65" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I65" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J65" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>480000</v>
+      </c>
+      <c r="K65" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L65" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M65" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N65" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="O65" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>2.4883000000000002</v>
+      </c>
+      <c r="P65" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>S1070</v>
+      </c>
+      <c r="Q65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="R65" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X7550</v>
+      </c>
+      <c r="S65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="T65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>252</v>
+      </c>
+      <c r="U65" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>500</v>
+      </c>
+      <c r="W65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y65" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>40/</v>
+      </c>
+      <c r="Z65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>750</v>
+      </c>
+      <c r="AA65" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB65" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;7 day.</v>
+      </c>
+      <c r="AC65" s="42">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="3:29">
+      <c r="C66" s="21" t="str">
+        <f t="shared" ca="1" si="33"/>
+        <v>L256 open</v>
+      </c>
+      <c r="E66" s="21" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Tsub.L256 open</v>
+      </c>
+      <c r="F66" s="18">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="13">
+        <f t="shared" ca="1" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="H66" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>120000</v>
+      </c>
+      <c r="K66" s="18">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L66" s="18">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M66" s="18" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>JPY</v>
+      </c>
+      <c r="N66" s="13">
+        <f t="shared" ca="1" si="30"/>
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="O66" s="13">
+        <f t="shared" ca="1" si="48"/>
+        <v>2.4883000000000002</v>
+      </c>
+      <c r="P66" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>S1070</v>
+      </c>
+      <c r="Q66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="R66" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>Xeon X7550</v>
+      </c>
+      <c r="S66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="T66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>252</v>
+      </c>
+      <c r="U66" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>SSD</v>
+      </c>
+      <c r="V66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>500</v>
+      </c>
+      <c r="W66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="X66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Y66" s="13" t="str">
+        <f t="shared" ca="1" si="50"/>
+        <v>40/</v>
+      </c>
+      <c r="Z66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>750</v>
+      </c>
+      <c r="AA66" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="AB66" s="15" t="str">
+        <f t="shared" ca="1" si="47"/>
+        <v>Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;8 day.</v>
+      </c>
+      <c r="AC66" s="42">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="V11:Z11 I19 E24:E25 G24:H29 D24:D33 I22:I28 D12:D16 D19:E22 V20:X26 V27:Z31 R20:U31 V36 N19:Q31 Z19:Z26 AA19:AA37 L19:M36 N33:U36 V33:Z35 N32:Z32 C19:C37 E32:E33 E28:E30 S50:V52 Z16 Y16:Y26 Y12:Z15 U11:U18 V12:X18 M52:Q52 M37:V49 C11:C16 C3:D10 L4:T16 AA6:AA16 Y38:AA58 R50:R58 H30:H58 L37:L58 J41:J58 E3:H3 E4:E16 G4:J6 G7:H10 G11:I16 G20:I22 G19 F4:F58 M3:T3">
+  <conditionalFormatting sqref="V11:AA11 I19 E24:E25 G24:H29 D24:D33 I22:I28 D12:D16 D19:E22 V20:X26 V27:AA31 R20:U31 V36 N19:Q31 Z19:AA26 AB19:AB37 L19:M36 N33:U36 V33:AA35 N32:AA32 C19:C37 E32:E33 E28:E30 S50:V52 Z16:AA16 Y16:Y26 Y12:AA15 U11:U18 V12:X18 M52:Q52 M37:V49 C11:C16 C3:D10 L4:T16 AB6:AB16 E3:H3 E4:E16 G4:J6 G7:H10 G11:I16 G20:I22 G19 M3:T3 R50:R66 H30:H66 L37:L66 J41:J66 F4:F66 Y38:AB66">
     <cfRule type="expression" dxfId="27" priority="145">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17401,7 +19409,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W36:Z36 Y37:Z37 U3:Y10 W37:X58">
+  <conditionalFormatting sqref="W36:AA36 Y37:AA37 U3:Y10 W37:X66">
     <cfRule type="expression" dxfId="25" priority="85">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17446,12 +19454,12 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29:I58">
+  <conditionalFormatting sqref="I29:I66">
     <cfRule type="expression" dxfId="16" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G30:G58">
+  <conditionalFormatting sqref="G30:G66">
     <cfRule type="expression" dxfId="15" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17461,22 +19469,22 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M53:Q58">
+  <conditionalFormatting sqref="M53:Q66">
     <cfRule type="expression" dxfId="13" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V53:V58 T53:T58">
+  <conditionalFormatting sqref="V53:V66 T53:T66">
     <cfRule type="expression" dxfId="12" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S53:S58">
+  <conditionalFormatting sqref="S53:S66">
     <cfRule type="expression" dxfId="11" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U53:U58">
+  <conditionalFormatting sqref="U53:U66">
     <cfRule type="expression" dxfId="10" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17491,7 +19499,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:E18 Z17:AA18 L17:T18 G17:I18">
+  <conditionalFormatting sqref="C17:E18 Z17:AB18 L17:T18 G17:I18">
     <cfRule type="expression" dxfId="7" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17511,7 +19519,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z10">
+  <conditionalFormatting sqref="Z3:AA10">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -17526,7 +19534,7 @@
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:L3 K4:K58">
+  <conditionalFormatting sqref="J3:L3 K4:K66">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Use special calculations of koeff3 of Tsubame 2.5. Tsubame2.5 has unique "continuous" parameter = 2.5. Only for time x cost graphs, cause koeff3 depends on job length, not rent period.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="48220" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="48220" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5105,7 +5105,18 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="152">
+  <dxfs count="153">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -7075,11 +7086,11 @@
   </sheetPr>
   <dimension ref="A1:FJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AC133" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="U139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AK155" sqref="AK155"/>
+      <selection pane="bottomRight" activeCell="AJ147" sqref="AJ147:AJ156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7117,7 +7128,7 @@
     <col min="32" max="32" width="12.6640625" style="12" customWidth="1"/>
     <col min="33" max="33" width="14.1640625" style="12" customWidth="1"/>
     <col min="34" max="34" width="8.83203125" style="12" customWidth="1"/>
-    <col min="35" max="35" width="12" style="13" customWidth="1"/>
+    <col min="35" max="35" width="17" style="13" customWidth="1"/>
     <col min="36" max="36" width="10.6640625" style="13" customWidth="1"/>
     <col min="37" max="37" width="93.6640625" style="15" customWidth="1"/>
     <col min="38" max="38" width="22.1640625" style="12" customWidth="1"/>
@@ -18016,7 +18027,7 @@
         <v>3000</v>
       </c>
       <c r="AJ147" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK147" s="15" t="s">
         <v>294</v>
@@ -18115,7 +18126,7 @@
         <v>3000</v>
       </c>
       <c r="AJ148" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK148" s="15" t="s">
         <v>421</v>
@@ -18213,7 +18224,7 @@
         <v>2500</v>
       </c>
       <c r="AJ149" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK149" s="15" t="s">
         <v>294</v>
@@ -18311,7 +18322,7 @@
         <v>2500</v>
       </c>
       <c r="AJ150" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK150" s="15" t="s">
         <v>421</v>
@@ -18410,7 +18421,7 @@
         <v>6000</v>
       </c>
       <c r="AJ151" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK151" s="15" t="s">
         <v>294</v>
@@ -18509,7 +18520,7 @@
         <v>6000</v>
       </c>
       <c r="AJ152" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK152" s="15" t="s">
         <v>421</v>
@@ -18607,7 +18618,7 @@
         <v>750</v>
       </c>
       <c r="AJ153" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK153" s="15" t="s">
         <v>294</v>
@@ -18705,7 +18716,7 @@
         <v>750</v>
       </c>
       <c r="AJ154" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK154" s="15" t="s">
         <v>421</v>
@@ -18803,7 +18814,7 @@
         <v>375</v>
       </c>
       <c r="AJ155" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK155" s="15" t="s">
         <v>294</v>
@@ -18901,7 +18912,7 @@
         <v>375</v>
       </c>
       <c r="AJ156" s="13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK156" s="15" t="s">
         <v>421</v>
@@ -19043,17 +19054,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 AH32:AJ32 A11:Q21 AL32:XFD33 A32:AC32 C33:AJ33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72">
-    <cfRule type="expression" dxfId="151" priority="235">
+    <cfRule type="expression" dxfId="152" priority="235">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="150" priority="222">
+    <cfRule type="expression" dxfId="151" priority="222">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="149" priority="211">
+    <cfRule type="expression" dxfId="150" priority="211">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19142,7 +19153,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="148" priority="203">
+    <cfRule type="expression" dxfId="149" priority="203">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19231,152 +19242,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="147" priority="200">
+    <cfRule type="expression" dxfId="148" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="146" priority="199">
+    <cfRule type="expression" dxfId="147" priority="199">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="145" priority="177">
+    <cfRule type="expression" dxfId="146" priority="177">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="144" priority="175">
+    <cfRule type="expression" dxfId="145" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="143" priority="174">
+    <cfRule type="expression" dxfId="144" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="142" priority="173">
+    <cfRule type="expression" dxfId="143" priority="173">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="141" priority="160">
+    <cfRule type="expression" dxfId="142" priority="160">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="140" priority="162">
+    <cfRule type="expression" dxfId="141" priority="162">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="139" priority="97">
+    <cfRule type="expression" dxfId="140" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="138" priority="128">
+    <cfRule type="expression" dxfId="139" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="137" priority="127">
+    <cfRule type="expression" dxfId="138" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="136" priority="126">
+    <cfRule type="expression" dxfId="137" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="135" priority="125">
+    <cfRule type="expression" dxfId="136" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="134" priority="124">
+    <cfRule type="expression" dxfId="135" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="133" priority="123">
+    <cfRule type="expression" dxfId="134" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="132" priority="122">
+    <cfRule type="expression" dxfId="133" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="131" priority="121">
+    <cfRule type="expression" dxfId="132" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="130" priority="120">
+    <cfRule type="expression" dxfId="131" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="129" priority="119">
+    <cfRule type="expression" dxfId="130" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="128" priority="118">
+    <cfRule type="expression" dxfId="129" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="127" priority="117">
+    <cfRule type="expression" dxfId="128" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="126" priority="116">
+    <cfRule type="expression" dxfId="127" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="125" priority="113">
+    <cfRule type="expression" dxfId="126" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="124" priority="115">
+    <cfRule type="expression" dxfId="125" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="123" priority="114">
+    <cfRule type="expression" dxfId="124" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="122" priority="112">
+    <cfRule type="expression" dxfId="123" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="121" priority="111">
+    <cfRule type="expression" dxfId="122" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="120" priority="110">
+    <cfRule type="expression" dxfId="121" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="119" priority="109">
+    <cfRule type="expression" dxfId="120" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="118" priority="108">
+    <cfRule type="expression" dxfId="119" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19465,97 +19476,97 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="117" priority="107">
+    <cfRule type="expression" dxfId="118" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="116" priority="106">
+    <cfRule type="expression" dxfId="117" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="115" priority="105">
+    <cfRule type="expression" dxfId="116" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="114" priority="104">
+    <cfRule type="expression" dxfId="115" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="113" priority="103">
+    <cfRule type="expression" dxfId="114" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="112" priority="102">
+    <cfRule type="expression" dxfId="113" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="111" priority="101">
+    <cfRule type="expression" dxfId="112" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="110" priority="100">
+    <cfRule type="expression" dxfId="111" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="109" priority="99">
+    <cfRule type="expression" dxfId="110" priority="99">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="108" priority="60">
+    <cfRule type="expression" dxfId="109" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="107" priority="96">
+    <cfRule type="expression" dxfId="108" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="106" priority="95">
+    <cfRule type="expression" dxfId="107" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="105" priority="94">
+    <cfRule type="expression" dxfId="106" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="104" priority="93">
+    <cfRule type="expression" dxfId="105" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="103" priority="92">
+    <cfRule type="expression" dxfId="104" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE35:AH36">
-    <cfRule type="expression" dxfId="102" priority="91">
+    <cfRule type="expression" dxfId="103" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="101" priority="90">
+    <cfRule type="expression" dxfId="102" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="100" priority="89">
+    <cfRule type="expression" dxfId="101" priority="89">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="99" priority="85">
+    <cfRule type="expression" dxfId="100" priority="85">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19596,7 +19607,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="98" priority="80">
+    <cfRule type="expression" dxfId="99" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19649,362 +19660,362 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="97" priority="79">
+    <cfRule type="expression" dxfId="98" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="96" priority="78">
+    <cfRule type="expression" dxfId="97" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="95" priority="77">
+    <cfRule type="expression" dxfId="96" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="94" priority="76">
+    <cfRule type="expression" dxfId="95" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="93" priority="75">
+    <cfRule type="expression" dxfId="94" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="92" priority="74">
+    <cfRule type="expression" dxfId="93" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="91" priority="73">
+    <cfRule type="expression" dxfId="92" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="90" priority="72">
+    <cfRule type="expression" dxfId="91" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="89" priority="68">
+    <cfRule type="expression" dxfId="90" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="88" priority="70">
+    <cfRule type="expression" dxfId="89" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="87" priority="69">
+    <cfRule type="expression" dxfId="88" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="86" priority="67">
+    <cfRule type="expression" dxfId="87" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="85" priority="66">
+    <cfRule type="expression" dxfId="86" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="84" priority="64">
+    <cfRule type="expression" dxfId="85" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="83" priority="63">
+    <cfRule type="expression" dxfId="84" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="82" priority="62">
+    <cfRule type="expression" dxfId="83" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="81" priority="61">
+    <cfRule type="expression" dxfId="82" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="80" priority="59">
+    <cfRule type="expression" dxfId="81" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="79" priority="57">
+    <cfRule type="expression" dxfId="80" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="78" priority="56">
+    <cfRule type="expression" dxfId="79" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="77" priority="54">
+    <cfRule type="expression" dxfId="78" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="76" priority="53">
+    <cfRule type="expression" dxfId="77" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="75" priority="52">
+    <cfRule type="expression" dxfId="76" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="74" priority="14">
+    <cfRule type="expression" dxfId="75" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="73" priority="3">
+    <cfRule type="expression" dxfId="74" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="expression" dxfId="72" priority="50">
+    <cfRule type="expression" dxfId="73" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="71" priority="51">
+    <cfRule type="expression" dxfId="72" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="70" priority="49">
+    <cfRule type="expression" dxfId="71" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="69" priority="48">
+    <cfRule type="expression" dxfId="70" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="68" priority="47">
+    <cfRule type="expression" dxfId="69" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="67" priority="46">
+    <cfRule type="expression" dxfId="68" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92:K93">
-    <cfRule type="expression" dxfId="66" priority="44">
+    <cfRule type="expression" dxfId="67" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="65" priority="45">
+    <cfRule type="expression" dxfId="66" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="64" priority="43">
+    <cfRule type="expression" dxfId="65" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="63" priority="42">
+    <cfRule type="expression" dxfId="64" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="62" priority="41">
+    <cfRule type="expression" dxfId="63" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="61" priority="40">
+    <cfRule type="expression" dxfId="62" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="60" priority="39">
+    <cfRule type="expression" dxfId="61" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="59" priority="38">
+    <cfRule type="expression" dxfId="60" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="58" priority="37">
+    <cfRule type="expression" dxfId="59" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="57" priority="36">
+    <cfRule type="expression" dxfId="58" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="56" priority="35">
+    <cfRule type="expression" dxfId="57" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="55" priority="34">
+    <cfRule type="expression" dxfId="56" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="54" priority="33">
+    <cfRule type="expression" dxfId="55" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="53" priority="32">
+    <cfRule type="expression" dxfId="54" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="52" priority="31">
+    <cfRule type="expression" dxfId="53" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="51" priority="30">
+    <cfRule type="expression" dxfId="52" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="50" priority="29">
+    <cfRule type="expression" dxfId="51" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="50" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="48" priority="26">
+    <cfRule type="expression" dxfId="49" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="48" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="46" priority="24">
+    <cfRule type="expression" dxfId="47" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="45" priority="23">
+    <cfRule type="expression" dxfId="46" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="45" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="43" priority="21">
+    <cfRule type="expression" dxfId="44" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="42" priority="20">
+    <cfRule type="expression" dxfId="43" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="41" priority="19">
+    <cfRule type="expression" dxfId="42" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="40" priority="17">
+    <cfRule type="expression" dxfId="41" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="39" priority="16">
+    <cfRule type="expression" dxfId="40" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="38" priority="15">
+    <cfRule type="expression" dxfId="39" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="38" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="36" priority="12">
+    <cfRule type="expression" dxfId="37" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="35" priority="11">
+    <cfRule type="expression" dxfId="36" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="34" priority="10">
+    <cfRule type="expression" dxfId="35" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="33" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="33" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="31" priority="7">
+    <cfRule type="expression" dxfId="32" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="31" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="29" priority="5">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20027,8 +20038,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE85"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="S159" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="R57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AA18" sqref="AA18"/>
@@ -28234,7 +28245,7 @@
       </c>
       <c r="AA76" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB76" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28343,7 +28354,7 @@
       </c>
       <c r="AA77" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB77" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28452,7 +28463,7 @@
       </c>
       <c r="AA78" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB78" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28561,7 +28572,7 @@
       </c>
       <c r="AA79" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB79" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28670,7 +28681,7 @@
       </c>
       <c r="AA80" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB80" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28779,7 +28790,7 @@
       </c>
       <c r="AA81" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB81" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28888,7 +28899,7 @@
       </c>
       <c r="AA82" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB82" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -28997,7 +29008,7 @@
       </c>
       <c r="AA83" s="13">
         <f t="shared" ca="1" si="59"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB83" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -29106,7 +29117,7 @@
       </c>
       <c r="AA84" s="13">
         <f t="shared" ca="1" si="59"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB84" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -29215,7 +29226,7 @@
       </c>
       <c r="AA85" s="13">
         <f t="shared" ca="1" si="59"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB85" s="15" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -29228,132 +29239,132 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="I22 V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 E3:H3 G4:J6 G7:H10 G11:I16 G22 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 I32 G32:H33 L31:U31 C31:F31 G23:I31 H34:H85 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65">
-    <cfRule type="expression" dxfId="25" priority="146">
+    <cfRule type="expression" dxfId="26" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="24" priority="86">
+    <cfRule type="expression" dxfId="25" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="23" priority="74">
+    <cfRule type="expression" dxfId="24" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="22" priority="72">
+    <cfRule type="expression" dxfId="23" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="21" priority="73">
+    <cfRule type="expression" dxfId="22" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="20" priority="71">
+    <cfRule type="expression" dxfId="21" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="19" priority="68">
+    <cfRule type="expression" dxfId="20" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I10">
-    <cfRule type="expression" dxfId="18" priority="62">
+    <cfRule type="expression" dxfId="19" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J44">
-    <cfRule type="expression" dxfId="17" priority="53">
+    <cfRule type="expression" dxfId="18" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J10">
-    <cfRule type="expression" dxfId="16" priority="52">
+    <cfRule type="expression" dxfId="17" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="15" priority="32">
+    <cfRule type="expression" dxfId="16" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:G85">
-    <cfRule type="expression" dxfId="14" priority="28">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="13" priority="27">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="12" priority="25">
+    <cfRule type="expression" dxfId="13" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="11" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="10" priority="21">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="9" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="8" priority="17">
+    <cfRule type="expression" dxfId="9" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:I21 L17:T21">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="8" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:L3 K4:K85">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated LeaderTelecom limited offer end. Legends on the second page.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="48220" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3080" yWindow="10400" windowWidth="38320" windowHeight="15140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2160,10 +2160,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of May 2017.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2176,10 +2172,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of May 2017.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>For individuals from educational or public organisations. Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2349,6 +2341,14 @@
   </si>
   <si>
     <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of July 2017.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of July 2017.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -5109,29 +5109,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="153">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="151">
     <dxf>
       <font>
         <color auto="1"/>
@@ -7091,10 +7069,10 @@
   <dimension ref="A1:FJ158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="P11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AH77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="AK96" sqref="AK96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9523,7 +9501,7 @@
     <row r="34" spans="1:166">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>356</v>
@@ -9701,7 +9679,7 @@
     <row r="36" spans="1:166" s="12" customFormat="1">
       <c r="A36" s="15"/>
       <c r="B36" s="21" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>363</v>
@@ -10455,10 +10433,10 @@
         <v>327</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D47">
         <v>8</v>
@@ -10622,7 +10600,7 @@
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AO48" s="31"/>
       <c r="AP48" s="31"/>
@@ -10836,7 +10814,7 @@
         <v>128</v>
       </c>
       <c r="AK49" s="15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="51" spans="1:37" s="12" customFormat="1">
@@ -11896,7 +11874,7 @@
     </row>
     <row r="67" spans="1:166">
       <c r="B67" s="21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>32</v>
@@ -11983,7 +11961,7 @@
     <row r="68" spans="1:166" s="12" customFormat="1">
       <c r="A68" s="2"/>
       <c r="B68" s="21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>32</v>
@@ -14394,7 +14372,7 @@
       <c r="AI89" s="26"/>
       <c r="AJ89" s="26"/>
       <c r="AK89" s="15" t="s">
-        <v>374</v>
+        <v>420</v>
       </c>
       <c r="AL89" s="13"/>
       <c r="AM89" s="13"/>
@@ -14492,7 +14470,7 @@
         <v>137</v>
       </c>
       <c r="AK90" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AL90" s="13"/>
       <c r="AM90" s="13"/>
@@ -14590,7 +14568,7 @@
         <v>137</v>
       </c>
       <c r="AK91" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AL91" s="13"/>
       <c r="AM91" s="13"/>
@@ -14690,7 +14668,7 @@
       <c r="AI92" s="26"/>
       <c r="AJ92" s="26"/>
       <c r="AK92" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AL92" s="13"/>
       <c r="AM92" s="13"/>
@@ -14790,7 +14768,7 @@
       <c r="AI93" s="26"/>
       <c r="AJ93" s="26"/>
       <c r="AK93" s="15" t="s">
-        <v>378</v>
+        <v>421</v>
       </c>
       <c r="AL93" s="13"/>
       <c r="AM93" s="13"/>
@@ -15149,7 +15127,7 @@
         <v>6912</v>
       </c>
       <c r="AK100" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AL100" s="13"/>
       <c r="AM100" s="13"/>
@@ -15250,7 +15228,7 @@
         <v>13824</v>
       </c>
       <c r="AK101" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AL101" s="13"/>
       <c r="AM101" s="13"/>
@@ -15349,7 +15327,7 @@
         <v>8640</v>
       </c>
       <c r="AK102" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AL102" s="13"/>
       <c r="AM102" s="13"/>
@@ -15448,7 +15426,7 @@
         <v>8640</v>
       </c>
       <c r="AK103" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AL103" s="13"/>
       <c r="AM103" s="13"/>
@@ -15548,7 +15526,7 @@
       </c>
       <c r="AJ104" s="13"/>
       <c r="AK104" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AL104" s="13"/>
       <c r="AM104" s="13"/>
@@ -15647,7 +15625,7 @@
         <v>8640</v>
       </c>
       <c r="AK105" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AL105" s="13"/>
       <c r="AM105" s="13"/>
@@ -16028,7 +16006,7 @@
       </c>
       <c r="J114" s="5"/>
       <c r="K114" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L114" s="5">
         <v>0.5</v>
@@ -16082,7 +16060,7 @@
         <v>149</v>
       </c>
       <c r="AK114" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AL114" s="13"/>
       <c r="AM114" s="13"/>
@@ -16097,7 +16075,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D115" s="5">
         <v>1</v>
@@ -16119,7 +16097,7 @@
       </c>
       <c r="J115" s="5"/>
       <c r="K115" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L115" s="5">
         <v>1</v>
@@ -16185,7 +16163,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D116" s="5">
         <v>2</v>
@@ -16207,7 +16185,7 @@
       </c>
       <c r="J116" s="5"/>
       <c r="K116" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L116" s="5">
         <v>2</v>
@@ -16271,7 +16249,7 @@
         <v>148</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D117" s="5">
         <v>2</v>
@@ -16293,7 +16271,7 @@
       </c>
       <c r="J117" s="5"/>
       <c r="K117" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L117" s="5">
         <v>2</v>
@@ -16352,7 +16330,7 @@
         <v>149</v>
       </c>
       <c r="AK117" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AL117" s="13"/>
       <c r="AM117" s="13"/>
@@ -16365,7 +16343,7 @@
         <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D118" s="5">
         <v>1</v>
@@ -16387,7 +16365,7 @@
       </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L118" s="5">
         <v>0.5</v>
@@ -16445,10 +16423,10 @@
     <row r="119" spans="1:41">
       <c r="A119" s="21"/>
       <c r="B119" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D119" s="5">
         <v>2</v>
@@ -16470,7 +16448,7 @@
       </c>
       <c r="J119" s="5"/>
       <c r="K119" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L119" s="5">
         <v>1</v>
@@ -16528,10 +16506,10 @@
     <row r="120" spans="1:41">
       <c r="A120" s="21"/>
       <c r="B120" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D120" s="5">
         <v>4</v>
@@ -16553,7 +16531,7 @@
       </c>
       <c r="J120" s="5"/>
       <c r="K120" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L120" s="5">
         <v>2</v>
@@ -16956,10 +16934,10 @@
         <v>201</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D129" s="5">
         <v>0.5</v>
@@ -17031,10 +17009,10 @@
         <v>202</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D130" s="5">
         <v>1</v>
@@ -17106,10 +17084,10 @@
         <v>203</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D131" s="5">
         <v>2</v>
@@ -17179,10 +17157,10 @@
     <row r="132" spans="1:41" ht="20" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D132" s="5">
         <v>2</v>
@@ -17252,10 +17230,10 @@
     <row r="133" spans="1:41" ht="20" customHeight="1">
       <c r="A133" s="21"/>
       <c r="B133" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D133" s="5">
         <v>4</v>
@@ -17607,7 +17585,7 @@
         <v>253</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>256</v>
@@ -17682,10 +17660,10 @@
       </c>
       <c r="AG141" s="13"/>
       <c r="AH141" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AK141" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AL141" s="13"/>
       <c r="AM141" s="13"/>
@@ -17697,7 +17675,7 @@
         <v>254</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>255</v>
@@ -17772,10 +17750,10 @@
       </c>
       <c r="AG142" s="13"/>
       <c r="AH142" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="AK142" s="15" t="s">
         <v>385</v>
-      </c>
-      <c r="AK142" s="15" t="s">
-        <v>387</v>
       </c>
       <c r="AL142" s="13"/>
       <c r="AM142" s="13"/>
@@ -18133,7 +18111,7 @@
         <v>2.5</v>
       </c>
       <c r="AK148" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL148" s="13"/>
       <c r="AM148" s="13"/>
@@ -18329,7 +18307,7 @@
         <v>2.5</v>
       </c>
       <c r="AK150" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL150" s="13"/>
       <c r="AM150" s="13"/>
@@ -18527,7 +18505,7 @@
         <v>2.5</v>
       </c>
       <c r="AK152" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL152" s="13"/>
       <c r="AM152" s="13"/>
@@ -18723,7 +18701,7 @@
         <v>2.5</v>
       </c>
       <c r="AK154" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL154" s="13"/>
       <c r="AM154" s="13"/>
@@ -18919,7 +18897,7 @@
         <v>2.5</v>
       </c>
       <c r="AK156" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL156" s="13"/>
       <c r="AM156" s="13"/>
@@ -19058,17 +19036,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 AH32:AJ32 A11:Q21 AL32:XFD33 A32:AC32 C33:AJ33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72">
-    <cfRule type="expression" dxfId="152" priority="235">
+    <cfRule type="expression" dxfId="150" priority="235">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="151" priority="222">
+    <cfRule type="expression" dxfId="149" priority="222">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="150" priority="211">
+    <cfRule type="expression" dxfId="148" priority="211">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19157,7 +19135,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="149" priority="203">
+    <cfRule type="expression" dxfId="147" priority="203">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19246,152 +19224,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="148" priority="200">
+    <cfRule type="expression" dxfId="146" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="147" priority="199">
+    <cfRule type="expression" dxfId="145" priority="199">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="146" priority="177">
+    <cfRule type="expression" dxfId="144" priority="177">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="145" priority="175">
+    <cfRule type="expression" dxfId="143" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="144" priority="174">
+    <cfRule type="expression" dxfId="142" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="143" priority="173">
+    <cfRule type="expression" dxfId="141" priority="173">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="142" priority="160">
+    <cfRule type="expression" dxfId="140" priority="160">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="141" priority="162">
+    <cfRule type="expression" dxfId="139" priority="162">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="140" priority="97">
+    <cfRule type="expression" dxfId="138" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="139" priority="128">
+    <cfRule type="expression" dxfId="137" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="138" priority="127">
+    <cfRule type="expression" dxfId="136" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="137" priority="126">
+    <cfRule type="expression" dxfId="135" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="136" priority="125">
+    <cfRule type="expression" dxfId="134" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="135" priority="124">
+    <cfRule type="expression" dxfId="133" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="134" priority="123">
+    <cfRule type="expression" dxfId="132" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="133" priority="122">
+    <cfRule type="expression" dxfId="131" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="132" priority="121">
+    <cfRule type="expression" dxfId="130" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="131" priority="120">
+    <cfRule type="expression" dxfId="129" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="130" priority="119">
+    <cfRule type="expression" dxfId="128" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="129" priority="118">
+    <cfRule type="expression" dxfId="127" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="128" priority="117">
+    <cfRule type="expression" dxfId="126" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="127" priority="116">
+    <cfRule type="expression" dxfId="125" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="126" priority="113">
+    <cfRule type="expression" dxfId="124" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="125" priority="115">
+    <cfRule type="expression" dxfId="123" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="124" priority="114">
+    <cfRule type="expression" dxfId="122" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="123" priority="112">
+    <cfRule type="expression" dxfId="121" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="122" priority="111">
+    <cfRule type="expression" dxfId="120" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="121" priority="110">
+    <cfRule type="expression" dxfId="119" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="120" priority="109">
+    <cfRule type="expression" dxfId="118" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="119" priority="108">
+    <cfRule type="expression" dxfId="117" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19480,97 +19458,97 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="118" priority="107">
+    <cfRule type="expression" dxfId="116" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="117" priority="106">
+    <cfRule type="expression" dxfId="115" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="116" priority="105">
+    <cfRule type="expression" dxfId="114" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="115" priority="104">
+    <cfRule type="expression" dxfId="113" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="114" priority="103">
+    <cfRule type="expression" dxfId="112" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="113" priority="102">
+    <cfRule type="expression" dxfId="111" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="112" priority="101">
+    <cfRule type="expression" dxfId="110" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="111" priority="100">
+    <cfRule type="expression" dxfId="109" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="110" priority="99">
+    <cfRule type="expression" dxfId="108" priority="99">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="109" priority="60">
+    <cfRule type="expression" dxfId="107" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="108" priority="96">
+    <cfRule type="expression" dxfId="106" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="107" priority="95">
+    <cfRule type="expression" dxfId="105" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="106" priority="94">
+    <cfRule type="expression" dxfId="104" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="105" priority="93">
+    <cfRule type="expression" dxfId="103" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="104" priority="92">
+    <cfRule type="expression" dxfId="102" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE35:AH36">
-    <cfRule type="expression" dxfId="103" priority="91">
+    <cfRule type="expression" dxfId="101" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="102" priority="90">
+    <cfRule type="expression" dxfId="100" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="101" priority="89">
+    <cfRule type="expression" dxfId="99" priority="89">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="100" priority="85">
+    <cfRule type="expression" dxfId="98" priority="85">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19611,7 +19589,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="99" priority="80">
+    <cfRule type="expression" dxfId="97" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19664,362 +19642,362 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="98" priority="79">
+    <cfRule type="expression" dxfId="96" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="97" priority="78">
+    <cfRule type="expression" dxfId="95" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="96" priority="77">
+    <cfRule type="expression" dxfId="94" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="95" priority="76">
+    <cfRule type="expression" dxfId="93" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="94" priority="75">
+    <cfRule type="expression" dxfId="92" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="93" priority="74">
+    <cfRule type="expression" dxfId="91" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="92" priority="73">
+    <cfRule type="expression" dxfId="90" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="91" priority="72">
+    <cfRule type="expression" dxfId="89" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="90" priority="68">
+    <cfRule type="expression" dxfId="88" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="89" priority="70">
+    <cfRule type="expression" dxfId="87" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="88" priority="69">
+    <cfRule type="expression" dxfId="86" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="87" priority="67">
+    <cfRule type="expression" dxfId="85" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="86" priority="66">
+    <cfRule type="expression" dxfId="84" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="85" priority="64">
+    <cfRule type="expression" dxfId="83" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="84" priority="63">
+    <cfRule type="expression" dxfId="82" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="83" priority="62">
+    <cfRule type="expression" dxfId="81" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="82" priority="61">
+    <cfRule type="expression" dxfId="80" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="81" priority="59">
+    <cfRule type="expression" dxfId="79" priority="59">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="80" priority="57">
+    <cfRule type="expression" dxfId="78" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="79" priority="56">
+    <cfRule type="expression" dxfId="77" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="78" priority="54">
+    <cfRule type="expression" dxfId="76" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="77" priority="53">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="76" priority="52">
+    <cfRule type="expression" dxfId="74" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="75" priority="14">
+    <cfRule type="expression" dxfId="73" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="74" priority="3">
+    <cfRule type="expression" dxfId="72" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="expression" dxfId="73" priority="50">
+    <cfRule type="expression" dxfId="71" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="72" priority="51">
+    <cfRule type="expression" dxfId="70" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="71" priority="49">
+    <cfRule type="expression" dxfId="69" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="70" priority="48">
+    <cfRule type="expression" dxfId="68" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="69" priority="47">
+    <cfRule type="expression" dxfId="67" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="68" priority="46">
+    <cfRule type="expression" dxfId="66" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92:K93">
-    <cfRule type="expression" dxfId="67" priority="44">
+    <cfRule type="expression" dxfId="65" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="66" priority="45">
+    <cfRule type="expression" dxfId="64" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="65" priority="43">
+    <cfRule type="expression" dxfId="63" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="64" priority="42">
+    <cfRule type="expression" dxfId="62" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="63" priority="41">
+    <cfRule type="expression" dxfId="61" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="62" priority="40">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="61" priority="39">
+    <cfRule type="expression" dxfId="59" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="60" priority="38">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="59" priority="37">
+    <cfRule type="expression" dxfId="57" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="58" priority="36">
+    <cfRule type="expression" dxfId="56" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="57" priority="35">
+    <cfRule type="expression" dxfId="55" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="56" priority="34">
+    <cfRule type="expression" dxfId="54" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="55" priority="33">
+    <cfRule type="expression" dxfId="53" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="54" priority="32">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="53" priority="31">
+    <cfRule type="expression" dxfId="51" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="52" priority="30">
+    <cfRule type="expression" dxfId="50" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="51" priority="29">
+    <cfRule type="expression" dxfId="49" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="50" priority="27">
+    <cfRule type="expression" dxfId="48" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="49" priority="26">
+    <cfRule type="expression" dxfId="47" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="48" priority="25">
+    <cfRule type="expression" dxfId="46" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="47" priority="24">
+    <cfRule type="expression" dxfId="45" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="46" priority="23">
+    <cfRule type="expression" dxfId="44" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="45" priority="22">
+    <cfRule type="expression" dxfId="43" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="44" priority="21">
+    <cfRule type="expression" dxfId="42" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="43" priority="20">
+    <cfRule type="expression" dxfId="41" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="42" priority="19">
+    <cfRule type="expression" dxfId="40" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="41" priority="17">
+    <cfRule type="expression" dxfId="39" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="40" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="39" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="38" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="37" priority="12">
+    <cfRule type="expression" dxfId="35" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="36" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="33" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="34" priority="9">
+    <cfRule type="expression" dxfId="32" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="33" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="32" priority="7">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="31" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="28" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20043,7 +20021,7 @@
   <dimension ref="A1:AE85"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
@@ -23451,7 +23429,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23559,7 +23537,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F33" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23776,7 +23754,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23884,7 +23862,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23992,7 +23970,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25555,7 +25533,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F51" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25647,7 +25625,7 @@
       </c>
       <c r="AB51" s="15" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of May 2017.</v>
+        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of July 2017.</v>
       </c>
       <c r="AC51" s="33">
         <v>89</v>
@@ -25671,7 +25649,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F52" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25779,7 +25757,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F53" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25887,7 +25865,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F54" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25999,7 +25977,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F55" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26091,7 +26069,7 @@
       </c>
       <c r="AB55" s="15" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of May 2017.</v>
+        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of July 2017.</v>
       </c>
       <c r="AC55" s="33">
         <v>93</v>
@@ -29396,127 +29374,127 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="26" priority="146">
+    <cfRule type="expression" dxfId="24" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="25" priority="86">
+    <cfRule type="expression" dxfId="23" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="24" priority="74">
+    <cfRule type="expression" dxfId="22" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="23" priority="72">
+    <cfRule type="expression" dxfId="21" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="22" priority="73">
+    <cfRule type="expression" dxfId="20" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="21" priority="71">
+    <cfRule type="expression" dxfId="19" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="20" priority="68">
+    <cfRule type="expression" dxfId="18" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="19" priority="62">
+    <cfRule type="expression" dxfId="17" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="18" priority="53">
+    <cfRule type="expression" dxfId="16" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="17" priority="52">
+    <cfRule type="expression" dxfId="15" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="16" priority="32">
+    <cfRule type="expression" dxfId="14" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="15" priority="28">
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="14" priority="27">
+    <cfRule type="expression" dxfId="12" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="10" priority="19">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Minor corrections to LeaderTelecom offer notes.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -2344,11 +2344,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of July 2017.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of July 2017.</t>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of August 2017.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of August 2017.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -7072,7 +7072,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="AH77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AK96" sqref="AK96"/>
+      <selection pane="bottomRight" activeCell="AI92" sqref="AI92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -20021,7 +20021,7 @@
   <dimension ref="A1:AE85"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="Z39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
@@ -25625,7 +25625,7 @@
       </c>
       <c r="AB51" s="15" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of July 2017.</v>
+        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of August 2017.</v>
       </c>
       <c r="AC51" s="33">
         <v>89</v>
@@ -26069,7 +26069,7 @@
       </c>
       <c r="AB55" s="15" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of July 2017.</v>
+        <v>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of August 2017.</v>
       </c>
       <c r="AC55" s="33">
         <v>93</v>

</xml_diff>

<commit_message>
IBM HDD RAID added.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="10400" windowWidth="38320" windowHeight="15140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25260" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="424">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1941,414 +1941,422 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No Internet traffic included.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/store/orderHourlyBareMetalInstance/178087/171?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1495792638&amp;cm_mc_sid_52640000=1495792638</t>
+  </si>
+  <si>
+    <t>P100 E5-2650v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60 E5-2620v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60 E5-2690v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/store/orderHourlyBareMetalInstance/178055/177?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1495792638&amp;cm_mc_sid_52640000=1495792638</t>
+  </si>
+  <si>
+    <t>www.nimbix.net/nimbix-cloud-demand-pricing</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.nimbix.net/blog/2016/10/04/ibm-nvidia-powerful-gpu-cloud/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Interconnect Gbps</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Internet Gbps</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60 E5-2620v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 160</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2620 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SATA</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47059,168829,2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47057,168829,2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>M60 E5-2650v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2650 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/553/176647,168829?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 160</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2xM60 E5-2620v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2xM60 E5-2690v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/553/178055,168829?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 160</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 2496</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 2496</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/orderHourlyBareMetalInstance/178087/153?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>2xK80 E5-2620v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K80 E5-2690v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47057%2C46480%2C2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>Grid K2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 1536</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/orderHourlyBareMetalInstance/178055/157?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>Grid K2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/141695%2C2739?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
+  </si>
+  <si>
+    <t>Grid K2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 1536</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x 4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/141695%2C47061%2C279?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251#category-disk0-title</t>
+  </si>
+  <si>
+    <t>AL</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec5/dedicated-hosts/pricing/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec6/dedicated-hosts/pricing/</t>
+  </si>
+  <si>
+    <t>P100 E5-2620v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K2 E5-2620v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Limited quantity available at this price</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,12 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,13 &amp;euro;/Gb.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>For individuals from educational or public organisations. Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>For groups from educational or public organisations. Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>For groups from educational or public organisations. Included 8640 node hours. Must pass review prior to usage. 4320 node hours if a parallel job used more nodes than applied for.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>RDMA capable</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JPY</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV12</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NV24</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>6c39m1g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>12c78m2g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>24c156m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>32c208m4g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>64c416m8g</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GPU.7XL P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GPU.7XL M40</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2690 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K80</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon E5-2690 v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K80</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M60</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K80</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2xK2 E5-2690v4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>K2 E5-2690v3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x8 x86</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P6000x8 x86</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P40x4 x86</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2-GPU POWER8/8 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x8</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT P100x2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080x4 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080Tix2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LT GTX1080Tix4 ltd.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR K80x8 x86</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR M40x8 x86</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>NG08</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>P100</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Provider web site mentions 32 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU, thus 0.5 CPUs.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Provider web site mentions 128 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU, thus 2 CPUs. </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of August 2017.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of August 2017.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>2xP100 E5-2690v4</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>SSD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>1TB of Internet traffic included.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>No Internet traffic included.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/store/orderHourlyBareMetalInstance/178087/171?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1495792638&amp;cm_mc_sid_52640000=1495792638</t>
-  </si>
-  <si>
-    <t>P100 E5-2650v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60 E5-2620v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60 E5-2690v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/store/orderHourlyBareMetalInstance/178055/177?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1495792638&amp;cm_mc_sid_52640000=1495792638</t>
-  </si>
-  <si>
-    <t>www.nimbix.net/nimbix-cloud-demand-pricing</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.nimbix.net/blog/2016/10/04/ibm-nvidia-powerful-gpu-cloud/</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Interconnect Gbps</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Internet Gbps</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60 E5-2620v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 160</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2620 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SATA</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47059,168829,2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47057,168829,2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>M60 E5-2650v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2650 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/553/176647,168829?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 160</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2xM60 E5-2620v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2xM60 E5-2690v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/553/178055,168829?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 160</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 2496</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 2496</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/orderHourlyBareMetalInstance/178087/153?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>2xK80 E5-2620v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K80 E5-2690v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/47057%2C46480%2C2397?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>Grid K2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 1536</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/orderHourlyBareMetalInstance/178055/157?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>Grid K2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/141695%2C2739?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251</t>
-  </si>
-  <si>
-    <t>Grid K2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 1536</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2 x 4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://www.softlayer.com/cloud-computing/bluemix/Store/configureOrder/251/141695%2C47061%2C279?language=en&amp;cm_mc_uid=85839695048713933876447&amp;cm_mc_sid_50200000=1496127251&amp;cm_mc_sid_52640000=1496127251#category-disk0-title</t>
-  </si>
-  <si>
-    <t>AL</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec5/dedicated-hosts/pricing/</t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/ec6/dedicated-hosts/pricing/</t>
-  </si>
-  <si>
-    <t>P100 E5-2620v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K2 E5-2620v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Limited quantity available at this price</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,11 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,12 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,13 &amp;euro;/Gb.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>For individuals from educational or public organisations. Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>For groups from educational or public organisations. Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>For groups from educational or public organisations. Included 8640 node hours. Must pass review prior to usage. 4320 node hours if a parallel job used more nodes than applied for.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1 GPU in specification is 1/2 of K80 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>RDMA capable</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>JPY</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NV12</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NV24</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>6c39m1g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>12c78m2g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>24c156m4g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>32c208m4g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>64c416m8g</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GPU.7XL P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>GPU.7XL M40</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2690 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K80</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon E5-2690 v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K80</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>M60</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K80</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>2xK2 E5-2690v4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>K2 E5-2690v3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P100x8 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P6000x8 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR P40x4 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">2-GPU POWER8/8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT P100x2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080x4 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080Tix2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>LT GTX1080Tix4 ltd.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR K80x8 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>CR M40x8 x86</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>NG08</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>P100</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Provider web site mentions 32 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU, thus 0.5 CPUs.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Provider web site mentions 128 threads, and Wikipedia says each core has 8 thread, while 1 CPU has 8 cores. That gives 64 threads per 1 CPU, thus 2 CPUs. </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of August 2017.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,14 &amp;euro;/Gb. Special price till end of August 2017.</t>
+    <t xml:space="preserve">SATA RAID1 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SATA RAID1</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2691,7 +2699,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1155">
+  <cellStyleXfs count="1157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3526,6 +3534,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3952,7 +3962,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1155">
+  <cellStyles count="1157">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -4597,6 +4607,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1156" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -5098,6 +5109,7 @@
     <cellStyle name="Hyperlink" xfId="1149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1155" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -5109,7 +5121,29 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="151">
+  <dxfs count="153">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -7068,11 +7102,11 @@
   </sheetPr>
   <dimension ref="A1:FJ158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AH77" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI92" sqref="AI92"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7384,10 +7418,10 @@
         <v>9</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="Z4" s="16" t="s">
         <v>134</v>
@@ -7836,7 +7870,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -7845,7 +7879,7 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>226</v>
@@ -7910,7 +7944,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -7919,7 +7953,7 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>226</v>
@@ -7974,7 +8008,7 @@
         <v>130</v>
       </c>
       <c r="AL11" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:166">
@@ -7989,7 +8023,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F12" s="5">
         <v>8.74</v>
@@ -7998,7 +8032,7 @@
         <v>2.91</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>227</v>
@@ -8048,7 +8082,7 @@
         <v>128</v>
       </c>
       <c r="AL12" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:166" s="12" customFormat="1">
@@ -8451,7 +8485,7 @@
         <v>307</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>303</v>
@@ -8547,7 +8581,7 @@
         <v>308</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>303</v>
@@ -8641,13 +8675,13 @@
     <row r="25" spans="1:38">
       <c r="A25" s="15"/>
       <c r="B25" s="21" t="s">
-        <v>316</v>
+        <v>420</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>303</v>
       </c>
       <c r="D25" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="13">
         <v>3584</v>
@@ -8694,7 +8728,7 @@
         <v>128</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U25" s="5">
         <v>960</v>
@@ -8726,7 +8760,7 @@
         <v>128</v>
       </c>
       <c r="AK25" s="15" t="s">
-        <v>318</v>
+        <v>421</v>
       </c>
       <c r="AL25" s="15" t="s">
         <v>312</v>
@@ -8735,10 +8769,10 @@
     <row r="26" spans="1:38" s="12" customFormat="1">
       <c r="A26" s="15"/>
       <c r="B26" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -8794,7 +8828,7 @@
         <v>1000</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>313</v>
+        <v>422</v>
       </c>
       <c r="W26" s="5">
         <v>1000</v>
@@ -8826,19 +8860,19 @@
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
       <c r="AK26" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AL26" s="15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="12" customFormat="1">
       <c r="A27" s="15"/>
       <c r="B27" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -8894,7 +8928,7 @@
         <v>4000</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>313</v>
+        <v>423</v>
       </c>
       <c r="W27" s="5">
         <v>4000</v>
@@ -8926,19 +8960,19 @@
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
       <c r="AK27" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AL27" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="12" customFormat="1">
       <c r="A28" s="15"/>
       <c r="B28" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -8953,14 +8987,14 @@
         <v>0.3</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L28" s="5">
         <v>2</v>
@@ -8988,7 +9022,7 @@
         <v>64</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="U28" s="5">
         <v>1000</v>
@@ -9023,16 +9057,16 @@
         <v>315</v>
       </c>
       <c r="AL28" s="15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:38" s="12" customFormat="1">
       <c r="A29" s="15"/>
       <c r="B29" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -9047,14 +9081,14 @@
         <v>0.3</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -9082,7 +9116,7 @@
         <v>64</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="U29" s="5">
         <v>1000</v>
@@ -9117,16 +9151,16 @@
         <v>315</v>
       </c>
       <c r="AL29" s="15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:38" s="12" customFormat="1">
       <c r="A30" s="15"/>
       <c r="B30" s="21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D30" s="5">
         <v>2</v>
@@ -9141,10 +9175,10 @@
         <v>0.3</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="5" t="s">
@@ -9176,7 +9210,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U30" s="5">
         <v>960</v>
@@ -9211,16 +9245,16 @@
         <v>315</v>
       </c>
       <c r="AL30" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" s="15"/>
       <c r="B31" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="26" t="s">
         <v>345</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>347</v>
       </c>
       <c r="D31" s="5">
         <v>2</v>
@@ -9235,10 +9269,10 @@
         <v>0.3</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5" t="s">
@@ -9270,7 +9304,7 @@
         <v>256</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U31" s="5">
         <v>960</v>
@@ -9303,13 +9337,13 @@
         <v>315</v>
       </c>
       <c r="AL31" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="12" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="21" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>26</v>
@@ -9391,23 +9425,23 @@
       <c r="AD32" s="23"/>
       <c r="AE32" s="10"/>
       <c r="AF32" s="10"/>
-      <c r="AG32" s="10"/>
+      <c r="AG32" s="23"/>
       <c r="AH32" s="15" t="s">
         <v>128</v>
       </c>
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
       <c r="AK32" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AL32" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:166" s="12" customFormat="1">
       <c r="A33" s="15"/>
       <c r="B33" s="21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>48</v>
@@ -9495,22 +9529,22 @@
         <v>315</v>
       </c>
       <c r="AL33" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:166">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D34" s="13">
         <v>2</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F34" s="13">
         <f>2*2.28864</f>
@@ -9518,7 +9552,7 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -9575,29 +9609,30 @@
       <c r="AB34" s="23">
         <v>3.9590000000000001</v>
       </c>
+      <c r="AG34" s="23"/>
       <c r="AH34" s="15" t="s">
         <v>128</v>
       </c>
       <c r="AK34" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AL34" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:166">
       <c r="A35" s="15"/>
       <c r="B35" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F35" s="5">
         <f>2*2.28864</f>
@@ -9605,12 +9640,12 @@
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L35" s="5">
         <v>2</v>
@@ -9638,7 +9673,7 @@
         <v>64</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="U35" s="5">
         <v>1000</v>
@@ -9671,7 +9706,7 @@
         <v>315</v>
       </c>
       <c r="AL35" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AO35" s="12"/>
       <c r="AP35" s="12"/>
@@ -9679,16 +9714,16 @@
     <row r="36" spans="1:166" s="12" customFormat="1">
       <c r="A36" s="15"/>
       <c r="B36" s="21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F36" s="5">
         <f>2*2.28864</f>
@@ -9696,7 +9731,7 @@
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -9764,7 +9799,7 @@
         <v>315</v>
       </c>
       <c r="AL36" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:166" s="12" customFormat="1">
@@ -10126,7 +10161,7 @@
     </row>
     <row r="45" spans="1:166" s="12" customFormat="1">
       <c r="A45" s="15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>41</v>
@@ -10430,13 +10465,13 @@
     </row>
     <row r="47" spans="1:166">
       <c r="A47" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D47">
         <v>8</v>
@@ -10600,7 +10635,7 @@
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="15" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AO48" s="31"/>
       <c r="AP48" s="31"/>
@@ -10814,7 +10849,7 @@
         <v>128</v>
       </c>
       <c r="AK49" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="51" spans="1:37" s="12" customFormat="1">
@@ -11156,7 +11191,7 @@
         <v>128</v>
       </c>
       <c r="AK58" s="15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:37">
@@ -11246,7 +11281,7 @@
         <v>128</v>
       </c>
       <c r="AK59" s="15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="1:37" s="12" customFormat="1">
@@ -11874,7 +11909,7 @@
     </row>
     <row r="67" spans="1:166">
       <c r="B67" s="21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>32</v>
@@ -11961,7 +11996,7 @@
     <row r="68" spans="1:166" s="12" customFormat="1">
       <c r="A68" s="2"/>
       <c r="B68" s="21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>32</v>
@@ -14270,7 +14305,7 @@
       <c r="AI88" s="26"/>
       <c r="AJ88" s="26"/>
       <c r="AK88" s="15" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="AL88" s="13"/>
       <c r="AM88" s="13"/>
@@ -14372,7 +14407,7 @@
       <c r="AI89" s="26"/>
       <c r="AJ89" s="26"/>
       <c r="AK89" s="15" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="AL89" s="13"/>
       <c r="AM89" s="13"/>
@@ -14470,7 +14505,7 @@
         <v>137</v>
       </c>
       <c r="AK90" s="15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AL90" s="13"/>
       <c r="AM90" s="13"/>
@@ -14568,7 +14603,7 @@
         <v>137</v>
       </c>
       <c r="AK91" s="15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AL91" s="13"/>
       <c r="AM91" s="13"/>
@@ -14668,7 +14703,7 @@
       <c r="AI92" s="26"/>
       <c r="AJ92" s="26"/>
       <c r="AK92" s="15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AL92" s="13"/>
       <c r="AM92" s="13"/>
@@ -14768,7 +14803,7 @@
       <c r="AI93" s="26"/>
       <c r="AJ93" s="26"/>
       <c r="AK93" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL93" s="13"/>
       <c r="AM93" s="13"/>
@@ -15127,7 +15162,7 @@
         <v>6912</v>
       </c>
       <c r="AK100" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AL100" s="13"/>
       <c r="AM100" s="13"/>
@@ -15228,7 +15263,7 @@
         <v>13824</v>
       </c>
       <c r="AK101" s="15" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AL101" s="13"/>
       <c r="AM101" s="13"/>
@@ -15327,7 +15362,7 @@
         <v>8640</v>
       </c>
       <c r="AK102" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AL102" s="13"/>
       <c r="AM102" s="13"/>
@@ -15426,7 +15461,7 @@
         <v>8640</v>
       </c>
       <c r="AK103" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AL103" s="13"/>
       <c r="AM103" s="13"/>
@@ -15526,7 +15561,7 @@
       </c>
       <c r="AJ104" s="13"/>
       <c r="AK104" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AL104" s="13"/>
       <c r="AM104" s="13"/>
@@ -15625,7 +15660,7 @@
         <v>8640</v>
       </c>
       <c r="AK105" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AL105" s="13"/>
       <c r="AM105" s="13"/>
@@ -16006,7 +16041,7 @@
       </c>
       <c r="J114" s="5"/>
       <c r="K114" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L114" s="5">
         <v>0.5</v>
@@ -16060,7 +16095,7 @@
         <v>149</v>
       </c>
       <c r="AK114" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="AL114" s="13"/>
       <c r="AM114" s="13"/>
@@ -16075,7 +16110,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D115" s="5">
         <v>1</v>
@@ -16097,7 +16132,7 @@
       </c>
       <c r="J115" s="5"/>
       <c r="K115" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L115" s="5">
         <v>1</v>
@@ -16163,7 +16198,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D116" s="5">
         <v>2</v>
@@ -16185,7 +16220,7 @@
       </c>
       <c r="J116" s="5"/>
       <c r="K116" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L116" s="5">
         <v>2</v>
@@ -16249,7 +16284,7 @@
         <v>148</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D117" s="5">
         <v>2</v>
@@ -16271,7 +16306,7 @@
       </c>
       <c r="J117" s="5"/>
       <c r="K117" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L117" s="5">
         <v>2</v>
@@ -16330,7 +16365,7 @@
         <v>149</v>
       </c>
       <c r="AK117" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="AL117" s="13"/>
       <c r="AM117" s="13"/>
@@ -16343,7 +16378,7 @@
         <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D118" s="5">
         <v>1</v>
@@ -16365,7 +16400,7 @@
       </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L118" s="5">
         <v>0.5</v>
@@ -16423,10 +16458,10 @@
     <row r="119" spans="1:41">
       <c r="A119" s="21"/>
       <c r="B119" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D119" s="5">
         <v>2</v>
@@ -16448,7 +16483,7 @@
       </c>
       <c r="J119" s="5"/>
       <c r="K119" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L119" s="5">
         <v>1</v>
@@ -16506,10 +16541,10 @@
     <row r="120" spans="1:41">
       <c r="A120" s="21"/>
       <c r="B120" s="21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D120" s="5">
         <v>4</v>
@@ -16531,7 +16566,7 @@
       </c>
       <c r="J120" s="5"/>
       <c r="K120" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L120" s="5">
         <v>2</v>
@@ -16934,10 +16969,10 @@
         <v>201</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D129" s="5">
         <v>0.5</v>
@@ -17009,10 +17044,10 @@
         <v>202</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D130" s="5">
         <v>1</v>
@@ -17084,10 +17119,10 @@
         <v>203</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D131" s="5">
         <v>2</v>
@@ -17157,10 +17192,10 @@
     <row r="132" spans="1:41" ht="20" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" s="21" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D132" s="5">
         <v>2</v>
@@ -17230,10 +17265,10 @@
     <row r="133" spans="1:41" ht="20" customHeight="1">
       <c r="A133" s="21"/>
       <c r="B133" s="21" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D133" s="5">
         <v>4</v>
@@ -17585,7 +17620,7 @@
         <v>253</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>256</v>
@@ -17660,10 +17695,10 @@
       </c>
       <c r="AG141" s="13"/>
       <c r="AH141" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="AK141" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AL141" s="13"/>
       <c r="AM141" s="13"/>
@@ -17675,7 +17710,7 @@
         <v>254</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>255</v>
@@ -17750,10 +17785,10 @@
       </c>
       <c r="AG142" s="13"/>
       <c r="AH142" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="AK142" s="15" t="s">
         <v>383</v>
-      </c>
-      <c r="AK142" s="15" t="s">
-        <v>385</v>
       </c>
       <c r="AL142" s="13"/>
       <c r="AM142" s="13"/>
@@ -18111,7 +18146,7 @@
         <v>2.5</v>
       </c>
       <c r="AK148" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL148" s="13"/>
       <c r="AM148" s="13"/>
@@ -18307,7 +18342,7 @@
         <v>2.5</v>
       </c>
       <c r="AK150" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL150" s="13"/>
       <c r="AM150" s="13"/>
@@ -18505,7 +18540,7 @@
         <v>2.5</v>
       </c>
       <c r="AK152" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL152" s="13"/>
       <c r="AM152" s="13"/>
@@ -18701,7 +18736,7 @@
         <v>2.5</v>
       </c>
       <c r="AK154" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL154" s="13"/>
       <c r="AM154" s="13"/>
@@ -18897,7 +18932,7 @@
         <v>2.5</v>
       </c>
       <c r="AK156" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL156" s="13"/>
       <c r="AM156" s="13"/>
@@ -18964,7 +18999,7 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AL77:AL79">
-    <cfRule type="colorScale" priority="249">
+    <cfRule type="colorScale" priority="250">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18976,7 +19011,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM77:AM79">
-    <cfRule type="colorScale" priority="248">
+    <cfRule type="colorScale" priority="249">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18988,7 +19023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL80:AL87">
-    <cfRule type="colorScale" priority="244">
+    <cfRule type="colorScale" priority="245">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19000,7 +19035,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM80:AM87">
-    <cfRule type="colorScale" priority="243">
+    <cfRule type="colorScale" priority="244">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19012,7 +19047,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL80:AL87">
-    <cfRule type="colorScale" priority="242">
+    <cfRule type="colorScale" priority="243">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19024,7 +19059,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM80:AM87">
-    <cfRule type="colorScale" priority="241">
+    <cfRule type="colorScale" priority="242">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19035,23 +19070,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 AH32:AJ32 A11:Q21 AL32:XFD33 A32:AC32 C33:AJ33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72">
-    <cfRule type="expression" dxfId="150" priority="235">
+  <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72 AH32:AJ33">
+    <cfRule type="expression" dxfId="152" priority="236">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="149" priority="222">
+    <cfRule type="expression" dxfId="151" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="148" priority="211">
+    <cfRule type="expression" dxfId="150" priority="212">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48">
-    <cfRule type="colorScale" priority="212">
+    <cfRule type="colorScale" priority="213">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19063,7 +19098,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="213">
+    <cfRule type="colorScale" priority="214">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19075,7 +19110,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48">
-    <cfRule type="colorScale" priority="214">
+    <cfRule type="colorScale" priority="215">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19087,7 +19122,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="215">
+    <cfRule type="colorScale" priority="216">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19099,7 +19134,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN48">
-    <cfRule type="colorScale" priority="216">
+    <cfRule type="colorScale" priority="217">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19111,7 +19146,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48">
-    <cfRule type="colorScale" priority="217">
+    <cfRule type="colorScale" priority="218">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19123,7 +19158,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="218">
+    <cfRule type="colorScale" priority="219">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19135,12 +19170,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="147" priority="203">
+    <cfRule type="expression" dxfId="149" priority="204">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="204">
+    <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19152,7 +19187,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="205">
+    <cfRule type="colorScale" priority="206">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19164,7 +19199,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="206">
+    <cfRule type="colorScale" priority="207">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19176,7 +19211,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="207">
+    <cfRule type="colorScale" priority="208">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19188,7 +19223,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN46">
-    <cfRule type="colorScale" priority="208">
+    <cfRule type="colorScale" priority="209">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19200,7 +19235,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="209">
+    <cfRule type="colorScale" priority="210">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19212,7 +19247,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="210">
+    <cfRule type="colorScale" priority="211">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19224,157 +19259,157 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="146" priority="200">
+    <cfRule type="expression" dxfId="148" priority="201">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="145" priority="199">
+    <cfRule type="expression" dxfId="147" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="144" priority="177">
+    <cfRule type="expression" dxfId="146" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="143" priority="175">
+    <cfRule type="expression" dxfId="145" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="142" priority="174">
+    <cfRule type="expression" dxfId="144" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="141" priority="173">
+    <cfRule type="expression" dxfId="143" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="140" priority="160">
+    <cfRule type="expression" dxfId="142" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="139" priority="162">
+    <cfRule type="expression" dxfId="141" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="138" priority="97">
+    <cfRule type="expression" dxfId="140" priority="98">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="137" priority="128">
+    <cfRule type="expression" dxfId="139" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="136" priority="127">
+    <cfRule type="expression" dxfId="138" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="135" priority="126">
+    <cfRule type="expression" dxfId="137" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="134" priority="125">
+    <cfRule type="expression" dxfId="136" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="133" priority="124">
+    <cfRule type="expression" dxfId="135" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="132" priority="123">
+    <cfRule type="expression" dxfId="134" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="131" priority="122">
+    <cfRule type="expression" dxfId="133" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="130" priority="121">
+    <cfRule type="expression" dxfId="132" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="129" priority="120">
+    <cfRule type="expression" dxfId="131" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="128" priority="119">
+    <cfRule type="expression" dxfId="130" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="127" priority="118">
+    <cfRule type="expression" dxfId="129" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="126" priority="117">
+    <cfRule type="expression" dxfId="128" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
+    <cfRule type="expression" dxfId="127" priority="117">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T30:U31">
+    <cfRule type="expression" dxfId="126" priority="114">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK28:AK31">
     <cfRule type="expression" dxfId="125" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="124" priority="113">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="123" priority="115">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="122" priority="114">
+    <cfRule type="expression" dxfId="124" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="121" priority="112">
+    <cfRule type="expression" dxfId="123" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="120" priority="111">
+    <cfRule type="expression" dxfId="122" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="119" priority="110">
+    <cfRule type="expression" dxfId="121" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="118" priority="109">
+    <cfRule type="expression" dxfId="120" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="117" priority="108">
+    <cfRule type="expression" dxfId="119" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL87 AL47">
-    <cfRule type="colorScale" priority="418">
+    <cfRule type="colorScale" priority="419">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19386,7 +19421,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM87 AM47">
-    <cfRule type="colorScale" priority="423">
+    <cfRule type="colorScale" priority="424">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19398,7 +19433,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL79 AL47">
-    <cfRule type="colorScale" priority="429">
+    <cfRule type="colorScale" priority="430">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19410,7 +19445,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM79 AM47">
-    <cfRule type="colorScale" priority="434">
+    <cfRule type="colorScale" priority="435">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19422,7 +19457,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN5:AN30 AN37:AN45 AN32:AN33 AN49 AN51:AN87 AN47">
-    <cfRule type="colorScale" priority="440">
+    <cfRule type="colorScale" priority="441">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19434,7 +19469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL76 AL47">
-    <cfRule type="colorScale" priority="446">
+    <cfRule type="colorScale" priority="447">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19446,7 +19481,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM76 AM47">
-    <cfRule type="colorScale" priority="450">
+    <cfRule type="colorScale" priority="451">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19458,110 +19493,98 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="116" priority="107">
+    <cfRule type="expression" dxfId="118" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="115" priority="106">
+    <cfRule type="expression" dxfId="117" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="114" priority="105">
+    <cfRule type="expression" dxfId="116" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="113" priority="104">
+    <cfRule type="expression" dxfId="115" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="112" priority="103">
+    <cfRule type="expression" dxfId="114" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="111" priority="102">
+    <cfRule type="expression" dxfId="113" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="110" priority="101">
+    <cfRule type="expression" dxfId="112" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="109" priority="100">
+    <cfRule type="expression" dxfId="111" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="108" priority="99">
+    <cfRule type="expression" dxfId="110" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="107" priority="60">
+    <cfRule type="expression" dxfId="109" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="106" priority="96">
+    <cfRule type="expression" dxfId="108" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="105" priority="95">
+    <cfRule type="expression" dxfId="107" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="104" priority="94">
+    <cfRule type="expression" dxfId="106" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="103" priority="93">
+    <cfRule type="expression" dxfId="105" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="102" priority="92">
+    <cfRule type="expression" dxfId="104" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE35:AH36">
-    <cfRule type="expression" dxfId="101" priority="91">
+  <conditionalFormatting sqref="AE36:AH36 AE35:AF35 AH35">
+    <cfRule type="expression" dxfId="103" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="100" priority="90">
+    <cfRule type="expression" dxfId="102" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="99" priority="89">
+    <cfRule type="expression" dxfId="101" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="98" priority="85">
+    <cfRule type="expression" dxfId="100" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
@@ -19588,21 +19611,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="97" priority="80">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AM36">
-    <cfRule type="colorScale" priority="81">
+  <conditionalFormatting sqref="AL35:AL36">
+    <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
+    <cfRule type="expression" dxfId="99" priority="81">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AM36">
@@ -19617,8 +19640,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AM35:AM36">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AN35:AN36">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19630,7 +19665,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AM36">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19642,362 +19677,367 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="96" priority="79">
+    <cfRule type="expression" dxfId="98" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="95" priority="78">
+    <cfRule type="expression" dxfId="97" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="94" priority="77">
+    <cfRule type="expression" dxfId="96" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="93" priority="76">
+    <cfRule type="expression" dxfId="95" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="92" priority="75">
+    <cfRule type="expression" dxfId="94" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="91" priority="74">
+    <cfRule type="expression" dxfId="93" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="90" priority="73">
+    <cfRule type="expression" dxfId="92" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="89" priority="72">
+    <cfRule type="expression" dxfId="91" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="88" priority="68">
+    <cfRule type="expression" dxfId="90" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="87" priority="70">
+    <cfRule type="expression" dxfId="89" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="86" priority="69">
+    <cfRule type="expression" dxfId="88" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="85" priority="67">
+    <cfRule type="expression" dxfId="87" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="84" priority="66">
+    <cfRule type="expression" dxfId="86" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="83" priority="64">
+    <cfRule type="expression" dxfId="85" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="82" priority="63">
+    <cfRule type="expression" dxfId="84" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="81" priority="62">
+    <cfRule type="expression" dxfId="83" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="80" priority="61">
+    <cfRule type="expression" dxfId="82" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="79" priority="59">
+    <cfRule type="expression" dxfId="81" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="78" priority="57">
+    <cfRule type="expression" dxfId="80" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="77" priority="56">
+    <cfRule type="expression" dxfId="79" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="76" priority="54">
+    <cfRule type="expression" dxfId="78" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="75" priority="53">
+    <cfRule type="expression" dxfId="77" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="74" priority="52">
+    <cfRule type="expression" dxfId="76" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="73" priority="14">
+    <cfRule type="expression" dxfId="75" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="72" priority="3">
+    <cfRule type="expression" dxfId="74" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
+    <cfRule type="expression" dxfId="73" priority="51">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L88:R89">
+    <cfRule type="expression" dxfId="72" priority="52">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C89">
     <cfRule type="expression" dxfId="71" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="70" priority="51">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="69" priority="49">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="68" priority="48">
+    <cfRule type="expression" dxfId="70" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="67" priority="47">
+    <cfRule type="expression" dxfId="69" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
+    <cfRule type="expression" dxfId="68" priority="47">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K92:K93">
+    <cfRule type="expression" dxfId="67" priority="45">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L92:R93">
     <cfRule type="expression" dxfId="66" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K92:K93">
+  <conditionalFormatting sqref="C92:C93">
     <cfRule type="expression" dxfId="65" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="64" priority="45">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="63" priority="43">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="62" priority="42">
+    <cfRule type="expression" dxfId="64" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="61" priority="41">
+    <cfRule type="expression" dxfId="63" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="60" priority="40">
+    <cfRule type="expression" dxfId="62" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="59" priority="39">
+    <cfRule type="expression" dxfId="61" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="58" priority="38">
+    <cfRule type="expression" dxfId="60" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="57" priority="37">
+    <cfRule type="expression" dxfId="59" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="56" priority="36">
+    <cfRule type="expression" dxfId="58" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="55" priority="35">
+    <cfRule type="expression" dxfId="57" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="54" priority="34">
+    <cfRule type="expression" dxfId="56" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="53" priority="33">
+    <cfRule type="expression" dxfId="55" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="52" priority="32">
+    <cfRule type="expression" dxfId="54" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="51" priority="31">
+    <cfRule type="expression" dxfId="53" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="50" priority="30">
+    <cfRule type="expression" dxfId="52" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="49" priority="29">
+    <cfRule type="expression" dxfId="51" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="48" priority="27">
+    <cfRule type="expression" dxfId="50" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="47" priority="26">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="46" priority="25">
+    <cfRule type="expression" dxfId="48" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="45" priority="24">
+    <cfRule type="expression" dxfId="47" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="44" priority="23">
+    <cfRule type="expression" dxfId="46" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="43" priority="22">
+    <cfRule type="expression" dxfId="45" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="42" priority="21">
+    <cfRule type="expression" dxfId="44" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="41" priority="20">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="40" priority="19">
+    <cfRule type="expression" dxfId="42" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="39" priority="17">
+    <cfRule type="expression" dxfId="41" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="40" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="37" priority="15">
+    <cfRule type="expression" dxfId="39" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="35" priority="12">
+    <cfRule type="expression" dxfId="37" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="36" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="35" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="34" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="33" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="32" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="27" priority="4">
+    <cfRule type="expression" dxfId="29" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="27" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG32:AG35">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20020,8 +20060,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE85"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="Z39" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="Z22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
@@ -20062,7 +20102,7 @@
         <v>111</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="36" t="s">
@@ -21359,7 +21399,7 @@
       </c>
       <c r="O13" s="13">
         <f t="shared" ca="1" si="13"/>
-        <v>19</v>
+        <v>9.5</v>
       </c>
       <c r="P13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -21367,7 +21407,7 @@
       </c>
       <c r="Q13" s="13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -21508,7 +21548,7 @@
       </c>
       <c r="W14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>SATA</v>
+        <v>SATA RAID1</v>
       </c>
       <c r="X14" s="13">
         <f t="shared" ca="1" si="4"/>
@@ -23429,7 +23469,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23537,7 +23577,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F33" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23754,7 +23794,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23862,7 +23902,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23970,7 +24010,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25533,7 +25573,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F51" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25649,7 +25689,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F52" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25757,7 +25797,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F53" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25865,7 +25905,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F54" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25977,7 +26017,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F55" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -29374,127 +29414,127 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="24" priority="146">
+    <cfRule type="expression" dxfId="26" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="23" priority="86">
+    <cfRule type="expression" dxfId="25" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="22" priority="74">
+    <cfRule type="expression" dxfId="24" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="21" priority="72">
+    <cfRule type="expression" dxfId="23" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="20" priority="73">
+    <cfRule type="expression" dxfId="22" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="19" priority="71">
+    <cfRule type="expression" dxfId="21" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="18" priority="68">
+    <cfRule type="expression" dxfId="20" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="17" priority="62">
+    <cfRule type="expression" dxfId="19" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="16" priority="53">
+    <cfRule type="expression" dxfId="18" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="15" priority="52">
+    <cfRule type="expression" dxfId="17" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="14" priority="32">
+    <cfRule type="expression" dxfId="16" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="13" priority="28">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="13" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="9" priority="21">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Note about max job run time for Tsubame2.5.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25260" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="500" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1859,10 +1859,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Reedbush-H dedicated reviewed (educational)</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2332,10 +2328,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>InternetIncluded  traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb. Special price till end of August 2017.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2357,6 +2349,14 @@
   </si>
   <si>
     <t>SATA RAID1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -5121,7 +5121,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="152">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5129,18 +5129,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5415,7 +5404,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7103,10 +7092,10 @@
   <dimension ref="A1:FJ158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="Q130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="AK156" sqref="AK156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7220,7 +7209,7 @@
         <v>30</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AM3" s="12"/>
       <c r="AN3" s="12"/>
@@ -7418,10 +7407,10 @@
         <v>9</v>
       </c>
       <c r="X4" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y4" s="16" t="s">
         <v>326</v>
-      </c>
-      <c r="Y4" s="16" t="s">
-        <v>327</v>
       </c>
       <c r="Z4" s="16" t="s">
         <v>134</v>
@@ -7436,7 +7425,7 @@
         <v>142</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AE4" s="16" t="s">
         <v>143</v>
@@ -7870,7 +7859,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -7879,7 +7868,7 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>226</v>
@@ -7944,7 +7933,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -7953,7 +7942,7 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>226</v>
@@ -8008,7 +7997,7 @@
         <v>130</v>
       </c>
       <c r="AL11" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:166">
@@ -8023,7 +8012,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F12" s="5">
         <v>8.74</v>
@@ -8032,7 +8021,7 @@
         <v>2.91</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>227</v>
@@ -8082,7 +8071,7 @@
         <v>128</v>
       </c>
       <c r="AL12" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:166" s="12" customFormat="1">
@@ -8482,13 +8471,13 @@
     </row>
     <row r="23" spans="1:38" ht="20">
       <c r="A23" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -8510,7 +8499,7 @@
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L23" s="5">
         <v>2</v>
@@ -8538,7 +8527,7 @@
         <v>64</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U23" s="5">
         <v>1000</v>
@@ -8570,21 +8559,21 @@
         <v>128</v>
       </c>
       <c r="AK23" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL23" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -8606,7 +8595,7 @@
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L24" s="5">
         <v>2</v>
@@ -8634,7 +8623,7 @@
         <v>64</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U24" s="5">
         <v>1000</v>
@@ -8666,19 +8655,19 @@
         <v>128</v>
       </c>
       <c r="AK24" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL24" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="15"/>
       <c r="B25" s="21" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -8700,7 +8689,7 @@
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L25" s="5">
         <v>2</v>
@@ -8728,7 +8717,7 @@
         <v>128</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U25" s="5">
         <v>960</v>
@@ -8760,19 +8749,19 @@
         <v>128</v>
       </c>
       <c r="AK25" s="15" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="AL25" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:38" s="12" customFormat="1">
       <c r="A26" s="15"/>
       <c r="B26" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -8794,7 +8783,7 @@
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L26" s="5">
         <v>2</v>
@@ -8822,13 +8811,13 @@
         <v>128</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U26" s="5">
         <v>1000</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="W26" s="5">
         <v>1000</v>
@@ -8860,19 +8849,19 @@
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
       <c r="AK26" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="AL26" s="15" t="s">
         <v>318</v>
-      </c>
-      <c r="AL26" s="15" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="12" customFormat="1">
       <c r="A27" s="15"/>
       <c r="B27" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -8894,7 +8883,7 @@
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L27" s="5">
         <v>2</v>
@@ -8922,13 +8911,13 @@
         <v>256</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U27" s="5">
         <v>4000</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="W27" s="5">
         <v>4000</v>
@@ -8960,19 +8949,19 @@
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
       <c r="AK27" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AL27" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="12" customFormat="1">
       <c r="A28" s="15"/>
       <c r="B28" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>328</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>329</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -8987,14 +8976,14 @@
         <v>0.3</v>
       </c>
       <c r="H28" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="I28" s="7" t="s">
         <v>330</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L28" s="5">
         <v>2</v>
@@ -9022,7 +9011,7 @@
         <v>64</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U28" s="5">
         <v>1000</v>
@@ -9054,19 +9043,19 @@
       <c r="AI28" s="13"/>
       <c r="AJ28" s="13"/>
       <c r="AK28" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL28" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:38" s="12" customFormat="1">
       <c r="A29" s="15"/>
       <c r="B29" s="21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -9081,14 +9070,14 @@
         <v>0.3</v>
       </c>
       <c r="H29" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>330</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>331</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -9116,7 +9105,7 @@
         <v>64</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U29" s="5">
         <v>1000</v>
@@ -9148,19 +9137,19 @@
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
       <c r="AK29" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL29" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:38" s="12" customFormat="1">
       <c r="A30" s="15"/>
       <c r="B30" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D30" s="5">
         <v>2</v>
@@ -9175,14 +9164,14 @@
         <v>0.3</v>
       </c>
       <c r="H30" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I30" s="7" t="s">
         <v>340</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>341</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L30" s="5">
         <v>2</v>
@@ -9210,7 +9199,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U30" s="5">
         <v>960</v>
@@ -9242,19 +9231,19 @@
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
       <c r="AK30" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL30" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" s="15"/>
       <c r="B31" s="21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D31" s="5">
         <v>2</v>
@@ -9269,14 +9258,14 @@
         <v>0.3</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L31" s="5">
         <v>2</v>
@@ -9304,7 +9293,7 @@
         <v>256</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="U31" s="5">
         <v>960</v>
@@ -9334,16 +9323,16 @@
         <v>128</v>
       </c>
       <c r="AK31" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL31" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="12" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>26</v>
@@ -9432,16 +9421,16 @@
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
       <c r="AK32" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AL32" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:166" s="12" customFormat="1">
       <c r="A33" s="15"/>
       <c r="B33" s="21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>48</v>
@@ -9526,25 +9515,25 @@
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
       <c r="AK33" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL33" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34" spans="1:166">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D34" s="13">
         <v>2</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F34" s="13">
         <f>2*2.28864</f>
@@ -9552,12 +9541,12 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L34" s="5">
         <v>2</v>
@@ -9585,13 +9574,13 @@
         <v>128</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U34" s="5">
         <v>4000</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="W34" s="5">
         <v>4000</v>
@@ -9614,25 +9603,25 @@
         <v>128</v>
       </c>
       <c r="AK34" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AL34" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="35" spans="1:166">
       <c r="A35" s="15"/>
       <c r="B35" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F35" s="5">
         <f>2*2.28864</f>
@@ -9640,12 +9629,12 @@
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L35" s="5">
         <v>2</v>
@@ -9673,7 +9662,7 @@
         <v>64</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U35" s="5">
         <v>1000</v>
@@ -9703,10 +9692,10 @@
         <v>128</v>
       </c>
       <c r="AK35" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL35" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AO35" s="12"/>
       <c r="AP35" s="12"/>
@@ -9714,16 +9703,16 @@
     <row r="36" spans="1:166" s="12" customFormat="1">
       <c r="A36" s="15"/>
       <c r="B36" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F36" s="5">
         <f>2*2.28864</f>
@@ -9731,7 +9720,7 @@
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -9796,10 +9785,10 @@
       <c r="AI36" s="13"/>
       <c r="AJ36" s="13"/>
       <c r="AK36" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AL36" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="37" spans="1:166" s="12" customFormat="1">
@@ -10161,7 +10150,7 @@
     </row>
     <row r="45" spans="1:166" s="12" customFormat="1">
       <c r="A45" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>41</v>
@@ -10465,13 +10454,13 @@
     </row>
     <row r="47" spans="1:166">
       <c r="A47" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C47" s="26" t="s">
         <v>413</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>414</v>
       </c>
       <c r="D47">
         <v>8</v>
@@ -10635,7 +10624,7 @@
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AO48" s="31"/>
       <c r="AP48" s="31"/>
@@ -10849,7 +10838,7 @@
         <v>128</v>
       </c>
       <c r="AK49" s="15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="51" spans="1:37" s="12" customFormat="1">
@@ -11191,7 +11180,7 @@
         <v>128</v>
       </c>
       <c r="AK58" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:37">
@@ -11281,7 +11270,7 @@
         <v>128</v>
       </c>
       <c r="AK59" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="60" spans="1:37" s="12" customFormat="1">
@@ -11909,7 +11898,7 @@
     </row>
     <row r="67" spans="1:166">
       <c r="B67" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>32</v>
@@ -11996,7 +11985,7 @@
     <row r="68" spans="1:166" s="12" customFormat="1">
       <c r="A68" s="2"/>
       <c r="B68" s="21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>32</v>
@@ -14305,7 +14294,7 @@
       <c r="AI88" s="26"/>
       <c r="AJ88" s="26"/>
       <c r="AK88" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AL88" s="13"/>
       <c r="AM88" s="13"/>
@@ -14407,7 +14396,7 @@
       <c r="AI89" s="26"/>
       <c r="AJ89" s="26"/>
       <c r="AK89" s="15" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AL89" s="13"/>
       <c r="AM89" s="13"/>
@@ -14505,7 +14494,7 @@
         <v>137</v>
       </c>
       <c r="AK90" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AL90" s="13"/>
       <c r="AM90" s="13"/>
@@ -14603,7 +14592,7 @@
         <v>137</v>
       </c>
       <c r="AK91" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AL91" s="13"/>
       <c r="AM91" s="13"/>
@@ -14613,10 +14602,10 @@
     <row r="92" spans="1:41" s="12" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="C92" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="D92" s="5">
         <v>2</v>
@@ -14703,7 +14692,7 @@
       <c r="AI92" s="26"/>
       <c r="AJ92" s="26"/>
       <c r="AK92" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AL92" s="13"/>
       <c r="AM92" s="13"/>
@@ -14713,10 +14702,10 @@
     <row r="93" spans="1:41" s="12" customFormat="1">
       <c r="A93" s="21"/>
       <c r="B93" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D93" s="5">
         <v>4</v>
@@ -14803,7 +14792,7 @@
       <c r="AI93" s="26"/>
       <c r="AJ93" s="26"/>
       <c r="AK93" s="15" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL93" s="13"/>
       <c r="AM93" s="13"/>
@@ -15073,7 +15062,7 @@
         <v>138</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>139</v>
@@ -15162,7 +15151,7 @@
         <v>6912</v>
       </c>
       <c r="AK100" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AL100" s="13"/>
       <c r="AM100" s="13"/>
@@ -15263,7 +15252,7 @@
         <v>13824</v>
       </c>
       <c r="AK101" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AL101" s="13"/>
       <c r="AM101" s="13"/>
@@ -15362,7 +15351,7 @@
         <v>8640</v>
       </c>
       <c r="AK102" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AL102" s="13"/>
       <c r="AM102" s="13"/>
@@ -15461,7 +15450,7 @@
         <v>8640</v>
       </c>
       <c r="AK103" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AL103" s="13"/>
       <c r="AM103" s="13"/>
@@ -15471,7 +15460,7 @@
     <row r="104" spans="1:41" s="12" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>139</v>
@@ -15561,7 +15550,7 @@
       </c>
       <c r="AJ104" s="13"/>
       <c r="AK104" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AL104" s="13"/>
       <c r="AM104" s="13"/>
@@ -15571,7 +15560,7 @@
     <row r="105" spans="1:41">
       <c r="A105" s="21"/>
       <c r="B105" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>139</v>
@@ -15660,7 +15649,7 @@
         <v>8640</v>
       </c>
       <c r="AK105" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AL105" s="13"/>
       <c r="AM105" s="13"/>
@@ -16041,7 +16030,7 @@
       </c>
       <c r="J114" s="5"/>
       <c r="K114" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L114" s="5">
         <v>0.5</v>
@@ -16095,7 +16084,7 @@
         <v>149</v>
       </c>
       <c r="AK114" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AL114" s="13"/>
       <c r="AM114" s="13"/>
@@ -16110,7 +16099,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D115" s="5">
         <v>1</v>
@@ -16132,7 +16121,7 @@
       </c>
       <c r="J115" s="5"/>
       <c r="K115" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L115" s="5">
         <v>1</v>
@@ -16198,7 +16187,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D116" s="5">
         <v>2</v>
@@ -16220,7 +16209,7 @@
       </c>
       <c r="J116" s="5"/>
       <c r="K116" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L116" s="5">
         <v>2</v>
@@ -16284,7 +16273,7 @@
         <v>148</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D117" s="5">
         <v>2</v>
@@ -16306,7 +16295,7 @@
       </c>
       <c r="J117" s="5"/>
       <c r="K117" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L117" s="5">
         <v>2</v>
@@ -16365,7 +16354,7 @@
         <v>149</v>
       </c>
       <c r="AK117" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AL117" s="13"/>
       <c r="AM117" s="13"/>
@@ -16378,7 +16367,7 @@
         <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D118" s="5">
         <v>1</v>
@@ -16400,7 +16389,7 @@
       </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L118" s="5">
         <v>0.5</v>
@@ -16458,10 +16447,10 @@
     <row r="119" spans="1:41">
       <c r="A119" s="21"/>
       <c r="B119" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D119" s="5">
         <v>2</v>
@@ -16483,7 +16472,7 @@
       </c>
       <c r="J119" s="5"/>
       <c r="K119" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L119" s="5">
         <v>1</v>
@@ -16541,10 +16530,10 @@
     <row r="120" spans="1:41">
       <c r="A120" s="21"/>
       <c r="B120" s="21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D120" s="5">
         <v>4</v>
@@ -16566,7 +16555,7 @@
       </c>
       <c r="J120" s="5"/>
       <c r="K120" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L120" s="5">
         <v>2</v>
@@ -16969,10 +16958,10 @@
         <v>201</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D129" s="5">
         <v>0.5</v>
@@ -17044,10 +17033,10 @@
         <v>202</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D130" s="5">
         <v>1</v>
@@ -17119,10 +17108,10 @@
         <v>203</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D131" s="5">
         <v>2</v>
@@ -17192,10 +17181,10 @@
     <row r="132" spans="1:41" ht="20" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D132" s="5">
         <v>2</v>
@@ -17265,10 +17254,10 @@
     <row r="133" spans="1:41" ht="20" customHeight="1">
       <c r="A133" s="21"/>
       <c r="B133" s="21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D133" s="5">
         <v>4</v>
@@ -17620,7 +17609,7 @@
         <v>253</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>256</v>
@@ -17695,10 +17684,10 @@
       </c>
       <c r="AG141" s="13"/>
       <c r="AH141" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="AK141" s="15" t="s">
         <v>381</v>
-      </c>
-      <c r="AK141" s="15" t="s">
-        <v>382</v>
       </c>
       <c r="AL141" s="13"/>
       <c r="AM141" s="13"/>
@@ -17710,7 +17699,7 @@
         <v>254</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>255</v>
@@ -17785,10 +17774,10 @@
       </c>
       <c r="AG142" s="13"/>
       <c r="AH142" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AK142" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AL142" s="13"/>
       <c r="AM142" s="13"/>
@@ -18047,7 +18036,7 @@
         <v>2.5</v>
       </c>
       <c r="AK147" s="15" t="s">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="AL147" s="13"/>
       <c r="AM147" s="13"/>
@@ -18146,7 +18135,7 @@
         <v>2.5</v>
       </c>
       <c r="AK148" s="15" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AL148" s="13"/>
       <c r="AM148" s="13"/>
@@ -18244,7 +18233,7 @@
         <v>2.5</v>
       </c>
       <c r="AK149" s="15" t="s">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="AL149" s="13"/>
       <c r="AM149" s="13"/>
@@ -18342,7 +18331,7 @@
         <v>2.5</v>
       </c>
       <c r="AK150" s="15" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AL150" s="13"/>
       <c r="AM150" s="13"/>
@@ -18441,7 +18430,7 @@
         <v>2.5</v>
       </c>
       <c r="AK151" s="15" t="s">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="AL151" s="13"/>
       <c r="AM151" s="13"/>
@@ -18540,7 +18529,7 @@
         <v>2.5</v>
       </c>
       <c r="AK152" s="15" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AL152" s="13"/>
       <c r="AM152" s="13"/>
@@ -18638,7 +18627,7 @@
         <v>2.5</v>
       </c>
       <c r="AK153" s="15" t="s">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="AL153" s="13"/>
       <c r="AM153" s="13"/>
@@ -18736,7 +18725,7 @@
         <v>2.5</v>
       </c>
       <c r="AK154" s="15" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AL154" s="13"/>
       <c r="AM154" s="13"/>
@@ -18746,7 +18735,7 @@
     <row r="155" spans="1:41">
       <c r="A155" s="21"/>
       <c r="B155" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C155" s="5" t="s">
         <v>284</v>
@@ -18834,7 +18823,7 @@
         <v>2.5</v>
       </c>
       <c r="AK155" s="15" t="s">
-        <v>294</v>
+        <v>422</v>
       </c>
       <c r="AL155" s="13"/>
       <c r="AM155" s="13"/>
@@ -18844,7 +18833,7 @@
     <row r="156" spans="1:41">
       <c r="A156" s="21"/>
       <c r="B156" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>284</v>
@@ -18932,7 +18921,7 @@
         <v>2.5</v>
       </c>
       <c r="AK156" s="15" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AL156" s="13"/>
       <c r="AM156" s="13"/>
@@ -19071,17 +19060,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72 AH32:AJ33">
-    <cfRule type="expression" dxfId="152" priority="236">
+    <cfRule type="expression" dxfId="151" priority="236">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="151" priority="223">
+    <cfRule type="expression" dxfId="150" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="150" priority="212">
+    <cfRule type="expression" dxfId="149" priority="212">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19170,7 +19159,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="149" priority="204">
+    <cfRule type="expression" dxfId="148" priority="204">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19259,152 +19248,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="148" priority="201">
+    <cfRule type="expression" dxfId="147" priority="201">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="147" priority="200">
+    <cfRule type="expression" dxfId="146" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="146" priority="178">
+    <cfRule type="expression" dxfId="145" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="145" priority="176">
+    <cfRule type="expression" dxfId="144" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="144" priority="175">
+    <cfRule type="expression" dxfId="143" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="143" priority="174">
+    <cfRule type="expression" dxfId="142" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="142" priority="161">
+    <cfRule type="expression" dxfId="141" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="141" priority="163">
+    <cfRule type="expression" dxfId="140" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="140" priority="98">
+    <cfRule type="expression" dxfId="139" priority="98">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="139" priority="129">
+    <cfRule type="expression" dxfId="138" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="138" priority="128">
+    <cfRule type="expression" dxfId="137" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="137" priority="127">
+    <cfRule type="expression" dxfId="136" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="136" priority="126">
+    <cfRule type="expression" dxfId="135" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="135" priority="125">
+    <cfRule type="expression" dxfId="134" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="134" priority="124">
+    <cfRule type="expression" dxfId="133" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="133" priority="123">
+    <cfRule type="expression" dxfId="132" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="132" priority="122">
+    <cfRule type="expression" dxfId="131" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="131" priority="121">
+    <cfRule type="expression" dxfId="130" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="130" priority="120">
+    <cfRule type="expression" dxfId="129" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="129" priority="119">
+    <cfRule type="expression" dxfId="128" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="128" priority="118">
+    <cfRule type="expression" dxfId="127" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="127" priority="117">
+    <cfRule type="expression" dxfId="126" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="126" priority="114">
+    <cfRule type="expression" dxfId="125" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="125" priority="116">
+    <cfRule type="expression" dxfId="124" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="124" priority="115">
+    <cfRule type="expression" dxfId="123" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="123" priority="113">
+    <cfRule type="expression" dxfId="122" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="122" priority="112">
+    <cfRule type="expression" dxfId="121" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="121" priority="111">
+    <cfRule type="expression" dxfId="120" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="120" priority="110">
+    <cfRule type="expression" dxfId="119" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="119" priority="109">
+    <cfRule type="expression" dxfId="118" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19493,97 +19482,97 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="118" priority="108">
+    <cfRule type="expression" dxfId="117" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="117" priority="107">
+    <cfRule type="expression" dxfId="116" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="116" priority="106">
+    <cfRule type="expression" dxfId="115" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="115" priority="105">
+    <cfRule type="expression" dxfId="114" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="114" priority="104">
+    <cfRule type="expression" dxfId="113" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="113" priority="103">
+    <cfRule type="expression" dxfId="112" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="112" priority="102">
+    <cfRule type="expression" dxfId="111" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="111" priority="101">
+    <cfRule type="expression" dxfId="110" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="110" priority="100">
+    <cfRule type="expression" dxfId="109" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="109" priority="61">
+    <cfRule type="expression" dxfId="108" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="108" priority="97">
+    <cfRule type="expression" dxfId="107" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="107" priority="96">
+    <cfRule type="expression" dxfId="106" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="106" priority="95">
+    <cfRule type="expression" dxfId="105" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="105" priority="94">
+    <cfRule type="expression" dxfId="104" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="104" priority="93">
+    <cfRule type="expression" dxfId="103" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE36:AH36 AE35:AF35 AH35">
-    <cfRule type="expression" dxfId="103" priority="92">
+    <cfRule type="expression" dxfId="102" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="102" priority="91">
+    <cfRule type="expression" dxfId="101" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="101" priority="90">
+    <cfRule type="expression" dxfId="100" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="100" priority="86">
+    <cfRule type="expression" dxfId="99" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19624,7 +19613,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="99" priority="81">
+    <cfRule type="expression" dxfId="98" priority="81">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19677,367 +19666,367 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="98" priority="80">
+    <cfRule type="expression" dxfId="97" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="97" priority="79">
+    <cfRule type="expression" dxfId="96" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="96" priority="78">
+    <cfRule type="expression" dxfId="95" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="95" priority="77">
+    <cfRule type="expression" dxfId="94" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="94" priority="76">
+    <cfRule type="expression" dxfId="93" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="93" priority="75">
+    <cfRule type="expression" dxfId="92" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="92" priority="74">
+    <cfRule type="expression" dxfId="91" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="91" priority="73">
+    <cfRule type="expression" dxfId="90" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="90" priority="69">
+    <cfRule type="expression" dxfId="89" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="89" priority="71">
+    <cfRule type="expression" dxfId="88" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="88" priority="70">
+    <cfRule type="expression" dxfId="87" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="87" priority="68">
+    <cfRule type="expression" dxfId="86" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="86" priority="67">
+    <cfRule type="expression" dxfId="85" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="85" priority="65">
+    <cfRule type="expression" dxfId="84" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="84" priority="64">
+    <cfRule type="expression" dxfId="83" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="83" priority="63">
+    <cfRule type="expression" dxfId="82" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="82" priority="62">
+    <cfRule type="expression" dxfId="81" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="81" priority="60">
+    <cfRule type="expression" dxfId="80" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="80" priority="58">
+    <cfRule type="expression" dxfId="79" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="79" priority="57">
+    <cfRule type="expression" dxfId="78" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="78" priority="55">
+    <cfRule type="expression" dxfId="77" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="77" priority="54">
+    <cfRule type="expression" dxfId="76" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="76" priority="53">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="75" priority="15">
+    <cfRule type="expression" dxfId="74" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="74" priority="4">
+    <cfRule type="expression" dxfId="73" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="expression" dxfId="73" priority="51">
+    <cfRule type="expression" dxfId="72" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="72" priority="52">
+    <cfRule type="expression" dxfId="71" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="71" priority="50">
+    <cfRule type="expression" dxfId="70" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="70" priority="49">
+    <cfRule type="expression" dxfId="69" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="69" priority="48">
+    <cfRule type="expression" dxfId="68" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="68" priority="47">
+    <cfRule type="expression" dxfId="67" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92:K93">
-    <cfRule type="expression" dxfId="67" priority="45">
+    <cfRule type="expression" dxfId="66" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="66" priority="46">
+    <cfRule type="expression" dxfId="65" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="65" priority="44">
+    <cfRule type="expression" dxfId="64" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="64" priority="43">
+    <cfRule type="expression" dxfId="63" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="63" priority="42">
+    <cfRule type="expression" dxfId="62" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="62" priority="41">
+    <cfRule type="expression" dxfId="61" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="61" priority="40">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="60" priority="39">
+    <cfRule type="expression" dxfId="59" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="59" priority="38">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="58" priority="37">
+    <cfRule type="expression" dxfId="57" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="57" priority="36">
+    <cfRule type="expression" dxfId="56" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="56" priority="35">
+    <cfRule type="expression" dxfId="55" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="55" priority="34">
+    <cfRule type="expression" dxfId="54" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="54" priority="33">
+    <cfRule type="expression" dxfId="53" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="53" priority="32">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="52" priority="31">
+    <cfRule type="expression" dxfId="51" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="51" priority="30">
+    <cfRule type="expression" dxfId="50" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="49" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="48" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="48" priority="26">
+    <cfRule type="expression" dxfId="47" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="46" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="46" priority="24">
+    <cfRule type="expression" dxfId="45" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="45" priority="23">
+    <cfRule type="expression" dxfId="44" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="43" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="43" priority="21">
+    <cfRule type="expression" dxfId="42" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="42" priority="20">
+    <cfRule type="expression" dxfId="41" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="41" priority="18">
+    <cfRule type="expression" dxfId="40" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="40" priority="17">
+    <cfRule type="expression" dxfId="39" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="39" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="38" priority="14">
+    <cfRule type="expression" dxfId="37" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="36" priority="12">
+    <cfRule type="expression" dxfId="35" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="35" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="34" priority="10">
+    <cfRule type="expression" dxfId="33" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="33" priority="9">
+    <cfRule type="expression" dxfId="32" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="31" priority="7">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="30" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="29" priority="5">
+    <cfRule type="expression" dxfId="28" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG35">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20102,7 +20091,7 @@
         <v>111</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="36" t="s">
@@ -23469,7 +23458,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23577,7 +23566,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F33" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23794,7 +23783,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23902,7 +23891,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -24010,7 +23999,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25573,7 +25562,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F51" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25689,7 +25678,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F52" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25797,7 +25786,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F53" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25905,7 +25894,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F54" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26017,7 +26006,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F55" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -28424,7 +28413,7 @@
       </c>
       <c r="AB76" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC76" s="33">
         <v>147</v>
@@ -28533,7 +28522,7 @@
       </c>
       <c r="AB77" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC77" s="33">
         <v>148</v>
@@ -28642,7 +28631,7 @@
       </c>
       <c r="AB78" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC78" s="33">
         <v>149</v>
@@ -28751,7 +28740,7 @@
       </c>
       <c r="AB79" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC79" s="33">
         <v>150</v>
@@ -28860,7 +28849,7 @@
       </c>
       <c r="AB80" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC80" s="33">
         <v>151</v>
@@ -28969,7 +28958,7 @@
       </c>
       <c r="AB81" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC81" s="33">
         <v>152</v>
@@ -29078,7 +29067,7 @@
       </c>
       <c r="AB82" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC82" s="33">
         <v>153</v>
@@ -29187,7 +29176,7 @@
       </c>
       <c r="AB83" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC83" s="33">
         <v>154</v>
@@ -29296,7 +29285,7 @@
       </c>
       <c r="AB84" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC84" s="33">
         <v>155</v>
@@ -29405,7 +29394,7 @@
       </c>
       <c r="AB85" s="15" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC85" s="33">
         <v>156</v>
@@ -29414,127 +29403,127 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="26" priority="146">
+    <cfRule type="expression" dxfId="24" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="25" priority="86">
+    <cfRule type="expression" dxfId="23" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="24" priority="74">
+    <cfRule type="expression" dxfId="22" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="23" priority="72">
+    <cfRule type="expression" dxfId="21" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="22" priority="73">
+    <cfRule type="expression" dxfId="20" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="21" priority="71">
+    <cfRule type="expression" dxfId="19" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="20" priority="68">
+    <cfRule type="expression" dxfId="18" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="19" priority="62">
+    <cfRule type="expression" dxfId="17" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="18" priority="53">
+    <cfRule type="expression" dxfId="16" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="17" priority="52">
+    <cfRule type="expression" dxfId="15" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="16" priority="32">
+    <cfRule type="expression" dxfId="14" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="15" priority="28">
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="14" priority="27">
+    <cfRule type="expression" dxfId="12" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="10" priority="19">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed Tsubame2.5 offers which cannot use GPU: L265 and L512.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="500" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="415">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -1800,14 +1800,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>L256</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>L256 open</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>K20</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1820,26 +1812,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>S1070</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4x98.5</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>4x4</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Xeon X7550</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>SSD</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>http://tsubame.gsic.titech.ac.jp/en/paid-services</t>
   </si>
   <si>
@@ -1868,14 +1840,6 @@
   </si>
   <si>
     <t>Reedbush-H dedicated reviewed</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>L512</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>L512 open</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -5121,7 +5085,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="152">
+  <dxfs count="153">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5129,7 +5093,18 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5404,7 +5379,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7092,10 +7067,10 @@
   <dimension ref="A1:FJ158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="Q130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AK156" sqref="AK156"/>
+      <selection pane="bottomRight" activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -7203,13 +7178,13 @@
         <v>158</v>
       </c>
       <c r="AJ3" s="45" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="AM3" s="12"/>
       <c r="AN3" s="12"/>
@@ -7407,10 +7382,10 @@
         <v>9</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="Z4" s="16" t="s">
         <v>134</v>
@@ -7425,7 +7400,7 @@
         <v>142</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="AE4" s="16" t="s">
         <v>143</v>
@@ -7859,7 +7834,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="F10" s="5">
         <v>8.74</v>
@@ -7868,7 +7843,7 @@
         <v>2.91</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>226</v>
@@ -7933,7 +7908,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="F11" s="5">
         <v>8.74</v>
@@ -7942,7 +7917,7 @@
         <v>2.91</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>226</v>
@@ -7997,7 +7972,7 @@
         <v>130</v>
       </c>
       <c r="AL11" s="15" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:166">
@@ -8012,7 +7987,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="F12" s="5">
         <v>8.74</v>
@@ -8021,7 +7996,7 @@
         <v>2.91</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>227</v>
@@ -8071,7 +8046,7 @@
         <v>128</v>
       </c>
       <c r="AL12" s="15" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:166" s="12" customFormat="1">
@@ -8471,13 +8446,13 @@
     </row>
     <row r="23" spans="1:38" ht="20">
       <c r="A23" s="20" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -8499,7 +8474,7 @@
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="5" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="L23" s="5">
         <v>2</v>
@@ -8527,7 +8502,7 @@
         <v>64</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="U23" s="5">
         <v>1000</v>
@@ -8559,21 +8534,21 @@
         <v>128</v>
       </c>
       <c r="AK23" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL23" s="15" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -8595,7 +8570,7 @@
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="5" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="L24" s="5">
         <v>2</v>
@@ -8623,7 +8598,7 @@
         <v>64</v>
       </c>
       <c r="T24" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="U24" s="5">
         <v>1000</v>
@@ -8655,19 +8630,19 @@
         <v>128</v>
       </c>
       <c r="AK24" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL24" s="15" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="15"/>
       <c r="B25" s="21" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -8689,7 +8664,7 @@
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L25" s="5">
         <v>2</v>
@@ -8717,7 +8692,7 @@
         <v>128</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="U25" s="5">
         <v>960</v>
@@ -8749,19 +8724,19 @@
         <v>128</v>
       </c>
       <c r="AK25" s="15" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="AL25" s="15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:38" s="12" customFormat="1">
       <c r="A26" s="15"/>
       <c r="B26" s="21" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -8783,7 +8758,7 @@
       </c>
       <c r="J26" s="7"/>
       <c r="K26" s="5" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="L26" s="5">
         <v>2</v>
@@ -8811,13 +8786,13 @@
         <v>128</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="U26" s="5">
         <v>1000</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="W26" s="5">
         <v>1000</v>
@@ -8849,19 +8824,19 @@
       <c r="AI26" s="13"/>
       <c r="AJ26" s="13"/>
       <c r="AK26" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="AL26" s="15" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:38" s="12" customFormat="1">
       <c r="A27" s="15"/>
       <c r="B27" s="21" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -8883,7 +8858,7 @@
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L27" s="5">
         <v>2</v>
@@ -8911,13 +8886,13 @@
         <v>256</v>
       </c>
       <c r="T27" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="U27" s="5">
         <v>4000</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="W27" s="5">
         <v>4000</v>
@@ -8949,19 +8924,19 @@
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
       <c r="AK27" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="AL27" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="12" customFormat="1">
       <c r="A28" s="15"/>
       <c r="B28" s="21" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
@@ -8976,14 +8951,14 @@
         <v>0.3</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="5" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="L28" s="5">
         <v>2</v>
@@ -9011,7 +8986,7 @@
         <v>64</v>
       </c>
       <c r="T28" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="U28" s="5">
         <v>1000</v>
@@ -9043,19 +9018,19 @@
       <c r="AI28" s="13"/>
       <c r="AJ28" s="13"/>
       <c r="AK28" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL28" s="15" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:38" s="12" customFormat="1">
       <c r="A29" s="15"/>
       <c r="B29" s="21" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -9070,14 +9045,14 @@
         <v>0.3</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="5" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -9105,7 +9080,7 @@
         <v>64</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="U29" s="5">
         <v>1000</v>
@@ -9137,19 +9112,19 @@
       <c r="AI29" s="13"/>
       <c r="AJ29" s="13"/>
       <c r="AK29" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL29" s="15" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:38" s="12" customFormat="1">
       <c r="A30" s="15"/>
       <c r="B30" s="21" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D30" s="5">
         <v>2</v>
@@ -9164,14 +9139,14 @@
         <v>0.3</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="5" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="L30" s="5">
         <v>2</v>
@@ -9199,7 +9174,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="U30" s="5">
         <v>960</v>
@@ -9231,19 +9206,19 @@
       <c r="AI30" s="13"/>
       <c r="AJ30" s="13"/>
       <c r="AK30" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL30" s="15" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" s="15"/>
       <c r="B31" s="21" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D31" s="5">
         <v>2</v>
@@ -9258,14 +9233,14 @@
         <v>0.3</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L31" s="5">
         <v>2</v>
@@ -9293,7 +9268,7 @@
         <v>256</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="U31" s="5">
         <v>960</v>
@@ -9323,16 +9298,16 @@
         <v>128</v>
       </c>
       <c r="AK31" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL31" s="15" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:38" s="12" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="21" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>26</v>
@@ -9421,16 +9396,16 @@
       <c r="AI32" s="13"/>
       <c r="AJ32" s="13"/>
       <c r="AK32" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="AL32" s="15" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:166" s="12" customFormat="1">
       <c r="A33" s="15"/>
       <c r="B33" s="21" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>48</v>
@@ -9515,25 +9490,25 @@
       <c r="AI33" s="13"/>
       <c r="AJ33" s="13"/>
       <c r="AK33" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL33" s="15" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:166">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D34" s="13">
         <v>2</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="F34" s="13">
         <f>2*2.28864</f>
@@ -9541,12 +9516,12 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L34" s="5">
         <v>2</v>
@@ -9574,13 +9549,13 @@
         <v>128</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="U34" s="5">
         <v>4000</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="W34" s="5">
         <v>4000</v>
@@ -9603,25 +9578,25 @@
         <v>128</v>
       </c>
       <c r="AK34" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="AL34" s="15" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" spans="1:166">
       <c r="A35" s="15"/>
       <c r="B35" s="21" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="F35" s="5">
         <f>2*2.28864</f>
@@ -9629,12 +9604,12 @@
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="7" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="5" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="L35" s="5">
         <v>2</v>
@@ -9662,7 +9637,7 @@
         <v>64</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="U35" s="5">
         <v>1000</v>
@@ -9692,10 +9667,10 @@
         <v>128</v>
       </c>
       <c r="AK35" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL35" s="15" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="AO35" s="12"/>
       <c r="AP35" s="12"/>
@@ -9703,16 +9678,16 @@
     <row r="36" spans="1:166" s="12" customFormat="1">
       <c r="A36" s="15"/>
       <c r="B36" s="21" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="F36" s="5">
         <f>2*2.28864</f>
@@ -9720,7 +9695,7 @@
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="7" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -9785,10 +9760,10 @@
       <c r="AI36" s="13"/>
       <c r="AJ36" s="13"/>
       <c r="AK36" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="AL36" s="15" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:166" s="12" customFormat="1">
@@ -10150,7 +10125,7 @@
     </row>
     <row r="45" spans="1:166" s="12" customFormat="1">
       <c r="A45" s="15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>41</v>
@@ -10454,13 +10429,13 @@
     </row>
     <row r="47" spans="1:166">
       <c r="A47" s="15" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="D47">
         <v>8</v>
@@ -10624,7 +10599,7 @@
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="15" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="AO48" s="31"/>
       <c r="AP48" s="31"/>
@@ -10838,7 +10813,7 @@
         <v>128</v>
       </c>
       <c r="AK49" s="15" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="51" spans="1:37" s="12" customFormat="1">
@@ -11180,7 +11155,7 @@
         <v>128</v>
       </c>
       <c r="AK58" s="15" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="59" spans="1:37">
@@ -11270,7 +11245,7 @@
         <v>128</v>
       </c>
       <c r="AK59" s="15" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="60" spans="1:37" s="12" customFormat="1">
@@ -11898,7 +11873,7 @@
     </row>
     <row r="67" spans="1:166">
       <c r="B67" s="21" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>32</v>
@@ -11985,7 +11960,7 @@
     <row r="68" spans="1:166" s="12" customFormat="1">
       <c r="A68" s="2"/>
       <c r="B68" s="21" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>32</v>
@@ -14294,7 +14269,7 @@
       <c r="AI88" s="26"/>
       <c r="AJ88" s="26"/>
       <c r="AK88" s="15" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="AL88" s="13"/>
       <c r="AM88" s="13"/>
@@ -14396,7 +14371,7 @@
       <c r="AI89" s="26"/>
       <c r="AJ89" s="26"/>
       <c r="AK89" s="15" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="AL89" s="13"/>
       <c r="AM89" s="13"/>
@@ -14494,7 +14469,7 @@
         <v>137</v>
       </c>
       <c r="AK90" s="15" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="AL90" s="13"/>
       <c r="AM90" s="13"/>
@@ -14592,7 +14567,7 @@
         <v>137</v>
       </c>
       <c r="AK91" s="15" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="AL91" s="13"/>
       <c r="AM91" s="13"/>
@@ -14602,10 +14577,10 @@
     <row r="92" spans="1:41" s="12" customFormat="1">
       <c r="A92" s="21"/>
       <c r="B92" s="21" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D92" s="5">
         <v>2</v>
@@ -14692,7 +14667,7 @@
       <c r="AI92" s="26"/>
       <c r="AJ92" s="26"/>
       <c r="AK92" s="15" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="AL92" s="13"/>
       <c r="AM92" s="13"/>
@@ -14702,10 +14677,10 @@
     <row r="93" spans="1:41" s="12" customFormat="1">
       <c r="A93" s="21"/>
       <c r="B93" s="21" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D93" s="5">
         <v>4</v>
@@ -14792,7 +14767,7 @@
       <c r="AI93" s="26"/>
       <c r="AJ93" s="26"/>
       <c r="AK93" s="15" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="AL93" s="13"/>
       <c r="AM93" s="13"/>
@@ -15062,7 +15037,7 @@
         <v>138</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>139</v>
@@ -15151,7 +15126,7 @@
         <v>6912</v>
       </c>
       <c r="AK100" s="15" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="AL100" s="13"/>
       <c r="AM100" s="13"/>
@@ -15160,7 +15135,7 @@
     </row>
     <row r="101" spans="1:41">
       <c r="A101" s="15" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B101" s="21" t="s">
         <v>233</v>
@@ -15252,7 +15227,7 @@
         <v>13824</v>
       </c>
       <c r="AK101" s="15" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="AL101" s="13"/>
       <c r="AM101" s="13"/>
@@ -15351,7 +15326,7 @@
         <v>8640</v>
       </c>
       <c r="AK102" s="15" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="AL102" s="13"/>
       <c r="AM102" s="13"/>
@@ -15450,7 +15425,7 @@
         <v>8640</v>
       </c>
       <c r="AK103" s="15" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="AL103" s="13"/>
       <c r="AM103" s="13"/>
@@ -15460,7 +15435,7 @@
     <row r="104" spans="1:41" s="12" customFormat="1">
       <c r="A104" s="21"/>
       <c r="B104" s="21" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>139</v>
@@ -15550,7 +15525,7 @@
       </c>
       <c r="AJ104" s="13"/>
       <c r="AK104" s="15" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="AL104" s="13"/>
       <c r="AM104" s="13"/>
@@ -15560,7 +15535,7 @@
     <row r="105" spans="1:41">
       <c r="A105" s="21"/>
       <c r="B105" s="21" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>139</v>
@@ -15649,7 +15624,7 @@
         <v>8640</v>
       </c>
       <c r="AK105" s="15" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="AL105" s="13"/>
       <c r="AM105" s="13"/>
@@ -16030,7 +16005,7 @@
       </c>
       <c r="J114" s="5"/>
       <c r="K114" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="L114" s="5">
         <v>0.5</v>
@@ -16084,7 +16059,7 @@
         <v>149</v>
       </c>
       <c r="AK114" s="15" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AL114" s="13"/>
       <c r="AM114" s="13"/>
@@ -16099,7 +16074,7 @@
         <v>146</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="D115" s="5">
         <v>1</v>
@@ -16121,7 +16096,7 @@
       </c>
       <c r="J115" s="5"/>
       <c r="K115" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L115" s="5">
         <v>1</v>
@@ -16187,7 +16162,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D116" s="5">
         <v>2</v>
@@ -16209,7 +16184,7 @@
       </c>
       <c r="J116" s="5"/>
       <c r="K116" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L116" s="5">
         <v>2</v>
@@ -16273,7 +16248,7 @@
         <v>148</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D117" s="5">
         <v>2</v>
@@ -16295,7 +16270,7 @@
       </c>
       <c r="J117" s="5"/>
       <c r="K117" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L117" s="5">
         <v>2</v>
@@ -16354,7 +16329,7 @@
         <v>149</v>
       </c>
       <c r="AK117" s="15" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AL117" s="13"/>
       <c r="AM117" s="13"/>
@@ -16367,7 +16342,7 @@
         <v>175</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D118" s="5">
         <v>1</v>
@@ -16389,7 +16364,7 @@
       </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L118" s="5">
         <v>0.5</v>
@@ -16447,10 +16422,10 @@
     <row r="119" spans="1:41">
       <c r="A119" s="21"/>
       <c r="B119" s="21" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D119" s="5">
         <v>2</v>
@@ -16472,7 +16447,7 @@
       </c>
       <c r="J119" s="5"/>
       <c r="K119" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L119" s="5">
         <v>1</v>
@@ -16530,10 +16505,10 @@
     <row r="120" spans="1:41">
       <c r="A120" s="21"/>
       <c r="B120" s="21" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D120" s="5">
         <v>4</v>
@@ -16555,7 +16530,7 @@
       </c>
       <c r="J120" s="5"/>
       <c r="K120" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="L120" s="5">
         <v>2</v>
@@ -16958,10 +16933,10 @@
         <v>201</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D129" s="5">
         <v>0.5</v>
@@ -17033,10 +17008,10 @@
         <v>202</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D130" s="5">
         <v>1</v>
@@ -17108,10 +17083,10 @@
         <v>203</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D131" s="5">
         <v>2</v>
@@ -17181,10 +17156,10 @@
     <row r="132" spans="1:41" ht="20" customHeight="1">
       <c r="A132" s="21"/>
       <c r="B132" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C132" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>397</v>
       </c>
       <c r="D132" s="5">
         <v>2</v>
@@ -17254,10 +17229,10 @@
     <row r="133" spans="1:41" ht="20" customHeight="1">
       <c r="A133" s="21"/>
       <c r="B133" s="21" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D133" s="5">
         <v>4</v>
@@ -17609,7 +17584,7 @@
         <v>253</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>256</v>
@@ -17684,10 +17659,10 @@
       </c>
       <c r="AG141" s="13"/>
       <c r="AH141" s="15" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="AK141" s="15" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="AL141" s="13"/>
       <c r="AM141" s="13"/>
@@ -17699,7 +17674,7 @@
         <v>254</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>255</v>
@@ -17774,10 +17749,10 @@
       </c>
       <c r="AG142" s="13"/>
       <c r="AH142" s="15" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="AK142" s="15" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="AL142" s="13"/>
       <c r="AM142" s="13"/>
@@ -17952,7 +17927,7 @@
         <v>274</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D147" s="5">
         <v>3</v>
@@ -17974,7 +17949,7 @@
       </c>
       <c r="J147" s="5"/>
       <c r="K147" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L147" s="5">
         <v>2</v>
@@ -18002,7 +17977,7 @@
         <v>54</v>
       </c>
       <c r="T147" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U147" s="13">
         <v>50</v>
@@ -18036,7 +18011,7 @@
         <v>2.5</v>
       </c>
       <c r="AK147" s="15" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="AL147" s="13"/>
       <c r="AM147" s="13"/>
@@ -18045,13 +18020,13 @@
     </row>
     <row r="148" spans="1:41">
       <c r="A148" s="15" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B148" s="21" t="s">
         <v>276</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D148" s="5">
         <v>3</v>
@@ -18073,7 +18048,7 @@
       </c>
       <c r="J148" s="5"/>
       <c r="K148" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L148" s="5">
         <v>2</v>
@@ -18101,7 +18076,7 @@
         <v>54</v>
       </c>
       <c r="T148" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U148" s="13">
         <v>50</v>
@@ -18135,7 +18110,7 @@
         <v>2.5</v>
       </c>
       <c r="AK148" s="15" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="AL148" s="13"/>
       <c r="AM148" s="13"/>
@@ -18148,7 +18123,7 @@
         <v>277</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D149" s="5">
         <v>3</v>
@@ -18170,7 +18145,7 @@
       </c>
       <c r="J149" s="5"/>
       <c r="K149" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L149" s="5">
         <v>2</v>
@@ -18198,7 +18173,7 @@
         <v>96</v>
       </c>
       <c r="T149" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U149" s="13">
         <v>50</v>
@@ -18233,7 +18208,7 @@
         <v>2.5</v>
       </c>
       <c r="AK149" s="15" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="AL149" s="13"/>
       <c r="AM149" s="13"/>
@@ -18246,7 +18221,7 @@
         <v>278</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D150" s="5">
         <v>3</v>
@@ -18268,7 +18243,7 @@
       </c>
       <c r="J150" s="5"/>
       <c r="K150" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L150" s="5">
         <v>2</v>
@@ -18296,7 +18271,7 @@
         <v>96</v>
       </c>
       <c r="T150" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U150" s="13">
         <v>50</v>
@@ -18331,7 +18306,7 @@
         <v>2.5</v>
       </c>
       <c r="AK150" s="15" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="AL150" s="13"/>
       <c r="AM150" s="13"/>
@@ -18344,7 +18319,7 @@
         <v>273</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D151" s="5">
         <v>3</v>
@@ -18366,7 +18341,7 @@
       </c>
       <c r="J151" s="5"/>
       <c r="K151" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L151" s="5">
         <f>2/3</f>
@@ -18395,7 +18370,7 @@
         <v>25</v>
       </c>
       <c r="T151" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U151" s="13">
         <v>30</v>
@@ -18430,7 +18405,7 @@
         <v>2.5</v>
       </c>
       <c r="AK151" s="15" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="AL151" s="13"/>
       <c r="AM151" s="13"/>
@@ -18443,7 +18418,7 @@
         <v>275</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D152" s="5">
         <v>3</v>
@@ -18465,7 +18440,7 @@
       </c>
       <c r="J152" s="5"/>
       <c r="K152" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L152" s="5">
         <f>2/3</f>
@@ -18494,7 +18469,7 @@
         <v>25</v>
       </c>
       <c r="T152" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="U152" s="13">
         <v>30</v>
@@ -18529,7 +18504,7 @@
         <v>2.5</v>
       </c>
       <c r="AK152" s="15" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="AL152" s="13"/>
       <c r="AM152" s="13"/>
@@ -18538,97 +18513,39 @@
     </row>
     <row r="153" spans="1:41">
       <c r="A153" s="21"/>
-      <c r="B153" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D153" s="5">
-        <v>1</v>
-      </c>
-      <c r="E153" s="13">
-        <v>960</v>
-      </c>
-      <c r="F153" s="13">
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="G153" s="13">
-        <v>311</v>
-      </c>
-      <c r="H153" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="I153" s="13" t="s">
-        <v>285</v>
-      </c>
+      <c r="B153" s="21"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="13"/>
       <c r="J153" s="5"/>
-      <c r="K153" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L153" s="5">
-        <v>4</v>
-      </c>
-      <c r="M153" s="5">
-        <v>8</v>
-      </c>
-      <c r="N153" s="5">
-        <v>2</v>
-      </c>
-      <c r="O153" s="5">
-        <v>4</v>
-      </c>
-      <c r="P153" s="5">
-        <v>8</v>
-      </c>
-      <c r="Q153" s="13">
-        <f t="shared" si="40"/>
-        <v>0.128</v>
-      </c>
-      <c r="R153" s="13">
-        <v>1066</v>
-      </c>
-      <c r="S153" s="13">
-        <v>252</v>
-      </c>
-      <c r="T153" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="U153" s="13">
-        <v>500</v>
-      </c>
+      <c r="K153" s="5"/>
+      <c r="L153" s="5"/>
+      <c r="M153" s="5"/>
+      <c r="N153" s="5"/>
+      <c r="O153" s="5"/>
+      <c r="P153" s="5"/>
+      <c r="Q153" s="13"/>
+      <c r="R153" s="13"/>
+      <c r="S153" s="13"/>
+      <c r="T153" s="13"/>
+      <c r="U153" s="13"/>
       <c r="V153" s="13"/>
       <c r="W153" s="13"/>
-      <c r="X153" s="13">
-        <v>40</v>
-      </c>
+      <c r="X153" s="13"/>
       <c r="Y153" s="13"/>
-      <c r="Z153" s="13" t="str">
-        <f t="shared" si="41"/>
-        <v>40/</v>
-      </c>
+      <c r="Z153" s="13"/>
       <c r="AA153" s="13"/>
       <c r="AB153" s="13"/>
       <c r="AC153" s="13"/>
       <c r="AD153" s="13"/>
-      <c r="AE153" s="39">
-        <v>480000</v>
-      </c>
+      <c r="AE153" s="39"/>
       <c r="AF153" s="13"/>
       <c r="AG153" s="13"/>
-      <c r="AH153" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI153" s="13">
-        <f>3000/4</f>
-        <v>750</v>
-      </c>
-      <c r="AJ153" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="AK153" s="15" t="s">
-        <v>422</v>
-      </c>
+      <c r="AH153" s="15"/>
       <c r="AL153" s="13"/>
       <c r="AM153" s="13"/>
       <c r="AN153" s="13"/>
@@ -18636,97 +18553,39 @@
     </row>
     <row r="154" spans="1:41">
       <c r="A154" s="21"/>
-      <c r="B154" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D154" s="5">
-        <v>1</v>
-      </c>
-      <c r="E154" s="13">
-        <v>960</v>
-      </c>
-      <c r="F154" s="13">
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="G154" s="13">
-        <v>311</v>
-      </c>
-      <c r="H154" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="I154" s="13" t="s">
-        <v>285</v>
-      </c>
+      <c r="B154" s="21"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
+      <c r="I154" s="13"/>
       <c r="J154" s="5"/>
-      <c r="K154" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L154" s="5">
-        <v>4</v>
-      </c>
-      <c r="M154" s="5">
-        <v>8</v>
-      </c>
-      <c r="N154" s="5">
-        <v>2</v>
-      </c>
-      <c r="O154" s="5">
-        <v>4</v>
-      </c>
-      <c r="P154" s="5">
-        <v>8</v>
-      </c>
-      <c r="Q154" s="13">
-        <f t="shared" ref="Q154:Q155" si="42">M154*N154*P154/1000</f>
-        <v>0.128</v>
-      </c>
-      <c r="R154" s="13">
-        <v>1066</v>
-      </c>
-      <c r="S154" s="13">
-        <v>252</v>
-      </c>
-      <c r="T154" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="U154" s="13">
-        <v>500</v>
-      </c>
+      <c r="K154" s="5"/>
+      <c r="L154" s="5"/>
+      <c r="M154" s="5"/>
+      <c r="N154" s="5"/>
+      <c r="O154" s="5"/>
+      <c r="P154" s="5"/>
+      <c r="Q154" s="13"/>
+      <c r="R154" s="13"/>
+      <c r="S154" s="13"/>
+      <c r="T154" s="13"/>
+      <c r="U154" s="13"/>
       <c r="V154" s="13"/>
       <c r="W154" s="13"/>
-      <c r="X154" s="13">
-        <v>40</v>
-      </c>
+      <c r="X154" s="13"/>
       <c r="Y154" s="13"/>
-      <c r="Z154" s="13" t="str">
-        <f t="shared" si="41"/>
-        <v>40/</v>
-      </c>
+      <c r="Z154" s="13"/>
       <c r="AA154" s="13"/>
       <c r="AB154" s="13"/>
       <c r="AC154" s="13"/>
       <c r="AD154" s="13"/>
-      <c r="AE154" s="39">
-        <v>120000</v>
-      </c>
+      <c r="AE154" s="39"/>
       <c r="AF154" s="13"/>
       <c r="AG154" s="13"/>
-      <c r="AH154" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI154" s="13">
-        <f>3000/4</f>
-        <v>750</v>
-      </c>
-      <c r="AJ154" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="AK154" s="15" t="s">
-        <v>423</v>
-      </c>
+      <c r="AH154" s="15"/>
       <c r="AL154" s="13"/>
       <c r="AM154" s="13"/>
       <c r="AN154" s="13"/>
@@ -18734,97 +18593,39 @@
     </row>
     <row r="155" spans="1:41">
       <c r="A155" s="21"/>
-      <c r="B155" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="C155" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D155" s="5">
-        <v>1</v>
-      </c>
-      <c r="E155" s="13">
-        <v>960</v>
-      </c>
-      <c r="F155" s="13">
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="G155" s="13">
-        <v>311</v>
-      </c>
-      <c r="H155" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="I155" s="13" t="s">
-        <v>285</v>
-      </c>
+      <c r="B155" s="21"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+      <c r="G155" s="13"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="13"/>
       <c r="J155" s="5"/>
-      <c r="K155" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L155" s="5">
-        <v>4</v>
-      </c>
-      <c r="M155" s="5">
-        <v>8</v>
-      </c>
-      <c r="N155" s="5">
-        <v>2</v>
-      </c>
-      <c r="O155" s="5">
-        <v>4</v>
-      </c>
-      <c r="P155" s="5">
-        <v>8</v>
-      </c>
-      <c r="Q155" s="13">
-        <f t="shared" si="42"/>
-        <v>0.128</v>
-      </c>
-      <c r="R155" s="13">
-        <v>1066</v>
-      </c>
-      <c r="S155" s="13">
-        <v>504</v>
-      </c>
-      <c r="T155" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="U155" s="13">
-        <v>500</v>
-      </c>
+      <c r="K155" s="5"/>
+      <c r="L155" s="5"/>
+      <c r="M155" s="5"/>
+      <c r="N155" s="5"/>
+      <c r="O155" s="5"/>
+      <c r="P155" s="5"/>
+      <c r="Q155" s="13"/>
+      <c r="R155" s="13"/>
+      <c r="S155" s="13"/>
+      <c r="T155" s="13"/>
+      <c r="U155" s="13"/>
       <c r="V155" s="13"/>
       <c r="W155" s="13"/>
-      <c r="X155" s="13">
-        <v>40</v>
-      </c>
+      <c r="X155" s="13"/>
       <c r="Y155" s="13"/>
-      <c r="Z155" s="13" t="str">
-        <f t="shared" ref="Z155:Z156" si="43">X155&amp;"/"&amp;Y155</f>
-        <v>40/</v>
-      </c>
+      <c r="Z155" s="13"/>
       <c r="AA155" s="13"/>
       <c r="AB155" s="13"/>
       <c r="AC155" s="13"/>
       <c r="AD155" s="13"/>
-      <c r="AE155" s="39">
-        <v>480000</v>
-      </c>
+      <c r="AE155" s="39"/>
       <c r="AF155" s="13"/>
       <c r="AG155" s="13"/>
-      <c r="AH155" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI155" s="13">
-        <f>3000/8</f>
-        <v>375</v>
-      </c>
-      <c r="AJ155" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="AK155" s="15" t="s">
-        <v>422</v>
-      </c>
+      <c r="AH155" s="15"/>
       <c r="AL155" s="13"/>
       <c r="AM155" s="13"/>
       <c r="AN155" s="13"/>
@@ -18832,97 +18633,39 @@
     </row>
     <row r="156" spans="1:41">
       <c r="A156" s="21"/>
-      <c r="B156" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D156" s="5">
-        <v>1</v>
-      </c>
-      <c r="E156" s="13">
-        <v>960</v>
-      </c>
-      <c r="F156" s="13">
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="G156" s="13">
-        <v>311</v>
-      </c>
-      <c r="H156" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="I156" s="13" t="s">
-        <v>285</v>
-      </c>
+      <c r="B156" s="21"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="13"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="13"/>
       <c r="J156" s="5"/>
-      <c r="K156" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="L156" s="5">
-        <v>4</v>
-      </c>
-      <c r="M156" s="5">
-        <v>8</v>
-      </c>
-      <c r="N156" s="5">
-        <v>2</v>
-      </c>
-      <c r="O156" s="5">
-        <v>4</v>
-      </c>
-      <c r="P156" s="5">
-        <v>8</v>
-      </c>
-      <c r="Q156" s="13">
-        <f t="shared" ref="Q156" si="44">M156*N156*P156/1000</f>
-        <v>0.128</v>
-      </c>
-      <c r="R156" s="13">
-        <v>1066</v>
-      </c>
-      <c r="S156" s="13">
-        <v>504</v>
-      </c>
-      <c r="T156" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="U156" s="13">
-        <v>500</v>
-      </c>
+      <c r="K156" s="5"/>
+      <c r="L156" s="5"/>
+      <c r="M156" s="5"/>
+      <c r="N156" s="5"/>
+      <c r="O156" s="5"/>
+      <c r="P156" s="5"/>
+      <c r="Q156" s="13"/>
+      <c r="R156" s="13"/>
+      <c r="S156" s="13"/>
+      <c r="T156" s="13"/>
+      <c r="U156" s="13"/>
       <c r="V156" s="13"/>
       <c r="W156" s="13"/>
-      <c r="X156" s="13">
-        <v>40</v>
-      </c>
+      <c r="X156" s="13"/>
       <c r="Y156" s="13"/>
-      <c r="Z156" s="13" t="str">
-        <f t="shared" si="43"/>
-        <v>40/</v>
-      </c>
+      <c r="Z156" s="13"/>
       <c r="AA156" s="13"/>
       <c r="AB156" s="13"/>
       <c r="AC156" s="13"/>
       <c r="AD156" s="13"/>
-      <c r="AE156" s="39">
-        <v>120000</v>
-      </c>
+      <c r="AE156" s="39"/>
       <c r="AF156" s="13"/>
       <c r="AG156" s="13"/>
-      <c r="AH156" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI156" s="13">
-        <f>3000/8</f>
-        <v>375</v>
-      </c>
-      <c r="AJ156" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="AK156" s="15" t="s">
-        <v>423</v>
-      </c>
+      <c r="AH156" s="15"/>
       <c r="AL156" s="13"/>
       <c r="AM156" s="13"/>
       <c r="AN156" s="13"/>
@@ -19060,17 +18803,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72 AH32:AJ33">
-    <cfRule type="expression" dxfId="151" priority="236">
+    <cfRule type="expression" dxfId="152" priority="236">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="150" priority="223">
+    <cfRule type="expression" dxfId="151" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="149" priority="212">
+    <cfRule type="expression" dxfId="150" priority="212">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19159,7 +18902,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="148" priority="204">
+    <cfRule type="expression" dxfId="149" priority="204">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19248,152 +18991,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="147" priority="201">
+    <cfRule type="expression" dxfId="148" priority="201">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="146" priority="200">
+    <cfRule type="expression" dxfId="147" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="145" priority="178">
+    <cfRule type="expression" dxfId="146" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="144" priority="176">
+    <cfRule type="expression" dxfId="145" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="143" priority="175">
+    <cfRule type="expression" dxfId="144" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="142" priority="174">
+    <cfRule type="expression" dxfId="143" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="141" priority="161">
+    <cfRule type="expression" dxfId="142" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="140" priority="163">
+    <cfRule type="expression" dxfId="141" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="139" priority="98">
+    <cfRule type="expression" dxfId="140" priority="98">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="138" priority="129">
+    <cfRule type="expression" dxfId="139" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="137" priority="128">
+    <cfRule type="expression" dxfId="138" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="136" priority="127">
+    <cfRule type="expression" dxfId="137" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="135" priority="126">
+    <cfRule type="expression" dxfId="136" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="134" priority="125">
+    <cfRule type="expression" dxfId="135" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="133" priority="124">
+    <cfRule type="expression" dxfId="134" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="132" priority="123">
+    <cfRule type="expression" dxfId="133" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="131" priority="122">
+    <cfRule type="expression" dxfId="132" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="130" priority="121">
+    <cfRule type="expression" dxfId="131" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="129" priority="120">
+    <cfRule type="expression" dxfId="130" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="128" priority="119">
+    <cfRule type="expression" dxfId="129" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="127" priority="118">
+    <cfRule type="expression" dxfId="128" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="126" priority="117">
+    <cfRule type="expression" dxfId="127" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="125" priority="114">
+    <cfRule type="expression" dxfId="126" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="124" priority="116">
+    <cfRule type="expression" dxfId="125" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="123" priority="115">
+    <cfRule type="expression" dxfId="124" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="122" priority="113">
+    <cfRule type="expression" dxfId="123" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="121" priority="112">
+    <cfRule type="expression" dxfId="122" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="120" priority="111">
+    <cfRule type="expression" dxfId="121" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="119" priority="110">
+    <cfRule type="expression" dxfId="120" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="118" priority="109">
+    <cfRule type="expression" dxfId="119" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19482,97 +19225,97 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="117" priority="108">
+    <cfRule type="expression" dxfId="118" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="116" priority="107">
+    <cfRule type="expression" dxfId="117" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="115" priority="106">
+    <cfRule type="expression" dxfId="116" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="114" priority="105">
+    <cfRule type="expression" dxfId="115" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="113" priority="104">
+    <cfRule type="expression" dxfId="114" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="112" priority="103">
+    <cfRule type="expression" dxfId="113" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="111" priority="102">
+    <cfRule type="expression" dxfId="112" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="110" priority="101">
+    <cfRule type="expression" dxfId="111" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="109" priority="100">
+    <cfRule type="expression" dxfId="110" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="108" priority="61">
+    <cfRule type="expression" dxfId="109" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="107" priority="97">
+    <cfRule type="expression" dxfId="108" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="106" priority="96">
+    <cfRule type="expression" dxfId="107" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="105" priority="95">
+    <cfRule type="expression" dxfId="106" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="104" priority="94">
+    <cfRule type="expression" dxfId="105" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="103" priority="93">
+    <cfRule type="expression" dxfId="104" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE36:AH36 AE35:AF35 AH35">
-    <cfRule type="expression" dxfId="102" priority="92">
+    <cfRule type="expression" dxfId="103" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="101" priority="91">
+    <cfRule type="expression" dxfId="102" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="100" priority="90">
+    <cfRule type="expression" dxfId="101" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="99" priority="86">
+    <cfRule type="expression" dxfId="100" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19613,7 +19356,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="98" priority="81">
+    <cfRule type="expression" dxfId="99" priority="81">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19666,367 +19409,367 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="97" priority="80">
+    <cfRule type="expression" dxfId="98" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="96" priority="79">
+    <cfRule type="expression" dxfId="97" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="95" priority="78">
+    <cfRule type="expression" dxfId="96" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="94" priority="77">
+    <cfRule type="expression" dxfId="95" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="93" priority="76">
+    <cfRule type="expression" dxfId="94" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="92" priority="75">
+    <cfRule type="expression" dxfId="93" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="91" priority="74">
+    <cfRule type="expression" dxfId="92" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="90" priority="73">
+    <cfRule type="expression" dxfId="91" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="89" priority="69">
+    <cfRule type="expression" dxfId="90" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="88" priority="71">
+    <cfRule type="expression" dxfId="89" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="87" priority="70">
+    <cfRule type="expression" dxfId="88" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="86" priority="68">
+    <cfRule type="expression" dxfId="87" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="85" priority="67">
+    <cfRule type="expression" dxfId="86" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="84" priority="65">
+    <cfRule type="expression" dxfId="85" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="83" priority="64">
+    <cfRule type="expression" dxfId="84" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="82" priority="63">
+    <cfRule type="expression" dxfId="83" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="81" priority="62">
+    <cfRule type="expression" dxfId="82" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="80" priority="60">
+    <cfRule type="expression" dxfId="81" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="79" priority="58">
+    <cfRule type="expression" dxfId="80" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="78" priority="57">
+    <cfRule type="expression" dxfId="79" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="77" priority="55">
+    <cfRule type="expression" dxfId="78" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="76" priority="54">
+    <cfRule type="expression" dxfId="77" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="75" priority="53">
+    <cfRule type="expression" dxfId="76" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="74" priority="15">
+    <cfRule type="expression" dxfId="75" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="73" priority="4">
+    <cfRule type="expression" dxfId="74" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="expression" dxfId="72" priority="51">
+    <cfRule type="expression" dxfId="73" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="71" priority="52">
+    <cfRule type="expression" dxfId="72" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="70" priority="50">
+    <cfRule type="expression" dxfId="71" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="69" priority="49">
+    <cfRule type="expression" dxfId="70" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="68" priority="48">
+    <cfRule type="expression" dxfId="69" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="67" priority="47">
+    <cfRule type="expression" dxfId="68" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92:K93">
-    <cfRule type="expression" dxfId="66" priority="45">
+    <cfRule type="expression" dxfId="67" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="65" priority="46">
+    <cfRule type="expression" dxfId="66" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="64" priority="44">
+    <cfRule type="expression" dxfId="65" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="63" priority="43">
+    <cfRule type="expression" dxfId="64" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="62" priority="42">
+    <cfRule type="expression" dxfId="63" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="61" priority="41">
+    <cfRule type="expression" dxfId="62" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="60" priority="40">
+    <cfRule type="expression" dxfId="61" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="59" priority="39">
+    <cfRule type="expression" dxfId="60" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="58" priority="38">
+    <cfRule type="expression" dxfId="59" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="57" priority="37">
+    <cfRule type="expression" dxfId="58" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="56" priority="36">
+    <cfRule type="expression" dxfId="57" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="55" priority="35">
+    <cfRule type="expression" dxfId="56" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="54" priority="34">
+    <cfRule type="expression" dxfId="55" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="53" priority="33">
+    <cfRule type="expression" dxfId="54" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="52" priority="32">
+    <cfRule type="expression" dxfId="53" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="51" priority="31">
+    <cfRule type="expression" dxfId="52" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="50" priority="30">
+    <cfRule type="expression" dxfId="51" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="49" priority="28">
+    <cfRule type="expression" dxfId="50" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="48" priority="27">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="47" priority="26">
+    <cfRule type="expression" dxfId="48" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="46" priority="25">
+    <cfRule type="expression" dxfId="47" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="45" priority="24">
+    <cfRule type="expression" dxfId="46" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="44" priority="23">
+    <cfRule type="expression" dxfId="45" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="43" priority="22">
+    <cfRule type="expression" dxfId="44" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="42" priority="21">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="41" priority="20">
+    <cfRule type="expression" dxfId="42" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="40" priority="18">
+    <cfRule type="expression" dxfId="41" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="39" priority="17">
+    <cfRule type="expression" dxfId="40" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="39" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="37" priority="14">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="37" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="35" priority="12">
+    <cfRule type="expression" dxfId="36" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="35" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="33" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="32" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="31" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG35">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20091,7 +19834,7 @@
         <v>111</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E1" s="35"/>
       <c r="F1" s="36" t="s">
@@ -20158,10 +19901,10 @@
         <v>267</v>
       </c>
       <c r="AA1" s="36" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="AB1" s="36" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="11" customFormat="1" ht="21" thickBot="1">
@@ -20244,7 +19987,7 @@
         <v>159</v>
       </c>
       <c r="AA2" s="28" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="AB2" s="28" t="s">
         <v>101</v>
@@ -23458,7 +23201,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23566,7 +23309,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="F33" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23783,7 +23526,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23891,7 +23634,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -23999,7 +23742,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25562,7 +25305,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="F51" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25678,7 +25421,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="F52" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25786,7 +25529,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="F53" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -25894,7 +25637,7 @@
         <v>0</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="F54" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26006,7 +25749,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="F55" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -28965,9 +28708,9 @@
       </c>
     </row>
     <row r="82" spans="3:29">
-      <c r="C82" s="21" t="str">
+      <c r="C82" s="21">
         <f t="shared" ca="1" si="57"/>
-        <v>L256</v>
+        <v>0</v>
       </c>
       <c r="D82" s="15">
         <f t="shared" ca="1" si="57"/>
@@ -28975,7 +28718,7 @@
       </c>
       <c r="E82" s="21" t="str">
         <f t="shared" ca="1" si="59"/>
-        <v>Tsub.L256</v>
+        <v>Tsub.0</v>
       </c>
       <c r="F82" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -28995,7 +28738,7 @@
       </c>
       <c r="J82" s="18">
         <f t="shared" ca="1" si="58"/>
-        <v>480000</v>
+        <v>0</v>
       </c>
       <c r="K82" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29005,45 +28748,45 @@
         <f t="shared" ca="1" si="58"/>
         <v>0</v>
       </c>
-      <c r="M82" s="18" t="str">
+      <c r="M82" s="18">
         <f t="shared" ca="1" si="50"/>
-        <v>JPY</v>
+        <v>0</v>
       </c>
       <c r="N82" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>0.51200000000000001</v>
+        <v>0</v>
       </c>
       <c r="O82" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="P82" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="P82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>S1070</v>
+        <v>0</v>
       </c>
       <c r="Q82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>1</v>
-      </c>
-      <c r="R82" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="R82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>Xeon X7550</v>
+        <v>0</v>
       </c>
       <c r="S82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>252</v>
-      </c>
-      <c r="U82" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="U82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>SSD</v>
+        <v>0</v>
       </c>
       <c r="V82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="W82" s="13">
         <f t="shared" ca="1" si="56"/>
@@ -29053,30 +28796,30 @@
         <f t="shared" ca="1" si="56"/>
         <v>0</v>
       </c>
-      <c r="Y82" s="13" t="str">
+      <c r="Y82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>40/</v>
+        <v>0</v>
       </c>
       <c r="Z82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="AA82" s="13">
         <f t="shared" ca="1" si="56"/>
-        <v>2.5</v>
-      </c>
-      <c r="AB82" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="15">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>0</v>
       </c>
       <c r="AC82" s="33">
         <v>153</v>
       </c>
     </row>
     <row r="83" spans="3:29">
-      <c r="C83" s="21" t="str">
+      <c r="C83" s="21">
         <f t="shared" ca="1" si="57"/>
-        <v>L256 open</v>
+        <v>0</v>
       </c>
       <c r="D83" s="15">
         <f t="shared" ca="1" si="57"/>
@@ -29084,7 +28827,7 @@
       </c>
       <c r="E83" s="21" t="str">
         <f t="shared" ca="1" si="59"/>
-        <v>Tsub.L256 open</v>
+        <v>Tsub.0</v>
       </c>
       <c r="F83" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29104,7 +28847,7 @@
       </c>
       <c r="J83" s="18">
         <f t="shared" ca="1" si="58"/>
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="K83" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29114,45 +28857,45 @@
         <f t="shared" ca="1" si="58"/>
         <v>0</v>
       </c>
-      <c r="M83" s="18" t="str">
+      <c r="M83" s="18">
         <f t="shared" ca="1" si="50"/>
-        <v>JPY</v>
+        <v>0</v>
       </c>
       <c r="N83" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>0.51200000000000001</v>
+        <v>0</v>
       </c>
       <c r="O83" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="P83" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="P83" s="13">
         <f t="shared" ref="P83:U85" ca="1" si="60">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>S1070</v>
+        <v>0</v>
       </c>
       <c r="Q83" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>1</v>
-      </c>
-      <c r="R83" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="R83" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>Xeon X7550</v>
+        <v>0</v>
       </c>
       <c r="S83" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T83" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>252</v>
-      </c>
-      <c r="U83" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="U83" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>SSD</v>
+        <v>0</v>
       </c>
       <c r="V83" s="13">
         <f t="shared" ref="V83:AA85" ca="1" si="61">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="W83" s="13">
         <f t="shared" ca="1" si="61"/>
@@ -29162,30 +28905,30 @@
         <f t="shared" ca="1" si="61"/>
         <v>0</v>
       </c>
-      <c r="Y83" s="13" t="str">
+      <c r="Y83" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>40/</v>
+        <v>0</v>
       </c>
       <c r="Z83" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="AA83" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>2.5</v>
-      </c>
-      <c r="AB83" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="15">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>0</v>
       </c>
       <c r="AC83" s="33">
         <v>154</v>
       </c>
     </row>
     <row r="84" spans="3:29">
-      <c r="C84" s="21" t="str">
+      <c r="C84" s="21">
         <f t="shared" ca="1" si="57"/>
-        <v>L512</v>
+        <v>0</v>
       </c>
       <c r="D84" s="15">
         <f t="shared" ca="1" si="57"/>
@@ -29193,7 +28936,7 @@
       </c>
       <c r="E84" s="21" t="str">
         <f t="shared" ca="1" si="59"/>
-        <v>Tsub.L512</v>
+        <v>Tsub.0</v>
       </c>
       <c r="F84" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29213,7 +28956,7 @@
       </c>
       <c r="J84" s="18">
         <f t="shared" ca="1" si="58"/>
-        <v>480000</v>
+        <v>0</v>
       </c>
       <c r="K84" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29223,45 +28966,45 @@
         <f t="shared" ca="1" si="58"/>
         <v>0</v>
       </c>
-      <c r="M84" s="18" t="str">
+      <c r="M84" s="18">
         <f t="shared" ca="1" si="50"/>
-        <v>JPY</v>
+        <v>0</v>
       </c>
       <c r="N84" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>0.51200000000000001</v>
+        <v>0</v>
       </c>
       <c r="O84" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="P84" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="P84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>S1070</v>
+        <v>0</v>
       </c>
       <c r="Q84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>1</v>
-      </c>
-      <c r="R84" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="R84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>Xeon X7550</v>
+        <v>0</v>
       </c>
       <c r="S84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>504</v>
-      </c>
-      <c r="U84" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="U84" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>SSD</v>
+        <v>0</v>
       </c>
       <c r="V84" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="W84" s="13">
         <f t="shared" ca="1" si="61"/>
@@ -29271,30 +29014,30 @@
         <f t="shared" ca="1" si="61"/>
         <v>0</v>
       </c>
-      <c r="Y84" s="13" t="str">
+      <c r="Y84" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>40/</v>
+        <v>0</v>
       </c>
       <c r="Z84" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="AA84" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>2.5</v>
-      </c>
-      <c r="AB84" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="15">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>0</v>
       </c>
       <c r="AC84" s="33">
         <v>155</v>
       </c>
     </row>
     <row r="85" spans="3:29">
-      <c r="C85" s="21" t="str">
+      <c r="C85" s="21">
         <f t="shared" ca="1" si="57"/>
-        <v>L512 open</v>
+        <v>0</v>
       </c>
       <c r="D85" s="15">
         <f t="shared" ca="1" si="57"/>
@@ -29302,7 +29045,7 @@
       </c>
       <c r="E85" s="21" t="str">
         <f t="shared" ref="E85" ca="1" si="62">"Tsub." &amp; C85</f>
-        <v>Tsub.L512 open</v>
+        <v>Tsub.0</v>
       </c>
       <c r="F85" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29322,7 +29065,7 @@
       </c>
       <c r="J85" s="18">
         <f t="shared" ca="1" si="58"/>
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="K85" s="18">
         <f t="shared" ca="1" si="58"/>
@@ -29332,45 +29075,45 @@
         <f t="shared" ca="1" si="58"/>
         <v>0</v>
       </c>
-      <c r="M85" s="18" t="str">
+      <c r="M85" s="18">
         <f t="shared" ca="1" si="50"/>
-        <v>JPY</v>
+        <v>0</v>
       </c>
       <c r="N85" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>0.51200000000000001</v>
+        <v>0</v>
       </c>
       <c r="O85" s="13">
         <f t="shared" ca="1" si="54"/>
-        <v>2.4883000000000002</v>
-      </c>
-      <c r="P85" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="P85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>S1070</v>
+        <v>0</v>
       </c>
       <c r="Q85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>1</v>
-      </c>
-      <c r="R85" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="R85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>Xeon X7550</v>
+        <v>0</v>
       </c>
       <c r="S85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>504</v>
-      </c>
-      <c r="U85" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="U85" s="13">
         <f t="shared" ca="1" si="60"/>
-        <v>SSD</v>
+        <v>0</v>
       </c>
       <c r="V85" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="W85" s="13">
         <f t="shared" ca="1" si="61"/>
@@ -29380,21 +29123,21 @@
         <f t="shared" ca="1" si="61"/>
         <v>0</v>
       </c>
-      <c r="Y85" s="13" t="str">
+      <c r="Y85" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>40/</v>
+        <v>0</v>
       </c>
       <c r="Z85" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="AA85" s="13">
         <f t="shared" ca="1" si="61"/>
-        <v>2.5</v>
-      </c>
-      <c r="AB85" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="15">
         <f t="shared" ca="1" si="53"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>0</v>
       </c>
       <c r="AC85" s="33">
         <v>156</v>
@@ -29403,127 +29146,127 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="24" priority="146">
+    <cfRule type="expression" dxfId="26" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="23" priority="86">
+    <cfRule type="expression" dxfId="25" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="22" priority="74">
+    <cfRule type="expression" dxfId="24" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="21" priority="72">
+    <cfRule type="expression" dxfId="23" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="20" priority="73">
+    <cfRule type="expression" dxfId="22" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="19" priority="71">
+    <cfRule type="expression" dxfId="21" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="18" priority="68">
+    <cfRule type="expression" dxfId="20" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="17" priority="62">
+    <cfRule type="expression" dxfId="19" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="16" priority="53">
+    <cfRule type="expression" dxfId="18" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="15" priority="52">
+    <cfRule type="expression" dxfId="17" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="14" priority="32">
+    <cfRule type="expression" dxfId="16" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="13" priority="28">
+    <cfRule type="expression" dxfId="15" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="14" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="13" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="9" priority="21">
+    <cfRule type="expression" dxfId="11" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed csv file. More opaque markers on cost per 1TFlops graph. Less saturated colors on Time slice bar charts.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5085,7 +5085,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="153">
+  <dxfs count="152">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5093,18 +5093,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5379,7 +5368,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7066,7 +7055,7 @@
   </sheetPr>
   <dimension ref="A1:FJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -18360,7 +18349,7 @@
         <v>8</v>
       </c>
       <c r="Q151" s="13">
-        <f t="shared" ref="Q151:Q153" si="40">M151*N151*P151/1000</f>
+        <f t="shared" ref="Q151:Q152" si="40">M151*N151*P151/1000</f>
         <v>0.14064000000000002</v>
       </c>
       <c r="R151" s="13">
@@ -18382,7 +18371,7 @@
       </c>
       <c r="Y151" s="13"/>
       <c r="Z151" s="13" t="str">
-        <f t="shared" ref="Z151:Z154" si="41">X151&amp;"/"&amp;Y151</f>
+        <f t="shared" ref="Z151:Z152" si="41">X151&amp;"/"&amp;Y151</f>
         <v>80/</v>
       </c>
       <c r="AA151" s="13"/>
@@ -18803,17 +18792,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72 AH32:AJ33">
-    <cfRule type="expression" dxfId="152" priority="236">
+    <cfRule type="expression" dxfId="151" priority="236">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="151" priority="223">
+    <cfRule type="expression" dxfId="150" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="150" priority="212">
+    <cfRule type="expression" dxfId="149" priority="212">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18902,7 +18891,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="149" priority="204">
+    <cfRule type="expression" dxfId="148" priority="204">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18991,152 +18980,152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="148" priority="201">
+    <cfRule type="expression" dxfId="147" priority="201">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="147" priority="200">
+    <cfRule type="expression" dxfId="146" priority="200">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="146" priority="178">
+    <cfRule type="expression" dxfId="145" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="145" priority="176">
+    <cfRule type="expression" dxfId="144" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="144" priority="175">
+    <cfRule type="expression" dxfId="143" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="143" priority="174">
+    <cfRule type="expression" dxfId="142" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="142" priority="161">
+    <cfRule type="expression" dxfId="141" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="141" priority="163">
+    <cfRule type="expression" dxfId="140" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="140" priority="98">
+    <cfRule type="expression" dxfId="139" priority="98">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="139" priority="129">
+    <cfRule type="expression" dxfId="138" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="138" priority="128">
+    <cfRule type="expression" dxfId="137" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="137" priority="127">
+    <cfRule type="expression" dxfId="136" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="136" priority="126">
+    <cfRule type="expression" dxfId="135" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="135" priority="125">
+    <cfRule type="expression" dxfId="134" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="134" priority="124">
+    <cfRule type="expression" dxfId="133" priority="124">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="133" priority="123">
+    <cfRule type="expression" dxfId="132" priority="123">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="132" priority="122">
+    <cfRule type="expression" dxfId="131" priority="122">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="131" priority="121">
+    <cfRule type="expression" dxfId="130" priority="121">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
-    <cfRule type="expression" dxfId="130" priority="120">
+    <cfRule type="expression" dxfId="129" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:P27 R27">
-    <cfRule type="expression" dxfId="129" priority="119">
+    <cfRule type="expression" dxfId="128" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="128" priority="118">
+    <cfRule type="expression" dxfId="127" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="127" priority="117">
+    <cfRule type="expression" dxfId="126" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="126" priority="114">
+    <cfRule type="expression" dxfId="125" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="125" priority="116">
+    <cfRule type="expression" dxfId="124" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="124" priority="115">
+    <cfRule type="expression" dxfId="123" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="123" priority="113">
+    <cfRule type="expression" dxfId="122" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="122" priority="112">
+    <cfRule type="expression" dxfId="121" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="121" priority="111">
+    <cfRule type="expression" dxfId="120" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="120" priority="110">
+    <cfRule type="expression" dxfId="119" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="119" priority="109">
+    <cfRule type="expression" dxfId="118" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19225,97 +19214,97 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="118" priority="108">
+    <cfRule type="expression" dxfId="117" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="117" priority="107">
+    <cfRule type="expression" dxfId="116" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="116" priority="106">
+    <cfRule type="expression" dxfId="115" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="115" priority="105">
+    <cfRule type="expression" dxfId="114" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="114" priority="104">
+    <cfRule type="expression" dxfId="113" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="113" priority="103">
+    <cfRule type="expression" dxfId="112" priority="103">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="112" priority="102">
+    <cfRule type="expression" dxfId="111" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="111" priority="101">
+    <cfRule type="expression" dxfId="110" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="110" priority="100">
+    <cfRule type="expression" dxfId="109" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="109" priority="61">
+    <cfRule type="expression" dxfId="108" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="108" priority="97">
+    <cfRule type="expression" dxfId="107" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="107" priority="96">
+    <cfRule type="expression" dxfId="106" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="106" priority="95">
+    <cfRule type="expression" dxfId="105" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="105" priority="94">
+    <cfRule type="expression" dxfId="104" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="104" priority="93">
+    <cfRule type="expression" dxfId="103" priority="93">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE36:AH36 AE35:AF35 AH35">
-    <cfRule type="expression" dxfId="103" priority="92">
+    <cfRule type="expression" dxfId="102" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="102" priority="91">
+    <cfRule type="expression" dxfId="101" priority="91">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="101" priority="90">
+    <cfRule type="expression" dxfId="100" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="100" priority="86">
+    <cfRule type="expression" dxfId="99" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19356,7 +19345,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="99" priority="81">
+    <cfRule type="expression" dxfId="98" priority="81">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19409,367 +19398,367 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="98" priority="80">
+    <cfRule type="expression" dxfId="97" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="97" priority="79">
+    <cfRule type="expression" dxfId="96" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="96" priority="78">
+    <cfRule type="expression" dxfId="95" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="95" priority="77">
+    <cfRule type="expression" dxfId="94" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="94" priority="76">
+    <cfRule type="expression" dxfId="93" priority="76">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="93" priority="75">
+    <cfRule type="expression" dxfId="92" priority="75">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="92" priority="74">
+    <cfRule type="expression" dxfId="91" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="91" priority="73">
+    <cfRule type="expression" dxfId="90" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
-    <cfRule type="expression" dxfId="90" priority="69">
+    <cfRule type="expression" dxfId="89" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="89" priority="71">
+    <cfRule type="expression" dxfId="88" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="88" priority="70">
+    <cfRule type="expression" dxfId="87" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="87" priority="68">
+    <cfRule type="expression" dxfId="86" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="86" priority="67">
+    <cfRule type="expression" dxfId="85" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="85" priority="65">
+    <cfRule type="expression" dxfId="84" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="84" priority="64">
+    <cfRule type="expression" dxfId="83" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="83" priority="63">
+    <cfRule type="expression" dxfId="82" priority="63">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="82" priority="62">
+    <cfRule type="expression" dxfId="81" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="81" priority="60">
+    <cfRule type="expression" dxfId="80" priority="60">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="80" priority="58">
+    <cfRule type="expression" dxfId="79" priority="58">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="79" priority="57">
+    <cfRule type="expression" dxfId="78" priority="57">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
-    <cfRule type="expression" dxfId="78" priority="55">
+    <cfRule type="expression" dxfId="77" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="77" priority="54">
+    <cfRule type="expression" dxfId="76" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="76" priority="53">
+    <cfRule type="expression" dxfId="75" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="75" priority="15">
+    <cfRule type="expression" dxfId="74" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="74" priority="4">
+    <cfRule type="expression" dxfId="73" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="expression" dxfId="73" priority="51">
+    <cfRule type="expression" dxfId="72" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="72" priority="52">
+    <cfRule type="expression" dxfId="71" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="71" priority="50">
+    <cfRule type="expression" dxfId="70" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="70" priority="49">
+    <cfRule type="expression" dxfId="69" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="69" priority="48">
+    <cfRule type="expression" dxfId="68" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="68" priority="47">
+    <cfRule type="expression" dxfId="67" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92:K93">
-    <cfRule type="expression" dxfId="67" priority="45">
+    <cfRule type="expression" dxfId="66" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="66" priority="46">
+    <cfRule type="expression" dxfId="65" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="65" priority="44">
+    <cfRule type="expression" dxfId="64" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="64" priority="43">
+    <cfRule type="expression" dxfId="63" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="63" priority="42">
+    <cfRule type="expression" dxfId="62" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="62" priority="41">
+    <cfRule type="expression" dxfId="61" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="61" priority="40">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="60" priority="39">
+    <cfRule type="expression" dxfId="59" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="59" priority="38">
+    <cfRule type="expression" dxfId="58" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="58" priority="37">
+    <cfRule type="expression" dxfId="57" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="57" priority="36">
+    <cfRule type="expression" dxfId="56" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="56" priority="35">
+    <cfRule type="expression" dxfId="55" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="55" priority="34">
+    <cfRule type="expression" dxfId="54" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="54" priority="33">
+    <cfRule type="expression" dxfId="53" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="53" priority="32">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="52" priority="31">
+    <cfRule type="expression" dxfId="51" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="51" priority="30">
+    <cfRule type="expression" dxfId="50" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="50" priority="28">
+    <cfRule type="expression" dxfId="49" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="49" priority="27">
+    <cfRule type="expression" dxfId="48" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="48" priority="26">
+    <cfRule type="expression" dxfId="47" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="47" priority="25">
+    <cfRule type="expression" dxfId="46" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="46" priority="24">
+    <cfRule type="expression" dxfId="45" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="45" priority="23">
+    <cfRule type="expression" dxfId="44" priority="23">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="44" priority="22">
+    <cfRule type="expression" dxfId="43" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="43" priority="21">
+    <cfRule type="expression" dxfId="42" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="42" priority="20">
+    <cfRule type="expression" dxfId="41" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="41" priority="18">
+    <cfRule type="expression" dxfId="40" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="40" priority="17">
+    <cfRule type="expression" dxfId="39" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="39" priority="16">
+    <cfRule type="expression" dxfId="38" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="38" priority="14">
+    <cfRule type="expression" dxfId="37" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="37" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="36" priority="12">
+    <cfRule type="expression" dxfId="35" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="34" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="33" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="34" priority="9">
+    <cfRule type="expression" dxfId="32" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="33" priority="8">
+    <cfRule type="expression" dxfId="31" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="32" priority="7">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="31" priority="6">
+    <cfRule type="expression" dxfId="29" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="28" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG35">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19792,11 +19781,11 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE85"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="Z22" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="R32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -28708,565 +28697,245 @@
       </c>
     </row>
     <row r="82" spans="3:29">
-      <c r="C82" s="21">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="D82" s="15">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="E82" s="21" t="str">
-        <f t="shared" ca="1" si="59"/>
-        <v>Tsub.0</v>
-      </c>
-      <c r="F82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="G82" s="13">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="H82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="I82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="J82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="K82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="L82" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="M82" s="18">
-        <f t="shared" ca="1" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="N82" s="13">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="O82" s="13">
-        <f t="shared" ca="1" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="P82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="Q82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="R82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="S82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="T82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="U82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="V82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="W82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="X82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="Y82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="Z82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="AA82" s="13">
-        <f t="shared" ca="1" si="56"/>
-        <v>0</v>
-      </c>
-      <c r="AB82" s="15">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="AC82" s="33">
-        <v>153</v>
-      </c>
+      <c r="C82" s="21"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="13"/>
+      <c r="O82" s="13"/>
+      <c r="P82" s="13"/>
+      <c r="Q82" s="13"/>
+      <c r="R82" s="13"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
+      <c r="U82" s="13"/>
+      <c r="V82" s="13"/>
+      <c r="W82" s="13"/>
+      <c r="X82" s="13"/>
+      <c r="Y82" s="13"/>
+      <c r="Z82" s="13"/>
+      <c r="AA82" s="13"/>
+      <c r="AB82" s="15"/>
+      <c r="AC82" s="33"/>
     </row>
     <row r="83" spans="3:29">
-      <c r="C83" s="21">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="D83" s="15">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="E83" s="21" t="str">
-        <f t="shared" ca="1" si="59"/>
-        <v>Tsub.0</v>
-      </c>
-      <c r="F83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="G83" s="13">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="H83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="I83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="J83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="K83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="L83" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="M83" s="18">
-        <f t="shared" ca="1" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="N83" s="13">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="O83" s="13">
-        <f t="shared" ca="1" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="P83" s="13">
-        <f t="shared" ref="P83:U85" ca="1" si="60">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>0</v>
-      </c>
-      <c r="Q83" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="R83" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="S83" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="T83" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="U83" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="V83" s="13">
-        <f t="shared" ref="V83:AA85" ca="1" si="61">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>0</v>
-      </c>
-      <c r="W83" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="X83" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Y83" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Z83" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AA83" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AB83" s="15">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="AC83" s="33">
-        <v>154</v>
-      </c>
+      <c r="C83" s="21"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="13"/>
+      <c r="O83" s="13"/>
+      <c r="P83" s="13"/>
+      <c r="Q83" s="13"/>
+      <c r="R83" s="13"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="13"/>
+      <c r="U83" s="13"/>
+      <c r="V83" s="13"/>
+      <c r="W83" s="13"/>
+      <c r="X83" s="13"/>
+      <c r="Y83" s="13"/>
+      <c r="Z83" s="13"/>
+      <c r="AA83" s="13"/>
+      <c r="AB83" s="15"/>
+      <c r="AC83" s="33"/>
     </row>
     <row r="84" spans="3:29">
-      <c r="C84" s="21">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="D84" s="15">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="E84" s="21" t="str">
-        <f t="shared" ca="1" si="59"/>
-        <v>Tsub.0</v>
-      </c>
-      <c r="F84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="G84" s="13">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="H84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="I84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="J84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="K84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="L84" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="M84" s="18">
-        <f t="shared" ca="1" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="N84" s="13">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="O84" s="13">
-        <f t="shared" ca="1" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="P84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="Q84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="R84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="S84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="T84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="U84" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="V84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="X84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Y84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Z84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AA84" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AB84" s="15">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="AC84" s="33">
-        <v>155</v>
-      </c>
+      <c r="C84" s="21"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="13"/>
+      <c r="O84" s="13"/>
+      <c r="P84" s="13"/>
+      <c r="Q84" s="13"/>
+      <c r="R84" s="13"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
+      <c r="U84" s="13"/>
+      <c r="V84" s="13"/>
+      <c r="W84" s="13"/>
+      <c r="X84" s="13"/>
+      <c r="Y84" s="13"/>
+      <c r="Z84" s="13"/>
+      <c r="AA84" s="13"/>
+      <c r="AB84" s="15"/>
+      <c r="AC84" s="33"/>
     </row>
     <row r="85" spans="3:29">
-      <c r="C85" s="21">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="D85" s="15">
-        <f t="shared" ca="1" si="57"/>
-        <v>0</v>
-      </c>
-      <c r="E85" s="21" t="str">
-        <f t="shared" ref="E85" ca="1" si="62">"Tsub." &amp; C85</f>
-        <v>Tsub.0</v>
-      </c>
-      <c r="F85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="G85" s="13">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="H85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="I85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="J85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="K85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="L85" s="18">
-        <f t="shared" ca="1" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="M85" s="18">
-        <f t="shared" ca="1" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="N85" s="13">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="O85" s="13">
-        <f t="shared" ca="1" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="P85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="Q85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="R85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="S85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="T85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="U85" s="13">
-        <f t="shared" ca="1" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="V85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="X85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Y85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="Z85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AA85" s="13">
-        <f t="shared" ca="1" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="AB85" s="15">
-        <f t="shared" ca="1" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="AC85" s="33">
-        <v>156</v>
-      </c>
+      <c r="C85" s="21"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="13"/>
+      <c r="R85" s="13"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="13"/>
+      <c r="U85" s="13"/>
+      <c r="V85" s="13"/>
+      <c r="W85" s="13"/>
+      <c r="X85" s="13"/>
+      <c r="Y85" s="13"/>
+      <c r="Z85" s="13"/>
+      <c r="AA85" s="13"/>
+      <c r="AB85" s="15"/>
+      <c r="AC85" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="26" priority="146">
+    <cfRule type="expression" dxfId="24" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="25" priority="86">
+    <cfRule type="expression" dxfId="23" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="24" priority="74">
+    <cfRule type="expression" dxfId="22" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="23" priority="72">
+    <cfRule type="expression" dxfId="21" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="22" priority="73">
+    <cfRule type="expression" dxfId="20" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="21" priority="71">
+    <cfRule type="expression" dxfId="19" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="20" priority="68">
+    <cfRule type="expression" dxfId="18" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="19" priority="62">
+    <cfRule type="expression" dxfId="17" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="18" priority="53">
+    <cfRule type="expression" dxfId="16" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="17" priority="52">
+    <cfRule type="expression" dxfId="15" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="16" priority="32">
+    <cfRule type="expression" dxfId="14" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="15" priority="28">
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="14" priority="27">
+    <cfRule type="expression" dxfId="12" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="13" priority="25">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="11" priority="21">
+    <cfRule type="expression" dxfId="9" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="10" priority="19">
+    <cfRule type="expression" dxfId="8" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added link for Reedbush-H offers. Changed update date.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="0" windowWidth="25180" windowHeight="28260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="37000" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="418">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -2322,6 +2322,17 @@
   <si>
     <t>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU ded. rev edu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TU ded. rev</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</t>
   </si>
 </sst>
 </file>
@@ -2663,7 +2674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1157">
+  <cellStyleXfs count="1159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3498,6 +3509,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3926,7 +3939,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1157">
+  <cellStyles count="1159">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -4572,6 +4585,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1158" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -5074,6 +5088,7 @@
     <cellStyle name="Hyperlink" xfId="1151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1157" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -5085,7 +5100,62 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="152">
+  <dxfs count="157">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -7056,10 +7126,10 @@
   <dimension ref="A1:FJ158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AK106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A156" sqref="A156"/>
+      <selection pane="bottomRight" activeCell="AM104" sqref="AM104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9793,6 +9863,7 @@
       <c r="AI37" s="13"/>
       <c r="AJ37" s="13"/>
       <c r="AK37" s="15"/>
+      <c r="AL37" s="15"/>
     </row>
     <row r="38" spans="1:166" s="12" customFormat="1">
       <c r="A38" s="15"/>
@@ -9832,6 +9903,7 @@
       <c r="AI38" s="13"/>
       <c r="AJ38" s="13"/>
       <c r="AK38" s="15"/>
+      <c r="AL38" s="15"/>
     </row>
     <row r="39" spans="1:166" s="12" customFormat="1">
       <c r="A39" s="15"/>
@@ -9871,6 +9943,7 @@
       <c r="AI39" s="13"/>
       <c r="AJ39" s="13"/>
       <c r="AK39" s="15"/>
+      <c r="AL39" s="15"/>
     </row>
     <row r="40" spans="1:166" s="12" customFormat="1">
       <c r="A40" s="15"/>
@@ -9910,6 +9983,7 @@
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
       <c r="AK40" s="15"/>
+      <c r="AL40" s="15"/>
     </row>
     <row r="41" spans="1:166" s="12" customFormat="1">
       <c r="A41" s="15"/>
@@ -9949,6 +10023,7 @@
       <c r="AI41" s="13"/>
       <c r="AJ41" s="13"/>
       <c r="AK41" s="15"/>
+      <c r="AL41" s="15"/>
     </row>
     <row r="42" spans="1:166" s="12" customFormat="1">
       <c r="A42" s="15"/>
@@ -9988,6 +10063,7 @@
       <c r="AI42" s="13"/>
       <c r="AJ42" s="13"/>
       <c r="AK42" s="15"/>
+      <c r="AL42" s="15"/>
     </row>
     <row r="43" spans="1:166">
       <c r="B43" s="21"/>
@@ -10023,6 +10099,7 @@
       <c r="AF43" s="23"/>
       <c r="AG43" s="23"/>
       <c r="AH43" s="15"/>
+      <c r="AL43" s="15"/>
     </row>
     <row r="44" spans="1:166" ht="20">
       <c r="A44" s="20" t="s">
@@ -10111,6 +10188,7 @@
       <c r="AK44" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="AL44" s="15"/>
     </row>
     <row r="45" spans="1:166" s="12" customFormat="1">
       <c r="A45" s="15" t="s">
@@ -10201,6 +10279,7 @@
       <c r="AK45" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="AL45" s="15"/>
     </row>
     <row r="46" spans="1:166" s="12" customFormat="1">
       <c r="A46" s="15"/>
@@ -10289,6 +10368,7 @@
       <c r="AK46" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="AL46" s="15"/>
       <c r="AO46" s="31"/>
       <c r="AP46" s="31"/>
       <c r="AQ46" s="31"/>
@@ -10502,6 +10582,7 @@
       <c r="AK47" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="AL47" s="15"/>
     </row>
     <row r="48" spans="1:166" s="12" customFormat="1" ht="20">
       <c r="A48" s="30"/>
@@ -10590,6 +10671,7 @@
       <c r="AK48" s="15" t="s">
         <v>405</v>
       </c>
+      <c r="AL48" s="15"/>
       <c r="AO48" s="31"/>
       <c r="AP48" s="31"/>
       <c r="AQ48" s="31"/>
@@ -10717,7 +10799,7 @@
       <c r="FI48" s="31"/>
       <c r="FJ48" s="31"/>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:38">
       <c r="A49" s="15" t="s">
         <v>197</v>
       </c>
@@ -10804,8 +10886,12 @@
       <c r="AK49" s="15" t="s">
         <v>406</v>
       </c>
+      <c r="AL49" s="15"/>
     </row>
-    <row r="51" spans="1:37" s="12" customFormat="1">
+    <row r="50" spans="1:38">
+      <c r="AL50" s="15"/>
+    </row>
+    <row r="51" spans="1:38" s="12" customFormat="1">
       <c r="A51" s="15"/>
       <c r="B51" s="21"/>
       <c r="C51" s="26"/>
@@ -10841,8 +10927,9 @@
       <c r="AI51" s="13"/>
       <c r="AJ51" s="13"/>
       <c r="AK51" s="15"/>
+      <c r="AL51" s="15"/>
     </row>
-    <row r="52" spans="1:37" s="12" customFormat="1">
+    <row r="52" spans="1:38" s="12" customFormat="1">
       <c r="A52" s="15"/>
       <c r="B52" s="21"/>
       <c r="C52" s="26"/>
@@ -10878,8 +10965,9 @@
       <c r="AI52" s="13"/>
       <c r="AJ52" s="13"/>
       <c r="AK52" s="15"/>
+      <c r="AL52" s="15"/>
     </row>
-    <row r="53" spans="1:37" s="12" customFormat="1">
+    <row r="53" spans="1:38" s="12" customFormat="1">
       <c r="A53" s="15"/>
       <c r="B53" s="21"/>
       <c r="C53" s="26"/>
@@ -10915,8 +11003,9 @@
       <c r="AI53" s="13"/>
       <c r="AJ53" s="13"/>
       <c r="AK53" s="15"/>
+      <c r="AL53" s="15"/>
     </row>
-    <row r="54" spans="1:37" s="12" customFormat="1">
+    <row r="54" spans="1:38" s="12" customFormat="1">
       <c r="A54" s="15"/>
       <c r="B54" s="21"/>
       <c r="C54" s="26"/>
@@ -10952,8 +11041,9 @@
       <c r="AI54" s="13"/>
       <c r="AJ54" s="13"/>
       <c r="AK54" s="15"/>
+      <c r="AL54" s="15"/>
     </row>
-    <row r="55" spans="1:37" s="12" customFormat="1">
+    <row r="55" spans="1:38" s="12" customFormat="1">
       <c r="A55" s="15"/>
       <c r="B55" s="21"/>
       <c r="C55" s="26"/>
@@ -10989,8 +11079,9 @@
       <c r="AI55" s="13"/>
       <c r="AJ55" s="13"/>
       <c r="AK55" s="15"/>
+      <c r="AL55" s="15"/>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:38">
       <c r="A56" s="15"/>
       <c r="B56" s="21"/>
       <c r="C56" s="26"/>
@@ -11023,8 +11114,9 @@
       <c r="AF56" s="23"/>
       <c r="AG56" s="23"/>
       <c r="AH56" s="15"/>
+      <c r="AL56" s="15"/>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:38">
       <c r="B57" s="21"/>
       <c r="C57" s="26"/>
       <c r="E57" s="13"/>
@@ -11056,8 +11148,9 @@
       <c r="AF57" s="23"/>
       <c r="AG57" s="23"/>
       <c r="AH57" s="15"/>
+      <c r="AL57" s="15"/>
     </row>
-    <row r="58" spans="1:37" ht="20">
+    <row r="58" spans="1:38" ht="20">
       <c r="A58" s="20" t="s">
         <v>40</v>
       </c>
@@ -11146,8 +11239,9 @@
       <c r="AK58" s="15" t="s">
         <v>360</v>
       </c>
+      <c r="AL58" s="15"/>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:38">
       <c r="A59" s="15" t="s">
         <v>244</v>
       </c>
@@ -11236,8 +11330,9 @@
       <c r="AK59" s="15" t="s">
         <v>360</v>
       </c>
+      <c r="AL59" s="15"/>
     </row>
-    <row r="60" spans="1:37" s="12" customFormat="1">
+    <row r="60" spans="1:38" s="12" customFormat="1">
       <c r="A60" s="2"/>
       <c r="B60" s="21" t="s">
         <v>164</v>
@@ -11324,8 +11419,9 @@
       <c r="AI60" s="13"/>
       <c r="AJ60" s="13"/>
       <c r="AK60" s="15"/>
+      <c r="AL60" s="15"/>
     </row>
-    <row r="61" spans="1:37" s="12" customFormat="1">
+    <row r="61" spans="1:38" s="12" customFormat="1">
       <c r="A61" s="2"/>
       <c r="B61" s="21" t="s">
         <v>165</v>
@@ -11412,8 +11508,9 @@
       <c r="AI61" s="13"/>
       <c r="AJ61" s="13"/>
       <c r="AK61" s="15"/>
+      <c r="AL61" s="15"/>
     </row>
-    <row r="62" spans="1:37" s="12" customFormat="1">
+    <row r="62" spans="1:38" s="12" customFormat="1">
       <c r="A62" s="2"/>
       <c r="B62" s="21" t="s">
         <v>166</v>
@@ -11500,8 +11597,9 @@
       <c r="AI62" s="13"/>
       <c r="AJ62" s="13"/>
       <c r="AK62" s="15"/>
+      <c r="AL62" s="15"/>
     </row>
-    <row r="63" spans="1:37" s="12" customFormat="1">
+    <row r="63" spans="1:38" s="12" customFormat="1">
       <c r="A63" s="2"/>
       <c r="B63" s="21" t="s">
         <v>167</v>
@@ -11588,8 +11686,9 @@
       <c r="AI63" s="13"/>
       <c r="AJ63" s="13"/>
       <c r="AK63" s="15"/>
+      <c r="AL63" s="15"/>
     </row>
-    <row r="64" spans="1:37" s="12" customFormat="1">
+    <row r="64" spans="1:38" s="12" customFormat="1">
       <c r="A64" s="2"/>
       <c r="B64" s="21" t="s">
         <v>168</v>
@@ -11676,6 +11775,7 @@
       <c r="AI64" s="13"/>
       <c r="AJ64" s="13"/>
       <c r="AK64" s="15"/>
+      <c r="AL64" s="15"/>
     </row>
     <row r="65" spans="1:166" s="12" customFormat="1">
       <c r="A65" s="2"/>
@@ -11764,6 +11864,7 @@
       <c r="AI65" s="13"/>
       <c r="AJ65" s="13"/>
       <c r="AK65" s="15"/>
+      <c r="AL65" s="15"/>
     </row>
     <row r="66" spans="1:166">
       <c r="B66" s="21" t="s">
@@ -11859,6 +11960,7 @@
       <c r="AK66" s="15" t="s">
         <v>77</v>
       </c>
+      <c r="AL66" s="15"/>
     </row>
     <row r="67" spans="1:166">
       <c r="B67" s="21" t="s">
@@ -11945,6 +12047,7 @@
       <c r="AH67" s="15" t="s">
         <v>128</v>
       </c>
+      <c r="AL67" s="15"/>
     </row>
     <row r="68" spans="1:166" s="12" customFormat="1">
       <c r="A68" s="2"/>
@@ -12031,6 +12134,7 @@
       <c r="AI68" s="13"/>
       <c r="AJ68" s="13"/>
       <c r="AK68" s="15"/>
+      <c r="AL68" s="15"/>
       <c r="AO68" s="32"/>
       <c r="AP68" s="32"/>
       <c r="AQ68" s="32"/>
@@ -12195,6 +12299,7 @@
       <c r="AI69" s="13"/>
       <c r="AJ69" s="13"/>
       <c r="AK69" s="15"/>
+      <c r="AL69" s="15"/>
       <c r="AO69" s="32"/>
       <c r="AP69" s="32"/>
       <c r="AQ69" s="32"/>
@@ -12359,6 +12464,7 @@
       <c r="AI70" s="13"/>
       <c r="AJ70" s="13"/>
       <c r="AK70" s="15"/>
+      <c r="AL70" s="15"/>
       <c r="AO70" s="32"/>
       <c r="AP70" s="32"/>
       <c r="AQ70" s="32"/>
@@ -12523,6 +12629,7 @@
       <c r="AI71" s="13"/>
       <c r="AJ71" s="13"/>
       <c r="AK71" s="15"/>
+      <c r="AL71" s="15"/>
       <c r="AO71" s="32"/>
       <c r="AP71" s="32"/>
       <c r="AQ71" s="32"/>
@@ -12687,6 +12794,7 @@
       <c r="AI72" s="13"/>
       <c r="AJ72" s="13"/>
       <c r="AK72" s="15"/>
+      <c r="AL72" s="15"/>
       <c r="AO72" s="32"/>
       <c r="AP72" s="32"/>
       <c r="AQ72" s="32"/>
@@ -12851,6 +12959,7 @@
       <c r="AI73" s="13"/>
       <c r="AJ73" s="13"/>
       <c r="AK73" s="15"/>
+      <c r="AL73" s="15"/>
       <c r="AO73" s="32"/>
       <c r="AP73" s="32"/>
       <c r="AQ73" s="32"/>
@@ -13015,6 +13124,7 @@
       <c r="AI74" s="13"/>
       <c r="AJ74" s="13"/>
       <c r="AK74" s="15"/>
+      <c r="AL74" s="15"/>
       <c r="AO74" s="32"/>
       <c r="AP74" s="32"/>
       <c r="AQ74" s="32"/>
@@ -13179,6 +13289,7 @@
       <c r="AI75" s="13"/>
       <c r="AJ75" s="13"/>
       <c r="AK75" s="15"/>
+      <c r="AL75" s="15"/>
       <c r="AO75" s="32"/>
       <c r="AP75" s="32"/>
       <c r="AQ75" s="32"/>
@@ -13340,6 +13451,7 @@
       <c r="AF76" s="23"/>
       <c r="AG76" s="23"/>
       <c r="AH76" s="15"/>
+      <c r="AL76" s="15"/>
     </row>
     <row r="77" spans="1:166" ht="20">
       <c r="A77" s="20" t="s">
@@ -13434,6 +13546,7 @@
       <c r="AH77" s="15" t="s">
         <v>136</v>
       </c>
+      <c r="AL77" s="15"/>
     </row>
     <row r="78" spans="1:166" s="12" customFormat="1">
       <c r="A78" s="15" t="s">
@@ -13531,6 +13644,7 @@
       <c r="AI78" s="13"/>
       <c r="AJ78" s="13"/>
       <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
     </row>
     <row r="79" spans="1:166" s="12" customFormat="1">
       <c r="A79" s="21"/>
@@ -13626,6 +13740,7 @@
       <c r="AI79" s="13"/>
       <c r="AJ79" s="13"/>
       <c r="AK79" s="15"/>
+      <c r="AL79" s="15"/>
     </row>
     <row r="80" spans="1:166">
       <c r="A80" s="21"/>
@@ -13718,6 +13833,7 @@
       <c r="AH80" s="15" t="s">
         <v>136</v>
       </c>
+      <c r="AL80" s="15"/>
     </row>
     <row r="81" spans="1:41">
       <c r="A81" s="21"/>
@@ -13812,6 +13928,7 @@
       <c r="AH81" s="15" t="s">
         <v>136</v>
       </c>
+      <c r="AL81" s="15"/>
     </row>
     <row r="82" spans="1:41" s="12" customFormat="1">
       <c r="A82" s="21"/>
@@ -13909,6 +14026,7 @@
       <c r="AI82" s="13"/>
       <c r="AJ82" s="13"/>
       <c r="AK82" s="15"/>
+      <c r="AL82" s="15"/>
     </row>
     <row r="83" spans="1:41" s="12" customFormat="1">
       <c r="A83" s="21"/>
@@ -14006,6 +14124,7 @@
       <c r="AI83" s="13"/>
       <c r="AJ83" s="13"/>
       <c r="AK83" s="15"/>
+      <c r="AL83" s="15"/>
     </row>
     <row r="84" spans="1:41" s="12" customFormat="1">
       <c r="A84" s="21"/>
@@ -14045,6 +14164,7 @@
       <c r="AI84" s="39"/>
       <c r="AJ84" s="39"/>
       <c r="AK84" s="15"/>
+      <c r="AL84" s="15"/>
     </row>
     <row r="85" spans="1:41" s="12" customFormat="1">
       <c r="A85" s="21"/>
@@ -14084,6 +14204,7 @@
       <c r="AI85" s="39"/>
       <c r="AJ85" s="39"/>
       <c r="AK85" s="15"/>
+      <c r="AL85" s="15"/>
     </row>
     <row r="86" spans="1:41" s="12" customFormat="1">
       <c r="A86" s="21"/>
@@ -14123,6 +14244,7 @@
       <c r="AI86" s="13"/>
       <c r="AJ86" s="13"/>
       <c r="AK86" s="15"/>
+      <c r="AL86" s="15"/>
     </row>
     <row r="87" spans="1:41" s="12" customFormat="1">
       <c r="A87" s="21"/>
@@ -14162,6 +14284,7 @@
       <c r="AI87" s="13"/>
       <c r="AJ87" s="13"/>
       <c r="AK87" s="15"/>
+      <c r="AL87" s="15"/>
     </row>
     <row r="88" spans="1:41" ht="23" customHeight="1">
       <c r="A88" s="20" t="s">
@@ -14260,7 +14383,7 @@
       <c r="AK88" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="AL88" s="13"/>
+      <c r="AL88" s="15"/>
       <c r="AM88" s="13"/>
       <c r="AN88" s="13"/>
       <c r="AO88" s="13"/>
@@ -14362,7 +14485,7 @@
       <c r="AK89" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="AL89" s="13"/>
+      <c r="AL89" s="15"/>
       <c r="AM89" s="13"/>
       <c r="AN89" s="13"/>
       <c r="AO89" s="13"/>
@@ -14460,7 +14583,7 @@
       <c r="AK90" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="AL90" s="13"/>
+      <c r="AL90" s="15"/>
       <c r="AM90" s="13"/>
       <c r="AN90" s="13"/>
       <c r="AO90" s="13"/>
@@ -14558,7 +14681,7 @@
       <c r="AK91" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="AL91" s="13"/>
+      <c r="AL91" s="15"/>
       <c r="AM91" s="13"/>
       <c r="AN91" s="13"/>
       <c r="AO91" s="13"/>
@@ -14658,7 +14781,7 @@
       <c r="AK92" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="AL92" s="13"/>
+      <c r="AL92" s="15"/>
       <c r="AM92" s="13"/>
       <c r="AN92" s="13"/>
       <c r="AO92" s="13"/>
@@ -14758,7 +14881,7 @@
       <c r="AK93" s="15" t="s">
         <v>408</v>
       </c>
-      <c r="AL93" s="13"/>
+      <c r="AL93" s="15"/>
       <c r="AM93" s="13"/>
       <c r="AN93" s="13"/>
       <c r="AO93" s="13"/>
@@ -14801,7 +14924,7 @@
       <c r="AI94" s="13"/>
       <c r="AJ94" s="13"/>
       <c r="AK94" s="15"/>
-      <c r="AL94" s="13"/>
+      <c r="AL94" s="15"/>
       <c r="AM94" s="13"/>
       <c r="AN94" s="13"/>
       <c r="AO94" s="13"/>
@@ -14844,7 +14967,7 @@
       <c r="AI95" s="13"/>
       <c r="AJ95" s="13"/>
       <c r="AK95" s="15"/>
-      <c r="AL95" s="13"/>
+      <c r="AL95" s="15"/>
       <c r="AM95" s="13"/>
       <c r="AN95" s="13"/>
       <c r="AO95" s="13"/>
@@ -14887,7 +15010,7 @@
       <c r="AI96" s="13"/>
       <c r="AJ96" s="13"/>
       <c r="AK96" s="15"/>
-      <c r="AL96" s="13"/>
+      <c r="AL96" s="15"/>
       <c r="AM96" s="13"/>
       <c r="AN96" s="13"/>
       <c r="AO96" s="13"/>
@@ -14930,7 +15053,7 @@
       <c r="AI97" s="13"/>
       <c r="AJ97" s="13"/>
       <c r="AK97" s="15"/>
-      <c r="AL97" s="13"/>
+      <c r="AL97" s="15"/>
       <c r="AM97" s="13"/>
       <c r="AN97" s="13"/>
       <c r="AO97" s="13"/>
@@ -14973,7 +15096,7 @@
       <c r="AI98" s="13"/>
       <c r="AJ98" s="13"/>
       <c r="AK98" s="15"/>
-      <c r="AL98" s="13"/>
+      <c r="AL98" s="15"/>
       <c r="AM98" s="13"/>
       <c r="AN98" s="13"/>
       <c r="AO98" s="13"/>
@@ -15016,7 +15139,7 @@
       <c r="AI99" s="13"/>
       <c r="AJ99" s="13"/>
       <c r="AK99" s="15"/>
-      <c r="AL99" s="13"/>
+      <c r="AL99" s="15"/>
       <c r="AM99" s="13"/>
       <c r="AN99" s="13"/>
       <c r="AO99" s="13"/>
@@ -15117,7 +15240,9 @@
       <c r="AK100" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="AL100" s="13"/>
+      <c r="AL100" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM100" s="13"/>
       <c r="AN100" s="13"/>
       <c r="AO100" s="13"/>
@@ -15218,7 +15343,9 @@
       <c r="AK101" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="AL101" s="13"/>
+      <c r="AL101" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM101" s="13"/>
       <c r="AN101" s="13"/>
       <c r="AO101" s="13"/>
@@ -15317,7 +15444,9 @@
       <c r="AK102" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="AL102" s="13"/>
+      <c r="AL102" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM102" s="13"/>
       <c r="AN102" s="13"/>
       <c r="AO102" s="13"/>
@@ -15416,7 +15545,9 @@
       <c r="AK103" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="AL103" s="13"/>
+      <c r="AL103" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM103" s="13"/>
       <c r="AN103" s="13"/>
       <c r="AO103" s="13"/>
@@ -15516,7 +15647,9 @@
       <c r="AK104" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="AL104" s="13"/>
+      <c r="AL104" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM104" s="13"/>
       <c r="AN104" s="13"/>
       <c r="AO104" s="13"/>
@@ -15615,7 +15748,9 @@
       <c r="AK105" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="AL105" s="13"/>
+      <c r="AL105" s="15" t="s">
+        <v>417</v>
+      </c>
       <c r="AM105" s="13"/>
       <c r="AN105" s="13"/>
       <c r="AO105" s="13"/>
@@ -15658,7 +15793,7 @@
       <c r="AI106" s="13"/>
       <c r="AJ106" s="13"/>
       <c r="AK106" s="15"/>
-      <c r="AL106" s="13"/>
+      <c r="AL106" s="15"/>
       <c r="AM106" s="13"/>
       <c r="AN106" s="13"/>
       <c r="AO106" s="13"/>
@@ -15701,7 +15836,7 @@
       <c r="AI107" s="13"/>
       <c r="AJ107" s="13"/>
       <c r="AK107" s="15"/>
-      <c r="AL107" s="13"/>
+      <c r="AL107" s="15"/>
       <c r="AM107" s="13"/>
       <c r="AN107" s="13"/>
       <c r="AO107" s="13"/>
@@ -15744,7 +15879,7 @@
       <c r="AI108" s="13"/>
       <c r="AJ108" s="13"/>
       <c r="AK108" s="15"/>
-      <c r="AL108" s="13"/>
+      <c r="AL108" s="15"/>
       <c r="AM108" s="13"/>
       <c r="AN108" s="13"/>
       <c r="AO108" s="13"/>
@@ -15787,7 +15922,7 @@
       <c r="AI109" s="13"/>
       <c r="AJ109" s="13"/>
       <c r="AK109" s="15"/>
-      <c r="AL109" s="13"/>
+      <c r="AL109" s="15"/>
       <c r="AM109" s="13"/>
       <c r="AN109" s="13"/>
       <c r="AO109" s="13"/>
@@ -15830,7 +15965,7 @@
       <c r="AI110" s="13"/>
       <c r="AJ110" s="13"/>
       <c r="AK110" s="15"/>
-      <c r="AL110" s="13"/>
+      <c r="AL110" s="15"/>
       <c r="AM110" s="13"/>
       <c r="AN110" s="13"/>
       <c r="AO110" s="13"/>
@@ -15873,7 +16008,7 @@
       <c r="AI111" s="13"/>
       <c r="AJ111" s="13"/>
       <c r="AK111" s="15"/>
-      <c r="AL111" s="13"/>
+      <c r="AL111" s="15"/>
       <c r="AM111" s="13"/>
       <c r="AN111" s="13"/>
       <c r="AO111" s="13"/>
@@ -15916,7 +16051,7 @@
       <c r="AI112" s="13"/>
       <c r="AJ112" s="13"/>
       <c r="AK112" s="15"/>
-      <c r="AL112" s="13"/>
+      <c r="AL112" s="15"/>
       <c r="AM112" s="13"/>
       <c r="AN112" s="13"/>
       <c r="AO112" s="13"/>
@@ -15959,7 +16094,7 @@
       <c r="AI113" s="13"/>
       <c r="AJ113" s="13"/>
       <c r="AK113" s="15"/>
-      <c r="AL113" s="13"/>
+      <c r="AL113" s="15"/>
       <c r="AM113" s="13"/>
       <c r="AN113" s="13"/>
       <c r="AO113" s="13"/>
@@ -16050,7 +16185,7 @@
       <c r="AK114" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="AL114" s="13"/>
+      <c r="AL114" s="15"/>
       <c r="AM114" s="13"/>
       <c r="AN114" s="13"/>
       <c r="AO114" s="13"/>
@@ -16138,7 +16273,7 @@
       <c r="AH115" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AL115" s="13"/>
+      <c r="AL115" s="15"/>
       <c r="AM115" s="13"/>
       <c r="AN115" s="13"/>
       <c r="AO115" s="13"/>
@@ -16226,7 +16361,7 @@
       <c r="AH116" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AL116" s="13"/>
+      <c r="AL116" s="15"/>
       <c r="AM116" s="13"/>
       <c r="AN116" s="13"/>
       <c r="AO116" s="13"/>
@@ -16320,7 +16455,7 @@
       <c r="AK117" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="AL117" s="13"/>
+      <c r="AL117" s="15"/>
       <c r="AM117" s="13"/>
       <c r="AN117" s="13"/>
       <c r="AO117" s="13"/>
@@ -16403,7 +16538,7 @@
       <c r="AH118" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AL118" s="13"/>
+      <c r="AL118" s="15"/>
       <c r="AM118" s="13"/>
       <c r="AN118" s="13"/>
       <c r="AO118" s="13"/>
@@ -16486,7 +16621,7 @@
       <c r="AH119" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="AL119" s="13"/>
+      <c r="AL119" s="15"/>
       <c r="AM119" s="13"/>
       <c r="AN119" s="13"/>
       <c r="AO119" s="13"/>
@@ -16570,7 +16705,7 @@
         <v>149</v>
       </c>
       <c r="AK120" s="13"/>
-      <c r="AL120" s="13"/>
+      <c r="AL120" s="15"/>
       <c r="AM120" s="13"/>
       <c r="AN120" s="13"/>
       <c r="AO120" s="13"/>
@@ -16613,7 +16748,7 @@
       <c r="AI121" s="13"/>
       <c r="AJ121" s="13"/>
       <c r="AK121" s="13"/>
-      <c r="AL121" s="13"/>
+      <c r="AL121" s="15"/>
       <c r="AM121" s="13"/>
       <c r="AN121" s="13"/>
       <c r="AO121" s="13"/>
@@ -16656,7 +16791,7 @@
       <c r="AI122" s="13"/>
       <c r="AJ122" s="13"/>
       <c r="AK122" s="13"/>
-      <c r="AL122" s="13"/>
+      <c r="AL122" s="15"/>
       <c r="AM122" s="13"/>
       <c r="AN122" s="13"/>
       <c r="AO122" s="13"/>
@@ -16699,7 +16834,7 @@
       <c r="AI123" s="13"/>
       <c r="AJ123" s="13"/>
       <c r="AK123" s="13"/>
-      <c r="AL123" s="13"/>
+      <c r="AL123" s="15"/>
       <c r="AM123" s="13"/>
       <c r="AN123" s="13"/>
       <c r="AO123" s="13"/>
@@ -16742,7 +16877,7 @@
       <c r="AI124" s="13"/>
       <c r="AJ124" s="13"/>
       <c r="AK124" s="13"/>
-      <c r="AL124" s="13"/>
+      <c r="AL124" s="15"/>
       <c r="AM124" s="13"/>
       <c r="AN124" s="13"/>
       <c r="AO124" s="13"/>
@@ -16785,7 +16920,7 @@
       <c r="AI125" s="13"/>
       <c r="AJ125" s="13"/>
       <c r="AK125" s="13"/>
-      <c r="AL125" s="13"/>
+      <c r="AL125" s="15"/>
       <c r="AM125" s="13"/>
       <c r="AN125" s="13"/>
       <c r="AO125" s="13"/>
@@ -16828,7 +16963,7 @@
       <c r="AI126" s="13"/>
       <c r="AJ126" s="13"/>
       <c r="AK126" s="13"/>
-      <c r="AL126" s="13"/>
+      <c r="AL126" s="15"/>
       <c r="AM126" s="13"/>
       <c r="AN126" s="13"/>
       <c r="AO126" s="13"/>
@@ -16871,7 +17006,7 @@
       <c r="AI127" s="13"/>
       <c r="AJ127" s="13"/>
       <c r="AK127" s="13"/>
-      <c r="AL127" s="13"/>
+      <c r="AL127" s="15"/>
       <c r="AM127" s="13"/>
       <c r="AN127" s="13"/>
       <c r="AO127" s="13"/>
@@ -16912,7 +17047,7 @@
       <c r="AG128" s="13"/>
       <c r="AH128" s="15"/>
       <c r="AK128" s="13"/>
-      <c r="AL128" s="13"/>
+      <c r="AL128" s="15"/>
       <c r="AM128" s="13"/>
       <c r="AN128" s="13"/>
       <c r="AO128" s="13"/>
@@ -16987,7 +17122,7 @@
       <c r="AK129" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AL129" s="13"/>
+      <c r="AL129" s="15"/>
       <c r="AM129" s="13"/>
       <c r="AN129" s="13"/>
       <c r="AO129" s="13"/>
@@ -17062,7 +17197,7 @@
       <c r="AK130" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AL130" s="13"/>
+      <c r="AL130" s="15"/>
       <c r="AM130" s="13"/>
       <c r="AN130" s="13"/>
       <c r="AO130" s="13"/>
@@ -17137,7 +17272,7 @@
       <c r="AK131" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AL131" s="13"/>
+      <c r="AL131" s="15"/>
       <c r="AM131" s="13"/>
       <c r="AN131" s="13"/>
       <c r="AO131" s="13"/>
@@ -17210,7 +17345,7 @@
       <c r="AK132" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AL132" s="13"/>
+      <c r="AL132" s="15"/>
       <c r="AM132" s="13"/>
       <c r="AN132" s="13"/>
       <c r="AO132" s="13"/>
@@ -17283,7 +17418,7 @@
       <c r="AK133" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="AL133" s="13"/>
+      <c r="AL133" s="15"/>
       <c r="AM133" s="13"/>
       <c r="AN133" s="13"/>
       <c r="AO133" s="13"/>
@@ -17323,7 +17458,7 @@
       <c r="AF134" s="13"/>
       <c r="AG134" s="13"/>
       <c r="AH134" s="15"/>
-      <c r="AL134" s="13"/>
+      <c r="AL134" s="15"/>
       <c r="AM134" s="13"/>
       <c r="AN134" s="13"/>
       <c r="AO134" s="13"/>
@@ -17363,7 +17498,7 @@
       <c r="AF135" s="13"/>
       <c r="AG135" s="13"/>
       <c r="AH135" s="15"/>
-      <c r="AL135" s="13"/>
+      <c r="AL135" s="15"/>
       <c r="AM135" s="13"/>
       <c r="AN135" s="13"/>
       <c r="AO135" s="13"/>
@@ -17403,7 +17538,7 @@
       <c r="AF136" s="13"/>
       <c r="AG136" s="13"/>
       <c r="AH136" s="15"/>
-      <c r="AL136" s="13"/>
+      <c r="AL136" s="15"/>
       <c r="AM136" s="13"/>
       <c r="AN136" s="13"/>
       <c r="AO136" s="13"/>
@@ -17443,7 +17578,7 @@
       <c r="AF137" s="13"/>
       <c r="AG137" s="13"/>
       <c r="AH137" s="15"/>
-      <c r="AL137" s="13"/>
+      <c r="AL137" s="15"/>
       <c r="AM137" s="13"/>
       <c r="AN137" s="13"/>
       <c r="AO137" s="13"/>
@@ -17483,7 +17618,7 @@
       <c r="AF138" s="13"/>
       <c r="AG138" s="13"/>
       <c r="AH138" s="15"/>
-      <c r="AL138" s="13"/>
+      <c r="AL138" s="15"/>
       <c r="AM138" s="13"/>
       <c r="AN138" s="13"/>
       <c r="AO138" s="13"/>
@@ -17523,7 +17658,7 @@
       <c r="AF139" s="13"/>
       <c r="AG139" s="13"/>
       <c r="AH139" s="15"/>
-      <c r="AL139" s="13"/>
+      <c r="AL139" s="15"/>
       <c r="AM139" s="13"/>
       <c r="AN139" s="13"/>
       <c r="AO139" s="13"/>
@@ -17563,7 +17698,7 @@
       <c r="AF140" s="13"/>
       <c r="AG140" s="13"/>
       <c r="AH140" s="15"/>
-      <c r="AL140" s="13"/>
+      <c r="AL140" s="15"/>
       <c r="AM140" s="13"/>
       <c r="AN140" s="13"/>
       <c r="AO140" s="13"/>
@@ -17653,7 +17788,7 @@
       <c r="AK141" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="AL141" s="13"/>
+      <c r="AL141" s="15"/>
       <c r="AM141" s="13"/>
       <c r="AN141" s="13"/>
       <c r="AO141" s="13"/>
@@ -17743,7 +17878,7 @@
       <c r="AK142" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="AL142" s="13"/>
+      <c r="AL142" s="15"/>
       <c r="AM142" s="13"/>
       <c r="AN142" s="13"/>
       <c r="AO142" s="13"/>
@@ -17783,7 +17918,7 @@
       <c r="AF143" s="13"/>
       <c r="AG143" s="13"/>
       <c r="AH143" s="15"/>
-      <c r="AL143" s="13"/>
+      <c r="AL143" s="15"/>
       <c r="AM143" s="13"/>
       <c r="AN143" s="13"/>
       <c r="AO143" s="13"/>
@@ -17823,7 +17958,7 @@
       <c r="AF144" s="13"/>
       <c r="AG144" s="13"/>
       <c r="AH144" s="15"/>
-      <c r="AL144" s="13"/>
+      <c r="AL144" s="15"/>
       <c r="AM144" s="13"/>
       <c r="AN144" s="13"/>
       <c r="AO144" s="13"/>
@@ -17863,7 +17998,7 @@
       <c r="AF145" s="13"/>
       <c r="AG145" s="13"/>
       <c r="AH145" s="15"/>
-      <c r="AL145" s="13"/>
+      <c r="AL145" s="15"/>
       <c r="AM145" s="13"/>
       <c r="AN145" s="13"/>
       <c r="AO145" s="13"/>
@@ -17903,7 +18038,7 @@
       <c r="AF146" s="13"/>
       <c r="AG146" s="13"/>
       <c r="AH146" s="15"/>
-      <c r="AL146" s="13"/>
+      <c r="AL146" s="15"/>
       <c r="AM146" s="13"/>
       <c r="AN146" s="13"/>
       <c r="AO146" s="13"/>
@@ -18002,7 +18137,7 @@
       <c r="AK147" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="AL147" s="13"/>
+      <c r="AL147" s="15"/>
       <c r="AM147" s="13"/>
       <c r="AN147" s="13"/>
       <c r="AO147" s="13"/>
@@ -18101,7 +18236,7 @@
       <c r="AK148" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="AL148" s="13"/>
+      <c r="AL148" s="15"/>
       <c r="AM148" s="13"/>
       <c r="AN148" s="13"/>
       <c r="AO148" s="13"/>
@@ -18199,7 +18334,7 @@
       <c r="AK149" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="AL149" s="13"/>
+      <c r="AL149" s="15"/>
       <c r="AM149" s="13"/>
       <c r="AN149" s="13"/>
       <c r="AO149" s="13"/>
@@ -18297,7 +18432,7 @@
       <c r="AK150" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="AL150" s="13"/>
+      <c r="AL150" s="15"/>
       <c r="AM150" s="13"/>
       <c r="AN150" s="13"/>
       <c r="AO150" s="13"/>
@@ -18396,7 +18531,7 @@
       <c r="AK151" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="AL151" s="13"/>
+      <c r="AL151" s="15"/>
       <c r="AM151" s="13"/>
       <c r="AN151" s="13"/>
       <c r="AO151" s="13"/>
@@ -18495,7 +18630,7 @@
       <c r="AK152" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="AL152" s="13"/>
+      <c r="AL152" s="15"/>
       <c r="AM152" s="13"/>
       <c r="AN152" s="13"/>
       <c r="AO152" s="13"/>
@@ -18535,7 +18670,7 @@
       <c r="AF153" s="13"/>
       <c r="AG153" s="13"/>
       <c r="AH153" s="15"/>
-      <c r="AL153" s="13"/>
+      <c r="AL153" s="15"/>
       <c r="AM153" s="13"/>
       <c r="AN153" s="13"/>
       <c r="AO153" s="13"/>
@@ -18575,7 +18710,7 @@
       <c r="AF154" s="13"/>
       <c r="AG154" s="13"/>
       <c r="AH154" s="15"/>
-      <c r="AL154" s="13"/>
+      <c r="AL154" s="15"/>
       <c r="AM154" s="13"/>
       <c r="AN154" s="13"/>
       <c r="AO154" s="13"/>
@@ -18615,7 +18750,7 @@
       <c r="AF155" s="13"/>
       <c r="AG155" s="13"/>
       <c r="AH155" s="15"/>
-      <c r="AL155" s="13"/>
+      <c r="AL155" s="15"/>
       <c r="AM155" s="13"/>
       <c r="AN155" s="13"/>
       <c r="AO155" s="13"/>
@@ -18655,7 +18790,7 @@
       <c r="AF156" s="13"/>
       <c r="AG156" s="13"/>
       <c r="AH156" s="15"/>
-      <c r="AL156" s="13"/>
+      <c r="AL156" s="15"/>
       <c r="AM156" s="13"/>
       <c r="AN156" s="13"/>
       <c r="AO156" s="13"/>
@@ -18719,8 +18854,83 @@
     <mergeCell ref="X3:Z3"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="AL77:AL79">
-    <cfRule type="colorScale" priority="250">
+  <conditionalFormatting sqref="AM77:AM79">
+    <cfRule type="colorScale" priority="253">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM80:AM87">
+    <cfRule type="colorScale" priority="248">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM80:AM87">
+    <cfRule type="colorScale" priority="246">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AM77:XFD80 AM81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AM67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AM48:AN48 W44:Y46 T49:V49 AM49:XFD49 AM51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH37:AK49 R66:Y66 R67:AG72 AH32:AJ33 AM47:XFD47 AM37:XFD45 AM46:AN46">
+    <cfRule type="expression" dxfId="156" priority="240">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD32">
+    <cfRule type="expression" dxfId="155" priority="227">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48:J48 T48:V48">
+    <cfRule type="expression" dxfId="154" priority="216">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM48">
+    <cfRule type="colorScale" priority="218">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM48">
+    <cfRule type="colorScale" priority="220">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN48">
+    <cfRule type="colorScale" priority="221">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18731,8 +18941,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM77:AM79">
-    <cfRule type="colorScale" priority="249">
+  <conditionalFormatting sqref="AM48">
+    <cfRule type="colorScale" priority="223">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18743,20 +18953,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL80:AL87">
-    <cfRule type="colorScale" priority="245">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+  <conditionalFormatting sqref="B46 S48:S49 S46:V46">
+    <cfRule type="expression" dxfId="153" priority="208">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM80:AM87">
-    <cfRule type="colorScale" priority="244">
+  <conditionalFormatting sqref="AM46">
+    <cfRule type="colorScale" priority="210">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18767,20 +18970,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL80:AL87">
-    <cfRule type="colorScale" priority="243">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM80:AM87">
-    <cfRule type="colorScale" priority="242">
+  <conditionalFormatting sqref="AM46">
+    <cfRule type="colorScale" priority="212">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18791,22 +18982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FK68:XFD75 A44 B45:I45 AB45:AG45 A22:AG22 A5:M8 AL77:XFD80 AL81:AN87 AB66:AG66 A63:B65 J63:O65 Q8:AG8 Q9:Q10 S45:V45 A59:O62 P59:AG65 A66:K66 L66:Q75 B9:C9 D9:M10 R6:AG7 R5:AK5 Q5:Q7 N5:P10 A49:B49 AH79:AH80 B79:B80 AI79:AJ83 L78:T80 V78:W80 U78:U85 A10:C10 Z78:AB80 A37:AG43 A23:A25 AH6:AK22 S26:S27 X78:Y85 A26:J27 A28:P29 R28:Y29 S30 AL22:XFD30 A30:J30 C31:J31 V30:Y31 AI26:AJ31 AA26:AG31 AL31 A11:Q21 AL32:XFD33 A32:AC32 C33:AF33 K36:U36 AI36:AJ36 AP36:XFD36 AB48:AG48 AF46:AG46 AF49:AG49 R9:AG21 AM5:XFD21 L76:AB77 A87:B87 B86 A79:A86 A33:B36 R73:AB75 AC73:AG84 AO67:XFD67 AO76:XFD76 AL67:AN76 AK64:AK87 K67 A67:B78 C67:J81 A47:D47 FK46:XFD46 FK48:XFD48 AL48:AN48 AK46:AN46 W44:Y46 AH37:AJ46 T49:V49 AL49:XFD49 AL51:XFD66 AK51:AK56 W48:W49 AH51:AJ78 A51:AG58 T47:W47 AA47:AG47 X47:Y49 AH47:AH49 AK37:XFD45 AI47:XFD47 AI48:AK49 R66:Y66 R67:AG72 AH32:AJ33">
-    <cfRule type="expression" dxfId="151" priority="236">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD32">
-    <cfRule type="expression" dxfId="150" priority="223">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B48:J48 T48:V48">
-    <cfRule type="expression" dxfId="149" priority="212">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL48">
+  <conditionalFormatting sqref="AN46">
     <cfRule type="colorScale" priority="213">
       <colorScale>
         <cfvo type="min"/>
@@ -18818,157 +18994,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="214">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL48">
+  <conditionalFormatting sqref="AM46">
     <cfRule type="colorScale" priority="215">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="216">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN48">
-    <cfRule type="colorScale" priority="217">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL48">
-    <cfRule type="colorScale" priority="218">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM48">
-    <cfRule type="colorScale" priority="219">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46 S48:S49 S46:V46">
-    <cfRule type="expression" dxfId="148" priority="204">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="205">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="206">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="207">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="208">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN46">
-    <cfRule type="colorScale" priority="209">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL46">
-    <cfRule type="colorScale" priority="210">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM46">
-    <cfRule type="colorScale" priority="211">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -18980,157 +19007,157 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45:AA45 AA48">
-    <cfRule type="expression" dxfId="147" priority="201">
+    <cfRule type="expression" dxfId="152" priority="205">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:AA66">
-    <cfRule type="expression" dxfId="146" priority="200">
+    <cfRule type="expression" dxfId="151" priority="204">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:I65">
-    <cfRule type="expression" dxfId="145" priority="178">
+    <cfRule type="expression" dxfId="150" priority="182">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q45 Q48">
-    <cfRule type="expression" dxfId="144" priority="176">
+    <cfRule type="expression" dxfId="149" priority="180">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68:K76">
-    <cfRule type="expression" dxfId="143" priority="175">
+    <cfRule type="expression" dxfId="148" priority="179">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45 K48">
-    <cfRule type="expression" dxfId="142" priority="174">
+    <cfRule type="expression" dxfId="147" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:K85">
-    <cfRule type="expression" dxfId="141" priority="161">
+    <cfRule type="expression" dxfId="146" priority="165">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B85 B82:J82 L81:T85 V81:W85 Z85:AD85 AH81:AH83 Z81:AB84 B81">
-    <cfRule type="expression" dxfId="140" priority="163">
+    <cfRule type="expression" dxfId="145" priority="167">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:J36">
-    <cfRule type="expression" dxfId="139" priority="98">
+    <cfRule type="expression" dxfId="144" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:P25 B23:D25 J23 S23:Y23 R24:Y25 AK26:AK27 AA23:AG25 AI23:AK25">
-    <cfRule type="expression" dxfId="138" priority="129">
+    <cfRule type="expression" dxfId="143" priority="133">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:I25">
-    <cfRule type="expression" dxfId="137" priority="128">
+    <cfRule type="expression" dxfId="142" priority="132">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:R23 Q24:Q25">
-    <cfRule type="expression" dxfId="136" priority="127">
+    <cfRule type="expression" dxfId="141" priority="131">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z24">
-    <cfRule type="expression" dxfId="135" priority="126">
+    <cfRule type="expression" dxfId="140" priority="130">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="134" priority="125">
+    <cfRule type="expression" dxfId="139" priority="129">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:R26">
-    <cfRule type="expression" dxfId="133" priority="124">
+    <cfRule type="expression" dxfId="138" priority="128">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:U27">
-    <cfRule type="expression" dxfId="132" priority="123">
+    <cfRule type="expression" dxfId="137" priority="127">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V26:W27">
-    <cfRule type="expression" dxfId="131" priority="122">
+    <cfRule type="expression" dxfId="136" priority="126">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y27">
-    <cfRule type="expression" dxfId="130" priority="121">
+    <cfRule type="expression" dxfId="135" priority="125">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26:Z31">
+    <cfRule type="expression" dxfId="134" priority="124">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27:P27 R27">
+    <cfRule type="expression" dxfId="133" priority="123">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q27:Q29">
+    <cfRule type="expression" dxfId="132" priority="122">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH23:AH31">
+    <cfRule type="expression" dxfId="131" priority="121">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T30:U31">
+    <cfRule type="expression" dxfId="130" priority="118">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK28:AK31">
     <cfRule type="expression" dxfId="129" priority="120">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27:P27 R27">
+  <conditionalFormatting sqref="K30:R30">
     <cfRule type="expression" dxfId="128" priority="119">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="expression" dxfId="127" priority="118">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH23:AH31">
-    <cfRule type="expression" dxfId="126" priority="117">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T30:U31">
-    <cfRule type="expression" dxfId="125" priority="114">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK28:AK31">
-    <cfRule type="expression" dxfId="124" priority="116">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:R30">
-    <cfRule type="expression" dxfId="123" priority="115">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="122" priority="113">
+    <cfRule type="expression" dxfId="127" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:P31 R31">
-    <cfRule type="expression" dxfId="121" priority="112">
+    <cfRule type="expression" dxfId="126" priority="116">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31">
-    <cfRule type="expression" dxfId="120" priority="111">
+    <cfRule type="expression" dxfId="125" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S31">
-    <cfRule type="expression" dxfId="119" priority="110">
+    <cfRule type="expression" dxfId="124" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK32">
-    <cfRule type="expression" dxfId="118" priority="109">
+    <cfRule type="expression" dxfId="123" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL87 AL47">
-    <cfRule type="colorScale" priority="419">
+  <conditionalFormatting sqref="AL22:AL33">
+    <cfRule type="colorScale" priority="423">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19142,7 +19169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM87 AM47">
-    <cfRule type="colorScale" priority="424">
+    <cfRule type="colorScale" priority="428">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19153,8 +19180,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL79 AL47">
-    <cfRule type="colorScale" priority="430">
+  <conditionalFormatting sqref="AL22:AL33">
+    <cfRule type="colorScale" priority="434">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19166,7 +19193,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM79 AM47">
-    <cfRule type="colorScale" priority="435">
+    <cfRule type="colorScale" priority="439">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19178,7 +19205,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN5:AN30 AN37:AN45 AN32:AN33 AN49 AN51:AN87 AN47">
-    <cfRule type="colorScale" priority="441">
+    <cfRule type="colorScale" priority="445">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19189,8 +19216,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL37:AL45 AL22:AL33 AL49 AL51:AL76 AL47">
-    <cfRule type="colorScale" priority="447">
+  <conditionalFormatting sqref="AL22:AL33">
+    <cfRule type="colorScale" priority="451">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19202,7 +19229,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM30 AM37:AM45 AM32:AM33 AM49 AM51:AM76 AM47">
-    <cfRule type="colorScale" priority="451">
+    <cfRule type="colorScale" priority="455">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19214,102 +19241,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK33">
-    <cfRule type="expression" dxfId="117" priority="108">
+    <cfRule type="expression" dxfId="122" priority="112">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:P34 R34">
-    <cfRule type="expression" dxfId="116" priority="107">
+    <cfRule type="expression" dxfId="121" priority="111">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="expression" dxfId="115" priority="106">
+    <cfRule type="expression" dxfId="120" priority="110">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T34:U34">
-    <cfRule type="expression" dxfId="114" priority="105">
+    <cfRule type="expression" dxfId="119" priority="109">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V34:W34">
-    <cfRule type="expression" dxfId="113" priority="104">
+    <cfRule type="expression" dxfId="118" priority="108">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="expression" dxfId="112" priority="103">
+    <cfRule type="expression" dxfId="117" priority="107">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34">
-    <cfRule type="expression" dxfId="111" priority="102">
+    <cfRule type="expression" dxfId="116" priority="106">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH34:AJ34">
-    <cfRule type="expression" dxfId="110" priority="101">
+    <cfRule type="expression" dxfId="115" priority="105">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="109" priority="100">
+    <cfRule type="expression" dxfId="114" priority="104">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="108" priority="61">
+    <cfRule type="expression" dxfId="113" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:P35 R35:U35">
-    <cfRule type="expression" dxfId="107" priority="97">
+    <cfRule type="expression" dxfId="112" priority="101">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="expression" dxfId="106" priority="96">
+    <cfRule type="expression" dxfId="111" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:Y36 AA35:AC36">
-    <cfRule type="expression" dxfId="105" priority="95">
+    <cfRule type="expression" dxfId="110" priority="99">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z36">
-    <cfRule type="expression" dxfId="104" priority="94">
+    <cfRule type="expression" dxfId="109" priority="98">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35:AD36">
-    <cfRule type="expression" dxfId="103" priority="93">
+    <cfRule type="expression" dxfId="108" priority="97">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE36:AH36 AE35:AF35 AH35">
-    <cfRule type="expression" dxfId="102" priority="92">
+    <cfRule type="expression" dxfId="107" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI35:AJ35">
-    <cfRule type="expression" dxfId="101" priority="91">
+    <cfRule type="expression" dxfId="106" priority="95">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK35:AK36">
-    <cfRule type="expression" dxfId="100" priority="90">
+    <cfRule type="expression" dxfId="105" priority="94">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="expression" dxfId="99" priority="86">
+    <cfRule type="expression" dxfId="104" priority="90">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
-    <cfRule type="colorScale" priority="87">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19321,6 +19348,59 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35:AL36">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL35:AL36">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
+    <cfRule type="expression" dxfId="103" priority="85">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM35:AM36">
+    <cfRule type="colorScale" priority="86">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM35:AM36">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN35:AN36">
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
@@ -19332,61 +19412,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL35:AL36">
+  <conditionalFormatting sqref="AM35:AM36">
     <cfRule type="colorScale" priority="89">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AP35 AM36:AO36">
-    <cfRule type="expression" dxfId="98" priority="81">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AM36">
-    <cfRule type="colorScale" priority="82">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AM36">
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN35:AN36">
-    <cfRule type="colorScale" priority="84">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM35:AM36">
-    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19398,368 +19425,409 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="97" priority="80">
+    <cfRule type="expression" dxfId="102" priority="84">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:R44">
-    <cfRule type="expression" dxfId="96" priority="79">
+    <cfRule type="expression" dxfId="101" priority="83">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:R46">
-    <cfRule type="expression" dxfId="95" priority="78">
+    <cfRule type="expression" dxfId="100" priority="82">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:R49 E47:J47">
-    <cfRule type="expression" dxfId="94" priority="77">
+    <cfRule type="expression" dxfId="99" priority="81">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S44:V44">
-    <cfRule type="expression" dxfId="93" priority="76">
+    <cfRule type="expression" dxfId="98" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AC44">
-    <cfRule type="expression" dxfId="92" priority="75">
+    <cfRule type="expression" dxfId="97" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44">
-    <cfRule type="expression" dxfId="91" priority="74">
+    <cfRule type="expression" dxfId="96" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44">
-    <cfRule type="expression" dxfId="90" priority="73">
+    <cfRule type="expression" dxfId="95" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD46">
+    <cfRule type="expression" dxfId="94" priority="73">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA46:AC46">
+    <cfRule type="expression" dxfId="93" priority="75">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z46:Z49">
+    <cfRule type="expression" dxfId="92" priority="74">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE46">
+    <cfRule type="expression" dxfId="91" priority="72">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA49:AC49">
+    <cfRule type="expression" dxfId="90" priority="71">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD49">
     <cfRule type="expression" dxfId="89" priority="69">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA46:AC46">
-    <cfRule type="expression" dxfId="88" priority="71">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z46:Z49">
-    <cfRule type="expression" dxfId="87" priority="70">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE46">
-    <cfRule type="expression" dxfId="86" priority="68">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA49:AC49">
-    <cfRule type="expression" dxfId="85" priority="67">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD49">
-    <cfRule type="expression" dxfId="84" priority="65">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="83" priority="64">
+    <cfRule type="expression" dxfId="88" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AG44">
-    <cfRule type="expression" dxfId="82" priority="63">
+    <cfRule type="expression" dxfId="87" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="81" priority="62">
+    <cfRule type="expression" dxfId="86" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AL21">
-    <cfRule type="expression" dxfId="80" priority="60">
+    <cfRule type="expression" dxfId="85" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:C85">
-    <cfRule type="expression" dxfId="79" priority="58">
+    <cfRule type="expression" dxfId="84" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83:J85">
-    <cfRule type="expression" dxfId="78" priority="57">
+    <cfRule type="expression" dxfId="83" priority="61">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L86:AJ87">
+    <cfRule type="expression" dxfId="82" priority="59">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C86:K87">
+    <cfRule type="expression" dxfId="81" priority="58">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
+    <cfRule type="expression" dxfId="80" priority="57">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK93:AK119">
+    <cfRule type="expression" dxfId="79" priority="19">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B113 B115 B117">
+    <cfRule type="expression" dxfId="78" priority="8">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K88:K89">
     <cfRule type="expression" dxfId="77" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86:K87">
-    <cfRule type="expression" dxfId="76" priority="54">
+  <conditionalFormatting sqref="L88:R89">
+    <cfRule type="expression" dxfId="76" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE85:AJ85 AH84:AJ84">
-    <cfRule type="expression" dxfId="75" priority="53">
+  <conditionalFormatting sqref="C88:C89">
+    <cfRule type="expression" dxfId="75" priority="54">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK93:AK119">
-    <cfRule type="expression" dxfId="74" priority="15">
+  <conditionalFormatting sqref="D88:J89">
+    <cfRule type="expression" dxfId="74" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113 B115 B117">
-    <cfRule type="expression" dxfId="73" priority="4">
+  <conditionalFormatting sqref="L90:R91">
+    <cfRule type="expression" dxfId="73" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K88:K89">
+  <conditionalFormatting sqref="C90:K91">
     <cfRule type="expression" dxfId="72" priority="51">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L88:R89">
-    <cfRule type="expression" dxfId="71" priority="52">
+  <conditionalFormatting sqref="K92:K93">
+    <cfRule type="expression" dxfId="71" priority="49">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
+  <conditionalFormatting sqref="L92:R93">
     <cfRule type="expression" dxfId="70" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88:J89">
-    <cfRule type="expression" dxfId="69" priority="49">
+  <conditionalFormatting sqref="C92:C93">
+    <cfRule type="expression" dxfId="69" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L90:R91">
-    <cfRule type="expression" dxfId="68" priority="48">
+  <conditionalFormatting sqref="D92:J93">
+    <cfRule type="expression" dxfId="68" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C90:K91">
-    <cfRule type="expression" dxfId="67" priority="47">
+  <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AC100:AG157 AI157:AO157 AI120:AK156 AM88:AO156">
+    <cfRule type="expression" dxfId="67" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K92:K93">
+  <conditionalFormatting sqref="C94:K99">
     <cfRule type="expression" dxfId="66" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L92:R93">
-    <cfRule type="expression" dxfId="65" priority="46">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="64" priority="44">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D92:J93">
-    <cfRule type="expression" dxfId="63" priority="43">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L94:AG99 AI95:AJ119 AL88:AO119 AC100:AG157 AI120:AO157">
-    <cfRule type="expression" dxfId="62" priority="42">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C94:K99">
-    <cfRule type="expression" dxfId="61" priority="41">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A90:B90 B89 A88:A89">
-    <cfRule type="expression" dxfId="60" priority="40">
+    <cfRule type="expression" dxfId="65" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="59" priority="39">
+    <cfRule type="expression" dxfId="64" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:B93 B92 A91:A92">
-    <cfRule type="expression" dxfId="58" priority="38">
+    <cfRule type="expression" dxfId="63" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="57" priority="37">
+    <cfRule type="expression" dxfId="62" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95 B97 B99 A94:A99">
-    <cfRule type="expression" dxfId="56" priority="36">
+    <cfRule type="expression" dxfId="61" priority="40">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94 B96 B98">
-    <cfRule type="expression" dxfId="55" priority="35">
+    <cfRule type="expression" dxfId="60" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U88:U89 X88:Y89">
-    <cfRule type="expression" dxfId="54" priority="34">
+    <cfRule type="expression" dxfId="59" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S88:T89 V88:W89 Z88:AB89">
-    <cfRule type="expression" dxfId="53" priority="33">
+    <cfRule type="expression" dxfId="58" priority="37">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S90:AB91">
-    <cfRule type="expression" dxfId="52" priority="32">
+    <cfRule type="expression" dxfId="57" priority="36">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U92:U93 X92:Y93">
-    <cfRule type="expression" dxfId="51" priority="31">
+    <cfRule type="expression" dxfId="56" priority="35">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S92:T93 V92:W93 Z92:AB93">
-    <cfRule type="expression" dxfId="50" priority="30">
+    <cfRule type="expression" dxfId="55" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE88:AG89">
-    <cfRule type="expression" dxfId="49" priority="28">
+    <cfRule type="expression" dxfId="54" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC88:AD89">
-    <cfRule type="expression" dxfId="48" priority="27">
+    <cfRule type="expression" dxfId="53" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC90:AG91">
-    <cfRule type="expression" dxfId="47" priority="26">
+    <cfRule type="expression" dxfId="52" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE92:AG93">
-    <cfRule type="expression" dxfId="46" priority="25">
+    <cfRule type="expression" dxfId="51" priority="29">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC92:AD93">
-    <cfRule type="expression" dxfId="45" priority="24">
+    <cfRule type="expression" dxfId="50" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI94:AJ94">
-    <cfRule type="expression" dxfId="44" priority="23">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH88:AJ89">
-    <cfRule type="expression" dxfId="43" priority="22">
+    <cfRule type="expression" dxfId="48" priority="26">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH90:AJ91">
-    <cfRule type="expression" dxfId="42" priority="21">
+    <cfRule type="expression" dxfId="47" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH92:AJ93 AH94:AH157">
-    <cfRule type="expression" dxfId="41" priority="20">
+    <cfRule type="expression" dxfId="46" priority="24">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK57:AK61">
-    <cfRule type="expression" dxfId="40" priority="18">
+    <cfRule type="expression" dxfId="45" priority="22">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK62:AK63">
-    <cfRule type="expression" dxfId="39" priority="17">
+    <cfRule type="expression" dxfId="44" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK88:AK92">
-    <cfRule type="expression" dxfId="38" priority="16">
+    <cfRule type="expression" dxfId="43" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101 B103 B105:B112 A100:A112">
-    <cfRule type="expression" dxfId="37" priority="14">
+    <cfRule type="expression" dxfId="42" priority="18">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100 B102 B104">
-    <cfRule type="expression" dxfId="36" priority="13">
+    <cfRule type="expression" dxfId="41" priority="17">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L100:R157">
-    <cfRule type="expression" dxfId="35" priority="12">
+    <cfRule type="expression" dxfId="40" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:K157">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="39" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S100:AB112">
-    <cfRule type="expression" dxfId="33" priority="10">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S113:AB118">
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="37" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S119:AB131">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="36" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:AB137">
-    <cfRule type="expression" dxfId="30" priority="7">
+    <cfRule type="expression" dxfId="35" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S138:AB143 S144:Z158 AA144:AB157">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="34" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114 B116 B118:B156 A113:A156 A157:B157">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="33" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S47">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="32" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:R47">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="31" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG32:AG35">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="30" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL37:AL156">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL37:AL156">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL37:AL156">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL37:AL156">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -19782,10 +19850,10 @@
   <dimension ref="A1:AE85"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="R32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C87" sqref="C87"/>
+      <selection pane="bottomRight" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -23882,7 +23950,7 @@
         <v>USD</v>
       </c>
       <c r="N38" s="13">
-        <f t="shared" ref="N38:N85" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N38:N81" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>0.69120000000000004</v>
       </c>
       <c r="O38" s="13">
@@ -25849,9 +25917,9 @@
         <f t="shared" ca="1" si="37"/>
         <v>Reedbush-H Personal (educational)</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="15" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E56" s="21" t="s">
         <v>144</v>
@@ -25958,9 +26026,9 @@
         <f t="shared" ca="1" si="37"/>
         <v>Reedbush-H (educational)</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="15" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E57" s="21" t="s">
         <v>234</v>
@@ -26066,9 +26134,9 @@
         <f t="shared" ref="C58:D73" ca="1" si="48">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>Reedbush-H reviewed (educational)</v>
       </c>
-      <c r="D58" s="15">
+      <c r="D58" s="15" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E58" s="21" t="s">
         <v>163</v>
@@ -26102,7 +26170,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="18" t="str">
-        <f t="shared" ref="M58:M85" ca="1" si="50">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="M58:M81" ca="1" si="50">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>JPY</v>
       </c>
       <c r="N58" s="13">
@@ -26175,9 +26243,9 @@
         <f t="shared" ca="1" si="48"/>
         <v>Reedbush-H reviewed</v>
       </c>
-      <c r="D59" s="15">
+      <c r="D59" s="15" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E59" s="21" t="s">
         <v>162</v>
@@ -26271,7 +26339,7 @@
         <v>0</v>
       </c>
       <c r="AB59" s="15" t="str">
-        <f t="shared" ref="AB59:AB85" ca="1" si="53">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="AB59:AB81" ca="1" si="53">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
       <c r="AC59" s="33">
@@ -26283,12 +26351,12 @@
         <f t="shared" ca="1" si="48"/>
         <v>Reedbush-H dedicated reviewed (educational)</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="15" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>162</v>
+        <v>415</v>
       </c>
       <c r="F60" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26391,12 +26459,12 @@
         <f t="shared" ca="1" si="48"/>
         <v>Reedbush-H dedicated reviewed</v>
       </c>
-      <c r="D61" s="15">
+      <c r="D61" s="15" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>0</v>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>162</v>
+        <v>416</v>
       </c>
       <c r="F61" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26435,7 +26503,7 @@
         <v>2.4192000000000005</v>
       </c>
       <c r="O61" s="13">
-        <f t="shared" ref="O61:O85" ca="1" si="54">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="O61:O81" ca="1" si="54">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>19</v>
       </c>
       <c r="P61" s="13" t="str">
@@ -27099,7 +27167,7 @@
         <v>19.3</v>
       </c>
       <c r="P67" s="13" t="str">
-        <f t="shared" ref="P67:AA82" ca="1" si="56">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="P67:AA81" ca="1" si="56">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>M60</v>
       </c>
       <c r="Q67" s="13">
@@ -27820,7 +27888,7 @@
         <v>https://www.idcf.jp/service/deeplearning/</v>
       </c>
       <c r="C74" s="21" t="str">
-        <f t="shared" ref="C74:D85" ca="1" si="57">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="C74:D81" ca="1" si="57">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>GPU.7XL P100</v>
       </c>
       <c r="D74" s="15">
@@ -27939,7 +28007,7 @@
         <v>259</v>
       </c>
       <c r="F75" s="18">
-        <f t="shared" ref="F75:L85" ca="1" si="58">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="F75:L81" ca="1" si="58">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="G75" s="13">
@@ -28052,7 +28120,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="21" t="str">
-        <f t="shared" ref="E76:E84" ca="1" si="59">"Tsub." &amp; C76</f>
+        <f t="shared" ref="E76:E81" ca="1" si="59">"Tsub." &amp; C76</f>
         <v>Tsub.S</v>
       </c>
       <c r="F76" s="18">
@@ -28815,127 +28883,127 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V35:Y35 R23:U30 V40 L22:Q30 N37:U40 V37:Y39 N36:Y36 E45:E46 S57:V59 M59:Q59 L4:T16 M3:T3 M52:V56 R57:R85 L52:L85 E41:E43 C3:D30 E4:F30 E32:E38 C32:D85 V32:W34 N32:U35 L32:M40 L31:U31 C31:F31 J45:J85 F32:F85 U11:W18 U19:V21 V23:V31 W19:W31 Y66:AB85 L41:V51 Y42:Y55 Z28:Z55 Y56:Z65 AB6:AB65 AA23:AA65 E3:H3 I11:I32 H4:H85 G4:G42">
-    <cfRule type="expression" dxfId="24" priority="146">
+    <cfRule type="expression" dxfId="5" priority="146">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40:Y40 Y41 U3:Y3 U4:W10 X4:Y34 W41:X85">
-    <cfRule type="expression" dxfId="23" priority="86">
+    <cfRule type="expression" dxfId="29" priority="86">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
-    <cfRule type="expression" dxfId="22" priority="74">
+    <cfRule type="expression" dxfId="28" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22 T22">
-    <cfRule type="expression" dxfId="21" priority="72">
+    <cfRule type="expression" dxfId="27" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="20" priority="73">
+    <cfRule type="expression" dxfId="26" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22">
-    <cfRule type="expression" dxfId="19" priority="71">
+    <cfRule type="expression" dxfId="25" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="18" priority="68">
+    <cfRule type="expression" dxfId="24" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
-    <cfRule type="expression" dxfId="17" priority="62">
+    <cfRule type="expression" dxfId="23" priority="62">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:J44">
-    <cfRule type="expression" dxfId="16" priority="53">
+    <cfRule type="expression" dxfId="22" priority="53">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J25">
-    <cfRule type="expression" dxfId="15" priority="52">
+    <cfRule type="expression" dxfId="21" priority="52">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:I85">
-    <cfRule type="expression" dxfId="14" priority="32">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:G85">
-    <cfRule type="expression" dxfId="13" priority="28">
+    <cfRule type="expression" dxfId="19" priority="28">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M57:Q58">
-    <cfRule type="expression" dxfId="12" priority="27">
+    <cfRule type="expression" dxfId="18" priority="27">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60:Q85">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V60:V85 T60:T85">
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:S85">
-    <cfRule type="expression" dxfId="9" priority="21">
+    <cfRule type="expression" dxfId="15" priority="21">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U60:U85">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:T21">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z3:AA22 Z23:Z27">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3 K4:K85">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Cirrascale POWER9 and LeaderTelecom offers.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="20" windowWidth="34500" windowHeight="14840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="20" windowWidth="34500" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5708,29 +5708,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="109">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="103">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5904,50 +5882,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7205,11 +7139,11 @@
   </sheetPr>
   <dimension ref="A1:FJ156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="J83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AM68" sqref="AM68"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -14394,7 +14328,7 @@
         <v>97</v>
       </c>
       <c r="L89" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M89" s="5">
         <v>8</v>
@@ -18930,437 +18864,437 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="AH76:AH77 B76:B77 AI76:AJ82 S35:S36 R37:W38 S39 C40:J40 V39:Y40 AI35:AJ40 AA35:AG35 C42:Z42 K45:U45 AI45:AJ45 A86:B86 B85 AH41:AJ42 A24:AG28 A12:X14 A9:L9 J11:L11 J10:K10 A10:I11 M9:X11 Y6:Y14 A16:D16 A17:B17 A18:Y21 T16:Y17 A6:X8 AA16:AG23 A22:B23 L22:L23 A74:B75 L74:AB75 FK67:XFD67 A89:A91 B87:B97 AP6:XFD14 AP38:XFD39 AP16:XFD36 AO75:XFD75 A5:XFD5 Z6:AN11 AA12:AN14 A46:AN56 B57:AN64 AH74:AJ75 C98:R115 S111:AB115 AC98:AN115 AN124:AN126 AH124:AK126 A124:A154 AO87:AO154 A116:AN123 AP42:XFD45 B35:J36 B37:P38 A29:A36 B39:J39 B41:Z41 A38:A45 B42:B45 AO6:AO45 K29:K31 B29:D31 S29:W31 AA29:AG31 AH16:AN28 C78:D78 J78 A76:A85 L76:T77 V76:W77 U76:U84 Z76:AB77 X76:Y84 AC74:AG83 C74:J77 AP76:XFD77 AO76:AO82 K76:K84 AK74:AN97 AI29:AJ31 X29:Y40 AL29:AN31 FK74:XFD74 AO46:XFD65 A57:A65 A66:XFD66 A67:AN67 A68:XFD73">
-    <cfRule type="expression" dxfId="1" priority="296">
+    <cfRule type="expression" dxfId="102" priority="296">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74:K75">
-    <cfRule type="expression" dxfId="103" priority="235">
+    <cfRule type="expression" dxfId="101" priority="235">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B84 B79:J79 L78:T84 V78:W84 Z84:AD84 Z78:AB83 B78 AH78:AH97">
-    <cfRule type="expression" dxfId="102" priority="223">
+    <cfRule type="expression" dxfId="100" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:J45">
-    <cfRule type="expression" dxfId="101" priority="158">
+    <cfRule type="expression" dxfId="99" priority="158">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:P34 B32:D34 J32 S32:W32 AA32:AG34 AK35:AN36 AI32:AN34 R33:W34">
-    <cfRule type="expression" dxfId="100" priority="189">
+    <cfRule type="expression" dxfId="98" priority="189">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32:I34">
-    <cfRule type="expression" dxfId="99" priority="188">
+    <cfRule type="expression" dxfId="97" priority="188">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:R32 Q33:Q34">
-    <cfRule type="expression" dxfId="98" priority="187">
+    <cfRule type="expression" dxfId="96" priority="187">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z29:Z34">
-    <cfRule type="expression" dxfId="97" priority="186">
+    <cfRule type="expression" dxfId="95" priority="186">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:R35">
-    <cfRule type="expression" dxfId="96" priority="184">
+    <cfRule type="expression" dxfId="94" priority="184">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T35:U36">
-    <cfRule type="expression" dxfId="95" priority="183">
+    <cfRule type="expression" dxfId="93" priority="183">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:W36">
-    <cfRule type="expression" dxfId="94" priority="182">
+    <cfRule type="expression" dxfId="92" priority="182">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z40">
-    <cfRule type="expression" dxfId="93" priority="180">
+    <cfRule type="expression" dxfId="91" priority="180">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:P36 R36">
-    <cfRule type="expression" dxfId="92" priority="179">
+    <cfRule type="expression" dxfId="90" priority="179">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q36:Q38">
-    <cfRule type="expression" dxfId="91" priority="178">
+    <cfRule type="expression" dxfId="89" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH29:AH40">
-    <cfRule type="expression" dxfId="90" priority="177">
+    <cfRule type="expression" dxfId="88" priority="177">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39:U40">
-    <cfRule type="expression" dxfId="89" priority="174">
+    <cfRule type="expression" dxfId="87" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK37:AN40">
-    <cfRule type="expression" dxfId="88" priority="176">
+    <cfRule type="expression" dxfId="86" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:R39">
-    <cfRule type="expression" dxfId="87" priority="175">
+    <cfRule type="expression" dxfId="85" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="86" priority="173">
+    <cfRule type="expression" dxfId="84" priority="173">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:P40 R40">
-    <cfRule type="expression" dxfId="85" priority="172">
+    <cfRule type="expression" dxfId="83" priority="172">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q40">
-    <cfRule type="expression" dxfId="84" priority="171">
+    <cfRule type="expression" dxfId="82" priority="171">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40">
-    <cfRule type="expression" dxfId="83" priority="170">
+    <cfRule type="expression" dxfId="81" priority="170">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK41:AN41">
-    <cfRule type="expression" dxfId="82" priority="169">
+    <cfRule type="expression" dxfId="80" priority="169">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK42:AN42">
-    <cfRule type="expression" dxfId="81" priority="168">
+    <cfRule type="expression" dxfId="79" priority="168">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:P43 R43">
-    <cfRule type="expression" dxfId="80" priority="167">
+    <cfRule type="expression" dxfId="78" priority="167">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43">
-    <cfRule type="expression" dxfId="79" priority="166">
+    <cfRule type="expression" dxfId="77" priority="166">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43:U43">
-    <cfRule type="expression" dxfId="78" priority="165">
+    <cfRule type="expression" dxfId="76" priority="165">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43:W43">
-    <cfRule type="expression" dxfId="77" priority="164">
+    <cfRule type="expression" dxfId="75" priority="164">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X43:Y43">
-    <cfRule type="expression" dxfId="76" priority="163">
+    <cfRule type="expression" dxfId="74" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z43">
-    <cfRule type="expression" dxfId="75" priority="162">
+    <cfRule type="expression" dxfId="73" priority="162">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH43:AJ43">
-    <cfRule type="expression" dxfId="74" priority="161">
+    <cfRule type="expression" dxfId="72" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK43:AN43">
-    <cfRule type="expression" dxfId="73" priority="160">
+    <cfRule type="expression" dxfId="71" priority="160">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:P44 R44:U44">
-    <cfRule type="expression" dxfId="72" priority="157">
+    <cfRule type="expression" dxfId="70" priority="157">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="expression" dxfId="71" priority="156">
+    <cfRule type="expression" dxfId="69" priority="156">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V44:Y45 AA36:AC45">
-    <cfRule type="expression" dxfId="70" priority="155">
+    <cfRule type="expression" dxfId="68" priority="155">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44:Z45">
-    <cfRule type="expression" dxfId="69" priority="154">
+    <cfRule type="expression" dxfId="67" priority="154">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD36:AD45">
-    <cfRule type="expression" dxfId="68" priority="153">
+    <cfRule type="expression" dxfId="66" priority="153">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE45:AH45 AH44 AE36:AG44">
-    <cfRule type="expression" dxfId="67" priority="152">
+    <cfRule type="expression" dxfId="65" priority="152">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AJ44">
-    <cfRule type="expression" dxfId="66" priority="151">
+    <cfRule type="expression" dxfId="64" priority="151">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK44:AN45">
-    <cfRule type="expression" dxfId="65" priority="150">
+    <cfRule type="expression" dxfId="63" priority="150">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP41">
-    <cfRule type="expression" dxfId="64" priority="141">
+    <cfRule type="expression" dxfId="62" priority="141">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="63" priority="140">
+    <cfRule type="expression" dxfId="61" priority="140">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C84">
-    <cfRule type="expression" dxfId="62" priority="118">
+    <cfRule type="expression" dxfId="60" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D80:J84">
-    <cfRule type="expression" dxfId="61" priority="117">
+    <cfRule type="expression" dxfId="59" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:AG92 AI85:AJ97 L94:AG97 AA93:AG93">
-    <cfRule type="expression" dxfId="60" priority="115">
+    <cfRule type="expression" dxfId="58" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85:K92 C94:K97 J93">
-    <cfRule type="expression" dxfId="59" priority="114">
+    <cfRule type="expression" dxfId="57" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE84:AG84 AI83:AJ84">
-    <cfRule type="expression" dxfId="58" priority="113">
+    <cfRule type="expression" dxfId="56" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111 B113 B115">
-    <cfRule type="expression" dxfId="57" priority="64">
+    <cfRule type="expression" dxfId="55" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO155 AI127:AN155 AC124:AG155 AL124:AM126">
-    <cfRule type="expression" dxfId="56" priority="102">
+    <cfRule type="expression" dxfId="54" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87:A88">
-    <cfRule type="expression" dxfId="55" priority="100">
+    <cfRule type="expression" dxfId="53" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:A97">
-    <cfRule type="expression" dxfId="54" priority="96">
+    <cfRule type="expression" dxfId="52" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH127:AH155">
-    <cfRule type="expression" dxfId="53" priority="80">
+    <cfRule type="expression" dxfId="51" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99 B101 B103:B110 A98:A110">
-    <cfRule type="expression" dxfId="52" priority="74">
+    <cfRule type="expression" dxfId="50" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98 B100 B102">
-    <cfRule type="expression" dxfId="51" priority="73">
+    <cfRule type="expression" dxfId="49" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L135:R155 R133:R134 L124:R131">
-    <cfRule type="expression" dxfId="50" priority="72">
+    <cfRule type="expression" dxfId="48" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:K155 J124:K126 C124:C126">
-    <cfRule type="expression" dxfId="49" priority="71">
+    <cfRule type="expression" dxfId="47" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S98:AB110">
-    <cfRule type="expression" dxfId="48" priority="70">
+    <cfRule type="expression" dxfId="46" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S124:AB125 S127:AB129 S126:W126 AA126:AB126">
-    <cfRule type="expression" dxfId="47" priority="68">
+    <cfRule type="expression" dxfId="45" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S130:AB131 S135:AB135 S133:S134 V132:AB134">
-    <cfRule type="expression" dxfId="46" priority="67">
+    <cfRule type="expression" dxfId="44" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:AB141 S142:Z156 AA142:AB155">
-    <cfRule type="expression" dxfId="45" priority="66">
+    <cfRule type="expression" dxfId="43" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112 B114 A111:A115 A155:B155 B127:B154">
-    <cfRule type="expression" dxfId="44" priority="65">
+    <cfRule type="expression" dxfId="42" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z12:Z14 Z16:Z21">
-    <cfRule type="expression" dxfId="43" priority="56">
+    <cfRule type="expression" dxfId="41" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="expression" dxfId="42" priority="55">
+    <cfRule type="expression" dxfId="40" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:Y15 AP15:XFD15 AA15:AN15">
-    <cfRule type="expression" dxfId="41" priority="50">
+    <cfRule type="expression" dxfId="39" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z15">
-    <cfRule type="expression" dxfId="40" priority="48">
+    <cfRule type="expression" dxfId="38" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:S16 J17">
-    <cfRule type="expression" dxfId="39" priority="47">
+    <cfRule type="expression" dxfId="37" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:I17">
-    <cfRule type="expression" dxfId="38" priority="46">
+    <cfRule type="expression" dxfId="36" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:S17">
-    <cfRule type="expression" dxfId="37" priority="45">
+    <cfRule type="expression" dxfId="35" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:D23 T22:Y23">
-    <cfRule type="expression" dxfId="36" priority="44">
+    <cfRule type="expression" dxfId="34" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z22:Z23">
-    <cfRule type="expression" dxfId="35" priority="43">
+    <cfRule type="expression" dxfId="33" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:K23 M22:S23">
-    <cfRule type="expression" dxfId="34" priority="42">
+    <cfRule type="expression" dxfId="32" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65:AN65">
-    <cfRule type="expression" dxfId="33" priority="16">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L132:R132 L133:Q134">
-    <cfRule type="expression" dxfId="32" priority="15">
+    <cfRule type="expression" dxfId="30" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:U132 T133:U134">
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="29" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124 B126">
-    <cfRule type="expression" dxfId="30" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D124:I126">
-    <cfRule type="expression" dxfId="28" priority="11">
+    <cfRule type="expression" dxfId="26" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X126:Z126">
-    <cfRule type="expression" dxfId="27" priority="10">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:J31">
-    <cfRule type="expression" dxfId="26" priority="9">
+    <cfRule type="expression" dxfId="24" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:P31 R30:R31">
-    <cfRule type="expression" dxfId="25" priority="8">
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:R29 Q30:Q31">
-    <cfRule type="expression" dxfId="24" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:I78">
-    <cfRule type="expression" dxfId="23" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93:I93">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L93:Z93">
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K93">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK29:AK31">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19383,11 +19317,11 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD24"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -25438,7 +25372,7 @@
       </c>
       <c r="N56" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.43519999999999998</v>
+        <v>0.87039999999999995</v>
       </c>
       <c r="O56" s="13">
         <f t="shared" ca="1" si="34"/>
@@ -25458,7 +25392,7 @@
       </c>
       <c r="S56" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T56" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -29267,82 +29201,82 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="V43 N40:U43 V40:Y42 M3:T3 L35:M43 U21:W25 U26:V28 L44:V45 Y45 F93 H93 J93:L93 L21:T23 F91:M92 N35:Y39 J35:K45 Z35:AB45 L29:Q34 R30:V34 W26:W34 AA30:AA34 F21:K34 Z3:AA29 K4:T20 AB6:AB34 X4:Y34 J3:J20 C3:H20 F35:H47 C21:E47 C82:D93 E82:E89 F82:F90 J46:V59 R62:V93 M64:Q90 C48:H59 Y46:AB59 W44:X59 I35:I59 W61:AB93 C61:F81 G61:L90 M61:V61 C60:AB60">
-    <cfRule type="expression" dxfId="17" priority="152">
+    <cfRule type="expression" dxfId="15" priority="152">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43:Y43 Y44 U3:Y3 U4:W20">
-    <cfRule type="expression" dxfId="16" priority="92">
+    <cfRule type="expression" dxfId="14" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29">
-    <cfRule type="expression" dxfId="15" priority="80">
+    <cfRule type="expression" dxfId="13" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V29 T29">
-    <cfRule type="expression" dxfId="14" priority="78">
+    <cfRule type="expression" dxfId="12" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29">
-    <cfRule type="expression" dxfId="13" priority="79">
+    <cfRule type="expression" dxfId="11" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U29">
-    <cfRule type="expression" dxfId="12" priority="77">
+    <cfRule type="expression" dxfId="10" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I20">
-    <cfRule type="expression" dxfId="11" priority="68">
+    <cfRule type="expression" dxfId="9" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I93">
-    <cfRule type="expression" dxfId="10" priority="38">
+    <cfRule type="expression" dxfId="8" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G93">
-    <cfRule type="expression" dxfId="9" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M62:Q63">
-    <cfRule type="expression" dxfId="8" priority="33">
+    <cfRule type="expression" dxfId="6" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M93:Q93 N91:Q92">
-    <cfRule type="expression" dxfId="7" priority="31">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:T28">
-    <cfRule type="expression" dxfId="6" priority="19">
+    <cfRule type="expression" dxfId="4" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z30:Z34">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90:E93">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Cirrascale POWER8 P100x4 offer to 10 cores.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="20" windowWidth="34500" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="40" windowWidth="34500" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2365,15 +2365,15 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>CR P100x4 P8-8</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t xml:space="preserve">4-GPU P100 POWER8-8 </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t xml:space="preserve">2-GPU P100 POWER8-10 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4-GPU P100 POWER8-10 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>CR P100x4 P8-10</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -7140,10 +7140,10 @@
   <dimension ref="A1:FJ156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="J83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="J56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89:XFD89"/>
+      <selection pane="bottomRight" activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -12857,7 +12857,7 @@
         <v>2</v>
       </c>
       <c r="M69" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N69" s="5">
         <v>3.25</v>
@@ -12870,7 +12870,7 @@
       </c>
       <c r="Q69" s="13">
         <f>M69*N69*P69/1000</f>
-        <v>0.41599999999999998</v>
+        <v>0.52</v>
       </c>
       <c r="R69" s="5">
         <v>1333</v>
@@ -12918,13 +12918,13 @@
       </c>
       <c r="AM69" s="15"/>
       <c r="AN69" s="24" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="70" spans="1:166" s="12" customFormat="1">
       <c r="A70" s="2"/>
       <c r="B70" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C70" s="24" t="s">
         <v>323</v>
@@ -19318,7 +19318,7 @@
   <dimension ref="A1:AE93"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
@@ -24311,7 +24311,7 @@
       <c r="B47" s="15"/>
       <c r="C47" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v xml:space="preserve">4-GPU P100 POWER8-8 </v>
+        <v xml:space="preserve">4-GPU P100 POWER8-10 </v>
       </c>
       <c r="D47" s="15" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -24319,7 +24319,7 @@
       </c>
       <c r="E47" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>CR P100x4 P8-8</v>
+        <v>CR P100x4 P8-10</v>
       </c>
       <c r="F47" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -24355,7 +24355,7 @@
       </c>
       <c r="N47" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.83199999999999996</v>
+        <v>1.04</v>
       </c>
       <c r="O47" s="13">
         <f t="shared" ca="1" si="34"/>

</xml_diff>

<commit_message>
Added LeaderTelecom v100x2 nvlink offer.
</commit_message>
<xml_diff>
--- a/Comparison table updated 3.xlsx
+++ b/Comparison table updated 3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="40" windowWidth="34500" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="40" windowWidth="34500" windowHeight="14840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="470">
   <si>
     <t>Cloud server providers with GPU</t>
     <phoneticPr fontId="2"/>
@@ -2204,14 +2204,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till the end of February 2018.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till end of February 2018.</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>V100 2620</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2374,6 +2366,33 @@
   </si>
   <si>
     <t>CR P100x4 P8-10</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till the end of ..</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till end of ...</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2 x V100nvlink</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Xeon Silver 4114</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SSD</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb.</t>
+  </si>
+  <si>
+    <t>LT V100x2NVlink</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2699,7 +2718,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1457">
+  <cellStyleXfs count="1459">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4142,6 +4161,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4249,7 +4270,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1457">
+  <cellStyles count="1459">
     <cellStyle name="$Normal" xfId="356"/>
     <cellStyle name="¥ Normal" xfId="636"/>
     <cellStyle name="€ Normal" xfId="635"/>
@@ -5046,6 +5067,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1452" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1454" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1458" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 1 2" xfId="62"/>
     <cellStyle name="Heading 2" xfId="263" builtinId="17" customBuiltin="1"/>
@@ -5697,6 +5719,7 @@
     <cellStyle name="Hyperlink" xfId="1451" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1453" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1457" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="341" builtinId="20" hidden="1"/>
     <cellStyle name="Linked Cell" xfId="344" builtinId="24" hidden="1"/>
     <cellStyle name="Neutral" xfId="594" builtinId="28"/>
@@ -5708,7 +5731,7 @@
     <cellStyle name="Style 1" xfId="55"/>
     <cellStyle name="Title" xfId="340" builtinId="15" hidden="1"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="110">
     <dxf>
       <font>
         <color auto="1"/>
@@ -5882,6 +5905,83 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFEAF2F7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7139,11 +7239,11 @@
   </sheetPr>
   <dimension ref="A1:FJ156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="J56" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="AH83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O65" sqref="O65"/>
+      <selection pane="bottomRight" activeCell="AM94" sqref="AM94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -9429,10 +9529,10 @@
         <v>216</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -9456,7 +9556,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L29" s="5">
         <v>2</v>
@@ -9484,7 +9584,7 @@
         <v>64</v>
       </c>
       <c r="T29" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="U29" s="5">
         <v>1000</v>
@@ -9517,10 +9617,10 @@
         <v>220</v>
       </c>
       <c r="AL29" s="15" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AN29" s="24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AO29" s="12"/>
     </row>
@@ -9529,10 +9629,10 @@
         <v>217</v>
       </c>
       <c r="B30" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>424</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>426</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
@@ -9556,7 +9656,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L30" s="5">
         <v>2</v>
@@ -9584,7 +9684,7 @@
         <v>64</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="U30" s="5">
         <v>1000</v>
@@ -9617,20 +9717,20 @@
         <v>220</v>
       </c>
       <c r="AL30" s="15" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AN30" s="24" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AO30" s="12"/>
     </row>
     <row r="31" spans="1:41">
       <c r="A31" s="15"/>
       <c r="B31" s="21" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D31" s="5">
         <v>1</v>
@@ -9654,7 +9754,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L31" s="5">
         <v>2</v>
@@ -9682,7 +9782,7 @@
         <v>64</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="U31" s="5">
         <v>1000</v>
@@ -9715,17 +9815,17 @@
         <v>220</v>
       </c>
       <c r="AL31" s="15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AN31" s="24" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AO31" s="12"/>
     </row>
     <row r="32" spans="1:41" s="12" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>212</v>
@@ -9921,7 +10021,7 @@
     <row r="34" spans="1:42" s="12" customFormat="1">
       <c r="A34" s="15"/>
       <c r="B34" s="21" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>212</v>
@@ -10006,14 +10106,14 @@
       <c r="AI34" s="13"/>
       <c r="AJ34" s="13"/>
       <c r="AK34" s="15" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="AL34" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AM34" s="15"/>
       <c r="AN34" s="24" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:42" s="12" customFormat="1">
@@ -10115,13 +10215,13 @@
       </c>
       <c r="AM35" s="15"/>
       <c r="AN35" s="24" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:42" s="12" customFormat="1">
       <c r="A36" s="15"/>
       <c r="B36" s="21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>222</v>
@@ -10217,7 +10317,7 @@
       </c>
       <c r="AM36" s="15"/>
       <c r="AN36" s="24" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="1:42">
@@ -10312,7 +10412,7 @@
         <v>362</v>
       </c>
       <c r="AN37" s="24" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AO37" s="12"/>
     </row>
@@ -10407,17 +10507,17 @@
         <v>220</v>
       </c>
       <c r="AL38" s="15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AM38" s="15"/>
       <c r="AN38" s="24" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:42" s="12" customFormat="1">
       <c r="A39" s="15"/>
       <c r="B39" s="21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>236</v>
@@ -10509,13 +10609,13 @@
       </c>
       <c r="AM39" s="15"/>
       <c r="AN39" s="24" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:42">
       <c r="A40" s="15"/>
       <c r="B40" s="21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>239</v>
@@ -10604,7 +10704,7 @@
         <v>364</v>
       </c>
       <c r="AN40" s="24" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AO40" s="12"/>
     </row>
@@ -12524,10 +12624,10 @@
     <row r="67" spans="1:166" s="12" customFormat="1">
       <c r="A67" s="2"/>
       <c r="B67" s="21" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D67">
         <v>4</v>
@@ -12551,7 +12651,7 @@
         <v>2</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L67" s="5">
         <v>2</v>
@@ -12608,7 +12708,7 @@
       </c>
       <c r="AM67" s="15"/>
       <c r="AN67" s="24" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="AO67" s="28"/>
       <c r="AP67" s="28"/>
@@ -12739,7 +12839,7 @@
     </row>
     <row r="68" spans="1:166">
       <c r="B68" s="21" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C68" s="24" t="s">
         <v>322</v>
@@ -12766,7 +12866,7 @@
         <v>2</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L68" s="5">
         <v>2</v>
@@ -12817,14 +12917,14 @@
         <v>373</v>
       </c>
       <c r="AN68" s="24" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AO68" s="12"/>
     </row>
     <row r="69" spans="1:166" s="12" customFormat="1">
       <c r="A69" s="2"/>
       <c r="B69" s="21" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C69" s="24" t="s">
         <v>323</v>
@@ -12885,7 +12985,7 @@
         <v>1000</v>
       </c>
       <c r="V69" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="W69" s="13">
         <v>1000</v>
@@ -12918,13 +13018,13 @@
       </c>
       <c r="AM69" s="15"/>
       <c r="AN69" s="24" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="70" spans="1:166" s="12" customFormat="1">
       <c r="A70" s="2"/>
       <c r="B70" s="21" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C70" s="24" t="s">
         <v>323</v>
@@ -13014,7 +13114,7 @@
       </c>
       <c r="AM70" s="15"/>
       <c r="AN70" s="24" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="71" spans="1:166" s="12" customFormat="1">
@@ -13546,7 +13646,7 @@
     <row r="78" spans="1:166">
       <c r="A78" s="21"/>
       <c r="B78" s="21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>298</v>
@@ -13637,7 +13737,7 @@
         <v>110</v>
       </c>
       <c r="AN78" s="24" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="AO78" s="12"/>
     </row>
@@ -14263,15 +14363,14 @@
       <c r="V88" s="13"/>
       <c r="W88" s="13"/>
       <c r="X88" s="13">
-        <f>40</f>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="Y88" s="13">
         <v>1</v>
       </c>
       <c r="Z88" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>40/1</v>
+        <v>1/1</v>
       </c>
       <c r="AA88" s="13">
         <v>0.02</v>
@@ -14388,7 +14487,7 @@
         <v>337</v>
       </c>
       <c r="AK89" s="15" t="s">
-        <v>421</v>
+        <v>463</v>
       </c>
       <c r="AN89" s="24" t="s">
         <v>376</v>
@@ -14459,15 +14558,14 @@
       <c r="V90" s="13"/>
       <c r="W90" s="13"/>
       <c r="X90" s="13">
-        <f>40</f>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="Y90" s="13">
         <v>1</v>
       </c>
       <c r="Z90" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>40/1</v>
+        <v>1/1</v>
       </c>
       <c r="AA90" s="13">
         <v>0.02</v>
@@ -14589,7 +14687,7 @@
       <c r="AI91" s="13"/>
       <c r="AJ91" s="13"/>
       <c r="AK91" s="15" t="s">
-        <v>422</v>
+        <v>464</v>
       </c>
       <c r="AL91" s="15"/>
       <c r="AM91" s="15"/>
@@ -14701,7 +14799,7 @@
     <row r="93" spans="1:41" s="12" customFormat="1">
       <c r="A93" s="21"/>
       <c r="B93" s="21" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>31</v>
@@ -14744,7 +14842,7 @@
         <v>32</v>
       </c>
       <c r="Q93" s="13">
-        <f t="shared" ref="Q93" si="18">M93*N93*P93/1000</f>
+        <f t="shared" ref="Q93:Q94" si="18">M93*N93*P93/1000</f>
         <v>0.70399999999999996</v>
       </c>
       <c r="R93" s="5">
@@ -14769,7 +14867,7 @@
         <v>1</v>
       </c>
       <c r="Z93" s="13" t="str">
-        <f t="shared" ref="Z93" si="19">X93&amp;"/"&amp;Y93</f>
+        <f t="shared" ref="Z93:Z94" si="19">X93&amp;"/"&amp;Y93</f>
         <v>40/1</v>
       </c>
       <c r="AA93" s="13">
@@ -14796,51 +14894,111 @@
       <c r="AL93" s="15"/>
       <c r="AM93" s="15"/>
       <c r="AN93" s="24" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="AO93" s="13"/>
     </row>
     <row r="94" spans="1:41" s="12" customFormat="1">
       <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-      <c r="P94" s="5"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="5"/>
-      <c r="S94" s="5"/>
-      <c r="T94" s="5"/>
-      <c r="U94" s="5"/>
+      <c r="B94" s="21" t="s">
+        <v>465</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D94" s="5">
+        <v>2</v>
+      </c>
+      <c r="E94" s="5">
+        <v>5120</v>
+      </c>
+      <c r="F94" s="5">
+        <v>14.028</v>
+      </c>
+      <c r="G94" s="5">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="H94" s="5">
+        <v>16</v>
+      </c>
+      <c r="I94" s="5">
+        <v>900</v>
+      </c>
+      <c r="J94" s="5">
+        <v>1</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="L94" s="5">
+        <v>2</v>
+      </c>
+      <c r="M94" s="5">
+        <v>10</v>
+      </c>
+      <c r="N94" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O94" s="5">
+        <v>16</v>
+      </c>
+      <c r="P94" s="5">
+        <v>32</v>
+      </c>
+      <c r="Q94" s="13">
+        <f t="shared" si="18"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="R94" s="5">
+        <v>2400</v>
+      </c>
+      <c r="S94" s="5">
+        <v>128</v>
+      </c>
+      <c r="T94" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="U94" s="5">
+        <v>960</v>
+      </c>
       <c r="V94" s="13"/>
       <c r="W94" s="13"/>
-      <c r="X94" s="13"/>
-      <c r="Y94" s="13"/>
-      <c r="Z94" s="13"/>
-      <c r="AA94" s="13"/>
+      <c r="X94" s="13">
+        <v>40</v>
+      </c>
+      <c r="Y94" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z94" s="13" t="str">
+        <f t="shared" si="19"/>
+        <v>40/1</v>
+      </c>
+      <c r="AA94" s="13">
+        <v>0.09</v>
+      </c>
       <c r="AB94" s="13"/>
-      <c r="AC94" s="13"/>
-      <c r="AD94" s="13"/>
+      <c r="AC94" s="13">
+        <v>466.35</v>
+      </c>
+      <c r="AD94" s="13">
+        <v>1866</v>
+      </c>
       <c r="AE94" s="13"/>
       <c r="AF94" s="13"/>
       <c r="AG94" s="13"/>
-      <c r="AH94" s="15"/>
+      <c r="AH94" s="15" t="s">
+        <v>337</v>
+      </c>
       <c r="AI94" s="13"/>
       <c r="AJ94" s="13"/>
-      <c r="AK94" s="15"/>
+      <c r="AK94" s="15" t="s">
+        <v>468</v>
+      </c>
       <c r="AL94" s="15"/>
       <c r="AM94" s="15"/>
-      <c r="AN94" s="24"/>
+      <c r="AN94" s="24" t="s">
+        <v>469</v>
+      </c>
       <c r="AO94" s="13"/>
     </row>
     <row r="95" spans="1:41" s="12" customFormat="1">
@@ -18863,438 +19021,438 @@
     <mergeCell ref="X3:Z3"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="AH76:AH77 B76:B77 AI76:AJ82 S35:S36 R37:W38 S39 C40:J40 V39:Y40 AI35:AJ40 AA35:AG35 C42:Z42 K45:U45 AI45:AJ45 A86:B86 B85 AH41:AJ42 A24:AG28 A12:X14 A9:L9 J11:L11 J10:K10 A10:I11 M9:X11 Y6:Y14 A16:D16 A17:B17 A18:Y21 T16:Y17 A6:X8 AA16:AG23 A22:B23 L22:L23 A74:B75 L74:AB75 FK67:XFD67 A89:A91 B87:B97 AP6:XFD14 AP38:XFD39 AP16:XFD36 AO75:XFD75 A5:XFD5 Z6:AN11 AA12:AN14 A46:AN56 B57:AN64 AH74:AJ75 C98:R115 S111:AB115 AC98:AN115 AN124:AN126 AH124:AK126 A124:A154 AO87:AO154 A116:AN123 AP42:XFD45 B35:J36 B37:P38 A29:A36 B39:J39 B41:Z41 A38:A45 B42:B45 AO6:AO45 K29:K31 B29:D31 S29:W31 AA29:AG31 AH16:AN28 C78:D78 J78 A76:A85 L76:T77 V76:W77 U76:U84 Z76:AB77 X76:Y84 AC74:AG83 C74:J77 AP76:XFD77 AO76:AO82 K76:K84 AK74:AN97 AI29:AJ31 X29:Y40 AL29:AN31 FK74:XFD74 AO46:XFD65 A57:A65 A66:XFD66 A67:AN67 A68:XFD73">
-    <cfRule type="expression" dxfId="102" priority="296">
+  <conditionalFormatting sqref="AH76:AH77 B76:B77 AI76:AJ82 S35:S36 R37:W38 S39 C40:J40 V39:Y40 AI35:AJ40 AA35:AG35 C42:Z42 K45:U45 AI45:AJ45 A86:B86 B85 AH41:AJ42 A24:AG28 A12:X14 A9:L9 J11:L11 J10:K10 A10:I11 M9:X11 Y6:Y14 A16:D16 A17:B17 A18:Y21 T16:Y17 A6:X8 AA16:AG23 A22:B23 L22:L23 A74:B75 L74:AB75 FK67:XFD67 A89:A91 B87:B97 AP6:XFD14 AP38:XFD39 AP16:XFD36 AO75:XFD75 A5:XFD5 Z6:AN11 AA12:AN14 A46:AN56 B57:AN64 AH74:AJ75 C98:R115 S111:AB115 AC98:AN115 AN124:AN126 AH124:AK126 A124:A154 AO87:AO154 A116:AN123 AP42:XFD45 B35:J36 B37:P38 A29:A36 B39:J39 B41:Z41 A38:A45 B42:B45 AO6:AO45 K29:K31 B29:D31 S29:W31 AA29:AG31 AH16:AN28 C78:D78 J78 A76:A85 L76:T77 V76:W77 U76:U84 Z76:AB77 X76:Y84 AC74:AG83 C74:J77 AP76:XFD77 AO76:AO82 K76:K84 AI29:AJ31 X29:Y40 AL29:AN31 FK74:XFD74 AO46:XFD65 A57:A65 A66:XFD66 A67:AN67 A68:XFD73 AK74:AN97">
+    <cfRule type="expression" dxfId="103" priority="296">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74:K75">
-    <cfRule type="expression" dxfId="101" priority="235">
+    <cfRule type="expression" dxfId="102" priority="235">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B84 B79:J79 L78:T84 V78:W84 Z84:AD84 Z78:AB83 B78 AH78:AH97">
-    <cfRule type="expression" dxfId="100" priority="223">
+    <cfRule type="expression" dxfId="101" priority="223">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:J45">
-    <cfRule type="expression" dxfId="99" priority="158">
+    <cfRule type="expression" dxfId="100" priority="158">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:P34 B32:D34 J32 S32:W32 AA32:AG34 AK35:AN36 AI32:AN34 R33:W34">
-    <cfRule type="expression" dxfId="98" priority="189">
+    <cfRule type="expression" dxfId="99" priority="189">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32:I34">
-    <cfRule type="expression" dxfId="97" priority="188">
+    <cfRule type="expression" dxfId="98" priority="188">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:R32 Q33:Q34">
-    <cfRule type="expression" dxfId="96" priority="187">
+    <cfRule type="expression" dxfId="97" priority="187">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z29:Z34">
-    <cfRule type="expression" dxfId="95" priority="186">
+    <cfRule type="expression" dxfId="96" priority="186">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:R35">
-    <cfRule type="expression" dxfId="94" priority="184">
+    <cfRule type="expression" dxfId="95" priority="184">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T35:U36">
-    <cfRule type="expression" dxfId="93" priority="183">
+    <cfRule type="expression" dxfId="94" priority="183">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V35:W36">
-    <cfRule type="expression" dxfId="92" priority="182">
+    <cfRule type="expression" dxfId="93" priority="182">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z35:Z40">
-    <cfRule type="expression" dxfId="91" priority="180">
+    <cfRule type="expression" dxfId="92" priority="180">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:P36 R36">
-    <cfRule type="expression" dxfId="90" priority="179">
+    <cfRule type="expression" dxfId="91" priority="179">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q36:Q38">
-    <cfRule type="expression" dxfId="89" priority="178">
+    <cfRule type="expression" dxfId="90" priority="178">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH29:AH40">
-    <cfRule type="expression" dxfId="88" priority="177">
+    <cfRule type="expression" dxfId="89" priority="177">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39:U40">
-    <cfRule type="expression" dxfId="87" priority="174">
+    <cfRule type="expression" dxfId="88" priority="174">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK37:AN40">
-    <cfRule type="expression" dxfId="86" priority="176">
+    <cfRule type="expression" dxfId="87" priority="176">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:R39">
-    <cfRule type="expression" dxfId="85" priority="175">
+    <cfRule type="expression" dxfId="86" priority="175">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="84" priority="173">
+    <cfRule type="expression" dxfId="85" priority="173">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:P40 R40">
-    <cfRule type="expression" dxfId="83" priority="172">
+    <cfRule type="expression" dxfId="84" priority="172">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q40">
-    <cfRule type="expression" dxfId="82" priority="171">
+    <cfRule type="expression" dxfId="83" priority="171">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40">
-    <cfRule type="expression" dxfId="81" priority="170">
+    <cfRule type="expression" dxfId="82" priority="170">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK41:AN41">
-    <cfRule type="expression" dxfId="80" priority="169">
+    <cfRule type="expression" dxfId="81" priority="169">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK42:AN42">
-    <cfRule type="expression" dxfId="79" priority="168">
+    <cfRule type="expression" dxfId="80" priority="168">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:P43 R43">
-    <cfRule type="expression" dxfId="78" priority="167">
+    <cfRule type="expression" dxfId="79" priority="167">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q43">
-    <cfRule type="expression" dxfId="77" priority="166">
+    <cfRule type="expression" dxfId="78" priority="166">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43:U43">
-    <cfRule type="expression" dxfId="76" priority="165">
+    <cfRule type="expression" dxfId="77" priority="165">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43:W43">
-    <cfRule type="expression" dxfId="75" priority="164">
+    <cfRule type="expression" dxfId="76" priority="164">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X43:Y43">
-    <cfRule type="expression" dxfId="74" priority="163">
+    <cfRule type="expression" dxfId="75" priority="163">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z43">
-    <cfRule type="expression" dxfId="73" priority="162">
+    <cfRule type="expression" dxfId="74" priority="162">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH43:AJ43">
-    <cfRule type="expression" dxfId="72" priority="161">
+    <cfRule type="expression" dxfId="73" priority="161">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK43:AN43">
-    <cfRule type="expression" dxfId="71" priority="160">
+    <cfRule type="expression" dxfId="72" priority="160">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:P44 R44:U44">
-    <cfRule type="expression" dxfId="70" priority="157">
+    <cfRule type="expression" dxfId="71" priority="157">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q44">
-    <cfRule type="expression" dxfId="69" priority="156">
+    <cfRule type="expression" dxfId="70" priority="156">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V44:Y45 AA36:AC45">
-    <cfRule type="expression" dxfId="68" priority="155">
+    <cfRule type="expression" dxfId="69" priority="155">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44:Z45">
-    <cfRule type="expression" dxfId="67" priority="154">
+    <cfRule type="expression" dxfId="68" priority="154">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD36:AD45">
-    <cfRule type="expression" dxfId="66" priority="153">
+    <cfRule type="expression" dxfId="67" priority="153">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE45:AH45 AH44 AE36:AG44">
-    <cfRule type="expression" dxfId="65" priority="152">
+    <cfRule type="expression" dxfId="66" priority="152">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI44:AJ44">
-    <cfRule type="expression" dxfId="64" priority="151">
+    <cfRule type="expression" dxfId="65" priority="151">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK44:AN45">
-    <cfRule type="expression" dxfId="63" priority="150">
+    <cfRule type="expression" dxfId="64" priority="150">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP41">
-    <cfRule type="expression" dxfId="62" priority="141">
+    <cfRule type="expression" dxfId="63" priority="141">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="61" priority="140">
+    <cfRule type="expression" dxfId="62" priority="140">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C84">
-    <cfRule type="expression" dxfId="60" priority="118">
+    <cfRule type="expression" dxfId="61" priority="118">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D80:J84">
-    <cfRule type="expression" dxfId="59" priority="117">
+    <cfRule type="expression" dxfId="60" priority="117">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L85:AG92 AI85:AJ97 L94:AG97 AA93:AG93">
-    <cfRule type="expression" dxfId="58" priority="115">
+  <conditionalFormatting sqref="L85:AG92 AI85:AJ97 L95:AG97 L94:P94 R94:Y94 AA93:AG94">
+    <cfRule type="expression" dxfId="59" priority="115">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85:K92 C94:K97 J93">
-    <cfRule type="expression" dxfId="57" priority="114">
+  <conditionalFormatting sqref="C85:K92 J93 C94:K97">
+    <cfRule type="expression" dxfId="58" priority="114">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE84:AG84 AI83:AJ84">
-    <cfRule type="expression" dxfId="56" priority="113">
+    <cfRule type="expression" dxfId="57" priority="113">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111 B113 B115">
-    <cfRule type="expression" dxfId="55" priority="64">
+    <cfRule type="expression" dxfId="56" priority="64">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO155 AI127:AN155 AC124:AG155 AL124:AM126">
-    <cfRule type="expression" dxfId="54" priority="102">
+    <cfRule type="expression" dxfId="55" priority="102">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87:A88">
-    <cfRule type="expression" dxfId="53" priority="100">
+    <cfRule type="expression" dxfId="54" priority="100">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:A97">
-    <cfRule type="expression" dxfId="52" priority="96">
+    <cfRule type="expression" dxfId="53" priority="96">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH127:AH155">
-    <cfRule type="expression" dxfId="51" priority="80">
+    <cfRule type="expression" dxfId="52" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99 B101 B103:B110 A98:A110">
-    <cfRule type="expression" dxfId="50" priority="74">
+    <cfRule type="expression" dxfId="51" priority="74">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98 B100 B102">
-    <cfRule type="expression" dxfId="49" priority="73">
+    <cfRule type="expression" dxfId="50" priority="73">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L135:R155 R133:R134 L124:R131">
-    <cfRule type="expression" dxfId="48" priority="72">
+    <cfRule type="expression" dxfId="49" priority="72">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:K155 J124:K126 C124:C126">
-    <cfRule type="expression" dxfId="47" priority="71">
+    <cfRule type="expression" dxfId="48" priority="71">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S98:AB110">
-    <cfRule type="expression" dxfId="46" priority="70">
+    <cfRule type="expression" dxfId="47" priority="70">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S124:AB125 S127:AB129 S126:W126 AA126:AB126">
-    <cfRule type="expression" dxfId="45" priority="68">
+    <cfRule type="expression" dxfId="46" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S130:AB131 S135:AB135 S133:S134 V132:AB134">
-    <cfRule type="expression" dxfId="44" priority="67">
+    <cfRule type="expression" dxfId="45" priority="67">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S136:AB141 S142:Z156 AA142:AB155">
-    <cfRule type="expression" dxfId="43" priority="66">
+    <cfRule type="expression" dxfId="44" priority="66">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112 B114 A111:A115 A155:B155 B127:B154">
-    <cfRule type="expression" dxfId="42" priority="65">
+    <cfRule type="expression" dxfId="43" priority="65">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z12:Z14 Z16:Z21">
-    <cfRule type="expression" dxfId="41" priority="56">
+    <cfRule type="expression" dxfId="42" priority="56">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="expression" dxfId="40" priority="55">
+    <cfRule type="expression" dxfId="41" priority="55">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:Y15 AP15:XFD15 AA15:AN15">
-    <cfRule type="expression" dxfId="39" priority="50">
+    <cfRule type="expression" dxfId="40" priority="50">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z15">
-    <cfRule type="expression" dxfId="38" priority="48">
+    <cfRule type="expression" dxfId="39" priority="48">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:S16 J17">
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="38" priority="47">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:I17">
-    <cfRule type="expression" dxfId="36" priority="46">
+    <cfRule type="expression" dxfId="37" priority="46">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:S17">
-    <cfRule type="expression" dxfId="35" priority="45">
+    <cfRule type="expression" dxfId="36" priority="45">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:D23 T22:Y23">
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="35" priority="44">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z22:Z23">
-    <cfRule type="expression" dxfId="33" priority="43">
+    <cfRule type="expression" dxfId="34" priority="43">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:K23 M22:S23">
-    <cfRule type="expression" dxfId="32" priority="42">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65:AN65">
-    <cfRule type="expression" dxfId="31" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L132:R132 L133:Q134">
-    <cfRule type="expression" dxfId="30" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S132:U132 T133:U134">
-    <cfRule type="expression" dxfId="29" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124 B126">
-    <cfRule type="expression" dxfId="28" priority="12">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="expression" dxfId="27" priority="13">
+    <cfRule type="expression" dxfId="28" priority="13">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D124:I126">
-    <cfRule type="expression" dxfId="26" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X126:Z126">
-    <cfRule type="expression" dxfId="25" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:J31">
-    <cfRule type="expression" dxfId="24" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:P31 R30:R31">
-    <cfRule type="expression" dxfId="23" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:R29 Q30:Q31">
-    <cfRule type="expression" dxfId="22" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:I78">
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="20" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93:I93">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L93:Z93">
-    <cfRule type="expression" dxfId="18" priority="3">
+  <conditionalFormatting sqref="L93:Z93 Q94 Z94">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K93">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK29:AK31">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19315,13 +19473,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AE93"/>
+  <dimension ref="A1:AE94"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -19656,7 +19814,7 @@
         <v>AZ p2.8xl-</v>
       </c>
       <c r="F4" s="18">
-        <f t="shared" ref="F4:H82" ca="1" si="5">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="F4:H83" ca="1" si="5">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="G4" s="18">
@@ -21576,7 +21734,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="18">
-        <f t="shared" ref="L22:L88" ca="1" si="16">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="L22:L89" ca="1" si="16">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="M22" s="18" t="str">
@@ -23054,7 +23212,7 @@
         <v>1000</v>
       </c>
       <c r="W35" s="13" t="str">
-        <f t="shared" ref="W35:W61" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="W35:W62" ca="1" si="29">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>SATA</v>
       </c>
       <c r="X35" s="13">
@@ -23074,7 +23232,7 @@
         <v>0</v>
       </c>
       <c r="AB35" s="15">
-        <f t="shared" ref="AB35:AB63" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="AB35:AB64" ca="1" si="30">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="AC35" s="29">
@@ -23686,11 +23844,11 @@
         <v>USD</v>
       </c>
       <c r="N41" s="13">
-        <f t="shared" ref="N41:N89" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="N41:N90" ca="1" si="33">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!L"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>1.4079999999999999</v>
       </c>
       <c r="O41" s="13">
-        <f t="shared" ref="O41:O61" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="O41:O62" ca="1" si="34">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>94.063999999999993</v>
       </c>
       <c r="P41" s="13" t="str">
@@ -23977,7 +24135,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="21" t="str">
-        <f t="shared" ref="C44:E62" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="C44:E63" ca="1" si="36">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>16-GPU x86 K80 ltd.</v>
       </c>
       <c r="D44" s="15" t="str">
@@ -24732,7 +24890,7 @@
         <v>SSD</v>
       </c>
       <c r="X50" s="13">
-        <f t="shared" ref="X50:Y61" ca="1" si="38">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="X50:Y62" ca="1" si="38">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>480</v>
       </c>
       <c r="Y50" s="13" t="str">
@@ -24740,7 +24898,7 @@
         <v>10/0.1</v>
       </c>
       <c r="Z50" s="13">
-        <f t="shared" ref="Z50:AA64" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="Z50:AA65" ca="1" si="39">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="AA50" s="13">
@@ -24781,7 +24939,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="18">
-        <f t="shared" ref="H51:I62" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="H51:I63" ca="1" si="40">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="I51" s="18">
@@ -24789,7 +24947,7 @@
         <v>115000</v>
       </c>
       <c r="J51" s="18">
-        <f t="shared" ref="J51:K68" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="J51:K69" ca="1" si="41">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="K51" s="18">
@@ -25035,7 +25193,7 @@
         <v>9.5</v>
       </c>
       <c r="P53" s="13" t="str">
-        <f t="shared" ref="P53:X71" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="P53:X72" ca="1" si="42">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>P100</v>
       </c>
       <c r="Q53" s="13">
@@ -25299,7 +25457,7 @@
       </c>
       <c r="Y55" s="13" t="str">
         <f t="shared" ca="1" si="38"/>
-        <v>40/1</v>
+        <v>1/1</v>
       </c>
       <c r="Z55" s="13">
         <f t="shared" ca="1" si="39"/>
@@ -25428,7 +25586,7 @@
       </c>
       <c r="AB56" s="15" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till the end of February 2018.</v>
+        <v>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till the end of ..</v>
       </c>
       <c r="AC56" s="29">
         <v>89</v>
@@ -25525,7 +25683,7 @@
       </c>
       <c r="Y57" s="13" t="str">
         <f t="shared" ca="1" si="38"/>
-        <v>40/1</v>
+        <v>1/1</v>
       </c>
       <c r="Z57" s="13">
         <f t="shared" ca="1" si="39"/>
@@ -25561,7 +25719,7 @@
         <v>0.03</v>
       </c>
       <c r="G58" s="13">
-        <f t="shared" ref="G58:G84" ca="1" si="43">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ref="G58:G85" ca="1" si="43">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="H58" s="18">
@@ -25646,7 +25804,7 @@
       </c>
       <c r="AB58" s="15" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till end of February 2018.</v>
+        <v>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,09 &amp;euro;/Gb. Special price till end of ...</v>
       </c>
       <c r="AC58" s="29">
         <v>91</v>
@@ -25875,30 +26033,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="19">
-      <c r="A61" s="35" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>The University of Tokyo</v>
-      </c>
-      <c r="B61" s="15" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
-        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</v>
-      </c>
+    <row r="61" spans="1:29" s="12" customFormat="1" ht="20">
+      <c r="A61" s="36"/>
       <c r="C61" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>Reedbush-H Personal (educational)</v>
-      </c>
-      <c r="D61" s="15" t="str">
+        <v>2 x V100nvlink</v>
+      </c>
+      <c r="D61" s="15">
         <f t="shared" ca="1" si="36"/>
-        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
+        <v>0</v>
       </c>
       <c r="E61" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>TU personal</v>
+        <v>LT V100x2NVlink</v>
       </c>
       <c r="F61" s="18">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="G61" s="13">
         <f t="shared" ca="1" si="43"/>
@@ -25906,15 +26057,15 @@
       </c>
       <c r="H61" s="18">
         <f t="shared" ca="1" si="40"/>
-        <v>0</v>
+        <v>466.35</v>
       </c>
       <c r="I61" s="18">
         <f t="shared" ca="1" si="40"/>
-        <v>0</v>
+        <v>1866</v>
       </c>
       <c r="J61" s="18">
         <f t="shared" ca="1" si="41"/>
-        <v>138888.88888888888</v>
+        <v>0</v>
       </c>
       <c r="K61" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -25926,19 +26077,19 @@
       </c>
       <c r="M61" s="18" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>JPY</v>
+        <v>EUR</v>
       </c>
       <c r="N61" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>2.4192000000000005</v>
+        <v>1.4079999999999999</v>
       </c>
       <c r="O61" s="13">
         <f t="shared" ca="1" si="34"/>
-        <v>19</v>
+        <v>28.056000000000001</v>
       </c>
       <c r="P61" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>P100</v>
+        <v>V100</v>
       </c>
       <c r="Q61" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -25946,7 +26097,7 @@
       </c>
       <c r="R61" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>Xeon E5-2695 v4</v>
+        <v>Xeon Silver 4114</v>
       </c>
       <c r="S61" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -25954,15 +26105,15 @@
       </c>
       <c r="T61" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="U61" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>PFS</v>
+        <v>SSD</v>
       </c>
       <c r="V61" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1000</v>
+        <v>960</v>
       </c>
       <c r="W61" s="13">
         <f t="shared" ca="1" si="29"/>
@@ -25974,11 +26125,11 @@
       </c>
       <c r="Y61" s="13" t="str">
         <f t="shared" ca="1" si="38"/>
-        <v>109.12/</v>
+        <v>40/1</v>
       </c>
       <c r="Z61" s="13">
-        <f t="shared" ref="Z61:Z71" ca="1" si="44">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>6912</v>
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
       </c>
       <c r="AA61" s="13">
         <f t="shared" ca="1" si="39"/>
@@ -25986,17 +26137,24 @@
       </c>
       <c r="AB61" s="15" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>For individuals from educational or public organisations. Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
+        <v>Included Internet traffic for monthly based payments: 10 Tb/month; weekly based payments: 2.5 Tb/week; minute/hourly based payments: 0 Gb. Additional 1Gb (not included): 0,10 &amp;euro;/Gb.</v>
       </c>
       <c r="AC61" s="29">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="20">
-      <c r="A62" s="36"/>
+    <row r="62" spans="1:29" ht="19">
+      <c r="A62" s="35" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>The University of Tokyo</v>
+      </c>
+      <c r="B62" s="15" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_intro.html</v>
+      </c>
       <c r="C62" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>Reedbush-H (educational)</v>
+        <v>Reedbush-H Personal (educational)</v>
       </c>
       <c r="D62" s="15" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -26004,7 +26162,7 @@
       </c>
       <c r="E62" s="21" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>TU edu</v>
+        <v>TU personal</v>
       </c>
       <c r="F62" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26024,7 +26182,7 @@
       </c>
       <c r="J62" s="18">
         <f t="shared" ca="1" si="41"/>
-        <v>277777.77777777775</v>
+        <v>138888.88888888888</v>
       </c>
       <c r="K62" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -26043,7 +26201,7 @@
         <v>2.4192000000000005</v>
       </c>
       <c r="O62" s="13">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>19</v>
       </c>
       <c r="P62" s="13" t="str">
@@ -26072,23 +26230,23 @@
       </c>
       <c r="V62" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="W62" s="13">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="X62" s="13">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y62" s="13" t="str">
-        <f t="shared" ref="Y62:Y71" ca="1" si="45">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="38"/>
         <v>109.12/</v>
       </c>
       <c r="Z62" s="13">
-        <f t="shared" ca="1" si="44"/>
-        <v>13824</v>
+        <f t="shared" ref="Z62:Z72" ca="1" si="44">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>6912</v>
       </c>
       <c r="AA62" s="13">
         <f t="shared" ca="1" si="39"/>
@@ -26096,24 +26254,25 @@
       </c>
       <c r="AB62" s="15" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>For groups from educational or public organisations. Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
+        <v>For individuals from educational or public organisations. Max 2 nodes. Included (17280/2.5=)6912 node hours if 1 node is used, 3456 node hours if more than 1 node is used by a parallel job.</v>
       </c>
       <c r="AC62" s="29">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:29">
+    <row r="63" spans="1:29" ht="20">
+      <c r="A63" s="36"/>
       <c r="C63" s="21" t="str">
-        <f t="shared" ref="C63:E79" ca="1" si="46">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Reedbush-H reviewed (educational)</v>
+        <f t="shared" ca="1" si="36"/>
+        <v>Reedbush-H (educational)</v>
       </c>
       <c r="D63" s="15" t="str">
-        <f t="shared" ca="1" si="46"/>
+        <f t="shared" ca="1" si="36"/>
         <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
       </c>
       <c r="E63" s="21" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>TU rev edu</v>
+        <f t="shared" ca="1" si="36"/>
+        <v>TU edu</v>
       </c>
       <c r="F63" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26124,16 +26283,16 @@
         <v>0</v>
       </c>
       <c r="H63" s="18">
-        <f t="shared" ref="H63:K82" ca="1" si="47">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
       <c r="I63" s="18">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
       <c r="J63" s="18">
         <f t="shared" ca="1" si="41"/>
-        <v>166666.66666666666</v>
+        <v>277777.77777777775</v>
       </c>
       <c r="K63" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -26144,7 +26303,7 @@
         <v>0</v>
       </c>
       <c r="M63" s="18" t="str">
-        <f t="shared" ref="M63:M89" ca="1" si="48">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>JPY</v>
       </c>
       <c r="N63" s="13">
@@ -26192,12 +26351,12 @@
         <v>0</v>
       </c>
       <c r="Y63" s="13" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ref="Y63:Y72" ca="1" si="45">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>109.12/</v>
       </c>
       <c r="Z63" s="13">
         <f t="shared" ca="1" si="44"/>
-        <v>8640</v>
+        <v>13824</v>
       </c>
       <c r="AA63" s="13">
         <f t="shared" ca="1" si="39"/>
@@ -26205,17 +26364,16 @@
       </c>
       <c r="AB63" s="15" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>For groups from educational or public organisations. Included 8640 node hours. Must pass review prior to usage. 4320 node hours if a parallel job used more nodes than applied for.</v>
+        <v>For groups from educational or public organisations. Included 13824 node hours if 1 node is used, 6912 node hours if 2-4 nodes are used by a parallel job.</v>
       </c>
       <c r="AC63" s="29">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="20">
-      <c r="A64" s="36"/>
+    <row r="64" spans="1:29">
       <c r="C64" s="21" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>Reedbush-H reviewed</v>
+        <f t="shared" ref="C64:E80" ca="1" si="46">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>Reedbush-H reviewed (educational)</v>
       </c>
       <c r="D64" s="15" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -26223,7 +26381,7 @@
       </c>
       <c r="E64" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>TU rev</v>
+        <v>TU rev edu</v>
       </c>
       <c r="F64" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26234,7 +26392,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="18">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ref="H64:K83" ca="1" si="47">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="I64" s="18">
@@ -26243,7 +26401,7 @@
       </c>
       <c r="J64" s="18">
         <f t="shared" ca="1" si="41"/>
-        <v>200000</v>
+        <v>166666.66666666666</v>
       </c>
       <c r="K64" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -26254,7 +26412,7 @@
         <v>0</v>
       </c>
       <c r="M64" s="18" t="str">
-        <f t="shared" ca="1" si="48"/>
+        <f t="shared" ref="M64:M90" ca="1" si="48">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>JPY</v>
       </c>
       <c r="N64" s="13">
@@ -26314,17 +26472,18 @@
         <v>0</v>
       </c>
       <c r="AB64" s="15" t="str">
-        <f t="shared" ref="AB64:AB89" ca="1" si="49">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+        <f t="shared" ca="1" si="30"/>
+        <v>For groups from educational or public organisations. Included 8640 node hours. Must pass review prior to usage. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
       <c r="AC64" s="29">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:29">
+    <row r="65" spans="1:29" ht="20">
+      <c r="A65" s="36"/>
       <c r="C65" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>Reedbush-H dedicated reviewed (educational)</v>
+        <v>Reedbush-H reviewed</v>
       </c>
       <c r="D65" s="15" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -26332,7 +26491,7 @@
       </c>
       <c r="E65" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>TU ded. rev edu</v>
+        <v>TU rev</v>
       </c>
       <c r="F65" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26352,7 +26511,7 @@
       </c>
       <c r="J65" s="18">
         <f t="shared" ca="1" si="41"/>
-        <v>249999.99999999997</v>
+        <v>200000</v>
       </c>
       <c r="K65" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -26363,7 +26522,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="18" t="str">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="48"/>
         <v>JPY</v>
       </c>
       <c r="N65" s="13">
@@ -26419,21 +26578,21 @@
         <v>8640</v>
       </c>
       <c r="AA65" s="13">
-        <f t="shared" ref="AA65:AA72" ca="1" si="50">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="AB65" s="15" t="str">
-        <f t="shared" ca="1" si="49"/>
+        <f t="shared" ref="AB65:AB90" ca="1" si="49">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
       <c r="AC65" s="29">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:29">
       <c r="C66" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>Reedbush-H dedicated reviewed</v>
+        <v>Reedbush-H dedicated reviewed (educational)</v>
       </c>
       <c r="D66" s="15" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -26441,7 +26600,7 @@
       </c>
       <c r="E66" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>TU ded. rev</v>
+        <v>TU ded. rev edu</v>
       </c>
       <c r="F66" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26460,8 +26619,8 @@
         <v>0</v>
       </c>
       <c r="J66" s="18">
-        <f t="shared" ca="1" si="47"/>
-        <v>300000</v>
+        <f t="shared" ca="1" si="41"/>
+        <v>249999.99999999997</v>
       </c>
       <c r="K66" s="18">
         <f t="shared" ca="1" si="41"/>
@@ -26472,7 +26631,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="18" t="str">
-        <f t="shared" ca="1" si="48"/>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>JPY</v>
       </c>
       <c r="N66" s="13">
@@ -26480,7 +26639,7 @@
         <v>2.4192000000000005</v>
       </c>
       <c r="O66" s="13">
-        <f t="shared" ref="O66:O89" ca="1" si="51">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
         <v>19</v>
       </c>
       <c r="P66" s="13" t="str">
@@ -26528,7 +26687,7 @@
         <v>8640</v>
       </c>
       <c r="AA66" s="13">
-        <f t="shared" ca="1" si="50"/>
+        <f t="shared" ref="AA66:AA73" ca="1" si="50">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="AB66" s="15" t="str">
@@ -26536,146 +26695,146 @@
         <v>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
       </c>
       <c r="AC66" s="29">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29">
+      <c r="C67" s="21" t="str">
+        <f t="shared" ca="1" si="46"/>
+        <v>Reedbush-H dedicated reviewed</v>
+      </c>
+      <c r="D67" s="15" t="str">
+        <f t="shared" ca="1" si="46"/>
+        <v>http://www.cc.u-tokyo.ac.jp/system/reedbush/reedbush_course.html</v>
+      </c>
+      <c r="E67" s="21" t="str">
+        <f t="shared" ca="1" si="46"/>
+        <v>TU ded. rev</v>
+      </c>
+      <c r="F67" s="18">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="13">
+        <f t="shared" ca="1" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="H67" s="18">
+        <f t="shared" ca="1" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="I67" s="18">
+        <f t="shared" ca="1" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="18">
+        <f t="shared" ca="1" si="47"/>
+        <v>300000</v>
+      </c>
+      <c r="K67" s="18">
+        <f t="shared" ca="1" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="18">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M67" s="18" t="str">
+        <f t="shared" ca="1" si="48"/>
+        <v>JPY</v>
+      </c>
+      <c r="N67" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>2.4192000000000005</v>
+      </c>
+      <c r="O67" s="13">
+        <f t="shared" ref="O67:O90" ca="1" si="51">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW())) * INDIRECT("Sheet1!D"&amp; INDIRECT("AC"&amp;ROW()))</f>
+        <v>19</v>
+      </c>
+      <c r="P67" s="13" t="str">
+        <f t="shared" ca="1" si="42"/>
+        <v>P100</v>
+      </c>
+      <c r="Q67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>2</v>
+      </c>
+      <c r="R67" s="13" t="str">
+        <f t="shared" ca="1" si="42"/>
+        <v>Xeon E5-2695 v4</v>
+      </c>
+      <c r="S67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>2</v>
+      </c>
+      <c r="T67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>256</v>
+      </c>
+      <c r="U67" s="13" t="str">
+        <f t="shared" ca="1" si="42"/>
+        <v>PFS</v>
+      </c>
+      <c r="V67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>4000</v>
+      </c>
+      <c r="W67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="X67" s="13">
+        <f t="shared" ca="1" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="Y67" s="13" t="str">
+        <f t="shared" ca="1" si="45"/>
+        <v>109.12/</v>
+      </c>
+      <c r="Z67" s="13">
+        <f t="shared" ca="1" si="44"/>
+        <v>8640</v>
+      </c>
+      <c r="AA67" s="13">
+        <f t="shared" ca="1" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AB67" s="15" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Must pass review prior to usage. Included 8640 node hours. 4320 node hours if a parallel job used more nodes than applied for.</v>
+      </c>
+      <c r="AC67" s="29">
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:29" ht="19">
-      <c r="A67" s="35" t="str">
+    <row r="68" spans="1:29" ht="19">
+      <c r="A68" s="35" t="str">
         <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
         <v>MS Azure</v>
       </c>
-      <c r="B67" s="15" t="str">
+      <c r="B68" s="15" t="str">
         <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
         <v>https://azure.microsoft.com/en-us/pricing/details/virtual-machines/linux/</v>
       </c>
-      <c r="C67" s="21" t="str">
+      <c r="C68" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
         <v>NC6</v>
       </c>
-      <c r="D67" s="15">
+      <c r="D68" s="15">
         <f t="shared" ca="1" si="46"/>
         <v>0</v>
       </c>
-      <c r="E67" s="21" t="str">
+      <c r="E68" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
         <v>MS NC6</v>
       </c>
-      <c r="F67" s="18">
+      <c r="F68" s="18">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G68" s="13">
         <f t="shared" ca="1" si="43"/>
         <v>0.9</v>
-      </c>
-      <c r="H67" s="18">
-        <f t="shared" ca="1" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="I67" s="18">
-        <f t="shared" ca="1" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="J67" s="18">
-        <f t="shared" ca="1" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="K67" s="18">
-        <f t="shared" ca="1" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="L67" s="18">
-        <f t="shared" ca="1" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M67" s="18" t="str">
-        <f t="shared" ca="1" si="48"/>
-        <v>USD</v>
-      </c>
-      <c r="N67" s="13">
-        <f t="shared" ca="1" si="33"/>
-        <v>0.24960000000000002</v>
-      </c>
-      <c r="O67" s="13">
-        <f t="shared" ca="1" si="51"/>
-        <v>4.37</v>
-      </c>
-      <c r="P67" s="13" t="str">
-        <f t="shared" ca="1" si="42"/>
-        <v>K80</v>
-      </c>
-      <c r="Q67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.5</v>
-      </c>
-      <c r="R67" s="13" t="str">
-        <f t="shared" ca="1" si="42"/>
-        <v>Xeon E5-2690 v3</v>
-      </c>
-      <c r="S67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>0.25</v>
-      </c>
-      <c r="T67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>56</v>
-      </c>
-      <c r="U67" s="13" t="str">
-        <f t="shared" ca="1" si="42"/>
-        <v>SSD</v>
-      </c>
-      <c r="V67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>340</v>
-      </c>
-      <c r="W67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="X67" s="13">
-        <f t="shared" ca="1" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="Y67" s="13">
-        <f t="shared" ca="1" si="45"/>
-        <v>0</v>
-      </c>
-      <c r="Z67" s="13">
-        <f t="shared" ca="1" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="AA67" s="13">
-        <f t="shared" ca="1" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="AB67" s="15" t="str">
-        <f t="shared" ca="1" si="49"/>
-        <v>Prices for West US 2 region. Charged per minute. 1 GPU in specification is 1/2 of K80 board.</v>
-      </c>
-      <c r="AC67" s="29">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:29">
-      <c r="C68" s="21" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>NC12</v>
-      </c>
-      <c r="D68" s="15">
-        <f t="shared" ca="1" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="E68" s="21" t="str">
-        <f t="shared" ca="1" si="46"/>
-        <v>MS NC12</v>
-      </c>
-      <c r="F68" s="18">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G68" s="13">
-        <f t="shared" ca="1" si="43"/>
-        <v>1.8</v>
       </c>
       <c r="H68" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -26703,11 +26862,11 @@
       </c>
       <c r="N68" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.49920000000000003</v>
+        <v>0.24960000000000002</v>
       </c>
       <c r="O68" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>8.74</v>
+        <v>4.37</v>
       </c>
       <c r="P68" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26715,7 +26874,7 @@
       </c>
       <c r="Q68" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R68" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26723,11 +26882,11 @@
       </c>
       <c r="S68" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="T68" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="U68" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26735,7 +26894,7 @@
       </c>
       <c r="V68" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="W68" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -26759,18 +26918,16 @@
       </c>
       <c r="AB68" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
+        <v>Prices for West US 2 region. Charged per minute. 1 GPU in specification is 1/2 of K80 board.</v>
       </c>
       <c r="AC68" s="29">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="20">
-      <c r="A69" s="36"/>
-      <c r="B69" s="15"/>
+    <row r="69" spans="1:29">
       <c r="C69" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>NC24</v>
+        <v>NC12</v>
       </c>
       <c r="D69" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -26778,7 +26935,7 @@
       </c>
       <c r="E69" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>MS NC24</v>
+        <v>MS NC12</v>
       </c>
       <c r="F69" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26786,7 +26943,7 @@
       </c>
       <c r="G69" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>3.6</v>
+        <v>1.8</v>
       </c>
       <c r="H69" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -26801,7 +26958,7 @@
         <v>0</v>
       </c>
       <c r="K69" s="18">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="41"/>
         <v>0</v>
       </c>
       <c r="L69" s="18">
@@ -26814,11 +26971,11 @@
       </c>
       <c r="N69" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.99840000000000007</v>
+        <v>0.49920000000000003</v>
       </c>
       <c r="O69" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>17.48</v>
+        <v>8.74</v>
       </c>
       <c r="P69" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26826,7 +26983,7 @@
       </c>
       <c r="Q69" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R69" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26834,11 +26991,11 @@
       </c>
       <c r="S69" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T69" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="U69" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -26846,7 +27003,7 @@
       </c>
       <c r="V69" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1440</v>
+        <v>680</v>
       </c>
       <c r="W69" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -26873,13 +27030,15 @@
         <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
       </c>
       <c r="AC69" s="29">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:29">
+    <row r="70" spans="1:29" ht="20">
+      <c r="A70" s="36"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>NC24r</v>
+        <v>NC24</v>
       </c>
       <c r="D70" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -26887,7 +27046,7 @@
       </c>
       <c r="E70" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>MS NC24r</v>
+        <v>MS NC24</v>
       </c>
       <c r="F70" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -26895,7 +27054,7 @@
       </c>
       <c r="G70" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>3.96</v>
+        <v>3.6</v>
       </c>
       <c r="H70" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -26965,9 +27124,9 @@
         <f t="shared" ca="1" si="42"/>
         <v>0</v>
       </c>
-      <c r="Y70" s="13" t="str">
+      <c r="Y70" s="13">
         <f t="shared" ca="1" si="45"/>
-        <v>Infiniband/</v>
+        <v>0</v>
       </c>
       <c r="Z70" s="13">
         <f t="shared" ca="1" si="44"/>
@@ -26979,18 +27138,16 @@
       </c>
       <c r="AB70" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Prices for West US 2 region.. Charged per minute. RDMA capable.</v>
+        <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
       </c>
       <c r="AC70" s="29">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="20">
-      <c r="A71" s="36"/>
-      <c r="B71" s="15"/>
+    <row r="71" spans="1:29">
       <c r="C71" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>NV6</v>
+        <v>NC24r</v>
       </c>
       <c r="D71" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -26998,7 +27155,7 @@
       </c>
       <c r="E71" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>MS NV6</v>
+        <v>MS NC24r</v>
       </c>
       <c r="F71" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27006,7 +27163,7 @@
       </c>
       <c r="G71" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>1.24</v>
+        <v>3.96</v>
       </c>
       <c r="H71" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27034,19 +27191,19 @@
       </c>
       <c r="N71" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.24960000000000002</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="O71" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>9.65</v>
+        <v>17.48</v>
       </c>
       <c r="P71" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>M60</v>
+        <v>K80</v>
       </c>
       <c r="Q71" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R71" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -27054,11 +27211,11 @@
       </c>
       <c r="S71" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="T71" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>56</v>
+        <v>224</v>
       </c>
       <c r="U71" s="13" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -27066,7 +27223,7 @@
       </c>
       <c r="V71" s="13">
         <f t="shared" ca="1" si="42"/>
-        <v>340</v>
+        <v>1440</v>
       </c>
       <c r="W71" s="13">
         <f t="shared" ca="1" si="42"/>
@@ -27076,9 +27233,9 @@
         <f t="shared" ca="1" si="42"/>
         <v>0</v>
       </c>
-      <c r="Y71" s="13">
+      <c r="Y71" s="13" t="str">
         <f t="shared" ca="1" si="45"/>
-        <v>0</v>
+        <v>Infiniband/</v>
       </c>
       <c r="Z71" s="13">
         <f t="shared" ca="1" si="44"/>
@@ -27090,16 +27247,18 @@
       </c>
       <c r="AB71" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
+        <v>Prices for West US 2 region.. Charged per minute. RDMA capable.</v>
       </c>
       <c r="AC71" s="29">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:29">
+    <row r="72" spans="1:29" ht="20">
+      <c r="A72" s="36"/>
+      <c r="B72" s="15"/>
       <c r="C72" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>NV12</v>
+        <v>NV6</v>
       </c>
       <c r="D72" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27107,7 +27266,7 @@
       </c>
       <c r="E72" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>MS NV12</v>
+        <v>MS NV6</v>
       </c>
       <c r="F72" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27115,7 +27274,7 @@
       </c>
       <c r="G72" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>2.48</v>
+        <v>1.24</v>
       </c>
       <c r="H72" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27143,54 +27302,54 @@
       </c>
       <c r="N72" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.49920000000000003</v>
+        <v>0.24960000000000002</v>
       </c>
       <c r="O72" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>19.3</v>
+        <v>9.65</v>
       </c>
       <c r="P72" s="13" t="str">
-        <f t="shared" ref="P72:AA89" ca="1" si="52">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="42"/>
         <v>M60</v>
       </c>
       <c r="Q72" s="13">
-        <f t="shared" ca="1" si="52"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="42"/>
+        <v>1</v>
       </c>
       <c r="R72" s="13" t="str">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="42"/>
         <v>Xeon E5-2690 v3</v>
       </c>
       <c r="S72" s="13">
-        <f t="shared" ca="1" si="52"/>
-        <v>0.5</v>
+        <f t="shared" ca="1" si="42"/>
+        <v>0.25</v>
       </c>
       <c r="T72" s="13">
-        <f t="shared" ca="1" si="52"/>
-        <v>112</v>
+        <f t="shared" ca="1" si="42"/>
+        <v>56</v>
       </c>
       <c r="U72" s="13" t="str">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="42"/>
         <v>SSD</v>
       </c>
       <c r="V72" s="13">
-        <f t="shared" ca="1" si="52"/>
-        <v>680</v>
+        <f t="shared" ca="1" si="42"/>
+        <v>340</v>
       </c>
       <c r="W72" s="13">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="42"/>
         <v>0</v>
       </c>
       <c r="X72" s="13">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="42"/>
         <v>0</v>
       </c>
       <c r="Y72" s="13">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="45"/>
         <v>0</v>
       </c>
       <c r="Z72" s="13">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="44"/>
         <v>0</v>
       </c>
       <c r="AA72" s="13">
@@ -27202,13 +27361,13 @@
         <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
       </c>
       <c r="AC72" s="29">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:29">
       <c r="C73" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>NV24</v>
+        <v>NV12</v>
       </c>
       <c r="D73" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27216,7 +27375,7 @@
       </c>
       <c r="E73" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>MS NV24</v>
+        <v>MS NV12</v>
       </c>
       <c r="F73" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27224,7 +27383,7 @@
       </c>
       <c r="G73" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>4.97</v>
+        <v>2.48</v>
       </c>
       <c r="H73" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27252,19 +27411,19 @@
       </c>
       <c r="N73" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.99840000000000007</v>
+        <v>0.49920000000000003</v>
       </c>
       <c r="O73" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>38.6</v>
+        <v>19.3</v>
       </c>
       <c r="P73" s="13" t="str">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ref="P73:AA90" ca="1" si="52">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>M60</v>
       </c>
       <c r="Q73" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R73" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27272,11 +27431,11 @@
       </c>
       <c r="S73" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T73" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>224</v>
+        <v>112</v>
       </c>
       <c r="U73" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27284,7 +27443,7 @@
       </c>
       <c r="V73" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>1440</v>
+        <v>680</v>
       </c>
       <c r="W73" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27303,7 +27462,7 @@
         <v>0</v>
       </c>
       <c r="AA73" s="13">
-        <f t="shared" ca="1" si="52"/>
+        <f t="shared" ca="1" si="50"/>
         <v>0</v>
       </c>
       <c r="AB73" s="15" t="str">
@@ -27311,21 +27470,13 @@
         <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
       </c>
       <c r="AC73" s="29">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:29" ht="19">
-      <c r="A74" s="35" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>Google</v>
-      </c>
-      <c r="B74" s="15" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
-        <v>https://cloud.google.com/compute/docs/machine-types</v>
-      </c>
+    <row r="74" spans="1:29">
       <c r="C74" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>8c52mK80</v>
+        <v>NV24</v>
       </c>
       <c r="D74" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27333,7 +27484,7 @@
       </c>
       <c r="E74" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 8c52mK80</v>
+        <v>MS NV24</v>
       </c>
       <c r="F74" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27341,7 +27492,7 @@
       </c>
       <c r="G74" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>0.99</v>
+        <v>4.97</v>
       </c>
       <c r="H74" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27369,31 +27520,31 @@
       </c>
       <c r="N74" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.28160000000000002</v>
+        <v>0.99840000000000007</v>
       </c>
       <c r="O74" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>4.37</v>
+        <v>38.6</v>
       </c>
       <c r="P74" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>K80</v>
+        <v>M60</v>
       </c>
       <c r="Q74" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>0.5</v>
-      </c>
-      <c r="R74" s="13">
+        <v>4</v>
+      </c>
+      <c r="R74" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>0</v>
+        <v>Xeon E5-2690 v3</v>
       </c>
       <c r="S74" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T74" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="U74" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27401,7 +27552,7 @@
       </c>
       <c r="V74" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>375</v>
+        <v>1440</v>
       </c>
       <c r="W74" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27424,17 +27575,25 @@
         <v>0</v>
       </c>
       <c r="AB74" s="15" t="str">
-        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 2 hyper threads per physical core.</v>
+        <f t="shared" ca="1" si="49"/>
+        <v xml:space="preserve">Prices for West US 2 region. Charged per minute. </v>
       </c>
       <c r="AC74" s="29">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:29">
+    <row r="75" spans="1:29" ht="19">
+      <c r="A75" s="35" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>Google</v>
+      </c>
+      <c r="B75" s="15" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
+        <v>https://cloud.google.com/compute/docs/machine-types</v>
+      </c>
       <c r="C75" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>12c78mK80x2</v>
+        <v>8c52mK80</v>
       </c>
       <c r="D75" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27442,7 +27601,7 @@
       </c>
       <c r="E75" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 12c78mK80x2</v>
+        <v>GL 8c52mK80</v>
       </c>
       <c r="F75" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27450,7 +27609,7 @@
       </c>
       <c r="G75" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>1.69</v>
+        <v>0.99</v>
       </c>
       <c r="H75" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27478,11 +27637,11 @@
       </c>
       <c r="N75" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.4224</v>
+        <v>0.28160000000000002</v>
       </c>
       <c r="O75" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>8.74</v>
+        <v>4.37</v>
       </c>
       <c r="P75" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27490,7 +27649,7 @@
       </c>
       <c r="Q75" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R75" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27498,11 +27657,11 @@
       </c>
       <c r="S75" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="T75" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="U75" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27534,16 +27693,16 @@
       </c>
       <c r="AB75" s="15" t="str">
         <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
+        <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 2 hyper threads per physical core.</v>
       </c>
       <c r="AC75" s="29">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:29">
       <c r="C76" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>24c156mK80x4</v>
+        <v>12c78mK80x2</v>
       </c>
       <c r="D76" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27551,7 +27710,7 @@
       </c>
       <c r="E76" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 24c156mK80x4</v>
+        <v>GL 12c78mK80x2</v>
       </c>
       <c r="F76" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27559,7 +27718,7 @@
       </c>
       <c r="G76" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>3.33</v>
+        <v>1.69</v>
       </c>
       <c r="H76" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27587,11 +27746,11 @@
       </c>
       <c r="N76" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.8448</v>
+        <v>0.4224</v>
       </c>
       <c r="O76" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>17.48</v>
+        <v>8.74</v>
       </c>
       <c r="P76" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27599,7 +27758,7 @@
       </c>
       <c r="Q76" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R76" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27607,11 +27766,11 @@
       </c>
       <c r="S76" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="T76" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="U76" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27642,17 +27801,17 @@
         <v>0</v>
       </c>
       <c r="AB76" s="15" t="str">
-        <f t="shared" ca="1" si="49"/>
+        <f ca="1">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC76" s="29">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:29">
       <c r="C77" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>32c208mK80x4</v>
+        <v>24c156mK80x4</v>
       </c>
       <c r="D77" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27660,7 +27819,7 @@
       </c>
       <c r="E77" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 32c208mK80x4</v>
+        <v>GL 24c156mK80x4</v>
       </c>
       <c r="F77" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27668,7 +27827,7 @@
       </c>
       <c r="G77" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>3.79</v>
+        <v>3.33</v>
       </c>
       <c r="H77" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27696,7 +27855,7 @@
       </c>
       <c r="N77" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>1.1264000000000001</v>
+        <v>0.8448</v>
       </c>
       <c r="O77" s="13">
         <f t="shared" ca="1" si="51"/>
@@ -27716,11 +27875,11 @@
       </c>
       <c r="S77" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="T77" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="U77" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27755,13 +27914,13 @@
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC77" s="29">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:29">
       <c r="C78" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>64c416mK80x8</v>
+        <v>32c208mK80x4</v>
       </c>
       <c r="D78" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27769,7 +27928,7 @@
       </c>
       <c r="E78" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 64c416mK80x8</v>
+        <v>GL 32c208mK80x4</v>
       </c>
       <c r="F78" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27777,7 +27936,7 @@
       </c>
       <c r="G78" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>7.61</v>
+        <v>3.79</v>
       </c>
       <c r="H78" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27805,11 +27964,11 @@
       </c>
       <c r="N78" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>2.2528000000000001</v>
+        <v>1.1264000000000001</v>
       </c>
       <c r="O78" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>34.96</v>
+        <v>17.48</v>
       </c>
       <c r="P78" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27817,7 +27976,7 @@
       </c>
       <c r="Q78" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R78" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27825,11 +27984,11 @@
       </c>
       <c r="S78" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="T78" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>416</v>
+        <v>208</v>
       </c>
       <c r="U78" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27864,13 +28023,13 @@
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC78" s="29">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:29" s="12" customFormat="1">
+    <row r="79" spans="1:29">
       <c r="C79" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>8c52mP100</v>
+        <v>64c416mK80x8</v>
       </c>
       <c r="D79" s="15">
         <f t="shared" ca="1" si="46"/>
@@ -27878,7 +28037,7 @@
       </c>
       <c r="E79" s="21" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>GL 8c52mP100</v>
+        <v>GL 64c416mK80x8</v>
       </c>
       <c r="F79" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27886,7 +28045,7 @@
       </c>
       <c r="G79" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>2</v>
+        <v>7.61</v>
       </c>
       <c r="H79" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -27914,19 +28073,19 @@
       </c>
       <c r="N79" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.28160000000000002</v>
+        <v>2.2528000000000001</v>
       </c>
       <c r="O79" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>9.5</v>
+        <v>34.96</v>
       </c>
       <c r="P79" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>P100</v>
+        <v>K80</v>
       </c>
       <c r="Q79" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R79" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -27934,11 +28093,11 @@
       </c>
       <c r="S79" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="T79" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>52</v>
+        <v>416</v>
       </c>
       <c r="U79" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -27973,21 +28132,21 @@
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC79" s="29">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:29" s="12" customFormat="1">
       <c r="C80" s="21" t="str">
-        <f t="shared" ref="C80:E81" ca="1" si="53">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>24c156mP100x2</v>
+        <f t="shared" ca="1" si="46"/>
+        <v>8c52mP100</v>
       </c>
       <c r="D80" s="15">
-        <f t="shared" ca="1" si="53"/>
+        <f t="shared" ca="1" si="46"/>
         <v>0</v>
       </c>
       <c r="E80" s="21" t="str">
-        <f t="shared" ca="1" si="53"/>
-        <v>GL 24c156mP100x2</v>
+        <f t="shared" ca="1" si="46"/>
+        <v>GL 8c52mP100</v>
       </c>
       <c r="F80" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -27995,7 +28154,7 @@
       </c>
       <c r="G80" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>4.45</v>
+        <v>2</v>
       </c>
       <c r="H80" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -28023,11 +28182,11 @@
       </c>
       <c r="N80" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.8448</v>
+        <v>0.28160000000000002</v>
       </c>
       <c r="O80" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>19</v>
+        <v>9.5</v>
       </c>
       <c r="P80" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28035,7 +28194,7 @@
       </c>
       <c r="Q80" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R80" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28043,11 +28202,11 @@
       </c>
       <c r="S80" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="T80" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>156</v>
+        <v>52</v>
       </c>
       <c r="U80" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28082,13 +28241,13 @@
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC80" s="29">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:29" s="12" customFormat="1">
       <c r="C81" s="21" t="str">
-        <f t="shared" ca="1" si="53"/>
-        <v>64c416mP100x4</v>
+        <f t="shared" ref="C81:E82" ca="1" si="53">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>24c156mP100x2</v>
       </c>
       <c r="D81" s="15">
         <f t="shared" ca="1" si="53"/>
@@ -28096,7 +28255,7 @@
       </c>
       <c r="E81" s="21" t="str">
         <f t="shared" ca="1" si="53"/>
-        <v>GL 64c416mP100x4</v>
+        <v>GL 24c156mP100x2</v>
       </c>
       <c r="F81" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -28104,7 +28263,7 @@
       </c>
       <c r="G81" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>9.85</v>
+        <v>4.45</v>
       </c>
       <c r="H81" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -28132,11 +28291,11 @@
       </c>
       <c r="N81" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>2.2528000000000001</v>
+        <v>0.8448</v>
       </c>
       <c r="O81" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="P81" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28144,7 +28303,7 @@
       </c>
       <c r="Q81" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R81" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28152,11 +28311,11 @@
       </c>
       <c r="S81" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="T81" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>416</v>
+        <v>156</v>
       </c>
       <c r="U81" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28191,29 +28350,21 @@
         <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC81" s="29">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:29" ht="19">
-      <c r="A82" s="35" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>IDCF</v>
-      </c>
-      <c r="B82" s="15" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
-        <v>https://www.idcf.jp/service/deeplearning/</v>
-      </c>
+    <row r="82" spans="1:29" s="12" customFormat="1">
       <c r="C82" s="21" t="str">
-        <f t="shared" ref="C82:E89" ca="1" si="54">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
-        <v>GPU.7XL P100</v>
+        <f t="shared" ca="1" si="53"/>
+        <v>64c416mP100x4</v>
       </c>
       <c r="D82" s="15">
-        <f t="shared" ca="1" si="54"/>
+        <f t="shared" ca="1" si="53"/>
         <v>0</v>
       </c>
       <c r="E82" s="21" t="str">
-        <f t="shared" ca="1" si="54"/>
-        <v>IDCF P100</v>
+        <f t="shared" ca="1" si="53"/>
+        <v>GL 64c416mP100x4</v>
       </c>
       <c r="F82" s="18">
         <f t="shared" ca="1" si="5"/>
@@ -28221,7 +28372,7 @@
       </c>
       <c r="G82" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>440</v>
+        <v>9.85</v>
       </c>
       <c r="H82" s="18">
         <f t="shared" ca="1" si="47"/>
@@ -28237,7 +28388,7 @@
       </c>
       <c r="K82" s="18">
         <f t="shared" ca="1" si="47"/>
-        <v>220000</v>
+        <v>0</v>
       </c>
       <c r="L82" s="18">
         <f t="shared" ca="1" si="16"/>
@@ -28245,15 +28396,15 @@
       </c>
       <c r="M82" s="18" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>JPY</v>
+        <v>USD</v>
       </c>
       <c r="N82" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>2.2400000000000002</v>
+        <v>2.2528000000000001</v>
       </c>
       <c r="O82" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>9.5</v>
+        <v>38</v>
       </c>
       <c r="P82" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28261,7 +28412,7 @@
       </c>
       <c r="Q82" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R82" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28269,11 +28420,11 @@
       </c>
       <c r="S82" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="T82" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>256</v>
+        <v>416</v>
       </c>
       <c r="U82" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28281,7 +28432,7 @@
       </c>
       <c r="V82" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2100</v>
+        <v>375</v>
       </c>
       <c r="W82" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28305,16 +28456,24 @@
       </c>
       <c r="AB82" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</v>
+        <v>Prices for Oregon region, custom machine types. Virtual CPU is implemented as a single hardware hyper-thread. CPU performance is calculated for a 2.2 GHz Intel Xeon E5 v4 (Broadwell).&lt;br&gt;Assumption: CPU considered to have 3 hyper threads per physical core</v>
       </c>
       <c r="AC82" s="29">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
-    <row r="83" spans="1:29">
+    <row r="83" spans="1:29" ht="19">
+      <c r="A83" s="35" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>IDCF</v>
+      </c>
+      <c r="B83" s="15" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
+        <v>https://www.idcf.jp/service/deeplearning/</v>
+      </c>
       <c r="C83" s="21" t="str">
-        <f t="shared" ca="1" si="54"/>
-        <v>GPU.7XL M40</v>
+        <f t="shared" ref="C83:E90" ca="1" si="54">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <v>GPU.7XL P100</v>
       </c>
       <c r="D83" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28322,31 +28481,31 @@
       </c>
       <c r="E83" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>IDCF M40</v>
+        <v>IDCF P100</v>
       </c>
       <c r="F83" s="18">
-        <f t="shared" ref="F83:L89" ca="1" si="55">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G83" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>400</v>
+        <v>440</v>
       </c>
       <c r="H83" s="18">
-        <f t="shared" ref="H83:K84" ca="1" si="56">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
+        <f t="shared" ca="1" si="47"/>
         <v>0</v>
       </c>
       <c r="I83" s="18">
-        <f t="shared" ca="1" si="56"/>
+        <f t="shared" ca="1" si="47"/>
         <v>0</v>
       </c>
       <c r="J83" s="18">
-        <f t="shared" ca="1" si="56"/>
+        <f t="shared" ca="1" si="47"/>
         <v>0</v>
       </c>
       <c r="K83" s="18">
-        <f t="shared" ca="1" si="56"/>
-        <v>198000</v>
+        <f t="shared" ca="1" si="47"/>
+        <v>220000</v>
       </c>
       <c r="L83" s="18">
         <f t="shared" ca="1" si="16"/>
@@ -28362,11 +28521,11 @@
       </c>
       <c r="O83" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>6.8440000000000003</v>
+        <v>9.5</v>
       </c>
       <c r="P83" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>M40</v>
+        <v>P100</v>
       </c>
       <c r="Q83" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28414,24 +28573,16 @@
       </c>
       <c r="AB83" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</v>
+        <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30000 JPY.</v>
       </c>
       <c r="AC83" s="29">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:29" ht="19">
-      <c r="A84" s="35" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
-        <v>Tsubame 2.5</v>
-      </c>
-      <c r="B84" s="15" t="str">
-        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
-        <v>http://tsubame.gsic.titech.ac.jp/en/paid-services</v>
-      </c>
+    <row r="84" spans="1:29">
       <c r="C84" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>S</v>
+        <v>GPU.7XL M40</v>
       </c>
       <c r="D84" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28439,18 +28590,18 @@
       </c>
       <c r="E84" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.S</v>
+        <v>IDCF M40</v>
       </c>
       <c r="F84" s="18">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ref="F84:L90" ca="1" si="55">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="G84" s="13">
         <f t="shared" ca="1" si="43"/>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="H84" s="18">
-        <f t="shared" ca="1" si="56"/>
+        <f t="shared" ref="H84:K85" ca="1" si="56">INDIRECT("Sheet1!"&amp;INDIRECT("R1C"&amp;COLUMN(),FALSE)&amp;INDIRECT("AC"&amp;ROW()))</f>
         <v>0</v>
       </c>
       <c r="I84" s="18">
@@ -28459,11 +28610,11 @@
       </c>
       <c r="J84" s="18">
         <f t="shared" ca="1" si="56"/>
-        <v>480000</v>
+        <v>0</v>
       </c>
       <c r="K84" s="18">
         <f t="shared" ca="1" si="56"/>
-        <v>0</v>
+        <v>198000</v>
       </c>
       <c r="L84" s="18">
         <f t="shared" ca="1" si="16"/>
@@ -28475,23 +28626,23 @@
       </c>
       <c r="N84" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>0.28128000000000003</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="O84" s="13">
         <f t="shared" ca="1" si="51"/>
-        <v>10.571999999999999</v>
+        <v>6.8440000000000003</v>
       </c>
       <c r="P84" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>K20</v>
+        <v>M40</v>
       </c>
       <c r="Q84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>3</v>
-      </c>
-      <c r="R84" s="13" t="str">
+        <v>1</v>
+      </c>
+      <c r="R84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>Xeon X5670</v>
+        <v>0</v>
       </c>
       <c r="S84" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28499,7 +28650,7 @@
       </c>
       <c r="T84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="U84" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28507,7 +28658,7 @@
       </c>
       <c r="V84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>50</v>
+        <v>2100</v>
       </c>
       <c r="W84" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28517,30 +28668,38 @@
         <f t="shared" ca="1" si="52"/>
         <v>0</v>
       </c>
-      <c r="Y84" s="13" t="str">
+      <c r="Y84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>80/</v>
+        <v>0</v>
       </c>
       <c r="Z84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AA84" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AB84" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>3.24GB of network traffic included with 10 JPY per additional 1 GB, or 100Mbps unlimited traffic for a flat monthly rate of 30001 JPY.</v>
       </c>
       <c r="AC84" s="29">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="85" spans="1:29">
+    <row r="85" spans="1:29" ht="19">
+      <c r="A85" s="35" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C"&amp;COLUMN(),FALSE) &amp; INDIRECT("AC" &amp; ROW()))</f>
+        <v>Tsubame 2.5</v>
+      </c>
+      <c r="B85" s="15" t="str">
+        <f ca="1">INDIRECT("Sheet1!" &amp; INDIRECT("R1C1",FALSE) &amp; (INDIRECT("AC" &amp; ROW())+1))</f>
+        <v>http://tsubame.gsic.titech.ac.jp/en/paid-services</v>
+      </c>
       <c r="C85" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>S open</v>
+        <v>S</v>
       </c>
       <c r="D85" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28548,30 +28707,30 @@
       </c>
       <c r="E85" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.S open</v>
+        <v>Tsub.S</v>
       </c>
       <c r="F85" s="18">
         <f t="shared" ca="1" si="55"/>
         <v>0</v>
       </c>
       <c r="G85" s="13">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ca="1" si="43"/>
         <v>0</v>
       </c>
       <c r="H85" s="18">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ca="1" si="56"/>
         <v>0</v>
       </c>
       <c r="I85" s="18">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ca="1" si="56"/>
         <v>0</v>
       </c>
       <c r="J85" s="18">
-        <f t="shared" ca="1" si="55"/>
-        <v>120000</v>
+        <f t="shared" ca="1" si="56"/>
+        <v>480000</v>
       </c>
       <c r="K85" s="18">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ca="1" si="56"/>
         <v>0</v>
       </c>
       <c r="L85" s="18">
@@ -28640,16 +28799,16 @@
       </c>
       <c r="AB85" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC85" s="29">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:29">
       <c r="C86" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>S96</v>
+        <v>S open</v>
       </c>
       <c r="D86" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28657,7 +28816,7 @@
       </c>
       <c r="E86" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.S96</v>
+        <v>Tsub.S open</v>
       </c>
       <c r="F86" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28677,7 +28836,7 @@
       </c>
       <c r="J86" s="18">
         <f t="shared" ca="1" si="55"/>
-        <v>480000</v>
+        <v>120000</v>
       </c>
       <c r="K86" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28717,7 +28876,7 @@
       </c>
       <c r="T86" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="U86" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28741,7 +28900,7 @@
       </c>
       <c r="Z86" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="AA86" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28749,16 +28908,16 @@
       </c>
       <c r="AB86" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC86" s="29">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:29">
       <c r="C87" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>S96 open</v>
+        <v>S96</v>
       </c>
       <c r="D87" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28766,7 +28925,7 @@
       </c>
       <c r="E87" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.S96 open</v>
+        <v>Tsub.S96</v>
       </c>
       <c r="F87" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28786,7 +28945,7 @@
       </c>
       <c r="J87" s="18">
         <f t="shared" ca="1" si="55"/>
-        <v>120000</v>
+        <v>480000</v>
       </c>
       <c r="K87" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28858,16 +29017,16 @@
       </c>
       <c r="AB87" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC87" s="29">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:29">
       <c r="C88" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>G</v>
+        <v>S96 open</v>
       </c>
       <c r="D88" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28875,7 +29034,7 @@
       </c>
       <c r="E88" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.G</v>
+        <v>Tsub.S96 open</v>
       </c>
       <c r="F88" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28895,7 +29054,7 @@
       </c>
       <c r="J88" s="18">
         <f t="shared" ca="1" si="55"/>
-        <v>480000</v>
+        <v>120000</v>
       </c>
       <c r="K88" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -28911,7 +29070,7 @@
       </c>
       <c r="N88" s="13">
         <f t="shared" ca="1" si="33"/>
-        <v>9.376000000000001E-2</v>
+        <v>0.28128000000000003</v>
       </c>
       <c r="O88" s="13">
         <f t="shared" ca="1" si="51"/>
@@ -28931,11 +29090,11 @@
       </c>
       <c r="S88" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>0.66666666666666663</v>
+        <v>2</v>
       </c>
       <c r="T88" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="U88" s="13" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -28943,7 +29102,7 @@
       </c>
       <c r="V88" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="W88" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28959,7 +29118,7 @@
       </c>
       <c r="Z88" s="13">
         <f t="shared" ca="1" si="52"/>
-        <v>6000</v>
+        <v>2500</v>
       </c>
       <c r="AA88" s="13">
         <f t="shared" ca="1" si="52"/>
@@ -28967,16 +29126,16 @@
       </c>
       <c r="AB88" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC88" s="29">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:29">
       <c r="C89" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>G open</v>
+        <v>G</v>
       </c>
       <c r="D89" s="15">
         <f t="shared" ca="1" si="54"/>
@@ -28984,7 +29143,7 @@
       </c>
       <c r="E89" s="21" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>Tsub.G open</v>
+        <v>Tsub.G</v>
       </c>
       <c r="F89" s="18">
         <f t="shared" ca="1" si="55"/>
@@ -29004,14 +29163,14 @@
       </c>
       <c r="J89" s="18">
         <f t="shared" ca="1" si="55"/>
-        <v>120000</v>
+        <v>480000</v>
       </c>
       <c r="K89" s="18">
         <f t="shared" ca="1" si="55"/>
         <v>0</v>
       </c>
       <c r="L89" s="18">
-        <f t="shared" ca="1" si="55"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="M89" s="18" t="str">
@@ -29076,53 +29235,133 @@
       </c>
       <c r="AB89" s="15" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+        <v>Research group must pass review prior to usage. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
       </c>
       <c r="AC89" s="29">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:29">
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="18"/>
-      <c r="M90" s="18"/>
-      <c r="N90" s="13"/>
-      <c r="O90" s="13"/>
-      <c r="P90" s="13"/>
-      <c r="Q90" s="13"/>
-      <c r="R90" s="13"/>
-      <c r="S90" s="13"/>
-      <c r="T90" s="13"/>
-      <c r="U90" s="13"/>
-      <c r="V90" s="13"/>
-      <c r="W90" s="13"/>
-      <c r="X90" s="13"/>
-      <c r="Y90" s="13"/>
-      <c r="Z90" s="13"/>
-      <c r="AA90" s="13"/>
-      <c r="AB90" s="15"/>
-      <c r="AC90" s="29"/>
+      <c r="C90" s="21" t="str">
+        <f t="shared" ca="1" si="54"/>
+        <v>G open</v>
+      </c>
+      <c r="D90" s="15">
+        <f t="shared" ca="1" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="E90" s="21" t="str">
+        <f t="shared" ca="1" si="54"/>
+        <v>Tsub.G open</v>
+      </c>
+      <c r="F90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="G90" s="13">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="H90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="I90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>120000</v>
+      </c>
+      <c r="K90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="18">
+        <f t="shared" ca="1" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="M90" s="18" t="str">
+        <f t="shared" ca="1" si="48"/>
+        <v>JPY</v>
+      </c>
+      <c r="N90" s="13">
+        <f t="shared" ca="1" si="33"/>
+        <v>9.376000000000001E-2</v>
+      </c>
+      <c r="O90" s="13">
+        <f t="shared" ca="1" si="51"/>
+        <v>10.571999999999999</v>
+      </c>
+      <c r="P90" s="13" t="str">
+        <f t="shared" ca="1" si="52"/>
+        <v>K20</v>
+      </c>
+      <c r="Q90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>3</v>
+      </c>
+      <c r="R90" s="13" t="str">
+        <f t="shared" ca="1" si="52"/>
+        <v>Xeon X5670</v>
+      </c>
+      <c r="S90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>25</v>
+      </c>
+      <c r="U90" s="13" t="str">
+        <f t="shared" ca="1" si="52"/>
+        <v>SSD</v>
+      </c>
+      <c r="V90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>30</v>
+      </c>
+      <c r="W90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="X90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="Y90" s="13" t="str">
+        <f t="shared" ca="1" si="52"/>
+        <v>80/</v>
+      </c>
+      <c r="Z90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>6000</v>
+      </c>
+      <c r="AA90" s="13">
+        <f t="shared" ca="1" si="52"/>
+        <v>2.5</v>
+      </c>
+      <c r="AB90" s="15" t="str">
+        <f t="shared" ca="1" si="49"/>
+        <v>Research group must pass review prior to usage. Research results must be published. Nodes*hours (hours limit) calculated for jobs that run &gt;1 hour and &lt;1 day. Maximum job run time is 4 days.</v>
+      </c>
+      <c r="AC90" s="29">
+        <v>150</v>
+      </c>
     </row>
     <row r="91" spans="1:29">
       <c r="C91" s="21"/>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
       <c r="F91" s="21"/>
-      <c r="G91" s="21"/>
-      <c r="H91" s="21"/>
-      <c r="I91" s="21"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
-      <c r="L91" s="21"/>
-      <c r="M91" s="21"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
       <c r="N91" s="13"/>
       <c r="O91" s="13"/>
       <c r="P91" s="13"/>
@@ -29171,16 +29410,16 @@
     </row>
     <row r="93" spans="1:29">
       <c r="C93" s="21"/>
-      <c r="D93" s="15"/>
+      <c r="D93" s="21"/>
       <c r="E93" s="21"/>
-      <c r="F93" s="18"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="18"/>
-      <c r="L93" s="18"/>
-      <c r="M93" s="18"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="21"/>
       <c r="N93" s="13"/>
       <c r="O93" s="13"/>
       <c r="P93" s="13"/>
@@ -29198,85 +29437,114 @@
       <c r="AB93" s="15"/>
       <c r="AC93" s="29"/>
     </row>
+    <row r="94" spans="1:29">
+      <c r="C94" s="21"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="13"/>
+      <c r="P94" s="13"/>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="13"/>
+      <c r="V94" s="13"/>
+      <c r="W94" s="13"/>
+      <c r="X94" s="13"/>
+      <c r="Y94" s="13"/>
+      <c r="Z94" s="13"/>
+      <c r="AA94" s="13"/>
+      <c r="AB94" s="15"/>
+      <c r="AC94" s="29"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="V43 N40:U43 V40:Y42 M3:T3 L35:M43 U21:W25 U26:V28 L44:V45 Y45 F93 H93 J93:L93 L21:T23 F91:M92 N35:Y39 J35:K45 Z35:AB45 L29:Q34 R30:V34 W26:W34 AA30:AA34 F21:K34 Z3:AA29 K4:T20 AB6:AB34 X4:Y34 J3:J20 C3:H20 F35:H47 C21:E47 C82:D93 E82:E89 F82:F90 J46:V59 R62:V93 M64:Q90 C48:H59 Y46:AB59 W44:X59 I35:I59 W61:AB93 C61:F81 G61:L90 M61:V61 C60:AB60">
-    <cfRule type="expression" dxfId="15" priority="152">
+  <conditionalFormatting sqref="V43 N40:U43 V40:Y42 M3:T3 L35:M43 U21:W25 U26:V28 L44:V45 Y45 F94 H94 J94:L94 L21:T23 F92:M93 N35:Y39 J35:K45 Z35:AB45 L29:Q34 R30:V34 W26:W34 AA30:AA34 F21:K34 Z3:AA29 K4:T20 AB6:AB34 X4:Y34 J3:J20 C3:H20 F35:H47 C21:E47 C83:D94 E83:E90 F83:F91 J46:V59 R63:V94 M65:Q91 C48:H59 Y46:AB59 W44:X59 I35:I59 W62:AB94 C62:F82 G62:L91 M62:V62 C60:AB61">
+    <cfRule type="expression" dxfId="16" priority="152">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43:Y43 Y44 U3:Y3 U4:W20">
-    <cfRule type="expression" dxfId="14" priority="92">
+    <cfRule type="expression" dxfId="15" priority="92">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R29">
-    <cfRule type="expression" dxfId="13" priority="80">
+    <cfRule type="expression" dxfId="14" priority="80">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V29 T29">
-    <cfRule type="expression" dxfId="12" priority="78">
+    <cfRule type="expression" dxfId="13" priority="78">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29">
-    <cfRule type="expression" dxfId="11" priority="79">
+    <cfRule type="expression" dxfId="12" priority="79">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U29">
-    <cfRule type="expression" dxfId="10" priority="77">
+    <cfRule type="expression" dxfId="11" priority="77">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I20">
-    <cfRule type="expression" dxfId="9" priority="68">
+    <cfRule type="expression" dxfId="10" priority="68">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I93">
-    <cfRule type="expression" dxfId="8" priority="38">
+  <conditionalFormatting sqref="I94">
+    <cfRule type="expression" dxfId="9" priority="38">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G93">
-    <cfRule type="expression" dxfId="7" priority="34">
+  <conditionalFormatting sqref="G94">
+    <cfRule type="expression" dxfId="8" priority="34">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M62:Q63">
-    <cfRule type="expression" dxfId="6" priority="33">
+  <conditionalFormatting sqref="M63:Q64">
+    <cfRule type="expression" dxfId="7" priority="33">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M93:Q93 N91:Q92">
-    <cfRule type="expression" dxfId="5" priority="31">
+  <conditionalFormatting sqref="M94:Q94 N92:Q93">
+    <cfRule type="expression" dxfId="6" priority="31">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:T28">
-    <cfRule type="expression" dxfId="4" priority="19">
+    <cfRule type="expression" dxfId="5" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z30:Z34">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7">
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:L3">
-    <cfRule type="expression" dxfId="1" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E90:E93">
-    <cfRule type="expression" dxfId="0" priority="6">
+  <conditionalFormatting sqref="E91:E94">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>